<commit_message>
more tips from the macbook 13 notes were added.
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/technical-tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8969B9F5-28C7-FF4C-A508-58EC8411AD6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4103535A-72E2-394F-91DB-C07524D6E4F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
+    <sheet name="Random Articles" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="410">
   <si>
     <t>docker</t>
   </si>
@@ -1197,6 +1198,75 @@
   </si>
   <si>
     <t>git switch -c &lt;non_existing_branch&gt;</t>
+  </si>
+  <si>
+    <t>5. To push your changes into your remote repo</t>
+  </si>
+  <si>
+    <t>git push &lt;your_remote_name&gt; &lt;your_branch&gt;</t>
+  </si>
+  <si>
+    <t>https://articles.assembla.com/en/articles/1136998-how-to-add-a-new-remote-to-your-git-repo</t>
+  </si>
+  <si>
+    <t>6. Overwrite existing repo content</t>
+  </si>
+  <si>
+    <t>git push -f origin master</t>
+  </si>
+  <si>
+    <t>https://gist.github.com/c0ldlimit/4089101</t>
+  </si>
+  <si>
+    <t>8. What If I Already Have It Checked In?</t>
+  </si>
+  <si>
+    <t>git rm --cached FILENAME</t>
+  </si>
+  <si>
+    <t>9. Setup global .gitignore Rules</t>
+  </si>
+  <si>
+    <t>git config --global core.excludesFile ~/.gitignore</t>
+  </si>
+  <si>
+    <t>1. setup global gitignore file</t>
+  </si>
+  <si>
+    <t>2. edit the ignore file</t>
+  </si>
+  <si>
+    <t>.gitignore Examples in Table</t>
+  </si>
+  <si>
+    <t>https://www.atlassian.com/git/tutorials/saving-changes/gitignore</t>
+  </si>
+  <si>
+    <t>How To Serve A React App From A Python Server</t>
+  </si>
+  <si>
+    <t>https://nitratine.net/blog/post/how-to-serve-a-react-app-from-a-python-server/</t>
+  </si>
+  <si>
+    <t>Python &amp; React</t>
+  </si>
+  <si>
+    <t>Markdown Cheatsheet</t>
+  </si>
+  <si>
+    <t>https://github.com/tchapi/markdown-cheatsheet/blob/master/README.md</t>
+  </si>
+  <si>
+    <t>Python Force Reload Module</t>
+  </si>
+  <si>
+    <t>1. import importlib</t>
+  </si>
+  <si>
+    <t>2. module = importlib.reload(module)</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/reloading-modules-python/</t>
   </si>
 </sst>
 </file>
@@ -1641,10 +1711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B3:I312"/>
+  <dimension ref="B3:I318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="F159" sqref="F159"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="D163" sqref="D163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2501,7 +2571,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D145" t="s">
         <v>355</v>
       </c>
@@ -2509,7 +2579,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D146" t="s">
         <v>356</v>
       </c>
@@ -2517,7 +2587,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C148" t="s">
         <v>370</v>
       </c>
@@ -2525,7 +2595,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D149" t="s">
         <v>371</v>
       </c>
@@ -2533,7 +2603,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D150" t="s">
         <v>373</v>
       </c>
@@ -2541,7 +2611,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D151" t="s">
         <v>375</v>
       </c>
@@ -2549,7 +2619,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D152" t="s">
         <v>377</v>
       </c>
@@ -2557,161 +2627,198 @@
         <v>378</v>
       </c>
     </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C154" t="s">
+    <row r="153" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D153" t="s">
+        <v>387</v>
+      </c>
+      <c r="E153" t="s">
+        <v>388</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="154" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D154" t="s">
+        <v>390</v>
+      </c>
+      <c r="E154" t="s">
+        <v>391</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="156" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C156" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D155" t="s">
+    <row r="157" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D157" t="s">
         <v>381</v>
       </c>
-      <c r="E155" t="s">
+      <c r="E157" t="s">
         <v>382</v>
       </c>
-      <c r="F155" t="s">
+      <c r="F157" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D156" t="s">
+    <row r="158" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D158" t="s">
         <v>383</v>
       </c>
-      <c r="E156" t="s">
+      <c r="E158" t="s">
         <v>384</v>
       </c>
-      <c r="F156" t="s">
+      <c r="F158" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F157" s="1"/>
-    </row>
-    <row r="159" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B159" t="s">
+    <row r="159" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="F159" s="1"/>
+    </row>
+    <row r="160" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C160" t="s">
+        <v>393</v>
+      </c>
+      <c r="E160" t="s">
+        <v>394</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="161" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C161" t="s">
+        <v>395</v>
+      </c>
+      <c r="F161" s="1"/>
+    </row>
+    <row r="162" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D162" t="s">
+        <v>397</v>
+      </c>
+      <c r="E162" t="s">
+        <v>396</v>
+      </c>
+      <c r="F162" s="1"/>
+    </row>
+    <row r="163" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D163" t="s">
+        <v>398</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="G163" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="165" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B165" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="160" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C160" t="s">
+    <row r="166" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C166" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="161" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D161" t="s">
+    <row r="167" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D167" t="s">
         <v>171</v>
       </c>
-      <c r="E161" s="1" t="s">
+      <c r="E167" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="162" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D162" t="s">
+    <row r="168" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D168" t="s">
         <v>175</v>
       </c>
-      <c r="E162" t="s">
+      <c r="E168" t="s">
         <v>173</v>
       </c>
-      <c r="F162" s="1" t="s">
+      <c r="F168" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="163" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C163" t="s">
+    <row r="169" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C169" t="s">
         <v>322</v>
       </c>
-      <c r="E163" s="1" t="s">
+      <c r="E169" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="F163" s="1"/>
-    </row>
-    <row r="164" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F164" s="1"/>
-    </row>
-    <row r="165" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F165" s="1"/>
-    </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F166" s="1"/>
-    </row>
-    <row r="169" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B169" t="s">
+      <c r="F169" s="1"/>
+    </row>
+    <row r="170" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C170" t="s">
+        <v>406</v>
+      </c>
+      <c r="D170" t="s">
+        <v>407</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="F170" s="1"/>
+    </row>
+    <row r="171" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D171" t="s">
+        <v>408</v>
+      </c>
+      <c r="F171" s="1"/>
+    </row>
+    <row r="172" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F172" s="1"/>
+    </row>
+    <row r="175" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B175" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="170" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C170" t="s">
+    <row r="176" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C176" t="s">
         <v>176</v>
       </c>
-      <c r="D170" s="1" t="s">
+      <c r="D176" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="171" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C171" t="s">
+    <row r="177" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C177" t="s">
         <v>178</v>
       </c>
-      <c r="D171" s="1" t="s">
+      <c r="D177" s="1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="172" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C172" t="s">
-        <v>293</v>
-      </c>
-      <c r="D172" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="173" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C173" t="s">
-        <v>294</v>
-      </c>
-      <c r="D173" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="174" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C174" t="s">
-        <v>297</v>
-      </c>
-      <c r="D174" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="175" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D175" s="1"/>
-    </row>
-    <row r="176" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D176" s="1"/>
-    </row>
-    <row r="177" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B177" t="s">
-        <v>343</v>
-      </c>
-      <c r="D177" s="1"/>
     </row>
     <row r="178" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C178" t="s">
-        <v>344</v>
-      </c>
-      <c r="D178" t="s">
-        <v>369</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>345</v>
+        <v>293</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="179" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D179" t="s">
-        <v>368</v>
-      </c>
-      <c r="E179" s="1" t="s">
-        <v>346</v>
+      <c r="C179" t="s">
+        <v>294</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="180" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D180" s="1"/>
+      <c r="C180" t="s">
+        <v>297</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="181" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D181" s="1"/>
@@ -2719,690 +2826,724 @@
     <row r="182" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D182" s="1"/>
     </row>
+    <row r="183" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B183" t="s">
+        <v>343</v>
+      </c>
+      <c r="D183" s="1"/>
+    </row>
+    <row r="184" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C184" t="s">
+        <v>344</v>
+      </c>
+      <c r="D184" t="s">
+        <v>369</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="185" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D185" t="s">
+        <v>368</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
     <row r="186" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B186" t="s">
+      <c r="D186" s="1"/>
+    </row>
+    <row r="187" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D187" s="1"/>
+    </row>
+    <row r="188" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D188" s="1"/>
+    </row>
+    <row r="192" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B192" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="187" spans="2:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="C187" s="4" t="s">
+    <row r="193" spans="3:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="C193" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D187" s="2" t="s">
+      <c r="D193" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E187" s="1" t="s">
+      <c r="E193" s="1" t="s">
         <v>186</v>
-      </c>
-    </row>
-    <row r="188" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C188" t="s">
-        <v>187</v>
-      </c>
-      <c r="E188" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="189" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C189" t="s">
-        <v>215</v>
-      </c>
-      <c r="E189" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="191" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D191" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="193" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C193" t="s">
-        <v>242</v>
-      </c>
-      <c r="D193" t="s">
-        <v>243</v>
-      </c>
-      <c r="E193" s="1" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="194" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C194" t="s">
-        <v>269</v>
-      </c>
-      <c r="D194" t="s">
-        <v>270</v>
+        <v>187</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>271</v>
+        <v>188</v>
       </c>
     </row>
     <row r="195" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C195" t="s">
-        <v>284</v>
+        <v>215</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="196" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E196" s="1" t="s">
-        <v>286</v>
+        <v>189</v>
       </c>
     </row>
     <row r="197" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E197" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="198" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C198" t="s">
-        <v>288</v>
-      </c>
-      <c r="E198" s="1" t="s">
-        <v>289</v>
+      <c r="D197" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="199" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C199" t="s">
-        <v>299</v>
+        <v>242</v>
+      </c>
+      <c r="D199" t="s">
+        <v>243</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>298</v>
+        <v>244</v>
       </c>
     </row>
     <row r="200" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E200" s="1"/>
+      <c r="C200" t="s">
+        <v>269</v>
+      </c>
+      <c r="D200" t="s">
+        <v>270</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="201" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C201" t="s">
+        <v>284</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="202" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E202" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="203" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E203" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="204" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C204" t="s">
+        <v>288</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="205" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C205" t="s">
+        <v>299</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="206" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E206" s="1"/>
+    </row>
+    <row r="207" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C207" t="s">
         <v>359</v>
       </c>
-      <c r="D201" t="s">
+      <c r="D207" t="s">
         <v>360</v>
       </c>
-      <c r="E201" s="1" t="s">
+      <c r="E207" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="202" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E202" s="1"/>
-    </row>
-    <row r="203" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C203" t="s">
+    <row r="208" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E208" s="1"/>
+    </row>
+    <row r="209" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C209" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="204" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D204" t="s">
+    <row r="210" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D210" t="s">
         <v>135</v>
       </c>
-      <c r="E204" t="s">
+      <c r="E210" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="205" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D205" t="s">
-        <v>136</v>
-      </c>
-      <c r="E205" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="206" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D206" t="s">
-        <v>140</v>
-      </c>
-      <c r="E206" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="207" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D207" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="208" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D208" t="s">
-        <v>142</v>
-      </c>
-      <c r="E208" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="210" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C210" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="211" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D211" t="s">
-        <v>73</v>
+        <v>136</v>
       </c>
       <c r="E211" t="s">
-        <v>74</v>
-      </c>
-      <c r="F211" s="1" t="s">
-        <v>75</v>
+        <v>139</v>
       </c>
     </row>
     <row r="212" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D212" t="s">
-        <v>76</v>
-      </c>
-      <c r="E212" s="1" t="s">
-        <v>77</v>
+        <v>140</v>
+      </c>
+      <c r="E212" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="213" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D213" t="s">
-        <v>78</v>
-      </c>
-      <c r="E213" s="1" t="s">
-        <v>79</v>
+        <v>137</v>
       </c>
     </row>
     <row r="214" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D214" t="s">
-        <v>81</v>
-      </c>
-      <c r="E214" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="215" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D215" t="s">
-        <v>362</v>
-      </c>
-      <c r="E215" t="s">
-        <v>365</v>
+        <v>142</v>
+      </c>
+      <c r="E214" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="216" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D216" t="s">
-        <v>363</v>
-      </c>
-      <c r="E216" t="s">
-        <v>364</v>
+      <c r="C216" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="217" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D217" t="s">
+        <v>73</v>
+      </c>
+      <c r="E217" t="s">
+        <v>74</v>
+      </c>
+      <c r="F217" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="218" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D218" t="s">
-        <v>82</v>
-      </c>
-      <c r="E218" t="s">
-        <v>83</v>
+        <v>76</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="219" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D219" t="s">
-        <v>84</v>
-      </c>
-      <c r="E219" t="s">
-        <v>85</v>
+        <v>78</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="220" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D220" t="s">
+        <v>81</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="221" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C221" t="s">
-        <v>366</v>
+      <c r="D221" t="s">
+        <v>362</v>
+      </c>
+      <c r="E221" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="222" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D222" t="s">
-        <v>73</v>
+        <v>363</v>
       </c>
       <c r="E222" t="s">
-        <v>131</v>
-      </c>
-      <c r="F222" s="1"/>
-    </row>
-    <row r="223" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D223" t="s">
-        <v>147</v>
-      </c>
-      <c r="E223" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F223" s="1"/>
+        <v>364</v>
+      </c>
     </row>
     <row r="224" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D224" t="s">
+        <v>82</v>
+      </c>
+      <c r="E224" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="225" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D225" t="s">
+        <v>84</v>
+      </c>
+      <c r="E225" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="227" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C227" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="228" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D228" t="s">
+        <v>73</v>
+      </c>
+      <c r="E228" t="s">
+        <v>131</v>
+      </c>
+      <c r="F228" s="1"/>
+    </row>
+    <row r="229" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D229" t="s">
+        <v>147</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F229" s="1"/>
+    </row>
+    <row r="230" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D230" t="s">
         <v>76</v>
       </c>
-      <c r="E224" s="1" t="s">
+      <c r="E230" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="225" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E225" s="1"/>
-    </row>
-    <row r="226" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D226" t="s">
+    <row r="231" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E231" s="1"/>
+    </row>
+    <row r="232" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D232" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="227" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E227" t="s">
+    <row r="233" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E233" t="s">
         <v>151</v>
       </c>
-      <c r="F227" t="s">
+      <c r="F233" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="228" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E228" t="s">
+    <row r="234" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E234" t="s">
         <v>152</v>
       </c>
-      <c r="F228" t="s">
+      <c r="F234" t="s">
         <v>145</v>
       </c>
-      <c r="G228" s="1" t="s">
+      <c r="G234" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="229" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D229" t="s">
+    <row r="235" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D235" t="s">
         <v>153</v>
       </c>
-      <c r="E229" s="1" t="s">
+      <c r="E235" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G229" s="1"/>
-    </row>
-    <row r="243" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E243" s="1"/>
-    </row>
-    <row r="245" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B245" t="s">
+      <c r="G235" s="1"/>
+    </row>
+    <row r="249" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E249" s="1"/>
+    </row>
+    <row r="251" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B251" t="s">
         <v>276</v>
-      </c>
-    </row>
-    <row r="246" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C246" t="s">
-        <v>277</v>
-      </c>
-      <c r="D246" t="s">
-        <v>279</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="247" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C247" t="s">
-        <v>281</v>
-      </c>
-      <c r="E247" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="F247" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="G247" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="248" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C248" t="s">
-        <v>290</v>
-      </c>
-      <c r="E248" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="249" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C249" t="s">
-        <v>304</v>
-      </c>
-      <c r="E249" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="250" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D250" t="s">
-        <v>306</v>
-      </c>
-      <c r="E250" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="251" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C251" t="s">
-        <v>324</v>
-      </c>
-      <c r="E251" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="252" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C252" t="s">
-        <v>308</v>
+        <v>277</v>
       </c>
       <c r="D252" t="s">
-        <v>309</v>
+        <v>279</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>310</v>
+        <v>278</v>
       </c>
     </row>
     <row r="253" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C253" t="s">
-        <v>311</v>
+        <v>281</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>312</v>
+        <v>280</v>
+      </c>
+      <c r="F253" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G253" s="1" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="254" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C254" t="s">
-        <v>316</v>
+        <v>290</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
     </row>
     <row r="255" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C255" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
     </row>
     <row r="256" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C256" t="s">
-        <v>319</v>
+      <c r="D256" t="s">
+        <v>306</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
     </row>
     <row r="257" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C257" t="s">
-        <v>326</v>
-      </c>
-      <c r="D257" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="258" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C258" t="s">
+        <v>308</v>
+      </c>
       <c r="D258" t="s">
-        <v>328</v>
+        <v>309</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>327</v>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="259" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C259" t="s">
+        <v>311</v>
+      </c>
+      <c r="E259" s="1" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="260" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C260" t="s">
-        <v>330</v>
-      </c>
-      <c r="D260" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>332</v>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="261" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C261" t="s">
+        <v>317</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="262" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C262" t="s">
+        <v>319</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="263" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C263" t="s">
+        <v>326</v>
+      </c>
+      <c r="D263" t="s">
+        <v>333</v>
+      </c>
+      <c r="E263" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="264" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D264" t="s">
+        <v>328</v>
+      </c>
+      <c r="E264" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="266" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C266" t="s">
+        <v>330</v>
+      </c>
+      <c r="D266" t="s">
+        <v>331</v>
+      </c>
+      <c r="E266" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="268" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C268" t="s">
         <v>336</v>
       </c>
-      <c r="D262" t="s">
+      <c r="D268" t="s">
         <v>338</v>
       </c>
-      <c r="E262" s="1" t="s">
+      <c r="E268" s="1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="266" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B266" t="s">
+    <row r="272" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B272" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="267" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C267" t="s">
+    <row r="273" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C273" t="s">
         <v>342</v>
       </c>
-      <c r="D267" t="s">
+      <c r="D273" t="s">
         <v>340</v>
       </c>
-      <c r="E267" s="1" t="s">
+      <c r="E273" s="1" t="s">
         <v>341</v>
-      </c>
-    </row>
-    <row r="273" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B273" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="274" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C274" t="s">
-        <v>87</v>
-      </c>
-      <c r="D274" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="275" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C275" t="s">
-        <v>89</v>
-      </c>
-      <c r="D275" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="276" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C276" t="s">
-        <v>96</v>
-      </c>
-      <c r="D276" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="277" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C277" t="s">
-        <v>98</v>
-      </c>
-      <c r="D277" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="279" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B279" t="s">
-        <v>91</v>
-      </c>
-      <c r="C279" t="s">
-        <v>92</v>
-      </c>
-      <c r="D279" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="280" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C280" t="s">
+        <v>87</v>
+      </c>
+      <c r="D280" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="281" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C281" t="s">
+        <v>89</v>
+      </c>
+      <c r="D281" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="282" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C282" t="s">
+        <v>96</v>
+      </c>
+      <c r="D282" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="283" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C283" t="s">
+        <v>98</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="285" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B285" t="s">
+        <v>91</v>
+      </c>
+      <c r="C285" t="s">
+        <v>92</v>
+      </c>
+      <c r="D285" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="286" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C286" t="s">
         <v>94</v>
       </c>
-      <c r="D280" t="s">
+      <c r="D286" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="283" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B283" t="s">
+    <row r="289" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B289" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="284" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C284" t="s">
+    <row r="290" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C290" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="285" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D285" t="s">
+    <row r="291" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D291" t="s">
         <v>105</v>
       </c>
-      <c r="E285" s="1" t="s">
+      <c r="E291" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="286" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D286" t="s">
+    <row r="292" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D292" t="s">
         <v>102</v>
       </c>
-      <c r="E286" s="1" t="s">
+      <c r="E292" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="287" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D287" t="s">
+    <row r="293" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D293" t="s">
         <v>103</v>
       </c>
-      <c r="E287" s="1" t="s">
+      <c r="E293" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="288" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D288" t="s">
+    <row r="294" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D294" t="s">
         <v>108</v>
       </c>
-      <c r="E288" t="s">
+      <c r="E294" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="290" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B290" t="s">
+    <row r="296" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B296" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="291" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C291" t="s">
+    <row r="297" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C297" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="292" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D292" t="s">
+    <row r="298" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D298" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="293" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D293" t="s">
+    <row r="299" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D299" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="294" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F294" s="1" t="s">
+    <row r="300" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F300" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="295" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B295" t="s">
+    <row r="301" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B301" t="s">
         <v>1</v>
       </c>
-      <c r="F295" s="1" t="s">
+      <c r="F301" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="296" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C296" t="s">
+    <row r="302" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C302" t="s">
         <v>113</v>
       </c>
-      <c r="D296" s="1" t="s">
+      <c r="D302" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="297" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D297" t="s">
+    <row r="303" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D303" t="s">
         <v>127</v>
       </c>
-      <c r="E297" s="1" t="s">
+      <c r="E303" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="298" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C298" t="s">
+    <row r="304" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C304" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="299" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D299" t="s">
+    <row r="305" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D305" t="s">
         <v>116</v>
       </c>
-      <c r="E299" s="1" t="s">
+      <c r="E305" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F299" t="s">
+      <c r="F305" t="s">
         <v>129</v>
       </c>
-      <c r="G299" s="1" t="s">
+      <c r="G305" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="300" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E300" t="s">
+    <row r="306" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E306" t="s">
         <v>122</v>
       </c>
-      <c r="G300" s="1"/>
-    </row>
-    <row r="301" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E301" t="s">
+      <c r="G306" s="1"/>
+    </row>
+    <row r="307" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E307" t="s">
         <v>125</v>
       </c>
-      <c r="G301" s="1"/>
-    </row>
-    <row r="302" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D302" t="s">
+      <c r="G307" s="1"/>
+    </row>
+    <row r="308" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D308" t="s">
         <v>118</v>
       </c>
-      <c r="E302" s="1" t="s">
+      <c r="E308" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G302" s="1"/>
-    </row>
-    <row r="303" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D303" t="s">
+      <c r="G308" s="1"/>
+    </row>
+    <row r="309" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D309" t="s">
         <v>120</v>
       </c>
-      <c r="E303" s="1" t="s">
+      <c r="E309" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G303" s="1"/>
-    </row>
-    <row r="304" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E304" s="1" t="s">
+      <c r="G309" s="1"/>
+    </row>
+    <row r="310" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E310" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="G304" s="1"/>
-    </row>
-    <row r="305" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E305" t="s">
+      <c r="G310" s="1"/>
+    </row>
+    <row r="311" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E311" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="306" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D306" t="s">
+    <row r="312" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D312" t="s">
         <v>302</v>
       </c>
-      <c r="E306" s="1" t="s">
+      <c r="E312" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="307" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D307" t="s">
+    <row r="313" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D313" t="s">
         <v>301</v>
       </c>
-      <c r="E307" s="1" t="s">
+      <c r="E313" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="312" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C312" t="s">
+    <row r="318" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C318" t="s">
         <v>132</v>
       </c>
-      <c r="D312" s="1" t="s">
+      <c r="D318" s="1" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3422,14 +3563,14 @@
     <hyperlink ref="D88" r:id="rId12" xr:uid="{BA9A8F05-4D7F-4942-886C-F8152208F0EA}"/>
     <hyperlink ref="F92" r:id="rId13" xr:uid="{22AE585F-7255-3F41-8A2E-808446F3A9AA}"/>
     <hyperlink ref="F94" r:id="rId14" xr:uid="{93472772-CF6C-D045-B634-2D574A3EE034}"/>
-    <hyperlink ref="E161" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
-    <hyperlink ref="F162" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
-    <hyperlink ref="D170" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
-    <hyperlink ref="D171" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
+    <hyperlink ref="E167" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
+    <hyperlink ref="F168" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
+    <hyperlink ref="D176" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
+    <hyperlink ref="D177" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
     <hyperlink ref="F95" r:id="rId19" xr:uid="{92BE3560-5393-C545-9D2D-2B773359B28F}"/>
-    <hyperlink ref="E187" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
-    <hyperlink ref="E188" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
-    <hyperlink ref="E189" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
+    <hyperlink ref="E193" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
+    <hyperlink ref="E194" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
+    <hyperlink ref="E195" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
     <hyperlink ref="E69" r:id="rId23" xr:uid="{1526D7DA-27DA-1443-928C-BEDA9E425734}"/>
     <hyperlink ref="E70" r:id="rId24" xr:uid="{4F363062-BE49-AB4F-8956-2C1F31D9B898}"/>
     <hyperlink ref="H96" r:id="rId25" xr:uid="{D9E13355-D59B-054F-B544-34A5A285A9E0}"/>
@@ -3446,7 +3587,7 @@
     <hyperlink ref="I96" r:id="rId36" xr:uid="{A03C56E4-1156-A148-A568-F50A5C33DB5C}"/>
     <hyperlink ref="F105" r:id="rId37" xr:uid="{12AC219C-4678-4E43-B328-6595FA10B8D3}"/>
     <hyperlink ref="E107" r:id="rId38" xr:uid="{44409621-28A2-704A-B283-3DCE1EFB1603}"/>
-    <hyperlink ref="E193" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
+    <hyperlink ref="E199" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
     <hyperlink ref="F108" r:id="rId40" xr:uid="{A9D0D792-87D1-8144-872F-5CA060D3C28F}"/>
     <hyperlink ref="F109" r:id="rId41" xr:uid="{87EF989D-17E9-1E45-A075-CD862D0B60F4}"/>
     <hyperlink ref="F111" r:id="rId42" xr:uid="{8406C6F0-DC69-A64D-AAD8-60A33C12D00B}"/>
@@ -3456,69 +3597,116 @@
     <hyperlink ref="F116" r:id="rId46" xr:uid="{3D1C62DB-D9B7-BE42-B21D-4EEBC4C9EFE1}"/>
     <hyperlink ref="F117" r:id="rId47" xr:uid="{F5021A21-70A2-D34E-B055-64CAC326E7EF}"/>
     <hyperlink ref="F118" r:id="rId48" xr:uid="{A8C010A1-8EE1-264B-8688-3BEA1B62E535}"/>
-    <hyperlink ref="E194" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
+    <hyperlink ref="E200" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
     <hyperlink ref="F113" r:id="rId50" location="113521" xr:uid="{EE1413C5-3B38-7D4D-8DF1-634A12F0BD81}"/>
     <hyperlink ref="E71" r:id="rId51" xr:uid="{00B1EF4A-7791-0343-8D8C-9A1E83248FC9}"/>
-    <hyperlink ref="E246" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
-    <hyperlink ref="E247" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
+    <hyperlink ref="E252" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
+    <hyperlink ref="E253" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
     <hyperlink ref="F120" r:id="rId54" xr:uid="{40A4B6A0-2F7E-A84D-8CC6-D814A33F5953}"/>
-    <hyperlink ref="E195" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
-    <hyperlink ref="E196" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
-    <hyperlink ref="E197" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
-    <hyperlink ref="E198" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
-    <hyperlink ref="E248" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
-    <hyperlink ref="D172" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
-    <hyperlink ref="D173" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
-    <hyperlink ref="D174" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
-    <hyperlink ref="E199" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
-    <hyperlink ref="E249" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
-    <hyperlink ref="E250" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
-    <hyperlink ref="E252" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
-    <hyperlink ref="E253" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
-    <hyperlink ref="F247" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
-    <hyperlink ref="G247" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
-    <hyperlink ref="E254" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
-    <hyperlink ref="E255" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
-    <hyperlink ref="E256" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
-    <hyperlink ref="E163" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
-    <hyperlink ref="E251" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
-    <hyperlink ref="E257" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
-    <hyperlink ref="E258" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
+    <hyperlink ref="E201" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
+    <hyperlink ref="E202" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
+    <hyperlink ref="E203" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
+    <hyperlink ref="E204" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
+    <hyperlink ref="E254" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
+    <hyperlink ref="D178" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
+    <hyperlink ref="D179" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
+    <hyperlink ref="D180" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
+    <hyperlink ref="E205" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
+    <hyperlink ref="E255" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
+    <hyperlink ref="E256" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
+    <hyperlink ref="E258" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
+    <hyperlink ref="E259" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
+    <hyperlink ref="F253" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
+    <hyperlink ref="G253" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
+    <hyperlink ref="E260" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
+    <hyperlink ref="E261" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
+    <hyperlink ref="E262" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
+    <hyperlink ref="E169" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
+    <hyperlink ref="E257" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
+    <hyperlink ref="E263" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
+    <hyperlink ref="E264" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
     <hyperlink ref="E73" r:id="rId77" location="code" xr:uid="{C0475FF8-517D-E949-887E-9A42D86E9640}"/>
-    <hyperlink ref="E260" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
+    <hyperlink ref="E266" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
     <hyperlink ref="E74" r:id="rId79" xr:uid="{277DBE6F-F3E5-8B4C-8DD8-BD92445D1A99}"/>
-    <hyperlink ref="E262" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
-    <hyperlink ref="E267" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
-    <hyperlink ref="E178" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
-    <hyperlink ref="E179" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
+    <hyperlink ref="E268" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
+    <hyperlink ref="E273" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
+    <hyperlink ref="E184" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
+    <hyperlink ref="E185" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
     <hyperlink ref="F141" r:id="rId84" xr:uid="{EB604865-A16B-0646-A5B5-0D047467449D}"/>
-    <hyperlink ref="E201" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
-    <hyperlink ref="D276" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
-    <hyperlink ref="D277" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
-    <hyperlink ref="E286" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
-    <hyperlink ref="E287" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
-    <hyperlink ref="E285" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
-    <hyperlink ref="D296" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
-    <hyperlink ref="E302" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
-    <hyperlink ref="E299" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
-    <hyperlink ref="E303" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
-    <hyperlink ref="F294" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
-    <hyperlink ref="F295" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
-    <hyperlink ref="E297" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
-    <hyperlink ref="G299" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
-    <hyperlink ref="D312" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
-    <hyperlink ref="E304" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
-    <hyperlink ref="E307" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
-    <hyperlink ref="E306" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
-    <hyperlink ref="F211" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
-    <hyperlink ref="E212" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
-    <hyperlink ref="E213" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
-    <hyperlink ref="E214" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
-    <hyperlink ref="G228" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
-    <hyperlink ref="E223" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
-    <hyperlink ref="E224" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
-    <hyperlink ref="E229" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
+    <hyperlink ref="E207" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
+    <hyperlink ref="D282" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
+    <hyperlink ref="D283" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
+    <hyperlink ref="E292" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
+    <hyperlink ref="E293" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
+    <hyperlink ref="E291" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
+    <hyperlink ref="D302" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
+    <hyperlink ref="E308" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
+    <hyperlink ref="E305" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
+    <hyperlink ref="E309" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
+    <hyperlink ref="F300" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
+    <hyperlink ref="F301" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
+    <hyperlink ref="E303" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
+    <hyperlink ref="G305" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
+    <hyperlink ref="D318" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
+    <hyperlink ref="E310" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
+    <hyperlink ref="E313" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
+    <hyperlink ref="E312" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
+    <hyperlink ref="F217" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
+    <hyperlink ref="E218" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
+    <hyperlink ref="E219" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
+    <hyperlink ref="E220" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
+    <hyperlink ref="G234" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
+    <hyperlink ref="E229" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
+    <hyperlink ref="E230" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
+    <hyperlink ref="E235" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
     <hyperlink ref="F148" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
+    <hyperlink ref="F153" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
+    <hyperlink ref="F154" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
+    <hyperlink ref="F160" r:id="rId114" xr:uid="{2B03B1F0-535A-3E4F-8FB3-35D2DE847218}"/>
+    <hyperlink ref="G163" r:id="rId115" xr:uid="{11045522-E183-B14C-B43D-5EA36E454600}"/>
+    <hyperlink ref="E170" r:id="rId116" xr:uid="{F1098A8C-3BC0-DB4F-8F9C-48B31145FEC1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
+  <dimension ref="B3:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="38.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C3" t="s">
+        <v>403</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>404</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{622F8353-6ECE-5D45-BC71-7C0259CBCD6A}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{E4AE5252-D67B-B04F-A57B-B5558D672E63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated on random sheet
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/technical-tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0462B81A-0A4C-884B-9150-38E4FF137BB6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC172B6A-64DF-4140-B78D-01A112CDB0D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="413">
   <si>
     <t>docker</t>
   </si>
@@ -1267,6 +1267,15 @@
   </si>
   <si>
     <t>https://www.geeksforgeeks.org/reloading-modules-python/</t>
+  </si>
+  <si>
+    <t>soup.select_one("a[href*=location]")</t>
+  </si>
+  <si>
+    <t>BeautifulSoup to find a link that contains a specific word</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/38252434/beautifulsoup-to-find-a-link-that-contains-a-specific-word</t>
   </si>
 </sst>
 </file>
@@ -1713,7 +1722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
   <dimension ref="B3:I318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+    <sheetView topLeftCell="A135" workbookViewId="0">
       <selection activeCell="D163" sqref="D163"/>
     </sheetView>
   </sheetViews>
@@ -3672,41 +3681,54 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B3:D4"/>
+  <dimension ref="B3:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="38.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="2" max="2" width="51.83203125" customWidth="1"/>
+    <col min="3" max="3" width="38.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>401</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>403</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>404</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>405</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>411</v>
+      </c>
+      <c r="C5" t="s">
+        <v>410</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>412</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{622F8353-6ECE-5D45-BC71-7C0259CBCD6A}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{E4AE5252-D67B-B04F-A57B-B5558D672E63}"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{622F8353-6ECE-5D45-BC71-7C0259CBCD6A}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{E4AE5252-D67B-B04F-A57B-B5558D672E63}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{824EDC81-FF73-F84B-B472-EEB71B3799F7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new sheet 'random tips' added
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/technical-tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC172B6A-64DF-4140-B78D-01A112CDB0D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C8EBE5-40A3-4847-827F-02E4070F47C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="416">
   <si>
     <t>docker</t>
   </si>
@@ -1276,6 +1276,15 @@
   </si>
   <si>
     <t>https://stackoverflow.com/questions/38252434/beautifulsoup-to-find-a-link-that-contains-a-specific-word</t>
+  </si>
+  <si>
+    <t>https://www.git-tower.com/learn/git/faq/undo-last-commit/</t>
+  </si>
+  <si>
+    <t>How can I undo the last commit?</t>
+  </si>
+  <si>
+    <t>git</t>
   </si>
 </sst>
 </file>
@@ -1722,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
   <dimension ref="B3:I318"/>
   <sheetViews>
-    <sheetView topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="D163" sqref="D163"/>
+    <sheetView topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="E163" sqref="E163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3681,10 +3690,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B3:E5"/>
+  <dimension ref="B3:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3724,11 +3733,23 @@
         <v>412</v>
       </c>
     </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>414</v>
+      </c>
+      <c r="D6" t="s">
+        <v>415</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{622F8353-6ECE-5D45-BC71-7C0259CBCD6A}"/>
     <hyperlink ref="E4" r:id="rId2" xr:uid="{E4AE5252-D67B-B04F-A57B-B5558D672E63}"/>
     <hyperlink ref="E5" r:id="rId3" xr:uid="{824EDC81-FF73-F84B-B472-EEB71B3799F7}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{5C86DC30-81A0-FA42-BE56-47F24B9E943B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
random tips sheet added.
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/technical-tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C8EBE5-40A3-4847-827F-02E4070F47C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E256F022-AF82-A740-974B-2B7E02C63E9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -1731,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
   <dimension ref="B3:I318"/>
   <sheetViews>
-    <sheetView topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="E163" sqref="E163"/>
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="B150" sqref="B150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2727,7 +2727,7 @@
       <c r="D163" t="s">
         <v>398</v>
       </c>
-      <c r="F163" s="1" t="s">
+      <c r="F163" t="s">
         <v>399</v>
       </c>
       <c r="G163" s="1" t="s">
@@ -3692,7 +3692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
   <dimension ref="B3:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added https://choosealicense.com as tip
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/technical-tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1A0C79-A3B4-D04C-B235-6E9DB2BE912C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A697F65A-E188-2B49-A363-33DEE6B6D2ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="433">
   <si>
     <t>docker</t>
   </si>
@@ -1330,6 +1330,12 @@
   </si>
   <si>
     <t>https://osxdaily.com/2018/11/10/force-refresh-webpage-without-cache-chrome/</t>
+  </si>
+  <si>
+    <t>Choose an open source license</t>
+  </si>
+  <si>
+    <t>https://choosealicense.com</t>
   </si>
 </sst>
 </file>
@@ -3780,10 +3786,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B3:E8"/>
+  <dimension ref="B3:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3853,6 +3859,14 @@
         <v>430</v>
       </c>
     </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>431</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{622F8353-6ECE-5D45-BC71-7C0259CBCD6A}"/>
@@ -3861,6 +3875,7 @@
     <hyperlink ref="E6" r:id="rId4" xr:uid="{5C86DC30-81A0-FA42-BE56-47F24B9E943B}"/>
     <hyperlink ref="E7" r:id="rId5" xr:uid="{88B61246-4C8E-624B-9227-4D7DCA52085C}"/>
     <hyperlink ref="E8" r:id="rId6" xr:uid="{FAEF115B-DD10-6B4F-8BA2-91D7F10AF164}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{D5678B1D-BFC1-2849-92FC-22CDFD8907E7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated with python and vscode
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/technical-tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAA2142-DAF3-C340-A5C6-14748114A7EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E543E4B-79B1-A247-85DC-666B8B2A36D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="447">
   <si>
     <t>docker</t>
   </si>
@@ -1269,9 +1269,6 @@
     <t>https://www.geeksforgeeks.org/reloading-modules-python/</t>
   </si>
   <si>
-    <t>soup.select_one("a[href*=location]")</t>
-  </si>
-  <si>
     <t>BeautifulSoup to find a link that contains a specific word</t>
   </si>
   <si>
@@ -1354,6 +1351,33 @@
   </si>
   <si>
     <t>https://stackoverflow.com/questions/215718/how-can-i-reset-or-revert-a-file-to-a-specific-revision</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>VS Code</t>
+  </si>
+  <si>
+    <t>Change environmental's fontsize</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/33701933/how-to-change-environments-font-size</t>
+  </si>
+  <si>
+    <t>{"editor.fontSize": 18, "window.zoomLevel": 1.5}</t>
+  </si>
+  <si>
+    <t>Logging logger not printing things</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/17523173/python-logging-streamhandler-is-not-sending-logs-to-stdout</t>
+  </si>
+  <si>
+    <t>https://towardsdatascience.com/using-the-pandas-resample-function-a231144194c4</t>
   </si>
 </sst>
 </file>
@@ -1800,7 +1824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
   <dimension ref="B3:I330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
+    <sheetView topLeftCell="A271" workbookViewId="0">
       <selection activeCell="F171" sqref="F171"/>
     </sheetView>
   </sheetViews>
@@ -2771,7 +2795,7 @@
         <v>393</v>
       </c>
       <c r="D160" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E160" t="s">
         <v>394</v>
@@ -2782,21 +2806,21 @@
     </row>
     <row r="161" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D161" t="s">
+        <v>422</v>
+      </c>
+      <c r="E161" t="s">
         <v>423</v>
       </c>
-      <c r="E161" t="s">
+      <c r="F161" s="1" t="s">
         <v>424</v>
-      </c>
-      <c r="F161" s="1" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="162" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D162" t="s">
+        <v>425</v>
+      </c>
+      <c r="E162" t="s">
         <v>426</v>
-      </c>
-      <c r="E162" t="s">
-        <v>427</v>
       </c>
       <c r="F162" s="1"/>
     </row>
@@ -2828,46 +2852,46 @@
     </row>
     <row r="166" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C166" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G166" s="1"/>
     </row>
     <row r="167" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E167" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G167" s="1"/>
     </row>
     <row r="168" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E168" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="169" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C169" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="170" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D170" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E170" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="171" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D171" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E171" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="177" spans="2:6" x14ac:dyDescent="0.2">
@@ -3829,96 +3853,134 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B3:E9"/>
+  <dimension ref="B2:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="51.83203125" customWidth="1"/>
-    <col min="3" max="3" width="38.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>438</v>
+      </c>
+      <c r="E2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>401</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" t="s">
         <v>403</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>404</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>410</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="C5" t="s">
-        <v>410</v>
-      </c>
-      <c r="E5" s="1" t="s">
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>413</v>
+      </c>
+      <c r="C6" t="s">
+        <v>414</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>414</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>415</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="F7" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
+        <v>428</v>
+      </c>
+      <c r="E8" t="s">
+        <v>427</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="D8" t="s">
-        <v>428</v>
-      </c>
-      <c r="E8" s="1" t="s">
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+      <c r="F9" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>432</v>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>441</v>
+      </c>
+      <c r="C10" t="s">
+        <v>440</v>
+      </c>
+      <c r="E10" t="s">
+        <v>443</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>444</v>
+      </c>
+      <c r="C11" t="s">
+        <v>169</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F12" s="1" t="s">
+        <v>446</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{622F8353-6ECE-5D45-BC71-7C0259CBCD6A}"/>
-    <hyperlink ref="E4" r:id="rId2" xr:uid="{E4AE5252-D67B-B04F-A57B-B5558D672E63}"/>
-    <hyperlink ref="E5" r:id="rId3" xr:uid="{824EDC81-FF73-F84B-B472-EEB71B3799F7}"/>
-    <hyperlink ref="E6" r:id="rId4" xr:uid="{5C86DC30-81A0-FA42-BE56-47F24B9E943B}"/>
-    <hyperlink ref="E7" r:id="rId5" xr:uid="{88B61246-4C8E-624B-9227-4D7DCA52085C}"/>
-    <hyperlink ref="E8" r:id="rId6" xr:uid="{FAEF115B-DD10-6B4F-8BA2-91D7F10AF164}"/>
-    <hyperlink ref="E9" r:id="rId7" xr:uid="{D5678B1D-BFC1-2849-92FC-22CDFD8907E7}"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{622F8353-6ECE-5D45-BC71-7C0259CBCD6A}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{E4AE5252-D67B-B04F-A57B-B5558D672E63}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{824EDC81-FF73-F84B-B472-EEB71B3799F7}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{5C86DC30-81A0-FA42-BE56-47F24B9E943B}"/>
+    <hyperlink ref="F7" r:id="rId5" xr:uid="{88B61246-4C8E-624B-9227-4D7DCA52085C}"/>
+    <hyperlink ref="F8" r:id="rId6" xr:uid="{FAEF115B-DD10-6B4F-8BA2-91D7F10AF164}"/>
+    <hyperlink ref="F9" r:id="rId7" xr:uid="{D5678B1D-BFC1-2849-92FC-22CDFD8907E7}"/>
+    <hyperlink ref="F10" r:id="rId8" xr:uid="{3870A6DA-3C8E-DB44-8768-9877BF1D68EA}"/>
+    <hyperlink ref="F11" r:id="rId9" xr:uid="{A9A7EB14-73E0-AD42-B419-977E7EA5FEA3}"/>
+    <hyperlink ref="F12" r:id="rId10" xr:uid="{E34E01E9-471A-6049-815A-36E8427E6F6A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated with tips on TimescaleDB.
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606D1506-7EC8-1B4F-AB13-640F9D099D3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79B8D79-2007-D64F-A9F2-341D801BF379}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="2120" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="2120" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="532">
   <si>
     <t>docker</t>
   </si>
@@ -1484,6 +1484,156 @@
   </si>
   <si>
     <t>merge two dictionaries in a single expression</t>
+  </si>
+  <si>
+    <t>https://kb.objectrocket.com/timescaledb/managing-tables-with-timescaledb-1601-z</t>
+  </si>
+  <si>
+    <t>TimescaleDB</t>
+  </si>
+  <si>
+    <t>switch to root user</t>
+  </si>
+  <si>
+    <t>sudo -s</t>
+  </si>
+  <si>
+    <t>sudo -i</t>
+  </si>
+  <si>
+    <t>return from root user</t>
+  </si>
+  <si>
+    <t>exit</t>
+  </si>
+  <si>
+    <t>quit</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>https://www.cyberciti.biz/faq/become-superuser-on-ubuntu-linux/</t>
+  </si>
+  <si>
+    <t>Installation</t>
+  </si>
+  <si>
+    <t>https://docs.timescale.com/latest/getting-started/installation/ubuntu/installation-apt-ubuntu</t>
+  </si>
+  <si>
+    <t>echo "deb http://apt.postgresql.org/pub/repos/apt/ $(lsb_release -c -s)-pgdg main" | sudo tee /etc/apt/sources.list.d/pgdg.list</t>
+  </si>
+  <si>
+    <t>1. get the latest PostgreSQL packages</t>
+  </si>
+  <si>
+    <t>wget --quiet -O - https://www.postgresql.org/media/keys/ACCC4CF8.asc | sudo apt-key add -</t>
+  </si>
+  <si>
+    <t>sudo apt-get update</t>
+  </si>
+  <si>
+    <t>2. add Personal Package Archive (PPA)</t>
+  </si>
+  <si>
+    <t>sudo add-apt-repository ppa:timescale/timescaledb-ppa</t>
+  </si>
+  <si>
+    <t>3. install appropriate package for PG (Postgresql) version</t>
+  </si>
+  <si>
+    <t>sudo apt install timescaledb-2-postgresql-13</t>
+  </si>
+  <si>
+    <t>Configure your database</t>
+  </si>
+  <si>
+    <t>2. Restart PostgreSQL instance</t>
+  </si>
+  <si>
+    <t>sudo service postgresql restart</t>
+  </si>
+  <si>
+    <t>1. update your postgresql.conf file</t>
+  </si>
+  <si>
+    <t>sudo timescaledb-tune</t>
+  </si>
+  <si>
+    <t>Connect to PostgreSQL</t>
+  </si>
+  <si>
+    <t>psql -U postgres -h localhost</t>
+  </si>
+  <si>
+    <t>sudo -u postgres psql</t>
+  </si>
+  <si>
+    <t>Option 1: using a superuser named 'postgres' (note this should be the OS user name)</t>
+  </si>
+  <si>
+    <t>Option 2: for other users with sudo privilege</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/7695962/postgresql-password-authentication-failed-for-user-postgres</t>
+  </si>
+  <si>
+    <t>https://heesuk-chad-son.medium.com/storing-realtime-iot-timeseries-data-in-python-timescale-db-raspberry-pi-phidget-sensors-227fab9e21c2</t>
+  </si>
+  <si>
+    <t>General Installation and User Tutorial</t>
+  </si>
+  <si>
+    <t>Check the location of pg_hba.conf file</t>
+  </si>
+  <si>
+    <t>SHOW hba_file;</t>
+  </si>
+  <si>
+    <t>https://askubuntu.com/questions/256534/how-do-i-find-the-path-to-pg-hba-conf-from-the-shell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setup for external connection </t>
+  </si>
+  <si>
+    <t>host all all 0.0.0.0/0 trust</t>
+  </si>
+  <si>
+    <t>1. add line in pg_hba.conf file</t>
+  </si>
+  <si>
+    <t>2. change line in postgresql.conf file</t>
+  </si>
+  <si>
+    <t>listen_addresses='*'</t>
+  </si>
+  <si>
+    <t>https://serverfault.com/questions/336596/opening-port-5432-on-ubuntu</t>
+  </si>
+  <si>
+    <t>Create New Database (and extend it with TimescaleDB)</t>
+  </si>
+  <si>
+    <t>\c tutorial</t>
+  </si>
+  <si>
+    <t>CREATE database name_of_new_database;</t>
+  </si>
+  <si>
+    <t>CREATE EXTENSION IF NOT EXISTS timescaledb;</t>
+  </si>
+  <si>
+    <t>2. Connect to the database</t>
+  </si>
+  <si>
+    <t>3. Extend the database with TimescaleDB</t>
+  </si>
+  <si>
+    <t>1. Create the new database</t>
+  </si>
+  <si>
+    <t>https://docs.timescale.com/latest/getting-started/setup</t>
   </si>
 </sst>
 </file>
@@ -1928,10 +2078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B3:I330"/>
+  <dimension ref="B3:I373"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A347" workbookViewId="0">
+      <selection activeCell="D370" sqref="D370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3255,580 +3405,810 @@
       <c r="E220" s="1"/>
     </row>
     <row r="221" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C221" t="s">
+      <c r="E221" s="1"/>
+    </row>
+    <row r="222" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E222" s="1"/>
+    </row>
+    <row r="223" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E223" s="1"/>
+    </row>
+    <row r="224" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E224" s="1"/>
+    </row>
+    <row r="225" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E225" s="1"/>
+    </row>
+    <row r="226" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E226" s="1"/>
+    </row>
+    <row r="227" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E227" s="1"/>
+    </row>
+    <row r="228" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C228" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="222" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D222" t="s">
+    <row r="229" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D229" t="s">
         <v>135</v>
       </c>
-      <c r="E222" t="s">
+      <c r="E229" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="223" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D223" t="s">
+    <row r="230" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D230" t="s">
         <v>136</v>
       </c>
-      <c r="E223" t="s">
+      <c r="E230" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="224" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D224" t="s">
+    <row r="231" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D231" t="s">
         <v>140</v>
       </c>
-      <c r="E224" t="s">
+      <c r="E231" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="225" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D225" t="s">
+    <row r="232" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D232" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="226" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D226" t="s">
+    <row r="233" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D233" t="s">
         <v>142</v>
       </c>
-      <c r="E226" t="s">
+      <c r="E233" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="228" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C228" t="s">
+    <row r="234" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D234" t="s">
+        <v>484</v>
+      </c>
+      <c r="E234" t="s">
+        <v>486</v>
+      </c>
+      <c r="F234" t="s">
+        <v>490</v>
+      </c>
+      <c r="G234" t="s">
+        <v>485</v>
+      </c>
+      <c r="H234" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="235" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D235" t="s">
+        <v>487</v>
+      </c>
+      <c r="E235" t="s">
+        <v>488</v>
+      </c>
+      <c r="G235" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="237" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C237" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="229" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D229" t="s">
+    <row r="238" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D238" t="s">
         <v>73</v>
       </c>
-      <c r="E229" t="s">
+      <c r="E238" t="s">
         <v>74</v>
       </c>
-      <c r="F229" s="1" t="s">
+      <c r="F238" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="230" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D230" t="s">
+    <row r="239" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D239" t="s">
         <v>76</v>
       </c>
-      <c r="E230" s="1" t="s">
+      <c r="E239" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="231" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D231" t="s">
+    <row r="240" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D240" t="s">
         <v>78</v>
       </c>
-      <c r="E231" s="1" t="s">
+      <c r="E240" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="232" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D232" t="s">
+    <row r="241" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D241" t="s">
         <v>81</v>
       </c>
-      <c r="E232" s="1" t="s">
+      <c r="E241" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="233" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D233" t="s">
+    <row r="242" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D242" t="s">
         <v>362</v>
       </c>
-      <c r="E233" t="s">
+      <c r="E242" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="234" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D234" t="s">
+    <row r="243" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D243" t="s">
         <v>363</v>
       </c>
-      <c r="E234" t="s">
+      <c r="E243" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="236" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D236" t="s">
+    <row r="245" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D245" t="s">
         <v>82</v>
       </c>
-      <c r="E236" t="s">
+      <c r="E245" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="237" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D237" t="s">
+    <row r="246" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D246" t="s">
         <v>84</v>
       </c>
-      <c r="E237" t="s">
+      <c r="E246" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="239" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C239" t="s">
+    <row r="248" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C248" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="240" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D240" t="s">
+    <row r="249" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D249" t="s">
         <v>73</v>
       </c>
-      <c r="E240" t="s">
+      <c r="E249" t="s">
         <v>131</v>
       </c>
-      <c r="F240" s="1"/>
-    </row>
-    <row r="241" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D241" t="s">
+      <c r="F249" s="1"/>
+    </row>
+    <row r="250" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D250" t="s">
         <v>147</v>
       </c>
-      <c r="E241" s="1" t="s">
+      <c r="E250" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F241" s="1"/>
-    </row>
-    <row r="242" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D242" t="s">
+      <c r="F250" s="1"/>
+    </row>
+    <row r="251" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D251" t="s">
         <v>76</v>
       </c>
-      <c r="E242" s="1" t="s">
+      <c r="E251" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="243" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E243" s="1"/>
-    </row>
-    <row r="244" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D244" t="s">
+    <row r="252" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E252" s="1"/>
+    </row>
+    <row r="253" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D253" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="245" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E245" t="s">
+    <row r="254" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E254" t="s">
         <v>151</v>
       </c>
-      <c r="F245" t="s">
+      <c r="F254" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="246" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E246" t="s">
+    <row r="255" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E255" t="s">
         <v>152</v>
       </c>
-      <c r="F246" t="s">
+      <c r="F255" t="s">
         <v>145</v>
       </c>
-      <c r="G246" s="1" t="s">
+      <c r="G255" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="247" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D247" t="s">
+    <row r="256" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D256" t="s">
         <v>153</v>
       </c>
-      <c r="E247" s="1" t="s">
+      <c r="E256" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G247" s="1"/>
-    </row>
-    <row r="261" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E261" s="1"/>
-    </row>
-    <row r="263" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B263" t="s">
+      <c r="G256" s="1"/>
+    </row>
+    <row r="270" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E270" s="1"/>
+    </row>
+    <row r="272" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B272" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="264" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C264" t="s">
+    <row r="273" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C273" t="s">
         <v>277</v>
       </c>
-      <c r="D264" t="s">
+      <c r="D273" t="s">
         <v>279</v>
       </c>
-      <c r="E264" s="1" t="s">
+      <c r="E273" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="265" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C265" t="s">
+    <row r="274" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C274" t="s">
         <v>281</v>
       </c>
-      <c r="E265" s="1" t="s">
+      <c r="E274" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="F265" s="1" t="s">
+      <c r="F274" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="G265" s="1" t="s">
+      <c r="G274" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="266" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C266" t="s">
+    <row r="275" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C275" t="s">
         <v>290</v>
       </c>
-      <c r="E266" s="1" t="s">
+      <c r="E275" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="267" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C267" t="s">
+    <row r="276" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C276" t="s">
         <v>304</v>
       </c>
-      <c r="E267" s="1" t="s">
+      <c r="E276" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="268" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D268" t="s">
+    <row r="277" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D277" t="s">
         <v>306</v>
       </c>
-      <c r="E268" s="1" t="s">
+      <c r="E277" s="1" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="269" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C269" t="s">
+    <row r="278" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C278" t="s">
         <v>324</v>
       </c>
-      <c r="E269" s="1" t="s">
+      <c r="E278" s="1" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="270" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C270" t="s">
+    <row r="279" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C279" t="s">
         <v>308</v>
       </c>
-      <c r="D270" t="s">
+      <c r="D279" t="s">
         <v>309</v>
       </c>
-      <c r="E270" s="1" t="s">
+      <c r="E279" s="1" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="271" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C271" t="s">
+    <row r="280" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C280" t="s">
         <v>311</v>
       </c>
-      <c r="E271" s="1" t="s">
+      <c r="E280" s="1" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="272" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C272" t="s">
+    <row r="281" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C281" t="s">
         <v>316</v>
       </c>
-      <c r="E272" s="1" t="s">
+      <c r="E281" s="1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="273" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C273" t="s">
+    <row r="282" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C282" t="s">
         <v>317</v>
       </c>
-      <c r="E273" s="1" t="s">
+      <c r="E282" s="1" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="274" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C274" t="s">
+    <row r="283" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C283" t="s">
         <v>319</v>
       </c>
-      <c r="E274" s="1" t="s">
+      <c r="E283" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="275" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C275" t="s">
+    <row r="284" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C284" t="s">
         <v>326</v>
       </c>
-      <c r="D275" t="s">
+      <c r="D284" t="s">
         <v>333</v>
       </c>
-      <c r="E275" s="1" t="s">
+      <c r="E284" s="1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="276" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D276" t="s">
+    <row r="285" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D285" t="s">
         <v>328</v>
       </c>
-      <c r="E276" s="1" t="s">
+      <c r="E285" s="1" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="278" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C278" t="s">
+    <row r="287" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C287" t="s">
         <v>330</v>
       </c>
-      <c r="D278" t="s">
+      <c r="D287" t="s">
         <v>331</v>
       </c>
-      <c r="E278" s="1" t="s">
+      <c r="E287" s="1" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="280" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C280" t="s">
+    <row r="289" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C289" t="s">
         <v>336</v>
       </c>
-      <c r="D280" t="s">
+      <c r="D289" t="s">
         <v>338</v>
       </c>
-      <c r="E280" s="1" t="s">
+      <c r="E289" s="1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="284" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B284" t="s">
+    <row r="293" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B293" t="s">
         <v>339</v>
-      </c>
-    </row>
-    <row r="285" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C285" t="s">
-        <v>342</v>
-      </c>
-      <c r="D285" t="s">
-        <v>340</v>
-      </c>
-      <c r="E285" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="291" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B291" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="292" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C292" t="s">
-        <v>87</v>
-      </c>
-      <c r="D292" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="293" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C293" t="s">
-        <v>89</v>
-      </c>
-      <c r="D293" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="294" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C294" t="s">
-        <v>96</v>
-      </c>
-      <c r="D294" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="295" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C295" t="s">
-        <v>98</v>
-      </c>
-      <c r="D295" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="297" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B297" t="s">
-        <v>91</v>
-      </c>
-      <c r="C297" t="s">
-        <v>92</v>
-      </c>
-      <c r="D297" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="298" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C298" t="s">
-        <v>94</v>
-      </c>
-      <c r="D298" t="s">
-        <v>95</v>
+        <v>342</v>
+      </c>
+      <c r="D294" t="s">
+        <v>340</v>
+      </c>
+      <c r="E294" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="300" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B300" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="301" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B301" t="s">
-        <v>100</v>
+      <c r="C301" t="s">
+        <v>87</v>
+      </c>
+      <c r="D301" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="302" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C302" t="s">
+        <v>89</v>
+      </c>
+      <c r="D302" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="303" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C303" t="s">
+        <v>96</v>
+      </c>
+      <c r="D303" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="304" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C304" t="s">
+        <v>98</v>
+      </c>
+      <c r="D304" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="306" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B306" t="s">
+        <v>91</v>
+      </c>
+      <c r="C306" t="s">
+        <v>92</v>
+      </c>
+      <c r="D306" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="307" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C307" t="s">
+        <v>94</v>
+      </c>
+      <c r="D307" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="310" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B310" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="311" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C311" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="303" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D303" t="s">
+    <row r="312" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D312" t="s">
         <v>105</v>
       </c>
-      <c r="E303" s="1" t="s">
+      <c r="E312" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="304" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D304" t="s">
+    <row r="313" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D313" t="s">
         <v>102</v>
       </c>
-      <c r="E304" s="1" t="s">
+      <c r="E313" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="305" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D305" t="s">
+    <row r="314" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D314" t="s">
         <v>103</v>
       </c>
-      <c r="E305" s="1" t="s">
+      <c r="E314" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="306" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D306" t="s">
+    <row r="315" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D315" t="s">
         <v>108</v>
       </c>
-      <c r="E306" t="s">
+      <c r="E315" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="308" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B308" t="s">
+    <row r="317" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B317" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="309" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C309" t="s">
+    <row r="318" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C318" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="310" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D310" t="s">
+    <row r="319" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D319" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="311" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D311" t="s">
+    <row r="320" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D320" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="312" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F312" s="1" t="s">
+    <row r="321" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F321" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="313" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B313" t="s">
+    <row r="322" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B322" t="s">
         <v>1</v>
       </c>
-      <c r="F313" s="1" t="s">
+      <c r="F322" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="314" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C314" t="s">
+    <row r="323" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C323" t="s">
         <v>113</v>
       </c>
-      <c r="D314" s="1" t="s">
+      <c r="D323" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="315" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D315" t="s">
+    <row r="324" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D324" t="s">
         <v>127</v>
       </c>
-      <c r="E315" s="1" t="s">
+      <c r="E324" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="316" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C316" t="s">
+    <row r="325" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C325" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="317" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D317" t="s">
+    <row r="326" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D326" t="s">
         <v>116</v>
       </c>
-      <c r="E317" s="1" t="s">
+      <c r="E326" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F317" t="s">
+      <c r="F326" t="s">
         <v>129</v>
       </c>
-      <c r="G317" s="1" t="s">
+      <c r="G326" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="318" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E318" t="s">
+    <row r="327" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E327" t="s">
         <v>122</v>
       </c>
-      <c r="G318" s="1"/>
-    </row>
-    <row r="319" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E319" t="s">
+      <c r="G327" s="1"/>
+    </row>
+    <row r="328" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E328" t="s">
         <v>125</v>
       </c>
-      <c r="G319" s="1"/>
-    </row>
-    <row r="320" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D320" t="s">
+      <c r="G328" s="1"/>
+    </row>
+    <row r="329" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D329" t="s">
         <v>118</v>
       </c>
-      <c r="E320" s="1" t="s">
+      <c r="E329" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G320" s="1"/>
-    </row>
-    <row r="321" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D321" t="s">
+      <c r="G329" s="1"/>
+    </row>
+    <row r="330" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D330" t="s">
         <v>120</v>
       </c>
-      <c r="E321" s="1" t="s">
+      <c r="E330" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G321" s="1"/>
-    </row>
-    <row r="322" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E322" s="1" t="s">
+      <c r="G330" s="1"/>
+    </row>
+    <row r="331" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E331" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="G322" s="1"/>
-    </row>
-    <row r="323" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E323" t="s">
+      <c r="G331" s="1"/>
+    </row>
+    <row r="332" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E332" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="324" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D324" t="s">
+    <row r="333" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D333" t="s">
         <v>302</v>
       </c>
-      <c r="E324" s="1" t="s">
+      <c r="E333" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="325" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D325" t="s">
+    <row r="334" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D334" t="s">
         <v>301</v>
       </c>
-      <c r="E325" s="1" t="s">
+      <c r="E334" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="330" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C330" t="s">
+    <row r="339" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C339" t="s">
         <v>132</v>
       </c>
-      <c r="D330" s="1" t="s">
+      <c r="D339" s="1" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="343" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B343" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="344" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C344" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="345" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D345" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="346" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E346" t="s">
+        <v>494</v>
+      </c>
+      <c r="F346" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="347" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E347" t="s">
+        <v>496</v>
+      </c>
+      <c r="F347" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="348" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E348" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="349" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D349" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="350" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E350" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="351" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E351" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="352" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D352" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="353" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E353" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="354" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C354" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="355" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D355" t="s">
+        <v>505</v>
+      </c>
+      <c r="E355" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="356" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D356" t="s">
+        <v>503</v>
+      </c>
+      <c r="E356" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="358" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C358" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="359" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D359" t="s">
+        <v>510</v>
+      </c>
+      <c r="E359" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="360" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D360" t="s">
+        <v>511</v>
+      </c>
+      <c r="E360" t="s">
+        <v>509</v>
+      </c>
+      <c r="G360" s="1" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="362" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C362" t="s">
+        <v>514</v>
+      </c>
+      <c r="G362" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="364" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C364" t="s">
+        <v>515</v>
+      </c>
+      <c r="E364" t="s">
+        <v>516</v>
+      </c>
+      <c r="G364" s="1" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="366" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C366" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="367" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D367" t="s">
+        <v>520</v>
+      </c>
+      <c r="E367" t="s">
+        <v>519</v>
+      </c>
+      <c r="G367" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="368" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D368" t="s">
+        <v>521</v>
+      </c>
+      <c r="E368" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="370" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C370" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="371" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D371" t="s">
+        <v>530</v>
+      </c>
+      <c r="E371" t="s">
+        <v>526</v>
+      </c>
+      <c r="G371" s="1" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="372" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D372" t="s">
+        <v>528</v>
+      </c>
+      <c r="E372" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="373" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D373" t="s">
+        <v>529</v>
+      </c>
+      <c r="E373" t="s">
+        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -3884,65 +4264,65 @@
     <hyperlink ref="E212" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
     <hyperlink ref="F113" r:id="rId50" location="113521" xr:uid="{EE1413C5-3B38-7D4D-8DF1-634A12F0BD81}"/>
     <hyperlink ref="E71" r:id="rId51" xr:uid="{00B1EF4A-7791-0343-8D8C-9A1E83248FC9}"/>
-    <hyperlink ref="E264" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
-    <hyperlink ref="E265" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
+    <hyperlink ref="E273" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
+    <hyperlink ref="E274" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
     <hyperlink ref="F120" r:id="rId54" xr:uid="{40A4B6A0-2F7E-A84D-8CC6-D814A33F5953}"/>
     <hyperlink ref="E213" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
     <hyperlink ref="E214" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
     <hyperlink ref="E215" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
     <hyperlink ref="E216" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
-    <hyperlink ref="E266" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
+    <hyperlink ref="E275" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
     <hyperlink ref="D190" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
     <hyperlink ref="D191" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
     <hyperlink ref="D192" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
     <hyperlink ref="E217" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
-    <hyperlink ref="E267" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
-    <hyperlink ref="E268" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
-    <hyperlink ref="E270" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
-    <hyperlink ref="E271" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
-    <hyperlink ref="F265" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
-    <hyperlink ref="G265" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
-    <hyperlink ref="E272" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
-    <hyperlink ref="E273" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
-    <hyperlink ref="E274" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
+    <hyperlink ref="E276" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
+    <hyperlink ref="E277" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
+    <hyperlink ref="E279" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
+    <hyperlink ref="E280" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
+    <hyperlink ref="F274" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
+    <hyperlink ref="G274" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
+    <hyperlink ref="E281" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
+    <hyperlink ref="E282" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
+    <hyperlink ref="E283" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
     <hyperlink ref="E181" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
-    <hyperlink ref="E269" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
-    <hyperlink ref="E275" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
-    <hyperlink ref="E276" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
+    <hyperlink ref="E278" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
+    <hyperlink ref="E284" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
+    <hyperlink ref="E285" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
     <hyperlink ref="E73" r:id="rId77" location="code" xr:uid="{C0475FF8-517D-E949-887E-9A42D86E9640}"/>
-    <hyperlink ref="E278" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
+    <hyperlink ref="E287" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
     <hyperlink ref="E74" r:id="rId79" xr:uid="{277DBE6F-F3E5-8B4C-8DD8-BD92445D1A99}"/>
-    <hyperlink ref="E280" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
-    <hyperlink ref="E285" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
+    <hyperlink ref="E289" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
+    <hyperlink ref="E294" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
     <hyperlink ref="E196" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
     <hyperlink ref="E197" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
     <hyperlink ref="F141" r:id="rId84" xr:uid="{EB604865-A16B-0646-A5B5-0D047467449D}"/>
     <hyperlink ref="E219" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
-    <hyperlink ref="D294" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
-    <hyperlink ref="D295" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
-    <hyperlink ref="E304" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
-    <hyperlink ref="E305" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
-    <hyperlink ref="E303" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
-    <hyperlink ref="D314" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
-    <hyperlink ref="E320" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
-    <hyperlink ref="E317" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
-    <hyperlink ref="E321" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
-    <hyperlink ref="F312" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
-    <hyperlink ref="F313" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
-    <hyperlink ref="E315" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
-    <hyperlink ref="G317" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
-    <hyperlink ref="D330" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
-    <hyperlink ref="E322" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
-    <hyperlink ref="E325" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
-    <hyperlink ref="E324" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
-    <hyperlink ref="F229" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
-    <hyperlink ref="E230" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
-    <hyperlink ref="E231" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
-    <hyperlink ref="E232" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
-    <hyperlink ref="G246" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
-    <hyperlink ref="E241" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
-    <hyperlink ref="E242" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
-    <hyperlink ref="E247" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
+    <hyperlink ref="D303" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
+    <hyperlink ref="D304" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
+    <hyperlink ref="E313" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
+    <hyperlink ref="E314" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
+    <hyperlink ref="E312" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
+    <hyperlink ref="D323" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
+    <hyperlink ref="E329" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
+    <hyperlink ref="E326" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
+    <hyperlink ref="E330" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
+    <hyperlink ref="F321" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
+    <hyperlink ref="F322" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
+    <hyperlink ref="E324" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
+    <hyperlink ref="G326" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
+    <hyperlink ref="D339" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
+    <hyperlink ref="E331" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
+    <hyperlink ref="E334" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
+    <hyperlink ref="E333" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
+    <hyperlink ref="F238" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
+    <hyperlink ref="E239" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
+    <hyperlink ref="E240" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
+    <hyperlink ref="E241" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
+    <hyperlink ref="G255" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
+    <hyperlink ref="E250" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
+    <hyperlink ref="E251" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
+    <hyperlink ref="E256" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
     <hyperlink ref="F148" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
     <hyperlink ref="F153" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
     <hyperlink ref="F154" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
@@ -3952,6 +4332,14 @@
     <hyperlink ref="F167" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
     <hyperlink ref="F161" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
     <hyperlink ref="F170" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
+    <hyperlink ref="H234" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
+    <hyperlink ref="F346" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
+    <hyperlink ref="G360" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
+    <hyperlink ref="F347" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
+    <hyperlink ref="G362" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
+    <hyperlink ref="G364" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
+    <hyperlink ref="G367" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
+    <hyperlink ref="G371" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3959,10 +4347,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G24"/>
+  <dimension ref="B2:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4232,6 +4620,17 @@
       </c>
       <c r="E24" t="s">
         <v>480</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C25" t="s">
+        <v>483</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>482</v>
       </c>
     </row>
   </sheetData>
@@ -4259,6 +4658,8 @@
     <hyperlink ref="G21" r:id="rId21" xr:uid="{DBFCC3ED-E1BC-1D4B-864D-767A27A012CB}"/>
     <hyperlink ref="F22" r:id="rId22" xr:uid="{B2FC5726-790C-6D4F-AFBE-486B456C2104}"/>
     <hyperlink ref="F23" r:id="rId23" xr:uid="{3BA61085-9387-0646-AC67-98A9E3A8AD5C}"/>
+    <hyperlink ref="B25" r:id="rId24" xr:uid="{3E826681-457D-1A40-AC0B-12F435FE47ED}"/>
+    <hyperlink ref="F25" r:id="rId25" xr:uid="{E62BCFDF-C9A7-0D42-B80E-EEE34097BDCF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added more information about python, pandas resample, timescaledb python server.
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79B8D79-2007-D64F-A9F2-341D801BF379}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44996FF8-807E-F242-A21B-6B44AC0F75EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="2120" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="2120" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="540">
   <si>
     <t>docker</t>
   </si>
@@ -1634,6 +1634,30 @@
   </si>
   <si>
     <t>https://docs.timescale.com/latest/getting-started/setup</t>
+  </si>
+  <si>
+    <t>Storing Realtime IoT Timeseries Data in Python — Timescale DB + Raspberry Pi + Phidget Sensors</t>
+  </si>
+  <si>
+    <t>Managing Tables with TimescaleDB</t>
+  </si>
+  <si>
+    <t>Python Server to Store IoT Timeseries Data</t>
+  </si>
+  <si>
+    <t>Django</t>
+  </si>
+  <si>
+    <t>https://medium.com/smart-digital-garden/timescaledb-and-django-5f2640b28ef1</t>
+  </si>
+  <si>
+    <t>TimescaleDB and Django</t>
+  </si>
+  <si>
+    <t>resample</t>
+  </si>
+  <si>
+    <t>Using the Pandas “Resample” Function</t>
   </si>
 </sst>
 </file>
@@ -2080,8 +2104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
   <dimension ref="B3:I373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A347" workbookViewId="0">
-      <selection activeCell="D370" sqref="D370"/>
+    <sheetView topLeftCell="A347" workbookViewId="0">
+      <selection activeCell="D365" sqref="D365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4347,10 +4371,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G25"/>
+  <dimension ref="B2:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4623,14 +4647,50 @@
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>482</v>
+      <c r="B25" t="s">
+        <v>533</v>
       </c>
       <c r="C25" t="s">
         <v>483</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>482</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>532</v>
+      </c>
+      <c r="E26" t="s">
+        <v>534</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>537</v>
+      </c>
+      <c r="C27" t="s">
+        <v>535</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>539</v>
+      </c>
+      <c r="C28" t="s">
+        <v>448</v>
+      </c>
+      <c r="E28" t="s">
+        <v>538</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -4658,8 +4718,11 @@
     <hyperlink ref="G21" r:id="rId21" xr:uid="{DBFCC3ED-E1BC-1D4B-864D-767A27A012CB}"/>
     <hyperlink ref="F22" r:id="rId22" xr:uid="{B2FC5726-790C-6D4F-AFBE-486B456C2104}"/>
     <hyperlink ref="F23" r:id="rId23" xr:uid="{3BA61085-9387-0646-AC67-98A9E3A8AD5C}"/>
-    <hyperlink ref="B25" r:id="rId24" xr:uid="{3E826681-457D-1A40-AC0B-12F435FE47ED}"/>
+    <hyperlink ref="B25" r:id="rId24" display="https://kb.objectrocket.com/timescaledb/managing-tables-with-timescaledb-1601-z" xr:uid="{3E826681-457D-1A40-AC0B-12F435FE47ED}"/>
     <hyperlink ref="F25" r:id="rId25" xr:uid="{E62BCFDF-C9A7-0D42-B80E-EEE34097BDCF}"/>
+    <hyperlink ref="F26" r:id="rId26" xr:uid="{3B04ECD2-7215-E44A-B2BA-78117512C321}"/>
+    <hyperlink ref="F27" r:id="rId27" xr:uid="{72C1FF05-0698-1044-AD35-779549D5FEE1}"/>
+    <hyperlink ref="F28" r:id="rId28" xr:uid="{FD52415E-DA54-844A-937E-E667C2082DAB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated with vimrc setup, link to awesome version.
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44996FF8-807E-F242-A21B-6B44AC0F75EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9CBD4E-FD09-A74A-B2DF-44F88647EFC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="2120" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="568">
   <si>
     <t>docker</t>
   </si>
@@ -1658,13 +1658,97 @@
   </si>
   <si>
     <t>Using the Pandas “Resample” Function</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Vim</t>
+  </si>
+  <si>
+    <t>Configuration file location</t>
+  </si>
+  <si>
+    <t>You usually create it as  ~/.vimrc</t>
+  </si>
+  <si>
+    <t>Color Syntax on</t>
+  </si>
+  <si>
+    <t>append code in .vimrc file</t>
+  </si>
+  <si>
+    <t>syntax on</t>
+  </si>
+  <si>
+    <t>https://www.cyberciti.biz/faq/turn-on-or-off-color-syntax-highlighting-in-vi-or-vim/</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/10921441/where-is-my-vimrc-file</t>
+  </si>
+  <si>
+    <t>Configure the tab and indent as 4 spaces</t>
+  </si>
+  <si>
+    <t>1. Set the width of TAB as 4 spaces</t>
+  </si>
+  <si>
+    <t>set tabstop=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Set the indent width as 4 spaces </t>
+  </si>
+  <si>
+    <t>set shiftwidth=4</t>
+  </si>
+  <si>
+    <t>3. Set the number of columns for a TAB</t>
+  </si>
+  <si>
+    <t>set softtabstop=4</t>
+  </si>
+  <si>
+    <t>4. Expand TABs to spaces</t>
+  </si>
+  <si>
+    <t>set expandtab</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/1878974/redefine-tab-as-4-spaces/1878983</t>
+  </si>
+  <si>
+    <t>Install awesome vimrc</t>
+  </si>
+  <si>
+    <t>1. Get source files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Run the installation </t>
+  </si>
+  <si>
+    <t>git clone --depth=1 https://github.com/amix/vimrc.git ~/.vim_runtime</t>
+  </si>
+  <si>
+    <t>sh ~/.vim_runtime/install_awesome_vimrc.sh</t>
+  </si>
+  <si>
+    <t>https://github.com/amix/vimrc</t>
+  </si>
+  <si>
+    <t>Cheat Sheets</t>
+  </si>
+  <si>
+    <t>https://www.cs.cmu.edu/~15131/f17/topics/vim/vim-cheatsheet.pdf</t>
+  </si>
+  <si>
+    <t>1. from CMU, Allison McKnight</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1687,13 +1771,26 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1709,7 +1806,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1719,6 +1816,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2102,10 +2203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B3:I373"/>
+  <dimension ref="B1:I393"/>
   <sheetViews>
-    <sheetView topLeftCell="A347" workbookViewId="0">
-      <selection activeCell="D365" sqref="D365"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A368" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D378" sqref="D378"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2116,752 +2218,760 @@
     <col min="5" max="5" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+    <row r="1" spans="2:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C4" t="s">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D6" t="s">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D7" t="s">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D9" t="s">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
         <v>4</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D10" t="s">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
         <v>11</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D11" t="s">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
         <v>8</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D15" t="s">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D21">
         <v>2</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D22">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D23">
         <v>1</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>22</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D26">
         <v>1</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C26" t="s">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D27">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D28">
         <v>1</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C30" t="s">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C33" t="s">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C36" t="s">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D37" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E39" t="s">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C40" t="s">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D41" t="s">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E42" t="s">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E43" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C43" t="s">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D44" t="s">
-        <v>36</v>
-      </c>
-      <c r="E44" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D45" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
         <v>30</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C47" t="s">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D48" t="s">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E49" t="s">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E50" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C52" t="s">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D53" t="s">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
         <v>48</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C54" t="s">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D55" t="s">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
         <v>51</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E56" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D56" t="s">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C57" t="s">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C58" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D58" t="s">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
         <v>54</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C60" t="s">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C61" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D61" t="s">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
         <v>58</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E62" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E62" s="1"/>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C63" t="s">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C64" t="s">
         <v>199</v>
       </c>
-      <c r="E63" s="1"/>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D64" t="s">
+      <c r="E64" s="1"/>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D65" t="s">
         <v>204</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E65" t="s">
         <v>54</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F65" t="s">
         <v>201</v>
       </c>
-      <c r="G64" s="1" t="s">
+      <c r="G65" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D65" t="s">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
         <v>205</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E66" t="s">
         <v>202</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F66" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E66" s="1"/>
-    </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C68" t="s">
+    <row r="68" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E68" s="1"/>
+    </row>
+    <row r="69" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C69" t="s">
         <v>193</v>
       </c>
-      <c r="E68" s="1"/>
-    </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D69" t="s">
+      <c r="E69" s="1"/>
+    </row>
+    <row r="70" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
         <v>194</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E70" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E70" s="1" t="s">
+    <row r="71" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E71" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E71" s="1" t="s">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E72" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E72" s="1"/>
-    </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D73" t="s">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E73" s="1"/>
+    </row>
+    <row r="74" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D74" t="s">
         <v>329</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E74" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D74" s="3" t="s">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D75" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="E75" s="1" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E75" s="1"/>
-    </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B85" t="s">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E76" s="1"/>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B86" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C86" t="s">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C87" t="s">
         <v>157</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="D87" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C87" t="s">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C88" t="s">
         <v>159</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="D88" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C88" t="s">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C89" t="s">
         <v>160</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D89" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C89" t="s">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
         <v>219</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D90" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="E90" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C91" t="s">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C92" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D92" t="s">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D93" t="s">
         <v>164</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E93" t="s">
         <v>163</v>
       </c>
-      <c r="F92" s="1" t="s">
+      <c r="F93" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="E93" t="s">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E94" t="s">
         <v>275</v>
       </c>
-      <c r="F93" s="1"/>
-    </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D94" t="s">
+      <c r="F94" s="1"/>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D95" t="s">
         <v>166</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E95" t="s">
         <v>167</v>
       </c>
-      <c r="F94" s="1" t="s">
+      <c r="F95" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D95" t="s">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D96" t="s">
         <v>180</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E96" t="s">
         <v>181</v>
       </c>
-      <c r="F95" s="1" t="s">
+      <c r="F96" s="1" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D96" t="s">
-        <v>190</v>
-      </c>
-      <c r="E96" t="s">
-        <v>192</v>
-      </c>
-      <c r="F96" t="s">
-        <v>196</v>
-      </c>
-      <c r="G96" t="s">
-        <v>191</v>
-      </c>
-      <c r="H96" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="I96" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="97" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D97" t="s">
-        <v>232</v>
+        <v>190</v>
       </c>
       <c r="E97" t="s">
-        <v>234</v>
+        <v>192</v>
+      </c>
+      <c r="F97" t="s">
+        <v>196</v>
+      </c>
+      <c r="G97" t="s">
+        <v>191</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>197</v>
       </c>
+      <c r="I97" s="1" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="98" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D98" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E98" t="s">
-        <v>235</v>
-      </c>
-      <c r="H98" s="1"/>
+        <v>234</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="99" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D99" t="s">
-        <v>206</v>
+        <v>233</v>
       </c>
       <c r="E99" t="s">
-        <v>207</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>208</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="H99" s="1"/>
     </row>
     <row r="100" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D100" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E100" t="s">
-        <v>210</v>
-      </c>
-      <c r="F100" t="s">
-        <v>211</v>
-      </c>
-      <c r="G100" t="s">
-        <v>214</v>
-      </c>
-      <c r="H100" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="I100" s="1" t="s">
-        <v>213</v>
+        <v>207</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="101" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D101" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="E101" t="s">
-        <v>221</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>222</v>
+        <v>210</v>
+      </c>
+      <c r="F101" t="s">
+        <v>211</v>
+      </c>
+      <c r="G101" t="s">
+        <v>214</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="102" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D102" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E102" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="103" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D103" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E103" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="104" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D104" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E104" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="105" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D105" t="s">
+        <v>229</v>
+      </c>
+      <c r="E105" t="s">
+        <v>230</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="106" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D106" t="s">
         <v>236</v>
       </c>
-      <c r="E105" t="s">
+      <c r="E106" t="s">
         <v>237</v>
       </c>
-      <c r="F105" s="1" t="s">
+      <c r="F106" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="106" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E106" t="s">
+    <row r="107" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E107" t="s">
         <v>238</v>
-      </c>
-      <c r="F106" s="1"/>
-    </row>
-    <row r="107" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D107" t="s">
-        <v>240</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="F107" s="1"/>
     </row>
     <row r="108" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D108" t="s">
-        <v>247</v>
-      </c>
-      <c r="E108" t="s">
-        <v>246</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>245</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F108" s="1"/>
     </row>
     <row r="109" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D109" t="s">
-        <v>248</v>
+        <v>247</v>
+      </c>
+      <c r="E109" t="s">
+        <v>246</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="110" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D110" t="s">
-        <v>250</v>
-      </c>
-      <c r="E110" t="s">
-        <v>207</v>
+        <v>248</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="111" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D111" t="s">
-        <v>252</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
+      </c>
+      <c r="E111" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="112" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D112" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D113" t="s">
-        <v>273</v>
+        <v>254</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D114" t="s">
-        <v>255</v>
-      </c>
-      <c r="E114" t="s">
-        <v>256</v>
+        <v>273</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>257</v>
+        <v>274</v>
       </c>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D115" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E115" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D116" t="s">
-        <v>262</v>
+        <v>258</v>
+      </c>
+      <c r="E116" t="s">
+        <v>259</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D117" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D118" t="s">
+        <v>264</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="119" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D119" t="s">
         <v>266</v>
       </c>
-      <c r="E118" t="s">
+      <c r="E119" t="s">
         <v>265</v>
       </c>
-      <c r="F118" s="1" t="s">
+      <c r="F119" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E119" t="s">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E120" t="s">
         <v>268</v>
       </c>
-      <c r="F119" s="1"/>
-    </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D120" t="s">
+      <c r="F120" s="1"/>
+    </row>
+    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D121" t="s">
         <v>283</v>
       </c>
-      <c r="F120" s="1" t="s">
+      <c r="F121" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F121" s="1"/>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F122" s="1"/>
@@ -2876,441 +2986,441 @@
       <c r="F125" s="1"/>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B126" t="s">
+      <c r="F126" s="1"/>
+    </row>
+    <row r="127" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B127" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C127" t="s">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C128" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D128" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="129" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D129" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="130" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D130" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="131" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C131" t="s">
+    <row r="132" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C132" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="132" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D132" s="1" t="s">
+    <row r="133" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D133" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="134" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C134" t="s">
+    <row r="135" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C135" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="135" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D135" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="136" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D136" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="137" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D137" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="138" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D138" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="139" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D139" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="140" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C140" t="s">
+    <row r="141" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C141" t="s">
         <v>347</v>
-      </c>
-    </row>
-    <row r="141" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D141" t="s">
-        <v>350</v>
-      </c>
-      <c r="E141" t="s">
-        <v>348</v>
-      </c>
-      <c r="F141" s="1" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="142" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D142" t="s">
+        <v>350</v>
+      </c>
+      <c r="E142" t="s">
+        <v>348</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="143" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D143" t="s">
         <v>351</v>
       </c>
-      <c r="E142" t="s">
+      <c r="E143" t="s">
         <v>352</v>
       </c>
-      <c r="F142" t="s">
+      <c r="F143" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="144" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C144" t="s">
+    <row r="145" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C145" t="s">
         <v>358</v>
-      </c>
-    </row>
-    <row r="145" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D145" t="s">
-        <v>355</v>
-      </c>
-      <c r="E145" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="146" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D146" t="s">
+        <v>355</v>
+      </c>
+      <c r="E146" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="147" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D147" t="s">
         <v>356</v>
       </c>
-      <c r="E146" t="s">
+      <c r="E147" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="148" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C148" t="s">
+    <row r="149" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C149" t="s">
         <v>370</v>
       </c>
-      <c r="F148" s="1" t="s">
+      <c r="F149" s="1" t="s">
         <v>379</v>
-      </c>
-    </row>
-    <row r="149" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D149" t="s">
-        <v>371</v>
-      </c>
-      <c r="E149" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="150" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D150" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E150" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="151" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D151" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E151" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="152" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D152" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E152" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="153" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D153" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="E153" t="s">
-        <v>388</v>
-      </c>
-      <c r="F153" s="1" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
     </row>
     <row r="154" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D154" t="s">
+        <v>387</v>
+      </c>
+      <c r="E154" t="s">
+        <v>388</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="155" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D155" t="s">
         <v>390</v>
       </c>
-      <c r="E154" t="s">
+      <c r="E155" t="s">
         <v>391</v>
       </c>
-      <c r="F154" s="1" t="s">
+      <c r="F155" s="1" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="156" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C156" t="s">
+    <row r="157" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C157" t="s">
         <v>380</v>
-      </c>
-    </row>
-    <row r="157" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D157" t="s">
-        <v>381</v>
-      </c>
-      <c r="E157" t="s">
-        <v>382</v>
-      </c>
-      <c r="F157" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="158" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D158" t="s">
+        <v>381</v>
+      </c>
+      <c r="E158" t="s">
+        <v>382</v>
+      </c>
+      <c r="F158" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="159" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D159" t="s">
         <v>383</v>
       </c>
-      <c r="E158" t="s">
+      <c r="E159" t="s">
         <v>384</v>
       </c>
-      <c r="F158" t="s">
+      <c r="F159" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="159" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="F159" s="1"/>
-    </row>
     <row r="160" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C160" t="s">
+      <c r="F160" s="1"/>
+    </row>
+    <row r="161" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C161" t="s">
         <v>393</v>
       </c>
-      <c r="D160" t="s">
+      <c r="D161" t="s">
         <v>421</v>
       </c>
-      <c r="E160" t="s">
+      <c r="E161" t="s">
         <v>394</v>
       </c>
-      <c r="F160" s="1" t="s">
+      <c r="F161" s="1" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="161" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D161" t="s">
-        <v>422</v>
-      </c>
-      <c r="E161" t="s">
-        <v>423</v>
-      </c>
-      <c r="F161" s="1" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="162" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D162" t="s">
+        <v>422</v>
+      </c>
+      <c r="E162" t="s">
+        <v>423</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="163" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D163" t="s">
         <v>425</v>
       </c>
-      <c r="E162" t="s">
+      <c r="E163" t="s">
         <v>426</v>
       </c>
-      <c r="F162" s="1"/>
-    </row>
-    <row r="163" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C163" t="s">
+      <c r="F163" s="1"/>
+    </row>
+    <row r="164" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C164" t="s">
         <v>395</v>
-      </c>
-      <c r="F163" s="1"/>
-    </row>
-    <row r="164" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D164" t="s">
-        <v>397</v>
-      </c>
-      <c r="E164" t="s">
-        <v>396</v>
       </c>
       <c r="F164" s="1"/>
     </row>
     <row r="165" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D165" t="s">
+        <v>397</v>
+      </c>
+      <c r="E165" t="s">
+        <v>396</v>
+      </c>
+      <c r="F165" s="1"/>
+    </row>
+    <row r="166" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D166" t="s">
         <v>398</v>
       </c>
-      <c r="F165" t="s">
+      <c r="F166" t="s">
         <v>399</v>
       </c>
-      <c r="G165" s="1" t="s">
+      <c r="G166" s="1" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="166" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C166" t="s">
+    <row r="167" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C167" t="s">
         <v>417</v>
-      </c>
-      <c r="G166" s="1"/>
-    </row>
-    <row r="167" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E167" t="s">
-        <v>418</v>
-      </c>
-      <c r="F167" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="G167" s="1"/>
     </row>
     <row r="168" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E168" t="s">
+        <v>418</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="G168" s="1"/>
+    </row>
+    <row r="169" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E169" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="169" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C169" t="s">
+    <row r="170" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C170" t="s">
         <v>432</v>
-      </c>
-    </row>
-    <row r="170" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D170" t="s">
-        <v>433</v>
-      </c>
-      <c r="E170" t="s">
-        <v>435</v>
-      </c>
-      <c r="F170" s="1" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="171" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D171" t="s">
+        <v>433</v>
+      </c>
+      <c r="E171" t="s">
+        <v>435</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="172" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D172" t="s">
         <v>434</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E172" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B177" t="s">
+    <row r="178" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B178" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C178" t="s">
+    <row r="179" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C179" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D179" t="s">
-        <v>171</v>
-      </c>
-      <c r="E179" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="180" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D180" t="s">
+        <v>171</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="181" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D181" t="s">
         <v>175</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E181" t="s">
         <v>173</v>
       </c>
-      <c r="F180" s="1" t="s">
+      <c r="F181" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="181" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C181" t="s">
-        <v>322</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="F181" s="1"/>
     </row>
     <row r="182" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C182" t="s">
+        <v>322</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F182" s="1"/>
+    </row>
+    <row r="183" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C183" t="s">
         <v>406</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D183" t="s">
         <v>407</v>
       </c>
-      <c r="E182" s="1" t="s">
+      <c r="E183" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="F182" s="1"/>
-    </row>
-    <row r="183" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D183" t="s">
+      <c r="F183" s="1"/>
+    </row>
+    <row r="184" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D184" t="s">
         <v>408</v>
       </c>
-      <c r="F183" s="1"/>
-    </row>
-    <row r="184" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F184" s="1"/>
     </row>
-    <row r="187" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B187" t="s">
+    <row r="185" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F185" s="1"/>
+    </row>
+    <row r="188" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B188" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="188" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C188" t="s">
-        <v>176</v>
-      </c>
-      <c r="D188" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="189" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C189" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="190" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C190" t="s">
-        <v>293</v>
+        <v>178</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>292</v>
+        <v>179</v>
       </c>
     </row>
     <row r="191" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C191" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="192" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C192" t="s">
+        <v>294</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="193" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C193" t="s">
         <v>297</v>
       </c>
-      <c r="D192" s="1" t="s">
+      <c r="D193" s="1" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="193" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D193" s="1"/>
     </row>
     <row r="194" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D194" s="1"/>
     </row>
     <row r="195" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B195" t="s">
+      <c r="D195" s="1"/>
+    </row>
+    <row r="196" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B196" t="s">
         <v>343</v>
       </c>
-      <c r="D195" s="1"/>
-    </row>
-    <row r="196" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C196" t="s">
+      <c r="D196" s="1"/>
+    </row>
+    <row r="197" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C197" t="s">
         <v>344</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D197" t="s">
         <v>369</v>
       </c>
-      <c r="E196" s="1" t="s">
+      <c r="E197" s="1" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="197" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D197" t="s">
+    <row r="198" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D198" t="s">
         <v>368</v>
       </c>
-      <c r="E197" s="1" t="s">
+      <c r="E198" s="1" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="198" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D198" s="1"/>
     </row>
     <row r="199" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D199" s="1"/>
@@ -3318,115 +3428,115 @@
     <row r="200" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D200" s="1"/>
     </row>
-    <row r="204" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B204" t="s">
+    <row r="201" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D201" s="1"/>
+    </row>
+    <row r="205" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B205" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="205" spans="2:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="C205" s="4" t="s">
+    <row r="206" spans="2:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="C206" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D205" s="2" t="s">
+      <c r="D206" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E205" s="1" t="s">
+      <c r="E206" s="1" t="s">
         <v>186</v>
-      </c>
-    </row>
-    <row r="206" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C206" t="s">
-        <v>187</v>
-      </c>
-      <c r="E206" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="207" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C207" t="s">
+        <v>187</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="208" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C208" t="s">
         <v>215</v>
       </c>
-      <c r="E207" s="1" t="s">
+      <c r="E208" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="209" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D209" t="s">
+    <row r="210" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D210" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="211" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C211" t="s">
-        <v>242</v>
-      </c>
-      <c r="D211" t="s">
-        <v>243</v>
-      </c>
-      <c r="E211" s="1" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="212" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C212" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="D212" t="s">
-        <v>270</v>
+        <v>243</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>271</v>
+        <v>244</v>
       </c>
     </row>
     <row r="213" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C213" t="s">
+        <v>269</v>
+      </c>
+      <c r="D213" t="s">
+        <v>270</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="214" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C214" t="s">
         <v>284</v>
       </c>
-      <c r="E213" s="1" t="s">
+      <c r="E214" s="1" t="s">
         <v>285</v>
-      </c>
-    </row>
-    <row r="214" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E214" s="1" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="215" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E215" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="216" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E216" s="1" t="s">
         <v>287</v>
-      </c>
-    </row>
-    <row r="216" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C216" t="s">
-        <v>288</v>
-      </c>
-      <c r="E216" s="1" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="217" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C217" t="s">
+        <v>288</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="218" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C218" t="s">
         <v>299</v>
       </c>
-      <c r="E217" s="1" t="s">
+      <c r="E218" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="218" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E218" s="1"/>
-    </row>
     <row r="219" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C219" t="s">
+      <c r="E219" s="1"/>
+    </row>
+    <row r="220" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C220" t="s">
         <v>359</v>
       </c>
-      <c r="D219" t="s">
+      <c r="D220" t="s">
         <v>360</v>
       </c>
-      <c r="E219" s="1" t="s">
+      <c r="E220" s="1" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="220" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E220" s="1"/>
     </row>
     <row r="221" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E221" s="1"/>
@@ -3450,920 +3560,1039 @@
       <c r="E227" s="1"/>
     </row>
     <row r="228" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C228" t="s">
+      <c r="E228" s="1"/>
+    </row>
+    <row r="229" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C229" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="229" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D229" t="s">
-        <v>135</v>
-      </c>
-      <c r="E229" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="230" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D230" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E230" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="231" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D231" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E231" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="232" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D232" t="s">
-        <v>137</v>
+        <v>140</v>
+      </c>
+      <c r="E232" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="233" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D233" t="s">
-        <v>142</v>
-      </c>
-      <c r="E233" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="234" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D234" t="s">
-        <v>484</v>
+        <v>142</v>
       </c>
       <c r="E234" t="s">
-        <v>486</v>
-      </c>
-      <c r="F234" t="s">
-        <v>490</v>
-      </c>
-      <c r="G234" t="s">
-        <v>485</v>
-      </c>
-      <c r="H234" s="1" t="s">
-        <v>491</v>
+        <v>143</v>
       </c>
     </row>
     <row r="235" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D235" t="s">
+        <v>484</v>
+      </c>
+      <c r="E235" t="s">
+        <v>486</v>
+      </c>
+      <c r="F235" t="s">
+        <v>490</v>
+      </c>
+      <c r="G235" t="s">
+        <v>485</v>
+      </c>
+      <c r="H235" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="236" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D236" t="s">
         <v>487</v>
       </c>
-      <c r="E235" t="s">
+      <c r="E236" t="s">
         <v>488</v>
       </c>
-      <c r="G235" t="s">
+      <c r="G236" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="237" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C237" t="s">
+    <row r="238" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C238" t="s">
         <v>367</v>
-      </c>
-    </row>
-    <row r="238" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D238" t="s">
-        <v>73</v>
-      </c>
-      <c r="E238" t="s">
-        <v>74</v>
-      </c>
-      <c r="F238" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="239" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D239" t="s">
-        <v>76</v>
-      </c>
-      <c r="E239" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
+      </c>
+      <c r="E239" t="s">
+        <v>74</v>
+      </c>
+      <c r="F239" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="240" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D240" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="241" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D241" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E241" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="242" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D242" t="s">
-        <v>362</v>
-      </c>
-      <c r="E242" t="s">
-        <v>365</v>
+        <v>81</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="243" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D243" t="s">
+        <v>362</v>
+      </c>
+      <c r="E243" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="244" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D244" t="s">
         <v>363</v>
       </c>
-      <c r="E243" t="s">
+      <c r="E244" t="s">
         <v>364</v>
-      </c>
-    </row>
-    <row r="245" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D245" t="s">
-        <v>82</v>
-      </c>
-      <c r="E245" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="246" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D246" t="s">
+        <v>82</v>
+      </c>
+      <c r="E246" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="247" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D247" t="s">
         <v>84</v>
       </c>
-      <c r="E246" t="s">
+      <c r="E247" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="248" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C248" t="s">
+    <row r="249" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C249" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="249" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D249" t="s">
-        <v>73</v>
-      </c>
-      <c r="E249" t="s">
-        <v>131</v>
-      </c>
-      <c r="F249" s="1"/>
     </row>
     <row r="250" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D250" t="s">
-        <v>147</v>
-      </c>
-      <c r="E250" s="1" t="s">
-        <v>148</v>
+        <v>73</v>
+      </c>
+      <c r="E250" t="s">
+        <v>131</v>
       </c>
       <c r="F250" s="1"/>
     </row>
     <row r="251" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D251" t="s">
+        <v>147</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F251" s="1"/>
+    </row>
+    <row r="252" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D252" t="s">
         <v>76</v>
       </c>
-      <c r="E251" s="1" t="s">
+      <c r="E252" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="252" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E252" s="1"/>
-    </row>
     <row r="253" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D253" t="s">
+      <c r="E253" s="1"/>
+    </row>
+    <row r="254" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D254" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="254" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E254" t="s">
-        <v>151</v>
-      </c>
-      <c r="F254" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="255" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E255" t="s">
+        <v>151</v>
+      </c>
+      <c r="F255" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="256" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E256" t="s">
         <v>152</v>
       </c>
-      <c r="F255" t="s">
+      <c r="F256" t="s">
         <v>145</v>
       </c>
-      <c r="G255" s="1" t="s">
+      <c r="G256" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="256" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D256" t="s">
+    <row r="257" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D257" t="s">
         <v>153</v>
       </c>
-      <c r="E256" s="1" t="s">
+      <c r="E257" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G256" s="1"/>
-    </row>
-    <row r="270" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E270" s="1"/>
-    </row>
-    <row r="272" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B272" t="s">
+      <c r="G257" s="1"/>
+    </row>
+    <row r="271" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E271" s="1"/>
+    </row>
+    <row r="273" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B273" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="273" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C273" t="s">
+    <row r="274" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C274" t="s">
         <v>277</v>
       </c>
-      <c r="D273" t="s">
+      <c r="D274" t="s">
         <v>279</v>
       </c>
-      <c r="E273" s="1" t="s">
+      <c r="E274" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="274" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C274" t="s">
+    <row r="275" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C275" t="s">
         <v>281</v>
       </c>
-      <c r="E274" s="1" t="s">
+      <c r="E275" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="F274" s="1" t="s">
+      <c r="F275" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="G274" s="1" t="s">
+      <c r="G275" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="275" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C275" t="s">
+    <row r="276" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C276" t="s">
         <v>290</v>
       </c>
-      <c r="E275" s="1" t="s">
+      <c r="E276" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="276" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C276" t="s">
+    <row r="277" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C277" t="s">
         <v>304</v>
       </c>
-      <c r="E276" s="1" t="s">
+      <c r="E277" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="277" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D277" t="s">
+    <row r="278" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D278" t="s">
         <v>306</v>
       </c>
-      <c r="E277" s="1" t="s">
+      <c r="E278" s="1" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="278" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C278" t="s">
+    <row r="279" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C279" t="s">
         <v>324</v>
       </c>
-      <c r="E278" s="1" t="s">
+      <c r="E279" s="1" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="279" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C279" t="s">
+    <row r="280" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C280" t="s">
         <v>308</v>
       </c>
-      <c r="D279" t="s">
+      <c r="D280" t="s">
         <v>309</v>
       </c>
-      <c r="E279" s="1" t="s">
+      <c r="E280" s="1" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="280" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C280" t="s">
+    <row r="281" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C281" t="s">
         <v>311</v>
       </c>
-      <c r="E280" s="1" t="s">
+      <c r="E281" s="1" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="281" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C281" t="s">
+    <row r="282" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C282" t="s">
         <v>316</v>
       </c>
-      <c r="E281" s="1" t="s">
+      <c r="E282" s="1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="282" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C282" t="s">
+    <row r="283" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C283" t="s">
         <v>317</v>
       </c>
-      <c r="E282" s="1" t="s">
+      <c r="E283" s="1" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="283" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C283" t="s">
+    <row r="284" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C284" t="s">
         <v>319</v>
       </c>
-      <c r="E283" s="1" t="s">
+      <c r="E284" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="284" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C284" t="s">
+    <row r="285" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C285" t="s">
         <v>326</v>
       </c>
-      <c r="D284" t="s">
+      <c r="D285" t="s">
         <v>333</v>
       </c>
-      <c r="E284" s="1" t="s">
+      <c r="E285" s="1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="285" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D285" t="s">
+    <row r="286" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D286" t="s">
         <v>328</v>
       </c>
-      <c r="E285" s="1" t="s">
+      <c r="E286" s="1" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="287" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C287" t="s">
+    <row r="288" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C288" t="s">
         <v>330</v>
       </c>
-      <c r="D287" t="s">
+      <c r="D288" t="s">
         <v>331</v>
       </c>
-      <c r="E287" s="1" t="s">
+      <c r="E288" s="1" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="289" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C289" t="s">
+    <row r="290" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C290" t="s">
         <v>336</v>
       </c>
-      <c r="D289" t="s">
+      <c r="D290" t="s">
         <v>338</v>
       </c>
-      <c r="E289" s="1" t="s">
+      <c r="E290" s="1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="293" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B293" t="s">
+    <row r="294" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B294" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="294" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C294" t="s">
+    <row r="295" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C295" t="s">
         <v>342</v>
       </c>
-      <c r="D294" t="s">
+      <c r="D295" t="s">
         <v>340</v>
       </c>
-      <c r="E294" s="1" t="s">
+      <c r="E295" s="1" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="300" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B300" t="s">
+    <row r="301" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B301" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="301" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C301" t="s">
-        <v>87</v>
-      </c>
-      <c r="D301" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="302" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C302" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D302" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="303" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C303" t="s">
-        <v>96</v>
-      </c>
-      <c r="D303" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
+      </c>
+      <c r="D303" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="304" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C304" t="s">
+        <v>96</v>
+      </c>
+      <c r="D304" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="305" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C305" t="s">
         <v>98</v>
       </c>
-      <c r="D304" s="1" t="s">
+      <c r="D305" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="306" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B306" t="s">
+    <row r="307" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B307" t="s">
         <v>91</v>
       </c>
-      <c r="C306" t="s">
+      <c r="C307" t="s">
         <v>92</v>
       </c>
-      <c r="D306" t="s">
+      <c r="D307" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="307" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C307" t="s">
+    <row r="308" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C308" t="s">
         <v>94</v>
       </c>
-      <c r="D307" t="s">
+      <c r="D308" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="310" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B310" t="s">
+    <row r="311" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B311" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="311" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C311" t="s">
+    <row r="312" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C312" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="312" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D312" t="s">
-        <v>105</v>
-      </c>
-      <c r="E312" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="313" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D313" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E313" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="314" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D314" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E314" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="315" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D315" t="s">
+        <v>103</v>
+      </c>
+      <c r="E315" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="316" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D316" t="s">
         <v>108</v>
       </c>
-      <c r="E315" t="s">
+      <c r="E316" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="317" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B317" t="s">
+    <row r="318" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B318" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="318" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C318" t="s">
+    <row r="319" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C319" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="319" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D319" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="320" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D320" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="321" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D321" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="321" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F321" s="1" t="s">
+    <row r="322" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F322" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="322" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B322" t="s">
+    <row r="323" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B323" t="s">
         <v>1</v>
       </c>
-      <c r="F322" s="1" t="s">
+      <c r="F323" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="323" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C323" t="s">
+    <row r="324" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C324" t="s">
         <v>113</v>
       </c>
-      <c r="D323" s="1" t="s">
+      <c r="D324" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="324" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D324" t="s">
+    <row r="325" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D325" t="s">
         <v>127</v>
       </c>
-      <c r="E324" s="1" t="s">
+      <c r="E325" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="325" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C325" t="s">
+    <row r="326" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C326" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="326" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D326" t="s">
+    <row r="327" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D327" t="s">
         <v>116</v>
       </c>
-      <c r="E326" s="1" t="s">
+      <c r="E327" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F326" t="s">
+      <c r="F327" t="s">
         <v>129</v>
       </c>
-      <c r="G326" s="1" t="s">
+      <c r="G327" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="327" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E327" t="s">
-        <v>122</v>
-      </c>
-      <c r="G327" s="1"/>
     </row>
     <row r="328" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E328" t="s">
+        <v>122</v>
+      </c>
+      <c r="G328" s="1"/>
+    </row>
+    <row r="329" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E329" t="s">
         <v>125</v>
-      </c>
-      <c r="G328" s="1"/>
-    </row>
-    <row r="329" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D329" t="s">
-        <v>118</v>
-      </c>
-      <c r="E329" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="G329" s="1"/>
     </row>
     <row r="330" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D330" t="s">
+        <v>118</v>
+      </c>
+      <c r="E330" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G330" s="1"/>
+    </row>
+    <row r="331" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D331" t="s">
         <v>120</v>
       </c>
-      <c r="E330" s="1" t="s">
+      <c r="E331" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G330" s="1"/>
-    </row>
-    <row r="331" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E331" s="1" t="s">
+      <c r="G331" s="1"/>
+    </row>
+    <row r="332" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E332" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="G331" s="1"/>
-    </row>
-    <row r="332" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E332" t="s">
+      <c r="G332" s="1"/>
+    </row>
+    <row r="333" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E333" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="333" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D333" t="s">
-        <v>302</v>
-      </c>
-      <c r="E333" s="1" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="334" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D334" t="s">
+        <v>302</v>
+      </c>
+      <c r="E334" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="335" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D335" t="s">
         <v>301</v>
       </c>
-      <c r="E334" s="1" t="s">
+      <c r="E335" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="339" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C339" t="s">
+    <row r="340" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C340" t="s">
         <v>132</v>
       </c>
-      <c r="D339" s="1" t="s">
+      <c r="D340" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="343" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B343" t="s">
+    <row r="344" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B344" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="344" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C344" t="s">
+    <row r="345" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C345" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="345" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D345" t="s">
+    <row r="346" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D346" t="s">
         <v>495</v>
-      </c>
-    </row>
-    <row r="346" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E346" t="s">
-        <v>494</v>
-      </c>
-      <c r="F346" s="1" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="347" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E347" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F347" s="1" t="s">
-        <v>513</v>
+        <v>493</v>
       </c>
     </row>
     <row r="348" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E348" t="s">
+        <v>496</v>
+      </c>
+      <c r="F348" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="349" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E349" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="349" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D349" t="s">
+    <row r="350" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D350" t="s">
         <v>498</v>
-      </c>
-    </row>
-    <row r="350" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E350" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="351" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E351" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="352" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E352" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="352" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D352" t="s">
+    <row r="353" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D353" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="353" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E353" t="s">
+    <row r="354" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E354" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="354" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C354" t="s">
+    <row r="355" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C355" t="s">
         <v>502</v>
-      </c>
-    </row>
-    <row r="355" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D355" t="s">
-        <v>505</v>
-      </c>
-      <c r="E355" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="356" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D356" t="s">
+        <v>505</v>
+      </c>
+      <c r="E356" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="357" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D357" t="s">
         <v>503</v>
       </c>
-      <c r="E356" t="s">
+      <c r="E357" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="358" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C358" t="s">
+    <row r="359" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C359" t="s">
         <v>507</v>
-      </c>
-    </row>
-    <row r="359" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D359" t="s">
-        <v>510</v>
-      </c>
-      <c r="E359" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="360" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D360" t="s">
+        <v>510</v>
+      </c>
+      <c r="E360" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="361" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D361" t="s">
         <v>511</v>
       </c>
-      <c r="E360" t="s">
+      <c r="E361" t="s">
         <v>509</v>
       </c>
-      <c r="G360" s="1" t="s">
+      <c r="G361" s="1" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="362" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C362" t="s">
+    <row r="363" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C363" t="s">
         <v>514</v>
       </c>
-      <c r="G362" s="1" t="s">
+      <c r="G363" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="364" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C364" t="s">
+    <row r="365" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C365" t="s">
         <v>515</v>
       </c>
-      <c r="E364" t="s">
+      <c r="E365" t="s">
         <v>516</v>
       </c>
-      <c r="G364" s="1" t="s">
+      <c r="G365" s="1" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="366" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C366" t="s">
+    <row r="367" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C367" t="s">
         <v>518</v>
-      </c>
-    </row>
-    <row r="367" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D367" t="s">
-        <v>520</v>
-      </c>
-      <c r="E367" t="s">
-        <v>519</v>
-      </c>
-      <c r="G367" s="1" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="368" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D368" t="s">
+        <v>520</v>
+      </c>
+      <c r="E368" t="s">
+        <v>519</v>
+      </c>
+      <c r="G368" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="369" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D369" t="s">
         <v>521</v>
       </c>
-      <c r="E368" t="s">
+      <c r="E369" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="370" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C370" t="s">
+    <row r="371" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C371" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="371" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D371" t="s">
+    <row r="372" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D372" t="s">
         <v>530</v>
       </c>
-      <c r="E371" t="s">
+      <c r="E372" t="s">
         <v>526</v>
       </c>
-      <c r="G371" s="1" t="s">
+      <c r="G372" s="1" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="372" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D372" t="s">
+    <row r="373" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D373" t="s">
         <v>528</v>
       </c>
-      <c r="E372" t="s">
+      <c r="E373" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="373" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D373" t="s">
+    <row r="374" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D374" t="s">
         <v>529</v>
       </c>
-      <c r="E373" t="s">
+      <c r="E374" t="s">
         <v>527</v>
+      </c>
+    </row>
+    <row r="376" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B376" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="377" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C377" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="378" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D378" t="s">
+        <v>543</v>
+      </c>
+      <c r="G378" s="1" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="379" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C379" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="380" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D380" t="s">
+        <v>545</v>
+      </c>
+      <c r="E380" t="s">
+        <v>546</v>
+      </c>
+      <c r="G380" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="382" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C382" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="383" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D383" t="s">
+        <v>550</v>
+      </c>
+      <c r="E383" t="s">
+        <v>551</v>
+      </c>
+      <c r="G383" s="1" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="384" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D384" t="s">
+        <v>552</v>
+      </c>
+      <c r="E384" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="385" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D385" t="s">
+        <v>554</v>
+      </c>
+      <c r="E385" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="386" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D386" t="s">
+        <v>556</v>
+      </c>
+      <c r="E386" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="388" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C388" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="389" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D389" t="s">
+        <v>560</v>
+      </c>
+      <c r="E389" t="s">
+        <v>562</v>
+      </c>
+      <c r="G389" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="390" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D390" t="s">
+        <v>561</v>
+      </c>
+      <c r="E390" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="392" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C392" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="393" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D393" t="s">
+        <v>567</v>
+      </c>
+      <c r="G393" s="1" t="s">
+        <v>566</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C14" r:id="rId1" xr:uid="{18CCA2F1-1074-664C-AB52-48BBB42F9065}"/>
-    <hyperlink ref="D30" r:id="rId2" location=".X6ktTC-l0Us" xr:uid="{02227101-F5A2-3446-ADC1-32F3342C625C}"/>
-    <hyperlink ref="D33" r:id="rId3" xr:uid="{6360CC1D-0E6F-6B45-B16E-E9F323959E32}"/>
-    <hyperlink ref="E45" r:id="rId4" xr:uid="{96980E2B-5D77-D04D-8463-2374C6B90C21}"/>
-    <hyperlink ref="E55" r:id="rId5" xr:uid="{5081034D-5E40-F340-99D2-B8E4DFC0468C}"/>
-    <hyperlink ref="E58" r:id="rId6" location=":~:text=You%20can%20verify%20whether%20it,password%20and%20ESSID%20are%20correct." xr:uid="{3BA51E9E-8709-874E-B6EC-40074894ACA9}"/>
-    <hyperlink ref="E53" r:id="rId7" xr:uid="{30BD9D61-AAB4-2544-987A-0386CA068398}"/>
-    <hyperlink ref="E61" r:id="rId8" xr:uid="{1824F9BF-1BD9-3842-A565-00C06FF5E50F}"/>
-    <hyperlink ref="D132" r:id="rId9" xr:uid="{E488AECD-B504-A04E-8F27-807A3A08802C}"/>
-    <hyperlink ref="D86" r:id="rId10" location="89804" xr:uid="{E34C14F5-E723-0A48-894F-222B3F74BBF9}"/>
-    <hyperlink ref="D87" r:id="rId11" xr:uid="{6C20672B-9F8F-094F-9AC8-3D1FC1C85319}"/>
-    <hyperlink ref="D88" r:id="rId12" xr:uid="{BA9A8F05-4D7F-4942-886C-F8152208F0EA}"/>
-    <hyperlink ref="F92" r:id="rId13" xr:uid="{22AE585F-7255-3F41-8A2E-808446F3A9AA}"/>
-    <hyperlink ref="F94" r:id="rId14" xr:uid="{93472772-CF6C-D045-B634-2D574A3EE034}"/>
-    <hyperlink ref="E179" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
-    <hyperlink ref="F180" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
-    <hyperlink ref="D188" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
-    <hyperlink ref="D189" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
-    <hyperlink ref="F95" r:id="rId19" xr:uid="{92BE3560-5393-C545-9D2D-2B773359B28F}"/>
-    <hyperlink ref="E205" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
-    <hyperlink ref="E206" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
-    <hyperlink ref="E207" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
-    <hyperlink ref="E69" r:id="rId23" xr:uid="{1526D7DA-27DA-1443-928C-BEDA9E425734}"/>
-    <hyperlink ref="E70" r:id="rId24" xr:uid="{4F363062-BE49-AB4F-8956-2C1F31D9B898}"/>
-    <hyperlink ref="H96" r:id="rId25" xr:uid="{D9E13355-D59B-054F-B544-34A5A285A9E0}"/>
-    <hyperlink ref="G64" r:id="rId26" xr:uid="{170917BF-0643-9848-BCA9-A3BF5219EE3E}"/>
-    <hyperlink ref="F99" r:id="rId27" xr:uid="{5D45F2D3-11BC-6E43-BEFF-29E4E04A041E}"/>
-    <hyperlink ref="I100" r:id="rId28" xr:uid="{7D985D09-6A9A-FF4D-9F4A-4C56CC604DCE}"/>
-    <hyperlink ref="D89" r:id="rId29" xr:uid="{784C3F11-339F-8242-911D-6E4E893DD319}"/>
-    <hyperlink ref="E89" r:id="rId30" xr:uid="{FC907203-09BF-654B-9028-A8528783DAFE}"/>
-    <hyperlink ref="F101" r:id="rId31" xr:uid="{EFD3653A-B2F2-614F-8DEE-A2CB34111C94}"/>
-    <hyperlink ref="F102" r:id="rId32" xr:uid="{774B592D-11A5-9C49-BB9A-61014C8D8C81}"/>
-    <hyperlink ref="F103" r:id="rId33" xr:uid="{BD793670-4C63-C04D-B52D-974AF8E59FA4}"/>
-    <hyperlink ref="F104" r:id="rId34" location="96077" xr:uid="{B9804BBD-5312-714B-97EA-CC7D2C647F2C}"/>
-    <hyperlink ref="H97" r:id="rId35" xr:uid="{7BC5BAB5-D297-0043-BAAF-45AD255D5C84}"/>
-    <hyperlink ref="I96" r:id="rId36" xr:uid="{A03C56E4-1156-A148-A568-F50A5C33DB5C}"/>
-    <hyperlink ref="F105" r:id="rId37" xr:uid="{12AC219C-4678-4E43-B328-6595FA10B8D3}"/>
-    <hyperlink ref="E107" r:id="rId38" xr:uid="{44409621-28A2-704A-B283-3DCE1EFB1603}"/>
-    <hyperlink ref="E211" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
-    <hyperlink ref="F108" r:id="rId40" xr:uid="{A9D0D792-87D1-8144-872F-5CA060D3C28F}"/>
-    <hyperlink ref="F109" r:id="rId41" xr:uid="{87EF989D-17E9-1E45-A075-CD862D0B60F4}"/>
-    <hyperlink ref="F111" r:id="rId42" xr:uid="{8406C6F0-DC69-A64D-AAD8-60A33C12D00B}"/>
-    <hyperlink ref="F112" r:id="rId43" location="108593" xr:uid="{3C38F59E-6E71-4048-9BCA-CBC77D3907E0}"/>
-    <hyperlink ref="F114" r:id="rId44" xr:uid="{EEBE2A3E-36CA-F94F-9B1D-EE463DB6425F}"/>
-    <hyperlink ref="F115" r:id="rId45" xr:uid="{3782B43D-9E6F-2940-A013-34AA5D6B4DB3}"/>
-    <hyperlink ref="F116" r:id="rId46" xr:uid="{3D1C62DB-D9B7-BE42-B21D-4EEBC4C9EFE1}"/>
-    <hyperlink ref="F117" r:id="rId47" xr:uid="{F5021A21-70A2-D34E-B055-64CAC326E7EF}"/>
-    <hyperlink ref="F118" r:id="rId48" xr:uid="{A8C010A1-8EE1-264B-8688-3BEA1B62E535}"/>
-    <hyperlink ref="E212" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
-    <hyperlink ref="F113" r:id="rId50" location="113521" xr:uid="{EE1413C5-3B38-7D4D-8DF1-634A12F0BD81}"/>
-    <hyperlink ref="E71" r:id="rId51" xr:uid="{00B1EF4A-7791-0343-8D8C-9A1E83248FC9}"/>
-    <hyperlink ref="E273" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
-    <hyperlink ref="E274" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
-    <hyperlink ref="F120" r:id="rId54" xr:uid="{40A4B6A0-2F7E-A84D-8CC6-D814A33F5953}"/>
-    <hyperlink ref="E213" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
-    <hyperlink ref="E214" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
-    <hyperlink ref="E215" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
-    <hyperlink ref="E216" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
-    <hyperlink ref="E275" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
-    <hyperlink ref="D190" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
-    <hyperlink ref="D191" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
-    <hyperlink ref="D192" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
-    <hyperlink ref="E217" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
-    <hyperlink ref="E276" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
-    <hyperlink ref="E277" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
-    <hyperlink ref="E279" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
-    <hyperlink ref="E280" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
-    <hyperlink ref="F274" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
-    <hyperlink ref="G274" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
-    <hyperlink ref="E281" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
-    <hyperlink ref="E282" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
-    <hyperlink ref="E283" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
-    <hyperlink ref="E181" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
-    <hyperlink ref="E278" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
-    <hyperlink ref="E284" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
-    <hyperlink ref="E285" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
-    <hyperlink ref="E73" r:id="rId77" location="code" xr:uid="{C0475FF8-517D-E949-887E-9A42D86E9640}"/>
-    <hyperlink ref="E287" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
-    <hyperlink ref="E74" r:id="rId79" xr:uid="{277DBE6F-F3E5-8B4C-8DD8-BD92445D1A99}"/>
-    <hyperlink ref="E289" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
-    <hyperlink ref="E294" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
-    <hyperlink ref="E196" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
-    <hyperlink ref="E197" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
-    <hyperlink ref="F141" r:id="rId84" xr:uid="{EB604865-A16B-0646-A5B5-0D047467449D}"/>
-    <hyperlink ref="E219" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
-    <hyperlink ref="D303" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
-    <hyperlink ref="D304" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
-    <hyperlink ref="E313" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
-    <hyperlink ref="E314" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
-    <hyperlink ref="E312" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
-    <hyperlink ref="D323" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
-    <hyperlink ref="E329" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
-    <hyperlink ref="E326" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
-    <hyperlink ref="E330" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
-    <hyperlink ref="F321" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
-    <hyperlink ref="F322" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
-    <hyperlink ref="E324" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
-    <hyperlink ref="G326" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
-    <hyperlink ref="D339" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
-    <hyperlink ref="E331" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
-    <hyperlink ref="E334" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
-    <hyperlink ref="E333" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
-    <hyperlink ref="F238" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
-    <hyperlink ref="E239" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
-    <hyperlink ref="E240" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
-    <hyperlink ref="E241" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
-    <hyperlink ref="G255" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
-    <hyperlink ref="E250" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
-    <hyperlink ref="E251" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
-    <hyperlink ref="E256" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
-    <hyperlink ref="F148" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
-    <hyperlink ref="F153" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
-    <hyperlink ref="F154" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
-    <hyperlink ref="F160" r:id="rId114" xr:uid="{2B03B1F0-535A-3E4F-8FB3-35D2DE847218}"/>
-    <hyperlink ref="G165" r:id="rId115" xr:uid="{11045522-E183-B14C-B43D-5EA36E454600}"/>
-    <hyperlink ref="E182" r:id="rId116" xr:uid="{F1098A8C-3BC0-DB4F-8F9C-48B31145FEC1}"/>
-    <hyperlink ref="F167" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
-    <hyperlink ref="F161" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
-    <hyperlink ref="F170" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
-    <hyperlink ref="H234" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
-    <hyperlink ref="F346" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
-    <hyperlink ref="G360" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
-    <hyperlink ref="F347" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
-    <hyperlink ref="G362" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
-    <hyperlink ref="G364" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
-    <hyperlink ref="G367" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
-    <hyperlink ref="G371" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
+    <hyperlink ref="C15" r:id="rId1" xr:uid="{18CCA2F1-1074-664C-AB52-48BBB42F9065}"/>
+    <hyperlink ref="D31" r:id="rId2" location=".X6ktTC-l0Us" xr:uid="{02227101-F5A2-3446-ADC1-32F3342C625C}"/>
+    <hyperlink ref="D34" r:id="rId3" xr:uid="{6360CC1D-0E6F-6B45-B16E-E9F323959E32}"/>
+    <hyperlink ref="E46" r:id="rId4" xr:uid="{96980E2B-5D77-D04D-8463-2374C6B90C21}"/>
+    <hyperlink ref="E56" r:id="rId5" xr:uid="{5081034D-5E40-F340-99D2-B8E4DFC0468C}"/>
+    <hyperlink ref="E59" r:id="rId6" location=":~:text=You%20can%20verify%20whether%20it,password%20and%20ESSID%20are%20correct." xr:uid="{3BA51E9E-8709-874E-B6EC-40074894ACA9}"/>
+    <hyperlink ref="E54" r:id="rId7" xr:uid="{30BD9D61-AAB4-2544-987A-0386CA068398}"/>
+    <hyperlink ref="E62" r:id="rId8" xr:uid="{1824F9BF-1BD9-3842-A565-00C06FF5E50F}"/>
+    <hyperlink ref="D133" r:id="rId9" xr:uid="{E488AECD-B504-A04E-8F27-807A3A08802C}"/>
+    <hyperlink ref="D87" r:id="rId10" location="89804" xr:uid="{E34C14F5-E723-0A48-894F-222B3F74BBF9}"/>
+    <hyperlink ref="D88" r:id="rId11" xr:uid="{6C20672B-9F8F-094F-9AC8-3D1FC1C85319}"/>
+    <hyperlink ref="D89" r:id="rId12" xr:uid="{BA9A8F05-4D7F-4942-886C-F8152208F0EA}"/>
+    <hyperlink ref="F93" r:id="rId13" xr:uid="{22AE585F-7255-3F41-8A2E-808446F3A9AA}"/>
+    <hyperlink ref="F95" r:id="rId14" xr:uid="{93472772-CF6C-D045-B634-2D574A3EE034}"/>
+    <hyperlink ref="E180" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
+    <hyperlink ref="F181" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
+    <hyperlink ref="D189" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
+    <hyperlink ref="D190" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
+    <hyperlink ref="F96" r:id="rId19" xr:uid="{92BE3560-5393-C545-9D2D-2B773359B28F}"/>
+    <hyperlink ref="E206" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
+    <hyperlink ref="E207" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
+    <hyperlink ref="E208" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
+    <hyperlink ref="E70" r:id="rId23" xr:uid="{1526D7DA-27DA-1443-928C-BEDA9E425734}"/>
+    <hyperlink ref="E71" r:id="rId24" xr:uid="{4F363062-BE49-AB4F-8956-2C1F31D9B898}"/>
+    <hyperlink ref="H97" r:id="rId25" xr:uid="{D9E13355-D59B-054F-B544-34A5A285A9E0}"/>
+    <hyperlink ref="G65" r:id="rId26" xr:uid="{170917BF-0643-9848-BCA9-A3BF5219EE3E}"/>
+    <hyperlink ref="F100" r:id="rId27" xr:uid="{5D45F2D3-11BC-6E43-BEFF-29E4E04A041E}"/>
+    <hyperlink ref="I101" r:id="rId28" xr:uid="{7D985D09-6A9A-FF4D-9F4A-4C56CC604DCE}"/>
+    <hyperlink ref="D90" r:id="rId29" xr:uid="{784C3F11-339F-8242-911D-6E4E893DD319}"/>
+    <hyperlink ref="E90" r:id="rId30" xr:uid="{FC907203-09BF-654B-9028-A8528783DAFE}"/>
+    <hyperlink ref="F102" r:id="rId31" xr:uid="{EFD3653A-B2F2-614F-8DEE-A2CB34111C94}"/>
+    <hyperlink ref="F103" r:id="rId32" xr:uid="{774B592D-11A5-9C49-BB9A-61014C8D8C81}"/>
+    <hyperlink ref="F104" r:id="rId33" xr:uid="{BD793670-4C63-C04D-B52D-974AF8E59FA4}"/>
+    <hyperlink ref="F105" r:id="rId34" location="96077" xr:uid="{B9804BBD-5312-714B-97EA-CC7D2C647F2C}"/>
+    <hyperlink ref="H98" r:id="rId35" xr:uid="{7BC5BAB5-D297-0043-BAAF-45AD255D5C84}"/>
+    <hyperlink ref="I97" r:id="rId36" xr:uid="{A03C56E4-1156-A148-A568-F50A5C33DB5C}"/>
+    <hyperlink ref="F106" r:id="rId37" xr:uid="{12AC219C-4678-4E43-B328-6595FA10B8D3}"/>
+    <hyperlink ref="E108" r:id="rId38" xr:uid="{44409621-28A2-704A-B283-3DCE1EFB1603}"/>
+    <hyperlink ref="E212" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
+    <hyperlink ref="F109" r:id="rId40" xr:uid="{A9D0D792-87D1-8144-872F-5CA060D3C28F}"/>
+    <hyperlink ref="F110" r:id="rId41" xr:uid="{87EF989D-17E9-1E45-A075-CD862D0B60F4}"/>
+    <hyperlink ref="F112" r:id="rId42" xr:uid="{8406C6F0-DC69-A64D-AAD8-60A33C12D00B}"/>
+    <hyperlink ref="F113" r:id="rId43" location="108593" xr:uid="{3C38F59E-6E71-4048-9BCA-CBC77D3907E0}"/>
+    <hyperlink ref="F115" r:id="rId44" xr:uid="{EEBE2A3E-36CA-F94F-9B1D-EE463DB6425F}"/>
+    <hyperlink ref="F116" r:id="rId45" xr:uid="{3782B43D-9E6F-2940-A013-34AA5D6B4DB3}"/>
+    <hyperlink ref="F117" r:id="rId46" xr:uid="{3D1C62DB-D9B7-BE42-B21D-4EEBC4C9EFE1}"/>
+    <hyperlink ref="F118" r:id="rId47" xr:uid="{F5021A21-70A2-D34E-B055-64CAC326E7EF}"/>
+    <hyperlink ref="F119" r:id="rId48" xr:uid="{A8C010A1-8EE1-264B-8688-3BEA1B62E535}"/>
+    <hyperlink ref="E213" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
+    <hyperlink ref="F114" r:id="rId50" location="113521" xr:uid="{EE1413C5-3B38-7D4D-8DF1-634A12F0BD81}"/>
+    <hyperlink ref="E72" r:id="rId51" xr:uid="{00B1EF4A-7791-0343-8D8C-9A1E83248FC9}"/>
+    <hyperlink ref="E274" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
+    <hyperlink ref="E275" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
+    <hyperlink ref="F121" r:id="rId54" xr:uid="{40A4B6A0-2F7E-A84D-8CC6-D814A33F5953}"/>
+    <hyperlink ref="E214" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
+    <hyperlink ref="E215" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
+    <hyperlink ref="E216" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
+    <hyperlink ref="E217" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
+    <hyperlink ref="E276" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
+    <hyperlink ref="D191" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
+    <hyperlink ref="D192" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
+    <hyperlink ref="D193" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
+    <hyperlink ref="E218" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
+    <hyperlink ref="E277" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
+    <hyperlink ref="E278" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
+    <hyperlink ref="E280" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
+    <hyperlink ref="E281" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
+    <hyperlink ref="F275" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
+    <hyperlink ref="G275" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
+    <hyperlink ref="E282" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
+    <hyperlink ref="E283" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
+    <hyperlink ref="E284" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
+    <hyperlink ref="E182" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
+    <hyperlink ref="E279" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
+    <hyperlink ref="E285" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
+    <hyperlink ref="E286" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
+    <hyperlink ref="E74" r:id="rId77" location="code" xr:uid="{C0475FF8-517D-E949-887E-9A42D86E9640}"/>
+    <hyperlink ref="E288" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
+    <hyperlink ref="E75" r:id="rId79" xr:uid="{277DBE6F-F3E5-8B4C-8DD8-BD92445D1A99}"/>
+    <hyperlink ref="E290" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
+    <hyperlink ref="E295" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
+    <hyperlink ref="E197" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
+    <hyperlink ref="E198" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
+    <hyperlink ref="F142" r:id="rId84" xr:uid="{EB604865-A16B-0646-A5B5-0D047467449D}"/>
+    <hyperlink ref="E220" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
+    <hyperlink ref="D304" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
+    <hyperlink ref="D305" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
+    <hyperlink ref="E314" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
+    <hyperlink ref="E315" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
+    <hyperlink ref="E313" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
+    <hyperlink ref="D324" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
+    <hyperlink ref="E330" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
+    <hyperlink ref="E327" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
+    <hyperlink ref="E331" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
+    <hyperlink ref="F322" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
+    <hyperlink ref="F323" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
+    <hyperlink ref="E325" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
+    <hyperlink ref="G327" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
+    <hyperlink ref="D340" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
+    <hyperlink ref="E332" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
+    <hyperlink ref="E335" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
+    <hyperlink ref="E334" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
+    <hyperlink ref="F239" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
+    <hyperlink ref="E240" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
+    <hyperlink ref="E241" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
+    <hyperlink ref="E242" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
+    <hyperlink ref="G256" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
+    <hyperlink ref="E251" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
+    <hyperlink ref="E252" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
+    <hyperlink ref="E257" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
+    <hyperlink ref="F149" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
+    <hyperlink ref="F154" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
+    <hyperlink ref="F155" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
+    <hyperlink ref="F161" r:id="rId114" xr:uid="{2B03B1F0-535A-3E4F-8FB3-35D2DE847218}"/>
+    <hyperlink ref="G166" r:id="rId115" xr:uid="{11045522-E183-B14C-B43D-5EA36E454600}"/>
+    <hyperlink ref="E183" r:id="rId116" xr:uid="{F1098A8C-3BC0-DB4F-8F9C-48B31145FEC1}"/>
+    <hyperlink ref="F168" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
+    <hyperlink ref="F162" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
+    <hyperlink ref="F171" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
+    <hyperlink ref="H235" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
+    <hyperlink ref="F347" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
+    <hyperlink ref="G361" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
+    <hyperlink ref="F348" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
+    <hyperlink ref="G363" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
+    <hyperlink ref="G365" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
+    <hyperlink ref="G368" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
+    <hyperlink ref="G372" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
+    <hyperlink ref="G380" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
+    <hyperlink ref="G378" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
+    <hyperlink ref="G383" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
+    <hyperlink ref="G389" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
+    <hyperlink ref="G393" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4373,7 +4602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
   <dimension ref="B2:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added recall the argument of previous bash command.
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9CBD4E-FD09-A74A-B2DF-44F88647EFC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6D7894-3E40-F848-8E7D-C09C5E1B5AA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="572">
   <si>
     <t>docker</t>
   </si>
@@ -1742,6 +1742,18 @@
   </si>
   <si>
     <t>1. from CMU, Allison McKnight</t>
+  </si>
+  <si>
+    <t>Bash Commands</t>
+  </si>
+  <si>
+    <t>Recall the argument of the previous bash command</t>
+  </si>
+  <si>
+    <t>$_ or !$</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/3371294/how-can-i-recall-the-argument-of-the-previous-bash-command</t>
   </si>
 </sst>
 </file>
@@ -2203,11 +2215,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I393"/>
+  <dimension ref="B1:I398"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A368" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D378" sqref="D378"/>
+      <pane ySplit="1" topLeftCell="A383" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D398" sqref="D398"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4406,7 +4418,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="385" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="385" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D385" t="s">
         <v>554</v>
       </c>
@@ -4414,7 +4426,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="386" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="386" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D386" t="s">
         <v>556</v>
       </c>
@@ -4422,12 +4434,12 @@
         <v>557</v>
       </c>
     </row>
-    <row r="388" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="388" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C388" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="389" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="389" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D389" t="s">
         <v>560</v>
       </c>
@@ -4438,7 +4450,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="390" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="390" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D390" t="s">
         <v>561</v>
       </c>
@@ -4446,17 +4458,35 @@
         <v>563</v>
       </c>
     </row>
-    <row r="392" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="392" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C392" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="393" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="393" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D393" t="s">
         <v>567</v>
       </c>
       <c r="G393" s="1" t="s">
         <v>566</v>
+      </c>
+    </row>
+    <row r="396" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B396" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="397" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C397" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="398" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E398" t="s">
+        <v>570</v>
+      </c>
+      <c r="G398" s="1" t="s">
+        <v>571</v>
       </c>
     </row>
   </sheetData>
@@ -4593,6 +4623,7 @@
     <hyperlink ref="G383" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
     <hyperlink ref="G389" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
     <hyperlink ref="G393" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
+    <hyperlink ref="G398" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for zsh binding keys as vim, and reloads pages without cache in Safari.
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6D7894-3E40-F848-8E7D-C09C5E1B5AA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44120F2E-3190-BB48-984D-40A53B990680}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="591">
   <si>
     <t>docker</t>
   </si>
@@ -1754,6 +1754,63 @@
   </si>
   <si>
     <t>https://stackoverflow.com/questions/3371294/how-can-i-recall-the-argument-of-the-previous-bash-command</t>
+  </si>
+  <si>
+    <t>Zsh Commands</t>
+  </si>
+  <si>
+    <t>Setup the terminal</t>
+  </si>
+  <si>
+    <t>1. Set the terminal command line to be vim style</t>
+  </si>
+  <si>
+    <t>in ~/.zshrc add the command</t>
+  </si>
+  <si>
+    <t>bindkey -v</t>
+  </si>
+  <si>
+    <t>https://www.techrepublic.com/blog/linux-and-open-source/using-vi-key-bindings-in-bash-and-zsh/</t>
+  </si>
+  <si>
+    <t>in ~/.bashrc add the command</t>
+  </si>
+  <si>
+    <t>set -o vi</t>
+  </si>
+  <si>
+    <t>Safari</t>
+  </si>
+  <si>
+    <t>reloads the page ignoring cache</t>
+  </si>
+  <si>
+    <t>CMD+OPTION+E</t>
+  </si>
+  <si>
+    <t>Option 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Empty cache with: </t>
+  </si>
+  <si>
+    <t>2. Refresh the page</t>
+  </si>
+  <si>
+    <t>CMD+R</t>
+  </si>
+  <si>
+    <t>https://superuser.com/questions/186594/how-can-i-force-safari-to-perform-a-full-page-reload-without-using-the-mouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Option 2 </t>
+  </si>
+  <si>
+    <t>CMD+OPTION+R</t>
+  </si>
+  <si>
+    <t>1. reloads the page ignoring cache</t>
   </si>
 </sst>
 </file>
@@ -2215,11 +2272,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I398"/>
+  <dimension ref="B1:I411"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A383" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D398" sqref="D398"/>
+      <pane ySplit="1" topLeftCell="A387" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E413" sqref="E413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2228,6 +2285,7 @@
     <col min="3" max="3" width="35.33203125" customWidth="1"/>
     <col min="4" max="4" width="43.33203125" customWidth="1"/>
     <col min="5" max="5" width="26.83203125" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4487,6 +4545,81 @@
       </c>
       <c r="G398" s="1" t="s">
         <v>571</v>
+      </c>
+    </row>
+    <row r="401" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B401" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="402" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C402" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="403" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D403" t="s">
+        <v>574</v>
+      </c>
+      <c r="E403" t="s">
+        <v>575</v>
+      </c>
+      <c r="F403" t="s">
+        <v>576</v>
+      </c>
+      <c r="G403" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="404" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E404" t="s">
+        <v>578</v>
+      </c>
+      <c r="F404" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="406" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B406" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="407" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C407" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="408" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D408" t="s">
+        <v>583</v>
+      </c>
+      <c r="E408" t="s">
+        <v>584</v>
+      </c>
+      <c r="F408" t="s">
+        <v>582</v>
+      </c>
+      <c r="G408" s="1" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="409" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E409" t="s">
+        <v>585</v>
+      </c>
+      <c r="F409" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="411" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D411" t="s">
+        <v>588</v>
+      </c>
+      <c r="E411" t="s">
+        <v>590</v>
+      </c>
+      <c r="F411" t="s">
+        <v>589</v>
       </c>
     </row>
   </sheetData>
@@ -4624,6 +4757,8 @@
     <hyperlink ref="G389" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
     <hyperlink ref="G393" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
     <hyperlink ref="G398" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
+    <hyperlink ref="G403" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
+    <hyperlink ref="G408" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips about ssh key
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44120F2E-3190-BB48-984D-40A53B990680}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A019259B-1CF3-E143-9F4B-69F8C7340DD7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="596">
   <si>
     <t>docker</t>
   </si>
@@ -1811,6 +1811,21 @@
   </si>
   <si>
     <t>1. reloads the page ignoring cache</t>
+  </si>
+  <si>
+    <t>Does ssh key need to be named id_rsa?</t>
+  </si>
+  <si>
+    <t>https://askubuntu.com/questions/30788/does-ssh-key-need-to-be-named-id-rsa</t>
+  </si>
+  <si>
+    <t>Store ssh_key in keychain</t>
+  </si>
+  <si>
+    <t>https://apple.stackexchange.com/questions/48502/how-can-i-permanently-add-my-ssh-private-key-to-keychain-so-it-is-automatically</t>
+  </si>
+  <si>
+    <t>ssh-add -K ~/.ssh/[your-private-key]</t>
   </si>
 </sst>
 </file>
@@ -2272,11 +2287,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I411"/>
+  <dimension ref="B1:I414"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A387" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E413" sqref="E413"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2386,64 +2401,71 @@
         <v>17</v>
       </c>
     </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>591</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>593</v>
+      </c>
+      <c r="D21" t="s">
+        <v>595</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D20">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D25">
         <v>1</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E25" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D21">
-        <v>2</v>
-      </c>
-      <c r="E21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
@@ -2451,1171 +2473,1178 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C31" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C34" t="s">
-        <v>30</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D38" t="s">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D39" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E40" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C41" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D42" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E43" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
         <v>36</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E48" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D46" t="s">
-        <v>30</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C48" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D49" t="s">
+        <v>30</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E50" t="s">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E53" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C53" t="s">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D54" t="s">
-        <v>48</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C55" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D56" t="s">
-        <v>51</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D57" t="s">
-        <v>52</v>
+        <v>48</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C58" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D59" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C61" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D62" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E63" s="1"/>
+        <v>55</v>
+      </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C64" t="s">
-        <v>199</v>
-      </c>
-      <c r="E64" s="1"/>
+        <v>57</v>
+      </c>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D65" t="s">
+        <v>58</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E66" s="1"/>
+    </row>
+    <row r="67" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C67" t="s">
+        <v>199</v>
+      </c>
+      <c r="E67" s="1"/>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
         <v>204</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E68" t="s">
         <v>54</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F68" t="s">
         <v>201</v>
       </c>
-      <c r="G65" s="1" t="s">
+      <c r="G68" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D66" t="s">
+    <row r="69" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D69" t="s">
         <v>205</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E69" t="s">
         <v>202</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F69" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E67" s="1"/>
-    </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E68" s="1"/>
-    </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C69" t="s">
+    <row r="70" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E70" s="1"/>
+    </row>
+    <row r="71" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E71" s="1"/>
+    </row>
+    <row r="72" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C72" t="s">
         <v>193</v>
       </c>
-      <c r="E69" s="1"/>
-    </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D70" t="s">
+      <c r="E72" s="1"/>
+    </row>
+    <row r="73" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D73" t="s">
         <v>194</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E73" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E71" s="1" t="s">
+    <row r="74" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E74" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E72" s="1" t="s">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E75" s="1" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E73" s="1"/>
-    </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D74" t="s">
-        <v>329</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D75" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E76" s="1"/>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B86" t="s">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D77" t="s">
+        <v>329</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="78" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D78" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="79" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E79" s="1"/>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C87" t="s">
-        <v>157</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C88" t="s">
-        <v>159</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C89" t="s">
-        <v>160</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C90" t="s">
-        <v>219</v>
+        <v>157</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>218</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C91" t="s">
+        <v>159</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C92" t="s">
+        <v>160</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C93" t="s">
+        <v>219</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C95" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D93" t="s">
-        <v>164</v>
-      </c>
-      <c r="E93" t="s">
-        <v>163</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E94" t="s">
-        <v>275</v>
-      </c>
-      <c r="F94" s="1"/>
-    </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D95" t="s">
-        <v>166</v>
-      </c>
-      <c r="E95" t="s">
-        <v>167</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D96" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="E96" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
     </row>
     <row r="97" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D97" t="s">
-        <v>190</v>
-      </c>
       <c r="E97" t="s">
-        <v>192</v>
-      </c>
-      <c r="F97" t="s">
-        <v>196</v>
-      </c>
-      <c r="G97" t="s">
-        <v>191</v>
-      </c>
-      <c r="H97" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="I97" s="1" t="s">
-        <v>198</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="F97" s="1"/>
     </row>
     <row r="98" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D98" t="s">
-        <v>232</v>
+        <v>166</v>
       </c>
       <c r="E98" t="s">
-        <v>234</v>
-      </c>
-      <c r="H98" s="1" t="s">
-        <v>197</v>
+        <v>167</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="99" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D99" t="s">
-        <v>233</v>
+        <v>180</v>
       </c>
       <c r="E99" t="s">
-        <v>235</v>
-      </c>
-      <c r="H99" s="1"/>
+        <v>181</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="100" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D100" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="E100" t="s">
-        <v>207</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>208</v>
+        <v>192</v>
+      </c>
+      <c r="F100" t="s">
+        <v>196</v>
+      </c>
+      <c r="G100" t="s">
+        <v>191</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="101" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D101" t="s">
-        <v>209</v>
+        <v>232</v>
       </c>
       <c r="E101" t="s">
-        <v>210</v>
-      </c>
-      <c r="F101" t="s">
-        <v>211</v>
-      </c>
-      <c r="G101" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="I101" s="1" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
     </row>
     <row r="102" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D102" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="E102" t="s">
-        <v>221</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>222</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="H102" s="1"/>
     </row>
     <row r="103" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D103" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="E103" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
     </row>
     <row r="104" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D104" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="E104" t="s">
-        <v>227</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>228</v>
+        <v>210</v>
+      </c>
+      <c r="F104" t="s">
+        <v>211</v>
+      </c>
+      <c r="G104" t="s">
+        <v>214</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="105" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D105" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="E105" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
     </row>
     <row r="106" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D106" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="E106" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
     </row>
     <row r="107" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D107" t="s">
+        <v>226</v>
+      </c>
       <c r="E107" t="s">
-        <v>238</v>
-      </c>
-      <c r="F107" s="1"/>
+        <v>227</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="108" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D108" t="s">
-        <v>240</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="F108" s="1"/>
+        <v>229</v>
+      </c>
+      <c r="E108" t="s">
+        <v>230</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="109" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D109" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E109" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="110" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D110" t="s">
-        <v>248</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>249</v>
-      </c>
+      <c r="E110" t="s">
+        <v>238</v>
+      </c>
+      <c r="F110" s="1"/>
     </row>
     <row r="111" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D111" t="s">
-        <v>250</v>
-      </c>
-      <c r="E111" t="s">
-        <v>207</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F111" s="1"/>
     </row>
     <row r="112" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D112" t="s">
+        <v>247</v>
+      </c>
+      <c r="E112" t="s">
+        <v>246</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="113" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D113" t="s">
+        <v>248</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="114" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D114" t="s">
+        <v>250</v>
+      </c>
+      <c r="E114" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="115" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D115" t="s">
         <v>252</v>
       </c>
-      <c r="F112" s="1" t="s">
+      <c r="F115" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D113" t="s">
+    <row r="116" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D116" t="s">
         <v>254</v>
       </c>
-      <c r="F113" s="1" t="s">
+      <c r="F116" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D114" t="s">
+    <row r="117" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D117" t="s">
         <v>273</v>
       </c>
-      <c r="F114" s="1" t="s">
+      <c r="F117" s="1" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D115" t="s">
+    <row r="118" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D118" t="s">
         <v>255</v>
       </c>
-      <c r="E115" t="s">
+      <c r="E118" t="s">
         <v>256</v>
       </c>
-      <c r="F115" s="1" t="s">
+      <c r="F118" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D116" t="s">
+    <row r="119" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D119" t="s">
         <v>258</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E119" t="s">
         <v>259</v>
       </c>
-      <c r="F116" s="1" t="s">
+      <c r="F119" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D117" t="s">
+    <row r="120" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D120" t="s">
         <v>262</v>
       </c>
-      <c r="F117" s="1" t="s">
+      <c r="F120" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D118" t="s">
+    <row r="121" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D121" t="s">
         <v>264</v>
       </c>
-      <c r="F118" s="1" t="s">
+      <c r="F121" s="1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D119" t="s">
+    <row r="122" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D122" t="s">
         <v>266</v>
       </c>
-      <c r="E119" t="s">
+      <c r="E122" t="s">
         <v>265</v>
       </c>
-      <c r="F119" s="1" t="s">
+      <c r="F122" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E120" t="s">
+    <row r="123" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E123" t="s">
         <v>268</v>
       </c>
-      <c r="F120" s="1"/>
-    </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D121" t="s">
+      <c r="F123" s="1"/>
+    </row>
+    <row r="124" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D124" t="s">
         <v>283</v>
       </c>
-      <c r="F121" s="1" t="s">
+      <c r="F124" s="1" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F122" s="1"/>
-    </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F123" s="1"/>
-    </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F124" s="1"/>
-    </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F125" s="1"/>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F126" s="1"/>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B127" t="s">
+    <row r="127" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="F127" s="1"/>
+    </row>
+    <row r="128" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="F128" s="1"/>
+    </row>
+    <row r="129" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F129" s="1"/>
+    </row>
+    <row r="130" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B130" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C128" t="s">
+    <row r="131" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C131" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="129" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D129" t="s">
+    <row r="132" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D132" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="130" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D130" t="s">
+    <row r="133" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D133" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="132" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C132" t="s">
+    <row r="135" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C135" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="133" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D133" s="1" t="s">
+    <row r="136" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D136" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="135" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C135" t="s">
+    <row r="138" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C138" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="136" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D136" t="s">
+    <row r="139" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D139" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="137" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D137" t="s">
+    <row r="140" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D140" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="138" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D138" t="s">
+    <row r="141" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D141" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="139" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D139" t="s">
+    <row r="142" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D142" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="141" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C141" t="s">
+    <row r="144" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C144" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="142" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D142" t="s">
+    <row r="145" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D145" t="s">
         <v>350</v>
       </c>
-      <c r="E142" t="s">
+      <c r="E145" t="s">
         <v>348</v>
       </c>
-      <c r="F142" s="1" t="s">
+      <c r="F145" s="1" t="s">
         <v>349</v>
-      </c>
-    </row>
-    <row r="143" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D143" t="s">
-        <v>351</v>
-      </c>
-      <c r="E143" t="s">
-        <v>352</v>
-      </c>
-      <c r="F143" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="145" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C145" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="146" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D146" t="s">
+        <v>351</v>
+      </c>
+      <c r="E146" t="s">
+        <v>352</v>
+      </c>
+      <c r="F146" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="148" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C148" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="149" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D149" t="s">
         <v>355</v>
       </c>
-      <c r="E146" t="s">
+      <c r="E149" t="s">
         <v>354</v>
-      </c>
-    </row>
-    <row r="147" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D147" t="s">
-        <v>356</v>
-      </c>
-      <c r="E147" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="149" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C149" t="s">
-        <v>370</v>
-      </c>
-      <c r="F149" s="1" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="150" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D150" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="E150" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="151" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D151" t="s">
-        <v>373</v>
-      </c>
-      <c r="E151" t="s">
-        <v>374</v>
+        <v>357</v>
       </c>
     </row>
     <row r="152" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D152" t="s">
-        <v>375</v>
-      </c>
-      <c r="E152" t="s">
-        <v>376</v>
+      <c r="C152" t="s">
+        <v>370</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="153" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D153" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="E153" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="154" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D154" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="E154" t="s">
-        <v>388</v>
-      </c>
-      <c r="F154" s="1" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
     </row>
     <row r="155" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D155" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
       <c r="E155" t="s">
-        <v>391</v>
-      </c>
-      <c r="F155" s="1" t="s">
-        <v>392</v>
+        <v>376</v>
+      </c>
+    </row>
+    <row r="156" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D156" t="s">
+        <v>377</v>
+      </c>
+      <c r="E156" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="157" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C157" t="s">
-        <v>380</v>
+      <c r="D157" t="s">
+        <v>387</v>
+      </c>
+      <c r="E157" t="s">
+        <v>388</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="158" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D158" t="s">
+        <v>390</v>
+      </c>
+      <c r="E158" t="s">
+        <v>391</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="160" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C160" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="161" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D161" t="s">
         <v>381</v>
       </c>
-      <c r="E158" t="s">
+      <c r="E161" t="s">
         <v>382</v>
       </c>
-      <c r="F158" t="s">
+      <c r="F161" t="s">
         <v>385</v>
-      </c>
-    </row>
-    <row r="159" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D159" t="s">
-        <v>383</v>
-      </c>
-      <c r="E159" t="s">
-        <v>384</v>
-      </c>
-      <c r="F159" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="160" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="F160" s="1"/>
-    </row>
-    <row r="161" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C161" t="s">
-        <v>393</v>
-      </c>
-      <c r="D161" t="s">
-        <v>421</v>
-      </c>
-      <c r="E161" t="s">
-        <v>394</v>
-      </c>
-      <c r="F161" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="162" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D162" t="s">
-        <v>422</v>
+        <v>383</v>
       </c>
       <c r="E162" t="s">
-        <v>423</v>
-      </c>
-      <c r="F162" s="1" t="s">
-        <v>424</v>
+        <v>384</v>
+      </c>
+      <c r="F162" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="163" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D163" t="s">
-        <v>425</v>
-      </c>
-      <c r="E163" t="s">
-        <v>426</v>
-      </c>
       <c r="F163" s="1"/>
     </row>
     <row r="164" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C164" t="s">
-        <v>395</v>
-      </c>
-      <c r="F164" s="1"/>
+        <v>393</v>
+      </c>
+      <c r="D164" t="s">
+        <v>421</v>
+      </c>
+      <c r="E164" t="s">
+        <v>394</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="165" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D165" t="s">
-        <v>397</v>
+        <v>422</v>
       </c>
       <c r="E165" t="s">
-        <v>396</v>
-      </c>
-      <c r="F165" s="1"/>
+        <v>423</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="166" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D166" t="s">
-        <v>398</v>
-      </c>
-      <c r="F166" t="s">
-        <v>399</v>
-      </c>
-      <c r="G166" s="1" t="s">
-        <v>400</v>
-      </c>
+        <v>425</v>
+      </c>
+      <c r="E166" t="s">
+        <v>426</v>
+      </c>
+      <c r="F166" s="1"/>
     </row>
     <row r="167" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C167" t="s">
-        <v>417</v>
-      </c>
-      <c r="G167" s="1"/>
+        <v>395</v>
+      </c>
+      <c r="F167" s="1"/>
     </row>
     <row r="168" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D168" t="s">
+        <v>397</v>
+      </c>
       <c r="E168" t="s">
-        <v>418</v>
-      </c>
-      <c r="F168" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="G168" s="1"/>
+        <v>396</v>
+      </c>
+      <c r="F168" s="1"/>
     </row>
     <row r="169" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E169" t="s">
-        <v>419</v>
+      <c r="D169" t="s">
+        <v>398</v>
+      </c>
+      <c r="F169" t="s">
+        <v>399</v>
+      </c>
+      <c r="G169" s="1" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="170" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C170" t="s">
+        <v>417</v>
+      </c>
+      <c r="G170" s="1"/>
+    </row>
+    <row r="171" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E171" t="s">
+        <v>418</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="G171" s="1"/>
+    </row>
+    <row r="172" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E172" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="173" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C173" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="171" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D171" t="s">
+    <row r="174" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D174" t="s">
         <v>433</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E174" t="s">
         <v>435</v>
       </c>
-      <c r="F171" s="1" t="s">
+      <c r="F174" s="1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="172" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D172" t="s">
+    <row r="175" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D175" t="s">
         <v>434</v>
       </c>
-      <c r="E172" t="s">
+      <c r="E175" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B178" t="s">
+    <row r="181" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B181" t="s">
         <v>169</v>
-      </c>
-    </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C179" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D180" t="s">
-        <v>171</v>
-      </c>
-      <c r="E180" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="181" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D181" t="s">
-        <v>175</v>
-      </c>
-      <c r="E181" t="s">
-        <v>173</v>
-      </c>
-      <c r="F181" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="182" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C182" t="s">
-        <v>322</v>
-      </c>
-      <c r="E182" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="F182" s="1"/>
+        <v>170</v>
+      </c>
     </row>
     <row r="183" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C183" t="s">
-        <v>406</v>
-      </c>
       <c r="D183" t="s">
-        <v>407</v>
+        <v>171</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="F183" s="1"/>
+        <v>172</v>
+      </c>
     </row>
     <row r="184" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D184" t="s">
+        <v>175</v>
+      </c>
+      <c r="E184" t="s">
+        <v>173</v>
+      </c>
+      <c r="F184" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="185" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C185" t="s">
+        <v>322</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F185" s="1"/>
+    </row>
+    <row r="186" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C186" t="s">
+        <v>406</v>
+      </c>
+      <c r="D186" t="s">
+        <v>407</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="F186" s="1"/>
+    </row>
+    <row r="187" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D187" t="s">
         <v>408</v>
       </c>
-      <c r="F184" s="1"/>
-    </row>
-    <row r="185" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F185" s="1"/>
+      <c r="F187" s="1"/>
     </row>
     <row r="188" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B188" t="s">
+      <c r="F188" s="1"/>
+    </row>
+    <row r="191" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B191" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="189" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C189" t="s">
-        <v>176</v>
-      </c>
-      <c r="D189" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="190" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C190" t="s">
-        <v>178</v>
-      </c>
-      <c r="D190" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="191" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C191" t="s">
-        <v>293</v>
-      </c>
-      <c r="D191" s="1" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="192" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C192" t="s">
-        <v>294</v>
+        <v>176</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>295</v>
+        <v>177</v>
       </c>
     </row>
     <row r="193" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C193" t="s">
+        <v>178</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="194" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C194" t="s">
+        <v>293</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="195" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C195" t="s">
+        <v>294</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="196" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C196" t="s">
         <v>297</v>
       </c>
-      <c r="D193" s="1" t="s">
+      <c r="D196" s="1" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="194" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D194" s="1"/>
-    </row>
-    <row r="195" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D195" s="1"/>
-    </row>
-    <row r="196" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B196" t="s">
+    <row r="197" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D197" s="1"/>
+    </row>
+    <row r="198" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D198" s="1"/>
+    </row>
+    <row r="199" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B199" t="s">
         <v>343</v>
       </c>
-      <c r="D196" s="1"/>
-    </row>
-    <row r="197" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C197" t="s">
+      <c r="D199" s="1"/>
+    </row>
+    <row r="200" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C200" t="s">
         <v>344</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D200" t="s">
         <v>369</v>
       </c>
-      <c r="E197" s="1" t="s">
+      <c r="E200" s="1" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="198" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D198" t="s">
+    <row r="201" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D201" t="s">
         <v>368</v>
       </c>
-      <c r="E198" s="1" t="s">
+      <c r="E201" s="1" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="199" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D199" s="1"/>
-    </row>
-    <row r="200" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D200" s="1"/>
-    </row>
-    <row r="201" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D201" s="1"/>
-    </row>
-    <row r="205" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B205" t="s">
+    <row r="202" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D202" s="1"/>
+    </row>
+    <row r="203" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D203" s="1"/>
+    </row>
+    <row r="204" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D204" s="1"/>
+    </row>
+    <row r="208" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B208" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="206" spans="2:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="C206" s="4" t="s">
+    <row r="209" spans="3:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="C209" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D206" s="2" t="s">
+      <c r="D209" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E206" s="1" t="s">
+      <c r="E209" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="207" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C207" t="s">
+    <row r="210" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C210" t="s">
         <v>187</v>
       </c>
-      <c r="E207" s="1" t="s">
+      <c r="E210" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="208" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C208" t="s">
+    <row r="211" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C211" t="s">
         <v>215</v>
       </c>
-      <c r="E208" s="1" t="s">
+      <c r="E211" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="210" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D210" t="s">
+    <row r="213" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D213" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="212" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C212" t="s">
+    <row r="215" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C215" t="s">
         <v>242</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D215" t="s">
         <v>243</v>
       </c>
-      <c r="E212" s="1" t="s">
+      <c r="E215" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="213" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C213" t="s">
+    <row r="216" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C216" t="s">
         <v>269</v>
       </c>
-      <c r="D213" t="s">
+      <c r="D216" t="s">
         <v>270</v>
       </c>
-      <c r="E213" s="1" t="s">
+      <c r="E216" s="1" t="s">
         <v>271</v>
-      </c>
-    </row>
-    <row r="214" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C214" t="s">
-        <v>284</v>
-      </c>
-      <c r="E214" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="215" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E215" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="216" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E216" s="1" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="217" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C217" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="218" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C218" t="s">
-        <v>299</v>
-      </c>
       <c r="E218" s="1" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
     </row>
     <row r="219" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E219" s="1"/>
+      <c r="E219" s="1" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="220" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C220" t="s">
-        <v>359</v>
-      </c>
-      <c r="D220" t="s">
-        <v>360</v>
+        <v>288</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>361</v>
+        <v>289</v>
       </c>
     </row>
     <row r="221" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E221" s="1"/>
+      <c r="C221" t="s">
+        <v>299</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="222" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E222" s="1"/>
     </row>
     <row r="223" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E223" s="1"/>
+      <c r="C223" t="s">
+        <v>359</v>
+      </c>
+      <c r="D223" t="s">
+        <v>360</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="224" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E224" s="1"/>
@@ -3633,654 +3662,648 @@
       <c r="E228" s="1"/>
     </row>
     <row r="229" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C229" t="s">
+      <c r="E229" s="1"/>
+    </row>
+    <row r="230" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E230" s="1"/>
+    </row>
+    <row r="231" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E231" s="1"/>
+    </row>
+    <row r="232" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C232" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="230" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D230" t="s">
-        <v>135</v>
-      </c>
-      <c r="E230" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="231" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D231" t="s">
-        <v>136</v>
-      </c>
-      <c r="E231" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="232" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D232" t="s">
-        <v>140</v>
-      </c>
-      <c r="E232" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="233" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D233" t="s">
-        <v>137</v>
+        <v>135</v>
+      </c>
+      <c r="E233" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="234" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D234" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E234" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="235" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D235" t="s">
-        <v>484</v>
+        <v>140</v>
       </c>
       <c r="E235" t="s">
-        <v>486</v>
-      </c>
-      <c r="F235" t="s">
-        <v>490</v>
-      </c>
-      <c r="G235" t="s">
-        <v>485</v>
-      </c>
-      <c r="H235" s="1" t="s">
-        <v>491</v>
+        <v>141</v>
       </c>
     </row>
     <row r="236" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D236" t="s">
-        <v>487</v>
-      </c>
-      <c r="E236" t="s">
-        <v>488</v>
-      </c>
-      <c r="G236" t="s">
-        <v>489</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="237" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D237" t="s">
+        <v>142</v>
+      </c>
+      <c r="E237" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="238" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C238" t="s">
-        <v>367</v>
+      <c r="D238" t="s">
+        <v>484</v>
+      </c>
+      <c r="E238" t="s">
+        <v>486</v>
+      </c>
+      <c r="F238" t="s">
+        <v>490</v>
+      </c>
+      <c r="G238" t="s">
+        <v>485</v>
+      </c>
+      <c r="H238" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="239" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D239" t="s">
+        <v>487</v>
+      </c>
+      <c r="E239" t="s">
+        <v>488</v>
+      </c>
+      <c r="G239" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="241" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C241" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="242" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D242" t="s">
         <v>73</v>
       </c>
-      <c r="E239" t="s">
+      <c r="E242" t="s">
         <v>74</v>
       </c>
-      <c r="F239" s="1" t="s">
+      <c r="F242" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="240" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D240" t="s">
+    <row r="243" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D243" t="s">
         <v>76</v>
       </c>
-      <c r="E240" s="1" t="s">
+      <c r="E243" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="241" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D241" t="s">
+    <row r="244" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D244" t="s">
         <v>78</v>
       </c>
-      <c r="E241" s="1" t="s">
+      <c r="E244" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="242" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D242" t="s">
+    <row r="245" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D245" t="s">
         <v>81</v>
       </c>
-      <c r="E242" s="1" t="s">
+      <c r="E245" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="243" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D243" t="s">
+    <row r="246" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D246" t="s">
         <v>362</v>
       </c>
-      <c r="E243" t="s">
+      <c r="E246" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="244" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D244" t="s">
+    <row r="247" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D247" t="s">
         <v>363</v>
       </c>
-      <c r="E244" t="s">
+      <c r="E247" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="246" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D246" t="s">
+    <row r="249" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D249" t="s">
         <v>82</v>
       </c>
-      <c r="E246" t="s">
+      <c r="E249" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="247" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D247" t="s">
+    <row r="250" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D250" t="s">
         <v>84</v>
       </c>
-      <c r="E247" t="s">
+      <c r="E250" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="249" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C249" t="s">
+    <row r="252" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C252" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="250" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D250" t="s">
+    <row r="253" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D253" t="s">
         <v>73</v>
       </c>
-      <c r="E250" t="s">
+      <c r="E253" t="s">
         <v>131</v>
       </c>
-      <c r="F250" s="1"/>
-    </row>
-    <row r="251" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D251" t="s">
+      <c r="F253" s="1"/>
+    </row>
+    <row r="254" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D254" t="s">
         <v>147</v>
       </c>
-      <c r="E251" s="1" t="s">
+      <c r="E254" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F251" s="1"/>
-    </row>
-    <row r="252" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D252" t="s">
+      <c r="F254" s="1"/>
+    </row>
+    <row r="255" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D255" t="s">
         <v>76</v>
       </c>
-      <c r="E252" s="1" t="s">
+      <c r="E255" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="253" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E253" s="1"/>
-    </row>
-    <row r="254" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D254" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="255" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E255" t="s">
-        <v>151</v>
-      </c>
-      <c r="F255" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="256" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E256" t="s">
-        <v>152</v>
-      </c>
-      <c r="F256" t="s">
-        <v>145</v>
-      </c>
-      <c r="G256" s="1" t="s">
-        <v>146</v>
-      </c>
+    <row r="256" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="E256" s="1"/>
     </row>
     <row r="257" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D257" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="258" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E258" t="s">
+        <v>151</v>
+      </c>
+      <c r="F258" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="259" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E259" t="s">
+        <v>152</v>
+      </c>
+      <c r="F259" t="s">
+        <v>145</v>
+      </c>
+      <c r="G259" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="260" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D260" t="s">
         <v>153</v>
       </c>
-      <c r="E257" s="1" t="s">
+      <c r="E260" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G257" s="1"/>
-    </row>
-    <row r="271" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E271" s="1"/>
-    </row>
-    <row r="273" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B273" t="s">
+      <c r="G260" s="1"/>
+    </row>
+    <row r="274" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E274" s="1"/>
+    </row>
+    <row r="276" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B276" t="s">
         <v>276</v>
-      </c>
-    </row>
-    <row r="274" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C274" t="s">
-        <v>277</v>
-      </c>
-      <c r="D274" t="s">
-        <v>279</v>
-      </c>
-      <c r="E274" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="275" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C275" t="s">
-        <v>281</v>
-      </c>
-      <c r="E275" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="F275" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="G275" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="276" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C276" t="s">
-        <v>290</v>
-      </c>
-      <c r="E276" s="1" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="277" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C277" t="s">
-        <v>304</v>
+        <v>277</v>
+      </c>
+      <c r="D277" t="s">
+        <v>279</v>
       </c>
       <c r="E277" s="1" t="s">
-        <v>305</v>
+        <v>278</v>
       </c>
     </row>
     <row r="278" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D278" t="s">
-        <v>306</v>
+      <c r="C278" t="s">
+        <v>281</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>307</v>
+        <v>280</v>
+      </c>
+      <c r="F278" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G278" s="1" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="279" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C279" t="s">
-        <v>324</v>
+        <v>290</v>
       </c>
       <c r="E279" s="1" t="s">
-        <v>323</v>
+        <v>291</v>
       </c>
     </row>
     <row r="280" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C280" t="s">
-        <v>308</v>
-      </c>
-      <c r="D280" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="E280" s="1" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="281" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C281" t="s">
-        <v>311</v>
+      <c r="D281" t="s">
+        <v>306</v>
       </c>
       <c r="E281" s="1" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="282" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C282" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="E282" s="1" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
     </row>
     <row r="283" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C283" t="s">
-        <v>317</v>
+        <v>308</v>
+      </c>
+      <c r="D283" t="s">
+        <v>309</v>
       </c>
       <c r="E283" s="1" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
     </row>
     <row r="284" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C284" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="E284" s="1" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="285" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C285" t="s">
-        <v>326</v>
-      </c>
-      <c r="D285" t="s">
-        <v>333</v>
+        <v>316</v>
       </c>
       <c r="E285" s="1" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
     </row>
     <row r="286" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D286" t="s">
-        <v>328</v>
+      <c r="C286" t="s">
+        <v>317</v>
       </c>
       <c r="E286" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
+      </c>
+    </row>
+    <row r="287" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C287" t="s">
+        <v>319</v>
+      </c>
+      <c r="E287" s="1" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="288" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C288" t="s">
+        <v>326</v>
+      </c>
+      <c r="D288" t="s">
+        <v>333</v>
+      </c>
+      <c r="E288" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="289" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D289" t="s">
+        <v>328</v>
+      </c>
+      <c r="E289" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="291" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C291" t="s">
         <v>330</v>
       </c>
-      <c r="D288" t="s">
+      <c r="D291" t="s">
         <v>331</v>
       </c>
-      <c r="E288" s="1" t="s">
+      <c r="E291" s="1" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="290" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C290" t="s">
+    <row r="293" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C293" t="s">
         <v>336</v>
       </c>
-      <c r="D290" t="s">
+      <c r="D293" t="s">
         <v>338</v>
       </c>
-      <c r="E290" s="1" t="s">
+      <c r="E293" s="1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="294" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B294" t="s">
+    <row r="297" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B297" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="295" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C295" t="s">
+    <row r="298" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C298" t="s">
         <v>342</v>
       </c>
-      <c r="D295" t="s">
+      <c r="D298" t="s">
         <v>340</v>
       </c>
-      <c r="E295" s="1" t="s">
+      <c r="E298" s="1" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="301" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B301" t="s">
+    <row r="304" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B304" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="302" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C302" t="s">
-        <v>87</v>
-      </c>
-      <c r="D302" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="303" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C303" t="s">
-        <v>89</v>
-      </c>
-      <c r="D303" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="304" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C304" t="s">
-        <v>96</v>
-      </c>
-      <c r="D304" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="305" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C305" t="s">
-        <v>98</v>
-      </c>
-      <c r="D305" s="1" t="s">
-        <v>99</v>
+        <v>87</v>
+      </c>
+      <c r="D305" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="306" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C306" t="s">
+        <v>89</v>
+      </c>
+      <c r="D306" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="307" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B307" t="s">
-        <v>91</v>
-      </c>
       <c r="C307" t="s">
-        <v>92</v>
-      </c>
-      <c r="D307" t="s">
-        <v>93</v>
+        <v>96</v>
+      </c>
+      <c r="D307" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="308" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C308" t="s">
+        <v>98</v>
+      </c>
+      <c r="D308" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="310" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B310" t="s">
+        <v>91</v>
+      </c>
+      <c r="C310" t="s">
+        <v>92</v>
+      </c>
+      <c r="D310" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="311" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C311" t="s">
         <v>94</v>
       </c>
-      <c r="D308" t="s">
+      <c r="D311" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="311" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B311" t="s">
+    <row r="314" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B314" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="312" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C312" t="s">
+    <row r="315" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C315" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="313" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D313" t="s">
-        <v>105</v>
-      </c>
-      <c r="E313" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="314" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D314" t="s">
-        <v>102</v>
-      </c>
-      <c r="E314" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="315" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D315" t="s">
-        <v>103</v>
-      </c>
-      <c r="E315" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="316" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D316" t="s">
+        <v>105</v>
+      </c>
+      <c r="E316" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="317" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D317" t="s">
+        <v>102</v>
+      </c>
+      <c r="E317" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="318" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D318" t="s">
+        <v>103</v>
+      </c>
+      <c r="E318" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="319" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D319" t="s">
         <v>108</v>
       </c>
-      <c r="E316" t="s">
+      <c r="E319" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="318" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B318" t="s">
+    <row r="321" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B321" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="319" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C319" t="s">
+    <row r="322" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C322" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="320" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D320" t="s">
+    <row r="323" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D323" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="321" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D321" t="s">
+    <row r="324" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D324" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="322" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F322" s="1" t="s">
+    <row r="325" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F325" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="323" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B323" t="s">
+    <row r="326" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B326" t="s">
         <v>1</v>
       </c>
-      <c r="F323" s="1" t="s">
+      <c r="F326" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="324" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C324" t="s">
+    <row r="327" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C327" t="s">
         <v>113</v>
       </c>
-      <c r="D324" s="1" t="s">
+      <c r="D327" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="325" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D325" t="s">
+    <row r="328" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D328" t="s">
         <v>127</v>
       </c>
-      <c r="E325" s="1" t="s">
+      <c r="E328" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="326" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C326" t="s">
+    <row r="329" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C329" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="327" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D327" t="s">
-        <v>116</v>
-      </c>
-      <c r="E327" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F327" t="s">
-        <v>129</v>
-      </c>
-      <c r="G327" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="328" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E328" t="s">
-        <v>122</v>
-      </c>
-      <c r="G328" s="1"/>
-    </row>
-    <row r="329" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E329" t="s">
-        <v>125</v>
-      </c>
-      <c r="G329" s="1"/>
     </row>
     <row r="330" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D330" t="s">
+        <v>116</v>
+      </c>
+      <c r="E330" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F330" t="s">
+        <v>129</v>
+      </c>
+      <c r="G330" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="331" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E331" t="s">
+        <v>122</v>
+      </c>
+      <c r="G331" s="1"/>
+    </row>
+    <row r="332" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E332" t="s">
+        <v>125</v>
+      </c>
+      <c r="G332" s="1"/>
+    </row>
+    <row r="333" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D333" t="s">
         <v>118</v>
       </c>
-      <c r="E330" s="1" t="s">
+      <c r="E333" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G330" s="1"/>
-    </row>
-    <row r="331" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D331" t="s">
-        <v>120</v>
-      </c>
-      <c r="E331" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G331" s="1"/>
-    </row>
-    <row r="332" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E332" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="G332" s="1"/>
-    </row>
-    <row r="333" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E333" t="s">
-        <v>128</v>
-      </c>
+      <c r="G333" s="1"/>
     </row>
     <row r="334" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D334" t="s">
+        <v>120</v>
+      </c>
+      <c r="E334" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G334" s="1"/>
+    </row>
+    <row r="335" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E335" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="G335" s="1"/>
+    </row>
+    <row r="336" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E336" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="337" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D337" t="s">
         <v>302</v>
       </c>
-      <c r="E334" s="1" t="s">
+      <c r="E337" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="335" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D335" t="s">
+    <row r="338" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D338" t="s">
         <v>301</v>
       </c>
-      <c r="E335" s="1" t="s">
+      <c r="E338" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="340" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C340" t="s">
+    <row r="343" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C343" t="s">
         <v>132</v>
       </c>
-      <c r="D340" s="1" t="s">
+      <c r="D343" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="344" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B344" t="s">
+    <row r="347" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B347" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="345" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C345" t="s">
+    <row r="348" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C348" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="346" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D346" t="s">
+    <row r="349" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D349" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="347" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E347" t="s">
+    <row r="350" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E350" t="s">
         <v>494</v>
       </c>
-      <c r="F347" s="1" t="s">
+      <c r="F350" s="1" t="s">
         <v>493</v>
-      </c>
-    </row>
-    <row r="348" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E348" t="s">
-        <v>496</v>
-      </c>
-      <c r="F348" s="1" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="349" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E349" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="350" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D350" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="351" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E351" t="s">
-        <v>499</v>
+        <v>496</v>
+      </c>
+      <c r="F351" s="1" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="352" spans="2:6" x14ac:dyDescent="0.2">
@@ -4290,475 +4313,492 @@
     </row>
     <row r="353" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D353" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="354" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E354" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="355" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C355" t="s">
-        <v>502</v>
+      <c r="E355" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="356" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D356" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="357" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E357" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="358" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C358" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="359" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D359" t="s">
         <v>505</v>
       </c>
-      <c r="E356" t="s">
+      <c r="E359" t="s">
         <v>506</v>
-      </c>
-    </row>
-    <row r="357" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D357" t="s">
-        <v>503</v>
-      </c>
-      <c r="E357" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="359" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C359" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="360" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D360" t="s">
+        <v>503</v>
+      </c>
+      <c r="E360" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="362" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C362" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="363" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D363" t="s">
         <v>510</v>
       </c>
-      <c r="E360" t="s">
+      <c r="E363" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="361" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D361" t="s">
+    <row r="364" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D364" t="s">
         <v>511</v>
       </c>
-      <c r="E361" t="s">
+      <c r="E364" t="s">
         <v>509</v>
       </c>
-      <c r="G361" s="1" t="s">
+      <c r="G364" s="1" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="363" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C363" t="s">
+    <row r="366" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C366" t="s">
         <v>514</v>
       </c>
-      <c r="G363" s="1" t="s">
+      <c r="G366" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="365" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C365" t="s">
+    <row r="368" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C368" t="s">
         <v>515</v>
       </c>
-      <c r="E365" t="s">
+      <c r="E368" t="s">
         <v>516</v>
       </c>
-      <c r="G365" s="1" t="s">
+      <c r="G368" s="1" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="367" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C367" t="s">
+    <row r="370" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C370" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="368" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D368" t="s">
+    <row r="371" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D371" t="s">
         <v>520</v>
       </c>
-      <c r="E368" t="s">
+      <c r="E371" t="s">
         <v>519</v>
       </c>
-      <c r="G368" s="1" t="s">
+      <c r="G371" s="1" t="s">
         <v>523</v>
-      </c>
-    </row>
-    <row r="369" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D369" t="s">
-        <v>521</v>
-      </c>
-      <c r="E369" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="371" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C371" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="372" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D372" t="s">
+        <v>521</v>
+      </c>
+      <c r="E372" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="374" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C374" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="375" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D375" t="s">
         <v>530</v>
       </c>
-      <c r="E372" t="s">
+      <c r="E375" t="s">
         <v>526</v>
       </c>
-      <c r="G372" s="1" t="s">
+      <c r="G375" s="1" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="373" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D373" t="s">
+    <row r="376" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D376" t="s">
         <v>528</v>
       </c>
-      <c r="E373" t="s">
+      <c r="E376" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="374" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D374" t="s">
+    <row r="377" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D377" t="s">
         <v>529</v>
       </c>
-      <c r="E374" t="s">
+      <c r="E377" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="376" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B376" t="s">
+    <row r="379" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B379" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="377" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C377" t="s">
+    <row r="380" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C380" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="378" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D378" t="s">
+    <row r="381" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D381" t="s">
         <v>543</v>
       </c>
-      <c r="G378" s="1" t="s">
+      <c r="G381" s="1" t="s">
         <v>548</v>
-      </c>
-    </row>
-    <row r="379" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C379" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="380" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D380" t="s">
-        <v>545</v>
-      </c>
-      <c r="E380" t="s">
-        <v>546</v>
-      </c>
-      <c r="G380" s="1" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="382" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C382" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
     </row>
     <row r="383" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D383" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="E383" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="G383" s="1" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="384" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D384" t="s">
-        <v>552</v>
-      </c>
-      <c r="E384" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
     </row>
     <row r="385" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D385" t="s">
-        <v>554</v>
-      </c>
-      <c r="E385" t="s">
-        <v>555</v>
+      <c r="C385" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="386" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D386" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="E386" t="s">
-        <v>557</v>
+        <v>551</v>
+      </c>
+      <c r="G386" s="1" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="387" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D387" t="s">
+        <v>552</v>
+      </c>
+      <c r="E387" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="388" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C388" t="s">
-        <v>559</v>
+      <c r="D388" t="s">
+        <v>554</v>
+      </c>
+      <c r="E388" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="389" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D389" t="s">
+        <v>556</v>
+      </c>
+      <c r="E389" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="391" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C391" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="392" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D392" t="s">
         <v>560</v>
       </c>
-      <c r="E389" t="s">
+      <c r="E392" t="s">
         <v>562</v>
       </c>
-      <c r="G389" s="1" t="s">
+      <c r="G392" s="1" t="s">
         <v>564</v>
-      </c>
-    </row>
-    <row r="390" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D390" t="s">
-        <v>561</v>
-      </c>
-      <c r="E390" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="392" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C392" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="393" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D393" t="s">
+        <v>561</v>
+      </c>
+      <c r="E393" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="395" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C395" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="396" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D396" t="s">
         <v>567</v>
       </c>
-      <c r="G393" s="1" t="s">
+      <c r="G396" s="1" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="396" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B396" t="s">
+    <row r="399" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B399" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="397" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C397" t="s">
+    <row r="400" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C400" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="398" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E398" t="s">
+    <row r="401" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E401" t="s">
         <v>570</v>
       </c>
-      <c r="G398" s="1" t="s">
+      <c r="G401" s="1" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="401" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B401" t="s">
+    <row r="404" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B404" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="402" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C402" t="s">
+    <row r="405" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C405" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="403" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D403" t="s">
+    <row r="406" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D406" t="s">
         <v>574</v>
       </c>
-      <c r="E403" t="s">
+      <c r="E406" t="s">
         <v>575</v>
       </c>
-      <c r="F403" t="s">
+      <c r="F406" t="s">
         <v>576</v>
       </c>
-      <c r="G403" s="1" t="s">
+      <c r="G406" s="1" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="404" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E404" t="s">
+    <row r="407" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E407" t="s">
         <v>578</v>
       </c>
-      <c r="F404" t="s">
+      <c r="F407" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="406" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B406" t="s">
+    <row r="409" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B409" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="407" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C407" t="s">
+    <row r="410" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C410" t="s">
         <v>581</v>
-      </c>
-    </row>
-    <row r="408" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D408" t="s">
-        <v>583</v>
-      </c>
-      <c r="E408" t="s">
-        <v>584</v>
-      </c>
-      <c r="F408" t="s">
-        <v>582</v>
-      </c>
-      <c r="G408" s="1" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="409" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E409" t="s">
-        <v>585</v>
-      </c>
-      <c r="F409" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="411" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D411" t="s">
+        <v>583</v>
+      </c>
+      <c r="E411" t="s">
+        <v>584</v>
+      </c>
+      <c r="F411" t="s">
+        <v>582</v>
+      </c>
+      <c r="G411" s="1" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="412" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E412" t="s">
+        <v>585</v>
+      </c>
+      <c r="F412" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="414" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D414" t="s">
         <v>588</v>
       </c>
-      <c r="E411" t="s">
+      <c r="E414" t="s">
         <v>590</v>
       </c>
-      <c r="F411" t="s">
+      <c r="F414" t="s">
         <v>589</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C15" r:id="rId1" xr:uid="{18CCA2F1-1074-664C-AB52-48BBB42F9065}"/>
-    <hyperlink ref="D31" r:id="rId2" location=".X6ktTC-l0Us" xr:uid="{02227101-F5A2-3446-ADC1-32F3342C625C}"/>
-    <hyperlink ref="D34" r:id="rId3" xr:uid="{6360CC1D-0E6F-6B45-B16E-E9F323959E32}"/>
-    <hyperlink ref="E46" r:id="rId4" xr:uid="{96980E2B-5D77-D04D-8463-2374C6B90C21}"/>
-    <hyperlink ref="E56" r:id="rId5" xr:uid="{5081034D-5E40-F340-99D2-B8E4DFC0468C}"/>
-    <hyperlink ref="E59" r:id="rId6" location=":~:text=You%20can%20verify%20whether%20it,password%20and%20ESSID%20are%20correct." xr:uid="{3BA51E9E-8709-874E-B6EC-40074894ACA9}"/>
-    <hyperlink ref="E54" r:id="rId7" xr:uid="{30BD9D61-AAB4-2544-987A-0386CA068398}"/>
-    <hyperlink ref="E62" r:id="rId8" xr:uid="{1824F9BF-1BD9-3842-A565-00C06FF5E50F}"/>
-    <hyperlink ref="D133" r:id="rId9" xr:uid="{E488AECD-B504-A04E-8F27-807A3A08802C}"/>
-    <hyperlink ref="D87" r:id="rId10" location="89804" xr:uid="{E34C14F5-E723-0A48-894F-222B3F74BBF9}"/>
-    <hyperlink ref="D88" r:id="rId11" xr:uid="{6C20672B-9F8F-094F-9AC8-3D1FC1C85319}"/>
-    <hyperlink ref="D89" r:id="rId12" xr:uid="{BA9A8F05-4D7F-4942-886C-F8152208F0EA}"/>
-    <hyperlink ref="F93" r:id="rId13" xr:uid="{22AE585F-7255-3F41-8A2E-808446F3A9AA}"/>
-    <hyperlink ref="F95" r:id="rId14" xr:uid="{93472772-CF6C-D045-B634-2D574A3EE034}"/>
-    <hyperlink ref="E180" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
-    <hyperlink ref="F181" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
-    <hyperlink ref="D189" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
-    <hyperlink ref="D190" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
-    <hyperlink ref="F96" r:id="rId19" xr:uid="{92BE3560-5393-C545-9D2D-2B773359B28F}"/>
-    <hyperlink ref="E206" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
-    <hyperlink ref="E207" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
-    <hyperlink ref="E208" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
-    <hyperlink ref="E70" r:id="rId23" xr:uid="{1526D7DA-27DA-1443-928C-BEDA9E425734}"/>
-    <hyperlink ref="E71" r:id="rId24" xr:uid="{4F363062-BE49-AB4F-8956-2C1F31D9B898}"/>
-    <hyperlink ref="H97" r:id="rId25" xr:uid="{D9E13355-D59B-054F-B544-34A5A285A9E0}"/>
-    <hyperlink ref="G65" r:id="rId26" xr:uid="{170917BF-0643-9848-BCA9-A3BF5219EE3E}"/>
-    <hyperlink ref="F100" r:id="rId27" xr:uid="{5D45F2D3-11BC-6E43-BEFF-29E4E04A041E}"/>
-    <hyperlink ref="I101" r:id="rId28" xr:uid="{7D985D09-6A9A-FF4D-9F4A-4C56CC604DCE}"/>
-    <hyperlink ref="D90" r:id="rId29" xr:uid="{784C3F11-339F-8242-911D-6E4E893DD319}"/>
-    <hyperlink ref="E90" r:id="rId30" xr:uid="{FC907203-09BF-654B-9028-A8528783DAFE}"/>
-    <hyperlink ref="F102" r:id="rId31" xr:uid="{EFD3653A-B2F2-614F-8DEE-A2CB34111C94}"/>
-    <hyperlink ref="F103" r:id="rId32" xr:uid="{774B592D-11A5-9C49-BB9A-61014C8D8C81}"/>
-    <hyperlink ref="F104" r:id="rId33" xr:uid="{BD793670-4C63-C04D-B52D-974AF8E59FA4}"/>
-    <hyperlink ref="F105" r:id="rId34" location="96077" xr:uid="{B9804BBD-5312-714B-97EA-CC7D2C647F2C}"/>
-    <hyperlink ref="H98" r:id="rId35" xr:uid="{7BC5BAB5-D297-0043-BAAF-45AD255D5C84}"/>
-    <hyperlink ref="I97" r:id="rId36" xr:uid="{A03C56E4-1156-A148-A568-F50A5C33DB5C}"/>
-    <hyperlink ref="F106" r:id="rId37" xr:uid="{12AC219C-4678-4E43-B328-6595FA10B8D3}"/>
-    <hyperlink ref="E108" r:id="rId38" xr:uid="{44409621-28A2-704A-B283-3DCE1EFB1603}"/>
-    <hyperlink ref="E212" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
-    <hyperlink ref="F109" r:id="rId40" xr:uid="{A9D0D792-87D1-8144-872F-5CA060D3C28F}"/>
-    <hyperlink ref="F110" r:id="rId41" xr:uid="{87EF989D-17E9-1E45-A075-CD862D0B60F4}"/>
-    <hyperlink ref="F112" r:id="rId42" xr:uid="{8406C6F0-DC69-A64D-AAD8-60A33C12D00B}"/>
-    <hyperlink ref="F113" r:id="rId43" location="108593" xr:uid="{3C38F59E-6E71-4048-9BCA-CBC77D3907E0}"/>
-    <hyperlink ref="F115" r:id="rId44" xr:uid="{EEBE2A3E-36CA-F94F-9B1D-EE463DB6425F}"/>
-    <hyperlink ref="F116" r:id="rId45" xr:uid="{3782B43D-9E6F-2940-A013-34AA5D6B4DB3}"/>
-    <hyperlink ref="F117" r:id="rId46" xr:uid="{3D1C62DB-D9B7-BE42-B21D-4EEBC4C9EFE1}"/>
-    <hyperlink ref="F118" r:id="rId47" xr:uid="{F5021A21-70A2-D34E-B055-64CAC326E7EF}"/>
-    <hyperlink ref="F119" r:id="rId48" xr:uid="{A8C010A1-8EE1-264B-8688-3BEA1B62E535}"/>
-    <hyperlink ref="E213" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
-    <hyperlink ref="F114" r:id="rId50" location="113521" xr:uid="{EE1413C5-3B38-7D4D-8DF1-634A12F0BD81}"/>
-    <hyperlink ref="E72" r:id="rId51" xr:uid="{00B1EF4A-7791-0343-8D8C-9A1E83248FC9}"/>
-    <hyperlink ref="E274" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
-    <hyperlink ref="E275" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
-    <hyperlink ref="F121" r:id="rId54" xr:uid="{40A4B6A0-2F7E-A84D-8CC6-D814A33F5953}"/>
-    <hyperlink ref="E214" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
-    <hyperlink ref="E215" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
-    <hyperlink ref="E216" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
-    <hyperlink ref="E217" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
-    <hyperlink ref="E276" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
-    <hyperlink ref="D191" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
-    <hyperlink ref="D192" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
-    <hyperlink ref="D193" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
-    <hyperlink ref="E218" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
-    <hyperlink ref="E277" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
-    <hyperlink ref="E278" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
-    <hyperlink ref="E280" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
-    <hyperlink ref="E281" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
-    <hyperlink ref="F275" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
-    <hyperlink ref="G275" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
-    <hyperlink ref="E282" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
-    <hyperlink ref="E283" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
-    <hyperlink ref="E284" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
-    <hyperlink ref="E182" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
-    <hyperlink ref="E279" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
-    <hyperlink ref="E285" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
-    <hyperlink ref="E286" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
-    <hyperlink ref="E74" r:id="rId77" location="code" xr:uid="{C0475FF8-517D-E949-887E-9A42D86E9640}"/>
-    <hyperlink ref="E288" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
-    <hyperlink ref="E75" r:id="rId79" xr:uid="{277DBE6F-F3E5-8B4C-8DD8-BD92445D1A99}"/>
-    <hyperlink ref="E290" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
-    <hyperlink ref="E295" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
-    <hyperlink ref="E197" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
-    <hyperlink ref="E198" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
-    <hyperlink ref="F142" r:id="rId84" xr:uid="{EB604865-A16B-0646-A5B5-0D047467449D}"/>
-    <hyperlink ref="E220" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
-    <hyperlink ref="D304" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
-    <hyperlink ref="D305" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
-    <hyperlink ref="E314" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
-    <hyperlink ref="E315" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
-    <hyperlink ref="E313" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
-    <hyperlink ref="D324" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
-    <hyperlink ref="E330" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
-    <hyperlink ref="E327" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
-    <hyperlink ref="E331" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
-    <hyperlink ref="F322" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
-    <hyperlink ref="F323" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
-    <hyperlink ref="E325" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
-    <hyperlink ref="G327" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
-    <hyperlink ref="D340" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
-    <hyperlink ref="E332" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
-    <hyperlink ref="E335" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
-    <hyperlink ref="E334" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
-    <hyperlink ref="F239" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
-    <hyperlink ref="E240" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
-    <hyperlink ref="E241" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
-    <hyperlink ref="E242" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
-    <hyperlink ref="G256" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
-    <hyperlink ref="E251" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
-    <hyperlink ref="E252" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
-    <hyperlink ref="E257" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
-    <hyperlink ref="F149" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
-    <hyperlink ref="F154" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
-    <hyperlink ref="F155" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
-    <hyperlink ref="F161" r:id="rId114" xr:uid="{2B03B1F0-535A-3E4F-8FB3-35D2DE847218}"/>
-    <hyperlink ref="G166" r:id="rId115" xr:uid="{11045522-E183-B14C-B43D-5EA36E454600}"/>
-    <hyperlink ref="E183" r:id="rId116" xr:uid="{F1098A8C-3BC0-DB4F-8F9C-48B31145FEC1}"/>
-    <hyperlink ref="F168" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
-    <hyperlink ref="F162" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
-    <hyperlink ref="F171" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
-    <hyperlink ref="H235" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
-    <hyperlink ref="F347" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
-    <hyperlink ref="G361" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
-    <hyperlink ref="F348" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
-    <hyperlink ref="G363" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
-    <hyperlink ref="G365" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
-    <hyperlink ref="G368" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
-    <hyperlink ref="G372" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
-    <hyperlink ref="G380" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
-    <hyperlink ref="G378" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
-    <hyperlink ref="G383" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
-    <hyperlink ref="G389" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
-    <hyperlink ref="G393" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
-    <hyperlink ref="G398" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
-    <hyperlink ref="G403" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
-    <hyperlink ref="G408" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
+    <hyperlink ref="D18" r:id="rId2" location=".X6ktTC-l0Us" xr:uid="{02227101-F5A2-3446-ADC1-32F3342C625C}"/>
+    <hyperlink ref="D37" r:id="rId3" xr:uid="{6360CC1D-0E6F-6B45-B16E-E9F323959E32}"/>
+    <hyperlink ref="E49" r:id="rId4" xr:uid="{96980E2B-5D77-D04D-8463-2374C6B90C21}"/>
+    <hyperlink ref="E59" r:id="rId5" xr:uid="{5081034D-5E40-F340-99D2-B8E4DFC0468C}"/>
+    <hyperlink ref="E62" r:id="rId6" location=":~:text=You%20can%20verify%20whether%20it,password%20and%20ESSID%20are%20correct." xr:uid="{3BA51E9E-8709-874E-B6EC-40074894ACA9}"/>
+    <hyperlink ref="E57" r:id="rId7" xr:uid="{30BD9D61-AAB4-2544-987A-0386CA068398}"/>
+    <hyperlink ref="E65" r:id="rId8" xr:uid="{1824F9BF-1BD9-3842-A565-00C06FF5E50F}"/>
+    <hyperlink ref="D136" r:id="rId9" xr:uid="{E488AECD-B504-A04E-8F27-807A3A08802C}"/>
+    <hyperlink ref="D90" r:id="rId10" location="89804" xr:uid="{E34C14F5-E723-0A48-894F-222B3F74BBF9}"/>
+    <hyperlink ref="D91" r:id="rId11" xr:uid="{6C20672B-9F8F-094F-9AC8-3D1FC1C85319}"/>
+    <hyperlink ref="D92" r:id="rId12" xr:uid="{BA9A8F05-4D7F-4942-886C-F8152208F0EA}"/>
+    <hyperlink ref="F96" r:id="rId13" xr:uid="{22AE585F-7255-3F41-8A2E-808446F3A9AA}"/>
+    <hyperlink ref="F98" r:id="rId14" xr:uid="{93472772-CF6C-D045-B634-2D574A3EE034}"/>
+    <hyperlink ref="E183" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
+    <hyperlink ref="F184" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
+    <hyperlink ref="D192" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
+    <hyperlink ref="D193" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
+    <hyperlink ref="F99" r:id="rId19" xr:uid="{92BE3560-5393-C545-9D2D-2B773359B28F}"/>
+    <hyperlink ref="E209" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
+    <hyperlink ref="E210" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
+    <hyperlink ref="E211" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
+    <hyperlink ref="E73" r:id="rId23" xr:uid="{1526D7DA-27DA-1443-928C-BEDA9E425734}"/>
+    <hyperlink ref="E74" r:id="rId24" xr:uid="{4F363062-BE49-AB4F-8956-2C1F31D9B898}"/>
+    <hyperlink ref="H100" r:id="rId25" xr:uid="{D9E13355-D59B-054F-B544-34A5A285A9E0}"/>
+    <hyperlink ref="G68" r:id="rId26" xr:uid="{170917BF-0643-9848-BCA9-A3BF5219EE3E}"/>
+    <hyperlink ref="F103" r:id="rId27" xr:uid="{5D45F2D3-11BC-6E43-BEFF-29E4E04A041E}"/>
+    <hyperlink ref="I104" r:id="rId28" xr:uid="{7D985D09-6A9A-FF4D-9F4A-4C56CC604DCE}"/>
+    <hyperlink ref="D93" r:id="rId29" xr:uid="{784C3F11-339F-8242-911D-6E4E893DD319}"/>
+    <hyperlink ref="E93" r:id="rId30" xr:uid="{FC907203-09BF-654B-9028-A8528783DAFE}"/>
+    <hyperlink ref="F105" r:id="rId31" xr:uid="{EFD3653A-B2F2-614F-8DEE-A2CB34111C94}"/>
+    <hyperlink ref="F106" r:id="rId32" xr:uid="{774B592D-11A5-9C49-BB9A-61014C8D8C81}"/>
+    <hyperlink ref="F107" r:id="rId33" xr:uid="{BD793670-4C63-C04D-B52D-974AF8E59FA4}"/>
+    <hyperlink ref="F108" r:id="rId34" location="96077" xr:uid="{B9804BBD-5312-714B-97EA-CC7D2C647F2C}"/>
+    <hyperlink ref="H101" r:id="rId35" xr:uid="{7BC5BAB5-D297-0043-BAAF-45AD255D5C84}"/>
+    <hyperlink ref="I100" r:id="rId36" xr:uid="{A03C56E4-1156-A148-A568-F50A5C33DB5C}"/>
+    <hyperlink ref="F109" r:id="rId37" xr:uid="{12AC219C-4678-4E43-B328-6595FA10B8D3}"/>
+    <hyperlink ref="E111" r:id="rId38" xr:uid="{44409621-28A2-704A-B283-3DCE1EFB1603}"/>
+    <hyperlink ref="E215" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
+    <hyperlink ref="F112" r:id="rId40" xr:uid="{A9D0D792-87D1-8144-872F-5CA060D3C28F}"/>
+    <hyperlink ref="F113" r:id="rId41" xr:uid="{87EF989D-17E9-1E45-A075-CD862D0B60F4}"/>
+    <hyperlink ref="F115" r:id="rId42" xr:uid="{8406C6F0-DC69-A64D-AAD8-60A33C12D00B}"/>
+    <hyperlink ref="F116" r:id="rId43" location="108593" xr:uid="{3C38F59E-6E71-4048-9BCA-CBC77D3907E0}"/>
+    <hyperlink ref="F118" r:id="rId44" xr:uid="{EEBE2A3E-36CA-F94F-9B1D-EE463DB6425F}"/>
+    <hyperlink ref="F119" r:id="rId45" xr:uid="{3782B43D-9E6F-2940-A013-34AA5D6B4DB3}"/>
+    <hyperlink ref="F120" r:id="rId46" xr:uid="{3D1C62DB-D9B7-BE42-B21D-4EEBC4C9EFE1}"/>
+    <hyperlink ref="F121" r:id="rId47" xr:uid="{F5021A21-70A2-D34E-B055-64CAC326E7EF}"/>
+    <hyperlink ref="F122" r:id="rId48" xr:uid="{A8C010A1-8EE1-264B-8688-3BEA1B62E535}"/>
+    <hyperlink ref="E216" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
+    <hyperlink ref="F117" r:id="rId50" location="113521" xr:uid="{EE1413C5-3B38-7D4D-8DF1-634A12F0BD81}"/>
+    <hyperlink ref="E75" r:id="rId51" xr:uid="{00B1EF4A-7791-0343-8D8C-9A1E83248FC9}"/>
+    <hyperlink ref="E277" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
+    <hyperlink ref="E278" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
+    <hyperlink ref="F124" r:id="rId54" xr:uid="{40A4B6A0-2F7E-A84D-8CC6-D814A33F5953}"/>
+    <hyperlink ref="E217" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
+    <hyperlink ref="E218" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
+    <hyperlink ref="E219" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
+    <hyperlink ref="E220" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
+    <hyperlink ref="E279" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
+    <hyperlink ref="D194" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
+    <hyperlink ref="D195" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
+    <hyperlink ref="D196" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
+    <hyperlink ref="E221" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
+    <hyperlink ref="E280" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
+    <hyperlink ref="E281" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
+    <hyperlink ref="E283" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
+    <hyperlink ref="E284" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
+    <hyperlink ref="F278" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
+    <hyperlink ref="G278" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
+    <hyperlink ref="E285" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
+    <hyperlink ref="E286" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
+    <hyperlink ref="E287" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
+    <hyperlink ref="E185" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
+    <hyperlink ref="E282" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
+    <hyperlink ref="E288" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
+    <hyperlink ref="E289" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
+    <hyperlink ref="E77" r:id="rId77" location="code" xr:uid="{C0475FF8-517D-E949-887E-9A42D86E9640}"/>
+    <hyperlink ref="E291" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
+    <hyperlink ref="E78" r:id="rId79" xr:uid="{277DBE6F-F3E5-8B4C-8DD8-BD92445D1A99}"/>
+    <hyperlink ref="E293" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
+    <hyperlink ref="E298" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
+    <hyperlink ref="E200" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
+    <hyperlink ref="E201" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
+    <hyperlink ref="F145" r:id="rId84" xr:uid="{EB604865-A16B-0646-A5B5-0D047467449D}"/>
+    <hyperlink ref="E223" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
+    <hyperlink ref="D307" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
+    <hyperlink ref="D308" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
+    <hyperlink ref="E317" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
+    <hyperlink ref="E318" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
+    <hyperlink ref="E316" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
+    <hyperlink ref="D327" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
+    <hyperlink ref="E333" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
+    <hyperlink ref="E330" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
+    <hyperlink ref="E334" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
+    <hyperlink ref="F325" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
+    <hyperlink ref="F326" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
+    <hyperlink ref="E328" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
+    <hyperlink ref="G330" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
+    <hyperlink ref="D343" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
+    <hyperlink ref="E335" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
+    <hyperlink ref="E338" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
+    <hyperlink ref="E337" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
+    <hyperlink ref="F242" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
+    <hyperlink ref="E243" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
+    <hyperlink ref="E244" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
+    <hyperlink ref="E245" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
+    <hyperlink ref="G259" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
+    <hyperlink ref="E254" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
+    <hyperlink ref="E255" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
+    <hyperlink ref="E260" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
+    <hyperlink ref="F152" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
+    <hyperlink ref="F157" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
+    <hyperlink ref="F158" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
+    <hyperlink ref="F164" r:id="rId114" xr:uid="{2B03B1F0-535A-3E4F-8FB3-35D2DE847218}"/>
+    <hyperlink ref="G169" r:id="rId115" xr:uid="{11045522-E183-B14C-B43D-5EA36E454600}"/>
+    <hyperlink ref="E186" r:id="rId116" xr:uid="{F1098A8C-3BC0-DB4F-8F9C-48B31145FEC1}"/>
+    <hyperlink ref="F171" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
+    <hyperlink ref="F165" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
+    <hyperlink ref="F174" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
+    <hyperlink ref="H238" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
+    <hyperlink ref="F350" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
+    <hyperlink ref="G364" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
+    <hyperlink ref="F351" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
+    <hyperlink ref="G366" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
+    <hyperlink ref="G368" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
+    <hyperlink ref="G371" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
+    <hyperlink ref="G375" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
+    <hyperlink ref="G383" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
+    <hyperlink ref="G381" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
+    <hyperlink ref="G386" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
+    <hyperlink ref="G392" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
+    <hyperlink ref="G396" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
+    <hyperlink ref="G401" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
+    <hyperlink ref="G406" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
+    <hyperlink ref="G411" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
+    <hyperlink ref="E20" r:id="rId136" xr:uid="{809CA2D1-39E9-0045-A4DF-E4C0C2E97FA2}"/>
+    <hyperlink ref="E21" r:id="rId137" xr:uid="{5DC44543-F2B9-F841-9097-6DB19C5EBD82}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips about ITerm split window and switch panels
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A019259B-1CF3-E143-9F4B-69F8C7340DD7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AD7B65-10C3-5C47-81D8-E8FE93E38B90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="560" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="611">
   <si>
     <t>docker</t>
   </si>
@@ -1826,6 +1826,51 @@
   </si>
   <si>
     <t>ssh-add -K ~/.ssh/[your-private-key]</t>
+  </si>
+  <si>
+    <t>Iterm</t>
+  </si>
+  <si>
+    <t>Create New Tab</t>
+  </si>
+  <si>
+    <t>Cmd T</t>
+  </si>
+  <si>
+    <t>Cmd N</t>
+  </si>
+  <si>
+    <t>Create New Window</t>
+  </si>
+  <si>
+    <t>Split window vertically</t>
+  </si>
+  <si>
+    <t>Cmd D</t>
+  </si>
+  <si>
+    <t>Split window horizontally</t>
+  </si>
+  <si>
+    <t>Shift + Cmd + D</t>
+  </si>
+  <si>
+    <t>Switch Tabs</t>
+  </si>
+  <si>
+    <t>Cmd + left/right arrow</t>
+  </si>
+  <si>
+    <t>Switch Panels</t>
+  </si>
+  <si>
+    <t>Cmd + alt + left/right arrow</t>
+  </si>
+  <si>
+    <t>Cmd + [/]</t>
+  </si>
+  <si>
+    <t>https://apple.stackexchange.com/questions/114177/iterm-whats-the-key-combo-to-switch-panes</t>
   </si>
 </sst>
 </file>
@@ -2287,11 +2332,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I414"/>
+  <dimension ref="B1:I425"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <pane ySplit="1" topLeftCell="A399" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G416" sqref="G416"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4617,46 +4662,105 @@
         <v>579</v>
       </c>
     </row>
+    <row r="408" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C408" t="s">
+        <v>596</v>
+      </c>
+    </row>
     <row r="409" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B409" t="s">
+      <c r="D409" t="s">
+        <v>597</v>
+      </c>
+      <c r="E409" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="410" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D410" t="s">
+        <v>600</v>
+      </c>
+      <c r="E410" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="412" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D412" t="s">
+        <v>601</v>
+      </c>
+      <c r="E412" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="413" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D413" t="s">
+        <v>603</v>
+      </c>
+      <c r="E413" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="415" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D415" t="s">
+        <v>605</v>
+      </c>
+      <c r="E415" t="s">
+        <v>606</v>
+      </c>
+      <c r="G415" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="416" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D416" t="s">
+        <v>607</v>
+      </c>
+      <c r="E416" t="s">
+        <v>608</v>
+      </c>
+      <c r="F416" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="420" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B420" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="410" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C410" t="s">
+    <row r="421" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C421" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="411" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D411" t="s">
+    <row r="422" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D422" t="s">
         <v>583</v>
       </c>
-      <c r="E411" t="s">
+      <c r="E422" t="s">
         <v>584</v>
       </c>
-      <c r="F411" t="s">
+      <c r="F422" t="s">
         <v>582</v>
       </c>
-      <c r="G411" s="1" t="s">
+      <c r="G422" s="1" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="412" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E412" t="s">
+    <row r="423" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E423" t="s">
         <v>585</v>
       </c>
-      <c r="F412" t="s">
+      <c r="F423" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="414" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D414" t="s">
+    <row r="425" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D425" t="s">
         <v>588</v>
       </c>
-      <c r="E414" t="s">
+      <c r="E425" t="s">
         <v>590</v>
       </c>
-      <c r="F414" t="s">
+      <c r="F425" t="s">
         <v>589</v>
       </c>
     </row>
@@ -4796,9 +4900,10 @@
     <hyperlink ref="G396" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
     <hyperlink ref="G401" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
     <hyperlink ref="G406" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
-    <hyperlink ref="G411" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
+    <hyperlink ref="G422" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
     <hyperlink ref="E20" r:id="rId136" xr:uid="{809CA2D1-39E9-0045-A4DF-E4C0C2E97FA2}"/>
     <hyperlink ref="E21" r:id="rId137" xr:uid="{5DC44543-F2B9-F841-9097-6DB19C5EBD82}"/>
+    <hyperlink ref="G415" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added more tips about pandas and timescaledb
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AD7B65-10C3-5C47-81D8-E8FE93E38B90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6036B1-377D-7641-A356-1333EEB860AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="560" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="25600" windowHeight="15340" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="670">
   <si>
     <t>docker</t>
   </si>
@@ -1871,6 +1871,184 @@
   </si>
   <si>
     <t>https://apple.stackexchange.com/questions/114177/iterm-whats-the-key-combo-to-switch-panes</t>
+  </si>
+  <si>
+    <t>Fix Legacy Parser Warning for snipMate</t>
+  </si>
+  <si>
+    <t>Add the following code to ~/.vimrc</t>
+  </si>
+  <si>
+    <t>let g:snipMate = { 'snippet_version' : 1 }</t>
+  </si>
+  <si>
+    <t>https://www.wiserfirst.com/blog/vim-tip-snipmate-legacy-parser-warning/</t>
+  </si>
+  <si>
+    <t>df1['HS_FIRST_NAME'] = df[4].sample(frac=1).values</t>
+  </si>
+  <si>
+    <t>Shuffle one column in pandas dataframe</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/54009400/shuffle-one-column-in-pandas-dataframe</t>
+  </si>
+  <si>
+    <t>Edit the legend in plot</t>
+  </si>
+  <si>
+    <t>ax.plot([1, 2, 3], label='Inline label')</t>
+  </si>
+  <si>
+    <t>https://matplotlib.org/stable/api/_as_gen/matplotlib.pyplot.legend.html</t>
+  </si>
+  <si>
+    <t>plt.gca().set_aspect('equal', adjustable='box')</t>
+  </si>
+  <si>
+    <t>equalize the scales of x-axis and y-axis in matplotlib</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/17990845/how-to-equalize-the-scales-of-x-axis-and-y-axis-in-matplotlib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apply function with multiple columns </t>
+  </si>
+  <si>
+    <t>df.apply(lambda x: x.a+x.b, axis = 1)</t>
+  </si>
+  <si>
+    <t>https://www.delftstack.com/howto/python-pandas/pandas-apply-multiple-columns/</t>
+  </si>
+  <si>
+    <t>new_df = pd.DataFrame(list(original['user']))</t>
+  </si>
+  <si>
+    <t>transfer pandas series with dict element to dataframe</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/29681906/python-pandas-dataframe-from-series-of-dict</t>
+  </si>
+  <si>
+    <t>df.set_index(['number','class'])</t>
+  </si>
+  <si>
+    <t>Set multi column index</t>
+  </si>
+  <si>
+    <t>Basic commands</t>
+  </si>
+  <si>
+    <t>1. List databases</t>
+  </si>
+  <si>
+    <t>\l</t>
+  </si>
+  <si>
+    <t>2. help</t>
+  </si>
+  <si>
+    <t>\?</t>
+  </si>
+  <si>
+    <t>3. connect to databases</t>
+  </si>
+  <si>
+    <t>\c name_of_database</t>
+  </si>
+  <si>
+    <t>\dt</t>
+  </si>
+  <si>
+    <t>4. List tables</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/62105409/automatically-print-the-next-line-variable-for-debugging-purpose</t>
+  </si>
+  <si>
+    <t>Automatically print the next line variable for debugging purpose\</t>
+  </si>
+  <si>
+    <t>from inspect import currentframe, getsourcelines</t>
+  </si>
+  <si>
+    <t>How to retrieve source code of Python functions</t>
+  </si>
+  <si>
+    <t>source_DF = inspect.getsource(pandas.DataFrame)</t>
+  </si>
+  <si>
+    <t>https://opensource.com/article/18/5/how-retrieve-source-code-python-functions</t>
+  </si>
+  <si>
+    <t>Install python packages manually</t>
+  </si>
+  <si>
+    <t>python setup.py install --user</t>
+  </si>
+  <si>
+    <t>https://scicomp.stackexchange.com/questions/2987/what-is-the-simplest-way-to-do-a-user-local-install-of-a-python-package</t>
+  </si>
+  <si>
+    <t>vim</t>
+  </si>
+  <si>
+    <t>latex</t>
+  </si>
+  <si>
+    <t>set mapleader</t>
+  </si>
+  <si>
+    <t>:let mapleader = ","</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/1764263/what-is-the-leader-in-a-vimrc-file</t>
+  </si>
+  <si>
+    <t>pandas' version of join</t>
+  </si>
+  <si>
+    <t>pd.merge()</t>
+  </si>
+  <si>
+    <t>https://pandas.pydata.org/pandas-docs/stable/user_guide/merging.html</t>
+  </si>
+  <si>
+    <t>Python Timer Functions: Three Ways to Monitor Your Code</t>
+  </si>
+  <si>
+    <t>https://realpython.com/python-timer/</t>
+  </si>
+  <si>
+    <t>with Timer("some_name"): do_something()</t>
+  </si>
+  <si>
+    <t>cd project_folder
+pip install [-e] .</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/43816791/importing-from-python-modules-inside-parent-directory-into-jupyter-notebook-file</t>
+  </si>
+  <si>
+    <t>Doing the opposite of pivot in pandas Python</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/48135994/doing-the-opposite-of-pivot-in-pandas-python</t>
+  </si>
+  <si>
+    <t>df.set_index('Date').stack().reset_index(name='Val').rename(columns={'level_1':'X'})</t>
+  </si>
+  <si>
+    <t>install python library</t>
+  </si>
+  <si>
+    <t>change pandas nano to postgresdb null</t>
+  </si>
+  <si>
+    <t>df.where(pd.notnull(df), None)</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/32107558/how-do-i-convert-numpy-nan-objects-to-sql-nulls</t>
   </si>
 </sst>
 </file>
@@ -2332,17 +2510,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I425"/>
+  <dimension ref="B1:I461"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A399" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G416" sqref="G416"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A380" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D401" sqref="D401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19.1640625" customWidth="1"/>
-    <col min="3" max="3" width="35.33203125" customWidth="1"/>
+    <col min="3" max="3" width="45.33203125" customWidth="1"/>
     <col min="4" max="4" width="43.33203125" customWidth="1"/>
     <col min="5" max="5" width="26.83203125" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
@@ -3499,1268 +3677,1430 @@
     <row r="188" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F188" s="1"/>
     </row>
+    <row r="189" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C189" t="s">
+        <v>618</v>
+      </c>
+      <c r="D189" t="s">
+        <v>619</v>
+      </c>
+      <c r="F189" s="1" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="190" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C190" t="s">
+        <v>622</v>
+      </c>
+      <c r="D190" t="s">
+        <v>621</v>
+      </c>
+      <c r="F190" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
     <row r="191" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B191" t="s">
+      <c r="F191" s="1"/>
+    </row>
+    <row r="192" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F192" s="1"/>
+    </row>
+    <row r="193" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F193" s="1"/>
+    </row>
+    <row r="194" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F194" s="1"/>
+    </row>
+    <row r="196" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B196" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="197" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C197" t="s">
+        <v>616</v>
+      </c>
+      <c r="D197" t="s">
+        <v>615</v>
+      </c>
+      <c r="F197" s="1" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="198" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C198" t="s">
+        <v>624</v>
+      </c>
+      <c r="D198" t="s">
+        <v>625</v>
+      </c>
+      <c r="F198" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="199" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C199" t="s">
+        <v>628</v>
+      </c>
+      <c r="D199" t="s">
+        <v>627</v>
+      </c>
+      <c r="F199" s="1" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="200" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C200" t="s">
+        <v>631</v>
+      </c>
+      <c r="D200" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="207" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B207" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="192" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C192" t="s">
+    <row r="208" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C208" t="s">
         <v>176</v>
       </c>
-      <c r="D192" s="1" t="s">
+      <c r="D208" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="193" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C193" t="s">
+    <row r="209" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C209" t="s">
         <v>178</v>
       </c>
-      <c r="D193" s="1" t="s">
+      <c r="D209" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="194" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C194" t="s">
+    <row r="210" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C210" t="s">
         <v>293</v>
       </c>
-      <c r="D194" s="1" t="s">
+      <c r="D210" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="195" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C195" t="s">
+    <row r="211" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C211" t="s">
         <v>294</v>
       </c>
-      <c r="D195" s="1" t="s">
+      <c r="D211" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="196" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C196" t="s">
+    <row r="212" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C212" t="s">
         <v>297</v>
       </c>
-      <c r="D196" s="1" t="s">
+      <c r="D212" s="1" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="197" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D197" s="1"/>
-    </row>
-    <row r="198" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D198" s="1"/>
-    </row>
-    <row r="199" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B199" t="s">
+    <row r="213" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D213" s="1"/>
+    </row>
+    <row r="214" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D214" s="1"/>
+    </row>
+    <row r="215" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B215" t="s">
         <v>343</v>
       </c>
-      <c r="D199" s="1"/>
-    </row>
-    <row r="200" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C200" t="s">
+      <c r="D215" s="1"/>
+    </row>
+    <row r="216" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C216" t="s">
         <v>344</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D216" t="s">
         <v>369</v>
       </c>
-      <c r="E200" s="1" t="s">
+      <c r="E216" s="1" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="201" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D201" t="s">
+    <row r="217" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D217" t="s">
         <v>368</v>
       </c>
-      <c r="E201" s="1" t="s">
+      <c r="E217" s="1" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="202" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D202" s="1"/>
-    </row>
-    <row r="203" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D203" s="1"/>
-    </row>
-    <row r="204" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D204" s="1"/>
-    </row>
-    <row r="208" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B208" t="s">
+    <row r="218" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D218" s="1"/>
+    </row>
+    <row r="219" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D219" s="1"/>
+    </row>
+    <row r="220" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D220" s="1"/>
+    </row>
+    <row r="224" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B224" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="209" spans="3:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="C209" s="4" t="s">
+    <row r="225" spans="3:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="C225" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D209" s="2" t="s">
+      <c r="D225" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E209" s="1" t="s">
+      <c r="E225" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="210" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C210" t="s">
+    <row r="226" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C226" t="s">
         <v>187</v>
       </c>
-      <c r="E210" s="1" t="s">
+      <c r="E226" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="211" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C211" t="s">
+    <row r="227" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C227" t="s">
         <v>215</v>
       </c>
-      <c r="E211" s="1" t="s">
+      <c r="E227" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="213" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D213" t="s">
+    <row r="229" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D229" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="215" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C215" t="s">
+    <row r="231" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C231" t="s">
         <v>242</v>
       </c>
-      <c r="D215" t="s">
+      <c r="D231" t="s">
         <v>243</v>
       </c>
-      <c r="E215" s="1" t="s">
+      <c r="E231" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="216" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C216" t="s">
+    <row r="232" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C232" t="s">
         <v>269</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D232" t="s">
         <v>270</v>
       </c>
-      <c r="E216" s="1" t="s">
+      <c r="E232" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="217" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C217" t="s">
+    <row r="233" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C233" t="s">
         <v>284</v>
       </c>
-      <c r="E217" s="1" t="s">
+      <c r="E233" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="218" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E218" s="1" t="s">
+    <row r="234" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E234" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="219" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E219" s="1" t="s">
+    <row r="235" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E235" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="220" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C220" t="s">
+    <row r="236" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C236" t="s">
         <v>288</v>
       </c>
-      <c r="E220" s="1" t="s">
+      <c r="E236" s="1" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="221" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C221" t="s">
+    <row r="237" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C237" t="s">
         <v>299</v>
       </c>
-      <c r="E221" s="1" t="s">
+      <c r="E237" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="222" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E222" s="1"/>
-    </row>
-    <row r="223" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C223" t="s">
+    <row r="238" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E238" s="1"/>
+    </row>
+    <row r="239" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C239" t="s">
         <v>359</v>
       </c>
-      <c r="D223" t="s">
+      <c r="D239" t="s">
         <v>360</v>
       </c>
-      <c r="E223" s="1" t="s">
+      <c r="E239" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="224" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E224" s="1"/>
-    </row>
-    <row r="225" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E225" s="1"/>
-    </row>
-    <row r="226" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E226" s="1"/>
-    </row>
-    <row r="227" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E227" s="1"/>
-    </row>
-    <row r="228" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E228" s="1"/>
-    </row>
-    <row r="229" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E229" s="1"/>
-    </row>
-    <row r="230" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E230" s="1"/>
-    </row>
-    <row r="231" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E231" s="1"/>
-    </row>
-    <row r="232" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C232" t="s">
+    <row r="240" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E240" s="1"/>
+    </row>
+    <row r="241" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E241" s="1"/>
+    </row>
+    <row r="242" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E242" s="1"/>
+    </row>
+    <row r="243" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E243" s="1"/>
+    </row>
+    <row r="244" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E244" s="1"/>
+    </row>
+    <row r="245" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E245" s="1"/>
+    </row>
+    <row r="246" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E246" s="1"/>
+    </row>
+    <row r="247" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E247" s="1"/>
+    </row>
+    <row r="248" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C248" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="233" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D233" t="s">
+    <row r="249" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D249" t="s">
         <v>135</v>
       </c>
-      <c r="E233" t="s">
+      <c r="E249" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="234" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D234" t="s">
+    <row r="250" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D250" t="s">
         <v>136</v>
       </c>
-      <c r="E234" t="s">
+      <c r="E250" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="235" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D235" t="s">
+    <row r="251" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D251" t="s">
         <v>140</v>
       </c>
-      <c r="E235" t="s">
+      <c r="E251" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="236" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D236" t="s">
+    <row r="252" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D252" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="237" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D237" t="s">
+    <row r="253" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D253" t="s">
         <v>142</v>
       </c>
-      <c r="E237" t="s">
+      <c r="E253" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="238" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D238" t="s">
+    <row r="254" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D254" t="s">
         <v>484</v>
       </c>
-      <c r="E238" t="s">
+      <c r="E254" t="s">
         <v>486</v>
       </c>
-      <c r="F238" t="s">
+      <c r="F254" t="s">
         <v>490</v>
       </c>
-      <c r="G238" t="s">
+      <c r="G254" t="s">
         <v>485</v>
       </c>
-      <c r="H238" s="1" t="s">
+      <c r="H254" s="1" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="239" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D239" t="s">
+    <row r="255" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D255" t="s">
         <v>487</v>
       </c>
-      <c r="E239" t="s">
+      <c r="E255" t="s">
         <v>488</v>
       </c>
-      <c r="G239" t="s">
+      <c r="G255" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="241" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C241" t="s">
+    <row r="257" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C257" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="242" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D242" t="s">
+    <row r="258" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D258" t="s">
         <v>73</v>
       </c>
-      <c r="E242" t="s">
+      <c r="E258" t="s">
         <v>74</v>
       </c>
-      <c r="F242" s="1" t="s">
+      <c r="F258" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="243" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D243" t="s">
+    <row r="259" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D259" t="s">
         <v>76</v>
       </c>
-      <c r="E243" s="1" t="s">
+      <c r="E259" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="244" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D244" t="s">
+    <row r="260" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D260" t="s">
         <v>78</v>
       </c>
-      <c r="E244" s="1" t="s">
+      <c r="E260" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="245" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D245" t="s">
+    <row r="261" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D261" t="s">
         <v>81</v>
       </c>
-      <c r="E245" s="1" t="s">
+      <c r="E261" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="246" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D246" t="s">
+    <row r="262" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D262" t="s">
         <v>362</v>
       </c>
-      <c r="E246" t="s">
+      <c r="E262" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="247" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D247" t="s">
+    <row r="263" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D263" t="s">
         <v>363</v>
       </c>
-      <c r="E247" t="s">
+      <c r="E263" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="249" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D249" t="s">
+    <row r="265" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D265" t="s">
         <v>82</v>
       </c>
-      <c r="E249" t="s">
+      <c r="E265" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="250" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D250" t="s">
+    <row r="266" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D266" t="s">
         <v>84</v>
       </c>
-      <c r="E250" t="s">
+      <c r="E266" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="252" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C252" t="s">
+    <row r="268" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C268" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="253" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D253" t="s">
+    <row r="269" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D269" t="s">
         <v>73</v>
       </c>
-      <c r="E253" t="s">
+      <c r="E269" t="s">
         <v>131</v>
       </c>
-      <c r="F253" s="1"/>
-    </row>
-    <row r="254" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D254" t="s">
+      <c r="F269" s="1"/>
+    </row>
+    <row r="270" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D270" t="s">
         <v>147</v>
       </c>
-      <c r="E254" s="1" t="s">
+      <c r="E270" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F254" s="1"/>
-    </row>
-    <row r="255" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D255" t="s">
+      <c r="F270" s="1"/>
+    </row>
+    <row r="271" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D271" t="s">
         <v>76</v>
       </c>
-      <c r="E255" s="1" t="s">
+      <c r="E271" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="256" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E256" s="1"/>
-    </row>
-    <row r="257" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D257" t="s">
+    <row r="272" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="E272" s="1"/>
+    </row>
+    <row r="273" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D273" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="258" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E258" t="s">
+    <row r="274" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E274" t="s">
         <v>151</v>
       </c>
-      <c r="F258" t="s">
+      <c r="F274" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="259" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E259" t="s">
+    <row r="275" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E275" t="s">
         <v>152</v>
       </c>
-      <c r="F259" t="s">
+      <c r="F275" t="s">
         <v>145</v>
       </c>
-      <c r="G259" s="1" t="s">
+      <c r="G275" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="260" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D260" t="s">
+    <row r="276" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D276" t="s">
         <v>153</v>
       </c>
-      <c r="E260" s="1" t="s">
+      <c r="E276" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G260" s="1"/>
-    </row>
-    <row r="274" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E274" s="1"/>
-    </row>
-    <row r="276" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B276" t="s">
+      <c r="G276" s="1"/>
+    </row>
+    <row r="290" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E290" s="1"/>
+    </row>
+    <row r="292" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B292" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="277" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C277" t="s">
+    <row r="293" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C293" t="s">
         <v>277</v>
       </c>
-      <c r="D277" t="s">
+      <c r="D293" t="s">
         <v>279</v>
       </c>
-      <c r="E277" s="1" t="s">
+      <c r="E293" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="278" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C278" t="s">
+    <row r="294" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C294" t="s">
         <v>281</v>
       </c>
-      <c r="E278" s="1" t="s">
+      <c r="E294" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="F278" s="1" t="s">
+      <c r="F294" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="G278" s="1" t="s">
+      <c r="G294" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="279" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C279" t="s">
+    <row r="295" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C295" t="s">
         <v>290</v>
       </c>
-      <c r="E279" s="1" t="s">
+      <c r="E295" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="280" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C280" t="s">
+    <row r="296" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C296" t="s">
         <v>304</v>
       </c>
-      <c r="E280" s="1" t="s">
+      <c r="E296" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="281" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D281" t="s">
+    <row r="297" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D297" t="s">
         <v>306</v>
       </c>
-      <c r="E281" s="1" t="s">
+      <c r="E297" s="1" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="282" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C282" t="s">
+    <row r="298" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C298" t="s">
         <v>324</v>
       </c>
-      <c r="E282" s="1" t="s">
+      <c r="E298" s="1" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="283" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C283" t="s">
+    <row r="299" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C299" t="s">
         <v>308</v>
       </c>
-      <c r="D283" t="s">
+      <c r="D299" t="s">
         <v>309</v>
       </c>
-      <c r="E283" s="1" t="s">
+      <c r="E299" s="1" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="284" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C284" t="s">
+    <row r="300" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C300" t="s">
         <v>311</v>
       </c>
-      <c r="E284" s="1" t="s">
+      <c r="E300" s="1" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="285" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C285" t="s">
+    <row r="301" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C301" t="s">
         <v>316</v>
       </c>
-      <c r="E285" s="1" t="s">
+      <c r="E301" s="1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="286" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C286" t="s">
+    <row r="302" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C302" t="s">
         <v>317</v>
       </c>
-      <c r="E286" s="1" t="s">
+      <c r="E302" s="1" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="287" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C287" t="s">
+    <row r="303" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C303" t="s">
         <v>319</v>
       </c>
-      <c r="E287" s="1" t="s">
+      <c r="E303" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="288" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C288" t="s">
+    <row r="304" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C304" t="s">
         <v>326</v>
       </c>
-      <c r="D288" t="s">
+      <c r="D304" t="s">
         <v>333</v>
       </c>
-      <c r="E288" s="1" t="s">
+      <c r="E304" s="1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="289" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D289" t="s">
+    <row r="305" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D305" t="s">
         <v>328</v>
       </c>
-      <c r="E289" s="1" t="s">
+      <c r="E305" s="1" t="s">
         <v>327</v>
-      </c>
-    </row>
-    <row r="291" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C291" t="s">
-        <v>330</v>
-      </c>
-      <c r="D291" t="s">
-        <v>331</v>
-      </c>
-      <c r="E291" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="293" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C293" t="s">
-        <v>336</v>
-      </c>
-      <c r="D293" t="s">
-        <v>338</v>
-      </c>
-      <c r="E293" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="297" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B297" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="298" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C298" t="s">
-        <v>342</v>
-      </c>
-      <c r="D298" t="s">
-        <v>340</v>
-      </c>
-      <c r="E298" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="304" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B304" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="305" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C305" t="s">
-        <v>87</v>
-      </c>
-      <c r="D305" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="306" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C306" t="s">
-        <v>89</v>
-      </c>
-      <c r="D306" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="307" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C307" t="s">
+        <v>330</v>
+      </c>
+      <c r="D307" t="s">
+        <v>331</v>
+      </c>
+      <c r="E307" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="309" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C309" t="s">
+        <v>336</v>
+      </c>
+      <c r="D309" t="s">
+        <v>338</v>
+      </c>
+      <c r="E309" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="313" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B313" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="314" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C314" t="s">
+        <v>342</v>
+      </c>
+      <c r="D314" t="s">
+        <v>340</v>
+      </c>
+      <c r="E314" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="320" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B320" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="321" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C321" t="s">
+        <v>87</v>
+      </c>
+      <c r="D321" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="322" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C322" t="s">
+        <v>89</v>
+      </c>
+      <c r="D322" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="323" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C323" t="s">
         <v>96</v>
       </c>
-      <c r="D307" s="1" t="s">
+      <c r="D323" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="308" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C308" t="s">
+    <row r="324" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C324" t="s">
         <v>98</v>
       </c>
-      <c r="D308" s="1" t="s">
+      <c r="D324" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="310" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B310" t="s">
+    <row r="326" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B326" t="s">
         <v>91</v>
       </c>
-      <c r="C310" t="s">
+      <c r="C326" t="s">
         <v>92</v>
       </c>
-      <c r="D310" t="s">
+      <c r="D326" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="311" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C311" t="s">
+    <row r="327" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C327" t="s">
         <v>94</v>
       </c>
-      <c r="D311" t="s">
+      <c r="D327" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="314" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B314" t="s">
+    <row r="330" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B330" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="315" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C315" t="s">
+    <row r="331" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C331" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="316" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D316" t="s">
+    <row r="332" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D332" t="s">
         <v>105</v>
       </c>
-      <c r="E316" s="1" t="s">
+      <c r="E332" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="317" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D317" t="s">
+    <row r="333" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D333" t="s">
         <v>102</v>
       </c>
-      <c r="E317" s="1" t="s">
+      <c r="E333" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="318" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D318" t="s">
+    <row r="334" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D334" t="s">
         <v>103</v>
       </c>
-      <c r="E318" s="1" t="s">
+      <c r="E334" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="319" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D319" t="s">
+    <row r="335" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D335" t="s">
         <v>108</v>
       </c>
-      <c r="E319" t="s">
+      <c r="E335" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="321" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B321" t="s">
+    <row r="337" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B337" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="322" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C322" t="s">
+    <row r="338" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C338" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="323" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D323" t="s">
+    <row r="339" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D339" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="324" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D324" t="s">
+    <row r="340" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D340" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="325" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F325" s="1" t="s">
+    <row r="341" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F341" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="326" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B326" t="s">
+    <row r="342" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B342" t="s">
         <v>1</v>
       </c>
-      <c r="F326" s="1" t="s">
+      <c r="F342" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="327" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C327" t="s">
+    <row r="343" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C343" t="s">
         <v>113</v>
       </c>
-      <c r="D327" s="1" t="s">
+      <c r="D343" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="328" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D328" t="s">
+    <row r="344" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D344" t="s">
         <v>127</v>
       </c>
-      <c r="E328" s="1" t="s">
+      <c r="E344" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="329" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C329" t="s">
+    <row r="345" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C345" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="330" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D330" t="s">
+    <row r="346" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D346" t="s">
         <v>116</v>
       </c>
-      <c r="E330" s="1" t="s">
+      <c r="E346" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F330" t="s">
+      <c r="F346" t="s">
         <v>129</v>
       </c>
-      <c r="G330" s="1" t="s">
+      <c r="G346" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="331" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E331" t="s">
+    <row r="347" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E347" t="s">
         <v>122</v>
       </c>
-      <c r="G331" s="1"/>
-    </row>
-    <row r="332" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E332" t="s">
+      <c r="G347" s="1"/>
+    </row>
+    <row r="348" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E348" t="s">
         <v>125</v>
       </c>
-      <c r="G332" s="1"/>
-    </row>
-    <row r="333" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D333" t="s">
+      <c r="G348" s="1"/>
+    </row>
+    <row r="349" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D349" t="s">
         <v>118</v>
       </c>
-      <c r="E333" s="1" t="s">
+      <c r="E349" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G333" s="1"/>
-    </row>
-    <row r="334" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D334" t="s">
+      <c r="G349" s="1"/>
+    </row>
+    <row r="350" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D350" t="s">
         <v>120</v>
       </c>
-      <c r="E334" s="1" t="s">
+      <c r="E350" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G334" s="1"/>
-    </row>
-    <row r="335" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E335" s="1" t="s">
+      <c r="G350" s="1"/>
+    </row>
+    <row r="351" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E351" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="G335" s="1"/>
-    </row>
-    <row r="336" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E336" t="s">
+      <c r="G351" s="1"/>
+    </row>
+    <row r="352" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E352" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="337" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D337" t="s">
+    <row r="353" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D353" t="s">
         <v>302</v>
       </c>
-      <c r="E337" s="1" t="s">
+      <c r="E353" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="338" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D338" t="s">
+    <row r="354" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D354" t="s">
         <v>301</v>
       </c>
-      <c r="E338" s="1" t="s">
+      <c r="E354" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="343" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C343" t="s">
+    <row r="359" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C359" t="s">
         <v>132</v>
       </c>
-      <c r="D343" s="1" t="s">
+      <c r="D359" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="347" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B347" t="s">
+    <row r="363" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B363" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="348" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C348" t="s">
+    <row r="364" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C364" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="349" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D349" t="s">
+    <row r="365" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D365" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="350" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E350" t="s">
+    <row r="366" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E366" t="s">
         <v>494</v>
       </c>
-      <c r="F350" s="1" t="s">
+      <c r="F366" s="1" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="351" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E351" t="s">
+    <row r="367" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E367" t="s">
         <v>496</v>
       </c>
-      <c r="F351" s="1" t="s">
+      <c r="F367" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="352" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E352" t="s">
+    <row r="368" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E368" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="353" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D353" t="s">
+    <row r="369" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D369" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="354" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E354" t="s">
+    <row r="370" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E370" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="355" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E355" t="s">
+    <row r="371" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E371" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="356" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D356" t="s">
+    <row r="372" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D372" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="357" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E357" t="s">
+    <row r="373" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E373" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="358" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C358" t="s">
+    <row r="374" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C374" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="359" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D359" t="s">
+    <row r="375" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D375" t="s">
         <v>505</v>
       </c>
-      <c r="E359" t="s">
+      <c r="E375" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="360" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D360" t="s">
+    <row r="376" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D376" t="s">
         <v>503</v>
       </c>
-      <c r="E360" t="s">
+      <c r="E376" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="362" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C362" t="s">
+    <row r="378" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C378" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="363" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D363" t="s">
+    <row r="379" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D379" t="s">
         <v>510</v>
       </c>
-      <c r="E363" t="s">
+      <c r="E379" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="364" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D364" t="s">
+    <row r="380" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D380" t="s">
         <v>511</v>
       </c>
-      <c r="E364" t="s">
+      <c r="E380" t="s">
         <v>509</v>
       </c>
-      <c r="G364" s="1" t="s">
+      <c r="G380" s="1" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="366" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C366" t="s">
+    <row r="382" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C382" t="s">
         <v>514</v>
       </c>
-      <c r="G366" s="1" t="s">
+      <c r="G382" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="368" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C368" t="s">
+    <row r="384" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C384" t="s">
         <v>515</v>
       </c>
-      <c r="E368" t="s">
+      <c r="E384" t="s">
         <v>516</v>
       </c>
-      <c r="G368" s="1" t="s">
+      <c r="G384" s="1" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="370" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C370" t="s">
+    <row r="386" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C386" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="371" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D371" t="s">
+    <row r="387" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D387" t="s">
         <v>520</v>
       </c>
-      <c r="E371" t="s">
+      <c r="E387" t="s">
         <v>519</v>
       </c>
-      <c r="G371" s="1" t="s">
+      <c r="G387" s="1" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="372" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D372" t="s">
+    <row r="388" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D388" t="s">
         <v>521</v>
       </c>
-      <c r="E372" t="s">
+      <c r="E388" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="374" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C374" t="s">
+    <row r="390" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C390" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="375" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D375" t="s">
+    <row r="391" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D391" t="s">
         <v>530</v>
       </c>
-      <c r="E375" t="s">
+      <c r="E391" t="s">
         <v>526</v>
       </c>
-      <c r="G375" s="1" t="s">
+      <c r="G391" s="1" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="376" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D376" t="s">
+    <row r="392" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D392" t="s">
         <v>528</v>
       </c>
-      <c r="E376" t="s">
+      <c r="E392" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="377" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D377" t="s">
+    <row r="393" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D393" t="s">
         <v>529</v>
       </c>
-      <c r="E377" t="s">
+      <c r="E393" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="379" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B379" t="s">
+    <row r="394" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C394" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="395" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D395" t="s">
+        <v>633</v>
+      </c>
+      <c r="E395" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="396" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D396" t="s">
+        <v>635</v>
+      </c>
+      <c r="E396" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="397" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D397" t="s">
+        <v>637</v>
+      </c>
+      <c r="E397" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="398" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D398" t="s">
+        <v>640</v>
+      </c>
+      <c r="E398" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="400" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C400" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="401" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D401">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="407" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B407" t="s">
         <v>541</v>
-      </c>
-    </row>
-    <row r="380" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C380" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="381" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D381" t="s">
-        <v>543</v>
-      </c>
-      <c r="G381" s="1" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="382" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C382" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="383" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D383" t="s">
-        <v>545</v>
-      </c>
-      <c r="E383" t="s">
-        <v>546</v>
-      </c>
-      <c r="G383" s="1" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="385" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C385" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="386" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D386" t="s">
-        <v>550</v>
-      </c>
-      <c r="E386" t="s">
-        <v>551</v>
-      </c>
-      <c r="G386" s="1" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="387" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D387" t="s">
-        <v>552</v>
-      </c>
-      <c r="E387" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="388" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D388" t="s">
-        <v>554</v>
-      </c>
-      <c r="E388" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="389" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D389" t="s">
-        <v>556</v>
-      </c>
-      <c r="E389" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="391" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C391" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="392" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D392" t="s">
-        <v>560</v>
-      </c>
-      <c r="E392" t="s">
-        <v>562</v>
-      </c>
-      <c r="G392" s="1" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="393" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D393" t="s">
-        <v>561</v>
-      </c>
-      <c r="E393" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="395" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C395" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="396" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D396" t="s">
-        <v>567</v>
-      </c>
-      <c r="G396" s="1" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="399" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B399" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="400" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C400" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="401" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E401" t="s">
-        <v>570</v>
-      </c>
-      <c r="G401" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="404" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B404" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="405" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C405" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="406" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D406" t="s">
-        <v>574</v>
-      </c>
-      <c r="E406" t="s">
-        <v>575</v>
-      </c>
-      <c r="F406" t="s">
-        <v>576</v>
-      </c>
-      <c r="G406" s="1" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="407" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E407" t="s">
-        <v>578</v>
-      </c>
-      <c r="F407" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="408" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C408" t="s">
-        <v>596</v>
+        <v>542</v>
       </c>
     </row>
     <row r="409" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D409" t="s">
-        <v>597</v>
-      </c>
-      <c r="E409" t="s">
-        <v>598</v>
+        <v>543</v>
+      </c>
+      <c r="G409" s="1" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="410" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D410" t="s">
-        <v>600</v>
-      </c>
-      <c r="E410" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="412" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D412" t="s">
-        <v>601</v>
-      </c>
-      <c r="E412" t="s">
-        <v>602</v>
+      <c r="C410" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="411" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D411" t="s">
+        <v>545</v>
+      </c>
+      <c r="E411" t="s">
+        <v>546</v>
+      </c>
+      <c r="G411" s="1" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="413" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D413" t="s">
-        <v>603</v>
-      </c>
-      <c r="E413" t="s">
-        <v>604</v>
+      <c r="C413" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="414" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D414" t="s">
+        <v>550</v>
+      </c>
+      <c r="E414" t="s">
+        <v>551</v>
+      </c>
+      <c r="G414" s="1" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="415" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D415" t="s">
-        <v>605</v>
+        <v>552</v>
       </c>
       <c r="E415" t="s">
-        <v>606</v>
-      </c>
-      <c r="G415" s="1" t="s">
-        <v>610</v>
+        <v>553</v>
       </c>
     </row>
     <row r="416" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D416" t="s">
+        <v>554</v>
+      </c>
+      <c r="E416" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="417" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D417" t="s">
+        <v>556</v>
+      </c>
+      <c r="E417" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="419" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C419" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="420" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D420" t="s">
+        <v>560</v>
+      </c>
+      <c r="E420" t="s">
+        <v>562</v>
+      </c>
+      <c r="G420" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="421" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D421" t="s">
+        <v>561</v>
+      </c>
+      <c r="E421" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="423" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C423" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="424" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D424" t="s">
+        <v>567</v>
+      </c>
+      <c r="G424" s="1" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="425" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C425" t="s">
+        <v>611</v>
+      </c>
+      <c r="G425" s="1"/>
+    </row>
+    <row r="426" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D426" t="s">
+        <v>612</v>
+      </c>
+      <c r="E426" t="s">
+        <v>613</v>
+      </c>
+      <c r="G426" s="1" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="427" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G427" s="1"/>
+    </row>
+    <row r="428" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G428" s="1"/>
+    </row>
+    <row r="429" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G429" s="1"/>
+    </row>
+    <row r="430" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G430" s="1"/>
+    </row>
+    <row r="431" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G431" s="1"/>
+    </row>
+    <row r="432" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G432" s="1"/>
+    </row>
+    <row r="435" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B435" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="436" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C436" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="437" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E437" t="s">
+        <v>570</v>
+      </c>
+      <c r="G437" s="1" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="440" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B440" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="441" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C441" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="442" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D442" t="s">
+        <v>574</v>
+      </c>
+      <c r="E442" t="s">
+        <v>575</v>
+      </c>
+      <c r="F442" t="s">
+        <v>576</v>
+      </c>
+      <c r="G442" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="443" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E443" t="s">
+        <v>578</v>
+      </c>
+      <c r="F443" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="444" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C444" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="445" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D445" t="s">
+        <v>597</v>
+      </c>
+      <c r="E445" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="446" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D446" t="s">
+        <v>600</v>
+      </c>
+      <c r="E446" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="448" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D448" t="s">
+        <v>601</v>
+      </c>
+      <c r="E448" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="449" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D449" t="s">
+        <v>603</v>
+      </c>
+      <c r="E449" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="451" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D451" t="s">
+        <v>605</v>
+      </c>
+      <c r="E451" t="s">
+        <v>606</v>
+      </c>
+      <c r="G451" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="452" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D452" t="s">
         <v>607</v>
       </c>
-      <c r="E416" t="s">
+      <c r="E452" t="s">
         <v>608</v>
       </c>
-      <c r="F416" t="s">
+      <c r="F452" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="420" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B420" t="s">
+    <row r="456" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B456" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="421" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C421" t="s">
+    <row r="457" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C457" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="422" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D422" t="s">
+    <row r="458" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D458" t="s">
         <v>583</v>
       </c>
-      <c r="E422" t="s">
+      <c r="E458" t="s">
         <v>584</v>
       </c>
-      <c r="F422" t="s">
+      <c r="F458" t="s">
         <v>582</v>
       </c>
-      <c r="G422" s="1" t="s">
+      <c r="G458" s="1" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="423" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E423" t="s">
+    <row r="459" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E459" t="s">
         <v>585</v>
       </c>
-      <c r="F423" t="s">
+      <c r="F459" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="425" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D425" t="s">
+    <row r="461" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D461" t="s">
         <v>588</v>
       </c>
-      <c r="E425" t="s">
+      <c r="E461" t="s">
         <v>590</v>
       </c>
-      <c r="F425" t="s">
+      <c r="F461" t="s">
         <v>589</v>
       </c>
     </row>
@@ -4782,12 +5122,12 @@
     <hyperlink ref="F98" r:id="rId14" xr:uid="{93472772-CF6C-D045-B634-2D574A3EE034}"/>
     <hyperlink ref="E183" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
     <hyperlink ref="F184" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
-    <hyperlink ref="D192" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
-    <hyperlink ref="D193" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
+    <hyperlink ref="D208" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
+    <hyperlink ref="D209" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
     <hyperlink ref="F99" r:id="rId19" xr:uid="{92BE3560-5393-C545-9D2D-2B773359B28F}"/>
-    <hyperlink ref="E209" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
-    <hyperlink ref="E210" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
-    <hyperlink ref="E211" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
+    <hyperlink ref="E225" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
+    <hyperlink ref="E226" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
+    <hyperlink ref="E227" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
     <hyperlink ref="E73" r:id="rId23" xr:uid="{1526D7DA-27DA-1443-928C-BEDA9E425734}"/>
     <hyperlink ref="E74" r:id="rId24" xr:uid="{4F363062-BE49-AB4F-8956-2C1F31D9B898}"/>
     <hyperlink ref="H100" r:id="rId25" xr:uid="{D9E13355-D59B-054F-B544-34A5A285A9E0}"/>
@@ -4804,7 +5144,7 @@
     <hyperlink ref="I100" r:id="rId36" xr:uid="{A03C56E4-1156-A148-A568-F50A5C33DB5C}"/>
     <hyperlink ref="F109" r:id="rId37" xr:uid="{12AC219C-4678-4E43-B328-6595FA10B8D3}"/>
     <hyperlink ref="E111" r:id="rId38" xr:uid="{44409621-28A2-704A-B283-3DCE1EFB1603}"/>
-    <hyperlink ref="E215" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
+    <hyperlink ref="E231" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
     <hyperlink ref="F112" r:id="rId40" xr:uid="{A9D0D792-87D1-8144-872F-5CA060D3C28F}"/>
     <hyperlink ref="F113" r:id="rId41" xr:uid="{87EF989D-17E9-1E45-A075-CD862D0B60F4}"/>
     <hyperlink ref="F115" r:id="rId42" xr:uid="{8406C6F0-DC69-A64D-AAD8-60A33C12D00B}"/>
@@ -4814,68 +5154,68 @@
     <hyperlink ref="F120" r:id="rId46" xr:uid="{3D1C62DB-D9B7-BE42-B21D-4EEBC4C9EFE1}"/>
     <hyperlink ref="F121" r:id="rId47" xr:uid="{F5021A21-70A2-D34E-B055-64CAC326E7EF}"/>
     <hyperlink ref="F122" r:id="rId48" xr:uid="{A8C010A1-8EE1-264B-8688-3BEA1B62E535}"/>
-    <hyperlink ref="E216" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
+    <hyperlink ref="E232" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
     <hyperlink ref="F117" r:id="rId50" location="113521" xr:uid="{EE1413C5-3B38-7D4D-8DF1-634A12F0BD81}"/>
     <hyperlink ref="E75" r:id="rId51" xr:uid="{00B1EF4A-7791-0343-8D8C-9A1E83248FC9}"/>
-    <hyperlink ref="E277" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
-    <hyperlink ref="E278" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
+    <hyperlink ref="E293" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
+    <hyperlink ref="E294" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
     <hyperlink ref="F124" r:id="rId54" xr:uid="{40A4B6A0-2F7E-A84D-8CC6-D814A33F5953}"/>
-    <hyperlink ref="E217" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
-    <hyperlink ref="E218" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
-    <hyperlink ref="E219" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
-    <hyperlink ref="E220" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
-    <hyperlink ref="E279" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
-    <hyperlink ref="D194" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
-    <hyperlink ref="D195" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
-    <hyperlink ref="D196" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
-    <hyperlink ref="E221" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
-    <hyperlink ref="E280" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
-    <hyperlink ref="E281" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
-    <hyperlink ref="E283" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
-    <hyperlink ref="E284" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
-    <hyperlink ref="F278" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
-    <hyperlink ref="G278" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
-    <hyperlink ref="E285" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
-    <hyperlink ref="E286" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
-    <hyperlink ref="E287" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
+    <hyperlink ref="E233" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
+    <hyperlink ref="E234" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
+    <hyperlink ref="E235" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
+    <hyperlink ref="E236" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
+    <hyperlink ref="E295" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
+    <hyperlink ref="D210" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
+    <hyperlink ref="D211" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
+    <hyperlink ref="D212" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
+    <hyperlink ref="E237" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
+    <hyperlink ref="E296" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
+    <hyperlink ref="E297" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
+    <hyperlink ref="E299" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
+    <hyperlink ref="E300" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
+    <hyperlink ref="F294" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
+    <hyperlink ref="G294" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
+    <hyperlink ref="E301" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
+    <hyperlink ref="E302" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
+    <hyperlink ref="E303" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
     <hyperlink ref="E185" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
-    <hyperlink ref="E282" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
-    <hyperlink ref="E288" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
-    <hyperlink ref="E289" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
+    <hyperlink ref="E298" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
+    <hyperlink ref="E304" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
+    <hyperlink ref="E305" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
     <hyperlink ref="E77" r:id="rId77" location="code" xr:uid="{C0475FF8-517D-E949-887E-9A42D86E9640}"/>
-    <hyperlink ref="E291" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
+    <hyperlink ref="E307" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
     <hyperlink ref="E78" r:id="rId79" xr:uid="{277DBE6F-F3E5-8B4C-8DD8-BD92445D1A99}"/>
-    <hyperlink ref="E293" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
-    <hyperlink ref="E298" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
-    <hyperlink ref="E200" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
-    <hyperlink ref="E201" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
+    <hyperlink ref="E309" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
+    <hyperlink ref="E314" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
+    <hyperlink ref="E216" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
+    <hyperlink ref="E217" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
     <hyperlink ref="F145" r:id="rId84" xr:uid="{EB604865-A16B-0646-A5B5-0D047467449D}"/>
-    <hyperlink ref="E223" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
-    <hyperlink ref="D307" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
-    <hyperlink ref="D308" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
-    <hyperlink ref="E317" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
-    <hyperlink ref="E318" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
-    <hyperlink ref="E316" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
-    <hyperlink ref="D327" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
-    <hyperlink ref="E333" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
-    <hyperlink ref="E330" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
-    <hyperlink ref="E334" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
-    <hyperlink ref="F325" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
-    <hyperlink ref="F326" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
-    <hyperlink ref="E328" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
-    <hyperlink ref="G330" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
-    <hyperlink ref="D343" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
-    <hyperlink ref="E335" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
-    <hyperlink ref="E338" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
-    <hyperlink ref="E337" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
-    <hyperlink ref="F242" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
-    <hyperlink ref="E243" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
-    <hyperlink ref="E244" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
-    <hyperlink ref="E245" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
-    <hyperlink ref="G259" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
-    <hyperlink ref="E254" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
-    <hyperlink ref="E255" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
-    <hyperlink ref="E260" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
+    <hyperlink ref="E239" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
+    <hyperlink ref="D323" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
+    <hyperlink ref="D324" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
+    <hyperlink ref="E333" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
+    <hyperlink ref="E334" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
+    <hyperlink ref="E332" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
+    <hyperlink ref="D343" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
+    <hyperlink ref="E349" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
+    <hyperlink ref="E346" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
+    <hyperlink ref="E350" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
+    <hyperlink ref="F341" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
+    <hyperlink ref="F342" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
+    <hyperlink ref="E344" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
+    <hyperlink ref="G346" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
+    <hyperlink ref="D359" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
+    <hyperlink ref="E351" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
+    <hyperlink ref="E354" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
+    <hyperlink ref="E353" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
+    <hyperlink ref="F258" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
+    <hyperlink ref="E259" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
+    <hyperlink ref="E260" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
+    <hyperlink ref="E261" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
+    <hyperlink ref="G275" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
+    <hyperlink ref="E270" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
+    <hyperlink ref="E271" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
+    <hyperlink ref="E276" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
     <hyperlink ref="F152" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
     <hyperlink ref="F157" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
     <hyperlink ref="F158" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
@@ -4885,25 +5225,31 @@
     <hyperlink ref="F171" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
     <hyperlink ref="F165" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
     <hyperlink ref="F174" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
-    <hyperlink ref="H238" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
-    <hyperlink ref="F350" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
-    <hyperlink ref="G364" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
-    <hyperlink ref="F351" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
-    <hyperlink ref="G366" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
-    <hyperlink ref="G368" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
-    <hyperlink ref="G371" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
-    <hyperlink ref="G375" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
-    <hyperlink ref="G383" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
-    <hyperlink ref="G381" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
-    <hyperlink ref="G386" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
-    <hyperlink ref="G392" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
-    <hyperlink ref="G396" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
-    <hyperlink ref="G401" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
-    <hyperlink ref="G406" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
-    <hyperlink ref="G422" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
+    <hyperlink ref="H254" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
+    <hyperlink ref="F366" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
+    <hyperlink ref="G380" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
+    <hyperlink ref="F367" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
+    <hyperlink ref="G382" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
+    <hyperlink ref="G384" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
+    <hyperlink ref="G387" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
+    <hyperlink ref="G391" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
+    <hyperlink ref="G411" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
+    <hyperlink ref="G409" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
+    <hyperlink ref="G414" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
+    <hyperlink ref="G420" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
+    <hyperlink ref="G424" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
+    <hyperlink ref="G437" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
+    <hyperlink ref="G442" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
+    <hyperlink ref="G458" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
     <hyperlink ref="E20" r:id="rId136" xr:uid="{809CA2D1-39E9-0045-A4DF-E4C0C2E97FA2}"/>
     <hyperlink ref="E21" r:id="rId137" xr:uid="{5DC44543-F2B9-F841-9097-6DB19C5EBD82}"/>
-    <hyperlink ref="G415" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
+    <hyperlink ref="G451" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
+    <hyperlink ref="G426" r:id="rId139" xr:uid="{7F4EA1D7-8774-1A4B-BF25-18ED0416CB20}"/>
+    <hyperlink ref="F197" r:id="rId140" xr:uid="{101513F3-87A1-DA41-8BF5-E4029309ECB8}"/>
+    <hyperlink ref="F189" r:id="rId141" xr:uid="{494E255E-6912-8643-B5CD-1D65E0DDCFFC}"/>
+    <hyperlink ref="F190" r:id="rId142" xr:uid="{828F749D-83DE-C14E-B637-56047AC1B384}"/>
+    <hyperlink ref="F198" r:id="rId143" xr:uid="{435D9B3C-98B6-5E49-BD30-EAA53523CDB7}"/>
+    <hyperlink ref="F199" r:id="rId144" xr:uid="{7D905409-0097-E04E-9593-2DEEBEEA0D0F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4911,15 +5257,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G28"/>
+  <dimension ref="B2:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="51.83203125" customWidth="1"/>
+    <col min="2" max="2" width="68.83203125" customWidth="1"/>
     <col min="3" max="3" width="25.33203125" customWidth="1"/>
     <col min="5" max="5" width="55.5" customWidth="1"/>
   </cols>
@@ -5231,6 +5577,117 @@
       </c>
       <c r="F28" s="1" t="s">
         <v>446</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>642</v>
+      </c>
+      <c r="C29" t="s">
+        <v>169</v>
+      </c>
+      <c r="E29" t="s">
+        <v>643</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>644</v>
+      </c>
+      <c r="E30" t="s">
+        <v>645</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="E31" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>647</v>
+      </c>
+      <c r="E32" t="s">
+        <v>648</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>652</v>
+      </c>
+      <c r="C33" t="s">
+        <v>650</v>
+      </c>
+      <c r="D33" t="s">
+        <v>651</v>
+      </c>
+      <c r="E33" t="s">
+        <v>653</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>655</v>
+      </c>
+      <c r="C34" t="s">
+        <v>169</v>
+      </c>
+      <c r="D34" t="s">
+        <v>448</v>
+      </c>
+      <c r="E34" t="s">
+        <v>656</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>658</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>663</v>
+      </c>
+      <c r="E36" t="s">
+        <v>665</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>667</v>
+      </c>
+      <c r="E37" t="s">
+        <v>668</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>669</v>
       </c>
     </row>
   </sheetData>
@@ -5263,6 +5720,15 @@
     <hyperlink ref="F26" r:id="rId26" xr:uid="{3B04ECD2-7215-E44A-B2BA-78117512C321}"/>
     <hyperlink ref="F27" r:id="rId27" xr:uid="{72C1FF05-0698-1044-AD35-779549D5FEE1}"/>
     <hyperlink ref="F28" r:id="rId28" xr:uid="{FD52415E-DA54-844A-937E-E667C2082DAB}"/>
+    <hyperlink ref="F29" r:id="rId29" xr:uid="{F49660D1-75B0-5640-A7B4-03E135260182}"/>
+    <hyperlink ref="F30" r:id="rId30" xr:uid="{0AD2DAAC-BAD7-6D4C-83DC-113CEB8ED428}"/>
+    <hyperlink ref="F32" r:id="rId31" xr:uid="{79BAFF11-A009-8142-B115-6F128D0D4E78}"/>
+    <hyperlink ref="F33" r:id="rId32" xr:uid="{4C21BF54-5FF1-7A46-8901-7EAE678178C0}"/>
+    <hyperlink ref="F34" r:id="rId33" xr:uid="{EA4A36B0-31D2-EC4D-891B-C199FD1AD007}"/>
+    <hyperlink ref="F35" r:id="rId34" xr:uid="{F9B90E3A-71B9-B343-8FAA-E06A737DA877}"/>
+    <hyperlink ref="F31" r:id="rId35" xr:uid="{A7216F86-E62C-AC48-B73F-76B2F894E6AD}"/>
+    <hyperlink ref="F36" r:id="rId36" xr:uid="{EF122EDE-6CCB-2440-885D-B71D42E7B9FC}"/>
+    <hyperlink ref="F37" r:id="rId37" xr:uid="{BF8E0884-4A84-1F45-BA3C-ED13206AFD16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added more tips about pandas and python mainly
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6036B1-377D-7641-A356-1333EEB860AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24249F2B-7225-B34B-A4A8-3A7CAF3568E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="560" windowWidth="25600" windowHeight="15340" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="25600" windowHeight="15340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
     <sheet name="Random Articles" sheetId="4" r:id="rId2"/>
+    <sheet name="Tips" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="710">
   <si>
     <t>docker</t>
   </si>
@@ -2049,6 +2050,126 @@
   </si>
   <si>
     <t>https://stackoverflow.com/questions/32107558/how-do-i-convert-numpy-nan-objects-to-sql-nulls</t>
+  </si>
+  <si>
+    <t>Pandas convert dataframe to array of tuples</t>
+  </si>
+  <si>
+    <t>tuples = [tuple(x) for x in subset.values]</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/9758450/pandas-convert-dataframe-to-array-of-tuples</t>
+  </si>
+  <si>
+    <t>check nan rows in pandas dataframe</t>
+  </si>
+  <si>
+    <t>df[df.isnull().any(axis=1)]</t>
+  </si>
+  <si>
+    <t>https://www.kite.com/python/answers/how-to-find-rows-with-nan-values-in-a-pandas-dataframe-in-python</t>
+  </si>
+  <si>
+    <t>https://www.psycopg.org/docs/usage.html</t>
+  </si>
+  <si>
+    <t>Adaptation of Python values to SQL types</t>
+  </si>
+  <si>
+    <t>4a. Store github credentials</t>
+  </si>
+  <si>
+    <t>1. start store (you will be asked about the credentials the first time you run "git pull")</t>
+  </si>
+  <si>
+    <t>git config --global credential.helper store</t>
+  </si>
+  <si>
+    <t>2. Input the credentials</t>
+  </si>
+  <si>
+    <t>git pull</t>
+  </si>
+  <si>
+    <t>3. Credential file location</t>
+  </si>
+  <si>
+    <t>~/.git-credentials</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/35942754/how-to-save-username-and-password-in-git</t>
+  </si>
+  <si>
+    <t>pip</t>
+  </si>
+  <si>
+    <t>check details of installed packages</t>
+  </si>
+  <si>
+    <t>List installed packages</t>
+  </si>
+  <si>
+    <t>pip show package</t>
+  </si>
+  <si>
+    <t>pip list</t>
+  </si>
+  <si>
+    <t>https://note.nkmk.me/en/python-package-version/</t>
+  </si>
+  <si>
+    <t>check package version</t>
+  </si>
+  <si>
+    <t>package.__version__</t>
+  </si>
+  <si>
+    <t>There are a lot of differences between 5.2.3 and 5.3.0</t>
+  </si>
+  <si>
+    <t>InfluxDB-python</t>
+  </si>
+  <si>
+    <t>https://github.com/influxdata/influxdb-python/issues/820</t>
+  </si>
+  <si>
+    <t>5. delete data in database</t>
+  </si>
+  <si>
+    <t>https://kb.objectrocket.com/timescaledb/delete-command-in-timescaledb-1566</t>
+  </si>
+  <si>
+    <t>DELETE FROM measurement;</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/47466255/subclassing-a-pandas-dataframe-updates</t>
+  </si>
+  <si>
+    <t>Subclassing a Pandas DataFrame, updates?</t>
+  </si>
+  <si>
+    <t>def _constructor(self): def _c(*args, **kwargs):</t>
+  </si>
+  <si>
+    <t>self._copy_attrs(df)</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/22155951/how-to-subclass-pandas-dataframe</t>
+  </si>
+  <si>
+    <t>variables = {'contract': float()}; df = pd.DataFrame(variables, index=[])</t>
+  </si>
+  <si>
+    <t>Create Empty Dataframe in Pandas specifying column types</t>
+  </si>
+  <si>
+    <t>install without dependences</t>
+  </si>
+  <si>
+    <t>pip install --no-deps package</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/52126116/prevent-pip-from-installing-some-dependencies</t>
   </si>
 </sst>
 </file>
@@ -2510,11 +2631,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I461"/>
+  <dimension ref="B1:I478"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A380" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D401" sqref="D401"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F203" sqref="F203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3403,1704 +3524,1799 @@
     </row>
     <row r="148" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C148" t="s">
-        <v>358</v>
+        <v>678</v>
       </c>
     </row>
     <row r="149" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D149" t="s">
-        <v>355</v>
+        <v>679</v>
       </c>
       <c r="E149" t="s">
-        <v>354</v>
+        <v>680</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="150" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D150" t="s">
-        <v>356</v>
+        <v>681</v>
       </c>
       <c r="E150" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="152" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C152" t="s">
-        <v>370</v>
-      </c>
-      <c r="F152" s="1" t="s">
-        <v>379</v>
+        <v>682</v>
+      </c>
+    </row>
+    <row r="151" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D151" t="s">
+        <v>683</v>
+      </c>
+      <c r="E151" t="s">
+        <v>684</v>
       </c>
     </row>
     <row r="153" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D153" t="s">
-        <v>371</v>
-      </c>
-      <c r="E153" t="s">
-        <v>372</v>
+      <c r="C153" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="154" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D154" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
       <c r="E154" t="s">
-        <v>374</v>
+        <v>354</v>
       </c>
     </row>
     <row r="155" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D155" t="s">
-        <v>375</v>
+        <v>356</v>
       </c>
       <c r="E155" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="156" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D156" t="s">
-        <v>377</v>
-      </c>
-      <c r="E156" t="s">
-        <v>378</v>
+        <v>357</v>
       </c>
     </row>
     <row r="157" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D157" t="s">
-        <v>387</v>
-      </c>
-      <c r="E157" t="s">
-        <v>388</v>
+      <c r="C157" t="s">
+        <v>370</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
     </row>
     <row r="158" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D158" t="s">
-        <v>390</v>
+        <v>371</v>
       </c>
       <c r="E158" t="s">
-        <v>391</v>
-      </c>
-      <c r="F158" s="1" t="s">
-        <v>392</v>
+        <v>372</v>
+      </c>
+    </row>
+    <row r="159" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D159" t="s">
+        <v>373</v>
+      </c>
+      <c r="E159" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="160" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C160" t="s">
-        <v>380</v>
+      <c r="D160" t="s">
+        <v>375</v>
+      </c>
+      <c r="E160" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="161" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D161" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="E161" t="s">
-        <v>382</v>
-      </c>
-      <c r="F161" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
     </row>
     <row r="162" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D162" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="E162" t="s">
-        <v>384</v>
-      </c>
-      <c r="F162" t="s">
-        <v>386</v>
+        <v>388</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="163" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="F163" s="1"/>
-    </row>
-    <row r="164" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C164" t="s">
-        <v>393</v>
-      </c>
-      <c r="D164" t="s">
-        <v>421</v>
-      </c>
-      <c r="E164" t="s">
-        <v>394</v>
-      </c>
-      <c r="F164" s="1" t="s">
-        <v>64</v>
+      <c r="D163" t="s">
+        <v>390</v>
+      </c>
+      <c r="E163" t="s">
+        <v>391</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="165" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D165" t="s">
-        <v>422</v>
-      </c>
-      <c r="E165" t="s">
-        <v>423</v>
-      </c>
-      <c r="F165" s="1" t="s">
-        <v>424</v>
+      <c r="C165" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="166" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D166" t="s">
+        <v>381</v>
+      </c>
+      <c r="E166" t="s">
+        <v>382</v>
+      </c>
+      <c r="F166" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="167" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D167" t="s">
+        <v>383</v>
+      </c>
+      <c r="E167" t="s">
+        <v>384</v>
+      </c>
+      <c r="F167" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="168" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F168" s="1"/>
+    </row>
+    <row r="169" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C169" t="s">
+        <v>393</v>
+      </c>
+      <c r="D169" t="s">
+        <v>421</v>
+      </c>
+      <c r="E169" t="s">
+        <v>394</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="170" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D170" t="s">
+        <v>422</v>
+      </c>
+      <c r="E170" t="s">
+        <v>423</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="171" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D171" t="s">
         <v>425</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E171" t="s">
         <v>426</v>
       </c>
-      <c r="F166" s="1"/>
-    </row>
-    <row r="167" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C167" t="s">
+      <c r="F171" s="1"/>
+    </row>
+    <row r="172" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C172" t="s">
         <v>395</v>
       </c>
-      <c r="F167" s="1"/>
-    </row>
-    <row r="168" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D168" t="s">
+      <c r="F172" s="1"/>
+    </row>
+    <row r="173" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D173" t="s">
         <v>397</v>
       </c>
-      <c r="E168" t="s">
+      <c r="E173" t="s">
         <v>396</v>
       </c>
-      <c r="F168" s="1"/>
-    </row>
-    <row r="169" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D169" t="s">
-        <v>398</v>
-      </c>
-      <c r="F169" t="s">
-        <v>399</v>
-      </c>
-      <c r="G169" s="1" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="170" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C170" t="s">
-        <v>417</v>
-      </c>
-      <c r="G170" s="1"/>
-    </row>
-    <row r="171" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E171" t="s">
-        <v>418</v>
-      </c>
-      <c r="F171" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="G171" s="1"/>
-    </row>
-    <row r="172" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E172" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="173" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C173" t="s">
-        <v>432</v>
-      </c>
+      <c r="F173" s="1"/>
     </row>
     <row r="174" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D174" t="s">
+        <v>398</v>
+      </c>
+      <c r="F174" t="s">
+        <v>399</v>
+      </c>
+      <c r="G174" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="175" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C175" t="s">
+        <v>417</v>
+      </c>
+      <c r="G175" s="1"/>
+    </row>
+    <row r="176" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E176" t="s">
+        <v>418</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="G176" s="1"/>
+    </row>
+    <row r="177" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E177" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="178" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C178" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="179" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D179" t="s">
         <v>433</v>
       </c>
-      <c r="E174" t="s">
+      <c r="E179" t="s">
         <v>435</v>
       </c>
-      <c r="F174" s="1" t="s">
+      <c r="F179" s="1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="175" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D175" t="s">
+    <row r="180" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D180" t="s">
         <v>434</v>
       </c>
-      <c r="E175" t="s">
+      <c r="E180" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="181" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B181" t="s">
+    <row r="186" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B186" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="182" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C182" t="s">
+    <row r="187" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C187" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="183" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D183" t="s">
+    <row r="188" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D188" t="s">
         <v>171</v>
       </c>
-      <c r="E183" s="1" t="s">
+      <c r="E188" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="184" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D184" t="s">
+    <row r="189" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D189" t="s">
         <v>175</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E189" t="s">
         <v>173</v>
       </c>
-      <c r="F184" s="1" t="s">
+      <c r="F189" s="1" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="185" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C185" t="s">
-        <v>322</v>
-      </c>
-      <c r="E185" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="F185" s="1"/>
-    </row>
-    <row r="186" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C186" t="s">
-        <v>406</v>
-      </c>
-      <c r="D186" t="s">
-        <v>407</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="F186" s="1"/>
-    </row>
-    <row r="187" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D187" t="s">
-        <v>408</v>
-      </c>
-      <c r="F187" s="1"/>
-    </row>
-    <row r="188" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F188" s="1"/>
-    </row>
-    <row r="189" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C189" t="s">
-        <v>618</v>
-      </c>
-      <c r="D189" t="s">
-        <v>619</v>
-      </c>
-      <c r="F189" s="1" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="190" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C190" t="s">
-        <v>622</v>
-      </c>
-      <c r="D190" t="s">
-        <v>621</v>
-      </c>
-      <c r="F190" s="1" t="s">
-        <v>623</v>
-      </c>
+        <v>322</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F190" s="1"/>
     </row>
     <row r="191" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C191" t="s">
+        <v>406</v>
+      </c>
+      <c r="D191" t="s">
+        <v>407</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>409</v>
+      </c>
       <c r="F191" s="1"/>
     </row>
     <row r="192" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D192" t="s">
+        <v>408</v>
+      </c>
       <c r="F192" s="1"/>
     </row>
     <row r="193" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F193" s="1"/>
     </row>
     <row r="194" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F194" s="1"/>
+      <c r="C194" t="s">
+        <v>618</v>
+      </c>
+      <c r="D194" t="s">
+        <v>619</v>
+      </c>
+      <c r="F194" s="1" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="195" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C195" t="s">
+        <v>622</v>
+      </c>
+      <c r="D195" t="s">
+        <v>621</v>
+      </c>
+      <c r="F195" s="1" t="s">
+        <v>623</v>
+      </c>
     </row>
     <row r="196" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B196" t="s">
-        <v>448</v>
-      </c>
+      <c r="F196" s="1"/>
     </row>
     <row r="197" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C197" t="s">
-        <v>616</v>
-      </c>
-      <c r="D197" t="s">
-        <v>615</v>
-      </c>
-      <c r="F197" s="1" t="s">
-        <v>617</v>
-      </c>
+      <c r="F197" s="1"/>
     </row>
     <row r="198" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C198" t="s">
-        <v>624</v>
-      </c>
-      <c r="D198" t="s">
-        <v>625</v>
-      </c>
-      <c r="F198" s="1" t="s">
-        <v>626</v>
-      </c>
+      <c r="B198" t="s">
+        <v>686</v>
+      </c>
+      <c r="F198" s="1"/>
     </row>
     <row r="199" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C199" t="s">
-        <v>628</v>
+        <v>687</v>
       </c>
       <c r="D199" t="s">
-        <v>627</v>
+        <v>689</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>629</v>
+        <v>691</v>
       </c>
     </row>
     <row r="200" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C200" t="s">
+        <v>688</v>
+      </c>
+      <c r="D200" t="s">
+        <v>690</v>
+      </c>
+      <c r="F200" s="1"/>
+    </row>
+    <row r="201" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C201" t="s">
+        <v>692</v>
+      </c>
+      <c r="D201" t="s">
+        <v>693</v>
+      </c>
+      <c r="F201" s="1"/>
+    </row>
+    <row r="202" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C202" t="s">
+        <v>707</v>
+      </c>
+      <c r="D202" t="s">
+        <v>708</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="203" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F203" s="1"/>
+    </row>
+    <row r="204" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F204" s="1"/>
+    </row>
+    <row r="205" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F205" s="1"/>
+    </row>
+    <row r="206" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F206" s="1"/>
+    </row>
+    <row r="208" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B208" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="209" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C209" t="s">
+        <v>616</v>
+      </c>
+      <c r="D209" t="s">
+        <v>615</v>
+      </c>
+      <c r="F209" s="1" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="210" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C210" t="s">
+        <v>624</v>
+      </c>
+      <c r="D210" t="s">
+        <v>625</v>
+      </c>
+      <c r="F210" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="211" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C211" t="s">
+        <v>628</v>
+      </c>
+      <c r="D211" t="s">
+        <v>627</v>
+      </c>
+      <c r="F211" s="1" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="212" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C212" t="s">
         <v>631</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D212" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="207" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B207" t="s">
+    <row r="219" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B219" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="208" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C208" t="s">
+    <row r="220" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C220" t="s">
         <v>176</v>
       </c>
-      <c r="D208" s="1" t="s">
+      <c r="D220" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="209" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C209" t="s">
+    <row r="221" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C221" t="s">
         <v>178</v>
       </c>
-      <c r="D209" s="1" t="s">
+      <c r="D221" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="210" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C210" t="s">
+    <row r="222" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C222" t="s">
         <v>293</v>
       </c>
-      <c r="D210" s="1" t="s">
+      <c r="D222" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="211" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C211" t="s">
+    <row r="223" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C223" t="s">
         <v>294</v>
       </c>
-      <c r="D211" s="1" t="s">
+      <c r="D223" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="212" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C212" t="s">
+    <row r="224" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C224" t="s">
         <v>297</v>
       </c>
-      <c r="D212" s="1" t="s">
+      <c r="D224" s="1" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="213" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D213" s="1"/>
-    </row>
-    <row r="214" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D214" s="1"/>
-    </row>
-    <row r="215" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B215" t="s">
+    <row r="225" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D225" s="1"/>
+    </row>
+    <row r="226" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D226" s="1"/>
+    </row>
+    <row r="227" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B227" t="s">
         <v>343</v>
       </c>
-      <c r="D215" s="1"/>
-    </row>
-    <row r="216" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C216" t="s">
+      <c r="D227" s="1"/>
+    </row>
+    <row r="228" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C228" t="s">
         <v>344</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D228" t="s">
         <v>369</v>
       </c>
-      <c r="E216" s="1" t="s">
+      <c r="E228" s="1" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="217" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D217" t="s">
+    <row r="229" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D229" t="s">
         <v>368</v>
       </c>
-      <c r="E217" s="1" t="s">
+      <c r="E229" s="1" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="218" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D218" s="1"/>
-    </row>
-    <row r="219" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D219" s="1"/>
-    </row>
-    <row r="220" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D220" s="1"/>
-    </row>
-    <row r="224" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B224" t="s">
+    <row r="230" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D230" s="1"/>
+    </row>
+    <row r="231" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D231" s="1"/>
+    </row>
+    <row r="232" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D232" s="1"/>
+    </row>
+    <row r="236" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B236" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="225" spans="3:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="C225" s="4" t="s">
+    <row r="237" spans="2:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="C237" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D225" s="2" t="s">
+      <c r="D237" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E225" s="1" t="s">
+      <c r="E237" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="226" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C226" t="s">
+    <row r="238" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C238" t="s">
         <v>187</v>
       </c>
-      <c r="E226" s="1" t="s">
+      <c r="E238" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="227" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C227" t="s">
+    <row r="239" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C239" t="s">
         <v>215</v>
       </c>
-      <c r="E227" s="1" t="s">
+      <c r="E239" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="229" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D229" t="s">
+    <row r="241" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D241" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="231" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C231" t="s">
+    <row r="243" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C243" t="s">
         <v>242</v>
       </c>
-      <c r="D231" t="s">
+      <c r="D243" t="s">
         <v>243</v>
       </c>
-      <c r="E231" s="1" t="s">
+      <c r="E243" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="232" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C232" t="s">
+    <row r="244" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C244" t="s">
         <v>269</v>
       </c>
-      <c r="D232" t="s">
+      <c r="D244" t="s">
         <v>270</v>
       </c>
-      <c r="E232" s="1" t="s">
+      <c r="E244" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="233" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C233" t="s">
+    <row r="245" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C245" t="s">
         <v>284</v>
       </c>
-      <c r="E233" s="1" t="s">
+      <c r="E245" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="234" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E234" s="1" t="s">
+    <row r="246" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E246" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="235" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E235" s="1" t="s">
+    <row r="247" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E247" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="236" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C236" t="s">
+    <row r="248" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C248" t="s">
         <v>288</v>
       </c>
-      <c r="E236" s="1" t="s">
+      <c r="E248" s="1" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="237" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C237" t="s">
+    <row r="249" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C249" t="s">
         <v>299</v>
       </c>
-      <c r="E237" s="1" t="s">
+      <c r="E249" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="238" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E238" s="1"/>
-    </row>
-    <row r="239" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C239" t="s">
+    <row r="250" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E250" s="1"/>
+    </row>
+    <row r="251" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C251" t="s">
         <v>359</v>
       </c>
-      <c r="D239" t="s">
+      <c r="D251" t="s">
         <v>360</v>
       </c>
-      <c r="E239" s="1" t="s">
+      <c r="E251" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="240" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E240" s="1"/>
-    </row>
-    <row r="241" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E241" s="1"/>
-    </row>
-    <row r="242" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E242" s="1"/>
-    </row>
-    <row r="243" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E243" s="1"/>
-    </row>
-    <row r="244" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E244" s="1"/>
-    </row>
-    <row r="245" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E245" s="1"/>
-    </row>
-    <row r="246" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E246" s="1"/>
-    </row>
-    <row r="247" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E247" s="1"/>
-    </row>
-    <row r="248" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C248" t="s">
+    <row r="252" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E252" s="1"/>
+    </row>
+    <row r="253" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E253" s="1"/>
+    </row>
+    <row r="254" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E254" s="1"/>
+    </row>
+    <row r="255" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E255" s="1"/>
+    </row>
+    <row r="256" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E256" s="1"/>
+    </row>
+    <row r="257" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E257" s="1"/>
+    </row>
+    <row r="258" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E258" s="1"/>
+    </row>
+    <row r="259" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E259" s="1"/>
+    </row>
+    <row r="260" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C260" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="249" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D249" t="s">
+    <row r="261" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D261" t="s">
         <v>135</v>
       </c>
-      <c r="E249" t="s">
+      <c r="E261" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="250" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D250" t="s">
+    <row r="262" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D262" t="s">
         <v>136</v>
       </c>
-      <c r="E250" t="s">
+      <c r="E262" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="251" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D251" t="s">
+    <row r="263" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D263" t="s">
         <v>140</v>
       </c>
-      <c r="E251" t="s">
+      <c r="E263" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="252" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D252" t="s">
+    <row r="264" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D264" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="253" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D253" t="s">
+    <row r="265" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D265" t="s">
         <v>142</v>
       </c>
-      <c r="E253" t="s">
+      <c r="E265" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="254" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D254" t="s">
+    <row r="266" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D266" t="s">
         <v>484</v>
       </c>
-      <c r="E254" t="s">
+      <c r="E266" t="s">
         <v>486</v>
       </c>
-      <c r="F254" t="s">
+      <c r="F266" t="s">
         <v>490</v>
       </c>
-      <c r="G254" t="s">
+      <c r="G266" t="s">
         <v>485</v>
       </c>
-      <c r="H254" s="1" t="s">
+      <c r="H266" s="1" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="255" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D255" t="s">
+    <row r="267" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D267" t="s">
         <v>487</v>
       </c>
-      <c r="E255" t="s">
+      <c r="E267" t="s">
         <v>488</v>
       </c>
-      <c r="G255" t="s">
+      <c r="G267" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="257" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C257" t="s">
+    <row r="269" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C269" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="258" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D258" t="s">
+    <row r="270" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D270" t="s">
         <v>73</v>
       </c>
-      <c r="E258" t="s">
+      <c r="E270" t="s">
         <v>74</v>
       </c>
-      <c r="F258" s="1" t="s">
+      <c r="F270" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="259" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D259" t="s">
-        <v>76</v>
-      </c>
-      <c r="E259" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="260" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D260" t="s">
-        <v>78</v>
-      </c>
-      <c r="E260" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="261" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D261" t="s">
-        <v>81</v>
-      </c>
-      <c r="E261" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="262" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D262" t="s">
-        <v>362</v>
-      </c>
-      <c r="E262" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="263" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D263" t="s">
-        <v>363</v>
-      </c>
-      <c r="E263" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="265" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D265" t="s">
-        <v>82</v>
-      </c>
-      <c r="E265" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="266" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D266" t="s">
-        <v>84</v>
-      </c>
-      <c r="E266" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="268" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C268" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="269" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D269" t="s">
-        <v>73</v>
-      </c>
-      <c r="E269" t="s">
-        <v>131</v>
-      </c>
-      <c r="F269" s="1"/>
-    </row>
-    <row r="270" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D270" t="s">
-        <v>147</v>
-      </c>
-      <c r="E270" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F270" s="1"/>
-    </row>
-    <row r="271" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="271" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D271" t="s">
         <v>76</v>
       </c>
       <c r="E271" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="272" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D272" t="s">
+        <v>78</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="273" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D273" t="s">
+        <v>81</v>
+      </c>
+      <c r="E273" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="274" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D274" t="s">
+        <v>362</v>
+      </c>
+      <c r="E274" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="275" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D275" t="s">
+        <v>363</v>
+      </c>
+      <c r="E275" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="277" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D277" t="s">
+        <v>82</v>
+      </c>
+      <c r="E277" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="278" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D278" t="s">
+        <v>84</v>
+      </c>
+      <c r="E278" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="280" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C280" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="281" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D281" t="s">
+        <v>73</v>
+      </c>
+      <c r="E281" t="s">
+        <v>131</v>
+      </c>
+      <c r="F281" s="1"/>
+    </row>
+    <row r="282" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D282" t="s">
+        <v>147</v>
+      </c>
+      <c r="E282" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F282" s="1"/>
+    </row>
+    <row r="283" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D283" t="s">
+        <v>76</v>
+      </c>
+      <c r="E283" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="272" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E272" s="1"/>
-    </row>
-    <row r="273" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D273" t="s">
+    <row r="284" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E284" s="1"/>
+    </row>
+    <row r="285" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D285" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="274" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E274" t="s">
+    <row r="286" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E286" t="s">
         <v>151</v>
       </c>
-      <c r="F274" t="s">
+      <c r="F286" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="275" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E275" t="s">
+    <row r="287" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E287" t="s">
         <v>152</v>
       </c>
-      <c r="F275" t="s">
+      <c r="F287" t="s">
         <v>145</v>
       </c>
-      <c r="G275" s="1" t="s">
+      <c r="G287" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="276" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D276" t="s">
+    <row r="288" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D288" t="s">
         <v>153</v>
       </c>
-      <c r="E276" s="1" t="s">
+      <c r="E288" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G276" s="1"/>
-    </row>
-    <row r="290" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E290" s="1"/>
-    </row>
-    <row r="292" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B292" t="s">
+      <c r="G288" s="1"/>
+    </row>
+    <row r="302" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E302" s="1"/>
+    </row>
+    <row r="304" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B304" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="293" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C293" t="s">
+    <row r="305" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C305" t="s">
         <v>277</v>
       </c>
-      <c r="D293" t="s">
+      <c r="D305" t="s">
         <v>279</v>
       </c>
-      <c r="E293" s="1" t="s">
+      <c r="E305" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="294" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C294" t="s">
+    <row r="306" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C306" t="s">
         <v>281</v>
       </c>
-      <c r="E294" s="1" t="s">
+      <c r="E306" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="F294" s="1" t="s">
+      <c r="F306" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="G294" s="1" t="s">
+      <c r="G306" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="295" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C295" t="s">
+    <row r="307" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C307" t="s">
         <v>290</v>
       </c>
-      <c r="E295" s="1" t="s">
+      <c r="E307" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="296" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C296" t="s">
+    <row r="308" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C308" t="s">
         <v>304</v>
       </c>
-      <c r="E296" s="1" t="s">
+      <c r="E308" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="297" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D297" t="s">
+    <row r="309" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D309" t="s">
         <v>306</v>
       </c>
-      <c r="E297" s="1" t="s">
+      <c r="E309" s="1" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="298" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C298" t="s">
+    <row r="310" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C310" t="s">
         <v>324</v>
       </c>
-      <c r="E298" s="1" t="s">
+      <c r="E310" s="1" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="299" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C299" t="s">
+    <row r="311" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C311" t="s">
         <v>308</v>
       </c>
-      <c r="D299" t="s">
+      <c r="D311" t="s">
         <v>309</v>
       </c>
-      <c r="E299" s="1" t="s">
+      <c r="E311" s="1" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="300" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C300" t="s">
+    <row r="312" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C312" t="s">
         <v>311</v>
       </c>
-      <c r="E300" s="1" t="s">
+      <c r="E312" s="1" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="301" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C301" t="s">
+    <row r="313" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C313" t="s">
         <v>316</v>
       </c>
-      <c r="E301" s="1" t="s">
+      <c r="E313" s="1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="302" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C302" t="s">
+    <row r="314" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C314" t="s">
         <v>317</v>
       </c>
-      <c r="E302" s="1" t="s">
+      <c r="E314" s="1" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="303" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C303" t="s">
+    <row r="315" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C315" t="s">
         <v>319</v>
       </c>
-      <c r="E303" s="1" t="s">
+      <c r="E315" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="304" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C304" t="s">
+    <row r="316" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C316" t="s">
         <v>326</v>
       </c>
-      <c r="D304" t="s">
+      <c r="D316" t="s">
         <v>333</v>
       </c>
-      <c r="E304" s="1" t="s">
+      <c r="E316" s="1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="305" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D305" t="s">
+    <row r="317" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D317" t="s">
         <v>328</v>
       </c>
-      <c r="E305" s="1" t="s">
+      <c r="E317" s="1" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="307" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C307" t="s">
+    <row r="319" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C319" t="s">
         <v>330</v>
       </c>
-      <c r="D307" t="s">
+      <c r="D319" t="s">
         <v>331</v>
       </c>
-      <c r="E307" s="1" t="s">
+      <c r="E319" s="1" t="s">
         <v>332</v>
-      </c>
-    </row>
-    <row r="309" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C309" t="s">
-        <v>336</v>
-      </c>
-      <c r="D309" t="s">
-        <v>338</v>
-      </c>
-      <c r="E309" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="313" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B313" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="314" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C314" t="s">
-        <v>342</v>
-      </c>
-      <c r="D314" t="s">
-        <v>340</v>
-      </c>
-      <c r="E314" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="320" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B320" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="321" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C321" t="s">
+        <v>336</v>
+      </c>
+      <c r="D321" t="s">
+        <v>338</v>
+      </c>
+      <c r="E321" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="325" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B325" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="326" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C326" t="s">
+        <v>342</v>
+      </c>
+      <c r="D326" t="s">
+        <v>340</v>
+      </c>
+      <c r="E326" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="332" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B332" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="333" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C333" t="s">
         <v>87</v>
       </c>
-      <c r="D321" t="s">
+      <c r="D333" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="322" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C322" t="s">
+    <row r="334" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C334" t="s">
         <v>89</v>
       </c>
-      <c r="D322" t="s">
+      <c r="D334" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="323" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C323" t="s">
+    <row r="335" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C335" t="s">
         <v>96</v>
       </c>
-      <c r="D323" s="1" t="s">
+      <c r="D335" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="324" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C324" t="s">
+    <row r="336" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C336" t="s">
         <v>98</v>
       </c>
-      <c r="D324" s="1" t="s">
+      <c r="D336" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="326" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B326" t="s">
+    <row r="338" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B338" t="s">
         <v>91</v>
       </c>
-      <c r="C326" t="s">
+      <c r="C338" t="s">
         <v>92</v>
       </c>
-      <c r="D326" t="s">
+      <c r="D338" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="327" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C327" t="s">
+    <row r="339" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C339" t="s">
         <v>94</v>
       </c>
-      <c r="D327" t="s">
+      <c r="D339" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="330" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B330" t="s">
+    <row r="342" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B342" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="331" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C331" t="s">
+    <row r="343" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C343" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="332" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D332" t="s">
+    <row r="344" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D344" t="s">
         <v>105</v>
       </c>
-      <c r="E332" s="1" t="s">
+      <c r="E344" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="333" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D333" t="s">
+    <row r="345" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D345" t="s">
         <v>102</v>
       </c>
-      <c r="E333" s="1" t="s">
+      <c r="E345" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="334" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D334" t="s">
+    <row r="346" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D346" t="s">
         <v>103</v>
       </c>
-      <c r="E334" s="1" t="s">
+      <c r="E346" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="335" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D335" t="s">
+    <row r="347" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D347" t="s">
         <v>108</v>
       </c>
-      <c r="E335" t="s">
+      <c r="E347" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="337" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B337" t="s">
+    <row r="349" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B349" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="338" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C338" t="s">
+    <row r="350" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C350" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="339" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D339" t="s">
+    <row r="351" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D351" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="340" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D340" t="s">
+    <row r="352" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D352" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="341" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F341" s="1" t="s">
+    <row r="353" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F353" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="342" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B342" t="s">
+    <row r="354" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B354" t="s">
         <v>1</v>
       </c>
-      <c r="F342" s="1" t="s">
+      <c r="F354" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="343" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C343" t="s">
+    <row r="355" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C355" t="s">
         <v>113</v>
       </c>
-      <c r="D343" s="1" t="s">
+      <c r="D355" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="344" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D344" t="s">
+    <row r="356" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D356" t="s">
         <v>127</v>
       </c>
-      <c r="E344" s="1" t="s">
+      <c r="E356" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="345" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C345" t="s">
+    <row r="357" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C357" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="346" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D346" t="s">
+    <row r="358" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D358" t="s">
         <v>116</v>
       </c>
-      <c r="E346" s="1" t="s">
+      <c r="E358" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F346" t="s">
+      <c r="F358" t="s">
         <v>129</v>
       </c>
-      <c r="G346" s="1" t="s">
+      <c r="G358" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="347" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E347" t="s">
+    <row r="359" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E359" t="s">
         <v>122</v>
       </c>
-      <c r="G347" s="1"/>
-    </row>
-    <row r="348" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E348" t="s">
+      <c r="G359" s="1"/>
+    </row>
+    <row r="360" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E360" t="s">
         <v>125</v>
       </c>
-      <c r="G348" s="1"/>
-    </row>
-    <row r="349" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D349" t="s">
+      <c r="G360" s="1"/>
+    </row>
+    <row r="361" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D361" t="s">
         <v>118</v>
       </c>
-      <c r="E349" s="1" t="s">
+      <c r="E361" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G349" s="1"/>
-    </row>
-    <row r="350" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D350" t="s">
+      <c r="G361" s="1"/>
+    </row>
+    <row r="362" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D362" t="s">
         <v>120</v>
       </c>
-      <c r="E350" s="1" t="s">
+      <c r="E362" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G350" s="1"/>
-    </row>
-    <row r="351" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E351" s="1" t="s">
+      <c r="G362" s="1"/>
+    </row>
+    <row r="363" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E363" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="G351" s="1"/>
-    </row>
-    <row r="352" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E352" t="s">
+      <c r="G363" s="1"/>
+    </row>
+    <row r="364" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E364" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="353" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D353" t="s">
+    <row r="365" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D365" t="s">
         <v>302</v>
       </c>
-      <c r="E353" s="1" t="s">
+      <c r="E365" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="354" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D354" t="s">
+    <row r="366" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D366" t="s">
         <v>301</v>
       </c>
-      <c r="E354" s="1" t="s">
+      <c r="E366" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="359" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C359" t="s">
+    <row r="371" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C371" t="s">
         <v>132</v>
       </c>
-      <c r="D359" s="1" t="s">
+      <c r="D371" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="363" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B363" t="s">
+    <row r="375" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B375" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="364" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C364" t="s">
+    <row r="376" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C376" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="365" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D365" t="s">
+    <row r="377" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D377" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="366" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E366" t="s">
+    <row r="378" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E378" t="s">
         <v>494</v>
       </c>
-      <c r="F366" s="1" t="s">
+      <c r="F378" s="1" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="367" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E367" t="s">
+    <row r="379" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E379" t="s">
         <v>496</v>
       </c>
-      <c r="F367" s="1" t="s">
+      <c r="F379" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="368" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E368" t="s">
+    <row r="380" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E380" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="369" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D369" t="s">
+    <row r="381" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D381" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="370" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E370" t="s">
+    <row r="382" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E382" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="371" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E371" t="s">
+    <row r="383" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E383" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="372" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D372" t="s">
+    <row r="384" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D384" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="373" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E373" t="s">
+    <row r="385" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E385" t="s">
         <v>501</v>
-      </c>
-    </row>
-    <row r="374" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C374" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="375" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D375" t="s">
-        <v>505</v>
-      </c>
-      <c r="E375" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="376" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D376" t="s">
-        <v>503</v>
-      </c>
-      <c r="E376" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="378" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C378" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="379" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D379" t="s">
-        <v>510</v>
-      </c>
-      <c r="E379" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="380" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D380" t="s">
-        <v>511</v>
-      </c>
-      <c r="E380" t="s">
-        <v>509</v>
-      </c>
-      <c r="G380" s="1" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="382" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C382" t="s">
-        <v>514</v>
-      </c>
-      <c r="G382" s="1" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="384" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C384" t="s">
-        <v>515</v>
-      </c>
-      <c r="E384" t="s">
-        <v>516</v>
-      </c>
-      <c r="G384" s="1" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="386" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C386" t="s">
-        <v>518</v>
+        <v>502</v>
       </c>
     </row>
     <row r="387" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D387" t="s">
-        <v>520</v>
+        <v>505</v>
       </c>
       <c r="E387" t="s">
-        <v>519</v>
-      </c>
-      <c r="G387" s="1" t="s">
-        <v>523</v>
+        <v>506</v>
       </c>
     </row>
     <row r="388" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D388" t="s">
-        <v>521</v>
+        <v>503</v>
       </c>
       <c r="E388" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
     </row>
     <row r="390" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C390" t="s">
-        <v>524</v>
+        <v>507</v>
       </c>
     </row>
     <row r="391" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D391" t="s">
-        <v>530</v>
+        <v>510</v>
       </c>
       <c r="E391" t="s">
-        <v>526</v>
-      </c>
-      <c r="G391" s="1" t="s">
-        <v>531</v>
+        <v>508</v>
       </c>
     </row>
     <row r="392" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D392" t="s">
-        <v>528</v>
+        <v>511</v>
       </c>
       <c r="E392" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="393" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D393" t="s">
-        <v>529</v>
-      </c>
-      <c r="E393" t="s">
-        <v>527</v>
+        <v>509</v>
+      </c>
+      <c r="G392" s="1" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="394" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C394" t="s">
+        <v>514</v>
+      </c>
+      <c r="G394" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="396" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C396" t="s">
+        <v>515</v>
+      </c>
+      <c r="E396" t="s">
+        <v>516</v>
+      </c>
+      <c r="G396" s="1" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="398" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C398" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="399" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D399" t="s">
+        <v>520</v>
+      </c>
+      <c r="E399" t="s">
+        <v>519</v>
+      </c>
+      <c r="G399" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="400" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D400" t="s">
+        <v>521</v>
+      </c>
+      <c r="E400" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="402" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C402" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="403" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D403" t="s">
+        <v>530</v>
+      </c>
+      <c r="E403" t="s">
+        <v>526</v>
+      </c>
+      <c r="G403" s="1" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="404" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D404" t="s">
+        <v>528</v>
+      </c>
+      <c r="E404" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="405" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D405" t="s">
+        <v>529</v>
+      </c>
+      <c r="E405" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="406" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C406" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="395" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D395" t="s">
+    <row r="407" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D407" t="s">
         <v>633</v>
       </c>
-      <c r="E395" t="s">
+      <c r="E407" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="396" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D396" t="s">
+    <row r="408" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D408" t="s">
         <v>635</v>
       </c>
-      <c r="E396" t="s">
+      <c r="E408" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="397" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D397" t="s">
+    <row r="409" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D409" t="s">
         <v>637</v>
       </c>
-      <c r="E397" t="s">
+      <c r="E409" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="398" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D398" t="s">
+    <row r="410" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D410" t="s">
         <v>640</v>
       </c>
-      <c r="E398" t="s">
+      <c r="E410" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="400" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C400" t="s">
+    <row r="411" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D411" t="s">
+        <v>697</v>
+      </c>
+      <c r="E411" t="s">
+        <v>699</v>
+      </c>
+      <c r="G411" s="1" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="417" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C417" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="401" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D401">
+    <row r="418" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D418">
         <v>1</v>
       </c>
     </row>
-    <row r="407" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B407" t="s">
+    <row r="424" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B424" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="408" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C408" t="s">
+    <row r="425" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C425" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="409" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D409" t="s">
+    <row r="426" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D426" t="s">
         <v>543</v>
       </c>
-      <c r="G409" s="1" t="s">
+      <c r="G426" s="1" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="410" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C410" t="s">
+    <row r="427" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C427" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="411" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D411" t="s">
+    <row r="428" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D428" t="s">
         <v>545</v>
       </c>
-      <c r="E411" t="s">
+      <c r="E428" t="s">
         <v>546</v>
       </c>
-      <c r="G411" s="1" t="s">
+      <c r="G428" s="1" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="413" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C413" t="s">
+    <row r="430" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C430" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="414" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D414" t="s">
+    <row r="431" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D431" t="s">
         <v>550</v>
       </c>
-      <c r="E414" t="s">
+      <c r="E431" t="s">
         <v>551</v>
       </c>
-      <c r="G414" s="1" t="s">
+      <c r="G431" s="1" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="415" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D415" t="s">
+    <row r="432" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D432" t="s">
         <v>552</v>
       </c>
-      <c r="E415" t="s">
+      <c r="E432" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="416" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D416" t="s">
+    <row r="433" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D433" t="s">
         <v>554</v>
       </c>
-      <c r="E416" t="s">
+      <c r="E433" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="417" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D417" t="s">
+    <row r="434" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D434" t="s">
         <v>556</v>
       </c>
-      <c r="E417" t="s">
+      <c r="E434" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="419" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C419" t="s">
+    <row r="436" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C436" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="420" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D420" t="s">
+    <row r="437" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D437" t="s">
         <v>560</v>
       </c>
-      <c r="E420" t="s">
+      <c r="E437" t="s">
         <v>562</v>
       </c>
-      <c r="G420" s="1" t="s">
+      <c r="G437" s="1" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="421" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D421" t="s">
+    <row r="438" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D438" t="s">
         <v>561</v>
       </c>
-      <c r="E421" t="s">
+      <c r="E438" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="423" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C423" t="s">
+    <row r="440" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C440" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="424" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D424" t="s">
+    <row r="441" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D441" t="s">
         <v>567</v>
       </c>
-      <c r="G424" s="1" t="s">
+      <c r="G441" s="1" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="425" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C425" t="s">
+    <row r="442" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C442" t="s">
         <v>611</v>
       </c>
-      <c r="G425" s="1"/>
-    </row>
-    <row r="426" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D426" t="s">
+      <c r="G442" s="1"/>
+    </row>
+    <row r="443" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D443" t="s">
         <v>612</v>
       </c>
-      <c r="E426" t="s">
+      <c r="E443" t="s">
         <v>613</v>
       </c>
-      <c r="G426" s="1" t="s">
+      <c r="G443" s="1" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="427" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="G427" s="1"/>
-    </row>
-    <row r="428" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="G428" s="1"/>
-    </row>
-    <row r="429" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="G429" s="1"/>
-    </row>
-    <row r="430" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="G430" s="1"/>
-    </row>
-    <row r="431" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="G431" s="1"/>
-    </row>
-    <row r="432" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="G432" s="1"/>
-    </row>
-    <row r="435" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B435" t="s">
+    <row r="444" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G444" s="1"/>
+    </row>
+    <row r="445" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G445" s="1"/>
+    </row>
+    <row r="446" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G446" s="1"/>
+    </row>
+    <row r="447" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G447" s="1"/>
+    </row>
+    <row r="448" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G448" s="1"/>
+    </row>
+    <row r="449" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G449" s="1"/>
+    </row>
+    <row r="452" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B452" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="436" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C436" t="s">
+    <row r="453" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C453" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="437" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E437" t="s">
+    <row r="454" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E454" t="s">
         <v>570</v>
       </c>
-      <c r="G437" s="1" t="s">
+      <c r="G454" s="1" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="440" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B440" t="s">
+    <row r="457" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B457" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="441" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C441" t="s">
+    <row r="458" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C458" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="442" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D442" t="s">
+    <row r="459" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D459" t="s">
         <v>574</v>
       </c>
-      <c r="E442" t="s">
+      <c r="E459" t="s">
         <v>575</v>
       </c>
-      <c r="F442" t="s">
+      <c r="F459" t="s">
         <v>576</v>
       </c>
-      <c r="G442" s="1" t="s">
+      <c r="G459" s="1" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="443" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E443" t="s">
+    <row r="460" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E460" t="s">
         <v>578</v>
       </c>
-      <c r="F443" t="s">
+      <c r="F460" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="444" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C444" t="s">
+    <row r="461" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C461" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="445" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D445" t="s">
+    <row r="462" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D462" t="s">
         <v>597</v>
       </c>
-      <c r="E445" t="s">
+      <c r="E462" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="446" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D446" t="s">
+    <row r="463" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D463" t="s">
         <v>600</v>
       </c>
-      <c r="E446" t="s">
+      <c r="E463" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="448" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D448" t="s">
+    <row r="465" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D465" t="s">
         <v>601</v>
       </c>
-      <c r="E448" t="s">
+      <c r="E465" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="449" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D449" t="s">
+    <row r="466" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D466" t="s">
         <v>603</v>
       </c>
-      <c r="E449" t="s">
+      <c r="E466" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="451" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D451" t="s">
+    <row r="468" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D468" t="s">
         <v>605</v>
       </c>
-      <c r="E451" t="s">
+      <c r="E468" t="s">
         <v>606</v>
       </c>
-      <c r="G451" s="1" t="s">
+      <c r="G468" s="1" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="452" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D452" t="s">
+    <row r="469" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D469" t="s">
         <v>607</v>
       </c>
-      <c r="E452" t="s">
+      <c r="E469" t="s">
         <v>608</v>
       </c>
-      <c r="F452" t="s">
+      <c r="F469" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="456" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B456" t="s">
+    <row r="473" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B473" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="457" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C457" t="s">
+    <row r="474" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C474" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="458" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D458" t="s">
+    <row r="475" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D475" t="s">
         <v>583</v>
       </c>
-      <c r="E458" t="s">
+      <c r="E475" t="s">
         <v>584</v>
       </c>
-      <c r="F458" t="s">
+      <c r="F475" t="s">
         <v>582</v>
       </c>
-      <c r="G458" s="1" t="s">
+      <c r="G475" s="1" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="459" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E459" t="s">
+    <row r="476" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E476" t="s">
         <v>585</v>
       </c>
-      <c r="F459" t="s">
+      <c r="F476" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="461" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D461" t="s">
+    <row r="478" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D478" t="s">
         <v>588</v>
       </c>
-      <c r="E461" t="s">
+      <c r="E478" t="s">
         <v>590</v>
       </c>
-      <c r="F461" t="s">
+      <c r="F478" t="s">
         <v>589</v>
       </c>
     </row>
@@ -5120,14 +5336,14 @@
     <hyperlink ref="D92" r:id="rId12" xr:uid="{BA9A8F05-4D7F-4942-886C-F8152208F0EA}"/>
     <hyperlink ref="F96" r:id="rId13" xr:uid="{22AE585F-7255-3F41-8A2E-808446F3A9AA}"/>
     <hyperlink ref="F98" r:id="rId14" xr:uid="{93472772-CF6C-D045-B634-2D574A3EE034}"/>
-    <hyperlink ref="E183" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
-    <hyperlink ref="F184" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
-    <hyperlink ref="D208" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
-    <hyperlink ref="D209" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
+    <hyperlink ref="E188" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
+    <hyperlink ref="F189" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
+    <hyperlink ref="D220" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
+    <hyperlink ref="D221" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
     <hyperlink ref="F99" r:id="rId19" xr:uid="{92BE3560-5393-C545-9D2D-2B773359B28F}"/>
-    <hyperlink ref="E225" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
-    <hyperlink ref="E226" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
-    <hyperlink ref="E227" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
+    <hyperlink ref="E237" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
+    <hyperlink ref="E238" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
+    <hyperlink ref="E239" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
     <hyperlink ref="E73" r:id="rId23" xr:uid="{1526D7DA-27DA-1443-928C-BEDA9E425734}"/>
     <hyperlink ref="E74" r:id="rId24" xr:uid="{4F363062-BE49-AB4F-8956-2C1F31D9B898}"/>
     <hyperlink ref="H100" r:id="rId25" xr:uid="{D9E13355-D59B-054F-B544-34A5A285A9E0}"/>
@@ -5144,7 +5360,7 @@
     <hyperlink ref="I100" r:id="rId36" xr:uid="{A03C56E4-1156-A148-A568-F50A5C33DB5C}"/>
     <hyperlink ref="F109" r:id="rId37" xr:uid="{12AC219C-4678-4E43-B328-6595FA10B8D3}"/>
     <hyperlink ref="E111" r:id="rId38" xr:uid="{44409621-28A2-704A-B283-3DCE1EFB1603}"/>
-    <hyperlink ref="E231" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
+    <hyperlink ref="E243" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
     <hyperlink ref="F112" r:id="rId40" xr:uid="{A9D0D792-87D1-8144-872F-5CA060D3C28F}"/>
     <hyperlink ref="F113" r:id="rId41" xr:uid="{87EF989D-17E9-1E45-A075-CD862D0B60F4}"/>
     <hyperlink ref="F115" r:id="rId42" xr:uid="{8406C6F0-DC69-A64D-AAD8-60A33C12D00B}"/>
@@ -5154,102 +5370,106 @@
     <hyperlink ref="F120" r:id="rId46" xr:uid="{3D1C62DB-D9B7-BE42-B21D-4EEBC4C9EFE1}"/>
     <hyperlink ref="F121" r:id="rId47" xr:uid="{F5021A21-70A2-D34E-B055-64CAC326E7EF}"/>
     <hyperlink ref="F122" r:id="rId48" xr:uid="{A8C010A1-8EE1-264B-8688-3BEA1B62E535}"/>
-    <hyperlink ref="E232" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
+    <hyperlink ref="E244" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
     <hyperlink ref="F117" r:id="rId50" location="113521" xr:uid="{EE1413C5-3B38-7D4D-8DF1-634A12F0BD81}"/>
     <hyperlink ref="E75" r:id="rId51" xr:uid="{00B1EF4A-7791-0343-8D8C-9A1E83248FC9}"/>
-    <hyperlink ref="E293" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
-    <hyperlink ref="E294" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
+    <hyperlink ref="E305" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
+    <hyperlink ref="E306" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
     <hyperlink ref="F124" r:id="rId54" xr:uid="{40A4B6A0-2F7E-A84D-8CC6-D814A33F5953}"/>
-    <hyperlink ref="E233" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
-    <hyperlink ref="E234" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
-    <hyperlink ref="E235" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
-    <hyperlink ref="E236" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
-    <hyperlink ref="E295" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
-    <hyperlink ref="D210" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
-    <hyperlink ref="D211" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
-    <hyperlink ref="D212" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
-    <hyperlink ref="E237" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
-    <hyperlink ref="E296" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
-    <hyperlink ref="E297" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
-    <hyperlink ref="E299" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
-    <hyperlink ref="E300" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
-    <hyperlink ref="F294" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
-    <hyperlink ref="G294" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
-    <hyperlink ref="E301" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
-    <hyperlink ref="E302" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
-    <hyperlink ref="E303" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
-    <hyperlink ref="E185" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
-    <hyperlink ref="E298" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
-    <hyperlink ref="E304" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
-    <hyperlink ref="E305" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
+    <hyperlink ref="E245" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
+    <hyperlink ref="E246" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
+    <hyperlink ref="E247" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
+    <hyperlink ref="E248" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
+    <hyperlink ref="E307" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
+    <hyperlink ref="D222" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
+    <hyperlink ref="D223" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
+    <hyperlink ref="D224" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
+    <hyperlink ref="E249" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
+    <hyperlink ref="E308" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
+    <hyperlink ref="E309" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
+    <hyperlink ref="E311" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
+    <hyperlink ref="E312" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
+    <hyperlink ref="F306" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
+    <hyperlink ref="G306" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
+    <hyperlink ref="E313" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
+    <hyperlink ref="E314" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
+    <hyperlink ref="E315" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
+    <hyperlink ref="E190" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
+    <hyperlink ref="E310" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
+    <hyperlink ref="E316" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
+    <hyperlink ref="E317" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
     <hyperlink ref="E77" r:id="rId77" location="code" xr:uid="{C0475FF8-517D-E949-887E-9A42D86E9640}"/>
-    <hyperlink ref="E307" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
+    <hyperlink ref="E319" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
     <hyperlink ref="E78" r:id="rId79" xr:uid="{277DBE6F-F3E5-8B4C-8DD8-BD92445D1A99}"/>
-    <hyperlink ref="E309" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
-    <hyperlink ref="E314" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
-    <hyperlink ref="E216" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
-    <hyperlink ref="E217" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
+    <hyperlink ref="E321" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
+    <hyperlink ref="E326" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
+    <hyperlink ref="E228" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
+    <hyperlink ref="E229" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
     <hyperlink ref="F145" r:id="rId84" xr:uid="{EB604865-A16B-0646-A5B5-0D047467449D}"/>
-    <hyperlink ref="E239" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
-    <hyperlink ref="D323" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
-    <hyperlink ref="D324" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
-    <hyperlink ref="E333" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
-    <hyperlink ref="E334" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
-    <hyperlink ref="E332" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
-    <hyperlink ref="D343" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
-    <hyperlink ref="E349" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
-    <hyperlink ref="E346" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
-    <hyperlink ref="E350" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
-    <hyperlink ref="F341" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
-    <hyperlink ref="F342" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
-    <hyperlink ref="E344" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
-    <hyperlink ref="G346" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
-    <hyperlink ref="D359" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
-    <hyperlink ref="E351" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
-    <hyperlink ref="E354" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
-    <hyperlink ref="E353" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
-    <hyperlink ref="F258" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
-    <hyperlink ref="E259" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
-    <hyperlink ref="E260" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
-    <hyperlink ref="E261" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
-    <hyperlink ref="G275" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
-    <hyperlink ref="E270" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
-    <hyperlink ref="E271" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
-    <hyperlink ref="E276" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
-    <hyperlink ref="F152" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
-    <hyperlink ref="F157" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
-    <hyperlink ref="F158" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
-    <hyperlink ref="F164" r:id="rId114" xr:uid="{2B03B1F0-535A-3E4F-8FB3-35D2DE847218}"/>
-    <hyperlink ref="G169" r:id="rId115" xr:uid="{11045522-E183-B14C-B43D-5EA36E454600}"/>
-    <hyperlink ref="E186" r:id="rId116" xr:uid="{F1098A8C-3BC0-DB4F-8F9C-48B31145FEC1}"/>
-    <hyperlink ref="F171" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
-    <hyperlink ref="F165" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
-    <hyperlink ref="F174" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
-    <hyperlink ref="H254" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
-    <hyperlink ref="F366" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
-    <hyperlink ref="G380" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
-    <hyperlink ref="F367" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
-    <hyperlink ref="G382" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
-    <hyperlink ref="G384" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
-    <hyperlink ref="G387" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
-    <hyperlink ref="G391" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
-    <hyperlink ref="G411" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
-    <hyperlink ref="G409" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
-    <hyperlink ref="G414" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
-    <hyperlink ref="G420" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
-    <hyperlink ref="G424" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
-    <hyperlink ref="G437" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
-    <hyperlink ref="G442" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
-    <hyperlink ref="G458" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
+    <hyperlink ref="E251" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
+    <hyperlink ref="D335" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
+    <hyperlink ref="D336" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
+    <hyperlink ref="E345" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
+    <hyperlink ref="E346" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
+    <hyperlink ref="E344" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
+    <hyperlink ref="D355" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
+    <hyperlink ref="E361" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
+    <hyperlink ref="E358" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
+    <hyperlink ref="E362" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
+    <hyperlink ref="F353" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
+    <hyperlink ref="F354" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
+    <hyperlink ref="E356" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
+    <hyperlink ref="G358" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
+    <hyperlink ref="D371" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
+    <hyperlink ref="E363" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
+    <hyperlink ref="E366" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
+    <hyperlink ref="E365" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
+    <hyperlink ref="F270" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
+    <hyperlink ref="E271" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
+    <hyperlink ref="E272" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
+    <hyperlink ref="E273" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
+    <hyperlink ref="G287" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
+    <hyperlink ref="E282" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
+    <hyperlink ref="E283" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
+    <hyperlink ref="E288" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
+    <hyperlink ref="F157" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
+    <hyperlink ref="F162" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
+    <hyperlink ref="F163" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
+    <hyperlink ref="F169" r:id="rId114" xr:uid="{2B03B1F0-535A-3E4F-8FB3-35D2DE847218}"/>
+    <hyperlink ref="G174" r:id="rId115" xr:uid="{11045522-E183-B14C-B43D-5EA36E454600}"/>
+    <hyperlink ref="E191" r:id="rId116" xr:uid="{F1098A8C-3BC0-DB4F-8F9C-48B31145FEC1}"/>
+    <hyperlink ref="F176" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
+    <hyperlink ref="F170" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
+    <hyperlink ref="F179" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
+    <hyperlink ref="H266" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
+    <hyperlink ref="F378" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
+    <hyperlink ref="G392" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
+    <hyperlink ref="F379" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
+    <hyperlink ref="G394" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
+    <hyperlink ref="G396" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
+    <hyperlink ref="G399" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
+    <hyperlink ref="G403" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
+    <hyperlink ref="G428" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
+    <hyperlink ref="G426" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
+    <hyperlink ref="G431" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
+    <hyperlink ref="G437" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
+    <hyperlink ref="G441" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
+    <hyperlink ref="G454" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
+    <hyperlink ref="G459" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
+    <hyperlink ref="G475" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
     <hyperlink ref="E20" r:id="rId136" xr:uid="{809CA2D1-39E9-0045-A4DF-E4C0C2E97FA2}"/>
     <hyperlink ref="E21" r:id="rId137" xr:uid="{5DC44543-F2B9-F841-9097-6DB19C5EBD82}"/>
-    <hyperlink ref="G451" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
-    <hyperlink ref="G426" r:id="rId139" xr:uid="{7F4EA1D7-8774-1A4B-BF25-18ED0416CB20}"/>
-    <hyperlink ref="F197" r:id="rId140" xr:uid="{101513F3-87A1-DA41-8BF5-E4029309ECB8}"/>
-    <hyperlink ref="F189" r:id="rId141" xr:uid="{494E255E-6912-8643-B5CD-1D65E0DDCFFC}"/>
-    <hyperlink ref="F190" r:id="rId142" xr:uid="{828F749D-83DE-C14E-B637-56047AC1B384}"/>
-    <hyperlink ref="F198" r:id="rId143" xr:uid="{435D9B3C-98B6-5E49-BD30-EAA53523CDB7}"/>
-    <hyperlink ref="F199" r:id="rId144" xr:uid="{7D905409-0097-E04E-9593-2DEEBEEA0D0F}"/>
+    <hyperlink ref="G468" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
+    <hyperlink ref="G443" r:id="rId139" xr:uid="{7F4EA1D7-8774-1A4B-BF25-18ED0416CB20}"/>
+    <hyperlink ref="F209" r:id="rId140" xr:uid="{101513F3-87A1-DA41-8BF5-E4029309ECB8}"/>
+    <hyperlink ref="F194" r:id="rId141" xr:uid="{494E255E-6912-8643-B5CD-1D65E0DDCFFC}"/>
+    <hyperlink ref="F195" r:id="rId142" xr:uid="{828F749D-83DE-C14E-B637-56047AC1B384}"/>
+    <hyperlink ref="F210" r:id="rId143" xr:uid="{435D9B3C-98B6-5E49-BD30-EAA53523CDB7}"/>
+    <hyperlink ref="F211" r:id="rId144" xr:uid="{7D905409-0097-E04E-9593-2DEEBEEA0D0F}"/>
+    <hyperlink ref="F149" r:id="rId145" xr:uid="{64451146-E88A-9A47-9888-71BEAC8B984E}"/>
+    <hyperlink ref="F199" r:id="rId146" xr:uid="{28F6BA28-EB9B-374C-A8A0-4077C800D23A}"/>
+    <hyperlink ref="G411" r:id="rId147" xr:uid="{20B4F69E-7592-784A-8C2E-123726A51D93}"/>
+    <hyperlink ref="F202" r:id="rId148" xr:uid="{E3C3D7C6-1E6E-FF40-8CC7-6CF1C77457E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5257,10 +5477,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G37"/>
+  <dimension ref="B2:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5683,11 +5903,77 @@
       <c r="B37" t="s">
         <v>667</v>
       </c>
+      <c r="D37" t="s">
+        <v>448</v>
+      </c>
       <c r="E37" t="s">
         <v>668</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>669</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>670</v>
+      </c>
+      <c r="E38" t="s">
+        <v>671</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>673</v>
+      </c>
+      <c r="E39" t="s">
+        <v>674</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>677</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>701</v>
+      </c>
+      <c r="C41" t="s">
+        <v>169</v>
+      </c>
+      <c r="D41" t="s">
+        <v>448</v>
+      </c>
+      <c r="E41" t="s">
+        <v>702</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E42" t="s">
+        <v>703</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>706</v>
+      </c>
+      <c r="E43" t="s">
+        <v>705</v>
       </c>
     </row>
   </sheetData>
@@ -5729,6 +6015,45 @@
     <hyperlink ref="F31" r:id="rId35" xr:uid="{A7216F86-E62C-AC48-B73F-76B2F894E6AD}"/>
     <hyperlink ref="F36" r:id="rId36" xr:uid="{EF122EDE-6CCB-2440-885D-B71D42E7B9FC}"/>
     <hyperlink ref="F37" r:id="rId37" xr:uid="{BF8E0884-4A84-1F45-BA3C-ED13206AFD16}"/>
+    <hyperlink ref="F38" r:id="rId38" xr:uid="{9681BD46-5396-7440-B882-B1583CAE5943}"/>
+    <hyperlink ref="F39" r:id="rId39" xr:uid="{39C3E3AB-01D7-2F4D-9A3A-06298BFC708F}"/>
+    <hyperlink ref="B40" r:id="rId40" display="https://www.psycopg.org/docs/usage.html" xr:uid="{C9644E87-5A6B-A846-9339-6FA311DD0BA2}"/>
+    <hyperlink ref="F40" r:id="rId41" xr:uid="{E6B6E8F4-8639-C840-8681-46C64199EB24}"/>
+    <hyperlink ref="F41" r:id="rId42" xr:uid="{40E80A1C-8ED4-6A46-9A85-FCDFAE78A259}"/>
+    <hyperlink ref="F42" r:id="rId43" xr:uid="{9D29BD03-9629-9E49-96DD-B8A60F3ED613}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0197339E-8847-2643-B704-6685D2B6003F}">
+  <dimension ref="B2:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="43.5" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>694</v>
+      </c>
+      <c r="C2" t="s">
+        <v>695</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>696</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{873D2056-9786-E449-90A5-241092683CCA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added directory 'Cheat Sheets' and its subdirectories
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24249F2B-7225-B34B-A4A8-3A7CAF3568E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AC8B24-C7CE-864B-8F1E-87F4D8004526}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="560" windowWidth="25600" windowHeight="15340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="726">
   <si>
     <t>docker</t>
   </si>
@@ -2170,6 +2170,54 @@
   </si>
   <si>
     <t>https://stackoverflow.com/questions/52126116/prevent-pip-from-installing-some-dependencies</t>
+  </si>
+  <si>
+    <t>Software License Explained</t>
+  </si>
+  <si>
+    <t>The MIT, BSD, and ISC licenses</t>
+  </si>
+  <si>
+    <t>The Apache license</t>
+  </si>
+  <si>
+    <t>The GPL licenses (GPLv3, GPLv2, LGPL, Affero GPL)</t>
+  </si>
+  <si>
+    <t>do whatever you want with this, just don’t sue me.</t>
+  </si>
+  <si>
+    <t>does so (MIT) with many more words</t>
+  </si>
+  <si>
+    <t>if you make a derivative work of this, you have to provide the source code under this license</t>
+  </si>
+  <si>
+    <t>https://exygy.com/blog/which-license-should-i-use-mit-vs-apache-vs-gpl/</t>
+  </si>
+  <si>
+    <t>https://www.datacamp.com/community/tutorials/docstrings-python</t>
+  </si>
+  <si>
+    <t>Docstrings in Python</t>
+  </si>
+  <si>
+    <t>https://www.freecodecamp.org/news/build-your-first-python-package/</t>
+  </si>
+  <si>
+    <t>from subtract import subtract</t>
+  </si>
+  <si>
+    <t>./build_deploy.sh --test</t>
+  </si>
+  <si>
+    <t>https://towardsdatascience.com/how-to-build-your-first-python-package-6a00b02635c9</t>
+  </si>
+  <si>
+    <t>How to Build Your First Python Package</t>
+  </si>
+  <si>
+    <t>How to Build Your Very First Python Package (simple version)</t>
   </si>
 </sst>
 </file>
@@ -2631,11 +2679,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I478"/>
+  <dimension ref="B1:I484"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F203" sqref="F203"/>
+      <pane ySplit="1" topLeftCell="A468" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C490" sqref="C490"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5318,6 +5366,38 @@
       </c>
       <c r="F478" t="s">
         <v>589</v>
+      </c>
+    </row>
+    <row r="481" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B481" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="482" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C482" t="s">
+        <v>711</v>
+      </c>
+      <c r="D482" t="s">
+        <v>714</v>
+      </c>
+      <c r="G482" s="1" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="483" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C483" t="s">
+        <v>712</v>
+      </c>
+      <c r="D483" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="484" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C484" t="s">
+        <v>713</v>
+      </c>
+      <c r="D484" t="s">
+        <v>716</v>
       </c>
     </row>
   </sheetData>
@@ -5470,6 +5550,7 @@
     <hyperlink ref="F199" r:id="rId146" xr:uid="{28F6BA28-EB9B-374C-A8A0-4077C800D23A}"/>
     <hyperlink ref="G411" r:id="rId147" xr:uid="{20B4F69E-7592-784A-8C2E-123726A51D93}"/>
     <hyperlink ref="F202" r:id="rId148" xr:uid="{E3C3D7C6-1E6E-FF40-8CC7-6CF1C77457E4}"/>
+    <hyperlink ref="G482" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5477,10 +5558,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G43"/>
+  <dimension ref="B2:G46"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5974,6 +6055,36 @@
       </c>
       <c r="E43" t="s">
         <v>705</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>719</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>725</v>
+      </c>
+      <c r="E45" t="s">
+        <v>721</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>724</v>
+      </c>
+      <c r="E46" t="s">
+        <v>722</v>
+      </c>
+      <c r="F46" t="s">
+        <v>723</v>
       </c>
     </row>
   </sheetData>
@@ -6021,6 +6132,8 @@
     <hyperlink ref="F40" r:id="rId41" xr:uid="{E6B6E8F4-8639-C840-8681-46C64199EB24}"/>
     <hyperlink ref="F41" r:id="rId42" xr:uid="{40E80A1C-8ED4-6A46-9A85-FCDFAE78A259}"/>
     <hyperlink ref="F42" r:id="rId43" xr:uid="{9D29BD03-9629-9E49-96DD-B8A60F3ED613}"/>
+    <hyperlink ref="F44" r:id="rId44" xr:uid="{534D43BE-9A8C-7046-82FA-3CCA4C01475A}"/>
+    <hyperlink ref="F45" r:id="rId45" xr:uid="{721A8C5E-A827-9D4D-A7B9-B660588D9790}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for pandas pipe
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8356D61-2495-9A45-BB02-AE3A897F149E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68077F15-37CA-7C4F-90CB-B90465904499}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="734">
   <si>
     <t>docker</t>
   </si>
@@ -2233,6 +2233,15 @@
   </si>
   <si>
     <t>Google Python Style Guide</t>
+  </si>
+  <si>
+    <t>https://towardsdatascience.com/using-pandas-pipe-function-to-improve-code-readability-96d66abfaf8</t>
+  </si>
+  <si>
+    <t>Using Pandas pipe function to improve code readability</t>
+  </si>
+  <si>
+    <t>df.pipe(), return df</t>
   </si>
 </sst>
 </file>
@@ -5577,10 +5586,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G48"/>
+  <dimension ref="B2:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45:F45"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6120,6 +6129,20 @@
       </c>
       <c r="F48" s="1" t="s">
         <v>726</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>732</v>
+      </c>
+      <c r="D49" t="s">
+        <v>448</v>
+      </c>
+      <c r="E49" t="s">
+        <v>733</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>731</v>
       </c>
     </row>
   </sheetData>
@@ -6171,6 +6194,7 @@
     <hyperlink ref="F46" r:id="rId45" xr:uid="{721A8C5E-A827-9D4D-A7B9-B660588D9790}"/>
     <hyperlink ref="F48" r:id="rId46" xr:uid="{84D26437-907E-7D45-A77A-85E9B9E6A208}"/>
     <hyperlink ref="F45" r:id="rId47" xr:uid="{40310FEF-9179-3C46-97A9-94459A181192}"/>
+    <hyperlink ref="F49" r:id="rId48" xr:uid="{23062DE1-DBA6-6945-AC55-802C0A2CD844}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for SQL
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68077F15-37CA-7C4F-90CB-B90465904499}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6918D6F-CB1C-904B-92C5-79378E6B34BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="734">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="746">
   <si>
     <t>docker</t>
   </si>
@@ -2242,6 +2242,42 @@
   </si>
   <si>
     <t>df.pipe(), return df</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>build derived table</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/39803103/select-the-first-row-for-each-group-in-mysql</t>
+  </si>
+  <si>
+    <t>online playground</t>
+  </si>
+  <si>
+    <t>https://www.db-fiddle.com</t>
+  </si>
+  <si>
+    <t>CONCAT_WS</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/15055540/mysql-create-freqency-distribution</t>
+  </si>
+  <si>
+    <t>Mysql create freqency distribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cumulative Sum-Running </t>
+  </si>
+  <si>
+    <t xml:space="preserve">running_total </t>
+  </si>
+  <si>
+    <t>https://popsql.com/learn-sql/mysql/how-to-calculate-cumulative-sum-running-total-in-mysql</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/2563918/create-a-cumulative-sum-column-in-mysql</t>
   </si>
 </sst>
 </file>
@@ -2703,11 +2739,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I484"/>
+  <dimension ref="B1:I490"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G170" sqref="G170"/>
+      <pane ySplit="1" topLeftCell="A474" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C491" sqref="C491"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5425,6 +5461,38 @@
       </c>
       <c r="D484" t="s">
         <v>716</v>
+      </c>
+    </row>
+    <row r="487" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B487" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="488" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C488" t="s">
+        <v>735</v>
+      </c>
+      <c r="G488" s="1" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="489" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C489" t="s">
+        <v>737</v>
+      </c>
+      <c r="G489" s="1" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="490" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C490" t="s">
+        <v>741</v>
+      </c>
+      <c r="F490" t="s">
+        <v>739</v>
+      </c>
+      <c r="G490" s="1" t="s">
+        <v>740</v>
       </c>
     </row>
   </sheetData>
@@ -5579,6 +5647,9 @@
     <hyperlink ref="F202" r:id="rId148" xr:uid="{E3C3D7C6-1E6E-FF40-8CC7-6CF1C77457E4}"/>
     <hyperlink ref="G482" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
     <hyperlink ref="G169" r:id="rId150" xr:uid="{9BECD448-C575-B64B-BA3F-BEE8D1CBBD43}"/>
+    <hyperlink ref="G488" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
+    <hyperlink ref="G489" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
+    <hyperlink ref="G490" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5586,10 +5657,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G49"/>
+  <dimension ref="B2:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6143,6 +6214,22 @@
       </c>
       <c r="F49" s="1" t="s">
         <v>731</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>742</v>
+      </c>
+      <c r="E51" t="s">
+        <v>743</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F52" s="1" t="s">
+        <v>745</v>
       </c>
     </row>
   </sheetData>
@@ -6195,6 +6282,8 @@
     <hyperlink ref="F48" r:id="rId46" xr:uid="{84D26437-907E-7D45-A77A-85E9B9E6A208}"/>
     <hyperlink ref="F45" r:id="rId47" xr:uid="{40310FEF-9179-3C46-97A9-94459A181192}"/>
     <hyperlink ref="F49" r:id="rId48" xr:uid="{23062DE1-DBA6-6945-AC55-802C0A2CD844}"/>
+    <hyperlink ref="F51" r:id="rId49" xr:uid="{FF9072C2-3183-A945-AF8E-32D4E261E3A9}"/>
+    <hyperlink ref="F52" r:id="rId50" xr:uid="{3C8AC7EE-5054-294D-87D4-1A6913F0B8B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for Faust
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6918D6F-CB1C-904B-92C5-79378E6B34BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05551C29-617A-2249-A3FE-634F5296C497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
     <sheet name="Random Articles" sheetId="4" r:id="rId2"/>
     <sheet name="Tips" sheetId="5" r:id="rId3"/>
+    <sheet name="Websites" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="758">
   <si>
     <t>docker</t>
   </si>
@@ -2278,6 +2279,42 @@
   </si>
   <si>
     <t>https://stackoverflow.com/questions/2563918/create-a-cumulative-sum-column-in-mysql</t>
+  </si>
+  <si>
+    <t>Faust</t>
+  </si>
+  <si>
+    <t>Integration with other tools</t>
+  </si>
+  <si>
+    <t>redis, http, influxDB, elasticsearch</t>
+  </si>
+  <si>
+    <t>https://robinhood.engineering/adding-faust-to-your-existing-architecture-39b0ebd1f7c9</t>
+  </si>
+  <si>
+    <t>Faust-Example Docker</t>
+  </si>
+  <si>
+    <t>Ryan Whitten</t>
+  </si>
+  <si>
+    <t>https://github.com/rwhitten577/faust-example</t>
+  </si>
+  <si>
+    <t>How to send an email with python logger?</t>
+  </si>
+  <si>
+    <t>logging.handlers.SMTPHandler</t>
+  </si>
+  <si>
+    <t>https://medium.com/@sutharprashant199722/how-to-send-an-email-with-python-logger-785961c89465</t>
+  </si>
+  <si>
+    <t>Circuits and Simulate</t>
+  </si>
+  <si>
+    <t>https://www.multisim.com/</t>
   </si>
 </sst>
 </file>
@@ -2342,7 +2379,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2356,6 +2393,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2739,11 +2777,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I490"/>
+  <dimension ref="B1:I494"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A474" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C491" sqref="C491"/>
+      <pane ySplit="1" topLeftCell="A472" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A492" sqref="A492:XFD494"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5493,6 +5531,33 @@
       </c>
       <c r="G490" s="1" t="s">
         <v>740</v>
+      </c>
+    </row>
+    <row r="492" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B492" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="493" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C493" t="s">
+        <v>747</v>
+      </c>
+      <c r="D493" t="s">
+        <v>748</v>
+      </c>
+      <c r="G493" s="1" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="494" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C494" t="s">
+        <v>750</v>
+      </c>
+      <c r="D494" t="s">
+        <v>751</v>
+      </c>
+      <c r="G494" s="1" t="s">
+        <v>752</v>
       </c>
     </row>
   </sheetData>
@@ -5650,6 +5715,8 @@
     <hyperlink ref="G488" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
     <hyperlink ref="G489" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
     <hyperlink ref="G490" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
+    <hyperlink ref="G493" r:id="rId154" xr:uid="{FB93E0B8-2537-FD47-8420-84D2A706F697}"/>
+    <hyperlink ref="G494" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5657,10 +5724,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G52"/>
+  <dimension ref="B2:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6216,19 +6283,30 @@
         <v>731</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>753</v>
+      </c>
+      <c r="E50" t="s">
+        <v>754</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
         <v>742</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E52" t="s">
         <v>743</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>744</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F52" s="1" t="s">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F53" s="1" t="s">
         <v>745</v>
       </c>
     </row>
@@ -6282,8 +6360,9 @@
     <hyperlink ref="F48" r:id="rId46" xr:uid="{84D26437-907E-7D45-A77A-85E9B9E6A208}"/>
     <hyperlink ref="F45" r:id="rId47" xr:uid="{40310FEF-9179-3C46-97A9-94459A181192}"/>
     <hyperlink ref="F49" r:id="rId48" xr:uid="{23062DE1-DBA6-6945-AC55-802C0A2CD844}"/>
-    <hyperlink ref="F51" r:id="rId49" xr:uid="{FF9072C2-3183-A945-AF8E-32D4E261E3A9}"/>
-    <hyperlink ref="F52" r:id="rId50" xr:uid="{3C8AC7EE-5054-294D-87D4-1A6913F0B8B2}"/>
+    <hyperlink ref="F52" r:id="rId49" xr:uid="{FF9072C2-3183-A945-AF8E-32D4E261E3A9}"/>
+    <hyperlink ref="F53" r:id="rId50" xr:uid="{3C8AC7EE-5054-294D-87D4-1A6913F0B8B2}"/>
+    <hyperlink ref="F50" r:id="rId51" xr:uid="{B9356038-CF05-854A-AFF1-D7384A989DFB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6320,4 +6399,31 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069EEB69-0D57-C040-8545-840D5862E858}">
+  <dimension ref="B2:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>756</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="D2" s="7"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{87D156EE-D133-464D-8B0D-7B076D239955}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added tips for git
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05551C29-617A-2249-A3FE-634F5296C497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AAF8B8-597C-DA4A-A835-3D0477390FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3380" yWindow="2280" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="766">
   <si>
     <t>docker</t>
   </si>
@@ -2315,6 +2315,30 @@
   </si>
   <si>
     <t>https://www.multisim.com/</t>
+  </si>
+  <si>
+    <t>12. reduce the size of .git file</t>
+  </si>
+  <si>
+    <t>git gc --prune=now --aggressive</t>
+  </si>
+  <si>
+    <t>git reflog expire --all --expire=now</t>
+  </si>
+  <si>
+    <t>1.  cleaning the reflog can help</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/2116778/reduce-git-repository-size/2116892#2116892</t>
+  </si>
+  <si>
+    <t>3. show branches</t>
+  </si>
+  <si>
+    <t>git branch -vv   # doubly verbose!</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/4950725/how-can-i-see-which-git-branches-are-tracking-which-remote-upstream-branch</t>
   </si>
 </sst>
 </file>
@@ -2777,11 +2801,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I494"/>
+  <dimension ref="B1:I500"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A472" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A492" sqref="A492:XFD494"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G169" sqref="G169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3811,384 +3835,382 @@
       </c>
     </row>
     <row r="168" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="F168" s="1"/>
+      <c r="D168" t="s">
+        <v>763</v>
+      </c>
+      <c r="E168" t="s">
+        <v>764</v>
+      </c>
+      <c r="G168" s="1" t="s">
+        <v>765</v>
+      </c>
     </row>
     <row r="169" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C169" t="s">
+      <c r="F169" s="1"/>
+    </row>
+    <row r="170" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C170" t="s">
         <v>393</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D170" t="s">
         <v>421</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E170" t="s">
         <v>394</v>
       </c>
-      <c r="F169" s="1" t="s">
+      <c r="F170" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G169" s="1" t="s">
+      <c r="G170" s="1" t="s">
         <v>728</v>
-      </c>
-    </row>
-    <row r="170" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D170" t="s">
-        <v>422</v>
-      </c>
-      <c r="E170" t="s">
-        <v>423</v>
-      </c>
-      <c r="F170" s="1" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="171" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D171" t="s">
+        <v>422</v>
+      </c>
+      <c r="E171" t="s">
+        <v>423</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="172" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D172" t="s">
         <v>425</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E172" t="s">
         <v>426</v>
       </c>
-      <c r="F171" s="1"/>
-    </row>
-    <row r="172" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C172" t="s">
+      <c r="F172" s="1"/>
+    </row>
+    <row r="173" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C173" t="s">
         <v>395</v>
-      </c>
-      <c r="F172" s="1"/>
-    </row>
-    <row r="173" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D173" t="s">
-        <v>397</v>
-      </c>
-      <c r="E173" t="s">
-        <v>396</v>
       </c>
       <c r="F173" s="1"/>
     </row>
     <row r="174" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D174" t="s">
+        <v>397</v>
+      </c>
+      <c r="E174" t="s">
+        <v>396</v>
+      </c>
+      <c r="F174" s="1"/>
+    </row>
+    <row r="175" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D175" t="s">
         <v>398</v>
       </c>
-      <c r="F174" t="s">
+      <c r="F175" t="s">
         <v>399</v>
       </c>
-      <c r="G174" s="1" t="s">
+      <c r="G175" s="1" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="175" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C175" t="s">
+    <row r="176" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C176" t="s">
         <v>417</v>
       </c>
-      <c r="G175" s="1"/>
-    </row>
-    <row r="176" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E176" t="s">
+      <c r="G176" s="1"/>
+    </row>
+    <row r="177" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E177" t="s">
         <v>418</v>
       </c>
-      <c r="F176" s="1" t="s">
+      <c r="F177" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="G176" s="1"/>
-    </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E177" t="s">
+      <c r="G177" s="1"/>
+    </row>
+    <row r="178" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E178" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C178" t="s">
+    <row r="179" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C179" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D179" t="s">
+    <row r="180" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D180" t="s">
         <v>433</v>
       </c>
-      <c r="E179" t="s">
+      <c r="E180" t="s">
         <v>435</v>
       </c>
-      <c r="F179" s="1" t="s">
+      <c r="F180" s="1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D180" t="s">
+    <row r="181" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D181" t="s">
         <v>434</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E181" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="186" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B186" t="s">
+    <row r="182" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C182" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="183" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D183" t="s">
+        <v>761</v>
+      </c>
+      <c r="E183" t="s">
+        <v>760</v>
+      </c>
+      <c r="F183" s="1" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="184" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E184" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="192" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B192" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="187" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C187" t="s">
+    <row r="193" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C193" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="188" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D188" t="s">
+    <row r="194" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D194" t="s">
         <v>171</v>
       </c>
-      <c r="E188" s="1" t="s">
+      <c r="E194" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="189" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D189" t="s">
+    <row r="195" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D195" t="s">
         <v>175</v>
       </c>
-      <c r="E189" t="s">
+      <c r="E195" t="s">
         <v>173</v>
       </c>
-      <c r="F189" s="1" t="s">
+      <c r="F195" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="190" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C190" t="s">
+    <row r="196" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C196" t="s">
         <v>322</v>
       </c>
-      <c r="E190" s="1" t="s">
+      <c r="E196" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="F190" s="1"/>
-    </row>
-    <row r="191" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C191" t="s">
+      <c r="F196" s="1"/>
+    </row>
+    <row r="197" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C197" t="s">
         <v>406</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D197" t="s">
         <v>407</v>
       </c>
-      <c r="E191" s="1" t="s">
+      <c r="E197" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="F191" s="1"/>
-    </row>
-    <row r="192" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D192" t="s">
+      <c r="F197" s="1"/>
+    </row>
+    <row r="198" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D198" t="s">
         <v>408</v>
       </c>
-      <c r="F192" s="1"/>
-    </row>
-    <row r="193" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F193" s="1"/>
-    </row>
-    <row r="194" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C194" t="s">
-        <v>618</v>
-      </c>
-      <c r="D194" t="s">
-        <v>619</v>
-      </c>
-      <c r="F194" s="1" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="195" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C195" t="s">
-        <v>622</v>
-      </c>
-      <c r="D195" t="s">
-        <v>621</v>
-      </c>
-      <c r="F195" s="1" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="196" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F196" s="1"/>
-    </row>
-    <row r="197" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F197" s="1"/>
-    </row>
-    <row r="198" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B198" t="s">
-        <v>686</v>
-      </c>
       <c r="F198" s="1"/>
     </row>
     <row r="199" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C199" t="s">
-        <v>687</v>
-      </c>
-      <c r="D199" t="s">
-        <v>689</v>
-      </c>
-      <c r="F199" s="1" t="s">
-        <v>691</v>
-      </c>
+      <c r="F199" s="1"/>
     </row>
     <row r="200" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C200" t="s">
-        <v>688</v>
+        <v>618</v>
       </c>
       <c r="D200" t="s">
-        <v>690</v>
-      </c>
-      <c r="F200" s="1"/>
+        <v>619</v>
+      </c>
+      <c r="F200" s="1" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="201" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C201" t="s">
-        <v>692</v>
+        <v>622</v>
       </c>
       <c r="D201" t="s">
-        <v>693</v>
-      </c>
-      <c r="F201" s="1"/>
+        <v>621</v>
+      </c>
+      <c r="F201" s="1" t="s">
+        <v>623</v>
+      </c>
     </row>
     <row r="202" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C202" t="s">
-        <v>707</v>
-      </c>
-      <c r="D202" t="s">
-        <v>708</v>
-      </c>
-      <c r="F202" s="1" t="s">
-        <v>709</v>
-      </c>
+      <c r="F202" s="1"/>
     </row>
     <row r="203" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F203" s="1"/>
     </row>
     <row r="204" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B204" t="s">
+        <v>686</v>
+      </c>
       <c r="F204" s="1"/>
     </row>
     <row r="205" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F205" s="1"/>
+      <c r="C205" t="s">
+        <v>687</v>
+      </c>
+      <c r="D205" t="s">
+        <v>689</v>
+      </c>
+      <c r="F205" s="1" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="206" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C206" t="s">
+        <v>688</v>
+      </c>
+      <c r="D206" t="s">
+        <v>690</v>
+      </c>
       <c r="F206" s="1"/>
     </row>
+    <row r="207" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C207" t="s">
+        <v>692</v>
+      </c>
+      <c r="D207" t="s">
+        <v>693</v>
+      </c>
+      <c r="F207" s="1"/>
+    </row>
     <row r="208" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B208" t="s">
+      <c r="C208" t="s">
+        <v>707</v>
+      </c>
+      <c r="D208" t="s">
+        <v>708</v>
+      </c>
+      <c r="F208" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="209" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F209" s="1"/>
+    </row>
+    <row r="210" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F210" s="1"/>
+    </row>
+    <row r="211" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F211" s="1"/>
+    </row>
+    <row r="212" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F212" s="1"/>
+    </row>
+    <row r="214" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B214" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="209" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C209" t="s">
+    <row r="215" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C215" t="s">
         <v>616</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D215" t="s">
         <v>615</v>
       </c>
-      <c r="F209" s="1" t="s">
+      <c r="F215" s="1" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="210" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C210" t="s">
+    <row r="216" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C216" t="s">
         <v>624</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D216" t="s">
         <v>625</v>
       </c>
-      <c r="F210" s="1" t="s">
+      <c r="F216" s="1" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C211" t="s">
+    <row r="217" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C217" t="s">
         <v>628</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D217" t="s">
         <v>627</v>
       </c>
-      <c r="F211" s="1" t="s">
+      <c r="F217" s="1" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="212" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C212" t="s">
+    <row r="218" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C218" t="s">
         <v>631</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D218" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="219" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B219" t="s">
+    <row r="225" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B225" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="220" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C220" t="s">
+    <row r="226" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C226" t="s">
         <v>176</v>
       </c>
-      <c r="D220" s="1" t="s">
+      <c r="D226" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="221" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C221" t="s">
+    <row r="227" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C227" t="s">
         <v>178</v>
       </c>
-      <c r="D221" s="1" t="s">
+      <c r="D227" s="1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="222" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C222" t="s">
-        <v>293</v>
-      </c>
-      <c r="D222" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="223" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C223" t="s">
-        <v>294</v>
-      </c>
-      <c r="D223" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="224" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C224" t="s">
-        <v>297</v>
-      </c>
-      <c r="D224" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="225" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D225" s="1"/>
-    </row>
-    <row r="226" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D226" s="1"/>
-    </row>
-    <row r="227" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B227" t="s">
-        <v>343</v>
-      </c>
-      <c r="D227" s="1"/>
     </row>
     <row r="228" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C228" t="s">
-        <v>344</v>
-      </c>
-      <c r="D228" t="s">
-        <v>369</v>
-      </c>
-      <c r="E228" s="1" t="s">
-        <v>345</v>
+        <v>293</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="229" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D229" t="s">
-        <v>368</v>
-      </c>
-      <c r="E229" s="1" t="s">
-        <v>346</v>
+      <c r="C229" t="s">
+        <v>294</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="230" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D230" s="1"/>
+      <c r="C230" t="s">
+        <v>297</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="231" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D231" s="1"/>
@@ -4196,130 +4218,146 @@
     <row r="232" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D232" s="1"/>
     </row>
+    <row r="233" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B233" t="s">
+        <v>343</v>
+      </c>
+      <c r="D233" s="1"/>
+    </row>
+    <row r="234" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C234" t="s">
+        <v>344</v>
+      </c>
+      <c r="D234" t="s">
+        <v>369</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="235" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D235" t="s">
+        <v>368</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
     <row r="236" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B236" t="s">
+      <c r="D236" s="1"/>
+    </row>
+    <row r="237" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D237" s="1"/>
+    </row>
+    <row r="238" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D238" s="1"/>
+    </row>
+    <row r="242" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B242" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="237" spans="2:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="C237" s="4" t="s">
+    <row r="243" spans="2:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="C243" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D237" s="2" t="s">
+      <c r="D243" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E237" s="1" t="s">
+      <c r="E243" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="238" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C238" t="s">
+    <row r="244" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C244" t="s">
         <v>187</v>
       </c>
-      <c r="E238" s="1" t="s">
+      <c r="E244" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="239" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C239" t="s">
+    <row r="245" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C245" t="s">
         <v>215</v>
       </c>
-      <c r="E239" s="1" t="s">
+      <c r="E245" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="241" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D241" t="s">
+    <row r="247" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D247" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="243" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C243" t="s">
+    <row r="249" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C249" t="s">
         <v>242</v>
       </c>
-      <c r="D243" t="s">
+      <c r="D249" t="s">
         <v>243</v>
       </c>
-      <c r="E243" s="1" t="s">
+      <c r="E249" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="244" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C244" t="s">
+    <row r="250" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C250" t="s">
         <v>269</v>
       </c>
-      <c r="D244" t="s">
+      <c r="D250" t="s">
         <v>270</v>
       </c>
-      <c r="E244" s="1" t="s">
+      <c r="E250" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="245" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C245" t="s">
+    <row r="251" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C251" t="s">
         <v>284</v>
       </c>
-      <c r="E245" s="1" t="s">
+      <c r="E251" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="246" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E246" s="1" t="s">
+    <row r="252" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E252" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="247" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E247" s="1" t="s">
+    <row r="253" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E253" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="248" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C248" t="s">
+    <row r="254" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C254" t="s">
         <v>288</v>
       </c>
-      <c r="E248" s="1" t="s">
+      <c r="E254" s="1" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="249" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C249" t="s">
+    <row r="255" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C255" t="s">
         <v>299</v>
       </c>
-      <c r="E249" s="1" t="s">
+      <c r="E255" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="250" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E250" s="1"/>
-    </row>
-    <row r="251" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C251" t="s">
+    <row r="256" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E256" s="1"/>
+    </row>
+    <row r="257" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C257" t="s">
         <v>359</v>
       </c>
-      <c r="D251" t="s">
+      <c r="D257" t="s">
         <v>360</v>
       </c>
-      <c r="E251" s="1" t="s">
+      <c r="E257" s="1" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="252" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E252" s="1"/>
-    </row>
-    <row r="253" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E253" s="1"/>
-    </row>
-    <row r="254" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E254" s="1"/>
-    </row>
-    <row r="255" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E255" s="1"/>
-    </row>
-    <row r="256" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E256" s="1"/>
-    </row>
-    <row r="257" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E257" s="1"/>
     </row>
     <row r="258" spans="3:8" x14ac:dyDescent="0.2">
       <c r="E258" s="1"/>
@@ -4328,1235 +4366,1253 @@
       <c r="E259" s="1"/>
     </row>
     <row r="260" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C260" t="s">
+      <c r="E260" s="1"/>
+    </row>
+    <row r="261" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E261" s="1"/>
+    </row>
+    <row r="262" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E262" s="1"/>
+    </row>
+    <row r="263" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E263" s="1"/>
+    </row>
+    <row r="264" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E264" s="1"/>
+    </row>
+    <row r="265" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E265" s="1"/>
+    </row>
+    <row r="266" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C266" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="261" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D261" t="s">
-        <v>135</v>
-      </c>
-      <c r="E261" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="262" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D262" t="s">
-        <v>136</v>
-      </c>
-      <c r="E262" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="263" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D263" t="s">
-        <v>140</v>
-      </c>
-      <c r="E263" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="264" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D264" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="265" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D265" t="s">
-        <v>142</v>
-      </c>
-      <c r="E265" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="266" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D266" t="s">
-        <v>484</v>
-      </c>
-      <c r="E266" t="s">
-        <v>486</v>
-      </c>
-      <c r="F266" t="s">
-        <v>490</v>
-      </c>
-      <c r="G266" t="s">
-        <v>485</v>
-      </c>
-      <c r="H266" s="1" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="267" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D267" t="s">
-        <v>487</v>
+        <v>135</v>
       </c>
       <c r="E267" t="s">
-        <v>488</v>
-      </c>
-      <c r="G267" t="s">
-        <v>489</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="268" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D268" t="s">
+        <v>136</v>
+      </c>
+      <c r="E268" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="269" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C269" t="s">
-        <v>367</v>
+      <c r="D269" t="s">
+        <v>140</v>
+      </c>
+      <c r="E269" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="270" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D270" t="s">
-        <v>73</v>
-      </c>
-      <c r="E270" t="s">
-        <v>74</v>
-      </c>
-      <c r="F270" s="1" t="s">
-        <v>75</v>
+        <v>137</v>
       </c>
     </row>
     <row r="271" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D271" t="s">
-        <v>76</v>
-      </c>
-      <c r="E271" s="1" t="s">
-        <v>77</v>
+        <v>142</v>
+      </c>
+      <c r="E271" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="272" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D272" t="s">
-        <v>78</v>
-      </c>
-      <c r="E272" s="1" t="s">
-        <v>79</v>
+        <v>484</v>
+      </c>
+      <c r="E272" t="s">
+        <v>486</v>
+      </c>
+      <c r="F272" t="s">
+        <v>490</v>
+      </c>
+      <c r="G272" t="s">
+        <v>485</v>
+      </c>
+      <c r="H272" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="273" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D273" t="s">
-        <v>81</v>
-      </c>
-      <c r="E273" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="274" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D274" t="s">
-        <v>362</v>
-      </c>
-      <c r="E274" t="s">
-        <v>365</v>
+        <v>487</v>
+      </c>
+      <c r="E273" t="s">
+        <v>488</v>
+      </c>
+      <c r="G273" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="275" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D275" t="s">
-        <v>363</v>
-      </c>
-      <c r="E275" t="s">
-        <v>364</v>
+      <c r="C275" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="276" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D276" t="s">
+        <v>73</v>
+      </c>
+      <c r="E276" t="s">
+        <v>74</v>
+      </c>
+      <c r="F276" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="277" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D277" t="s">
-        <v>82</v>
-      </c>
-      <c r="E277" t="s">
-        <v>83</v>
+        <v>76</v>
+      </c>
+      <c r="E277" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="278" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D278" t="s">
-        <v>84</v>
-      </c>
-      <c r="E278" t="s">
-        <v>85</v>
+        <v>78</v>
+      </c>
+      <c r="E278" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="279" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D279" t="s">
+        <v>81</v>
+      </c>
+      <c r="E279" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="280" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C280" t="s">
-        <v>366</v>
+      <c r="D280" t="s">
+        <v>362</v>
+      </c>
+      <c r="E280" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="281" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D281" t="s">
-        <v>73</v>
+        <v>363</v>
       </c>
       <c r="E281" t="s">
-        <v>131</v>
-      </c>
-      <c r="F281" s="1"/>
-    </row>
-    <row r="282" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D282" t="s">
-        <v>147</v>
-      </c>
-      <c r="E282" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F282" s="1"/>
+        <v>364</v>
+      </c>
     </row>
     <row r="283" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D283" t="s">
-        <v>76</v>
-      </c>
-      <c r="E283" s="1" t="s">
-        <v>149</v>
+        <v>82</v>
+      </c>
+      <c r="E283" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="284" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E284" s="1"/>
-    </row>
-    <row r="285" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D285" t="s">
-        <v>144</v>
+      <c r="D284" t="s">
+        <v>84</v>
+      </c>
+      <c r="E284" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="286" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E286" t="s">
-        <v>151</v>
-      </c>
-      <c r="F286" t="s">
-        <v>150</v>
+      <c r="C286" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="287" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D287" t="s">
+        <v>73</v>
+      </c>
       <c r="E287" t="s">
-        <v>152</v>
-      </c>
-      <c r="F287" t="s">
-        <v>145</v>
-      </c>
-      <c r="G287" s="1" t="s">
-        <v>146</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="F287" s="1"/>
     </row>
     <row r="288" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D288" t="s">
+        <v>147</v>
+      </c>
+      <c r="E288" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F288" s="1"/>
+    </row>
+    <row r="289" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D289" t="s">
+        <v>76</v>
+      </c>
+      <c r="E289" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="290" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E290" s="1"/>
+    </row>
+    <row r="291" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D291" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="292" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E292" t="s">
+        <v>151</v>
+      </c>
+      <c r="F292" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="293" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E293" t="s">
+        <v>152</v>
+      </c>
+      <c r="F293" t="s">
+        <v>145</v>
+      </c>
+      <c r="G293" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="294" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D294" t="s">
         <v>153</v>
       </c>
-      <c r="E288" s="1" t="s">
+      <c r="E294" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G288" s="1"/>
-    </row>
-    <row r="302" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E302" s="1"/>
-    </row>
-    <row r="304" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B304" t="s">
+      <c r="G294" s="1"/>
+    </row>
+    <row r="308" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E308" s="1"/>
+    </row>
+    <row r="310" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B310" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="305" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C305" t="s">
+    <row r="311" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C311" t="s">
         <v>277</v>
       </c>
-      <c r="D305" t="s">
+      <c r="D311" t="s">
         <v>279</v>
       </c>
-      <c r="E305" s="1" t="s">
+      <c r="E311" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="306" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C306" t="s">
+    <row r="312" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C312" t="s">
         <v>281</v>
       </c>
-      <c r="E306" s="1" t="s">
+      <c r="E312" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="F306" s="1" t="s">
+      <c r="F312" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="G306" s="1" t="s">
+      <c r="G312" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="307" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C307" t="s">
+    <row r="313" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C313" t="s">
         <v>290</v>
       </c>
-      <c r="E307" s="1" t="s">
+      <c r="E313" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="308" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C308" t="s">
+    <row r="314" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C314" t="s">
         <v>304</v>
       </c>
-      <c r="E308" s="1" t="s">
+      <c r="E314" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="309" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D309" t="s">
+    <row r="315" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D315" t="s">
         <v>306</v>
       </c>
-      <c r="E309" s="1" t="s">
+      <c r="E315" s="1" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="310" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C310" t="s">
+    <row r="316" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C316" t="s">
         <v>324</v>
       </c>
-      <c r="E310" s="1" t="s">
+      <c r="E316" s="1" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="311" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C311" t="s">
+    <row r="317" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C317" t="s">
         <v>308</v>
       </c>
-      <c r="D311" t="s">
+      <c r="D317" t="s">
         <v>309</v>
       </c>
-      <c r="E311" s="1" t="s">
+      <c r="E317" s="1" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="312" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C312" t="s">
+    <row r="318" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C318" t="s">
         <v>311</v>
       </c>
-      <c r="E312" s="1" t="s">
+      <c r="E318" s="1" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="313" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C313" t="s">
+    <row r="319" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C319" t="s">
         <v>316</v>
       </c>
-      <c r="E313" s="1" t="s">
+      <c r="E319" s="1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="314" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C314" t="s">
+    <row r="320" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C320" t="s">
         <v>317</v>
       </c>
-      <c r="E314" s="1" t="s">
+      <c r="E320" s="1" t="s">
         <v>318</v>
-      </c>
-    </row>
-    <row r="315" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C315" t="s">
-        <v>319</v>
-      </c>
-      <c r="E315" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="316" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C316" t="s">
-        <v>326</v>
-      </c>
-      <c r="D316" t="s">
-        <v>333</v>
-      </c>
-      <c r="E316" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="317" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D317" t="s">
-        <v>328</v>
-      </c>
-      <c r="E317" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="319" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C319" t="s">
-        <v>330</v>
-      </c>
-      <c r="D319" t="s">
-        <v>331</v>
-      </c>
-      <c r="E319" s="1" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="321" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C321" t="s">
+        <v>319</v>
+      </c>
+      <c r="E321" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="322" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C322" t="s">
+        <v>326</v>
+      </c>
+      <c r="D322" t="s">
+        <v>333</v>
+      </c>
+      <c r="E322" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="323" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D323" t="s">
+        <v>328</v>
+      </c>
+      <c r="E323" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="325" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C325" t="s">
+        <v>330</v>
+      </c>
+      <c r="D325" t="s">
+        <v>331</v>
+      </c>
+      <c r="E325" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="327" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C327" t="s">
         <v>336</v>
       </c>
-      <c r="D321" t="s">
+      <c r="D327" t="s">
         <v>338</v>
       </c>
-      <c r="E321" s="1" t="s">
+      <c r="E327" s="1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="325" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B325" t="s">
+    <row r="331" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B331" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="326" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C326" t="s">
+    <row r="332" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C332" t="s">
         <v>342</v>
       </c>
-      <c r="D326" t="s">
+      <c r="D332" t="s">
         <v>340</v>
       </c>
-      <c r="E326" s="1" t="s">
+      <c r="E332" s="1" t="s">
         <v>341</v>
-      </c>
-    </row>
-    <row r="332" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B332" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="333" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C333" t="s">
-        <v>87</v>
-      </c>
-      <c r="D333" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="334" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C334" t="s">
-        <v>89</v>
-      </c>
-      <c r="D334" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="335" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C335" t="s">
-        <v>96</v>
-      </c>
-      <c r="D335" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="336" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C336" t="s">
-        <v>98</v>
-      </c>
-      <c r="D336" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="338" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B338" t="s">
-        <v>91</v>
-      </c>
-      <c r="C338" t="s">
-        <v>92</v>
-      </c>
-      <c r="D338" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="339" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C339" t="s">
+        <v>87</v>
+      </c>
+      <c r="D339" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="340" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C340" t="s">
+        <v>89</v>
+      </c>
+      <c r="D340" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="341" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C341" t="s">
+        <v>96</v>
+      </c>
+      <c r="D341" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="342" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C342" t="s">
+        <v>98</v>
+      </c>
+      <c r="D342" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="344" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B344" t="s">
+        <v>91</v>
+      </c>
+      <c r="C344" t="s">
+        <v>92</v>
+      </c>
+      <c r="D344" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="345" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C345" t="s">
         <v>94</v>
       </c>
-      <c r="D339" t="s">
+      <c r="D345" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="342" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B342" t="s">
+    <row r="348" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B348" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="343" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C343" t="s">
+    <row r="349" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C349" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="344" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D344" t="s">
+    <row r="350" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D350" t="s">
         <v>105</v>
       </c>
-      <c r="E344" s="1" t="s">
+      <c r="E350" s="1" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="345" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D345" t="s">
-        <v>102</v>
-      </c>
-      <c r="E345" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="346" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D346" t="s">
-        <v>103</v>
-      </c>
-      <c r="E346" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="347" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D347" t="s">
-        <v>108</v>
-      </c>
-      <c r="E347" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="349" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B349" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="350" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C350" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="351" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D351" t="s">
-        <v>111</v>
+        <v>102</v>
+      </c>
+      <c r="E351" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="352" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D352" t="s">
-        <v>112</v>
+        <v>103</v>
+      </c>
+      <c r="E352" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="353" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F353" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="354" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B354" t="s">
-        <v>1</v>
-      </c>
-      <c r="F354" s="1" t="s">
-        <v>124</v>
+      <c r="D353" t="s">
+        <v>108</v>
+      </c>
+      <c r="E353" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="355" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C355" t="s">
-        <v>113</v>
-      </c>
-      <c r="D355" s="1" t="s">
-        <v>114</v>
+      <c r="B355" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="356" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D356" t="s">
-        <v>127</v>
-      </c>
-      <c r="E356" s="1" t="s">
-        <v>126</v>
+      <c r="C356" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="357" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C357" t="s">
-        <v>115</v>
+      <c r="D357" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="358" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D358" t="s">
-        <v>116</v>
-      </c>
-      <c r="E358" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F358" t="s">
-        <v>129</v>
-      </c>
-      <c r="G358" s="1" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
     </row>
     <row r="359" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E359" t="s">
-        <v>122</v>
-      </c>
-      <c r="G359" s="1"/>
+      <c r="F359" s="1" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="360" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E360" t="s">
-        <v>125</v>
-      </c>
-      <c r="G360" s="1"/>
+      <c r="B360" t="s">
+        <v>1</v>
+      </c>
+      <c r="F360" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="361" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D361" t="s">
-        <v>118</v>
-      </c>
-      <c r="E361" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G361" s="1"/>
+      <c r="C361" t="s">
+        <v>113</v>
+      </c>
+      <c r="D361" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="362" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D362" t="s">
+        <v>127</v>
+      </c>
+      <c r="E362" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="363" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C363" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="364" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D364" t="s">
+        <v>116</v>
+      </c>
+      <c r="E364" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F364" t="s">
+        <v>129</v>
+      </c>
+      <c r="G364" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="365" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E365" t="s">
+        <v>122</v>
+      </c>
+      <c r="G365" s="1"/>
+    </row>
+    <row r="366" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E366" t="s">
+        <v>125</v>
+      </c>
+      <c r="G366" s="1"/>
+    </row>
+    <row r="367" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D367" t="s">
+        <v>118</v>
+      </c>
+      <c r="E367" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G367" s="1"/>
+    </row>
+    <row r="368" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D368" t="s">
         <v>120</v>
       </c>
-      <c r="E362" s="1" t="s">
+      <c r="E368" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G362" s="1"/>
-    </row>
-    <row r="363" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E363" s="1" t="s">
+      <c r="G368" s="1"/>
+    </row>
+    <row r="369" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E369" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="G363" s="1"/>
-    </row>
-    <row r="364" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E364" t="s">
+      <c r="G369" s="1"/>
+    </row>
+    <row r="370" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E370" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="365" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D365" t="s">
+    <row r="371" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D371" t="s">
         <v>302</v>
       </c>
-      <c r="E365" s="1" t="s">
+      <c r="E371" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="366" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D366" t="s">
+    <row r="372" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D372" t="s">
         <v>301</v>
       </c>
-      <c r="E366" s="1" t="s">
+      <c r="E372" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="371" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C371" t="s">
+    <row r="377" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C377" t="s">
         <v>132</v>
       </c>
-      <c r="D371" s="1" t="s">
+      <c r="D377" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="375" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B375" t="s">
+    <row r="381" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B381" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="376" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C376" t="s">
+    <row r="382" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C382" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="377" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D377" t="s">
+    <row r="383" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D383" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="378" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E378" t="s">
+    <row r="384" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E384" t="s">
         <v>494</v>
       </c>
-      <c r="F378" s="1" t="s">
+      <c r="F384" s="1" t="s">
         <v>493</v>
-      </c>
-    </row>
-    <row r="379" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E379" t="s">
-        <v>496</v>
-      </c>
-      <c r="F379" s="1" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="380" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E380" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="381" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D381" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="382" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E382" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="383" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E383" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="384" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D384" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="385" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E385" t="s">
-        <v>501</v>
+        <v>496</v>
+      </c>
+      <c r="F385" s="1" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="386" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C386" t="s">
-        <v>502</v>
+      <c r="E386" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="387" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D387" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="388" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E388" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="389" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E389" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="390" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D390" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="391" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E391" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="392" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C392" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="393" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D393" t="s">
         <v>505</v>
       </c>
-      <c r="E387" t="s">
+      <c r="E393" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="388" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D388" t="s">
+    <row r="394" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D394" t="s">
         <v>503</v>
       </c>
-      <c r="E388" t="s">
+      <c r="E394" t="s">
         <v>504</v>
-      </c>
-    </row>
-    <row r="390" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C390" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="391" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D391" t="s">
-        <v>510</v>
-      </c>
-      <c r="E391" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="392" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D392" t="s">
-        <v>511</v>
-      </c>
-      <c r="E392" t="s">
-        <v>509</v>
-      </c>
-      <c r="G392" s="1" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="394" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C394" t="s">
-        <v>514</v>
-      </c>
-      <c r="G394" s="1" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="396" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C396" t="s">
-        <v>515</v>
-      </c>
-      <c r="E396" t="s">
-        <v>516</v>
-      </c>
-      <c r="G396" s="1" t="s">
-        <v>517</v>
+        <v>507</v>
+      </c>
+    </row>
+    <row r="397" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D397" t="s">
+        <v>510</v>
+      </c>
+      <c r="E397" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="398" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C398" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="399" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D399" t="s">
-        <v>520</v>
-      </c>
-      <c r="E399" t="s">
-        <v>519</v>
-      </c>
-      <c r="G399" s="1" t="s">
-        <v>523</v>
+      <c r="D398" t="s">
+        <v>511</v>
+      </c>
+      <c r="E398" t="s">
+        <v>509</v>
+      </c>
+      <c r="G398" s="1" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="400" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D400" t="s">
-        <v>521</v>
-      </c>
-      <c r="E400" t="s">
-        <v>522</v>
+      <c r="C400" t="s">
+        <v>514</v>
+      </c>
+      <c r="G400" s="1" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="402" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C402" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="403" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D403" t="s">
-        <v>530</v>
-      </c>
-      <c r="E403" t="s">
-        <v>526</v>
-      </c>
-      <c r="G403" s="1" t="s">
-        <v>531</v>
+        <v>515</v>
+      </c>
+      <c r="E402" t="s">
+        <v>516</v>
+      </c>
+      <c r="G402" s="1" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="404" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D404" t="s">
-        <v>528</v>
-      </c>
-      <c r="E404" t="s">
-        <v>525</v>
+      <c r="C404" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="405" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D405" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
       <c r="E405" t="s">
-        <v>527</v>
+        <v>519</v>
+      </c>
+      <c r="G405" s="1" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="406" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C406" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="407" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D407" t="s">
-        <v>633</v>
-      </c>
-      <c r="E407" t="s">
-        <v>634</v>
+      <c r="D406" t="s">
+        <v>521</v>
+      </c>
+      <c r="E406" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="408" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D408" t="s">
-        <v>635</v>
-      </c>
-      <c r="E408" t="s">
-        <v>636</v>
+      <c r="C408" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="409" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D409" t="s">
-        <v>637</v>
+        <v>530</v>
       </c>
       <c r="E409" t="s">
-        <v>638</v>
+        <v>526</v>
+      </c>
+      <c r="G409" s="1" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="410" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D410" t="s">
-        <v>640</v>
+        <v>528</v>
       </c>
       <c r="E410" t="s">
-        <v>639</v>
+        <v>525</v>
       </c>
     </row>
     <row r="411" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D411" t="s">
+        <v>529</v>
+      </c>
+      <c r="E411" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="412" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C412" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="413" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D413" t="s">
+        <v>633</v>
+      </c>
+      <c r="E413" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="414" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D414" t="s">
+        <v>635</v>
+      </c>
+      <c r="E414" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="415" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D415" t="s">
+        <v>637</v>
+      </c>
+      <c r="E415" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="416" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D416" t="s">
+        <v>640</v>
+      </c>
+      <c r="E416" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="417" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D417" t="s">
         <v>697</v>
       </c>
-      <c r="E411" t="s">
+      <c r="E417" t="s">
         <v>699</v>
       </c>
-      <c r="G411" s="1" t="s">
+      <c r="G417" s="1" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="417" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C417" t="s">
+    <row r="423" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C423" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="418" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D418">
+    <row r="424" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D424">
         <v>1</v>
       </c>
     </row>
-    <row r="424" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B424" t="s">
+    <row r="430" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B430" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="425" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C425" t="s">
+    <row r="431" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C431" t="s">
         <v>542</v>
-      </c>
-    </row>
-    <row r="426" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D426" t="s">
-        <v>543</v>
-      </c>
-      <c r="G426" s="1" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="427" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C427" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="428" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D428" t="s">
-        <v>545</v>
-      </c>
-      <c r="E428" t="s">
-        <v>546</v>
-      </c>
-      <c r="G428" s="1" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="430" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C430" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="431" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D431" t="s">
-        <v>550</v>
-      </c>
-      <c r="E431" t="s">
-        <v>551</v>
-      </c>
-      <c r="G431" s="1" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="432" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D432" t="s">
-        <v>552</v>
-      </c>
-      <c r="E432" t="s">
-        <v>553</v>
+        <v>543</v>
+      </c>
+      <c r="G432" s="1" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="433" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D433" t="s">
-        <v>554</v>
-      </c>
-      <c r="E433" t="s">
-        <v>555</v>
+      <c r="C433" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="434" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D434" t="s">
-        <v>556</v>
+        <v>545</v>
       </c>
       <c r="E434" t="s">
-        <v>557</v>
+        <v>546</v>
+      </c>
+      <c r="G434" s="1" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="436" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C436" t="s">
-        <v>559</v>
+        <v>549</v>
       </c>
     </row>
     <row r="437" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D437" t="s">
-        <v>560</v>
+        <v>550</v>
       </c>
       <c r="E437" t="s">
-        <v>562</v>
+        <v>551</v>
       </c>
       <c r="G437" s="1" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
     </row>
     <row r="438" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D438" t="s">
-        <v>561</v>
+        <v>552</v>
       </c>
       <c r="E438" t="s">
-        <v>563</v>
+        <v>553</v>
+      </c>
+    </row>
+    <row r="439" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D439" t="s">
+        <v>554</v>
+      </c>
+      <c r="E439" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="440" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C440" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="441" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D441" t="s">
-        <v>567</v>
-      </c>
-      <c r="G441" s="1" t="s">
-        <v>566</v>
+      <c r="D440" t="s">
+        <v>556</v>
+      </c>
+      <c r="E440" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="442" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C442" t="s">
-        <v>611</v>
-      </c>
-      <c r="G442" s="1"/>
+        <v>559</v>
+      </c>
     </row>
     <row r="443" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D443" t="s">
+        <v>560</v>
+      </c>
+      <c r="E443" t="s">
+        <v>562</v>
+      </c>
+      <c r="G443" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="444" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D444" t="s">
+        <v>561</v>
+      </c>
+      <c r="E444" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="446" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C446" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="447" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D447" t="s">
+        <v>567</v>
+      </c>
+      <c r="G447" s="1" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="448" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C448" t="s">
+        <v>611</v>
+      </c>
+      <c r="G448" s="1"/>
+    </row>
+    <row r="449" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D449" t="s">
         <v>612</v>
       </c>
-      <c r="E443" t="s">
+      <c r="E449" t="s">
         <v>613</v>
       </c>
-      <c r="G443" s="1" t="s">
+      <c r="G449" s="1" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="444" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="G444" s="1"/>
-    </row>
-    <row r="445" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="G445" s="1"/>
-    </row>
-    <row r="446" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="G446" s="1"/>
-    </row>
-    <row r="447" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="G447" s="1"/>
-    </row>
-    <row r="448" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="G448" s="1"/>
-    </row>
-    <row r="449" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G449" s="1"/>
+    <row r="450" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G450" s="1"/>
+    </row>
+    <row r="451" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G451" s="1"/>
     </row>
     <row r="452" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B452" t="s">
+      <c r="G452" s="1"/>
+    </row>
+    <row r="453" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G453" s="1"/>
+    </row>
+    <row r="454" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G454" s="1"/>
+    </row>
+    <row r="455" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G455" s="1"/>
+    </row>
+    <row r="458" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B458" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="453" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C453" t="s">
+    <row r="459" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C459" t="s">
         <v>569</v>
-      </c>
-    </row>
-    <row r="454" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E454" t="s">
-        <v>570</v>
-      </c>
-      <c r="G454" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="457" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B457" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="458" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C458" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="459" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D459" t="s">
-        <v>574</v>
-      </c>
-      <c r="E459" t="s">
-        <v>575</v>
-      </c>
-      <c r="F459" t="s">
-        <v>576</v>
-      </c>
-      <c r="G459" s="1" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="460" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E460" t="s">
-        <v>578</v>
-      </c>
-      <c r="F460" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="461" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C461" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="462" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D462" t="s">
-        <v>597</v>
-      </c>
-      <c r="E462" t="s">
-        <v>598</v>
+        <v>570</v>
+      </c>
+      <c r="G460" s="1" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="463" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D463" t="s">
-        <v>600</v>
-      </c>
-      <c r="E463" t="s">
-        <v>599</v>
+      <c r="B463" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="464" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C464" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="465" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D465" t="s">
-        <v>601</v>
+        <v>574</v>
       </c>
       <c r="E465" t="s">
-        <v>602</v>
+        <v>575</v>
+      </c>
+      <c r="F465" t="s">
+        <v>576</v>
+      </c>
+      <c r="G465" s="1" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="466" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D466" t="s">
-        <v>603</v>
-      </c>
       <c r="E466" t="s">
-        <v>604</v>
+        <v>578</v>
+      </c>
+      <c r="F466" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="467" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C467" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="468" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D468" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="E468" t="s">
-        <v>606</v>
-      </c>
-      <c r="G468" s="1" t="s">
-        <v>610</v>
+        <v>598</v>
       </c>
     </row>
     <row r="469" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D469" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
       <c r="E469" t="s">
-        <v>608</v>
-      </c>
-      <c r="F469" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="473" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B473" t="s">
-        <v>580</v>
+        <v>599</v>
+      </c>
+    </row>
+    <row r="471" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D471" t="s">
+        <v>601</v>
+      </c>
+      <c r="E471" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="472" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D472" t="s">
+        <v>603</v>
+      </c>
+      <c r="E472" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="474" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C474" t="s">
-        <v>581</v>
+      <c r="D474" t="s">
+        <v>605</v>
+      </c>
+      <c r="E474" t="s">
+        <v>606</v>
+      </c>
+      <c r="G474" s="1" t="s">
+        <v>610</v>
       </c>
     </row>
     <row r="475" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D475" t="s">
+        <v>607</v>
+      </c>
+      <c r="E475" t="s">
+        <v>608</v>
+      </c>
+      <c r="F475" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="479" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B479" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="480" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C480" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="481" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D481" t="s">
         <v>583</v>
       </c>
-      <c r="E475" t="s">
+      <c r="E481" t="s">
         <v>584</v>
       </c>
-      <c r="F475" t="s">
+      <c r="F481" t="s">
         <v>582</v>
       </c>
-      <c r="G475" s="1" t="s">
+      <c r="G481" s="1" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="476" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E476" t="s">
+    <row r="482" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E482" t="s">
         <v>585</v>
       </c>
-      <c r="F476" t="s">
+      <c r="F482" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="478" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D478" t="s">
+    <row r="484" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D484" t="s">
         <v>588</v>
       </c>
-      <c r="E478" t="s">
+      <c r="E484" t="s">
         <v>590</v>
       </c>
-      <c r="F478" t="s">
+      <c r="F484" t="s">
         <v>589</v>
-      </c>
-    </row>
-    <row r="481" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B481" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="482" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C482" t="s">
-        <v>711</v>
-      </c>
-      <c r="D482" t="s">
-        <v>714</v>
-      </c>
-      <c r="G482" s="1" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="483" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C483" t="s">
-        <v>712</v>
-      </c>
-      <c r="D483" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="484" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C484" t="s">
-        <v>713</v>
-      </c>
-      <c r="D484" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="487" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B487" t="s">
-        <v>734</v>
+        <v>710</v>
       </c>
     </row>
     <row r="488" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C488" t="s">
-        <v>735</v>
+        <v>711</v>
+      </c>
+      <c r="D488" t="s">
+        <v>714</v>
       </c>
       <c r="G488" s="1" t="s">
-        <v>736</v>
+        <v>717</v>
       </c>
     </row>
     <row r="489" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C489" t="s">
-        <v>737</v>
-      </c>
-      <c r="G489" s="1" t="s">
-        <v>738</v>
+        <v>712</v>
+      </c>
+      <c r="D489" t="s">
+        <v>715</v>
       </c>
     </row>
     <row r="490" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C490" t="s">
-        <v>741</v>
-      </c>
-      <c r="F490" t="s">
-        <v>739</v>
-      </c>
-      <c r="G490" s="1" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="492" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B492" t="s">
-        <v>746</v>
+        <v>713</v>
+      </c>
+      <c r="D490" t="s">
+        <v>716</v>
       </c>
     </row>
     <row r="493" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C493" t="s">
-        <v>747</v>
-      </c>
-      <c r="D493" t="s">
-        <v>748</v>
-      </c>
-      <c r="G493" s="1" t="s">
-        <v>749</v>
+      <c r="B493" t="s">
+        <v>734</v>
       </c>
     </row>
     <row r="494" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C494" t="s">
+        <v>735</v>
+      </c>
+      <c r="G494" s="1" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="495" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C495" t="s">
+        <v>737</v>
+      </c>
+      <c r="G495" s="1" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="496" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C496" t="s">
+        <v>741</v>
+      </c>
+      <c r="F496" t="s">
+        <v>739</v>
+      </c>
+      <c r="G496" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="498" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B498" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="499" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C499" t="s">
+        <v>747</v>
+      </c>
+      <c r="D499" t="s">
+        <v>748</v>
+      </c>
+      <c r="G499" s="1" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="500" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C500" t="s">
         <v>750</v>
       </c>
-      <c r="D494" t="s">
+      <c r="D500" t="s">
         <v>751</v>
       </c>
-      <c r="G494" s="1" t="s">
+      <c r="G500" s="1" t="s">
         <v>752</v>
       </c>
     </row>
@@ -5576,14 +5632,14 @@
     <hyperlink ref="D92" r:id="rId12" xr:uid="{BA9A8F05-4D7F-4942-886C-F8152208F0EA}"/>
     <hyperlink ref="F96" r:id="rId13" xr:uid="{22AE585F-7255-3F41-8A2E-808446F3A9AA}"/>
     <hyperlink ref="F98" r:id="rId14" xr:uid="{93472772-CF6C-D045-B634-2D574A3EE034}"/>
-    <hyperlink ref="E188" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
-    <hyperlink ref="F189" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
-    <hyperlink ref="D220" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
-    <hyperlink ref="D221" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
+    <hyperlink ref="E194" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
+    <hyperlink ref="F195" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
+    <hyperlink ref="D226" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
+    <hyperlink ref="D227" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
     <hyperlink ref="F99" r:id="rId19" xr:uid="{92BE3560-5393-C545-9D2D-2B773359B28F}"/>
-    <hyperlink ref="E237" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
-    <hyperlink ref="E238" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
-    <hyperlink ref="E239" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
+    <hyperlink ref="E243" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
+    <hyperlink ref="E244" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
+    <hyperlink ref="E245" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
     <hyperlink ref="E73" r:id="rId23" xr:uid="{1526D7DA-27DA-1443-928C-BEDA9E425734}"/>
     <hyperlink ref="E74" r:id="rId24" xr:uid="{4F363062-BE49-AB4F-8956-2C1F31D9B898}"/>
     <hyperlink ref="H100" r:id="rId25" xr:uid="{D9E13355-D59B-054F-B544-34A5A285A9E0}"/>
@@ -5600,7 +5656,7 @@
     <hyperlink ref="I100" r:id="rId36" xr:uid="{A03C56E4-1156-A148-A568-F50A5C33DB5C}"/>
     <hyperlink ref="F109" r:id="rId37" xr:uid="{12AC219C-4678-4E43-B328-6595FA10B8D3}"/>
     <hyperlink ref="E111" r:id="rId38" xr:uid="{44409621-28A2-704A-B283-3DCE1EFB1603}"/>
-    <hyperlink ref="E243" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
+    <hyperlink ref="E249" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
     <hyperlink ref="F112" r:id="rId40" xr:uid="{A9D0D792-87D1-8144-872F-5CA060D3C28F}"/>
     <hyperlink ref="F113" r:id="rId41" xr:uid="{87EF989D-17E9-1E45-A075-CD862D0B60F4}"/>
     <hyperlink ref="F115" r:id="rId42" xr:uid="{8406C6F0-DC69-A64D-AAD8-60A33C12D00B}"/>
@@ -5610,113 +5666,115 @@
     <hyperlink ref="F120" r:id="rId46" xr:uid="{3D1C62DB-D9B7-BE42-B21D-4EEBC4C9EFE1}"/>
     <hyperlink ref="F121" r:id="rId47" xr:uid="{F5021A21-70A2-D34E-B055-64CAC326E7EF}"/>
     <hyperlink ref="F122" r:id="rId48" xr:uid="{A8C010A1-8EE1-264B-8688-3BEA1B62E535}"/>
-    <hyperlink ref="E244" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
+    <hyperlink ref="E250" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
     <hyperlink ref="F117" r:id="rId50" location="113521" xr:uid="{EE1413C5-3B38-7D4D-8DF1-634A12F0BD81}"/>
     <hyperlink ref="E75" r:id="rId51" xr:uid="{00B1EF4A-7791-0343-8D8C-9A1E83248FC9}"/>
-    <hyperlink ref="E305" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
-    <hyperlink ref="E306" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
+    <hyperlink ref="E311" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
+    <hyperlink ref="E312" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
     <hyperlink ref="F124" r:id="rId54" xr:uid="{40A4B6A0-2F7E-A84D-8CC6-D814A33F5953}"/>
-    <hyperlink ref="E245" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
-    <hyperlink ref="E246" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
-    <hyperlink ref="E247" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
-    <hyperlink ref="E248" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
-    <hyperlink ref="E307" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
-    <hyperlink ref="D222" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
-    <hyperlink ref="D223" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
-    <hyperlink ref="D224" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
-    <hyperlink ref="E249" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
-    <hyperlink ref="E308" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
-    <hyperlink ref="E309" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
-    <hyperlink ref="E311" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
-    <hyperlink ref="E312" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
-    <hyperlink ref="F306" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
-    <hyperlink ref="G306" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
-    <hyperlink ref="E313" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
-    <hyperlink ref="E314" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
-    <hyperlink ref="E315" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
-    <hyperlink ref="E190" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
-    <hyperlink ref="E310" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
-    <hyperlink ref="E316" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
-    <hyperlink ref="E317" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
+    <hyperlink ref="E251" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
+    <hyperlink ref="E252" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
+    <hyperlink ref="E253" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
+    <hyperlink ref="E254" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
+    <hyperlink ref="E313" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
+    <hyperlink ref="D228" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
+    <hyperlink ref="D229" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
+    <hyperlink ref="D230" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
+    <hyperlink ref="E255" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
+    <hyperlink ref="E314" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
+    <hyperlink ref="E315" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
+    <hyperlink ref="E317" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
+    <hyperlink ref="E318" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
+    <hyperlink ref="F312" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
+    <hyperlink ref="G312" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
+    <hyperlink ref="E319" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
+    <hyperlink ref="E320" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
+    <hyperlink ref="E321" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
+    <hyperlink ref="E196" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
+    <hyperlink ref="E316" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
+    <hyperlink ref="E322" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
+    <hyperlink ref="E323" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
     <hyperlink ref="E77" r:id="rId77" location="code" xr:uid="{C0475FF8-517D-E949-887E-9A42D86E9640}"/>
-    <hyperlink ref="E319" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
+    <hyperlink ref="E325" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
     <hyperlink ref="E78" r:id="rId79" xr:uid="{277DBE6F-F3E5-8B4C-8DD8-BD92445D1A99}"/>
-    <hyperlink ref="E321" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
-    <hyperlink ref="E326" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
-    <hyperlink ref="E228" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
-    <hyperlink ref="E229" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
+    <hyperlink ref="E327" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
+    <hyperlink ref="E332" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
+    <hyperlink ref="E234" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
+    <hyperlink ref="E235" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
     <hyperlink ref="F145" r:id="rId84" xr:uid="{EB604865-A16B-0646-A5B5-0D047467449D}"/>
-    <hyperlink ref="E251" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
-    <hyperlink ref="D335" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
-    <hyperlink ref="D336" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
-    <hyperlink ref="E345" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
-    <hyperlink ref="E346" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
-    <hyperlink ref="E344" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
-    <hyperlink ref="D355" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
-    <hyperlink ref="E361" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
-    <hyperlink ref="E358" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
-    <hyperlink ref="E362" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
-    <hyperlink ref="F353" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
-    <hyperlink ref="F354" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
-    <hyperlink ref="E356" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
-    <hyperlink ref="G358" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
-    <hyperlink ref="D371" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
-    <hyperlink ref="E363" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
-    <hyperlink ref="E366" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
-    <hyperlink ref="E365" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
-    <hyperlink ref="F270" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
-    <hyperlink ref="E271" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
-    <hyperlink ref="E272" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
-    <hyperlink ref="E273" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
-    <hyperlink ref="G287" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
-    <hyperlink ref="E282" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
-    <hyperlink ref="E283" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
-    <hyperlink ref="E288" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
+    <hyperlink ref="E257" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
+    <hyperlink ref="D341" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
+    <hyperlink ref="D342" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
+    <hyperlink ref="E351" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
+    <hyperlink ref="E352" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
+    <hyperlink ref="E350" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
+    <hyperlink ref="D361" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
+    <hyperlink ref="E367" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
+    <hyperlink ref="E364" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
+    <hyperlink ref="E368" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
+    <hyperlink ref="F359" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
+    <hyperlink ref="F360" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
+    <hyperlink ref="E362" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
+    <hyperlink ref="G364" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
+    <hyperlink ref="D377" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
+    <hyperlink ref="E369" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
+    <hyperlink ref="E372" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
+    <hyperlink ref="E371" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
+    <hyperlink ref="F276" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
+    <hyperlink ref="E277" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
+    <hyperlink ref="E278" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
+    <hyperlink ref="E279" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
+    <hyperlink ref="G293" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
+    <hyperlink ref="E288" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
+    <hyperlink ref="E289" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
+    <hyperlink ref="E294" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
     <hyperlink ref="F157" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
     <hyperlink ref="F162" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
     <hyperlink ref="F163" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
-    <hyperlink ref="F169" r:id="rId114" xr:uid="{2B03B1F0-535A-3E4F-8FB3-35D2DE847218}"/>
-    <hyperlink ref="G174" r:id="rId115" xr:uid="{11045522-E183-B14C-B43D-5EA36E454600}"/>
-    <hyperlink ref="E191" r:id="rId116" xr:uid="{F1098A8C-3BC0-DB4F-8F9C-48B31145FEC1}"/>
-    <hyperlink ref="F176" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
-    <hyperlink ref="F170" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
-    <hyperlink ref="F179" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
-    <hyperlink ref="H266" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
-    <hyperlink ref="F378" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
-    <hyperlink ref="G392" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
-    <hyperlink ref="F379" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
-    <hyperlink ref="G394" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
-    <hyperlink ref="G396" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
-    <hyperlink ref="G399" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
-    <hyperlink ref="G403" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
-    <hyperlink ref="G428" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
-    <hyperlink ref="G426" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
-    <hyperlink ref="G431" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
-    <hyperlink ref="G437" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
-    <hyperlink ref="G441" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
-    <hyperlink ref="G454" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
-    <hyperlink ref="G459" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
-    <hyperlink ref="G475" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
+    <hyperlink ref="F170" r:id="rId114" xr:uid="{2B03B1F0-535A-3E4F-8FB3-35D2DE847218}"/>
+    <hyperlink ref="G175" r:id="rId115" xr:uid="{11045522-E183-B14C-B43D-5EA36E454600}"/>
+    <hyperlink ref="E197" r:id="rId116" xr:uid="{F1098A8C-3BC0-DB4F-8F9C-48B31145FEC1}"/>
+    <hyperlink ref="F177" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
+    <hyperlink ref="F171" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
+    <hyperlink ref="F180" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
+    <hyperlink ref="H272" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
+    <hyperlink ref="F384" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
+    <hyperlink ref="G398" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
+    <hyperlink ref="F385" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
+    <hyperlink ref="G400" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
+    <hyperlink ref="G402" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
+    <hyperlink ref="G405" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
+    <hyperlink ref="G409" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
+    <hyperlink ref="G434" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
+    <hyperlink ref="G432" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
+    <hyperlink ref="G437" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
+    <hyperlink ref="G443" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
+    <hyperlink ref="G447" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
+    <hyperlink ref="G460" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
+    <hyperlink ref="G465" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
+    <hyperlink ref="G481" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
     <hyperlink ref="E20" r:id="rId136" xr:uid="{809CA2D1-39E9-0045-A4DF-E4C0C2E97FA2}"/>
     <hyperlink ref="E21" r:id="rId137" xr:uid="{5DC44543-F2B9-F841-9097-6DB19C5EBD82}"/>
-    <hyperlink ref="G468" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
-    <hyperlink ref="G443" r:id="rId139" xr:uid="{7F4EA1D7-8774-1A4B-BF25-18ED0416CB20}"/>
-    <hyperlink ref="F209" r:id="rId140" xr:uid="{101513F3-87A1-DA41-8BF5-E4029309ECB8}"/>
-    <hyperlink ref="F194" r:id="rId141" xr:uid="{494E255E-6912-8643-B5CD-1D65E0DDCFFC}"/>
-    <hyperlink ref="F195" r:id="rId142" xr:uid="{828F749D-83DE-C14E-B637-56047AC1B384}"/>
-    <hyperlink ref="F210" r:id="rId143" xr:uid="{435D9B3C-98B6-5E49-BD30-EAA53523CDB7}"/>
-    <hyperlink ref="F211" r:id="rId144" xr:uid="{7D905409-0097-E04E-9593-2DEEBEEA0D0F}"/>
+    <hyperlink ref="G474" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
+    <hyperlink ref="G449" r:id="rId139" xr:uid="{7F4EA1D7-8774-1A4B-BF25-18ED0416CB20}"/>
+    <hyperlink ref="F215" r:id="rId140" xr:uid="{101513F3-87A1-DA41-8BF5-E4029309ECB8}"/>
+    <hyperlink ref="F200" r:id="rId141" xr:uid="{494E255E-6912-8643-B5CD-1D65E0DDCFFC}"/>
+    <hyperlink ref="F201" r:id="rId142" xr:uid="{828F749D-83DE-C14E-B637-56047AC1B384}"/>
+    <hyperlink ref="F216" r:id="rId143" xr:uid="{435D9B3C-98B6-5E49-BD30-EAA53523CDB7}"/>
+    <hyperlink ref="F217" r:id="rId144" xr:uid="{7D905409-0097-E04E-9593-2DEEBEEA0D0F}"/>
     <hyperlink ref="F149" r:id="rId145" xr:uid="{64451146-E88A-9A47-9888-71BEAC8B984E}"/>
-    <hyperlink ref="F199" r:id="rId146" xr:uid="{28F6BA28-EB9B-374C-A8A0-4077C800D23A}"/>
-    <hyperlink ref="G411" r:id="rId147" xr:uid="{20B4F69E-7592-784A-8C2E-123726A51D93}"/>
-    <hyperlink ref="F202" r:id="rId148" xr:uid="{E3C3D7C6-1E6E-FF40-8CC7-6CF1C77457E4}"/>
-    <hyperlink ref="G482" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
-    <hyperlink ref="G169" r:id="rId150" xr:uid="{9BECD448-C575-B64B-BA3F-BEE8D1CBBD43}"/>
-    <hyperlink ref="G488" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
-    <hyperlink ref="G489" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
-    <hyperlink ref="G490" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
-    <hyperlink ref="G493" r:id="rId154" xr:uid="{FB93E0B8-2537-FD47-8420-84D2A706F697}"/>
-    <hyperlink ref="G494" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
+    <hyperlink ref="F205" r:id="rId146" xr:uid="{28F6BA28-EB9B-374C-A8A0-4077C800D23A}"/>
+    <hyperlink ref="G417" r:id="rId147" xr:uid="{20B4F69E-7592-784A-8C2E-123726A51D93}"/>
+    <hyperlink ref="F208" r:id="rId148" xr:uid="{E3C3D7C6-1E6E-FF40-8CC7-6CF1C77457E4}"/>
+    <hyperlink ref="G488" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
+    <hyperlink ref="G170" r:id="rId150" xr:uid="{9BECD448-C575-B64B-BA3F-BEE8D1CBBD43}"/>
+    <hyperlink ref="G494" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
+    <hyperlink ref="G495" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
+    <hyperlink ref="G496" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
+    <hyperlink ref="G499" r:id="rId154" xr:uid="{FB93E0B8-2537-FD47-8420-84D2A706F697}"/>
+    <hyperlink ref="G500" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
+    <hyperlink ref="F183" r:id="rId156" location="2116892" xr:uid="{FF1C16E6-B146-B548-B694-396AC9D0B975}"/>
+    <hyperlink ref="G168" r:id="rId157" xr:uid="{ED09A21C-0057-1146-8BFF-213A32FC88DF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6405,7 +6463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069EEB69-0D57-C040-8545-840D5862E858}">
   <dimension ref="B2:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added tips for regex in python
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AAF8B8-597C-DA4A-A835-3D0477390FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A404700B-C4D7-1445-AB86-04F1A1D438E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="2280" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="773">
   <si>
     <t>docker</t>
   </si>
@@ -2339,6 +2339,27 @@
   </si>
   <si>
     <t>https://stackoverflow.com/questions/4950725/how-can-i-see-which-git-branches-are-tracking-which-remote-upstream-branch</t>
+  </si>
+  <si>
+    <t>How to use Flask with gevent (uWSGI and Gunicorn editions)</t>
+  </si>
+  <si>
+    <t>gevent, uWSGI and Gunicorn</t>
+  </si>
+  <si>
+    <t>https://iximiuz.com/en/posts/flask-gevent-tutorial/</t>
+  </si>
+  <si>
+    <t>remove text within parentheses with a regex</t>
+  </si>
+  <si>
+    <t>regex</t>
+  </si>
+  <si>
+    <t>\([^()]*\)</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/640001/how-can-i-remove-text-within-parentheses-with-a-regex</t>
   </si>
 </sst>
 </file>
@@ -5782,10 +5803,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G53"/>
+  <dimension ref="B2:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:XFD50"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6366,6 +6387,34 @@
     <row r="53" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F53" s="1" t="s">
         <v>745</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>766</v>
+      </c>
+      <c r="E54" t="s">
+        <v>767</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>769</v>
+      </c>
+      <c r="C55" t="s">
+        <v>469</v>
+      </c>
+      <c r="D55" t="s">
+        <v>770</v>
+      </c>
+      <c r="E55" t="s">
+        <v>771</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>772</v>
       </c>
     </row>
   </sheetData>
@@ -6421,6 +6470,8 @@
     <hyperlink ref="F52" r:id="rId49" xr:uid="{FF9072C2-3183-A945-AF8E-32D4E261E3A9}"/>
     <hyperlink ref="F53" r:id="rId50" xr:uid="{3C8AC7EE-5054-294D-87D4-1A6913F0B8B2}"/>
     <hyperlink ref="F50" r:id="rId51" xr:uid="{B9356038-CF05-854A-AFF1-D7384A989DFB}"/>
+    <hyperlink ref="F54" r:id="rId52" xr:uid="{61072865-D316-554C-A5B2-DE65C0BB4955}"/>
+    <hyperlink ref="F55" r:id="rId53" xr:uid="{3D288582-752C-394F-85D5-4AC8FCF2210E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for listdir
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A404700B-C4D7-1445-AB86-04F1A1D438E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902A25F7-6126-394F-8CA6-197D7432536A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="776">
   <si>
     <t>docker</t>
   </si>
@@ -2360,6 +2360,15 @@
   </si>
   <si>
     <t>https://stackoverflow.com/questions/640001/how-can-i-remove-text-within-parentheses-with-a-regex</t>
+  </si>
+  <si>
+    <t>onlyfiles = [f for f in listdir(mypath) if isfile(join(mypath, f))]</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/3207219/how-do-i-list-all-files-of-a-directory</t>
+  </si>
+  <si>
+    <t>How do I list all files of a directory?</t>
   </si>
 </sst>
 </file>
@@ -2824,7 +2833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
   <dimension ref="B1:I500"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G169" sqref="G169"/>
     </sheetView>
@@ -5803,10 +5812,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G55"/>
+  <dimension ref="B2:G56"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:XFD55"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6415,6 +6424,20 @@
       </c>
       <c r="F55" s="1" t="s">
         <v>772</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>775</v>
+      </c>
+      <c r="C56" t="s">
+        <v>469</v>
+      </c>
+      <c r="E56" t="s">
+        <v>773</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>774</v>
       </c>
     </row>
   </sheetData>
@@ -6472,6 +6495,7 @@
     <hyperlink ref="F50" r:id="rId51" xr:uid="{B9356038-CF05-854A-AFF1-D7384A989DFB}"/>
     <hyperlink ref="F54" r:id="rId52" xr:uid="{61072865-D316-554C-A5B2-DE65C0BB4955}"/>
     <hyperlink ref="F55" r:id="rId53" xr:uid="{3D288582-752C-394F-85D5-4AC8FCF2210E}"/>
+    <hyperlink ref="F56" r:id="rId54" xr:uid="{634A44CB-CBAB-AE4D-898A-98A6804C37BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for packaging python project
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902A25F7-6126-394F-8CA6-197D7432536A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68559CFA-B740-5C4C-B33E-4D3B93193FF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="776">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="779">
   <si>
     <t>docker</t>
   </si>
@@ -2369,6 +2369,15 @@
   </si>
   <si>
     <t>How do I list all files of a directory?</t>
+  </si>
+  <si>
+    <t>full list</t>
+  </si>
+  <si>
+    <t>https://setuptools.readthedocs.io/en/latest/pkg_resources.html</t>
+  </si>
+  <si>
+    <t>setuptools</t>
   </si>
 </sst>
 </file>
@@ -5812,10 +5821,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G56"/>
+  <dimension ref="B2:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6438,6 +6447,25 @@
       </c>
       <c r="F56" s="1" t="s">
         <v>774</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>727</v>
+      </c>
+      <c r="E57" t="s">
+        <v>776</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>778</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>777</v>
       </c>
     </row>
   </sheetData>
@@ -6496,6 +6524,8 @@
     <hyperlink ref="F54" r:id="rId52" xr:uid="{61072865-D316-554C-A5B2-DE65C0BB4955}"/>
     <hyperlink ref="F55" r:id="rId53" xr:uid="{3D288582-752C-394F-85D5-4AC8FCF2210E}"/>
     <hyperlink ref="F56" r:id="rId54" xr:uid="{634A44CB-CBAB-AE4D-898A-98A6804C37BE}"/>
+    <hyperlink ref="F57" r:id="rId55" xr:uid="{CBA3AB68-A9B5-7E45-AAF4-E420DC08CECB}"/>
+    <hyperlink ref="F58" r:id="rId56" xr:uid="{6513D8D1-CA9F-DB4F-8EE3-BB85344F470E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for matplotlib and postgresql
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68559CFA-B740-5C4C-B33E-4D3B93193FF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332824CC-3F39-EF41-90CD-42B4C4D8D842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="784">
   <si>
     <t>docker</t>
   </si>
@@ -2041,9 +2041,6 @@
     <t>df.set_index('Date').stack().reset_index(name='Val').rename(columns={'level_1':'X'})</t>
   </si>
   <si>
-    <t>install python library</t>
-  </si>
-  <si>
     <t>change pandas nano to postgresdb null</t>
   </si>
   <si>
@@ -2378,6 +2375,24 @@
   </si>
   <si>
     <t>setuptools</t>
+  </si>
+  <si>
+    <t>X-axis doesn't show entirely</t>
+  </si>
+  <si>
+    <t>plt.tight_layout()</t>
+  </si>
+  <si>
+    <t>https://github.com/matplotlib/matplotlib/issues/9183/</t>
+  </si>
+  <si>
+    <t>PostgresDB</t>
+  </si>
+  <si>
+    <t>Data types</t>
+  </si>
+  <si>
+    <t>https://www.postgresql.org/docs/9.1/datatype.html</t>
   </si>
 </sst>
 </file>
@@ -2842,9 +2857,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
   <dimension ref="B1:I500"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G169" sqref="G169"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A404" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D424" sqref="D424"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3733,34 +3748,34 @@
     </row>
     <row r="148" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C148" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="149" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D149" t="s">
+        <v>678</v>
+      </c>
+      <c r="E149" t="s">
         <v>679</v>
       </c>
-      <c r="E149" t="s">
-        <v>680</v>
-      </c>
       <c r="F149" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="150" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D150" t="s">
+        <v>680</v>
+      </c>
+      <c r="E150" t="s">
         <v>681</v>
-      </c>
-      <c r="E150" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="151" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D151" t="s">
+        <v>682</v>
+      </c>
+      <c r="E151" t="s">
         <v>683</v>
-      </c>
-      <c r="E151" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="153" spans="3:6" x14ac:dyDescent="0.2">
@@ -3875,13 +3890,13 @@
     </row>
     <row r="168" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D168" t="s">
+        <v>762</v>
+      </c>
+      <c r="E168" t="s">
         <v>763</v>
       </c>
-      <c r="E168" t="s">
+      <c r="G168" s="1" t="s">
         <v>764</v>
-      </c>
-      <c r="G168" s="1" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="169" spans="3:7" x14ac:dyDescent="0.2">
@@ -3901,7 +3916,7 @@
         <v>64</v>
       </c>
       <c r="G170" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="171" spans="3:7" x14ac:dyDescent="0.2">
@@ -3996,23 +4011,23 @@
     </row>
     <row r="182" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C182" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="183" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D183" t="s">
+        <v>760</v>
+      </c>
+      <c r="E183" t="s">
+        <v>759</v>
+      </c>
+      <c r="F183" s="1" t="s">
         <v>761</v>
-      </c>
-      <c r="E183" t="s">
-        <v>760</v>
-      </c>
-      <c r="F183" s="1" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="184" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E184" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="192" spans="2:7" x14ac:dyDescent="0.2">
@@ -4104,48 +4119,48 @@
     </row>
     <row r="204" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B204" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="F204" s="1"/>
     </row>
     <row r="205" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C205" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D205" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="F205" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="206" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C206" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D206" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="F206" s="1"/>
     </row>
     <row r="207" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C207" t="s">
+        <v>691</v>
+      </c>
+      <c r="D207" t="s">
         <v>692</v>
-      </c>
-      <c r="D207" t="s">
-        <v>693</v>
       </c>
       <c r="F207" s="1"/>
     </row>
     <row r="208" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C208" t="s">
+        <v>706</v>
+      </c>
+      <c r="D208" t="s">
         <v>707</v>
       </c>
-      <c r="D208" t="s">
+      <c r="F208" s="1" t="s">
         <v>708</v>
-      </c>
-      <c r="F208" s="1" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="209" spans="2:6" x14ac:dyDescent="0.2">
@@ -5247,23 +5262,26 @@
     </row>
     <row r="417" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D417" t="s">
+        <v>696</v>
+      </c>
+      <c r="E417" t="s">
+        <v>698</v>
+      </c>
+      <c r="G417" s="1" t="s">
         <v>697</v>
       </c>
-      <c r="E417" t="s">
-        <v>699</v>
-      </c>
-      <c r="G417" s="1" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="423" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C423" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="424" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D424">
-        <v>1</v>
+    </row>
+    <row r="420" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B420" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="421" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C421" t="s">
+        <v>782</v>
+      </c>
+      <c r="G421" s="1" t="s">
+        <v>783</v>
       </c>
     </row>
     <row r="430" spans="2:7" x14ac:dyDescent="0.2">
@@ -5566,93 +5584,93 @@
     </row>
     <row r="487" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B487" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="488" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C488" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D488" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="G488" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="489" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C489" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D489" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="490" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C490" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D490" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="493" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B493" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="494" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C494" t="s">
+        <v>734</v>
+      </c>
+      <c r="G494" s="1" t="s">
         <v>735</v>
-      </c>
-      <c r="G494" s="1" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="495" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C495" t="s">
+        <v>736</v>
+      </c>
+      <c r="G495" s="1" t="s">
         <v>737</v>
-      </c>
-      <c r="G495" s="1" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="496" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C496" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="F496" t="s">
+        <v>738</v>
+      </c>
+      <c r="G496" s="1" t="s">
         <v>739</v>
-      </c>
-      <c r="G496" s="1" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="498" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B498" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="499" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C499" t="s">
+        <v>746</v>
+      </c>
+      <c r="D499" t="s">
         <v>747</v>
       </c>
-      <c r="D499" t="s">
+      <c r="G499" s="1" t="s">
         <v>748</v>
-      </c>
-      <c r="G499" s="1" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="500" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C500" t="s">
+        <v>749</v>
+      </c>
+      <c r="D500" t="s">
         <v>750</v>
       </c>
-      <c r="D500" t="s">
+      <c r="G500" s="1" t="s">
         <v>751</v>
-      </c>
-      <c r="G500" s="1" t="s">
-        <v>752</v>
       </c>
     </row>
   </sheetData>
@@ -5814,6 +5832,7 @@
     <hyperlink ref="G500" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
     <hyperlink ref="F183" r:id="rId156" location="2116892" xr:uid="{FF1C16E6-B146-B548-B694-396AC9D0B975}"/>
     <hyperlink ref="G168" r:id="rId157" xr:uid="{ED09A21C-0057-1146-8BFF-213A32FC88DF}"/>
+    <hyperlink ref="G421" r:id="rId158" xr:uid="{F933A5C4-6DD5-5547-8BB3-B5D3FBA7A852}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5821,10 +5840,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G58"/>
+  <dimension ref="B2:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59:F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6245,51 +6264,51 @@
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D37" t="s">
         <v>448</v>
       </c>
       <c r="E37" t="s">
+        <v>667</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>668</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
+        <v>669</v>
+      </c>
+      <c r="E38" t="s">
         <v>670</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" s="1" t="s">
         <v>671</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
+        <v>672</v>
+      </c>
+      <c r="E39" t="s">
         <v>673</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" s="1" t="s">
         <v>674</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C41" t="s">
         <v>169</v>
@@ -6298,174 +6317,188 @@
         <v>448</v>
       </c>
       <c r="E41" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E42" t="s">
+        <v>702</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>703</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E43" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E46" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E47" t="s">
+        <v>721</v>
+      </c>
+      <c r="F47" t="s">
         <v>722</v>
-      </c>
-      <c r="F47" t="s">
-        <v>723</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D49" t="s">
         <v>448</v>
       </c>
       <c r="E49" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
+        <v>752</v>
+      </c>
+      <c r="E50" t="s">
         <v>753</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" s="1" t="s">
         <v>754</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
+        <v>741</v>
+      </c>
+      <c r="E52" t="s">
         <v>742</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" s="1" t="s">
         <v>743</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F53" s="1" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
+        <v>765</v>
+      </c>
+      <c r="E54" t="s">
         <v>766</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" s="1" t="s">
         <v>767</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C55" t="s">
         <v>469</v>
       </c>
       <c r="D55" t="s">
+        <v>769</v>
+      </c>
+      <c r="E55" t="s">
         <v>770</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" s="1" t="s">
         <v>771</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C56" t="s">
         <v>469</v>
       </c>
       <c r="E56" t="s">
+        <v>772</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>773</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E57" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
+        <v>777</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
         <v>778</v>
       </c>
-      <c r="F58" s="1" t="s">
-        <v>777</v>
+      <c r="C59" t="s">
+        <v>469</v>
+      </c>
+      <c r="E59" t="s">
+        <v>779</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>780</v>
       </c>
     </row>
   </sheetData>
@@ -6526,6 +6559,7 @@
     <hyperlink ref="F56" r:id="rId54" xr:uid="{634A44CB-CBAB-AE4D-898A-98A6804C37BE}"/>
     <hyperlink ref="F57" r:id="rId55" xr:uid="{CBA3AB68-A9B5-7E45-AAF4-E420DC08CECB}"/>
     <hyperlink ref="F58" r:id="rId56" xr:uid="{6513D8D1-CA9F-DB4F-8EE3-BB85344F470E}"/>
+    <hyperlink ref="F59" r:id="rId57" xr:uid="{F0C558B0-9D09-2E47-9A73-03B1EBC298EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6547,13 +6581,13 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>693</v>
+      </c>
+      <c r="C2" t="s">
         <v>694</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" s="1" t="s">
         <v>695</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>696</v>
       </c>
     </row>
   </sheetData>
@@ -6576,10 +6610,10 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>756</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>757</v>
       </c>
       <c r="D2" s="7"/>
     </row>

</xml_diff>

<commit_message>
added link for Airflow
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332824CC-3F39-EF41-90CD-42B4C4D8D842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F1CC7E-6E47-E941-9C2E-9502DE88C1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="792">
   <si>
     <t>docker</t>
   </si>
@@ -2393,6 +2393,30 @@
   </si>
   <si>
     <t>https://www.postgresql.org/docs/9.1/datatype.html</t>
+  </si>
+  <si>
+    <t>df.duplicated(keep=False)</t>
+  </si>
+  <si>
+    <t>https://pandas.pydata.org/pandas-docs/stable/reference/api/pandas.DataFrame.duplicated.html</t>
+  </si>
+  <si>
+    <t>python pandas, check duplicated rows</t>
+  </si>
+  <si>
+    <t>sns.heatmap(df, vmin=0, vmax=0.5)</t>
+  </si>
+  <si>
+    <t>sns</t>
+  </si>
+  <si>
+    <t>heatmap</t>
+  </si>
+  <si>
+    <t>Getting started with Apache Airflow</t>
+  </si>
+  <si>
+    <t>https://towardsdatascience.com/getting-started-with-apache-airflow-df1aa77d7b1b</t>
   </si>
 </sst>
 </file>
@@ -2857,8 +2881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
   <dimension ref="B1:I500"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A404" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A506" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D424" sqref="D424"/>
     </sheetView>
   </sheetViews>
@@ -5840,10 +5864,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G59"/>
+  <dimension ref="B2:G62"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59:F59"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6499,6 +6523,36 @@
       </c>
       <c r="F59" s="1" t="s">
         <v>780</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>786</v>
+      </c>
+      <c r="E60" t="s">
+        <v>784</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>789</v>
+      </c>
+      <c r="D61" t="s">
+        <v>788</v>
+      </c>
+      <c r="E61" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>790</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>791</v>
       </c>
     </row>
   </sheetData>
@@ -6560,6 +6614,8 @@
     <hyperlink ref="F57" r:id="rId55" xr:uid="{CBA3AB68-A9B5-7E45-AAF4-E420DC08CECB}"/>
     <hyperlink ref="F58" r:id="rId56" xr:uid="{6513D8D1-CA9F-DB4F-8EE3-BB85344F470E}"/>
     <hyperlink ref="F59" r:id="rId57" xr:uid="{F0C558B0-9D09-2E47-9A73-03B1EBC298EA}"/>
+    <hyperlink ref="F60" r:id="rId58" xr:uid="{0E6940AA-CCE2-A845-B000-88634DEE5413}"/>
+    <hyperlink ref="F62" r:id="rId59" xr:uid="{DB6C6106-7A38-1843-B3AC-F9FB615E4977}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for airflow
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F1CC7E-6E47-E941-9C2E-9502DE88C1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53F9696-6CE6-1F40-9E39-BB10B5CF3408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="794">
   <si>
     <t>docker</t>
   </si>
@@ -2417,6 +2417,12 @@
   </si>
   <si>
     <t>https://towardsdatascience.com/getting-started-with-apache-airflow-df1aa77d7b1b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">airflow </t>
+  </si>
+  <si>
+    <t>workflow and visualisation</t>
   </si>
 </sst>
 </file>
@@ -5866,8 +5872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
   <dimension ref="B2:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6550,6 +6556,12 @@
     <row r="62" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>790</v>
+      </c>
+      <c r="C62" t="s">
+        <v>792</v>
+      </c>
+      <c r="E62" t="s">
+        <v>793</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>791</v>

</xml_diff>

<commit_message>
added tips for latex hyperlink
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9024A29A-06B6-5042-AE87-CB024DAF58FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754106BF-30F0-8D4A-A47A-EB24A861D4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="804">
   <si>
     <t>docker</t>
   </si>
@@ -2435,6 +2435,24 @@
   </si>
   <si>
     <t>faust</t>
+  </si>
+  <si>
+    <t>Excel management with python</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/XlsxWriter/</t>
+  </si>
+  <si>
+    <t>XlsxWriter</t>
+  </si>
+  <si>
+    <t>Latex hyper links library</t>
+  </si>
+  <si>
+    <t>\usepackage{hyperref}, \url{} \href{}</t>
+  </si>
+  <si>
+    <t>https://latex-tutorial.com/tutorials/hyperlinks/</t>
   </si>
 </sst>
 </file>
@@ -2900,8 +2918,8 @@
   <dimension ref="B1:I500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A344" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D424" sqref="D424"/>
+      <pane ySplit="1" topLeftCell="A480" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F162" sqref="F162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5882,10 +5900,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G63"/>
+  <dimension ref="B2:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6415,7 +6433,7 @@
       <c r="E47" t="s">
         <v>721</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F47" t="s">
         <v>722</v>
       </c>
     </row>
@@ -6591,6 +6609,31 @@
       </c>
       <c r="F63" s="1" t="s">
         <v>795</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>798</v>
+      </c>
+      <c r="E64" t="s">
+        <v>800</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>801</v>
+      </c>
+      <c r="C65" t="s">
+        <v>651</v>
+      </c>
+      <c r="E65" t="s">
+        <v>802</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>803</v>
       </c>
     </row>
   </sheetData>
@@ -6655,7 +6698,8 @@
     <hyperlink ref="F60" r:id="rId58" xr:uid="{0E6940AA-CCE2-A845-B000-88634DEE5413}"/>
     <hyperlink ref="F62" r:id="rId59" xr:uid="{DB6C6106-7A38-1843-B3AC-F9FB615E4977}"/>
     <hyperlink ref="F63" r:id="rId60" xr:uid="{8AED1472-61F4-E646-89E7-A2D566BEF7A0}"/>
-    <hyperlink ref="F47" r:id="rId61" xr:uid="{911C2F05-FCBF-AB49-8D94-2E5E6FF59620}"/>
+    <hyperlink ref="F64" r:id="rId61" xr:uid="{D5875307-B681-3841-BE35-59A92CDCD038}"/>
+    <hyperlink ref="F65" r:id="rId62" xr:uid="{E6DDA861-2175-8242-9563-08D5A89ACF52}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for NodeRed
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754106BF-30F0-8D4A-A47A-EB24A861D4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F1C6B0-6B8B-0E45-BB57-9BA7F82303A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="811">
   <si>
     <t>docker</t>
   </si>
@@ -2453,6 +2453,27 @@
   </si>
   <si>
     <t>https://latex-tutorial.com/tutorials/hyperlinks/</t>
+  </si>
+  <si>
+    <t>NodeRed</t>
+  </si>
+  <si>
+    <t>installation</t>
+  </si>
+  <si>
+    <t>on MacOS/Linux/Raspian</t>
+  </si>
+  <si>
+    <t>sudo npm install -g --unsafe-perm node-red</t>
+  </si>
+  <si>
+    <t>https://diyprojects.io/installing-using-node-red-macos-windows/#.YLoDxOvTXX8</t>
+  </si>
+  <si>
+    <t>start the service</t>
+  </si>
+  <si>
+    <t>node-red</t>
   </si>
 </sst>
 </file>
@@ -2915,11 +2936,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I500"/>
+  <dimension ref="B1:I506"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A480" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F162" sqref="F162"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A485" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C507" sqref="C507"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5731,6 +5752,33 @@
       </c>
       <c r="G500" s="1" t="s">
         <v>751</v>
+      </c>
+    </row>
+    <row r="504" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B504" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="505" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C505" t="s">
+        <v>805</v>
+      </c>
+      <c r="D505" t="s">
+        <v>806</v>
+      </c>
+      <c r="E505" t="s">
+        <v>807</v>
+      </c>
+      <c r="G505" s="1" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="506" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C506" t="s">
+        <v>809</v>
+      </c>
+      <c r="E506" t="s">
+        <v>810</v>
       </c>
     </row>
   </sheetData>
@@ -5893,6 +5941,7 @@
     <hyperlink ref="F183" r:id="rId156" location="2116892" xr:uid="{FF1C16E6-B146-B548-B694-396AC9D0B975}"/>
     <hyperlink ref="G168" r:id="rId157" xr:uid="{ED09A21C-0057-1146-8BFF-213A32FC88DF}"/>
     <hyperlink ref="G421" r:id="rId158" xr:uid="{F933A5C4-6DD5-5547-8BB3-B5D3FBA7A852}"/>
+    <hyperlink ref="G505" r:id="rId159" location=".YLoDxOvTXX8" xr:uid="{8886E3AC-3A64-6449-A070-17D95B586F83}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5902,8 +5951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
   <dimension ref="B2:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added tips for linux command
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A139C0F-56D1-3E4E-B6E2-9D307DE6D429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1658AE02-A0C6-954E-BA96-F093CD5A8EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3320" yWindow="780" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
     <sheet name="Random Articles" sheetId="4" r:id="rId2"/>
     <sheet name="Tips" sheetId="5" r:id="rId3"/>
-    <sheet name="Websites" sheetId="6" r:id="rId4"/>
+    <sheet name="Temporary" sheetId="7" r:id="rId4"/>
+    <sheet name="Websites" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="811">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="831">
   <si>
     <t>docker</t>
   </si>
@@ -2474,6 +2475,66 @@
   </si>
   <si>
     <t>node-red</t>
+  </si>
+  <si>
+    <t>Latex</t>
+  </si>
+  <si>
+    <t>Multiple equations alignment</t>
+  </si>
+  <si>
+    <t>\begin{align} du &amp;= \frac{1}{1 + x^2}dx  &amp;  v  &amp;= x. \end{align}</t>
+  </si>
+  <si>
+    <t>https://latex.wikia.org/wiki/Align_(environment)</t>
+  </si>
+  <si>
+    <t>Delete first line of a file</t>
+  </si>
+  <si>
+    <t>sed '1d' file.txt &gt; tmpfile; mv tmpfile file.txt</t>
+  </si>
+  <si>
+    <t>https://unix.stackexchange.com/questions/96226/delete-first-line-of-a-file</t>
+  </si>
+  <si>
+    <t>For the academic paper</t>
+  </si>
+  <si>
+    <t>http://hyperphysics.phy-astr.gsu.edu/hbase/thermo/heatra.html</t>
+  </si>
+  <si>
+    <t>https://github.com/shravan-kuchkula</t>
+  </si>
+  <si>
+    <t>Shravan Kuchkula's github</t>
+  </si>
+  <si>
+    <t>https://www.sphinx-doc.org/en/master/usage/quickstart.html</t>
+  </si>
+  <si>
+    <t>Sphinx</t>
+  </si>
+  <si>
+    <t>Marcos Schroh's github</t>
+  </si>
+  <si>
+    <t>https://github.com/marcosschroh</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Ryan Whitten's github repository</t>
+  </si>
+  <si>
+    <t>Python Schema Registry Client</t>
+  </si>
+  <si>
+    <t>https://marcosschroh.github.io/python-schema-registry-client/faust/</t>
   </si>
 </sst>
 </file>
@@ -2936,11 +2997,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I506"/>
+  <dimension ref="B1:I512"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A425" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D147" sqref="D147"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A444" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G463" sqref="G463"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5497,13 +5558,24 @@
       <c r="G450" s="1"/>
     </row>
     <row r="451" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B451" t="s">
+        <v>811</v>
+      </c>
       <c r="G451" s="1"/>
     </row>
     <row r="452" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C452" t="s">
+        <v>812</v>
+      </c>
       <c r="G452" s="1"/>
     </row>
     <row r="453" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G453" s="1"/>
+      <c r="D453" t="s">
+        <v>813</v>
+      </c>
+      <c r="G453" s="1" t="s">
+        <v>814</v>
+      </c>
     </row>
     <row r="454" spans="2:7" x14ac:dyDescent="0.2">
       <c r="G454" s="1"/>
@@ -5529,255 +5601,281 @@
         <v>571</v>
       </c>
     </row>
+    <row r="461" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C461" t="s">
+        <v>815</v>
+      </c>
+      <c r="G461" s="1"/>
+    </row>
+    <row r="462" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D462" t="s">
+        <v>816</v>
+      </c>
+      <c r="G462" s="1" t="s">
+        <v>817</v>
+      </c>
+    </row>
     <row r="463" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B463" t="s">
+      <c r="G463" s="1"/>
+    </row>
+    <row r="464" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G464" s="1"/>
+    </row>
+    <row r="465" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G465" s="1"/>
+    </row>
+    <row r="466" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G466" s="1"/>
+    </row>
+    <row r="469" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B469" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="464" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C464" t="s">
+    <row r="470" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C470" t="s">
         <v>573</v>
-      </c>
-    </row>
-    <row r="465" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D465" t="s">
-        <v>574</v>
-      </c>
-      <c r="E465" t="s">
-        <v>575</v>
-      </c>
-      <c r="F465" t="s">
-        <v>576</v>
-      </c>
-      <c r="G465" s="1" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="466" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E466" t="s">
-        <v>578</v>
-      </c>
-      <c r="F466" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="467" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C467" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="468" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D468" t="s">
-        <v>597</v>
-      </c>
-      <c r="E468" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="469" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D469" t="s">
-        <v>600</v>
-      </c>
-      <c r="E469" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="471" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D471" t="s">
-        <v>601</v>
+        <v>574</v>
       </c>
       <c r="E471" t="s">
-        <v>602</v>
+        <v>575</v>
+      </c>
+      <c r="F471" t="s">
+        <v>576</v>
+      </c>
+      <c r="G471" s="1" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="472" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D472" t="s">
-        <v>603</v>
-      </c>
       <c r="E472" t="s">
-        <v>604</v>
+        <v>578</v>
+      </c>
+      <c r="F472" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="473" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C473" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="474" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D474" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="E474" t="s">
-        <v>606</v>
-      </c>
-      <c r="G474" s="1" t="s">
-        <v>610</v>
+        <v>598</v>
       </c>
     </row>
     <row r="475" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D475" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
       <c r="E475" t="s">
-        <v>608</v>
-      </c>
-      <c r="F475" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="479" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B479" t="s">
-        <v>580</v>
+        <v>599</v>
+      </c>
+    </row>
+    <row r="477" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D477" t="s">
+        <v>601</v>
+      </c>
+      <c r="E477" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="478" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D478" t="s">
+        <v>603</v>
+      </c>
+      <c r="E478" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="480" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C480" t="s">
-        <v>581</v>
+      <c r="D480" t="s">
+        <v>605</v>
+      </c>
+      <c r="E480" t="s">
+        <v>606</v>
+      </c>
+      <c r="G480" s="1" t="s">
+        <v>610</v>
       </c>
     </row>
     <row r="481" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D481" t="s">
+        <v>607</v>
+      </c>
+      <c r="E481" t="s">
+        <v>608</v>
+      </c>
+      <c r="F481" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="485" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B485" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="486" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C486" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="487" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D487" t="s">
         <v>583</v>
       </c>
-      <c r="E481" t="s">
+      <c r="E487" t="s">
         <v>584</v>
       </c>
-      <c r="F481" t="s">
+      <c r="F487" t="s">
         <v>582</v>
       </c>
-      <c r="G481" s="1" t="s">
+      <c r="G487" s="1" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="482" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E482" t="s">
+    <row r="488" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E488" t="s">
         <v>585</v>
       </c>
-      <c r="F482" t="s">
+      <c r="F488" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="484" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D484" t="s">
+    <row r="490" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D490" t="s">
         <v>588</v>
       </c>
-      <c r="E484" t="s">
+      <c r="E490" t="s">
         <v>590</v>
       </c>
-      <c r="F484" t="s">
+      <c r="F490" t="s">
         <v>589</v>
-      </c>
-    </row>
-    <row r="487" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B487" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="488" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C488" t="s">
-        <v>710</v>
-      </c>
-      <c r="D488" t="s">
-        <v>713</v>
-      </c>
-      <c r="G488" s="1" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="489" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C489" t="s">
-        <v>711</v>
-      </c>
-      <c r="D489" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="490" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C490" t="s">
-        <v>712</v>
-      </c>
-      <c r="D490" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="493" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B493" t="s">
-        <v>733</v>
+        <v>709</v>
       </c>
     </row>
     <row r="494" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C494" t="s">
-        <v>734</v>
+        <v>710</v>
+      </c>
+      <c r="D494" t="s">
+        <v>713</v>
       </c>
       <c r="G494" s="1" t="s">
-        <v>735</v>
+        <v>716</v>
       </c>
     </row>
     <row r="495" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C495" t="s">
-        <v>736</v>
-      </c>
-      <c r="G495" s="1" t="s">
-        <v>737</v>
+        <v>711</v>
+      </c>
+      <c r="D495" t="s">
+        <v>714</v>
       </c>
     </row>
     <row r="496" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C496" t="s">
-        <v>740</v>
-      </c>
-      <c r="F496" t="s">
-        <v>738</v>
-      </c>
-      <c r="G496" s="1" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="498" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B498" t="s">
-        <v>745</v>
+        <v>712</v>
+      </c>
+      <c r="D496" t="s">
+        <v>715</v>
       </c>
     </row>
     <row r="499" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C499" t="s">
-        <v>746</v>
-      </c>
-      <c r="D499" t="s">
-        <v>747</v>
-      </c>
-      <c r="G499" s="1" t="s">
-        <v>748</v>
+      <c r="B499" t="s">
+        <v>733</v>
       </c>
     </row>
     <row r="500" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C500" t="s">
-        <v>749</v>
-      </c>
-      <c r="D500" t="s">
-        <v>750</v>
+        <v>734</v>
       </c>
       <c r="G500" s="1" t="s">
-        <v>751</v>
+        <v>735</v>
+      </c>
+    </row>
+    <row r="501" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C501" t="s">
+        <v>736</v>
+      </c>
+      <c r="G501" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="502" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C502" t="s">
+        <v>740</v>
+      </c>
+      <c r="F502" t="s">
+        <v>738</v>
+      </c>
+      <c r="G502" s="1" t="s">
+        <v>739</v>
       </c>
     </row>
     <row r="504" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B504" t="s">
-        <v>804</v>
+        <v>745</v>
       </c>
     </row>
     <row r="505" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C505" t="s">
-        <v>805</v>
+        <v>746</v>
       </c>
       <c r="D505" t="s">
-        <v>806</v>
-      </c>
-      <c r="E505" t="s">
-        <v>807</v>
+        <v>747</v>
       </c>
       <c r="G505" s="1" t="s">
-        <v>808</v>
+        <v>748</v>
       </c>
     </row>
     <row r="506" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C506" t="s">
+        <v>749</v>
+      </c>
+      <c r="D506" t="s">
+        <v>750</v>
+      </c>
+      <c r="G506" s="1" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="510" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B510" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="511" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C511" t="s">
+        <v>805</v>
+      </c>
+      <c r="D511" t="s">
+        <v>806</v>
+      </c>
+      <c r="E511" t="s">
+        <v>807</v>
+      </c>
+      <c r="G511" s="1" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="512" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C512" t="s">
         <v>809</v>
       </c>
-      <c r="E506" t="s">
+      <c r="E512" t="s">
         <v>810</v>
       </c>
     </row>
@@ -5916,11 +6014,11 @@
     <hyperlink ref="G443" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
     <hyperlink ref="G447" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
     <hyperlink ref="G460" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
-    <hyperlink ref="G465" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
-    <hyperlink ref="G481" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
+    <hyperlink ref="G471" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
+    <hyperlink ref="G487" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
     <hyperlink ref="E20" r:id="rId136" xr:uid="{809CA2D1-39E9-0045-A4DF-E4C0C2E97FA2}"/>
     <hyperlink ref="E21" r:id="rId137" xr:uid="{5DC44543-F2B9-F841-9097-6DB19C5EBD82}"/>
-    <hyperlink ref="G474" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
+    <hyperlink ref="G480" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
     <hyperlink ref="G449" r:id="rId139" xr:uid="{7F4EA1D7-8774-1A4B-BF25-18ED0416CB20}"/>
     <hyperlink ref="F215" r:id="rId140" xr:uid="{101513F3-87A1-DA41-8BF5-E4029309ECB8}"/>
     <hyperlink ref="F200" r:id="rId141" xr:uid="{494E255E-6912-8643-B5CD-1D65E0DDCFFC}"/>
@@ -5931,17 +6029,19 @@
     <hyperlink ref="F205" r:id="rId146" xr:uid="{28F6BA28-EB9B-374C-A8A0-4077C800D23A}"/>
     <hyperlink ref="G417" r:id="rId147" xr:uid="{20B4F69E-7592-784A-8C2E-123726A51D93}"/>
     <hyperlink ref="F208" r:id="rId148" xr:uid="{E3C3D7C6-1E6E-FF40-8CC7-6CF1C77457E4}"/>
-    <hyperlink ref="G488" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
+    <hyperlink ref="G494" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
     <hyperlink ref="G170" r:id="rId150" xr:uid="{9BECD448-C575-B64B-BA3F-BEE8D1CBBD43}"/>
-    <hyperlink ref="G494" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
-    <hyperlink ref="G495" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
-    <hyperlink ref="G496" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
-    <hyperlink ref="G499" r:id="rId154" xr:uid="{FB93E0B8-2537-FD47-8420-84D2A706F697}"/>
-    <hyperlink ref="G500" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
+    <hyperlink ref="G500" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
+    <hyperlink ref="G501" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
+    <hyperlink ref="G502" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
+    <hyperlink ref="G505" r:id="rId154" xr:uid="{FB93E0B8-2537-FD47-8420-84D2A706F697}"/>
+    <hyperlink ref="G506" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
     <hyperlink ref="F183" r:id="rId156" location="2116892" xr:uid="{FF1C16E6-B146-B548-B694-396AC9D0B975}"/>
     <hyperlink ref="G168" r:id="rId157" xr:uid="{ED09A21C-0057-1146-8BFF-213A32FC88DF}"/>
     <hyperlink ref="G421" r:id="rId158" xr:uid="{F933A5C4-6DD5-5547-8BB3-B5D3FBA7A852}"/>
-    <hyperlink ref="G505" r:id="rId159" location=".YLoDxOvTXX8" xr:uid="{8886E3AC-3A64-6449-A070-17D95B586F83}"/>
+    <hyperlink ref="G511" r:id="rId159" location=".YLoDxOvTXX8" xr:uid="{8886E3AC-3A64-6449-A070-17D95B586F83}"/>
+    <hyperlink ref="G453" r:id="rId160" xr:uid="{7A90D044-C84B-914D-8B65-8F4F5A691E96}"/>
+    <hyperlink ref="G462" r:id="rId161" xr:uid="{95C0F152-F90E-9248-A902-813C5C41DB01}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5949,10 +6049,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G65"/>
+  <dimension ref="B2:G67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="B39" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66:F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6683,6 +6783,22 @@
       </c>
       <c r="F65" s="1" t="s">
         <v>803</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>821</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>824</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>825</v>
       </c>
     </row>
   </sheetData>
@@ -6749,6 +6865,8 @@
     <hyperlink ref="F63" r:id="rId60" xr:uid="{8AED1472-61F4-E646-89E7-A2D566BEF7A0}"/>
     <hyperlink ref="F64" r:id="rId61" xr:uid="{D5875307-B681-3841-BE35-59A92CDCD038}"/>
     <hyperlink ref="F65" r:id="rId62" xr:uid="{E6DDA861-2175-8242-9563-08D5A89ACF52}"/>
+    <hyperlink ref="F66" r:id="rId63" xr:uid="{2230F27B-338D-C945-8CA9-6B98BE649E4C}"/>
+    <hyperlink ref="F67" r:id="rId64" xr:uid="{0B7244FD-E49B-DE4D-9F94-C6C951012F2B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6788,27 +6906,128 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069EEB69-0D57-C040-8545-840D5862E858}">
-  <dimension ref="B2:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B54335-CC07-B040-8669-E1D4D0619931}">
+  <dimension ref="B2:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>755</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>756</v>
-      </c>
-      <c r="D2" s="7"/>
+        <v>818</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C3" s="1" t="s">
+        <v>819</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{87D156EE-D133-464D-8B0D-7B076D239955}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{084566D0-D804-FC44-BD4A-E37B44FD3304}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069EEB69-0D57-C040-8545-840D5862E858}">
+  <dimension ref="B2:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="22.33203125" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>827</v>
+      </c>
+      <c r="C2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>755</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>823</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>800</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>821</v>
+      </c>
+      <c r="C6" t="s">
+        <v>797</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>824</v>
+      </c>
+      <c r="C7" t="s">
+        <v>797</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="G7" t="s">
+        <v>829</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>828</v>
+      </c>
+      <c r="C8" t="s">
+        <v>797</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>751</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{87D156EE-D133-464D-8B0D-7B076D239955}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{2B38EE35-ACF8-A74A-9C2F-0DF51F1AB49F}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{D6617805-47DE-2F43-8466-FDBF731CF931}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{D0DDD94B-D7B8-8A4C-AB06-989277EF2D71}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{800C809C-38AD-B24C-AA69-37E1C3AEDEFD}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{DC75BE35-9EC4-2640-B31C-E8D1B7C498F4}"/>
+    <hyperlink ref="H7" r:id="rId7" xr:uid="{1DD7B025-3102-2340-9FD3-AAE9A08257D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for MacOS
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1658AE02-A0C6-954E-BA96-F093CD5A8EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608055A3-9B17-0541-A0FF-921AA2ADCC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3320" yWindow="780" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="838">
   <si>
     <t>docker</t>
   </si>
@@ -2535,6 +2535,27 @@
   </si>
   <si>
     <t>https://marcosschroh.github.io/python-schema-registry-client/faust/</t>
+  </si>
+  <si>
+    <t>MacOS</t>
+  </si>
+  <si>
+    <t>sudo chown -R $(whoami) $(brew --prefix)/*</t>
+  </si>
+  <si>
+    <t>bash/zsh</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/16432071/how-to-fix-homebrew-permissions</t>
+  </si>
+  <si>
+    <t>fix homebrew permissions</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-gb/cli/azure/</t>
+  </si>
+  <si>
+    <t>Azure Command-Line Interface (CLI) documentation</t>
   </si>
 </sst>
 </file>
@@ -2997,11 +3018,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I512"/>
+  <dimension ref="B1:I515"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A444" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G463" sqref="G463"/>
+      <pane ySplit="1" topLeftCell="A497" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C518" sqref="C518"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5877,6 +5898,25 @@
       </c>
       <c r="E512" t="s">
         <v>810</v>
+      </c>
+    </row>
+    <row r="514" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B514" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="515" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C515" t="s">
+        <v>835</v>
+      </c>
+      <c r="D515" t="s">
+        <v>833</v>
+      </c>
+      <c r="E515" t="s">
+        <v>832</v>
+      </c>
+      <c r="G515" s="1" t="s">
+        <v>834</v>
       </c>
     </row>
   </sheetData>
@@ -6042,6 +6082,7 @@
     <hyperlink ref="G511" r:id="rId159" location=".YLoDxOvTXX8" xr:uid="{8886E3AC-3A64-6449-A070-17D95B586F83}"/>
     <hyperlink ref="G453" r:id="rId160" xr:uid="{7A90D044-C84B-914D-8B65-8F4F5A691E96}"/>
     <hyperlink ref="G462" r:id="rId161" xr:uid="{95C0F152-F90E-9248-A902-813C5C41DB01}"/>
+    <hyperlink ref="G515" r:id="rId162" xr:uid="{FE36496B-7285-834C-A827-32E3CC704079}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6935,15 +6976,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069EEB69-0D57-C040-8545-840D5862E858}">
-  <dimension ref="B2:H8"/>
+  <dimension ref="B2:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
     <col min="7" max="7" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7017,6 +7059,14 @@
       </c>
       <c r="D8" s="1" t="s">
         <v>751</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>837</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>836</v>
       </c>
     </row>
   </sheetData>
@@ -7028,6 +7078,7 @@
     <hyperlink ref="D7" r:id="rId5" xr:uid="{800C809C-38AD-B24C-AA69-37E1C3AEDEFD}"/>
     <hyperlink ref="D8" r:id="rId6" xr:uid="{DC75BE35-9EC4-2640-B31C-E8D1B7C498F4}"/>
     <hyperlink ref="H7" r:id="rId7" xr:uid="{1DD7B025-3102-2340-9FD3-AAE9A08257D4}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{B4112F47-434F-9B4E-B456-EA24E2B927E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for screen
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309EA894-D70C-5348-9957-133C30C6ED5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FE6F34-7F66-234E-A812-612E32FF2881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="837">
   <si>
     <t>docker</t>
   </si>
@@ -2549,6 +2549,9 @@
   </si>
   <si>
     <t>https://gist.github.com/xirixiz/b6b0c6f4917ce17a90e00f9b60566278</t>
+  </si>
+  <si>
+    <t>remove a screen</t>
   </si>
 </sst>
 </file>
@@ -3011,11 +3014,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I521"/>
+  <dimension ref="B1:I524"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3309,590 +3312,594 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C52" t="s">
-        <v>30</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>32</v>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C55" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C58" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D56" t="s">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D57" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E58" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C59" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D60" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E61" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C62" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D63" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E64" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C65" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
         <v>35</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E66" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D64" t="s">
-        <v>30</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C66" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D67" t="s">
+        <v>30</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C69" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E68" t="s">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E71" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B70" t="s">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C71" t="s">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C74" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D72" t="s">
-        <v>47</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C73" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D74" t="s">
-        <v>50</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D75" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D77" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D78" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C79" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D80" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E81" s="1"/>
+        <v>54</v>
+      </c>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C82" t="s">
-        <v>198</v>
-      </c>
-      <c r="E82" s="1"/>
+        <v>56</v>
+      </c>
     </row>
     <row r="83" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D83" t="s">
+        <v>57</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="84" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E84" s="1"/>
+    </row>
+    <row r="85" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C85" t="s">
+        <v>198</v>
+      </c>
+      <c r="E85" s="1"/>
+    </row>
+    <row r="86" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D86" t="s">
         <v>203</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E86" t="s">
         <v>53</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F86" t="s">
         <v>200</v>
       </c>
-      <c r="G83" s="1" t="s">
+      <c r="G86" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D84" t="s">
+    <row r="87" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D87" t="s">
         <v>204</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E87" t="s">
         <v>201</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F87" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E85" s="1"/>
-    </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E86" s="1"/>
-    </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C87" t="s">
+    <row r="88" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E88" s="1"/>
+    </row>
+    <row r="89" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E89" s="1"/>
+    </row>
+    <row r="90" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
         <v>192</v>
       </c>
-      <c r="E87" s="1"/>
-    </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D88" t="s">
+      <c r="E90" s="1"/>
+    </row>
+    <row r="91" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D91" t="s">
         <v>193</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="E91" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E89" s="1" t="s">
+    <row r="92" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E92" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E90" s="1" t="s">
+    <row r="93" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E93" s="1" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E91" s="1"/>
-    </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D92" t="s">
-        <v>328</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D93" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="94" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E94" s="1"/>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B104" t="s">
+    <row r="95" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D95" t="s">
+        <v>328</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="96" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D96" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E97" s="1"/>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B107" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C105" t="s">
+    <row r="108" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C108" t="s">
         <v>156</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="D108" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C106" t="s">
+    <row r="109" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C109" t="s">
         <v>158</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="D109" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C107" t="s">
+    <row r="110" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C110" t="s">
         <v>159</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="D110" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C108" t="s">
+    <row r="111" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C111" t="s">
         <v>218</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="D111" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E108" s="1" t="s">
+      <c r="E111" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C110" t="s">
+    <row r="113" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C113" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D111" t="s">
+    <row r="114" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D114" t="s">
         <v>163</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E114" t="s">
         <v>162</v>
       </c>
-      <c r="F111" s="1" t="s">
+      <c r="F114" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E112" t="s">
+    <row r="115" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E115" t="s">
         <v>274</v>
       </c>
-      <c r="F112" s="1"/>
-    </row>
-    <row r="113" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D113" t="s">
+      <c r="F115" s="1"/>
+    </row>
+    <row r="116" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D116" t="s">
         <v>165</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E116" t="s">
         <v>166</v>
       </c>
-      <c r="F113" s="1" t="s">
+      <c r="F116" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="114" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D114" t="s">
+    <row r="117" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D117" t="s">
         <v>179</v>
       </c>
-      <c r="E114" t="s">
+      <c r="E117" t="s">
         <v>180</v>
       </c>
-      <c r="F114" s="1" t="s">
+      <c r="F117" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="115" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D115" t="s">
+    <row r="118" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D118" t="s">
         <v>189</v>
       </c>
-      <c r="E115" t="s">
+      <c r="E118" t="s">
         <v>191</v>
       </c>
-      <c r="F115" t="s">
+      <c r="F118" t="s">
         <v>195</v>
       </c>
-      <c r="G115" t="s">
+      <c r="G118" t="s">
         <v>190</v>
       </c>
-      <c r="H115" s="1" t="s">
+      <c r="H118" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="I115" s="1" t="s">
+      <c r="I118" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="116" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D116" t="s">
+    <row r="119" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D119" t="s">
         <v>231</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E119" t="s">
         <v>233</v>
       </c>
-      <c r="H116" s="1" t="s">
+      <c r="H119" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="117" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D117" t="s">
+    <row r="120" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D120" t="s">
         <v>232</v>
       </c>
-      <c r="E117" t="s">
+      <c r="E120" t="s">
         <v>234</v>
       </c>
-      <c r="H117" s="1"/>
-    </row>
-    <row r="118" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D118" t="s">
+      <c r="H120" s="1"/>
+    </row>
+    <row r="121" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D121" t="s">
         <v>205</v>
       </c>
-      <c r="E118" t="s">
+      <c r="E121" t="s">
         <v>206</v>
       </c>
-      <c r="F118" s="1" t="s">
+      <c r="F121" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="119" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D119" t="s">
+    <row r="122" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D122" t="s">
         <v>208</v>
       </c>
-      <c r="E119" t="s">
+      <c r="E122" t="s">
         <v>209</v>
       </c>
-      <c r="F119" t="s">
+      <c r="F122" t="s">
         <v>210</v>
       </c>
-      <c r="G119" t="s">
+      <c r="G122" t="s">
         <v>213</v>
       </c>
-      <c r="H119" s="1" t="s">
+      <c r="H122" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="I119" s="1" t="s">
+      <c r="I122" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="120" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D120" t="s">
+    <row r="123" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D123" t="s">
         <v>219</v>
       </c>
-      <c r="E120" t="s">
+      <c r="E123" t="s">
         <v>220</v>
       </c>
-      <c r="F120" s="1" t="s">
+      <c r="F123" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="121" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D121" t="s">
+    <row r="124" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D124" t="s">
         <v>223</v>
       </c>
-      <c r="E121" t="s">
+      <c r="E124" t="s">
         <v>222</v>
       </c>
-      <c r="F121" s="1" t="s">
+      <c r="F124" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="122" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D122" t="s">
+    <row r="125" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D125" t="s">
         <v>225</v>
       </c>
-      <c r="E122" t="s">
+      <c r="E125" t="s">
         <v>226</v>
       </c>
-      <c r="F122" s="1" t="s">
+      <c r="F125" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="123" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D123" t="s">
+    <row r="126" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D126" t="s">
         <v>228</v>
       </c>
-      <c r="E123" t="s">
+      <c r="E126" t="s">
         <v>229</v>
       </c>
-      <c r="F123" s="1" t="s">
+      <c r="F126" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="124" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D124" t="s">
+    <row r="127" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D127" t="s">
         <v>235</v>
       </c>
-      <c r="E124" t="s">
+      <c r="E127" t="s">
         <v>236</v>
       </c>
-      <c r="F124" s="1" t="s">
+      <c r="F127" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="125" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E125" t="s">
+    <row r="128" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E128" t="s">
         <v>237</v>
       </c>
-      <c r="F125" s="1"/>
-    </row>
-    <row r="126" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D126" t="s">
-        <v>239</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F126" s="1"/>
-    </row>
-    <row r="127" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D127" t="s">
-        <v>246</v>
-      </c>
-      <c r="E127" t="s">
-        <v>245</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="128" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D128" t="s">
-        <v>247</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>248</v>
-      </c>
+      <c r="F128" s="1"/>
     </row>
     <row r="129" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D129" t="s">
-        <v>249</v>
-      </c>
-      <c r="E129" t="s">
-        <v>206</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F129" s="1"/>
     </row>
     <row r="130" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D130" t="s">
-        <v>251</v>
+        <v>246</v>
+      </c>
+      <c r="E130" t="s">
+        <v>245</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="131" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D131" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="132" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D132" t="s">
-        <v>272</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>273</v>
+        <v>249</v>
+      </c>
+      <c r="E132" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="133" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D133" t="s">
-        <v>254</v>
-      </c>
-      <c r="E133" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="134" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D134" t="s">
-        <v>257</v>
-      </c>
-      <c r="E134" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="135" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D135" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
     </row>
     <row r="136" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D136" t="s">
-        <v>263</v>
+        <v>254</v>
+      </c>
+      <c r="E136" t="s">
+        <v>255</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="137" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D137" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="E137" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="138" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E138" t="s">
-        <v>267</v>
-      </c>
-      <c r="F138" s="1"/>
+      <c r="D138" t="s">
+        <v>261</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="139" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D139" t="s">
+        <v>263</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="140" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D140" t="s">
+        <v>265</v>
+      </c>
+      <c r="E140" t="s">
+        <v>264</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="141" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E141" t="s">
+        <v>267</v>
+      </c>
+      <c r="F141" s="1"/>
+    </row>
+    <row r="142" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D142" t="s">
         <v>282</v>
       </c>
-      <c r="F139" s="1" t="s">
+      <c r="F142" s="1" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="140" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F140" s="1"/>
-    </row>
-    <row r="141" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F141" s="1"/>
-    </row>
-    <row r="142" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F142" s="1"/>
     </row>
     <row r="143" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F143" s="1"/>
@@ -3901,1443 +3908,1437 @@
       <c r="F144" s="1"/>
     </row>
     <row r="145" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B145" t="s">
+      <c r="F145" s="1"/>
+    </row>
+    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F146" s="1"/>
+    </row>
+    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F147" s="1"/>
+    </row>
+    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B148" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C146" t="s">
+    <row r="149" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C149" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D147" t="s">
+    <row r="150" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D150" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D148" t="s">
+    <row r="151" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D151" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C150" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D151" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="153" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C153" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="154" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D154" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="156" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C156" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D154" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D155" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D156" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="157" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D157" t="s">
-        <v>69</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="158" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D158" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="159" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C159" t="s">
-        <v>346</v>
+      <c r="D159" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="160" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D160" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="162" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C162" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="163" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D163" t="s">
         <v>349</v>
       </c>
-      <c r="E160" t="s">
+      <c r="E163" t="s">
         <v>347</v>
       </c>
-      <c r="F160" s="1" t="s">
+      <c r="F163" s="1" t="s">
         <v>348</v>
-      </c>
-    </row>
-    <row r="161" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D161" t="s">
-        <v>350</v>
-      </c>
-      <c r="E161" t="s">
-        <v>351</v>
-      </c>
-      <c r="F161" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="163" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C163" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="164" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D164" t="s">
+        <v>350</v>
+      </c>
+      <c r="E164" t="s">
+        <v>351</v>
+      </c>
+      <c r="F164" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="166" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C166" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="167" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D167" t="s">
         <v>676</v>
       </c>
-      <c r="E164" t="s">
+      <c r="E167" t="s">
         <v>677</v>
       </c>
-      <c r="F164" s="1" t="s">
+      <c r="F167" s="1" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="165" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D165" t="s">
+    <row r="168" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D168" t="s">
         <v>678</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E168" t="s">
         <v>679</v>
-      </c>
-    </row>
-    <row r="166" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D166" t="s">
-        <v>680</v>
-      </c>
-      <c r="E166" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="168" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C168" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="169" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D169" t="s">
+        <v>680</v>
+      </c>
+      <c r="E169" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="171" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C171" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="172" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D172" t="s">
         <v>354</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E172" t="s">
         <v>353</v>
-      </c>
-    </row>
-    <row r="170" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D170" t="s">
-        <v>355</v>
-      </c>
-      <c r="E170" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="172" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C172" t="s">
-        <v>369</v>
-      </c>
-      <c r="F172" s="1" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="173" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D173" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="E173" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="174" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D174" t="s">
-        <v>372</v>
-      </c>
-      <c r="E174" t="s">
-        <v>373</v>
+        <v>356</v>
       </c>
     </row>
     <row r="175" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D175" t="s">
-        <v>374</v>
-      </c>
-      <c r="E175" t="s">
-        <v>375</v>
+      <c r="C175" t="s">
+        <v>369</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="176" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D176" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E176" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
     </row>
     <row r="177" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D177" t="s">
-        <v>385</v>
+        <v>372</v>
       </c>
       <c r="E177" t="s">
-        <v>386</v>
-      </c>
-      <c r="F177" s="1" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
     </row>
     <row r="178" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D178" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
       <c r="E178" t="s">
-        <v>389</v>
-      </c>
-      <c r="F178" s="1" t="s">
-        <v>390</v>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="179" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D179" t="s">
+        <v>376</v>
+      </c>
+      <c r="E179" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="180" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C180" t="s">
-        <v>379</v>
+      <c r="D180" t="s">
+        <v>385</v>
+      </c>
+      <c r="E180" t="s">
+        <v>386</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="181" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D181" t="s">
+        <v>388</v>
+      </c>
+      <c r="E181" t="s">
+        <v>389</v>
+      </c>
+      <c r="F181" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="183" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C183" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="184" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D184" t="s">
         <v>380</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E184" t="s">
         <v>381</v>
       </c>
-      <c r="F181" t="s">
+      <c r="F184" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="182" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D182" t="s">
+    <row r="185" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D185" t="s">
         <v>809</v>
       </c>
-      <c r="E182" t="s">
+      <c r="E185" t="s">
         <v>382</v>
       </c>
-      <c r="F182" t="s">
+      <c r="F185" t="s">
         <v>384</v>
-      </c>
-    </row>
-    <row r="183" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D183" t="s">
-        <v>760</v>
-      </c>
-      <c r="E183" t="s">
-        <v>761</v>
-      </c>
-      <c r="G183" s="1" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="184" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="F184" s="1"/>
-    </row>
-    <row r="185" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C185" t="s">
-        <v>391</v>
-      </c>
-      <c r="D185" t="s">
-        <v>419</v>
-      </c>
-      <c r="E185" t="s">
-        <v>392</v>
-      </c>
-      <c r="F185" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G185" s="1" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="186" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D186" t="s">
-        <v>420</v>
+        <v>760</v>
       </c>
       <c r="E186" t="s">
-        <v>421</v>
-      </c>
-      <c r="F186" s="1" t="s">
-        <v>422</v>
+        <v>761</v>
+      </c>
+      <c r="G186" s="1" t="s">
+        <v>762</v>
       </c>
     </row>
     <row r="187" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D187" t="s">
-        <v>423</v>
-      </c>
-      <c r="E187" t="s">
-        <v>424</v>
-      </c>
       <c r="F187" s="1"/>
     </row>
     <row r="188" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C188" t="s">
-        <v>393</v>
-      </c>
-      <c r="F188" s="1"/>
+        <v>391</v>
+      </c>
+      <c r="D188" t="s">
+        <v>419</v>
+      </c>
+      <c r="E188" t="s">
+        <v>392</v>
+      </c>
+      <c r="F188" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G188" s="1" t="s">
+        <v>725</v>
+      </c>
     </row>
     <row r="189" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D189" t="s">
-        <v>395</v>
+        <v>420</v>
       </c>
       <c r="E189" t="s">
-        <v>394</v>
-      </c>
-      <c r="F189" s="1"/>
+        <v>421</v>
+      </c>
+      <c r="F189" s="1" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="190" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D190" t="s">
-        <v>396</v>
-      </c>
-      <c r="F190" t="s">
-        <v>397</v>
-      </c>
-      <c r="G190" s="1" t="s">
-        <v>398</v>
-      </c>
+        <v>423</v>
+      </c>
+      <c r="E190" t="s">
+        <v>424</v>
+      </c>
+      <c r="F190" s="1"/>
     </row>
     <row r="191" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C191" t="s">
+        <v>393</v>
+      </c>
+      <c r="F191" s="1"/>
+    </row>
+    <row r="192" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D192" t="s">
+        <v>395</v>
+      </c>
+      <c r="E192" t="s">
+        <v>394</v>
+      </c>
+      <c r="F192" s="1"/>
+    </row>
+    <row r="193" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D193" t="s">
+        <v>396</v>
+      </c>
+      <c r="F193" t="s">
+        <v>397</v>
+      </c>
+      <c r="G193" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="194" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C194" t="s">
         <v>415</v>
       </c>
-      <c r="G191" s="1"/>
-    </row>
-    <row r="192" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E192" t="s">
+      <c r="G194" s="1"/>
+    </row>
+    <row r="195" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E195" t="s">
         <v>416</v>
       </c>
-      <c r="F192" s="1" t="s">
+      <c r="F195" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="G192" s="1"/>
-    </row>
-    <row r="193" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E193" t="s">
+      <c r="G195" s="1"/>
+    </row>
+    <row r="196" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E196" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="194" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C194" t="s">
+    <row r="197" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C197" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="195" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D195" t="s">
+    <row r="198" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D198" t="s">
         <v>431</v>
       </c>
-      <c r="E195" t="s">
+      <c r="E198" t="s">
         <v>433</v>
       </c>
-      <c r="F195" s="1" t="s">
+      <c r="F198" s="1" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="196" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D196" t="s">
+    <row r="199" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D199" t="s">
         <v>432</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E199" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="197" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C197" t="s">
+    <row r="200" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C200" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="198" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D198" t="s">
+    <row r="201" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D201" t="s">
         <v>758</v>
       </c>
-      <c r="E198" t="s">
+      <c r="E201" t="s">
         <v>757</v>
       </c>
-      <c r="F198" s="1" t="s">
+      <c r="F201" s="1" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="199" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E199" t="s">
+    <row r="202" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E202" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="200" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C200" t="s">
+    <row r="203" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C203" t="s">
         <v>810</v>
       </c>
     </row>
-    <row r="201" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D201" t="s">
+    <row r="204" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D204" t="s">
         <v>812</v>
       </c>
-      <c r="E201" t="s">
+      <c r="E204" t="s">
         <v>811</v>
       </c>
-      <c r="F201" s="1" t="s">
+      <c r="F204" s="1" t="s">
         <v>813</v>
       </c>
     </row>
-    <row r="207" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B207" t="s">
+    <row r="210" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B210" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="208" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C208" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="209" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D209" t="s">
-        <v>170</v>
-      </c>
-      <c r="E209" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="210" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D210" t="s">
-        <v>174</v>
-      </c>
-      <c r="E210" t="s">
-        <v>172</v>
-      </c>
-      <c r="F210" s="1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="211" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C211" t="s">
-        <v>321</v>
-      </c>
-      <c r="E211" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="F211" s="1"/>
+        <v>169</v>
+      </c>
     </row>
     <row r="212" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C212" t="s">
-        <v>404</v>
-      </c>
       <c r="D212" t="s">
-        <v>405</v>
+        <v>170</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="F212" s="1"/>
+        <v>171</v>
+      </c>
     </row>
     <row r="213" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D213" t="s">
-        <v>406</v>
-      </c>
-      <c r="F213" s="1"/>
+        <v>174</v>
+      </c>
+      <c r="E213" t="s">
+        <v>172</v>
+      </c>
+      <c r="F213" s="1" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="214" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C214" t="s">
+        <v>321</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="F214" s="1"/>
     </row>
     <row r="215" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C215" t="s">
-        <v>616</v>
+        <v>404</v>
       </c>
       <c r="D215" t="s">
-        <v>617</v>
-      </c>
-      <c r="F215" s="1" t="s">
-        <v>618</v>
-      </c>
+        <v>405</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="F215" s="1"/>
     </row>
     <row r="216" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C216" t="s">
-        <v>620</v>
-      </c>
       <c r="D216" t="s">
-        <v>619</v>
-      </c>
-      <c r="F216" s="1" t="s">
-        <v>621</v>
-      </c>
+        <v>406</v>
+      </c>
+      <c r="F216" s="1"/>
     </row>
     <row r="217" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F217" s="1"/>
     </row>
     <row r="218" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F218" s="1"/>
+      <c r="C218" t="s">
+        <v>616</v>
+      </c>
+      <c r="D218" t="s">
+        <v>617</v>
+      </c>
+      <c r="F218" s="1" t="s">
+        <v>618</v>
+      </c>
     </row>
     <row r="219" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B219" t="s">
+      <c r="C219" t="s">
+        <v>620</v>
+      </c>
+      <c r="D219" t="s">
+        <v>619</v>
+      </c>
+      <c r="F219" s="1" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="220" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F220" s="1"/>
+    </row>
+    <row r="221" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F221" s="1"/>
+    </row>
+    <row r="222" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B222" t="s">
         <v>683</v>
-      </c>
-      <c r="F219" s="1"/>
-    </row>
-    <row r="220" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C220" t="s">
-        <v>684</v>
-      </c>
-      <c r="D220" t="s">
-        <v>686</v>
-      </c>
-      <c r="F220" s="1" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="221" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C221" t="s">
-        <v>685</v>
-      </c>
-      <c r="D221" t="s">
-        <v>687</v>
-      </c>
-      <c r="F221" s="1"/>
-    </row>
-    <row r="222" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C222" t="s">
-        <v>689</v>
-      </c>
-      <c r="D222" t="s">
-        <v>690</v>
       </c>
       <c r="F222" s="1"/>
     </row>
     <row r="223" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C223" t="s">
+        <v>684</v>
+      </c>
+      <c r="D223" t="s">
+        <v>686</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="224" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C224" t="s">
+        <v>685</v>
+      </c>
+      <c r="D224" t="s">
+        <v>687</v>
+      </c>
+      <c r="F224" s="1"/>
+    </row>
+    <row r="225" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C225" t="s">
+        <v>689</v>
+      </c>
+      <c r="D225" t="s">
+        <v>690</v>
+      </c>
+      <c r="F225" s="1"/>
+    </row>
+    <row r="226" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C226" t="s">
         <v>704</v>
       </c>
-      <c r="D223" t="s">
+      <c r="D226" t="s">
         <v>705</v>
       </c>
-      <c r="F223" s="1" t="s">
+      <c r="F226" s="1" t="s">
         <v>706</v>
       </c>
-    </row>
-    <row r="224" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F224" s="1"/>
-    </row>
-    <row r="225" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F225" s="1"/>
-    </row>
-    <row r="226" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F226" s="1"/>
     </row>
     <row r="227" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F227" s="1"/>
     </row>
+    <row r="228" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F228" s="1"/>
+    </row>
     <row r="229" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B229" t="s">
+      <c r="F229" s="1"/>
+    </row>
+    <row r="230" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F230" s="1"/>
+    </row>
+    <row r="232" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B232" t="s">
         <v>446</v>
-      </c>
-    </row>
-    <row r="230" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C230" t="s">
-        <v>614</v>
-      </c>
-      <c r="D230" t="s">
-        <v>613</v>
-      </c>
-      <c r="F230" s="1" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="231" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C231" t="s">
-        <v>622</v>
-      </c>
-      <c r="D231" t="s">
-        <v>623</v>
-      </c>
-      <c r="F231" s="1" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="232" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C232" t="s">
-        <v>626</v>
-      </c>
-      <c r="D232" t="s">
-        <v>625</v>
-      </c>
-      <c r="F232" s="1" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="233" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C233" t="s">
+        <v>614</v>
+      </c>
+      <c r="D233" t="s">
+        <v>613</v>
+      </c>
+      <c r="F233" s="1" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="234" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C234" t="s">
+        <v>622</v>
+      </c>
+      <c r="D234" t="s">
+        <v>623</v>
+      </c>
+      <c r="F234" s="1" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="235" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C235" t="s">
+        <v>626</v>
+      </c>
+      <c r="D235" t="s">
+        <v>625</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="236" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C236" t="s">
         <v>629</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D236" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="240" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B240" t="s">
+    <row r="243" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B243" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="241" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C241" t="s">
-        <v>175</v>
-      </c>
-      <c r="D241" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="242" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C242" t="s">
-        <v>177</v>
-      </c>
-      <c r="D242" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="243" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C243" t="s">
-        <v>292</v>
-      </c>
-      <c r="D243" s="1" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="244" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C244" t="s">
-        <v>293</v>
+        <v>175</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>294</v>
+        <v>176</v>
       </c>
     </row>
     <row r="245" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C245" t="s">
+        <v>177</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="246" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C246" t="s">
+        <v>292</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="247" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C247" t="s">
+        <v>293</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="248" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C248" t="s">
         <v>296</v>
       </c>
-      <c r="D245" s="1" t="s">
+      <c r="D248" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="246" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D246" s="1"/>
-    </row>
-    <row r="247" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D247" s="1"/>
-    </row>
-    <row r="248" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B248" t="s">
+    <row r="249" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D249" s="1"/>
+    </row>
+    <row r="250" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D250" s="1"/>
+    </row>
+    <row r="251" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B251" t="s">
         <v>342</v>
       </c>
-      <c r="D248" s="1"/>
-    </row>
-    <row r="249" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C249" t="s">
+      <c r="D251" s="1"/>
+    </row>
+    <row r="252" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C252" t="s">
         <v>343</v>
       </c>
-      <c r="D249" t="s">
+      <c r="D252" t="s">
         <v>368</v>
       </c>
-      <c r="E249" s="1" t="s">
+      <c r="E252" s="1" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="250" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D250" t="s">
+    <row r="253" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D253" t="s">
         <v>367</v>
       </c>
-      <c r="E250" s="1" t="s">
+      <c r="E253" s="1" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="251" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D251" s="1"/>
-    </row>
-    <row r="252" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D252" s="1"/>
-    </row>
-    <row r="253" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D253" s="1"/>
-    </row>
-    <row r="257" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B257" t="s">
+    <row r="254" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D254" s="1"/>
+    </row>
+    <row r="255" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D255" s="1"/>
+    </row>
+    <row r="256" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D256" s="1"/>
+    </row>
+    <row r="260" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B260" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="258" spans="2:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="C258" s="4" t="s">
+    <row r="261" spans="2:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="C261" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="D258" s="2" t="s">
+      <c r="D261" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E258" s="1" t="s">
+      <c r="E261" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="259" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C259" t="s">
+    <row r="262" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C262" t="s">
         <v>186</v>
       </c>
-      <c r="E259" s="1" t="s">
+      <c r="E262" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="260" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C260" t="s">
+    <row r="263" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C263" t="s">
         <v>214</v>
       </c>
-      <c r="E260" s="1" t="s">
+      <c r="E263" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="262" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D262" t="s">
+    <row r="265" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D265" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="264" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C264" t="s">
+    <row r="267" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C267" t="s">
         <v>241</v>
       </c>
-      <c r="D264" t="s">
+      <c r="D267" t="s">
         <v>242</v>
       </c>
-      <c r="E264" s="1" t="s">
+      <c r="E267" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="265" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C265" t="s">
+    <row r="268" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C268" t="s">
         <v>268</v>
       </c>
-      <c r="D265" t="s">
+      <c r="D268" t="s">
         <v>269</v>
       </c>
-      <c r="E265" s="1" t="s">
+      <c r="E268" s="1" t="s">
         <v>270</v>
-      </c>
-    </row>
-    <row r="266" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C266" t="s">
-        <v>283</v>
-      </c>
-      <c r="E266" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="267" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E267" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="268" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E268" s="1" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="269" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C269" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="270" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C270" t="s">
-        <v>298</v>
-      </c>
       <c r="E270" s="1" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
     </row>
     <row r="271" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E271" s="1"/>
+      <c r="E271" s="1" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="272" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C272" t="s">
+        <v>287</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="273" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C273" t="s">
+        <v>298</v>
+      </c>
+      <c r="E273" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="274" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E274" s="1"/>
+    </row>
+    <row r="275" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C275" t="s">
         <v>358</v>
       </c>
-      <c r="D272" t="s">
+      <c r="D275" t="s">
         <v>359</v>
       </c>
-      <c r="E272" s="1" t="s">
+      <c r="E275" s="1" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="273" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E273" s="1"/>
-    </row>
-    <row r="274" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E274" s="1"/>
-    </row>
-    <row r="275" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E275" s="1"/>
-    </row>
-    <row r="276" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="276" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E276" s="1"/>
     </row>
-    <row r="277" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="277" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E277" s="1"/>
     </row>
-    <row r="278" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="278" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E278" s="1"/>
     </row>
-    <row r="279" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="279" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E279" s="1"/>
     </row>
-    <row r="280" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="280" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E280" s="1"/>
     </row>
-    <row r="281" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C281" t="s">
+    <row r="281" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E281" s="1"/>
+    </row>
+    <row r="282" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E282" s="1"/>
+    </row>
+    <row r="283" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E283" s="1"/>
+    </row>
+    <row r="284" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C284" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="282" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D282" t="s">
+    <row r="285" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D285" t="s">
         <v>134</v>
       </c>
-      <c r="E282" t="s">
+      <c r="E285" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="283" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D283" t="s">
+    <row r="286" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D286" t="s">
         <v>135</v>
       </c>
-      <c r="E283" t="s">
+      <c r="E286" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="284" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D284" t="s">
+    <row r="287" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D287" t="s">
         <v>139</v>
       </c>
-      <c r="E284" t="s">
+      <c r="E287" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="285" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D285" t="s">
+    <row r="288" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D288" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="286" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D286" t="s">
+    <row r="289" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D289" t="s">
         <v>141</v>
       </c>
-      <c r="E286" t="s">
+      <c r="E289" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="287" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D287" t="s">
+    <row r="290" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D290" t="s">
         <v>482</v>
       </c>
-      <c r="E287" t="s">
+      <c r="E290" t="s">
         <v>484</v>
       </c>
-      <c r="F287" t="s">
+      <c r="F290" t="s">
         <v>488</v>
       </c>
-      <c r="G287" t="s">
+      <c r="G290" t="s">
         <v>483</v>
       </c>
-      <c r="H287" s="1" t="s">
+      <c r="H290" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="288" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D288" t="s">
+    <row r="291" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D291" t="s">
         <v>485</v>
       </c>
-      <c r="E288" t="s">
+      <c r="E291" t="s">
         <v>486</v>
       </c>
-      <c r="G288" t="s">
+      <c r="G291" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="290" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C290" t="s">
+    <row r="293" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C293" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="291" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D291" t="s">
+    <row r="294" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D294" t="s">
         <v>72</v>
       </c>
-      <c r="E291" t="s">
+      <c r="E294" t="s">
         <v>73</v>
       </c>
-      <c r="F291" s="1" t="s">
+      <c r="F294" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="292" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D292" t="s">
+    <row r="295" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D295" t="s">
         <v>75</v>
       </c>
-      <c r="E292" s="1" t="s">
+      <c r="E295" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="293" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D293" t="s">
+    <row r="296" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D296" t="s">
         <v>77</v>
       </c>
-      <c r="E293" s="1" t="s">
+      <c r="E296" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="294" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D294" t="s">
+    <row r="297" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D297" t="s">
         <v>80</v>
       </c>
-      <c r="E294" s="1" t="s">
+      <c r="E297" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="295" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D295" t="s">
+    <row r="298" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D298" t="s">
         <v>361</v>
       </c>
-      <c r="E295" t="s">
+      <c r="E298" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="296" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D296" t="s">
+    <row r="299" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D299" t="s">
         <v>362</v>
       </c>
-      <c r="E296" t="s">
+      <c r="E299" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="298" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D298" t="s">
+    <row r="301" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D301" t="s">
         <v>81</v>
       </c>
-      <c r="E298" t="s">
+      <c r="E301" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="299" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D299" t="s">
+    <row r="302" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D302" t="s">
         <v>83</v>
       </c>
-      <c r="E299" t="s">
+      <c r="E302" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="301" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C301" t="s">
+    <row r="304" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C304" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="302" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D302" t="s">
+    <row r="305" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D305" t="s">
         <v>72</v>
       </c>
-      <c r="E302" t="s">
+      <c r="E305" t="s">
         <v>130</v>
       </c>
-      <c r="F302" s="1"/>
-    </row>
-    <row r="303" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D303" t="s">
-        <v>146</v>
-      </c>
-      <c r="E303" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F303" s="1"/>
-    </row>
-    <row r="304" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D304" t="s">
-        <v>75</v>
-      </c>
-      <c r="E304" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="305" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E305" s="1"/>
+      <c r="F305" s="1"/>
     </row>
     <row r="306" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D306" t="s">
-        <v>143</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="E306" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F306" s="1"/>
     </row>
     <row r="307" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E307" t="s">
-        <v>150</v>
-      </c>
-      <c r="F307" t="s">
-        <v>149</v>
+      <c r="D307" t="s">
+        <v>75</v>
+      </c>
+      <c r="E307" s="1" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="308" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E308" t="s">
-        <v>151</v>
-      </c>
-      <c r="F308" t="s">
-        <v>144</v>
-      </c>
-      <c r="G308" s="1" t="s">
-        <v>145</v>
-      </c>
+      <c r="E308" s="1"/>
     </row>
     <row r="309" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D309" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="310" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E310" t="s">
+        <v>150</v>
+      </c>
+      <c r="F310" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="311" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E311" t="s">
+        <v>151</v>
+      </c>
+      <c r="F311" t="s">
+        <v>144</v>
+      </c>
+      <c r="G311" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="312" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D312" t="s">
         <v>152</v>
       </c>
-      <c r="E309" s="1" t="s">
+      <c r="E312" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G309" s="1"/>
-    </row>
-    <row r="323" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E323" s="1"/>
-    </row>
-    <row r="325" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B325" t="s">
+      <c r="G312" s="1"/>
+    </row>
+    <row r="326" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E326" s="1"/>
+    </row>
+    <row r="328" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B328" t="s">
         <v>275</v>
-      </c>
-    </row>
-    <row r="326" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C326" t="s">
-        <v>276</v>
-      </c>
-      <c r="D326" t="s">
-        <v>278</v>
-      </c>
-      <c r="E326" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="327" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C327" t="s">
-        <v>280</v>
-      </c>
-      <c r="E327" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F327" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="G327" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="328" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C328" t="s">
-        <v>289</v>
-      </c>
-      <c r="E328" s="1" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="329" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C329" t="s">
-        <v>303</v>
+        <v>276</v>
+      </c>
+      <c r="D329" t="s">
+        <v>278</v>
       </c>
       <c r="E329" s="1" t="s">
-        <v>304</v>
+        <v>277</v>
       </c>
     </row>
     <row r="330" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D330" t="s">
-        <v>305</v>
+      <c r="C330" t="s">
+        <v>280</v>
       </c>
       <c r="E330" s="1" t="s">
-        <v>306</v>
+        <v>279</v>
+      </c>
+      <c r="F330" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="G330" s="1" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="331" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C331" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="E331" s="1" t="s">
-        <v>322</v>
+        <v>290</v>
       </c>
     </row>
     <row r="332" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C332" t="s">
-        <v>307</v>
-      </c>
-      <c r="D332" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="E332" s="1" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="333" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C333" t="s">
-        <v>310</v>
+      <c r="D333" t="s">
+        <v>305</v>
       </c>
       <c r="E333" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="334" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C334" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="E334" s="1" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
     </row>
     <row r="335" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C335" t="s">
-        <v>316</v>
+        <v>307</v>
+      </c>
+      <c r="D335" t="s">
+        <v>308</v>
       </c>
       <c r="E335" s="1" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="336" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C336" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="E336" s="1" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="337" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C337" t="s">
-        <v>325</v>
-      </c>
-      <c r="D337" t="s">
-        <v>332</v>
+        <v>315</v>
       </c>
       <c r="E337" s="1" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
     </row>
     <row r="338" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D338" t="s">
-        <v>327</v>
+      <c r="C338" t="s">
+        <v>316</v>
       </c>
       <c r="E338" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="339" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C339" t="s">
+        <v>318</v>
+      </c>
+      <c r="E339" s="1" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="340" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C340" t="s">
+        <v>325</v>
+      </c>
+      <c r="D340" t="s">
+        <v>332</v>
+      </c>
+      <c r="E340" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="341" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D341" t="s">
+        <v>327</v>
+      </c>
+      <c r="E341" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="343" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C343" t="s">
         <v>329</v>
       </c>
-      <c r="D340" t="s">
+      <c r="D343" t="s">
         <v>330</v>
       </c>
-      <c r="E340" s="1" t="s">
+      <c r="E343" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="342" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C342" t="s">
+    <row r="345" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C345" t="s">
         <v>335</v>
       </c>
-      <c r="D342" t="s">
+      <c r="D345" t="s">
         <v>337</v>
       </c>
-      <c r="E342" s="1" t="s">
+      <c r="E345" s="1" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="346" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B346" t="s">
+    <row r="349" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B349" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="347" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C347" t="s">
+    <row r="350" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C350" t="s">
         <v>341</v>
       </c>
-      <c r="D347" t="s">
+      <c r="D350" t="s">
         <v>339</v>
       </c>
-      <c r="E347" s="1" t="s">
+      <c r="E350" s="1" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="353" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B353" t="s">
+    <row r="356" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B356" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="354" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C354" t="s">
-        <v>86</v>
-      </c>
-      <c r="D354" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="355" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C355" t="s">
-        <v>88</v>
-      </c>
-      <c r="D355" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="356" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C356" t="s">
-        <v>95</v>
-      </c>
-      <c r="D356" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="357" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C357" t="s">
-        <v>97</v>
-      </c>
-      <c r="D357" s="1" t="s">
-        <v>98</v>
+        <v>86</v>
+      </c>
+      <c r="D357" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="358" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C358" t="s">
+        <v>88</v>
+      </c>
+      <c r="D358" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="359" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B359" t="s">
-        <v>90</v>
-      </c>
       <c r="C359" t="s">
-        <v>91</v>
-      </c>
-      <c r="D359" t="s">
-        <v>92</v>
+        <v>95</v>
+      </c>
+      <c r="D359" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="360" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C360" t="s">
+        <v>97</v>
+      </c>
+      <c r="D360" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="362" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B362" t="s">
+        <v>90</v>
+      </c>
+      <c r="C362" t="s">
+        <v>91</v>
+      </c>
+      <c r="D362" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="363" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C363" t="s">
         <v>93</v>
       </c>
-      <c r="D360" t="s">
+      <c r="D363" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="363" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B363" t="s">
+    <row r="366" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B366" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="364" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C364" t="s">
+    <row r="367" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C367" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="365" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D365" t="s">
-        <v>104</v>
-      </c>
-      <c r="E365" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="366" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D366" t="s">
-        <v>101</v>
-      </c>
-      <c r="E366" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="367" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D367" t="s">
-        <v>102</v>
-      </c>
-      <c r="E367" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="368" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D368" t="s">
+        <v>104</v>
+      </c>
+      <c r="E368" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="369" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D369" t="s">
+        <v>101</v>
+      </c>
+      <c r="E369" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="370" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D370" t="s">
+        <v>102</v>
+      </c>
+      <c r="E370" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="371" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D371" t="s">
         <v>107</v>
       </c>
-      <c r="E368" t="s">
+      <c r="E371" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="370" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B370" t="s">
+    <row r="373" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B373" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="371" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C371" t="s">
+    <row r="374" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C374" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="372" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D372" t="s">
+    <row r="375" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D375" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="373" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D373" t="s">
+    <row r="376" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D376" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="374" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F374" s="1" t="s">
+    <row r="377" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F377" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="375" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B375" t="s">
+    <row r="378" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B378" t="s">
         <v>1</v>
       </c>
-      <c r="F375" s="1" t="s">
+      <c r="F378" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="376" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C376" t="s">
+    <row r="379" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C379" t="s">
         <v>112</v>
       </c>
-      <c r="D376" s="1" t="s">
+      <c r="D379" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="377" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D377" t="s">
+    <row r="380" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D380" t="s">
         <v>126</v>
       </c>
-      <c r="E377" s="1" t="s">
+      <c r="E380" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="378" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C378" t="s">
+    <row r="381" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C381" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="379" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D379" t="s">
-        <v>115</v>
-      </c>
-      <c r="E379" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F379" t="s">
-        <v>128</v>
-      </c>
-      <c r="G379" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="380" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E380" t="s">
-        <v>121</v>
-      </c>
-      <c r="G380" s="1"/>
-    </row>
-    <row r="381" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E381" t="s">
-        <v>124</v>
-      </c>
-      <c r="G381" s="1"/>
     </row>
     <row r="382" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D382" t="s">
+        <v>115</v>
+      </c>
+      <c r="E382" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F382" t="s">
+        <v>128</v>
+      </c>
+      <c r="G382" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="383" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E383" t="s">
+        <v>121</v>
+      </c>
+      <c r="G383" s="1"/>
+    </row>
+    <row r="384" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E384" t="s">
+        <v>124</v>
+      </c>
+      <c r="G384" s="1"/>
+    </row>
+    <row r="385" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D385" t="s">
         <v>117</v>
       </c>
-      <c r="E382" s="1" t="s">
+      <c r="E385" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G382" s="1"/>
-    </row>
-    <row r="383" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D383" t="s">
+      <c r="G385" s="1"/>
+    </row>
+    <row r="386" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D386" t="s">
         <v>119</v>
       </c>
-      <c r="E383" s="1" t="s">
+      <c r="E386" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G383" s="1"/>
-    </row>
-    <row r="384" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E384" s="1" t="s">
+      <c r="G386" s="1"/>
+    </row>
+    <row r="387" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E387" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="G384" s="1"/>
-    </row>
-    <row r="385" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E385" t="s">
+      <c r="G387" s="1"/>
+    </row>
+    <row r="388" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E388" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="386" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D386" t="s">
+    <row r="389" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D389" t="s">
         <v>301</v>
       </c>
-      <c r="E386" s="1" t="s">
+      <c r="E389" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="387" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D387" t="s">
+    <row r="390" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D390" t="s">
         <v>300</v>
       </c>
-      <c r="E387" s="1" t="s">
+      <c r="E390" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="392" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C392" t="s">
+    <row r="395" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C395" t="s">
         <v>131</v>
       </c>
-      <c r="D392" s="1" t="s">
+      <c r="D395" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="396" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B396" t="s">
+    <row r="399" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B399" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="397" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C397" t="s">
+    <row r="400" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C400" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="398" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D398" t="s">
+    <row r="401" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D401" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="399" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E399" t="s">
+    <row r="402" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E402" t="s">
         <v>492</v>
       </c>
-      <c r="F399" s="1" t="s">
+      <c r="F402" s="1" t="s">
         <v>491</v>
-      </c>
-    </row>
-    <row r="400" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E400" t="s">
-        <v>494</v>
-      </c>
-      <c r="F400" s="1" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="401" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E401" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="402" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D402" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="403" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E403" t="s">
-        <v>497</v>
+        <v>494</v>
+      </c>
+      <c r="F403" s="1" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="404" spans="3:7" x14ac:dyDescent="0.2">
@@ -5347,331 +5348,337 @@
     </row>
     <row r="405" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D405" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="406" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E406" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="407" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C407" t="s">
-        <v>500</v>
+      <c r="E407" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="408" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D408" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="409" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E409" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="410" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C410" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="411" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D411" t="s">
         <v>503</v>
       </c>
-      <c r="E408" t="s">
+      <c r="E411" t="s">
         <v>504</v>
-      </c>
-    </row>
-    <row r="409" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D409" t="s">
-        <v>501</v>
-      </c>
-      <c r="E409" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="411" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C411" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="412" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D412" t="s">
+        <v>501</v>
+      </c>
+      <c r="E412" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="414" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C414" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="415" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D415" t="s">
         <v>508</v>
       </c>
-      <c r="E412" t="s">
+      <c r="E415" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="413" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D413" t="s">
+    <row r="416" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D416" t="s">
         <v>509</v>
       </c>
-      <c r="E413" t="s">
+      <c r="E416" t="s">
         <v>507</v>
       </c>
-      <c r="G413" s="1" t="s">
+      <c r="G416" s="1" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="415" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C415" t="s">
+    <row r="418" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C418" t="s">
         <v>512</v>
       </c>
-      <c r="G415" s="1" t="s">
+      <c r="G418" s="1" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="417" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C417" t="s">
+    <row r="420" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C420" t="s">
         <v>513</v>
       </c>
-      <c r="E417" t="s">
+      <c r="E420" t="s">
         <v>514</v>
       </c>
-      <c r="G417" s="1" t="s">
+      <c r="G420" s="1" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="419" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C419" t="s">
+    <row r="422" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C422" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="420" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D420" t="s">
+    <row r="423" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D423" t="s">
         <v>518</v>
       </c>
-      <c r="E420" t="s">
+      <c r="E423" t="s">
         <v>517</v>
       </c>
-      <c r="G420" s="1" t="s">
+      <c r="G423" s="1" t="s">
         <v>521</v>
-      </c>
-    </row>
-    <row r="421" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D421" t="s">
-        <v>519</v>
-      </c>
-      <c r="E421" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="423" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C423" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="424" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D424" t="s">
+        <v>519</v>
+      </c>
+      <c r="E424" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="426" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C426" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="427" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D427" t="s">
         <v>528</v>
       </c>
-      <c r="E424" t="s">
+      <c r="E427" t="s">
         <v>524</v>
       </c>
-      <c r="G424" s="1" t="s">
+      <c r="G427" s="1" t="s">
         <v>529</v>
-      </c>
-    </row>
-    <row r="425" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D425" t="s">
-        <v>526</v>
-      </c>
-      <c r="E425" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="426" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D426" t="s">
-        <v>527</v>
-      </c>
-      <c r="E426" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="427" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C427" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="428" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D428" t="s">
-        <v>631</v>
+        <v>526</v>
       </c>
       <c r="E428" t="s">
-        <v>632</v>
+        <v>523</v>
       </c>
     </row>
     <row r="429" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D429" t="s">
-        <v>633</v>
+        <v>527</v>
       </c>
       <c r="E429" t="s">
-        <v>634</v>
+        <v>525</v>
       </c>
     </row>
     <row r="430" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D430" t="s">
-        <v>635</v>
-      </c>
-      <c r="E430" t="s">
-        <v>636</v>
+      <c r="C430" t="s">
+        <v>630</v>
       </c>
     </row>
     <row r="431" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D431" t="s">
-        <v>638</v>
+        <v>631</v>
       </c>
       <c r="E431" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
     </row>
     <row r="432" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D432" t="s">
+        <v>633</v>
+      </c>
+      <c r="E432" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="433" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D433" t="s">
+        <v>635</v>
+      </c>
+      <c r="E433" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="434" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D434" t="s">
+        <v>638</v>
+      </c>
+      <c r="E434" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="435" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D435" t="s">
         <v>694</v>
       </c>
-      <c r="E432" t="s">
+      <c r="E435" t="s">
         <v>696</v>
       </c>
-      <c r="G432" s="1" t="s">
+      <c r="G435" s="1" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="435" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B435" t="s">
+    <row r="438" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B438" t="s">
         <v>779</v>
       </c>
     </row>
-    <row r="436" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C436" t="s">
+    <row r="439" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C439" t="s">
         <v>780</v>
       </c>
-      <c r="G436" s="1" t="s">
+      <c r="G439" s="1" t="s">
         <v>781</v>
       </c>
     </row>
-    <row r="445" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B445" t="s">
+    <row r="448" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B448" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="446" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C446" t="s">
+    <row r="449" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C449" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="447" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D447" t="s">
+    <row r="450" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D450" t="s">
         <v>541</v>
       </c>
-      <c r="G447" s="1" t="s">
+      <c r="G450" s="1" t="s">
         <v>546</v>
-      </c>
-    </row>
-    <row r="448" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C448" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="449" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D449" t="s">
-        <v>543</v>
-      </c>
-      <c r="E449" t="s">
-        <v>544</v>
-      </c>
-      <c r="G449" s="1" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="451" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C451" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
     </row>
     <row r="452" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D452" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="E452" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="G452" s="1" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="453" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D453" t="s">
-        <v>550</v>
-      </c>
-      <c r="E453" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
     </row>
     <row r="454" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D454" t="s">
-        <v>552</v>
-      </c>
-      <c r="E454" t="s">
-        <v>553</v>
+      <c r="C454" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="455" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D455" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="E455" t="s">
-        <v>555</v>
+        <v>549</v>
+      </c>
+      <c r="G455" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="456" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D456" t="s">
+        <v>550</v>
+      </c>
+      <c r="E456" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="457" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C457" t="s">
-        <v>557</v>
+      <c r="D457" t="s">
+        <v>552</v>
+      </c>
+      <c r="E457" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="458" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D458" t="s">
+        <v>554</v>
+      </c>
+      <c r="E458" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="460" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C460" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="461" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D461" t="s">
         <v>558</v>
       </c>
-      <c r="E458" t="s">
+      <c r="E461" t="s">
         <v>560</v>
       </c>
-      <c r="G458" s="1" t="s">
+      <c r="G461" s="1" t="s">
         <v>562</v>
-      </c>
-    </row>
-    <row r="459" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D459" t="s">
-        <v>559</v>
-      </c>
-      <c r="E459" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="461" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C461" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="462" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D462" t="s">
+        <v>559</v>
+      </c>
+      <c r="E462" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="464" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C464" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="465" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D465" t="s">
         <v>565</v>
       </c>
-      <c r="G462" s="1" t="s">
+      <c r="G465" s="1" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="463" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C463" t="s">
+    <row r="466" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C466" t="s">
         <v>609</v>
       </c>
-      <c r="G463" s="1"/>
-    </row>
-    <row r="464" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D464" t="s">
+      <c r="G466" s="1"/>
+    </row>
+    <row r="467" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D467" t="s">
         <v>610</v>
       </c>
-      <c r="E464" t="s">
+      <c r="E467" t="s">
         <v>611</v>
       </c>
-      <c r="G464" s="1" t="s">
+      <c r="G467" s="1" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="465" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G465" s="1"/>
-    </row>
-    <row r="466" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G466" s="1"/>
-    </row>
-    <row r="467" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G467" s="1"/>
     </row>
     <row r="468" spans="2:7" x14ac:dyDescent="0.2">
       <c r="G468" s="1"/>
@@ -5682,273 +5689,282 @@
     <row r="470" spans="2:7" x14ac:dyDescent="0.2">
       <c r="G470" s="1"/>
     </row>
+    <row r="471" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G471" s="1"/>
+    </row>
+    <row r="472" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G472" s="1"/>
+    </row>
     <row r="473" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B473" t="s">
+      <c r="G473" s="1"/>
+    </row>
+    <row r="476" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B476" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="474" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C474" t="s">
+    <row r="477" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C477" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="475" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E475" t="s">
+    <row r="478" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E478" t="s">
         <v>568</v>
       </c>
-      <c r="G475" s="1" t="s">
+      <c r="G478" s="1" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="478" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B478" t="s">
+    <row r="481" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B481" t="s">
         <v>570</v>
-      </c>
-    </row>
-    <row r="479" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C479" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="480" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D480" t="s">
-        <v>572</v>
-      </c>
-      <c r="E480" t="s">
-        <v>573</v>
-      </c>
-      <c r="F480" t="s">
-        <v>574</v>
-      </c>
-      <c r="G480" s="1" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="481" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E481" t="s">
-        <v>576</v>
-      </c>
-      <c r="F481" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="482" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C482" t="s">
-        <v>594</v>
+        <v>571</v>
       </c>
     </row>
     <row r="483" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D483" t="s">
-        <v>595</v>
+        <v>572</v>
       </c>
       <c r="E483" t="s">
-        <v>596</v>
+        <v>573</v>
+      </c>
+      <c r="F483" t="s">
+        <v>574</v>
+      </c>
+      <c r="G483" s="1" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="484" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D484" t="s">
-        <v>598</v>
-      </c>
       <c r="E484" t="s">
-        <v>597</v>
+        <v>576</v>
+      </c>
+      <c r="F484" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="485" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C485" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="486" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D486" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="E486" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
     </row>
     <row r="487" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D487" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="E487" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
     </row>
     <row r="489" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D489" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="E489" t="s">
-        <v>604</v>
-      </c>
-      <c r="G489" s="1" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
     </row>
     <row r="490" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D490" t="s">
+        <v>601</v>
+      </c>
+      <c r="E490" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="492" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D492" t="s">
+        <v>603</v>
+      </c>
+      <c r="E492" t="s">
+        <v>604</v>
+      </c>
+      <c r="G492" s="1" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="493" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D493" t="s">
         <v>605</v>
       </c>
-      <c r="E490" t="s">
+      <c r="E493" t="s">
         <v>606</v>
       </c>
-      <c r="F490" t="s">
+      <c r="F493" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="494" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B494" t="s">
+    <row r="497" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B497" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="495" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C495" t="s">
+    <row r="498" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C498" t="s">
         <v>579</v>
-      </c>
-    </row>
-    <row r="496" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D496" t="s">
-        <v>581</v>
-      </c>
-      <c r="E496" t="s">
-        <v>582</v>
-      </c>
-      <c r="F496" t="s">
-        <v>580</v>
-      </c>
-      <c r="G496" s="1" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="497" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E497" t="s">
-        <v>583</v>
-      </c>
-      <c r="F497" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="499" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D499" t="s">
+        <v>581</v>
+      </c>
+      <c r="E499" t="s">
+        <v>582</v>
+      </c>
+      <c r="F499" t="s">
+        <v>580</v>
+      </c>
+      <c r="G499" s="1" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="500" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E500" t="s">
+        <v>583</v>
+      </c>
+      <c r="F500" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="502" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D502" t="s">
         <v>586</v>
       </c>
-      <c r="E499" t="s">
+      <c r="E502" t="s">
         <v>588</v>
       </c>
-      <c r="F499" t="s">
+      <c r="F502" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="502" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B502" t="s">
+    <row r="505" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B505" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="503" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C503" t="s">
+    <row r="506" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C506" t="s">
         <v>708</v>
       </c>
-      <c r="D503" t="s">
+      <c r="D506" t="s">
         <v>711</v>
       </c>
-      <c r="G503" s="1" t="s">
+      <c r="G506" s="1" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="504" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C504" t="s">
+    <row r="507" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C507" t="s">
         <v>709</v>
       </c>
-      <c r="D504" t="s">
+      <c r="D507" t="s">
         <v>712</v>
       </c>
     </row>
-    <row r="505" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C505" t="s">
+    <row r="508" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C508" t="s">
         <v>710</v>
       </c>
-      <c r="D505" t="s">
+      <c r="D508" t="s">
         <v>713</v>
       </c>
     </row>
-    <row r="508" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B508" t="s">
+    <row r="511" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B511" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="509" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C509" t="s">
+    <row r="512" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C512" t="s">
         <v>732</v>
       </c>
-      <c r="G509" s="1" t="s">
+      <c r="G512" s="1" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="510" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C510" t="s">
+    <row r="513" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C513" t="s">
         <v>734</v>
       </c>
-      <c r="G510" s="1" t="s">
+      <c r="G513" s="1" t="s">
         <v>735</v>
-      </c>
-    </row>
-    <row r="511" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C511" t="s">
-        <v>738</v>
-      </c>
-      <c r="F511" t="s">
-        <v>736</v>
-      </c>
-      <c r="G511" s="1" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="513" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B513" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="514" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C514" t="s">
+        <v>738</v>
+      </c>
+      <c r="F514" t="s">
+        <v>736</v>
+      </c>
+      <c r="G514" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="516" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B516" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="517" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C517" t="s">
         <v>744</v>
       </c>
-      <c r="D514" t="s">
+      <c r="D517" t="s">
         <v>745</v>
       </c>
-      <c r="G514" s="1" t="s">
+      <c r="G517" s="1" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="515" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C515" t="s">
+    <row r="518" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C518" t="s">
         <v>747</v>
       </c>
-      <c r="D515" t="s">
+      <c r="D518" t="s">
         <v>748</v>
       </c>
-      <c r="G515" s="1" t="s">
+      <c r="G518" s="1" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="519" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B519" t="s">
+    <row r="522" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B522" t="s">
         <v>802</v>
       </c>
     </row>
-    <row r="520" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C520" t="s">
+    <row r="523" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C523" t="s">
         <v>803</v>
       </c>
-      <c r="D520" t="s">
+      <c r="D523" t="s">
         <v>804</v>
       </c>
-      <c r="E520" t="s">
+      <c r="E523" t="s">
         <v>805</v>
       </c>
-      <c r="G520" s="1" t="s">
+      <c r="G523" s="1" t="s">
         <v>806</v>
       </c>
     </row>
-    <row r="521" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C521" t="s">
+    <row r="524" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C524" t="s">
         <v>807</v>
       </c>
-      <c r="E521" t="s">
+      <c r="E524" t="s">
         <v>808</v>
       </c>
     </row>
@@ -5956,164 +5972,164 @@
   <hyperlinks>
     <hyperlink ref="C15" r:id="rId1" xr:uid="{18CCA2F1-1074-664C-AB52-48BBB42F9065}"/>
     <hyperlink ref="D18" r:id="rId2" xr:uid="{02227101-F5A2-3446-ADC1-32F3342C625C}"/>
-    <hyperlink ref="D52" r:id="rId3" xr:uid="{6360CC1D-0E6F-6B45-B16E-E9F323959E32}"/>
-    <hyperlink ref="E64" r:id="rId4" xr:uid="{96980E2B-5D77-D04D-8463-2374C6B90C21}"/>
-    <hyperlink ref="E74" r:id="rId5" xr:uid="{5081034D-5E40-F340-99D2-B8E4DFC0468C}"/>
-    <hyperlink ref="E77" r:id="rId6" location=":~:text=You%20can%20verify%20whether%20it,password%20and%20ESSID%20are%20correct." xr:uid="{3BA51E9E-8709-874E-B6EC-40074894ACA9}"/>
-    <hyperlink ref="E72" r:id="rId7" xr:uid="{30BD9D61-AAB4-2544-987A-0386CA068398}"/>
-    <hyperlink ref="E80" r:id="rId8" xr:uid="{1824F9BF-1BD9-3842-A565-00C06FF5E50F}"/>
-    <hyperlink ref="D151" r:id="rId9" xr:uid="{E488AECD-B504-A04E-8F27-807A3A08802C}"/>
-    <hyperlink ref="D105" r:id="rId10" location="89804" xr:uid="{E34C14F5-E723-0A48-894F-222B3F74BBF9}"/>
-    <hyperlink ref="D106" r:id="rId11" xr:uid="{6C20672B-9F8F-094F-9AC8-3D1FC1C85319}"/>
-    <hyperlink ref="D107" r:id="rId12" xr:uid="{BA9A8F05-4D7F-4942-886C-F8152208F0EA}"/>
-    <hyperlink ref="F111" r:id="rId13" xr:uid="{22AE585F-7255-3F41-8A2E-808446F3A9AA}"/>
-    <hyperlink ref="F113" r:id="rId14" xr:uid="{93472772-CF6C-D045-B634-2D574A3EE034}"/>
-    <hyperlink ref="E209" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
-    <hyperlink ref="F210" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
-    <hyperlink ref="D241" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
-    <hyperlink ref="D242" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
-    <hyperlink ref="F114" r:id="rId19" xr:uid="{92BE3560-5393-C545-9D2D-2B773359B28F}"/>
-    <hyperlink ref="E258" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
-    <hyperlink ref="E259" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
-    <hyperlink ref="E260" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
-    <hyperlink ref="E88" r:id="rId23" xr:uid="{1526D7DA-27DA-1443-928C-BEDA9E425734}"/>
-    <hyperlink ref="E89" r:id="rId24" xr:uid="{4F363062-BE49-AB4F-8956-2C1F31D9B898}"/>
-    <hyperlink ref="H115" r:id="rId25" xr:uid="{D9E13355-D59B-054F-B544-34A5A285A9E0}"/>
-    <hyperlink ref="G83" r:id="rId26" xr:uid="{170917BF-0643-9848-BCA9-A3BF5219EE3E}"/>
-    <hyperlink ref="F118" r:id="rId27" xr:uid="{5D45F2D3-11BC-6E43-BEFF-29E4E04A041E}"/>
-    <hyperlink ref="I119" r:id="rId28" xr:uid="{7D985D09-6A9A-FF4D-9F4A-4C56CC604DCE}"/>
-    <hyperlink ref="D108" r:id="rId29" xr:uid="{784C3F11-339F-8242-911D-6E4E893DD319}"/>
-    <hyperlink ref="E108" r:id="rId30" xr:uid="{FC907203-09BF-654B-9028-A8528783DAFE}"/>
-    <hyperlink ref="F120" r:id="rId31" xr:uid="{EFD3653A-B2F2-614F-8DEE-A2CB34111C94}"/>
-    <hyperlink ref="F121" r:id="rId32" xr:uid="{774B592D-11A5-9C49-BB9A-61014C8D8C81}"/>
-    <hyperlink ref="F122" r:id="rId33" xr:uid="{BD793670-4C63-C04D-B52D-974AF8E59FA4}"/>
-    <hyperlink ref="F123" r:id="rId34" location="96077" xr:uid="{B9804BBD-5312-714B-97EA-CC7D2C647F2C}"/>
-    <hyperlink ref="H116" r:id="rId35" xr:uid="{7BC5BAB5-D297-0043-BAAF-45AD255D5C84}"/>
-    <hyperlink ref="I115" r:id="rId36" xr:uid="{A03C56E4-1156-A148-A568-F50A5C33DB5C}"/>
-    <hyperlink ref="F124" r:id="rId37" xr:uid="{12AC219C-4678-4E43-B328-6595FA10B8D3}"/>
-    <hyperlink ref="E126" r:id="rId38" xr:uid="{44409621-28A2-704A-B283-3DCE1EFB1603}"/>
-    <hyperlink ref="E264" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
-    <hyperlink ref="F127" r:id="rId40" xr:uid="{A9D0D792-87D1-8144-872F-5CA060D3C28F}"/>
-    <hyperlink ref="F128" r:id="rId41" xr:uid="{87EF989D-17E9-1E45-A075-CD862D0B60F4}"/>
-    <hyperlink ref="F130" r:id="rId42" xr:uid="{8406C6F0-DC69-A64D-AAD8-60A33C12D00B}"/>
-    <hyperlink ref="F131" r:id="rId43" location="108593" xr:uid="{3C38F59E-6E71-4048-9BCA-CBC77D3907E0}"/>
-    <hyperlink ref="F133" r:id="rId44" xr:uid="{EEBE2A3E-36CA-F94F-9B1D-EE463DB6425F}"/>
-    <hyperlink ref="F134" r:id="rId45" xr:uid="{3782B43D-9E6F-2940-A013-34AA5D6B4DB3}"/>
-    <hyperlink ref="F135" r:id="rId46" xr:uid="{3D1C62DB-D9B7-BE42-B21D-4EEBC4C9EFE1}"/>
-    <hyperlink ref="F136" r:id="rId47" xr:uid="{F5021A21-70A2-D34E-B055-64CAC326E7EF}"/>
-    <hyperlink ref="F137" r:id="rId48" xr:uid="{A8C010A1-8EE1-264B-8688-3BEA1B62E535}"/>
-    <hyperlink ref="E265" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
-    <hyperlink ref="F132" r:id="rId50" location="113521" xr:uid="{EE1413C5-3B38-7D4D-8DF1-634A12F0BD81}"/>
-    <hyperlink ref="E90" r:id="rId51" xr:uid="{00B1EF4A-7791-0343-8D8C-9A1E83248FC9}"/>
-    <hyperlink ref="E326" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
-    <hyperlink ref="E327" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
-    <hyperlink ref="F139" r:id="rId54" xr:uid="{40A4B6A0-2F7E-A84D-8CC6-D814A33F5953}"/>
-    <hyperlink ref="E266" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
-    <hyperlink ref="E267" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
-    <hyperlink ref="E268" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
-    <hyperlink ref="E269" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
-    <hyperlink ref="E328" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
-    <hyperlink ref="D243" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
-    <hyperlink ref="D244" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
-    <hyperlink ref="D245" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
-    <hyperlink ref="E270" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
-    <hyperlink ref="E329" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
-    <hyperlink ref="E330" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
-    <hyperlink ref="E332" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
-    <hyperlink ref="E333" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
-    <hyperlink ref="F327" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
-    <hyperlink ref="G327" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
-    <hyperlink ref="E334" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
-    <hyperlink ref="E335" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
-    <hyperlink ref="E336" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
-    <hyperlink ref="E211" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
-    <hyperlink ref="E331" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
-    <hyperlink ref="E337" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
-    <hyperlink ref="E338" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
-    <hyperlink ref="E92" r:id="rId77" location="code" xr:uid="{C0475FF8-517D-E949-887E-9A42D86E9640}"/>
-    <hyperlink ref="E340" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
-    <hyperlink ref="E93" r:id="rId79" xr:uid="{277DBE6F-F3E5-8B4C-8DD8-BD92445D1A99}"/>
-    <hyperlink ref="E342" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
-    <hyperlink ref="E347" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
-    <hyperlink ref="E249" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
-    <hyperlink ref="E250" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
-    <hyperlink ref="F160" r:id="rId84" xr:uid="{EB604865-A16B-0646-A5B5-0D047467449D}"/>
-    <hyperlink ref="E272" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
-    <hyperlink ref="D356" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
-    <hyperlink ref="D357" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
-    <hyperlink ref="E366" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
-    <hyperlink ref="E367" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
-    <hyperlink ref="E365" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
-    <hyperlink ref="D376" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
-    <hyperlink ref="E382" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
-    <hyperlink ref="E379" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
-    <hyperlink ref="E383" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
-    <hyperlink ref="F374" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
-    <hyperlink ref="F375" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
-    <hyperlink ref="E377" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
-    <hyperlink ref="G379" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
-    <hyperlink ref="D392" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
-    <hyperlink ref="E384" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
-    <hyperlink ref="E387" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
-    <hyperlink ref="E386" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
-    <hyperlink ref="F291" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
-    <hyperlink ref="E292" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
-    <hyperlink ref="E293" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
-    <hyperlink ref="E294" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
-    <hyperlink ref="G308" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
-    <hyperlink ref="E303" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
-    <hyperlink ref="E304" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
-    <hyperlink ref="E309" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
-    <hyperlink ref="F172" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
-    <hyperlink ref="F177" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
-    <hyperlink ref="F178" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
-    <hyperlink ref="F185" r:id="rId114" xr:uid="{2B03B1F0-535A-3E4F-8FB3-35D2DE847218}"/>
-    <hyperlink ref="G190" r:id="rId115" xr:uid="{11045522-E183-B14C-B43D-5EA36E454600}"/>
-    <hyperlink ref="E212" r:id="rId116" xr:uid="{F1098A8C-3BC0-DB4F-8F9C-48B31145FEC1}"/>
-    <hyperlink ref="F192" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
-    <hyperlink ref="F186" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
-    <hyperlink ref="F195" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
-    <hyperlink ref="H287" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
-    <hyperlink ref="F399" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
-    <hyperlink ref="G413" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
-    <hyperlink ref="F400" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
-    <hyperlink ref="G415" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
-    <hyperlink ref="G417" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
-    <hyperlink ref="G420" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
-    <hyperlink ref="G424" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
-    <hyperlink ref="G449" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
-    <hyperlink ref="G447" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
-    <hyperlink ref="G452" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
-    <hyperlink ref="G458" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
-    <hyperlink ref="G462" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
-    <hyperlink ref="G475" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
-    <hyperlink ref="G480" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
-    <hyperlink ref="G496" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
+    <hyperlink ref="D55" r:id="rId3" xr:uid="{6360CC1D-0E6F-6B45-B16E-E9F323959E32}"/>
+    <hyperlink ref="E67" r:id="rId4" xr:uid="{96980E2B-5D77-D04D-8463-2374C6B90C21}"/>
+    <hyperlink ref="E77" r:id="rId5" xr:uid="{5081034D-5E40-F340-99D2-B8E4DFC0468C}"/>
+    <hyperlink ref="E80" r:id="rId6" location=":~:text=You%20can%20verify%20whether%20it,password%20and%20ESSID%20are%20correct." xr:uid="{3BA51E9E-8709-874E-B6EC-40074894ACA9}"/>
+    <hyperlink ref="E75" r:id="rId7" xr:uid="{30BD9D61-AAB4-2544-987A-0386CA068398}"/>
+    <hyperlink ref="E83" r:id="rId8" xr:uid="{1824F9BF-1BD9-3842-A565-00C06FF5E50F}"/>
+    <hyperlink ref="D154" r:id="rId9" xr:uid="{E488AECD-B504-A04E-8F27-807A3A08802C}"/>
+    <hyperlink ref="D108" r:id="rId10" location="89804" xr:uid="{E34C14F5-E723-0A48-894F-222B3F74BBF9}"/>
+    <hyperlink ref="D109" r:id="rId11" xr:uid="{6C20672B-9F8F-094F-9AC8-3D1FC1C85319}"/>
+    <hyperlink ref="D110" r:id="rId12" xr:uid="{BA9A8F05-4D7F-4942-886C-F8152208F0EA}"/>
+    <hyperlink ref="F114" r:id="rId13" xr:uid="{22AE585F-7255-3F41-8A2E-808446F3A9AA}"/>
+    <hyperlink ref="F116" r:id="rId14" xr:uid="{93472772-CF6C-D045-B634-2D574A3EE034}"/>
+    <hyperlink ref="E212" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
+    <hyperlink ref="F213" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
+    <hyperlink ref="D244" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
+    <hyperlink ref="D245" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
+    <hyperlink ref="F117" r:id="rId19" xr:uid="{92BE3560-5393-C545-9D2D-2B773359B28F}"/>
+    <hyperlink ref="E261" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
+    <hyperlink ref="E262" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
+    <hyperlink ref="E263" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
+    <hyperlink ref="E91" r:id="rId23" xr:uid="{1526D7DA-27DA-1443-928C-BEDA9E425734}"/>
+    <hyperlink ref="E92" r:id="rId24" xr:uid="{4F363062-BE49-AB4F-8956-2C1F31D9B898}"/>
+    <hyperlink ref="H118" r:id="rId25" xr:uid="{D9E13355-D59B-054F-B544-34A5A285A9E0}"/>
+    <hyperlink ref="G86" r:id="rId26" xr:uid="{170917BF-0643-9848-BCA9-A3BF5219EE3E}"/>
+    <hyperlink ref="F121" r:id="rId27" xr:uid="{5D45F2D3-11BC-6E43-BEFF-29E4E04A041E}"/>
+    <hyperlink ref="I122" r:id="rId28" xr:uid="{7D985D09-6A9A-FF4D-9F4A-4C56CC604DCE}"/>
+    <hyperlink ref="D111" r:id="rId29" xr:uid="{784C3F11-339F-8242-911D-6E4E893DD319}"/>
+    <hyperlink ref="E111" r:id="rId30" xr:uid="{FC907203-09BF-654B-9028-A8528783DAFE}"/>
+    <hyperlink ref="F123" r:id="rId31" xr:uid="{EFD3653A-B2F2-614F-8DEE-A2CB34111C94}"/>
+    <hyperlink ref="F124" r:id="rId32" xr:uid="{774B592D-11A5-9C49-BB9A-61014C8D8C81}"/>
+    <hyperlink ref="F125" r:id="rId33" xr:uid="{BD793670-4C63-C04D-B52D-974AF8E59FA4}"/>
+    <hyperlink ref="F126" r:id="rId34" location="96077" xr:uid="{B9804BBD-5312-714B-97EA-CC7D2C647F2C}"/>
+    <hyperlink ref="H119" r:id="rId35" xr:uid="{7BC5BAB5-D297-0043-BAAF-45AD255D5C84}"/>
+    <hyperlink ref="I118" r:id="rId36" xr:uid="{A03C56E4-1156-A148-A568-F50A5C33DB5C}"/>
+    <hyperlink ref="F127" r:id="rId37" xr:uid="{12AC219C-4678-4E43-B328-6595FA10B8D3}"/>
+    <hyperlink ref="E129" r:id="rId38" xr:uid="{44409621-28A2-704A-B283-3DCE1EFB1603}"/>
+    <hyperlink ref="E267" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
+    <hyperlink ref="F130" r:id="rId40" xr:uid="{A9D0D792-87D1-8144-872F-5CA060D3C28F}"/>
+    <hyperlink ref="F131" r:id="rId41" xr:uid="{87EF989D-17E9-1E45-A075-CD862D0B60F4}"/>
+    <hyperlink ref="F133" r:id="rId42" xr:uid="{8406C6F0-DC69-A64D-AAD8-60A33C12D00B}"/>
+    <hyperlink ref="F134" r:id="rId43" location="108593" xr:uid="{3C38F59E-6E71-4048-9BCA-CBC77D3907E0}"/>
+    <hyperlink ref="F136" r:id="rId44" xr:uid="{EEBE2A3E-36CA-F94F-9B1D-EE463DB6425F}"/>
+    <hyperlink ref="F137" r:id="rId45" xr:uid="{3782B43D-9E6F-2940-A013-34AA5D6B4DB3}"/>
+    <hyperlink ref="F138" r:id="rId46" xr:uid="{3D1C62DB-D9B7-BE42-B21D-4EEBC4C9EFE1}"/>
+    <hyperlink ref="F139" r:id="rId47" xr:uid="{F5021A21-70A2-D34E-B055-64CAC326E7EF}"/>
+    <hyperlink ref="F140" r:id="rId48" xr:uid="{A8C010A1-8EE1-264B-8688-3BEA1B62E535}"/>
+    <hyperlink ref="E268" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
+    <hyperlink ref="F135" r:id="rId50" location="113521" xr:uid="{EE1413C5-3B38-7D4D-8DF1-634A12F0BD81}"/>
+    <hyperlink ref="E93" r:id="rId51" xr:uid="{00B1EF4A-7791-0343-8D8C-9A1E83248FC9}"/>
+    <hyperlink ref="E329" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
+    <hyperlink ref="E330" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
+    <hyperlink ref="F142" r:id="rId54" xr:uid="{40A4B6A0-2F7E-A84D-8CC6-D814A33F5953}"/>
+    <hyperlink ref="E269" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
+    <hyperlink ref="E270" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
+    <hyperlink ref="E271" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
+    <hyperlink ref="E272" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
+    <hyperlink ref="E331" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
+    <hyperlink ref="D246" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
+    <hyperlink ref="D247" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
+    <hyperlink ref="D248" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
+    <hyperlink ref="E273" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
+    <hyperlink ref="E332" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
+    <hyperlink ref="E333" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
+    <hyperlink ref="E335" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
+    <hyperlink ref="E336" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
+    <hyperlink ref="F330" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
+    <hyperlink ref="G330" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
+    <hyperlink ref="E337" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
+    <hyperlink ref="E338" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
+    <hyperlink ref="E339" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
+    <hyperlink ref="E214" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
+    <hyperlink ref="E334" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
+    <hyperlink ref="E340" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
+    <hyperlink ref="E341" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
+    <hyperlink ref="E95" r:id="rId77" location="code" xr:uid="{C0475FF8-517D-E949-887E-9A42D86E9640}"/>
+    <hyperlink ref="E343" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
+    <hyperlink ref="E96" r:id="rId79" xr:uid="{277DBE6F-F3E5-8B4C-8DD8-BD92445D1A99}"/>
+    <hyperlink ref="E345" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
+    <hyperlink ref="E350" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
+    <hyperlink ref="E252" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
+    <hyperlink ref="E253" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
+    <hyperlink ref="F163" r:id="rId84" xr:uid="{EB604865-A16B-0646-A5B5-0D047467449D}"/>
+    <hyperlink ref="E275" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
+    <hyperlink ref="D359" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
+    <hyperlink ref="D360" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
+    <hyperlink ref="E369" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
+    <hyperlink ref="E370" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
+    <hyperlink ref="E368" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
+    <hyperlink ref="D379" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
+    <hyperlink ref="E385" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
+    <hyperlink ref="E382" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
+    <hyperlink ref="E386" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
+    <hyperlink ref="F377" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
+    <hyperlink ref="F378" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
+    <hyperlink ref="E380" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
+    <hyperlink ref="G382" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
+    <hyperlink ref="D395" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
+    <hyperlink ref="E387" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
+    <hyperlink ref="E390" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
+    <hyperlink ref="E389" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
+    <hyperlink ref="F294" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
+    <hyperlink ref="E295" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
+    <hyperlink ref="E296" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
+    <hyperlink ref="E297" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
+    <hyperlink ref="G311" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
+    <hyperlink ref="E306" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
+    <hyperlink ref="E307" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
+    <hyperlink ref="E312" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
+    <hyperlink ref="F175" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
+    <hyperlink ref="F180" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
+    <hyperlink ref="F181" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
+    <hyperlink ref="F188" r:id="rId114" xr:uid="{2B03B1F0-535A-3E4F-8FB3-35D2DE847218}"/>
+    <hyperlink ref="G193" r:id="rId115" xr:uid="{11045522-E183-B14C-B43D-5EA36E454600}"/>
+    <hyperlink ref="E215" r:id="rId116" xr:uid="{F1098A8C-3BC0-DB4F-8F9C-48B31145FEC1}"/>
+    <hyperlink ref="F195" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
+    <hyperlink ref="F189" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
+    <hyperlink ref="F198" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
+    <hyperlink ref="H290" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
+    <hyperlink ref="F402" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
+    <hyperlink ref="G416" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
+    <hyperlink ref="F403" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
+    <hyperlink ref="G418" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
+    <hyperlink ref="G420" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
+    <hyperlink ref="G423" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
+    <hyperlink ref="G427" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
+    <hyperlink ref="G452" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
+    <hyperlink ref="G450" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
+    <hyperlink ref="G455" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
+    <hyperlink ref="G461" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
+    <hyperlink ref="G465" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
+    <hyperlink ref="G478" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
+    <hyperlink ref="G483" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
+    <hyperlink ref="G499" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
     <hyperlink ref="E35" r:id="rId136" xr:uid="{809CA2D1-39E9-0045-A4DF-E4C0C2E97FA2}"/>
     <hyperlink ref="E36" r:id="rId137" xr:uid="{5DC44543-F2B9-F841-9097-6DB19C5EBD82}"/>
-    <hyperlink ref="G489" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
-    <hyperlink ref="G464" r:id="rId139" xr:uid="{7F4EA1D7-8774-1A4B-BF25-18ED0416CB20}"/>
-    <hyperlink ref="F230" r:id="rId140" xr:uid="{101513F3-87A1-DA41-8BF5-E4029309ECB8}"/>
-    <hyperlink ref="F215" r:id="rId141" xr:uid="{494E255E-6912-8643-B5CD-1D65E0DDCFFC}"/>
-    <hyperlink ref="F216" r:id="rId142" xr:uid="{828F749D-83DE-C14E-B637-56047AC1B384}"/>
-    <hyperlink ref="F231" r:id="rId143" xr:uid="{435D9B3C-98B6-5E49-BD30-EAA53523CDB7}"/>
-    <hyperlink ref="F232" r:id="rId144" xr:uid="{7D905409-0097-E04E-9593-2DEEBEEA0D0F}"/>
-    <hyperlink ref="F164" r:id="rId145" xr:uid="{64451146-E88A-9A47-9888-71BEAC8B984E}"/>
-    <hyperlink ref="F220" r:id="rId146" xr:uid="{28F6BA28-EB9B-374C-A8A0-4077C800D23A}"/>
-    <hyperlink ref="G432" r:id="rId147" xr:uid="{20B4F69E-7592-784A-8C2E-123726A51D93}"/>
-    <hyperlink ref="F223" r:id="rId148" xr:uid="{E3C3D7C6-1E6E-FF40-8CC7-6CF1C77457E4}"/>
-    <hyperlink ref="G503" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
-    <hyperlink ref="G185" r:id="rId150" xr:uid="{9BECD448-C575-B64B-BA3F-BEE8D1CBBD43}"/>
-    <hyperlink ref="G509" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
-    <hyperlink ref="G510" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
-    <hyperlink ref="G511" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
-    <hyperlink ref="G514" r:id="rId154" xr:uid="{FB93E0B8-2537-FD47-8420-84D2A706F697}"/>
-    <hyperlink ref="G515" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
-    <hyperlink ref="F198" r:id="rId156" location="2116892" xr:uid="{FF1C16E6-B146-B548-B694-396AC9D0B975}"/>
-    <hyperlink ref="G183" r:id="rId157" xr:uid="{ED09A21C-0057-1146-8BFF-213A32FC88DF}"/>
-    <hyperlink ref="G436" r:id="rId158" xr:uid="{F933A5C4-6DD5-5547-8BB3-B5D3FBA7A852}"/>
-    <hyperlink ref="G520" r:id="rId159" location=".YLoDxOvTXX8" xr:uid="{8886E3AC-3A64-6449-A070-17D95B586F83}"/>
-    <hyperlink ref="F201" r:id="rId160" xr:uid="{5140C3EB-4DFC-5A4A-9C02-C2EBFA052A41}"/>
+    <hyperlink ref="G492" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
+    <hyperlink ref="G467" r:id="rId139" xr:uid="{7F4EA1D7-8774-1A4B-BF25-18ED0416CB20}"/>
+    <hyperlink ref="F233" r:id="rId140" xr:uid="{101513F3-87A1-DA41-8BF5-E4029309ECB8}"/>
+    <hyperlink ref="F218" r:id="rId141" xr:uid="{494E255E-6912-8643-B5CD-1D65E0DDCFFC}"/>
+    <hyperlink ref="F219" r:id="rId142" xr:uid="{828F749D-83DE-C14E-B637-56047AC1B384}"/>
+    <hyperlink ref="F234" r:id="rId143" xr:uid="{435D9B3C-98B6-5E49-BD30-EAA53523CDB7}"/>
+    <hyperlink ref="F235" r:id="rId144" xr:uid="{7D905409-0097-E04E-9593-2DEEBEEA0D0F}"/>
+    <hyperlink ref="F167" r:id="rId145" xr:uid="{64451146-E88A-9A47-9888-71BEAC8B984E}"/>
+    <hyperlink ref="F223" r:id="rId146" xr:uid="{28F6BA28-EB9B-374C-A8A0-4077C800D23A}"/>
+    <hyperlink ref="G435" r:id="rId147" xr:uid="{20B4F69E-7592-784A-8C2E-123726A51D93}"/>
+    <hyperlink ref="F226" r:id="rId148" xr:uid="{E3C3D7C6-1E6E-FF40-8CC7-6CF1C77457E4}"/>
+    <hyperlink ref="G506" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
+    <hyperlink ref="G188" r:id="rId150" xr:uid="{9BECD448-C575-B64B-BA3F-BEE8D1CBBD43}"/>
+    <hyperlink ref="G512" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
+    <hyperlink ref="G513" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
+    <hyperlink ref="G514" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
+    <hyperlink ref="G517" r:id="rId154" xr:uid="{FB93E0B8-2537-FD47-8420-84D2A706F697}"/>
+    <hyperlink ref="G518" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
+    <hyperlink ref="F201" r:id="rId156" location="2116892" xr:uid="{FF1C16E6-B146-B548-B694-396AC9D0B975}"/>
+    <hyperlink ref="G186" r:id="rId157" xr:uid="{ED09A21C-0057-1146-8BFF-213A32FC88DF}"/>
+    <hyperlink ref="G439" r:id="rId158" xr:uid="{F933A5C4-6DD5-5547-8BB3-B5D3FBA7A852}"/>
+    <hyperlink ref="G523" r:id="rId159" location=".YLoDxOvTXX8" xr:uid="{8886E3AC-3A64-6449-A070-17D95B586F83}"/>
+    <hyperlink ref="F204" r:id="rId160" xr:uid="{5140C3EB-4DFC-5A4A-9C02-C2EBFA052A41}"/>
     <hyperlink ref="F28" r:id="rId161" xr:uid="{99992829-3CC1-2B43-BA73-7F09EAA955A4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added tip for vim :x and :wq
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FE6F34-7F66-234E-A812-612E32FF2881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C6EDED-CEF2-3F46-8F5E-8C9B1065B651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="840">
   <si>
     <t>docker</t>
   </si>
@@ -2552,6 +2552,15 @@
   </si>
   <si>
     <t>remove a screen</t>
+  </si>
+  <si>
+    <t>Difference between :wq and :x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The save time, :x will not change the time if the content is not changed </t>
+  </si>
+  <si>
+    <t>https://til.hashrocket.com/posts/2fdb6afb66-difference-between-wq-and-x</t>
   </si>
 </sst>
 </file>
@@ -3017,8 +3026,8 @@
   <dimension ref="B1:I524"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
+      <pane ySplit="1" topLeftCell="A447" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E472" sqref="E472"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5684,10 +5693,18 @@
       <c r="G468" s="1"/>
     </row>
     <row r="469" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C469" t="s">
+        <v>837</v>
+      </c>
       <c r="G469" s="1"/>
     </row>
     <row r="470" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G470" s="1"/>
+      <c r="D470" t="s">
+        <v>838</v>
+      </c>
+      <c r="G470" s="1" t="s">
+        <v>839</v>
+      </c>
     </row>
     <row r="471" spans="2:7" x14ac:dyDescent="0.2">
       <c r="G471" s="1"/>
@@ -6131,6 +6148,7 @@
     <hyperlink ref="G523" r:id="rId159" location=".YLoDxOvTXX8" xr:uid="{8886E3AC-3A64-6449-A070-17D95B586F83}"/>
     <hyperlink ref="F204" r:id="rId160" xr:uid="{5140C3EB-4DFC-5A4A-9C02-C2EBFA052A41}"/>
     <hyperlink ref="F28" r:id="rId161" xr:uid="{99992829-3CC1-2B43-BA73-7F09EAA955A4}"/>
+    <hyperlink ref="G470" r:id="rId162" xr:uid="{01E9516A-34A1-6D40-BED9-61916E777090}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for iterm
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C6EDED-CEF2-3F46-8F5E-8C9B1065B651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284052B0-41F7-EE46-ADB8-7A1E1FE22D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="854">
   <si>
     <t>docker</t>
   </si>
@@ -1851,9 +1851,6 @@
     <t>Shift + Cmd + D</t>
   </si>
   <si>
-    <t>Switch Tabs</t>
-  </si>
-  <si>
     <t>Cmd + left/right arrow</t>
   </si>
   <si>
@@ -2561,6 +2558,51 @@
   </si>
   <si>
     <t>https://til.hashrocket.com/posts/2fdb6afb66-difference-between-wq-and-x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cmd + number </t>
+  </si>
+  <si>
+    <t>Switch Tabs (to a specific one)</t>
+  </si>
+  <si>
+    <t>Switch Tabs (left or right neighbours)</t>
+  </si>
+  <si>
+    <t>Set option key as Meta key on Macbook</t>
+  </si>
+  <si>
+    <t>Terminal -&gt; Preferences -&gt; Profiles -&gt; Keyboard</t>
+  </si>
+  <si>
+    <t>Use Option as Meta key</t>
+  </si>
+  <si>
+    <t>https://www.shell-tips.com/mac/meta-key/</t>
+  </si>
+  <si>
+    <t>Rename sessions</t>
+  </si>
+  <si>
+    <t>1. type Cmd i, and type something</t>
+  </si>
+  <si>
+    <t>2. press Esc</t>
+  </si>
+  <si>
+    <t>https://superuser.com/questions/419775/with-bash-iterm2-how-to-name-tabs</t>
+  </si>
+  <si>
+    <t>for default terminal</t>
+  </si>
+  <si>
+    <t>for ITerm2</t>
+  </si>
+  <si>
+    <t>preferences (Cmd ,) -&gt; profiles -&gt; Keys -&gt; Left option key as "Esc +"</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/196357/making-iterm-to-translate-meta-key-in-the-same-way-as-in-other-oses</t>
   </si>
 </sst>
 </file>
@@ -3023,11 +3065,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I524"/>
+  <dimension ref="B1:I533"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A447" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E472" sqref="E472"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A474" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H497" sqref="H497"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3147,90 +3189,90 @@
         <v>30</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
+        <v>814</v>
+      </c>
+      <c r="E19" t="s">
         <v>815</v>
-      </c>
-      <c r="E19" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
+        <v>816</v>
+      </c>
+      <c r="E20" t="s">
         <v>817</v>
-      </c>
-      <c r="E20" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
+        <v>818</v>
+      </c>
+      <c r="E21" t="s">
         <v>819</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>820</v>
       </c>
-      <c r="F21" t="s">
-        <v>821</v>
-      </c>
       <c r="G21" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
+        <v>823</v>
+      </c>
+      <c r="E23" t="s">
         <v>824</v>
-      </c>
-      <c r="E23" t="s">
-        <v>825</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E24" t="s">
+        <v>825</v>
+      </c>
+      <c r="F24" t="s">
         <v>826</v>
-      </c>
-      <c r="F24" t="s">
-        <v>827</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E25" t="s">
+        <v>827</v>
+      </c>
+      <c r="F25" t="s">
         <v>828</v>
-      </c>
-      <c r="F25" t="s">
-        <v>829</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E26" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D27" t="s">
+        <v>830</v>
+      </c>
+      <c r="E27" t="s">
         <v>831</v>
-      </c>
-      <c r="E27" t="s">
-        <v>832</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
+        <v>832</v>
+      </c>
+      <c r="E28" t="s">
         <v>833</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" s="1" t="s">
         <v>834</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>835</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
@@ -3323,7 +3365,7 @@
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C49" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
@@ -4009,34 +4051,34 @@
     </row>
     <row r="166" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C166" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="167" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D167" t="s">
+        <v>675</v>
+      </c>
+      <c r="E167" t="s">
         <v>676</v>
       </c>
-      <c r="E167" t="s">
-        <v>677</v>
-      </c>
       <c r="F167" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="168" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D168" t="s">
+        <v>677</v>
+      </c>
+      <c r="E168" t="s">
         <v>678</v>
-      </c>
-      <c r="E168" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="169" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D169" t="s">
+        <v>679</v>
+      </c>
+      <c r="E169" t="s">
         <v>680</v>
-      </c>
-      <c r="E169" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="171" spans="3:6" x14ac:dyDescent="0.2">
@@ -4140,7 +4182,7 @@
     </row>
     <row r="185" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D185" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E185" t="s">
         <v>382</v>
@@ -4151,13 +4193,13 @@
     </row>
     <row r="186" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D186" t="s">
+        <v>759</v>
+      </c>
+      <c r="E186" t="s">
         <v>760</v>
       </c>
-      <c r="E186" t="s">
+      <c r="G186" s="1" t="s">
         <v>761</v>
-      </c>
-      <c r="G186" s="1" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="187" spans="3:7" x14ac:dyDescent="0.2">
@@ -4177,7 +4219,7 @@
         <v>63</v>
       </c>
       <c r="G188" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="189" spans="3:7" x14ac:dyDescent="0.2">
@@ -4272,39 +4314,39 @@
     </row>
     <row r="200" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C200" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="201" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D201" t="s">
+        <v>757</v>
+      </c>
+      <c r="E201" t="s">
+        <v>756</v>
+      </c>
+      <c r="F201" s="1" t="s">
         <v>758</v>
-      </c>
-      <c r="E201" t="s">
-        <v>757</v>
-      </c>
-      <c r="F201" s="1" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="202" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E202" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="203" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C203" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="204" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D204" t="s">
+        <v>811</v>
+      </c>
+      <c r="E204" t="s">
+        <v>810</v>
+      </c>
+      <c r="F204" s="1" t="s">
         <v>812</v>
-      </c>
-      <c r="E204" t="s">
-        <v>811</v>
-      </c>
-      <c r="F204" s="1" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="210" spans="2:6" x14ac:dyDescent="0.2">
@@ -4368,24 +4410,24 @@
     </row>
     <row r="218" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C218" t="s">
+        <v>615</v>
+      </c>
+      <c r="D218" t="s">
         <v>616</v>
       </c>
-      <c r="D218" t="s">
+      <c r="F218" s="1" t="s">
         <v>617</v>
-      </c>
-      <c r="F218" s="1" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="219" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C219" t="s">
+        <v>619</v>
+      </c>
+      <c r="D219" t="s">
+        <v>618</v>
+      </c>
+      <c r="F219" s="1" t="s">
         <v>620</v>
-      </c>
-      <c r="D219" t="s">
-        <v>619</v>
-      </c>
-      <c r="F219" s="1" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="220" spans="2:6" x14ac:dyDescent="0.2">
@@ -4396,48 +4438,48 @@
     </row>
     <row r="222" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B222" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="F222" s="1"/>
     </row>
     <row r="223" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C223" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D223" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="F223" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="224" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C224" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D224" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="F224" s="1"/>
     </row>
     <row r="225" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C225" t="s">
+        <v>688</v>
+      </c>
+      <c r="D225" t="s">
         <v>689</v>
-      </c>
-      <c r="D225" t="s">
-        <v>690</v>
       </c>
       <c r="F225" s="1"/>
     </row>
     <row r="226" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C226" t="s">
+        <v>703</v>
+      </c>
+      <c r="D226" t="s">
         <v>704</v>
       </c>
-      <c r="D226" t="s">
+      <c r="F226" s="1" t="s">
         <v>705</v>
-      </c>
-      <c r="F226" s="1" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="227" spans="2:6" x14ac:dyDescent="0.2">
@@ -4459,43 +4501,43 @@
     </row>
     <row r="233" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C233" t="s">
+        <v>613</v>
+      </c>
+      <c r="D233" t="s">
+        <v>612</v>
+      </c>
+      <c r="F233" s="1" t="s">
         <v>614</v>
-      </c>
-      <c r="D233" t="s">
-        <v>613</v>
-      </c>
-      <c r="F233" s="1" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="234" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C234" t="s">
+        <v>621</v>
+      </c>
+      <c r="D234" t="s">
         <v>622</v>
       </c>
-      <c r="D234" t="s">
+      <c r="F234" s="1" t="s">
         <v>623</v>
-      </c>
-      <c r="F234" s="1" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="235" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C235" t="s">
+        <v>625</v>
+      </c>
+      <c r="D235" t="s">
+        <v>624</v>
+      </c>
+      <c r="F235" s="1" t="s">
         <v>626</v>
-      </c>
-      <c r="D235" t="s">
-        <v>625</v>
-      </c>
-      <c r="F235" s="1" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="236" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C236" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D236" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="243" spans="2:5" x14ac:dyDescent="0.2">
@@ -5502,63 +5544,63 @@
     </row>
     <row r="430" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C430" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="431" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D431" t="s">
+        <v>630</v>
+      </c>
+      <c r="E431" t="s">
         <v>631</v>
-      </c>
-      <c r="E431" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="432" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D432" t="s">
+        <v>632</v>
+      </c>
+      <c r="E432" t="s">
         <v>633</v>
-      </c>
-      <c r="E432" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="433" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D433" t="s">
+        <v>634</v>
+      </c>
+      <c r="E433" t="s">
         <v>635</v>
-      </c>
-      <c r="E433" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="434" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D434" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E434" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="435" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D435" t="s">
+        <v>693</v>
+      </c>
+      <c r="E435" t="s">
+        <v>695</v>
+      </c>
+      <c r="G435" s="1" t="s">
         <v>694</v>
-      </c>
-      <c r="E435" t="s">
-        <v>696</v>
-      </c>
-      <c r="G435" s="1" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="438" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B438" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="439" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C439" t="s">
+        <v>779</v>
+      </c>
+      <c r="G439" s="1" t="s">
         <v>780</v>
-      </c>
-      <c r="G439" s="1" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="448" spans="2:7" x14ac:dyDescent="0.2">
@@ -5674,19 +5716,19 @@
     </row>
     <row r="466" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C466" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="G466" s="1"/>
     </row>
     <row r="467" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D467" t="s">
+        <v>609</v>
+      </c>
+      <c r="E467" t="s">
         <v>610</v>
       </c>
-      <c r="E467" t="s">
+      <c r="G467" s="1" t="s">
         <v>611</v>
-      </c>
-      <c r="G467" s="1" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="468" spans="2:7" x14ac:dyDescent="0.2">
@@ -5694,16 +5736,16 @@
     </row>
     <row r="469" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C469" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="G469" s="1"/>
     </row>
     <row r="470" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D470" t="s">
+        <v>837</v>
+      </c>
+      <c r="G470" s="1" t="s">
         <v>838</v>
-      </c>
-      <c r="G470" s="1" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="471" spans="2:7" x14ac:dyDescent="0.2">
@@ -5733,17 +5775,17 @@
         <v>569</v>
       </c>
     </row>
-    <row r="481" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="481" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B481" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="482" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="482" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C482" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="483" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="483" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D483" t="s">
         <v>572</v>
       </c>
@@ -5757,7 +5799,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="484" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="484" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E484" t="s">
         <v>576</v>
       </c>
@@ -5765,12 +5807,12 @@
         <v>577</v>
       </c>
     </row>
-    <row r="485" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="485" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C485" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="486" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="486" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D486" t="s">
         <v>595</v>
       </c>
@@ -5778,7 +5820,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="487" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="487" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D487" t="s">
         <v>598</v>
       </c>
@@ -5786,7 +5828,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="489" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="489" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D489" t="s">
         <v>599</v>
       </c>
@@ -5794,7 +5836,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="490" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="490" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D490" t="s">
         <v>601</v>
       </c>
@@ -5802,187 +5844,255 @@
         <v>602</v>
       </c>
     </row>
-    <row r="492" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="492" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D492" t="s">
+        <v>840</v>
+      </c>
+      <c r="E492" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="493" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D493" t="s">
+        <v>841</v>
+      </c>
+      <c r="E493" t="s">
         <v>603</v>
       </c>
-      <c r="E492" t="s">
+      <c r="G493" s="1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="494" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D494" t="s">
         <v>604</v>
       </c>
-      <c r="G492" s="1" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="493" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D493" t="s">
+      <c r="E494" t="s">
         <v>605</v>
       </c>
-      <c r="E493" t="s">
+      <c r="F494" t="s">
         <v>606</v>
       </c>
-      <c r="F493" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="497" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B497" t="s">
+    </row>
+    <row r="496" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D496" t="s">
+        <v>842</v>
+      </c>
+      <c r="E496" t="s">
+        <v>851</v>
+      </c>
+      <c r="F496" t="s">
+        <v>852</v>
+      </c>
+      <c r="H496" s="1" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="497" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="E497" t="s">
+        <v>850</v>
+      </c>
+      <c r="F497" t="s">
+        <v>843</v>
+      </c>
+      <c r="G497" t="s">
+        <v>844</v>
+      </c>
+      <c r="H497" s="1" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="498" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G498" s="1"/>
+    </row>
+    <row r="499" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D499" t="s">
+        <v>846</v>
+      </c>
+      <c r="E499" t="s">
+        <v>847</v>
+      </c>
+      <c r="G499" s="1" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="500" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="E500" t="s">
+        <v>848</v>
+      </c>
+      <c r="G500" s="1"/>
+    </row>
+    <row r="501" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G501" s="1"/>
+    </row>
+    <row r="502" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G502" s="1"/>
+    </row>
+    <row r="503" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G503" s="1"/>
+    </row>
+    <row r="504" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G504" s="1"/>
+    </row>
+    <row r="506" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B506" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="498" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C498" t="s">
+    <row r="507" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C507" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="499" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D499" t="s">
+    <row r="508" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D508" t="s">
         <v>581</v>
       </c>
-      <c r="E499" t="s">
+      <c r="E508" t="s">
         <v>582</v>
       </c>
-      <c r="F499" t="s">
+      <c r="F508" t="s">
         <v>580</v>
       </c>
-      <c r="G499" s="1" t="s">
+      <c r="G508" s="1" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="500" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E500" t="s">
+    <row r="509" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="E509" t="s">
         <v>583</v>
       </c>
-      <c r="F500" t="s">
+      <c r="F509" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="502" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D502" t="s">
+    <row r="511" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D511" t="s">
         <v>586</v>
       </c>
-      <c r="E502" t="s">
+      <c r="E511" t="s">
         <v>588</v>
       </c>
-      <c r="F502" t="s">
+      <c r="F511" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="505" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B505" t="s">
+    <row r="514" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B514" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="515" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C515" t="s">
         <v>707</v>
       </c>
-    </row>
-    <row r="506" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C506" t="s">
+      <c r="D515" t="s">
+        <v>710</v>
+      </c>
+      <c r="G515" s="1" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="516" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C516" t="s">
         <v>708</v>
       </c>
-      <c r="D506" t="s">
+      <c r="D516" t="s">
         <v>711</v>
-      </c>
-      <c r="G506" s="1" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="507" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C507" t="s">
-        <v>709</v>
-      </c>
-      <c r="D507" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="508" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C508" t="s">
-        <v>710</v>
-      </c>
-      <c r="D508" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="511" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B511" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="512" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C512" t="s">
-        <v>732</v>
-      </c>
-      <c r="G512" s="1" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="513" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C513" t="s">
-        <v>734</v>
-      </c>
-      <c r="G513" s="1" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="514" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C514" t="s">
-        <v>738</v>
-      </c>
-      <c r="F514" t="s">
-        <v>736</v>
-      </c>
-      <c r="G514" s="1" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="516" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B516" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="517" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C517" t="s">
-        <v>744</v>
+        <v>709</v>
       </c>
       <c r="D517" t="s">
-        <v>745</v>
-      </c>
-      <c r="G517" s="1" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="518" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C518" t="s">
-        <v>747</v>
-      </c>
-      <c r="D518" t="s">
-        <v>748</v>
-      </c>
-      <c r="G518" s="1" t="s">
-        <v>749</v>
+        <v>712</v>
+      </c>
+    </row>
+    <row r="520" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B520" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="521" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C521" t="s">
+        <v>731</v>
+      </c>
+      <c r="G521" s="1" t="s">
+        <v>732</v>
       </c>
     </row>
     <row r="522" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B522" t="s">
-        <v>802</v>
+      <c r="C522" t="s">
+        <v>733</v>
+      </c>
+      <c r="G522" s="1" t="s">
+        <v>734</v>
       </c>
     </row>
     <row r="523" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C523" t="s">
+        <v>737</v>
+      </c>
+      <c r="F523" t="s">
+        <v>735</v>
+      </c>
+      <c r="G523" s="1" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="525" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B525" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="526" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C526" t="s">
+        <v>743</v>
+      </c>
+      <c r="D526" t="s">
+        <v>744</v>
+      </c>
+      <c r="G526" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="527" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C527" t="s">
+        <v>746</v>
+      </c>
+      <c r="D527" t="s">
+        <v>747</v>
+      </c>
+      <c r="G527" s="1" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="531" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B531" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="532" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C532" t="s">
+        <v>802</v>
+      </c>
+      <c r="D532" t="s">
         <v>803</v>
       </c>
-      <c r="D523" t="s">
+      <c r="E532" t="s">
         <v>804</v>
       </c>
-      <c r="E523" t="s">
+      <c r="G532" s="1" t="s">
         <v>805</v>
       </c>
-      <c r="G523" s="1" t="s">
+    </row>
+    <row r="533" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C533" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="524" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C524" t="s">
+      <c r="E533" t="s">
         <v>807</v>
-      </c>
-      <c r="E524" t="s">
-        <v>808</v>
       </c>
     </row>
   </sheetData>
@@ -6121,10 +6231,10 @@
     <hyperlink ref="G465" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
     <hyperlink ref="G478" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
     <hyperlink ref="G483" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
-    <hyperlink ref="G499" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
+    <hyperlink ref="G508" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
     <hyperlink ref="E35" r:id="rId136" xr:uid="{809CA2D1-39E9-0045-A4DF-E4C0C2E97FA2}"/>
     <hyperlink ref="E36" r:id="rId137" xr:uid="{5DC44543-F2B9-F841-9097-6DB19C5EBD82}"/>
-    <hyperlink ref="G492" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
+    <hyperlink ref="G493" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
     <hyperlink ref="G467" r:id="rId139" xr:uid="{7F4EA1D7-8774-1A4B-BF25-18ED0416CB20}"/>
     <hyperlink ref="F233" r:id="rId140" xr:uid="{101513F3-87A1-DA41-8BF5-E4029309ECB8}"/>
     <hyperlink ref="F218" r:id="rId141" xr:uid="{494E255E-6912-8643-B5CD-1D65E0DDCFFC}"/>
@@ -6135,20 +6245,23 @@
     <hyperlink ref="F223" r:id="rId146" xr:uid="{28F6BA28-EB9B-374C-A8A0-4077C800D23A}"/>
     <hyperlink ref="G435" r:id="rId147" xr:uid="{20B4F69E-7592-784A-8C2E-123726A51D93}"/>
     <hyperlink ref="F226" r:id="rId148" xr:uid="{E3C3D7C6-1E6E-FF40-8CC7-6CF1C77457E4}"/>
-    <hyperlink ref="G506" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
+    <hyperlink ref="G515" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
     <hyperlink ref="G188" r:id="rId150" xr:uid="{9BECD448-C575-B64B-BA3F-BEE8D1CBBD43}"/>
-    <hyperlink ref="G512" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
-    <hyperlink ref="G513" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
-    <hyperlink ref="G514" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
-    <hyperlink ref="G517" r:id="rId154" xr:uid="{FB93E0B8-2537-FD47-8420-84D2A706F697}"/>
-    <hyperlink ref="G518" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
+    <hyperlink ref="G521" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
+    <hyperlink ref="G522" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
+    <hyperlink ref="G523" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
+    <hyperlink ref="G526" r:id="rId154" xr:uid="{FB93E0B8-2537-FD47-8420-84D2A706F697}"/>
+    <hyperlink ref="G527" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
     <hyperlink ref="F201" r:id="rId156" location="2116892" xr:uid="{FF1C16E6-B146-B548-B694-396AC9D0B975}"/>
     <hyperlink ref="G186" r:id="rId157" xr:uid="{ED09A21C-0057-1146-8BFF-213A32FC88DF}"/>
     <hyperlink ref="G439" r:id="rId158" xr:uid="{F933A5C4-6DD5-5547-8BB3-B5D3FBA7A852}"/>
-    <hyperlink ref="G523" r:id="rId159" location=".YLoDxOvTXX8" xr:uid="{8886E3AC-3A64-6449-A070-17D95B586F83}"/>
+    <hyperlink ref="G532" r:id="rId159" location=".YLoDxOvTXX8" xr:uid="{8886E3AC-3A64-6449-A070-17D95B586F83}"/>
     <hyperlink ref="F204" r:id="rId160" xr:uid="{5140C3EB-4DFC-5A4A-9C02-C2EBFA052A41}"/>
     <hyperlink ref="F28" r:id="rId161" xr:uid="{99992829-3CC1-2B43-BA73-7F09EAA955A4}"/>
     <hyperlink ref="G470" r:id="rId162" xr:uid="{01E9516A-34A1-6D40-BED9-61916E777090}"/>
+    <hyperlink ref="H497" r:id="rId163" xr:uid="{D3C22B64-1D55-1D47-8F15-25C4AA3D5B90}"/>
+    <hyperlink ref="G499" r:id="rId164" xr:uid="{8E28D310-73EF-1C47-A666-DEE78634BFDF}"/>
+    <hyperlink ref="H496" r:id="rId165" xr:uid="{66476745-9FC4-9E4B-952E-C3E33F678E5D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6480,68 +6593,68 @@
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C29" t="s">
         <v>168</v>
       </c>
       <c r="E29" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
+        <v>641</v>
+      </c>
+      <c r="E30" t="s">
         <v>642</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" s="1" t="s">
         <v>643</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="E31" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>659</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
+        <v>644</v>
+      </c>
+      <c r="E32" t="s">
         <v>645</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" s="1" t="s">
         <v>646</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
+        <v>649</v>
+      </c>
+      <c r="C33" t="s">
+        <v>647</v>
+      </c>
+      <c r="D33" t="s">
+        <v>648</v>
+      </c>
+      <c r="E33" t="s">
         <v>650</v>
       </c>
-      <c r="C33" t="s">
-        <v>648</v>
-      </c>
-      <c r="D33" t="s">
-        <v>649</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="F33" s="1" t="s">
         <v>651</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C34" t="s">
         <v>168</v>
@@ -6550,81 +6663,81 @@
         <v>446</v>
       </c>
       <c r="E34" t="s">
+        <v>653</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>654</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="35" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
+        <v>655</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>656</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>658</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
+        <v>660</v>
+      </c>
+      <c r="E36" t="s">
+        <v>662</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>661</v>
-      </c>
-      <c r="E36" t="s">
-        <v>663</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D37" t="s">
         <v>446</v>
       </c>
       <c r="E37" t="s">
+        <v>664</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>665</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
+        <v>666</v>
+      </c>
+      <c r="E38" t="s">
         <v>667</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" s="1" t="s">
         <v>668</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
+        <v>669</v>
+      </c>
+      <c r="E39" t="s">
         <v>670</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" s="1" t="s">
         <v>671</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C41" t="s">
         <v>168</v>
@@ -6633,263 +6746,263 @@
         <v>446</v>
       </c>
       <c r="E41" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E42" t="s">
+        <v>699</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>700</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E43" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E46" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E47" t="s">
+        <v>718</v>
+      </c>
+      <c r="F47" t="s">
         <v>719</v>
-      </c>
-      <c r="F47" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="D49" t="s">
         <v>446</v>
       </c>
       <c r="E49" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
+        <v>749</v>
+      </c>
+      <c r="E50" t="s">
         <v>750</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" s="1" t="s">
         <v>751</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
+        <v>738</v>
+      </c>
+      <c r="E52" t="s">
         <v>739</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" s="1" t="s">
         <v>740</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F53" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
+        <v>762</v>
+      </c>
+      <c r="E54" t="s">
         <v>763</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" s="1" t="s">
         <v>764</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C55" t="s">
         <v>467</v>
       </c>
       <c r="D55" t="s">
+        <v>766</v>
+      </c>
+      <c r="E55" t="s">
         <v>767</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" s="1" t="s">
         <v>768</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>769</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C56" t="s">
         <v>467</v>
       </c>
       <c r="E56" t="s">
+        <v>769</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>770</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>771</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E57" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C59" t="s">
         <v>467</v>
       </c>
       <c r="E59" t="s">
+        <v>776</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>777</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>778</v>
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E60" t="s">
+        <v>781</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>782</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D61" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E61" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
+        <v>787</v>
+      </c>
+      <c r="C62" t="s">
+        <v>789</v>
+      </c>
+      <c r="E62" t="s">
+        <v>790</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>788</v>
-      </c>
-      <c r="C62" t="s">
-        <v>790</v>
-      </c>
-      <c r="E62" t="s">
-        <v>791</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
+        <v>791</v>
+      </c>
+      <c r="C63" t="s">
+        <v>794</v>
+      </c>
+      <c r="E63" t="s">
+        <v>793</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>792</v>
-      </c>
-      <c r="C63" t="s">
-        <v>795</v>
-      </c>
-      <c r="E63" t="s">
-        <v>794</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>793</v>
       </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
+        <v>795</v>
+      </c>
+      <c r="E64" t="s">
+        <v>797</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>796</v>
-      </c>
-      <c r="E64" t="s">
-        <v>798</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>797</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
+        <v>798</v>
+      </c>
+      <c r="C65" t="s">
+        <v>648</v>
+      </c>
+      <c r="E65" t="s">
         <v>799</v>
       </c>
-      <c r="C65" t="s">
-        <v>649</v>
-      </c>
-      <c r="E65" t="s">
+      <c r="F65" s="1" t="s">
         <v>800</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>801</v>
       </c>
     </row>
   </sheetData>
@@ -6977,13 +7090,13 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>690</v>
+      </c>
+      <c r="C2" t="s">
         <v>691</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" s="1" t="s">
         <v>692</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>693</v>
       </c>
     </row>
   </sheetData>
@@ -7006,10 +7119,10 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>752</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>753</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>754</v>
       </c>
       <c r="D2" s="7"/>
     </row>

</xml_diff>

<commit_message>
updated tip for meta key in ITerm
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2585A25F-88F0-F443-BA05-0762C0D045D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEB5FBE-60F0-7F4D-ADDC-A988EAD2E85F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1280" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -2599,10 +2599,10 @@
     <t>for ITerm2</t>
   </si>
   <si>
-    <t>preferences (Cmd ,) -&gt; profiles -&gt; Keys -&gt; Left option key as "Esc +"</t>
-  </si>
-  <si>
     <t>https://stackoverflow.com/questions/196357/making-iterm-to-translate-meta-key-in-the-same-way-as-in-other-oses</t>
+  </si>
+  <si>
+    <t>preferences (Cmd ,) -&gt; profiles -&gt; Keys -&gt; Right option key as "Esc +"</t>
   </si>
 </sst>
 </file>
@@ -3068,8 +3068,8 @@
   <dimension ref="B1:I533"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A420" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B535" sqref="B535"/>
+      <pane ySplit="1" topLeftCell="A484" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F497" sqref="F497"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5882,10 +5882,10 @@
         <v>851</v>
       </c>
       <c r="F496" t="s">
+        <v>853</v>
+      </c>
+      <c r="H496" s="1" t="s">
         <v>852</v>
-      </c>
-      <c r="H496" s="1" t="s">
-        <v>853</v>
       </c>
     </row>
     <row r="497" spans="2:8" x14ac:dyDescent="0.2">
@@ -6271,7 +6271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
   <dimension ref="B2:G65"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added tips for zsh and bash and vim
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEB5FBE-60F0-7F4D-ADDC-A988EAD2E85F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9951E9-8A8C-3B4A-9164-86E4F90027EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="869">
   <si>
     <t>docker</t>
   </si>
@@ -2603,6 +2603,51 @@
   </si>
   <si>
     <t>preferences (Cmd ,) -&gt; profiles -&gt; Keys -&gt; Right option key as "Esc +"</t>
+  </si>
+  <si>
+    <t>Let’s Encrypt (certbot)</t>
+  </si>
+  <si>
+    <t>1. add the Certbot Ubuntu repository:</t>
+  </si>
+  <si>
+    <t>2. Install Certbot’s Nginx package with apt:</t>
+  </si>
+  <si>
+    <t>3. Securing the Application</t>
+  </si>
+  <si>
+    <t>sudo add-apt-repository ppa:certbot/certbot</t>
+  </si>
+  <si>
+    <t>sudo apt install python-certbot-nginx</t>
+  </si>
+  <si>
+    <t>sudo certbot --nginx -d your_domain -d www.your_domain</t>
+  </si>
+  <si>
+    <t>https://www.digitalocean.com/community/tutorials/how-to-serve-flask-applications-with-gunicorn-and-nginx-on-ubuntu-18-04</t>
+  </si>
+  <si>
+    <t>using vi key bindings in the terminal</t>
+  </si>
+  <si>
+    <t>in .zshrc add the following configuration</t>
+  </si>
+  <si>
+    <t>for bash, run the following command or add it to .bashrc</t>
+  </si>
+  <si>
+    <t>React</t>
+  </si>
+  <si>
+    <t>portfolio website</t>
+  </si>
+  <si>
+    <t>https://codeburst.io/learn-react-js-build-a-portfolio-single-page-application-spa-ba001082a711</t>
+  </si>
+  <si>
+    <t>Develop and Build React App With NodeJS</t>
   </si>
 </sst>
 </file>
@@ -3065,11 +3110,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I533"/>
+  <dimension ref="B1:I541"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A484" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F497" sqref="F497"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A487" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D504" sqref="D504"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5923,12 +5968,27 @@
       <c r="G500" s="1"/>
     </row>
     <row r="501" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C501" t="s">
+        <v>862</v>
+      </c>
       <c r="G501" s="1"/>
     </row>
     <row r="502" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D502" t="s">
+        <v>863</v>
+      </c>
+      <c r="E502" t="s">
+        <v>574</v>
+      </c>
       <c r="G502" s="1"/>
     </row>
     <row r="503" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D503" t="s">
+        <v>864</v>
+      </c>
+      <c r="E503" t="s">
+        <v>577</v>
+      </c>
       <c r="G503" s="1"/>
     </row>
     <row r="504" spans="2:8" x14ac:dyDescent="0.2">
@@ -6093,6 +6153,44 @@
       </c>
       <c r="E533" t="s">
         <v>807</v>
+      </c>
+    </row>
+    <row r="535" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B535" t="s">
+        <v>854</v>
+      </c>
+      <c r="G535" s="1" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="536" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C536" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="537" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D537" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="538" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C538" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="539" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D539" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="540" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C540" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="541" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D541" t="s">
+        <v>860</v>
       </c>
     </row>
   </sheetData>
@@ -6262,6 +6360,7 @@
     <hyperlink ref="H497" r:id="rId163" xr:uid="{D3C22B64-1D55-1D47-8F15-25C4AA3D5B90}"/>
     <hyperlink ref="G499" r:id="rId164" xr:uid="{8E28D310-73EF-1C47-A666-DEE78634BFDF}"/>
     <hyperlink ref="H496" r:id="rId165" xr:uid="{66476745-9FC4-9E4B-952E-C3E33F678E5D}"/>
+    <hyperlink ref="G535" r:id="rId166" xr:uid="{04D185B2-C246-8B4F-8813-F5A12B741A26}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7109,13 +7208,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069EEB69-0D57-C040-8545-840D5862E858}">
-  <dimension ref="B2:D2"/>
+  <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
@@ -7126,9 +7229,32 @@
       </c>
       <c r="D2" s="7"/>
     </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>866</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>868</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{87D156EE-D133-464D-8B0D-7B076D239955}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{6812A241-D9CB-E242-8838-F006FA23EEAA}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{4B055411-C0BB-1F40-94E0-26C52286F8A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added websites for react and flash
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9951E9-8A8C-3B4A-9164-86E4F90027EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6E6CF2-FAE7-3F42-9632-9D96B9F61BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="869">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="873">
   <si>
     <t>docker</t>
   </si>
@@ -2648,6 +2648,18 @@
   </si>
   <si>
     <t>Develop and Build React App With NodeJS</t>
+  </si>
+  <si>
+    <t>Flask</t>
+  </si>
+  <si>
+    <t>Serve Flask Applications with Gunicorn and Nginx on Ubuntu</t>
+  </si>
+  <si>
+    <t>https://www.digitalocean.com/community/tutorials/how-to-deploy-a-react-application-with-nginx-on-ubuntu-20-04</t>
+  </si>
+  <si>
+    <t>Deploy a React Application with Nginx</t>
   </si>
 </sst>
 </file>
@@ -7208,16 +7220,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069EEB69-0D57-C040-8545-840D5862E858}">
-  <dimension ref="B2:D6"/>
+  <dimension ref="B2:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19.1640625" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
@@ -7250,11 +7262,43 @@
         <v>414</v>
       </c>
     </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>872</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>870</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>861</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{87D156EE-D133-464D-8B0D-7B076D239955}"/>
     <hyperlink ref="D5" r:id="rId2" xr:uid="{6812A241-D9CB-E242-8838-F006FA23EEAA}"/>
     <hyperlink ref="D6" r:id="rId3" xr:uid="{4B055411-C0BB-1F40-94E0-26C52286F8A7}"/>
+    <hyperlink ref="D13" r:id="rId4" xr:uid="{285EBC06-8ECF-4C47-AB0D-38C1776297C3}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{DA30C5A1-BF15-2449-AD30-BFE122EB375C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for 'find' and 'locate' command
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E35D97-35FB-7D4B-9670-2DDC718EBDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B6D08B-8122-D34A-B4D9-F63951A3888E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="876">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="882">
   <si>
     <t>docker</t>
   </si>
@@ -2669,6 +2669,24 @@
   </si>
   <si>
     <t>https://www.2daygeek.com/how-to-check-all-running-services-in-linux/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">find a file in the file system </t>
+  </si>
+  <si>
+    <t>sudo find / -name "filename"</t>
+  </si>
+  <si>
+    <t>locate {file-name-or-path}</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/24655436/how-can-i-find-a-file-directory-that-could-be-anywhere-on-linux-command-line</t>
+  </si>
+  <si>
+    <t>option 1</t>
+  </si>
+  <si>
+    <t>option 2</t>
   </si>
 </sst>
 </file>
@@ -3133,9 +3151,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
   <dimension ref="B1:I541"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A487" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D504" sqref="D504"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A261" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D279" sqref="D279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4776,7 +4794,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="273" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="273" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C273" t="s">
         <v>298</v>
       </c>
@@ -4784,10 +4802,10 @@
         <v>297</v>
       </c>
     </row>
-    <row r="274" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="274" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E274" s="1"/>
     </row>
-    <row r="275" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="275" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C275" t="s">
         <v>358</v>
       </c>
@@ -4798,36 +4816,52 @@
         <v>360</v>
       </c>
     </row>
-    <row r="276" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="276" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E276" s="1"/>
     </row>
-    <row r="277" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E277" s="1"/>
-    </row>
-    <row r="278" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E278" s="1"/>
-    </row>
-    <row r="279" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="277" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C277" t="s">
+        <v>876</v>
+      </c>
+      <c r="D277" t="s">
+        <v>880</v>
+      </c>
+      <c r="E277" t="s">
+        <v>877</v>
+      </c>
+      <c r="F277" s="1" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="278" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D278" t="s">
+        <v>881</v>
+      </c>
+      <c r="E278" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="279" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E279" s="1"/>
     </row>
-    <row r="280" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="280" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E280" s="1"/>
     </row>
-    <row r="281" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="281" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E281" s="1"/>
     </row>
-    <row r="282" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="282" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E282" s="1"/>
     </row>
-    <row r="283" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="283" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E283" s="1"/>
     </row>
-    <row r="284" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="284" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C284" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="285" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="285" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D285" t="s">
         <v>134</v>
       </c>
@@ -4835,7 +4869,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="286" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="286" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D286" t="s">
         <v>135</v>
       </c>
@@ -4843,7 +4877,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="287" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="287" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D287" t="s">
         <v>139</v>
       </c>
@@ -4851,7 +4885,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="288" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="288" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D288" t="s">
         <v>136</v>
       </c>
@@ -6382,6 +6416,7 @@
     <hyperlink ref="G499" r:id="rId164" xr:uid="{8E28D310-73EF-1C47-A666-DEE78634BFDF}"/>
     <hyperlink ref="H496" r:id="rId165" xr:uid="{66476745-9FC4-9E4B-952E-C3E33F678E5D}"/>
     <hyperlink ref="G535" r:id="rId166" xr:uid="{04D185B2-C246-8B4F-8813-F5A12B741A26}"/>
+    <hyperlink ref="F277" r:id="rId167" xr:uid="{82506100-4BAC-4E48-9F8D-88B7E33868BA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7231,7 +7266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069EEB69-0D57-C040-8545-840D5862E858}">
   <dimension ref="B2:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added socket tutorial webpage
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B6D08B-8122-D34A-B4D9-F63951A3888E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8883C9-F88C-004E-8771-4BC58D7AB77B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="884">
   <si>
     <t>docker</t>
   </si>
@@ -2687,6 +2687,12 @@
   </si>
   <si>
     <t>option 2</t>
+  </si>
+  <si>
+    <t>https://www.tutorialspoint.com/unix_sockets/unix_sockets_discussion.htm</t>
+  </si>
+  <si>
+    <t>Unix socket tutorial</t>
   </si>
 </sst>
 </file>
@@ -3151,8 +3157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
   <dimension ref="B1:I541"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A261" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A253" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D279" sqref="D279"/>
     </sheetView>
   </sheetViews>
@@ -6424,10 +6430,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G65"/>
+  <dimension ref="B2:G67"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7158,6 +7164,14 @@
       </c>
       <c r="F65" s="1" t="s">
         <v>800</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>883</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>882</v>
       </c>
     </row>
   </sheetData>
@@ -7224,6 +7238,7 @@
     <hyperlink ref="F63" r:id="rId60" xr:uid="{8AED1472-61F4-E646-89E7-A2D566BEF7A0}"/>
     <hyperlink ref="F64" r:id="rId61" xr:uid="{D5875307-B681-3841-BE35-59A92CDCD038}"/>
     <hyperlink ref="F65" r:id="rId62" xr:uid="{E6DDA861-2175-8242-9563-08D5A89ACF52}"/>
+    <hyperlink ref="F67" r:id="rId63" xr:uid="{14F89032-FA45-0F42-9BB7-109EA9891E0E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for kubernetics
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8883C9-F88C-004E-8771-4BC58D7AB77B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483F3668-8EAD-F74B-84E2-58D49A6C618C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="884">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="880">
   <si>
     <t>docker</t>
   </si>
@@ -2671,28 +2671,16 @@
     <t>https://www.2daygeek.com/how-to-check-all-running-services-in-linux/</t>
   </si>
   <si>
-    <t xml:space="preserve">find a file in the file system </t>
-  </si>
-  <si>
-    <t>sudo find / -name "filename"</t>
-  </si>
-  <si>
-    <t>locate {file-name-or-path}</t>
-  </si>
-  <si>
-    <t>https://stackoverflow.com/questions/24655436/how-can-i-find-a-file-directory-that-could-be-anywhere-on-linux-command-line</t>
-  </si>
-  <si>
-    <t>option 1</t>
-  </si>
-  <si>
-    <t>option 2</t>
-  </si>
-  <si>
-    <t>https://www.tutorialspoint.com/unix_sockets/unix_sockets_discussion.htm</t>
-  </si>
-  <si>
-    <t>Unix socket tutorial</t>
+    <t>Kubernetics</t>
+  </si>
+  <si>
+    <t>Install K9s on Macbook</t>
+  </si>
+  <si>
+    <t>curl -sS https://webinstall.dev/k9s | bash</t>
+  </si>
+  <si>
+    <t>https://github.com/derailed/k9s</t>
   </si>
 </sst>
 </file>
@@ -3155,11 +3143,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I541"/>
+  <dimension ref="B1:I545"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A253" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D279" sqref="D279"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A532" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D556" sqref="D556"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4800,7 +4788,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="273" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="273" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C273" t="s">
         <v>298</v>
       </c>
@@ -4808,10 +4796,10 @@
         <v>297</v>
       </c>
     </row>
-    <row r="274" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="274" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E274" s="1"/>
     </row>
-    <row r="275" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="275" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C275" t="s">
         <v>358</v>
       </c>
@@ -4822,52 +4810,36 @@
         <v>360</v>
       </c>
     </row>
-    <row r="276" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="276" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E276" s="1"/>
     </row>
-    <row r="277" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C277" t="s">
-        <v>876</v>
-      </c>
-      <c r="D277" t="s">
-        <v>880</v>
-      </c>
-      <c r="E277" t="s">
-        <v>877</v>
-      </c>
-      <c r="F277" s="1" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="278" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D278" t="s">
-        <v>881</v>
-      </c>
-      <c r="E278" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="279" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="277" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E277" s="1"/>
+    </row>
+    <row r="278" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E278" s="1"/>
+    </row>
+    <row r="279" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E279" s="1"/>
     </row>
-    <row r="280" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="280" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E280" s="1"/>
     </row>
-    <row r="281" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="281" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E281" s="1"/>
     </row>
-    <row r="282" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="282" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E282" s="1"/>
     </row>
-    <row r="283" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="283" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E283" s="1"/>
     </row>
-    <row r="284" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="284" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C284" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="285" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="285" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D285" t="s">
         <v>134</v>
       </c>
@@ -4875,7 +4847,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="286" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="286" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D286" t="s">
         <v>135</v>
       </c>
@@ -4883,7 +4855,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="287" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="287" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D287" t="s">
         <v>139</v>
       </c>
@@ -4891,7 +4863,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="288" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="288" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D288" t="s">
         <v>136</v>
       </c>
@@ -6252,6 +6224,22 @@
     <row r="541" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D541" t="s">
         <v>860</v>
+      </c>
+    </row>
+    <row r="544" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B544" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="545" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C545" t="s">
+        <v>877</v>
+      </c>
+      <c r="D545" t="s">
+        <v>878</v>
+      </c>
+      <c r="G545" s="1" t="s">
+        <v>879</v>
       </c>
     </row>
   </sheetData>
@@ -6422,7 +6410,7 @@
     <hyperlink ref="G499" r:id="rId164" xr:uid="{8E28D310-73EF-1C47-A666-DEE78634BFDF}"/>
     <hyperlink ref="H496" r:id="rId165" xr:uid="{66476745-9FC4-9E4B-952E-C3E33F678E5D}"/>
     <hyperlink ref="G535" r:id="rId166" xr:uid="{04D185B2-C246-8B4F-8813-F5A12B741A26}"/>
-    <hyperlink ref="F277" r:id="rId167" xr:uid="{82506100-4BAC-4E48-9F8D-88B7E33868BA}"/>
+    <hyperlink ref="G545" r:id="rId167" xr:uid="{D89D9875-8DF0-3044-BF56-09B8E52D068E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6430,10 +6418,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G67"/>
+  <dimension ref="B2:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7164,14 +7152,6 @@
       </c>
       <c r="F65" s="1" t="s">
         <v>800</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
-        <v>883</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>882</v>
       </c>
     </row>
   </sheetData>
@@ -7238,7 +7218,6 @@
     <hyperlink ref="F63" r:id="rId60" xr:uid="{8AED1472-61F4-E646-89E7-A2D566BEF7A0}"/>
     <hyperlink ref="F64" r:id="rId61" xr:uid="{D5875307-B681-3841-BE35-59A92CDCD038}"/>
     <hyperlink ref="F65" r:id="rId62" xr:uid="{E6DDA861-2175-8242-9563-08D5A89ACF52}"/>
-    <hyperlink ref="F67" r:id="rId63" xr:uid="{14F89032-FA45-0F42-9BB7-109EA9891E0E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for docker
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483F3668-8EAD-F74B-84E2-58D49A6C618C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5AED25-5B5D-094B-A153-4F80630E70D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2480" yWindow="4200" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="880">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="886">
   <si>
     <t>docker</t>
   </si>
@@ -2681,6 +2681,24 @@
   </si>
   <si>
     <t>https://github.com/derailed/k9s</t>
+  </si>
+  <si>
+    <t>5. Push image to container repository</t>
+  </si>
+  <si>
+    <t>docker push local_service_name:version</t>
+  </si>
+  <si>
+    <t>6. Pull image from containerr repository</t>
+  </si>
+  <si>
+    <t>docker pull local_service_name:version</t>
+  </si>
+  <si>
+    <t>7. Tag image with a new name</t>
+  </si>
+  <si>
+    <t>docker tag old_name:version new_name:version</t>
   </si>
 </sst>
 </file>
@@ -3143,11 +3161,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I545"/>
+  <dimension ref="B1:I552"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A532" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D556" sqref="D556"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3543,1021 +3561,1008 @@
         <v>44</v>
       </c>
     </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C72" t="s">
+        <v>880</v>
+      </c>
+    </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B73" t="s">
-        <v>45</v>
+      <c r="D73" t="s">
+        <v>38</v>
+      </c>
+      <c r="E73" t="s">
+        <v>881</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C74" t="s">
-        <v>46</v>
+        <v>882</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D75" t="s">
-        <v>47</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>55</v>
+        <v>38</v>
+      </c>
+      <c r="E75" t="s">
+        <v>883</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
-        <v>48</v>
+        <v>884</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D77" t="s">
+        <v>38</v>
+      </c>
+      <c r="E77" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B80" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="81" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C81" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D82" t="s">
+        <v>47</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="83" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C83" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="84" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D84" t="s">
         <v>50</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E84" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D78" t="s">
+    <row r="85" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D85" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C79" t="s">
+    <row r="86" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C86" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D80" t="s">
-        <v>53</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C82" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D83" t="s">
-        <v>57</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E84" s="1"/>
-    </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C85" t="s">
-        <v>198</v>
-      </c>
-      <c r="E85" s="1"/>
-    </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D86" t="s">
-        <v>203</v>
-      </c>
-      <c r="E86" t="s">
-        <v>53</v>
-      </c>
-      <c r="F86" t="s">
-        <v>200</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="87" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D87" t="s">
+        <v>53</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="89" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C89" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="90" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D90" t="s">
+        <v>57</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="91" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E91" s="1"/>
+    </row>
+    <row r="92" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C92" t="s">
+        <v>198</v>
+      </c>
+      <c r="E92" s="1"/>
+    </row>
+    <row r="93" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D93" t="s">
+        <v>203</v>
+      </c>
+      <c r="E93" t="s">
+        <v>53</v>
+      </c>
+      <c r="F93" t="s">
+        <v>200</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="94" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
         <v>204</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E94" t="s">
         <v>201</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F94" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E88" s="1"/>
-    </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E89" s="1"/>
-    </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C90" t="s">
+    <row r="95" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E95" s="1"/>
+    </row>
+    <row r="96" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E96" s="1"/>
+    </row>
+    <row r="97" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C97" t="s">
         <v>192</v>
       </c>
-      <c r="E90" s="1"/>
-    </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D91" t="s">
+      <c r="E97" s="1"/>
+    </row>
+    <row r="98" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D98" t="s">
         <v>193</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="E98" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E92" s="1" t="s">
+    <row r="99" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E99" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E93" s="1" t="s">
+    <row r="100" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E100" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="94" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E94" s="1"/>
-    </row>
-    <row r="95" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D95" t="s">
+    <row r="101" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E101" s="1"/>
+    </row>
+    <row r="102" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D102" t="s">
         <v>328</v>
       </c>
-      <c r="E95" s="1" t="s">
+      <c r="E102" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="96" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D96" s="3" t="s">
+    <row r="103" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D103" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="E103" s="1" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E97" s="1"/>
-    </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B107" t="s">
+    <row r="104" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E104" s="1"/>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B114" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C108" t="s">
+    <row r="115" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C115" t="s">
         <v>156</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="D115" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C109" t="s">
+    <row r="116" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C116" t="s">
         <v>158</v>
       </c>
-      <c r="D109" s="1" t="s">
+      <c r="D116" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C110" t="s">
+    <row r="117" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C117" t="s">
         <v>159</v>
       </c>
-      <c r="D110" s="1" t="s">
+      <c r="D117" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C111" t="s">
+    <row r="118" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C118" t="s">
         <v>218</v>
       </c>
-      <c r="D111" s="1" t="s">
+      <c r="D118" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E111" s="1" t="s">
+      <c r="E118" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="113" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C113" t="s">
+    <row r="120" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C120" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D114" t="s">
+    <row r="121" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D121" t="s">
         <v>163</v>
       </c>
-      <c r="E114" t="s">
+      <c r="E121" t="s">
         <v>162</v>
       </c>
-      <c r="F114" s="1" t="s">
+      <c r="F121" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="115" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="E115" t="s">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E122" t="s">
         <v>274</v>
       </c>
-      <c r="F115" s="1"/>
-    </row>
-    <row r="116" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D116" t="s">
+      <c r="F122" s="1"/>
+    </row>
+    <row r="123" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D123" t="s">
         <v>165</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E123" t="s">
         <v>166</v>
       </c>
-      <c r="F116" s="1" t="s">
+      <c r="F123" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="117" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D117" t="s">
+    <row r="124" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D124" t="s">
         <v>179</v>
       </c>
-      <c r="E117" t="s">
+      <c r="E124" t="s">
         <v>180</v>
       </c>
-      <c r="F117" s="1" t="s">
+      <c r="F124" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="118" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D118" t="s">
+    <row r="125" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D125" t="s">
         <v>189</v>
       </c>
-      <c r="E118" t="s">
+      <c r="E125" t="s">
         <v>191</v>
       </c>
-      <c r="F118" t="s">
+      <c r="F125" t="s">
         <v>195</v>
       </c>
-      <c r="G118" t="s">
+      <c r="G125" t="s">
         <v>190</v>
       </c>
-      <c r="H118" s="1" t="s">
+      <c r="H125" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="I118" s="1" t="s">
+      <c r="I125" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="119" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D119" t="s">
+    <row r="126" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D126" t="s">
         <v>231</v>
       </c>
-      <c r="E119" t="s">
+      <c r="E126" t="s">
         <v>233</v>
       </c>
-      <c r="H119" s="1" t="s">
+      <c r="H126" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="120" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D120" t="s">
+    <row r="127" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D127" t="s">
         <v>232</v>
       </c>
-      <c r="E120" t="s">
+      <c r="E127" t="s">
         <v>234</v>
       </c>
-      <c r="H120" s="1"/>
-    </row>
-    <row r="121" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D121" t="s">
+      <c r="H127" s="1"/>
+    </row>
+    <row r="128" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D128" t="s">
         <v>205</v>
       </c>
-      <c r="E121" t="s">
+      <c r="E128" t="s">
         <v>206</v>
       </c>
-      <c r="F121" s="1" t="s">
+      <c r="F128" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="122" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D122" t="s">
+    <row r="129" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D129" t="s">
         <v>208</v>
       </c>
-      <c r="E122" t="s">
+      <c r="E129" t="s">
         <v>209</v>
       </c>
-      <c r="F122" t="s">
+      <c r="F129" t="s">
         <v>210</v>
       </c>
-      <c r="G122" t="s">
+      <c r="G129" t="s">
         <v>213</v>
       </c>
-      <c r="H122" s="1" t="s">
+      <c r="H129" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="I122" s="1" t="s">
+      <c r="I129" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="123" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D123" t="s">
+    <row r="130" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D130" t="s">
         <v>219</v>
       </c>
-      <c r="E123" t="s">
+      <c r="E130" t="s">
         <v>220</v>
       </c>
-      <c r="F123" s="1" t="s">
+      <c r="F130" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="124" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D124" t="s">
+    <row r="131" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D131" t="s">
         <v>223</v>
       </c>
-      <c r="E124" t="s">
+      <c r="E131" t="s">
         <v>222</v>
       </c>
-      <c r="F124" s="1" t="s">
+      <c r="F131" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="125" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D125" t="s">
+    <row r="132" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D132" t="s">
         <v>225</v>
       </c>
-      <c r="E125" t="s">
+      <c r="E132" t="s">
         <v>226</v>
       </c>
-      <c r="F125" s="1" t="s">
+      <c r="F132" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="126" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D126" t="s">
+    <row r="133" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D133" t="s">
         <v>228</v>
       </c>
-      <c r="E126" t="s">
+      <c r="E133" t="s">
         <v>229</v>
       </c>
-      <c r="F126" s="1" t="s">
+      <c r="F133" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="127" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D127" t="s">
+    <row r="134" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D134" t="s">
         <v>235</v>
       </c>
-      <c r="E127" t="s">
+      <c r="E134" t="s">
         <v>236</v>
       </c>
-      <c r="F127" s="1" t="s">
+      <c r="F134" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="128" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="E128" t="s">
+    <row r="135" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E135" t="s">
         <v>237</v>
       </c>
-      <c r="F128" s="1"/>
-    </row>
-    <row r="129" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D129" t="s">
+      <c r="F135" s="1"/>
+    </row>
+    <row r="136" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D136" t="s">
         <v>239</v>
       </c>
-      <c r="E129" s="1" t="s">
+      <c r="E136" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F129" s="1"/>
-    </row>
-    <row r="130" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D130" t="s">
+      <c r="F136" s="1"/>
+    </row>
+    <row r="137" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D137" t="s">
         <v>246</v>
       </c>
-      <c r="E130" t="s">
+      <c r="E137" t="s">
         <v>245</v>
       </c>
-      <c r="F130" s="1" t="s">
+      <c r="F137" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="131" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D131" t="s">
+    <row r="138" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D138" t="s">
         <v>247</v>
       </c>
-      <c r="F131" s="1" t="s">
+      <c r="F138" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="132" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D132" t="s">
+    <row r="139" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D139" t="s">
         <v>249</v>
       </c>
-      <c r="E132" t="s">
+      <c r="E139" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="133" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D133" t="s">
+    <row r="140" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D140" t="s">
         <v>251</v>
       </c>
-      <c r="F133" s="1" t="s">
+      <c r="F140" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="134" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D134" t="s">
+    <row r="141" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D141" t="s">
         <v>253</v>
       </c>
-      <c r="F134" s="1" t="s">
+      <c r="F141" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="135" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D135" t="s">
+    <row r="142" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D142" t="s">
         <v>272</v>
       </c>
-      <c r="F135" s="1" t="s">
+      <c r="F142" s="1" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="136" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D136" t="s">
+    <row r="143" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D143" t="s">
         <v>254</v>
       </c>
-      <c r="E136" t="s">
+      <c r="E143" t="s">
         <v>255</v>
       </c>
-      <c r="F136" s="1" t="s">
+      <c r="F143" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="137" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D137" t="s">
+    <row r="144" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D144" t="s">
         <v>257</v>
       </c>
-      <c r="E137" t="s">
+      <c r="E144" t="s">
         <v>258</v>
       </c>
-      <c r="F137" s="1" t="s">
+      <c r="F144" s="1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="138" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D138" t="s">
+    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D145" t="s">
         <v>261</v>
       </c>
-      <c r="F138" s="1" t="s">
+      <c r="F145" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="139" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D139" t="s">
+    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D146" t="s">
         <v>263</v>
       </c>
-      <c r="F139" s="1" t="s">
+      <c r="F146" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="140" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D140" t="s">
+    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D147" t="s">
         <v>265</v>
       </c>
-      <c r="E140" t="s">
+      <c r="E147" t="s">
         <v>264</v>
       </c>
-      <c r="F140" s="1" t="s">
+      <c r="F147" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="141" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E141" t="s">
+    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E148" t="s">
         <v>267</v>
       </c>
-      <c r="F141" s="1"/>
-    </row>
-    <row r="142" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D142" t="s">
+      <c r="F148" s="1"/>
+    </row>
+    <row r="149" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D149" t="s">
         <v>282</v>
       </c>
-      <c r="F142" s="1" t="s">
+      <c r="F149" s="1" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="143" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F143" s="1"/>
-    </row>
-    <row r="144" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F144" s="1"/>
-    </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F145" s="1"/>
-    </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F146" s="1"/>
-    </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F147" s="1"/>
-    </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B148" t="s">
+    <row r="150" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F150" s="1"/>
+    </row>
+    <row r="151" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F151" s="1"/>
+    </row>
+    <row r="152" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F152" s="1"/>
+    </row>
+    <row r="153" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F153" s="1"/>
+    </row>
+    <row r="154" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F154" s="1"/>
+    </row>
+    <row r="155" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B155" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C149" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D150" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D151" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="153" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C153" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D154" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="156" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C156" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="157" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D157" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="158" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D158" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="159" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D159" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="160" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D160" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="162" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C162" t="s">
-        <v>346</v>
+      <c r="C160" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="161" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D161" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="163" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D163" t="s">
-        <v>349</v>
-      </c>
-      <c r="E163" t="s">
-        <v>347</v>
-      </c>
-      <c r="F163" s="1" t="s">
-        <v>348</v>
+      <c r="C163" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="164" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D164" t="s">
-        <v>350</v>
-      </c>
-      <c r="E164" t="s">
-        <v>351</v>
-      </c>
-      <c r="F164" t="s">
-        <v>352</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="165" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D165" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="166" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C166" t="s">
-        <v>674</v>
+      <c r="D166" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="167" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D167" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="169" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C169" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="170" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D170" t="s">
+        <v>349</v>
+      </c>
+      <c r="E170" t="s">
+        <v>347</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="171" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D171" t="s">
+        <v>350</v>
+      </c>
+      <c r="E171" t="s">
+        <v>351</v>
+      </c>
+      <c r="F171" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="173" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C173" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="174" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D174" t="s">
         <v>675</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E174" t="s">
         <v>676</v>
       </c>
-      <c r="F167" s="1" t="s">
+      <c r="F174" s="1" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="168" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D168" t="s">
+    <row r="175" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D175" t="s">
         <v>677</v>
       </c>
-      <c r="E168" t="s">
+      <c r="E175" t="s">
         <v>678</v>
-      </c>
-    </row>
-    <row r="169" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D169" t="s">
-        <v>679</v>
-      </c>
-      <c r="E169" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="171" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C171" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="172" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D172" t="s">
-        <v>354</v>
-      </c>
-      <c r="E172" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="173" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D173" t="s">
-        <v>355</v>
-      </c>
-      <c r="E173" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="175" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C175" t="s">
-        <v>369</v>
-      </c>
-      <c r="F175" s="1" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="176" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D176" t="s">
+        <v>679</v>
+      </c>
+      <c r="E176" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="178" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C178" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="179" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D179" t="s">
+        <v>354</v>
+      </c>
+      <c r="E179" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="180" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D180" t="s">
+        <v>355</v>
+      </c>
+      <c r="E180" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="182" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C182" t="s">
+        <v>369</v>
+      </c>
+      <c r="F182" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="183" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D183" t="s">
         <v>370</v>
       </c>
-      <c r="E176" t="s">
+      <c r="E183" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="177" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D177" t="s">
+    <row r="184" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D184" t="s">
         <v>372</v>
       </c>
-      <c r="E177" t="s">
+      <c r="E184" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="178" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D178" t="s">
+    <row r="185" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D185" t="s">
         <v>374</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E185" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="179" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D179" t="s">
+    <row r="186" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D186" t="s">
         <v>376</v>
       </c>
-      <c r="E179" t="s">
+      <c r="E186" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="180" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D180" t="s">
+    <row r="187" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D187" t="s">
         <v>385</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E187" t="s">
         <v>386</v>
       </c>
-      <c r="F180" s="1" t="s">
+      <c r="F187" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="181" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D181" t="s">
+    <row r="188" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D188" t="s">
         <v>388</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E188" t="s">
         <v>389</v>
       </c>
-      <c r="F181" s="1" t="s">
+      <c r="F188" s="1" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="183" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C183" t="s">
+    <row r="190" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C190" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="184" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D184" t="s">
+    <row r="191" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D191" t="s">
         <v>380</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E191" t="s">
         <v>381</v>
       </c>
-      <c r="F184" t="s">
+      <c r="F191" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="185" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D185" t="s">
+    <row r="192" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D192" t="s">
         <v>808</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E192" t="s">
         <v>382</v>
       </c>
-      <c r="F185" t="s">
+      <c r="F192" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="186" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D186" t="s">
-        <v>759</v>
-      </c>
-      <c r="E186" t="s">
-        <v>760</v>
-      </c>
-      <c r="G186" s="1" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="187" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="F187" s="1"/>
-    </row>
-    <row r="188" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C188" t="s">
-        <v>391</v>
-      </c>
-      <c r="D188" t="s">
-        <v>419</v>
-      </c>
-      <c r="E188" t="s">
-        <v>392</v>
-      </c>
-      <c r="F188" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G188" s="1" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="189" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D189" t="s">
-        <v>420</v>
-      </c>
-      <c r="E189" t="s">
-        <v>421</v>
-      </c>
-      <c r="F189" s="1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="190" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D190" t="s">
-        <v>423</v>
-      </c>
-      <c r="E190" t="s">
-        <v>424</v>
-      </c>
-      <c r="F190" s="1"/>
-    </row>
-    <row r="191" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C191" t="s">
-        <v>393</v>
-      </c>
-      <c r="F191" s="1"/>
-    </row>
-    <row r="192" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D192" t="s">
-        <v>395</v>
-      </c>
-      <c r="E192" t="s">
-        <v>394</v>
-      </c>
-      <c r="F192" s="1"/>
     </row>
     <row r="193" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D193" t="s">
-        <v>396</v>
-      </c>
-      <c r="F193" t="s">
-        <v>397</v>
+        <v>759</v>
+      </c>
+      <c r="E193" t="s">
+        <v>760</v>
       </c>
       <c r="G193" s="1" t="s">
-        <v>398</v>
+        <v>761</v>
       </c>
     </row>
     <row r="194" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C194" t="s">
-        <v>415</v>
-      </c>
-      <c r="G194" s="1"/>
+      <c r="F194" s="1"/>
     </row>
     <row r="195" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C195" t="s">
+        <v>391</v>
+      </c>
+      <c r="D195" t="s">
+        <v>419</v>
+      </c>
       <c r="E195" t="s">
-        <v>416</v>
+        <v>392</v>
       </c>
       <c r="F195" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="G195" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="G195" s="1" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="196" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D196" t="s">
+        <v>420</v>
+      </c>
       <c r="E196" t="s">
-        <v>417</v>
+        <v>421</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="197" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C197" t="s">
-        <v>430</v>
-      </c>
+      <c r="D197" t="s">
+        <v>423</v>
+      </c>
+      <c r="E197" t="s">
+        <v>424</v>
+      </c>
+      <c r="F197" s="1"/>
     </row>
     <row r="198" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D198" t="s">
-        <v>431</v>
-      </c>
-      <c r="E198" t="s">
-        <v>433</v>
-      </c>
-      <c r="F198" s="1" t="s">
-        <v>435</v>
-      </c>
+      <c r="C198" t="s">
+        <v>393</v>
+      </c>
+      <c r="F198" s="1"/>
     </row>
     <row r="199" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D199" t="s">
-        <v>432</v>
+        <v>395</v>
       </c>
       <c r="E199" t="s">
-        <v>434</v>
-      </c>
+        <v>394</v>
+      </c>
+      <c r="F199" s="1"/>
     </row>
     <row r="200" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C200" t="s">
-        <v>754</v>
+      <c r="D200" t="s">
+        <v>396</v>
+      </c>
+      <c r="F200" t="s">
+        <v>397</v>
+      </c>
+      <c r="G200" s="1" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="201" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D201" t="s">
-        <v>757</v>
-      </c>
-      <c r="E201" t="s">
-        <v>756</v>
-      </c>
-      <c r="F201" s="1" t="s">
-        <v>758</v>
-      </c>
+      <c r="C201" t="s">
+        <v>415</v>
+      </c>
+      <c r="G201" s="1"/>
     </row>
     <row r="202" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E202" t="s">
+        <v>416</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="G202" s="1"/>
+    </row>
+    <row r="203" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E203" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="204" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C204" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="205" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D205" t="s">
+        <v>431</v>
+      </c>
+      <c r="E205" t="s">
+        <v>433</v>
+      </c>
+      <c r="F205" s="1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="206" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D206" t="s">
+        <v>432</v>
+      </c>
+      <c r="E206" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="207" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C207" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="208" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D208" t="s">
+        <v>757</v>
+      </c>
+      <c r="E208" t="s">
+        <v>756</v>
+      </c>
+      <c r="F208" s="1" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="209" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E209" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="203" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C203" t="s">
+    <row r="210" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C210" t="s">
         <v>809</v>
       </c>
     </row>
-    <row r="204" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D204" t="s">
+    <row r="211" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D211" t="s">
         <v>811</v>
       </c>
-      <c r="E204" t="s">
+      <c r="E211" t="s">
         <v>810</v>
       </c>
-      <c r="F204" s="1" t="s">
+      <c r="F211" s="1" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="210" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B210" t="s">
+    <row r="217" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B217" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C211" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="212" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D212" t="s">
-        <v>170</v>
-      </c>
-      <c r="E212" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="213" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D213" t="s">
-        <v>174</v>
-      </c>
-      <c r="E213" t="s">
-        <v>172</v>
-      </c>
-      <c r="F213" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="214" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C214" t="s">
-        <v>321</v>
-      </c>
-      <c r="E214" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="F214" s="1"/>
-    </row>
-    <row r="215" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C215" t="s">
-        <v>404</v>
-      </c>
-      <c r="D215" t="s">
-        <v>405</v>
-      </c>
-      <c r="E215" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="F215" s="1"/>
-    </row>
-    <row r="216" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D216" t="s">
-        <v>406</v>
-      </c>
-      <c r="F216" s="1"/>
-    </row>
-    <row r="217" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F217" s="1"/>
     </row>
     <row r="218" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C218" t="s">
-        <v>615</v>
-      </c>
-      <c r="D218" t="s">
-        <v>616</v>
-      </c>
-      <c r="F218" s="1" t="s">
-        <v>617</v>
+        <v>169</v>
       </c>
     </row>
     <row r="219" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C219" t="s">
-        <v>619</v>
-      </c>
       <c r="D219" t="s">
-        <v>618</v>
-      </c>
-      <c r="F219" s="1" t="s">
-        <v>620</v>
+        <v>170</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="220" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F220" s="1"/>
+      <c r="D220" t="s">
+        <v>174</v>
+      </c>
+      <c r="E220" t="s">
+        <v>172</v>
+      </c>
+      <c r="F220" s="1" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="221" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C221" t="s">
+        <v>321</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="F221" s="1"/>
     </row>
     <row r="222" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B222" t="s">
-        <v>682</v>
+      <c r="C222" t="s">
+        <v>404</v>
+      </c>
+      <c r="D222" t="s">
+        <v>405</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>407</v>
       </c>
       <c r="F222" s="1"/>
     </row>
     <row r="223" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C223" t="s">
-        <v>683</v>
-      </c>
       <c r="D223" t="s">
-        <v>685</v>
-      </c>
-      <c r="F223" s="1" t="s">
-        <v>687</v>
-      </c>
+        <v>406</v>
+      </c>
+      <c r="F223" s="1"/>
     </row>
     <row r="224" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C224" t="s">
-        <v>684</v>
-      </c>
-      <c r="D224" t="s">
-        <v>686</v>
-      </c>
       <c r="F224" s="1"/>
     </row>
     <row r="225" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C225" t="s">
-        <v>688</v>
+        <v>615</v>
       </c>
       <c r="D225" t="s">
-        <v>689</v>
-      </c>
-      <c r="F225" s="1"/>
+        <v>616</v>
+      </c>
+      <c r="F225" s="1" t="s">
+        <v>617</v>
+      </c>
     </row>
     <row r="226" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C226" t="s">
-        <v>703</v>
+        <v>619</v>
       </c>
       <c r="D226" t="s">
-        <v>704</v>
+        <v>618</v>
       </c>
       <c r="F226" s="1" t="s">
-        <v>705</v>
+        <v>620</v>
       </c>
     </row>
     <row r="227" spans="2:6" x14ac:dyDescent="0.2">
@@ -4567,1678 +4572,1730 @@
       <c r="F228" s="1"/>
     </row>
     <row r="229" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B229" t="s">
+        <v>682</v>
+      </c>
       <c r="F229" s="1"/>
     </row>
     <row r="230" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F230" s="1"/>
+      <c r="C230" t="s">
+        <v>683</v>
+      </c>
+      <c r="D230" t="s">
+        <v>685</v>
+      </c>
+      <c r="F230" s="1" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="231" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C231" t="s">
+        <v>684</v>
+      </c>
+      <c r="D231" t="s">
+        <v>686</v>
+      </c>
+      <c r="F231" s="1"/>
     </row>
     <row r="232" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B232" t="s">
-        <v>446</v>
-      </c>
+      <c r="C232" t="s">
+        <v>688</v>
+      </c>
+      <c r="D232" t="s">
+        <v>689</v>
+      </c>
+      <c r="F232" s="1"/>
     </row>
     <row r="233" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C233" t="s">
+        <v>703</v>
+      </c>
+      <c r="D233" t="s">
+        <v>704</v>
+      </c>
+      <c r="F233" s="1" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="234" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F234" s="1"/>
+    </row>
+    <row r="235" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F235" s="1"/>
+    </row>
+    <row r="236" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F236" s="1"/>
+    </row>
+    <row r="237" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F237" s="1"/>
+    </row>
+    <row r="239" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B239" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="240" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C240" t="s">
         <v>613</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D240" t="s">
         <v>612</v>
       </c>
-      <c r="F233" s="1" t="s">
+      <c r="F240" s="1" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="234" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C234" t="s">
+    <row r="241" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C241" t="s">
         <v>621</v>
       </c>
-      <c r="D234" t="s">
+      <c r="D241" t="s">
         <v>622</v>
       </c>
-      <c r="F234" s="1" t="s">
+      <c r="F241" s="1" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="235" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C235" t="s">
+    <row r="242" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C242" t="s">
         <v>625</v>
       </c>
-      <c r="D235" t="s">
+      <c r="D242" t="s">
         <v>624</v>
       </c>
-      <c r="F235" s="1" t="s">
+      <c r="F242" s="1" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="236" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C236" t="s">
+    <row r="243" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C243" t="s">
         <v>628</v>
       </c>
-      <c r="D236" t="s">
+      <c r="D243" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="243" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B243" t="s">
+    <row r="250" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B250" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="244" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C244" t="s">
+    <row r="251" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C251" t="s">
         <v>175</v>
       </c>
-      <c r="D244" s="1" t="s">
+      <c r="D251" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="245" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C245" t="s">
+    <row r="252" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C252" t="s">
         <v>177</v>
       </c>
-      <c r="D245" s="1" t="s">
+      <c r="D252" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="246" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C246" t="s">
+    <row r="253" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C253" t="s">
         <v>292</v>
       </c>
-      <c r="D246" s="1" t="s">
+      <c r="D253" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="247" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C247" t="s">
+    <row r="254" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C254" t="s">
         <v>293</v>
       </c>
-      <c r="D247" s="1" t="s">
+      <c r="D254" s="1" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="248" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C248" t="s">
+    <row r="255" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C255" t="s">
         <v>296</v>
       </c>
-      <c r="D248" s="1" t="s">
+      <c r="D255" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="249" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D249" s="1"/>
-    </row>
-    <row r="250" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D250" s="1"/>
-    </row>
-    <row r="251" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B251" t="s">
+    <row r="256" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D256" s="1"/>
+    </row>
+    <row r="257" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D257" s="1"/>
+    </row>
+    <row r="258" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B258" t="s">
         <v>342</v>
       </c>
-      <c r="D251" s="1"/>
-    </row>
-    <row r="252" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C252" t="s">
+      <c r="D258" s="1"/>
+    </row>
+    <row r="259" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C259" t="s">
         <v>343</v>
       </c>
-      <c r="D252" t="s">
+      <c r="D259" t="s">
         <v>368</v>
       </c>
-      <c r="E252" s="1" t="s">
+      <c r="E259" s="1" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="253" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D253" t="s">
+    <row r="260" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D260" t="s">
         <v>367</v>
       </c>
-      <c r="E253" s="1" t="s">
+      <c r="E260" s="1" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="254" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D254" s="1"/>
-    </row>
-    <row r="255" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D255" s="1"/>
-    </row>
-    <row r="256" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D256" s="1"/>
-    </row>
-    <row r="260" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B260" t="s">
+    <row r="261" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D261" s="1"/>
+    </row>
+    <row r="262" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D262" s="1"/>
+    </row>
+    <row r="263" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D263" s="1"/>
+    </row>
+    <row r="267" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B267" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="261" spans="2:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="C261" s="4" t="s">
+    <row r="268" spans="2:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="C268" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="D261" s="2" t="s">
+      <c r="D268" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E261" s="1" t="s">
+      <c r="E268" s="1" t="s">
         <v>185</v>
-      </c>
-    </row>
-    <row r="262" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C262" t="s">
-        <v>186</v>
-      </c>
-      <c r="E262" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="263" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C263" t="s">
-        <v>214</v>
-      </c>
-      <c r="E263" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="265" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D265" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="267" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C267" t="s">
-        <v>241</v>
-      </c>
-      <c r="D267" t="s">
-        <v>242</v>
-      </c>
-      <c r="E267" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="268" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C268" t="s">
-        <v>268</v>
-      </c>
-      <c r="D268" t="s">
-        <v>269</v>
-      </c>
-      <c r="E268" s="1" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="269" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C269" t="s">
-        <v>283</v>
+        <v>186</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>284</v>
+        <v>187</v>
       </c>
     </row>
     <row r="270" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C270" t="s">
+        <v>214</v>
+      </c>
       <c r="E270" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="271" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E271" s="1" t="s">
-        <v>286</v>
+        <v>188</v>
       </c>
     </row>
     <row r="272" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C272" t="s">
-        <v>287</v>
-      </c>
-      <c r="E272" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="273" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C273" t="s">
-        <v>298</v>
-      </c>
-      <c r="E273" s="1" t="s">
-        <v>297</v>
+      <c r="D272" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="274" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E274" s="1"/>
+      <c r="C274" t="s">
+        <v>241</v>
+      </c>
+      <c r="D274" t="s">
+        <v>242</v>
+      </c>
+      <c r="E274" s="1" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="275" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C275" t="s">
-        <v>358</v>
+        <v>268</v>
       </c>
       <c r="D275" t="s">
-        <v>359</v>
+        <v>269</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>360</v>
+        <v>270</v>
       </c>
     </row>
     <row r="276" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E276" s="1"/>
+      <c r="C276" t="s">
+        <v>283</v>
+      </c>
+      <c r="E276" s="1" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="277" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E277" s="1"/>
+      <c r="E277" s="1" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="278" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E278" s="1"/>
+      <c r="E278" s="1" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="279" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E279" s="1"/>
+      <c r="C279" t="s">
+        <v>287</v>
+      </c>
+      <c r="E279" s="1" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="280" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E280" s="1"/>
+      <c r="C280" t="s">
+        <v>298</v>
+      </c>
+      <c r="E280" s="1" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="281" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E281" s="1"/>
     </row>
     <row r="282" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E282" s="1"/>
+      <c r="C282" t="s">
+        <v>358</v>
+      </c>
+      <c r="D282" t="s">
+        <v>359</v>
+      </c>
+      <c r="E282" s="1" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="283" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E283" s="1"/>
     </row>
     <row r="284" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C284" t="s">
+      <c r="E284" s="1"/>
+    </row>
+    <row r="285" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E285" s="1"/>
+    </row>
+    <row r="286" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E286" s="1"/>
+    </row>
+    <row r="287" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E287" s="1"/>
+    </row>
+    <row r="288" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E288" s="1"/>
+    </row>
+    <row r="289" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E289" s="1"/>
+    </row>
+    <row r="290" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E290" s="1"/>
+    </row>
+    <row r="291" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C291" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="285" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D285" t="s">
+    <row r="292" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D292" t="s">
         <v>134</v>
       </c>
-      <c r="E285" t="s">
+      <c r="E292" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="286" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D286" t="s">
+    <row r="293" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D293" t="s">
         <v>135</v>
       </c>
-      <c r="E286" t="s">
+      <c r="E293" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="287" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D287" t="s">
-        <v>139</v>
-      </c>
-      <c r="E287" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="288" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D288" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="289" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D289" t="s">
-        <v>141</v>
-      </c>
-      <c r="E289" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="290" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D290" t="s">
-        <v>482</v>
-      </c>
-      <c r="E290" t="s">
-        <v>484</v>
-      </c>
-      <c r="F290" t="s">
-        <v>488</v>
-      </c>
-      <c r="G290" t="s">
-        <v>483</v>
-      </c>
-      <c r="H290" s="1" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="291" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D291" t="s">
-        <v>485</v>
-      </c>
-      <c r="E291" t="s">
-        <v>486</v>
-      </c>
-      <c r="G291" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="293" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C293" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="294" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D294" t="s">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="E294" t="s">
-        <v>73</v>
-      </c>
-      <c r="F294" s="1" t="s">
-        <v>74</v>
+        <v>140</v>
       </c>
     </row>
     <row r="295" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D295" t="s">
-        <v>75</v>
-      </c>
-      <c r="E295" s="1" t="s">
-        <v>76</v>
+        <v>136</v>
       </c>
     </row>
     <row r="296" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D296" t="s">
-        <v>77</v>
-      </c>
-      <c r="E296" s="1" t="s">
-        <v>78</v>
+        <v>141</v>
+      </c>
+      <c r="E296" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="297" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D297" t="s">
-        <v>80</v>
-      </c>
-      <c r="E297" s="1" t="s">
-        <v>79</v>
+        <v>482</v>
+      </c>
+      <c r="E297" t="s">
+        <v>484</v>
+      </c>
+      <c r="F297" t="s">
+        <v>488</v>
+      </c>
+      <c r="G297" t="s">
+        <v>483</v>
+      </c>
+      <c r="H297" s="1" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="298" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D298" t="s">
-        <v>361</v>
+        <v>485</v>
       </c>
       <c r="E298" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="299" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D299" t="s">
-        <v>362</v>
-      </c>
-      <c r="E299" t="s">
-        <v>363</v>
+        <v>486</v>
+      </c>
+      <c r="G298" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="300" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C300" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="301" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D301" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E301" t="s">
-        <v>82</v>
+        <v>73</v>
+      </c>
+      <c r="F301" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="302" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D302" t="s">
+        <v>75</v>
+      </c>
+      <c r="E302" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="303" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D303" t="s">
+        <v>77</v>
+      </c>
+      <c r="E303" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="304" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D304" t="s">
+        <v>80</v>
+      </c>
+      <c r="E304" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="305" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D305" t="s">
+        <v>361</v>
+      </c>
+      <c r="E305" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="306" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D306" t="s">
+        <v>362</v>
+      </c>
+      <c r="E306" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="308" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D308" t="s">
+        <v>81</v>
+      </c>
+      <c r="E308" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="309" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D309" t="s">
         <v>83</v>
       </c>
-      <c r="E302" t="s">
+      <c r="E309" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="304" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C304" t="s">
+    <row r="311" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C311" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="305" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D305" t="s">
+    <row r="312" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D312" t="s">
         <v>72</v>
       </c>
-      <c r="E305" t="s">
+      <c r="E312" t="s">
         <v>130</v>
       </c>
-      <c r="F305" s="1"/>
-    </row>
-    <row r="306" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D306" t="s">
+      <c r="F312" s="1"/>
+    </row>
+    <row r="313" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D313" t="s">
         <v>146</v>
       </c>
-      <c r="E306" s="1" t="s">
+      <c r="E313" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F306" s="1"/>
-    </row>
-    <row r="307" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D307" t="s">
+      <c r="F313" s="1"/>
+    </row>
+    <row r="314" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D314" t="s">
         <v>75</v>
       </c>
-      <c r="E307" s="1" t="s">
+      <c r="E314" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="308" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E308" s="1"/>
-    </row>
-    <row r="309" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D309" t="s">
+    <row r="315" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E315" s="1"/>
+    </row>
+    <row r="316" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D316" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="310" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E310" t="s">
+    <row r="317" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E317" t="s">
         <v>150</v>
       </c>
-      <c r="F310" t="s">
+      <c r="F317" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="311" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E311" t="s">
+    <row r="318" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E318" t="s">
         <v>151</v>
       </c>
-      <c r="F311" t="s">
+      <c r="F318" t="s">
         <v>144</v>
       </c>
-      <c r="G311" s="1" t="s">
+      <c r="G318" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="312" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D312" t="s">
+    <row r="319" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D319" t="s">
         <v>152</v>
       </c>
-      <c r="E312" s="1" t="s">
+      <c r="E319" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G312" s="1"/>
-    </row>
-    <row r="326" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E326" s="1"/>
-    </row>
-    <row r="328" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B328" t="s">
+      <c r="G319" s="1"/>
+    </row>
+    <row r="333" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E333" s="1"/>
+    </row>
+    <row r="335" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B335" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="329" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C329" t="s">
+    <row r="336" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C336" t="s">
         <v>276</v>
       </c>
-      <c r="D329" t="s">
+      <c r="D336" t="s">
         <v>278</v>
       </c>
-      <c r="E329" s="1" t="s">
+      <c r="E336" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="330" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C330" t="s">
+    <row r="337" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C337" t="s">
         <v>280</v>
       </c>
-      <c r="E330" s="1" t="s">
+      <c r="E337" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="F330" s="1" t="s">
+      <c r="F337" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="G330" s="1" t="s">
+      <c r="G337" s="1" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="331" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C331" t="s">
+    <row r="338" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C338" t="s">
         <v>289</v>
       </c>
-      <c r="E331" s="1" t="s">
+      <c r="E338" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="332" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C332" t="s">
+    <row r="339" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C339" t="s">
         <v>303</v>
       </c>
-      <c r="E332" s="1" t="s">
+      <c r="E339" s="1" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="333" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D333" t="s">
+    <row r="340" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D340" t="s">
         <v>305</v>
       </c>
-      <c r="E333" s="1" t="s">
+      <c r="E340" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="334" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C334" t="s">
+    <row r="341" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C341" t="s">
         <v>323</v>
       </c>
-      <c r="E334" s="1" t="s">
+      <c r="E341" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="335" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C335" t="s">
+    <row r="342" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C342" t="s">
         <v>307</v>
       </c>
-      <c r="D335" t="s">
+      <c r="D342" t="s">
         <v>308</v>
       </c>
-      <c r="E335" s="1" t="s">
+      <c r="E342" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="336" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C336" t="s">
+    <row r="343" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C343" t="s">
         <v>310</v>
       </c>
-      <c r="E336" s="1" t="s">
+      <c r="E343" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="337" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C337" t="s">
+    <row r="344" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C344" t="s">
         <v>315</v>
       </c>
-      <c r="E337" s="1" t="s">
+      <c r="E344" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="338" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C338" t="s">
+    <row r="345" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C345" t="s">
         <v>316</v>
       </c>
-      <c r="E338" s="1" t="s">
+      <c r="E345" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="339" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C339" t="s">
+    <row r="346" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C346" t="s">
         <v>318</v>
       </c>
-      <c r="E339" s="1" t="s">
+      <c r="E346" s="1" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="340" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C340" t="s">
+    <row r="347" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C347" t="s">
         <v>325</v>
       </c>
-      <c r="D340" t="s">
+      <c r="D347" t="s">
         <v>332</v>
       </c>
-      <c r="E340" s="1" t="s">
+      <c r="E347" s="1" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="341" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D341" t="s">
+    <row r="348" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D348" t="s">
         <v>327</v>
       </c>
-      <c r="E341" s="1" t="s">
+      <c r="E348" s="1" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="343" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C343" t="s">
+    <row r="350" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C350" t="s">
         <v>329</v>
       </c>
-      <c r="D343" t="s">
+      <c r="D350" t="s">
         <v>330</v>
       </c>
-      <c r="E343" s="1" t="s">
+      <c r="E350" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="345" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C345" t="s">
+    <row r="352" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C352" t="s">
         <v>335</v>
       </c>
-      <c r="D345" t="s">
+      <c r="D352" t="s">
         <v>337</v>
       </c>
-      <c r="E345" s="1" t="s">
+      <c r="E352" s="1" t="s">
         <v>336</v>
-      </c>
-    </row>
-    <row r="349" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B349" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="350" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C350" t="s">
-        <v>341</v>
-      </c>
-      <c r="D350" t="s">
-        <v>339</v>
-      </c>
-      <c r="E350" s="1" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="356" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B356" t="s">
-        <v>85</v>
+        <v>338</v>
       </c>
     </row>
     <row r="357" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C357" t="s">
+        <v>341</v>
+      </c>
+      <c r="D357" t="s">
+        <v>339</v>
+      </c>
+      <c r="E357" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="363" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B363" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="364" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C364" t="s">
         <v>86</v>
       </c>
-      <c r="D357" t="s">
+      <c r="D364" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="358" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C358" t="s">
+    <row r="365" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C365" t="s">
         <v>88</v>
       </c>
-      <c r="D358" t="s">
+      <c r="D365" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="359" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C359" t="s">
+    <row r="366" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C366" t="s">
         <v>95</v>
       </c>
-      <c r="D359" s="1" t="s">
+      <c r="D366" s="1" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="360" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C360" t="s">
-        <v>97</v>
-      </c>
-      <c r="D360" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="362" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B362" t="s">
-        <v>90</v>
-      </c>
-      <c r="C362" t="s">
-        <v>91</v>
-      </c>
-      <c r="D362" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="363" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C363" t="s">
-        <v>93</v>
-      </c>
-      <c r="D363" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="366" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B366" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="367" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C367" t="s">
+        <v>97</v>
+      </c>
+      <c r="D367" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="369" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B369" t="s">
+        <v>90</v>
+      </c>
+      <c r="C369" t="s">
+        <v>91</v>
+      </c>
+      <c r="D369" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="370" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C370" t="s">
+        <v>93</v>
+      </c>
+      <c r="D370" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="373" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B373" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="374" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C374" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="368" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D368" t="s">
+    <row r="375" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D375" t="s">
         <v>104</v>
       </c>
-      <c r="E368" s="1" t="s">
+      <c r="E375" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="369" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D369" t="s">
+    <row r="376" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D376" t="s">
         <v>101</v>
       </c>
-      <c r="E369" s="1" t="s">
+      <c r="E376" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="370" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D370" t="s">
+    <row r="377" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D377" t="s">
         <v>102</v>
       </c>
-      <c r="E370" s="1" t="s">
+      <c r="E377" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="371" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D371" t="s">
+    <row r="378" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D378" t="s">
         <v>107</v>
       </c>
-      <c r="E371" t="s">
+      <c r="E378" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="373" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B373" t="s">
+    <row r="380" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B380" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="374" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C374" t="s">
+    <row r="381" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C381" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="375" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D375" t="s">
+    <row r="382" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D382" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="376" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D376" t="s">
+    <row r="383" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D383" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="377" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F377" s="1" t="s">
+    <row r="384" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F384" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="378" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B378" t="s">
+    <row r="385" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B385" t="s">
         <v>1</v>
       </c>
-      <c r="F378" s="1" t="s">
+      <c r="F385" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="379" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C379" t="s">
+    <row r="386" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C386" t="s">
         <v>112</v>
       </c>
-      <c r="D379" s="1" t="s">
+      <c r="D386" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="380" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D380" t="s">
+    <row r="387" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D387" t="s">
         <v>126</v>
       </c>
-      <c r="E380" s="1" t="s">
+      <c r="E387" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="381" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C381" t="s">
+    <row r="388" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C388" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="382" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D382" t="s">
-        <v>115</v>
-      </c>
-      <c r="E382" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F382" t="s">
-        <v>128</v>
-      </c>
-      <c r="G382" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="383" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E383" t="s">
-        <v>121</v>
-      </c>
-      <c r="G383" s="1"/>
-    </row>
-    <row r="384" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E384" t="s">
-        <v>124</v>
-      </c>
-      <c r="G384" s="1"/>
-    </row>
-    <row r="385" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D385" t="s">
-        <v>117</v>
-      </c>
-      <c r="E385" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G385" s="1"/>
-    </row>
-    <row r="386" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D386" t="s">
-        <v>119</v>
-      </c>
-      <c r="E386" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G386" s="1"/>
-    </row>
-    <row r="387" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E387" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="G387" s="1"/>
-    </row>
-    <row r="388" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E388" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="389" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D389" t="s">
+        <v>115</v>
+      </c>
+      <c r="E389" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F389" t="s">
+        <v>128</v>
+      </c>
+      <c r="G389" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="390" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E390" t="s">
+        <v>121</v>
+      </c>
+      <c r="G390" s="1"/>
+    </row>
+    <row r="391" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E391" t="s">
+        <v>124</v>
+      </c>
+      <c r="G391" s="1"/>
+    </row>
+    <row r="392" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D392" t="s">
+        <v>117</v>
+      </c>
+      <c r="E392" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G392" s="1"/>
+    </row>
+    <row r="393" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D393" t="s">
+        <v>119</v>
+      </c>
+      <c r="E393" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G393" s="1"/>
+    </row>
+    <row r="394" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E394" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="G394" s="1"/>
+    </row>
+    <row r="395" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E395" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="396" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D396" t="s">
         <v>301</v>
       </c>
-      <c r="E389" s="1" t="s">
+      <c r="E396" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="390" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D390" t="s">
+    <row r="397" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D397" t="s">
         <v>300</v>
       </c>
-      <c r="E390" s="1" t="s">
+      <c r="E397" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="395" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C395" t="s">
+    <row r="402" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C402" t="s">
         <v>131</v>
       </c>
-      <c r="D395" s="1" t="s">
+      <c r="D402" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="399" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B399" t="s">
+    <row r="406" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B406" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="400" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C400" t="s">
+    <row r="407" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C407" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="401" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D401" t="s">
+    <row r="408" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D408" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="402" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E402" t="s">
+    <row r="409" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E409" t="s">
         <v>492</v>
       </c>
-      <c r="F402" s="1" t="s">
+      <c r="F409" s="1" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="403" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E403" t="s">
+    <row r="410" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E410" t="s">
         <v>494</v>
       </c>
-      <c r="F403" s="1" t="s">
+      <c r="F410" s="1" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="404" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E404" t="s">
+    <row r="411" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E411" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="405" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D405" t="s">
+    <row r="412" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D412" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="406" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E406" t="s">
+    <row r="413" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E413" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="407" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E407" t="s">
+    <row r="414" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E414" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="408" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D408" t="s">
+    <row r="415" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D415" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="409" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E409" t="s">
+    <row r="416" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E416" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="410" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C410" t="s">
+    <row r="417" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C417" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="411" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D411" t="s">
+    <row r="418" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D418" t="s">
         <v>503</v>
       </c>
-      <c r="E411" t="s">
+      <c r="E418" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="412" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D412" t="s">
+    <row r="419" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D419" t="s">
         <v>501</v>
       </c>
-      <c r="E412" t="s">
+      <c r="E419" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="414" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C414" t="s">
+    <row r="421" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C421" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="415" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D415" t="s">
+    <row r="422" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D422" t="s">
         <v>508</v>
       </c>
-      <c r="E415" t="s">
+      <c r="E422" t="s">
         <v>506</v>
-      </c>
-    </row>
-    <row r="416" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D416" t="s">
-        <v>509</v>
-      </c>
-      <c r="E416" t="s">
-        <v>507</v>
-      </c>
-      <c r="G416" s="1" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="418" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C418" t="s">
-        <v>512</v>
-      </c>
-      <c r="G418" s="1" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="420" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C420" t="s">
-        <v>513</v>
-      </c>
-      <c r="E420" t="s">
-        <v>514</v>
-      </c>
-      <c r="G420" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="422" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C422" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="423" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D423" t="s">
+        <v>509</v>
+      </c>
+      <c r="E423" t="s">
+        <v>507</v>
+      </c>
+      <c r="G423" s="1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="425" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C425" t="s">
+        <v>512</v>
+      </c>
+      <c r="G425" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="427" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C427" t="s">
+        <v>513</v>
+      </c>
+      <c r="E427" t="s">
+        <v>514</v>
+      </c>
+      <c r="G427" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="429" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C429" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="430" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D430" t="s">
         <v>518</v>
       </c>
-      <c r="E423" t="s">
+      <c r="E430" t="s">
         <v>517</v>
       </c>
-      <c r="G423" s="1" t="s">
+      <c r="G430" s="1" t="s">
         <v>521</v>
-      </c>
-    </row>
-    <row r="424" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D424" t="s">
-        <v>519</v>
-      </c>
-      <c r="E424" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="426" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C426" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="427" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D427" t="s">
-        <v>528</v>
-      </c>
-      <c r="E427" t="s">
-        <v>524</v>
-      </c>
-      <c r="G427" s="1" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="428" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D428" t="s">
-        <v>526</v>
-      </c>
-      <c r="E428" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="429" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D429" t="s">
-        <v>527</v>
-      </c>
-      <c r="E429" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="430" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C430" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="431" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D431" t="s">
-        <v>630</v>
+        <v>519</v>
       </c>
       <c r="E431" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="432" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D432" t="s">
-        <v>632</v>
-      </c>
-      <c r="E432" t="s">
-        <v>633</v>
+        <v>520</v>
       </c>
     </row>
     <row r="433" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D433" t="s">
-        <v>634</v>
-      </c>
-      <c r="E433" t="s">
-        <v>635</v>
+      <c r="C433" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="434" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D434" t="s">
-        <v>637</v>
+        <v>528</v>
       </c>
       <c r="E434" t="s">
-        <v>636</v>
+        <v>524</v>
+      </c>
+      <c r="G434" s="1" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="435" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D435" t="s">
+        <v>526</v>
+      </c>
+      <c r="E435" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="436" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D436" t="s">
+        <v>527</v>
+      </c>
+      <c r="E436" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="437" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C437" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="438" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D438" t="s">
+        <v>630</v>
+      </c>
+      <c r="E438" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="439" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D439" t="s">
+        <v>632</v>
+      </c>
+      <c r="E439" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="440" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D440" t="s">
+        <v>634</v>
+      </c>
+      <c r="E440" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="441" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D441" t="s">
+        <v>637</v>
+      </c>
+      <c r="E441" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="442" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D442" t="s">
         <v>693</v>
       </c>
-      <c r="E435" t="s">
+      <c r="E442" t="s">
         <v>695</v>
       </c>
-      <c r="G435" s="1" t="s">
+      <c r="G442" s="1" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="438" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B438" t="s">
+    <row r="445" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B445" t="s">
         <v>778</v>
       </c>
     </row>
-    <row r="439" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C439" t="s">
+    <row r="446" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C446" t="s">
         <v>779</v>
       </c>
-      <c r="G439" s="1" t="s">
+      <c r="G446" s="1" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="448" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B448" t="s">
+    <row r="455" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B455" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="449" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C449" t="s">
+    <row r="456" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C456" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="450" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D450" t="s">
+    <row r="457" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D457" t="s">
         <v>541</v>
       </c>
-      <c r="G450" s="1" t="s">
+      <c r="G457" s="1" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="451" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C451" t="s">
+    <row r="458" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C458" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="452" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D452" t="s">
+    <row r="459" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D459" t="s">
         <v>543</v>
       </c>
-      <c r="E452" t="s">
+      <c r="E459" t="s">
         <v>544</v>
       </c>
-      <c r="G452" s="1" t="s">
+      <c r="G459" s="1" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="454" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C454" t="s">
+    <row r="461" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C461" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="455" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D455" t="s">
+    <row r="462" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D462" t="s">
         <v>548</v>
       </c>
-      <c r="E455" t="s">
+      <c r="E462" t="s">
         <v>549</v>
       </c>
-      <c r="G455" s="1" t="s">
+      <c r="G462" s="1" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="456" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D456" t="s">
+    <row r="463" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D463" t="s">
         <v>550</v>
       </c>
-      <c r="E456" t="s">
+      <c r="E463" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="457" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D457" t="s">
+    <row r="464" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D464" t="s">
         <v>552</v>
       </c>
-      <c r="E457" t="s">
+      <c r="E464" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="458" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D458" t="s">
+    <row r="465" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D465" t="s">
         <v>554</v>
       </c>
-      <c r="E458" t="s">
+      <c r="E465" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="460" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C460" t="s">
+    <row r="467" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C467" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="461" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D461" t="s">
+    <row r="468" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D468" t="s">
         <v>558</v>
       </c>
-      <c r="E461" t="s">
+      <c r="E468" t="s">
         <v>560</v>
       </c>
-      <c r="G461" s="1" t="s">
+      <c r="G468" s="1" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="462" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D462" t="s">
+    <row r="469" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D469" t="s">
         <v>559</v>
       </c>
-      <c r="E462" t="s">
+      <c r="E469" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="464" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C464" t="s">
+    <row r="471" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C471" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="465" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D465" t="s">
+    <row r="472" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D472" t="s">
         <v>565</v>
       </c>
-      <c r="G465" s="1" t="s">
+      <c r="G472" s="1" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="466" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C466" t="s">
+    <row r="473" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C473" t="s">
         <v>608</v>
       </c>
-      <c r="G466" s="1"/>
-    </row>
-    <row r="467" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D467" t="s">
+      <c r="G473" s="1"/>
+    </row>
+    <row r="474" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D474" t="s">
         <v>609</v>
       </c>
-      <c r="E467" t="s">
+      <c r="E474" t="s">
         <v>610</v>
       </c>
-      <c r="G467" s="1" t="s">
+      <c r="G474" s="1" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="468" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G468" s="1"/>
-    </row>
-    <row r="469" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C469" t="s">
+    <row r="475" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G475" s="1"/>
+    </row>
+    <row r="476" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C476" t="s">
         <v>836</v>
       </c>
-      <c r="G469" s="1"/>
-    </row>
-    <row r="470" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D470" t="s">
+      <c r="G476" s="1"/>
+    </row>
+    <row r="477" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D477" t="s">
         <v>837</v>
       </c>
-      <c r="G470" s="1" t="s">
+      <c r="G477" s="1" t="s">
         <v>838</v>
       </c>
     </row>
-    <row r="471" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G471" s="1"/>
-    </row>
-    <row r="472" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G472" s="1"/>
-    </row>
-    <row r="473" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G473" s="1"/>
-    </row>
-    <row r="476" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B476" t="s">
+    <row r="478" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G478" s="1"/>
+    </row>
+    <row r="479" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G479" s="1"/>
+    </row>
+    <row r="480" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G480" s="1"/>
+    </row>
+    <row r="483" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B483" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="477" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C477" t="s">
+    <row r="484" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C484" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="478" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E478" t="s">
+    <row r="485" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E485" t="s">
         <v>568</v>
       </c>
-      <c r="G478" s="1" t="s">
+      <c r="G485" s="1" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="481" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B481" t="s">
+    <row r="488" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B488" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="482" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C482" t="s">
+    <row r="489" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C489" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="483" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D483" t="s">
+    <row r="490" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D490" t="s">
         <v>572</v>
       </c>
-      <c r="E483" t="s">
+      <c r="E490" t="s">
         <v>573</v>
       </c>
-      <c r="F483" t="s">
+      <c r="F490" t="s">
         <v>574</v>
       </c>
-      <c r="G483" s="1" t="s">
+      <c r="G490" s="1" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="484" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="E484" t="s">
+    <row r="491" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E491" t="s">
         <v>576</v>
       </c>
-      <c r="F484" t="s">
+      <c r="F491" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="485" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C485" t="s">
+    <row r="492" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C492" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="486" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D486" t="s">
+    <row r="493" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D493" t="s">
         <v>595</v>
       </c>
-      <c r="E486" t="s">
+      <c r="E493" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="487" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D487" t="s">
+    <row r="494" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D494" t="s">
         <v>598</v>
       </c>
-      <c r="E487" t="s">
+      <c r="E494" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="489" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D489" t="s">
+    <row r="496" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D496" t="s">
         <v>599</v>
       </c>
-      <c r="E489" t="s">
+      <c r="E496" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="490" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D490" t="s">
+    <row r="497" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D497" t="s">
         <v>601</v>
       </c>
-      <c r="E490" t="s">
+      <c r="E497" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="492" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D492" t="s">
+    <row r="499" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D499" t="s">
         <v>840</v>
       </c>
-      <c r="E492" t="s">
+      <c r="E499" t="s">
         <v>839</v>
       </c>
     </row>
-    <row r="493" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D493" t="s">
+    <row r="500" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D500" t="s">
         <v>841</v>
       </c>
-      <c r="E493" t="s">
+      <c r="E500" t="s">
         <v>603</v>
       </c>
-      <c r="G493" s="1" t="s">
+      <c r="G500" s="1" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="494" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D494" t="s">
+    <row r="501" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D501" t="s">
         <v>604</v>
       </c>
-      <c r="E494" t="s">
+      <c r="E501" t="s">
         <v>605</v>
       </c>
-      <c r="F494" t="s">
+      <c r="F501" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="496" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D496" t="s">
+    <row r="503" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D503" t="s">
         <v>842</v>
       </c>
-      <c r="E496" t="s">
+      <c r="E503" t="s">
         <v>851</v>
       </c>
-      <c r="F496" t="s">
+      <c r="F503" t="s">
         <v>853</v>
       </c>
-      <c r="H496" s="1" t="s">
+      <c r="H503" s="1" t="s">
         <v>852</v>
       </c>
     </row>
-    <row r="497" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="E497" t="s">
+    <row r="504" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E504" t="s">
         <v>850</v>
       </c>
-      <c r="F497" t="s">
+      <c r="F504" t="s">
         <v>843</v>
       </c>
-      <c r="G497" t="s">
+      <c r="G504" t="s">
         <v>844</v>
       </c>
-      <c r="H497" s="1" t="s">
+      <c r="H504" s="1" t="s">
         <v>845</v>
       </c>
     </row>
-    <row r="498" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G498" s="1"/>
-    </row>
-    <row r="499" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D499" t="s">
+    <row r="505" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="G505" s="1"/>
+    </row>
+    <row r="506" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D506" t="s">
         <v>846</v>
       </c>
-      <c r="E499" t="s">
+      <c r="E506" t="s">
         <v>847</v>
       </c>
-      <c r="G499" s="1" t="s">
+      <c r="G506" s="1" t="s">
         <v>849</v>
       </c>
     </row>
-    <row r="500" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="E500" t="s">
+    <row r="507" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E507" t="s">
         <v>848</v>
       </c>
-      <c r="G500" s="1"/>
-    </row>
-    <row r="501" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C501" t="s">
+      <c r="G507" s="1"/>
+    </row>
+    <row r="508" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C508" t="s">
         <v>862</v>
       </c>
-      <c r="G501" s="1"/>
-    </row>
-    <row r="502" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D502" t="s">
+      <c r="G508" s="1"/>
+    </row>
+    <row r="509" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D509" t="s">
         <v>863</v>
       </c>
-      <c r="E502" t="s">
+      <c r="E509" t="s">
         <v>574</v>
       </c>
-      <c r="G502" s="1"/>
-    </row>
-    <row r="503" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D503" t="s">
+      <c r="G509" s="1"/>
+    </row>
+    <row r="510" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D510" t="s">
         <v>864</v>
       </c>
-      <c r="E503" t="s">
+      <c r="E510" t="s">
         <v>577</v>
       </c>
-      <c r="G503" s="1"/>
-    </row>
-    <row r="504" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G504" s="1"/>
-    </row>
-    <row r="506" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B506" t="s">
+      <c r="G510" s="1"/>
+    </row>
+    <row r="511" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="G511" s="1"/>
+    </row>
+    <row r="513" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B513" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="507" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C507" t="s">
+    <row r="514" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C514" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="508" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D508" t="s">
+    <row r="515" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D515" t="s">
         <v>581</v>
       </c>
-      <c r="E508" t="s">
+      <c r="E515" t="s">
         <v>582</v>
       </c>
-      <c r="F508" t="s">
+      <c r="F515" t="s">
         <v>580</v>
       </c>
-      <c r="G508" s="1" t="s">
+      <c r="G515" s="1" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="509" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="E509" t="s">
+    <row r="516" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E516" t="s">
         <v>583</v>
       </c>
-      <c r="F509" t="s">
+      <c r="F516" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="511" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D511" t="s">
+    <row r="518" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D518" t="s">
         <v>586</v>
       </c>
-      <c r="E511" t="s">
+      <c r="E518" t="s">
         <v>588</v>
       </c>
-      <c r="F511" t="s">
+      <c r="F518" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="514" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B514" t="s">
+    <row r="521" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B521" t="s">
         <v>706</v>
-      </c>
-    </row>
-    <row r="515" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C515" t="s">
-        <v>707</v>
-      </c>
-      <c r="D515" t="s">
-        <v>710</v>
-      </c>
-      <c r="G515" s="1" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="516" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C516" t="s">
-        <v>708</v>
-      </c>
-      <c r="D516" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="517" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C517" t="s">
-        <v>709</v>
-      </c>
-      <c r="D517" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="520" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B520" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="521" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C521" t="s">
-        <v>731</v>
-      </c>
-      <c r="G521" s="1" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="522" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C522" t="s">
-        <v>733</v>
+        <v>707</v>
+      </c>
+      <c r="D522" t="s">
+        <v>710</v>
       </c>
       <c r="G522" s="1" t="s">
-        <v>734</v>
+        <v>713</v>
       </c>
     </row>
     <row r="523" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C523" t="s">
+        <v>708</v>
+      </c>
+      <c r="D523" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="524" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C524" t="s">
+        <v>709</v>
+      </c>
+      <c r="D524" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="527" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B527" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="528" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C528" t="s">
+        <v>731</v>
+      </c>
+      <c r="G528" s="1" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="529" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C529" t="s">
+        <v>733</v>
+      </c>
+      <c r="G529" s="1" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="530" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C530" t="s">
         <v>737</v>
       </c>
-      <c r="F523" t="s">
+      <c r="F530" t="s">
         <v>735</v>
       </c>
-      <c r="G523" s="1" t="s">
+      <c r="G530" s="1" t="s">
         <v>736</v>
       </c>
     </row>
-    <row r="525" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B525" t="s">
+    <row r="532" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B532" t="s">
         <v>742</v>
-      </c>
-    </row>
-    <row r="526" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C526" t="s">
-        <v>743</v>
-      </c>
-      <c r="D526" t="s">
-        <v>744</v>
-      </c>
-      <c r="G526" s="1" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="527" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C527" t="s">
-        <v>746</v>
-      </c>
-      <c r="D527" t="s">
-        <v>747</v>
-      </c>
-      <c r="G527" s="1" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="531" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B531" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="532" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C532" t="s">
-        <v>802</v>
-      </c>
-      <c r="D532" t="s">
-        <v>803</v>
-      </c>
-      <c r="E532" t="s">
-        <v>804</v>
-      </c>
-      <c r="G532" s="1" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="533" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C533" t="s">
-        <v>806</v>
-      </c>
-      <c r="E533" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="535" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B535" t="s">
-        <v>854</v>
-      </c>
-      <c r="G535" s="1" t="s">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="536" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C536" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="537" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D537" t="s">
-        <v>858</v>
+        <v>743</v>
+      </c>
+      <c r="D533" t="s">
+        <v>744</v>
+      </c>
+      <c r="G533" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="534" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C534" t="s">
+        <v>746</v>
+      </c>
+      <c r="D534" t="s">
+        <v>747</v>
+      </c>
+      <c r="G534" s="1" t="s">
+        <v>748</v>
       </c>
     </row>
     <row r="538" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C538" t="s">
-        <v>856</v>
+      <c r="B538" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="539" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C539" t="s">
+        <v>802</v>
+      </c>
       <c r="D539" t="s">
-        <v>859</v>
+        <v>803</v>
+      </c>
+      <c r="E539" t="s">
+        <v>804</v>
+      </c>
+      <c r="G539" s="1" t="s">
+        <v>805</v>
       </c>
     </row>
     <row r="540" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C540" t="s">
+        <v>806</v>
+      </c>
+      <c r="E540" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="542" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B542" t="s">
+        <v>854</v>
+      </c>
+      <c r="G542" s="1" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="543" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C543" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="544" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D544" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="545" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C545" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="546" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D546" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="547" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C547" t="s">
         <v>857</v>
       </c>
     </row>
-    <row r="541" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D541" t="s">
+    <row r="548" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D548" t="s">
         <v>860</v>
       </c>
     </row>
-    <row r="544" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B544" t="s">
+    <row r="551" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B551" t="s">
         <v>876</v>
       </c>
     </row>
-    <row r="545" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C545" t="s">
+    <row r="552" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C552" t="s">
         <v>877</v>
       </c>
-      <c r="D545" t="s">
+      <c r="D552" t="s">
         <v>878</v>
       </c>
-      <c r="G545" s="1" t="s">
+      <c r="G552" s="1" t="s">
         <v>879</v>
       </c>
     </row>
@@ -6248,169 +6305,169 @@
     <hyperlink ref="D18" r:id="rId2" xr:uid="{02227101-F5A2-3446-ADC1-32F3342C625C}"/>
     <hyperlink ref="D55" r:id="rId3" xr:uid="{6360CC1D-0E6F-6B45-B16E-E9F323959E32}"/>
     <hyperlink ref="E67" r:id="rId4" xr:uid="{96980E2B-5D77-D04D-8463-2374C6B90C21}"/>
-    <hyperlink ref="E77" r:id="rId5" xr:uid="{5081034D-5E40-F340-99D2-B8E4DFC0468C}"/>
-    <hyperlink ref="E80" r:id="rId6" location=":~:text=You%20can%20verify%20whether%20it,password%20and%20ESSID%20are%20correct." xr:uid="{3BA51E9E-8709-874E-B6EC-40074894ACA9}"/>
-    <hyperlink ref="E75" r:id="rId7" xr:uid="{30BD9D61-AAB4-2544-987A-0386CA068398}"/>
-    <hyperlink ref="E83" r:id="rId8" xr:uid="{1824F9BF-1BD9-3842-A565-00C06FF5E50F}"/>
-    <hyperlink ref="D154" r:id="rId9" xr:uid="{E488AECD-B504-A04E-8F27-807A3A08802C}"/>
-    <hyperlink ref="D108" r:id="rId10" location="89804" xr:uid="{E34C14F5-E723-0A48-894F-222B3F74BBF9}"/>
-    <hyperlink ref="D109" r:id="rId11" xr:uid="{6C20672B-9F8F-094F-9AC8-3D1FC1C85319}"/>
-    <hyperlink ref="D110" r:id="rId12" xr:uid="{BA9A8F05-4D7F-4942-886C-F8152208F0EA}"/>
-    <hyperlink ref="F114" r:id="rId13" xr:uid="{22AE585F-7255-3F41-8A2E-808446F3A9AA}"/>
-    <hyperlink ref="F116" r:id="rId14" xr:uid="{93472772-CF6C-D045-B634-2D574A3EE034}"/>
-    <hyperlink ref="E212" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
-    <hyperlink ref="F213" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
-    <hyperlink ref="D244" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
-    <hyperlink ref="D245" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
-    <hyperlink ref="F117" r:id="rId19" xr:uid="{92BE3560-5393-C545-9D2D-2B773359B28F}"/>
-    <hyperlink ref="E261" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
-    <hyperlink ref="E262" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
-    <hyperlink ref="E263" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
-    <hyperlink ref="E91" r:id="rId23" xr:uid="{1526D7DA-27DA-1443-928C-BEDA9E425734}"/>
-    <hyperlink ref="E92" r:id="rId24" xr:uid="{4F363062-BE49-AB4F-8956-2C1F31D9B898}"/>
-    <hyperlink ref="H118" r:id="rId25" xr:uid="{D9E13355-D59B-054F-B544-34A5A285A9E0}"/>
-    <hyperlink ref="G86" r:id="rId26" xr:uid="{170917BF-0643-9848-BCA9-A3BF5219EE3E}"/>
-    <hyperlink ref="F121" r:id="rId27" xr:uid="{5D45F2D3-11BC-6E43-BEFF-29E4E04A041E}"/>
-    <hyperlink ref="I122" r:id="rId28" xr:uid="{7D985D09-6A9A-FF4D-9F4A-4C56CC604DCE}"/>
-    <hyperlink ref="D111" r:id="rId29" xr:uid="{784C3F11-339F-8242-911D-6E4E893DD319}"/>
-    <hyperlink ref="E111" r:id="rId30" xr:uid="{FC907203-09BF-654B-9028-A8528783DAFE}"/>
-    <hyperlink ref="F123" r:id="rId31" xr:uid="{EFD3653A-B2F2-614F-8DEE-A2CB34111C94}"/>
-    <hyperlink ref="F124" r:id="rId32" xr:uid="{774B592D-11A5-9C49-BB9A-61014C8D8C81}"/>
-    <hyperlink ref="F125" r:id="rId33" xr:uid="{BD793670-4C63-C04D-B52D-974AF8E59FA4}"/>
-    <hyperlink ref="F126" r:id="rId34" location="96077" xr:uid="{B9804BBD-5312-714B-97EA-CC7D2C647F2C}"/>
-    <hyperlink ref="H119" r:id="rId35" xr:uid="{7BC5BAB5-D297-0043-BAAF-45AD255D5C84}"/>
-    <hyperlink ref="I118" r:id="rId36" xr:uid="{A03C56E4-1156-A148-A568-F50A5C33DB5C}"/>
-    <hyperlink ref="F127" r:id="rId37" xr:uid="{12AC219C-4678-4E43-B328-6595FA10B8D3}"/>
-    <hyperlink ref="E129" r:id="rId38" xr:uid="{44409621-28A2-704A-B283-3DCE1EFB1603}"/>
-    <hyperlink ref="E267" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
-    <hyperlink ref="F130" r:id="rId40" xr:uid="{A9D0D792-87D1-8144-872F-5CA060D3C28F}"/>
-    <hyperlink ref="F131" r:id="rId41" xr:uid="{87EF989D-17E9-1E45-A075-CD862D0B60F4}"/>
-    <hyperlink ref="F133" r:id="rId42" xr:uid="{8406C6F0-DC69-A64D-AAD8-60A33C12D00B}"/>
-    <hyperlink ref="F134" r:id="rId43" location="108593" xr:uid="{3C38F59E-6E71-4048-9BCA-CBC77D3907E0}"/>
-    <hyperlink ref="F136" r:id="rId44" xr:uid="{EEBE2A3E-36CA-F94F-9B1D-EE463DB6425F}"/>
-    <hyperlink ref="F137" r:id="rId45" xr:uid="{3782B43D-9E6F-2940-A013-34AA5D6B4DB3}"/>
-    <hyperlink ref="F138" r:id="rId46" xr:uid="{3D1C62DB-D9B7-BE42-B21D-4EEBC4C9EFE1}"/>
-    <hyperlink ref="F139" r:id="rId47" xr:uid="{F5021A21-70A2-D34E-B055-64CAC326E7EF}"/>
-    <hyperlink ref="F140" r:id="rId48" xr:uid="{A8C010A1-8EE1-264B-8688-3BEA1B62E535}"/>
-    <hyperlink ref="E268" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
-    <hyperlink ref="F135" r:id="rId50" location="113521" xr:uid="{EE1413C5-3B38-7D4D-8DF1-634A12F0BD81}"/>
-    <hyperlink ref="E93" r:id="rId51" xr:uid="{00B1EF4A-7791-0343-8D8C-9A1E83248FC9}"/>
-    <hyperlink ref="E329" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
-    <hyperlink ref="E330" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
-    <hyperlink ref="F142" r:id="rId54" xr:uid="{40A4B6A0-2F7E-A84D-8CC6-D814A33F5953}"/>
-    <hyperlink ref="E269" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
-    <hyperlink ref="E270" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
-    <hyperlink ref="E271" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
-    <hyperlink ref="E272" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
-    <hyperlink ref="E331" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
-    <hyperlink ref="D246" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
-    <hyperlink ref="D247" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
-    <hyperlink ref="D248" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
-    <hyperlink ref="E273" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
-    <hyperlink ref="E332" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
-    <hyperlink ref="E333" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
-    <hyperlink ref="E335" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
-    <hyperlink ref="E336" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
-    <hyperlink ref="F330" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
-    <hyperlink ref="G330" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
-    <hyperlink ref="E337" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
-    <hyperlink ref="E338" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
-    <hyperlink ref="E339" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
-    <hyperlink ref="E214" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
-    <hyperlink ref="E334" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
-    <hyperlink ref="E340" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
-    <hyperlink ref="E341" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
-    <hyperlink ref="E95" r:id="rId77" location="code" xr:uid="{C0475FF8-517D-E949-887E-9A42D86E9640}"/>
-    <hyperlink ref="E343" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
-    <hyperlink ref="E96" r:id="rId79" xr:uid="{277DBE6F-F3E5-8B4C-8DD8-BD92445D1A99}"/>
-    <hyperlink ref="E345" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
-    <hyperlink ref="E350" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
-    <hyperlink ref="E252" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
-    <hyperlink ref="E253" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
-    <hyperlink ref="F163" r:id="rId84" xr:uid="{EB604865-A16B-0646-A5B5-0D047467449D}"/>
-    <hyperlink ref="E275" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
-    <hyperlink ref="D359" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
-    <hyperlink ref="D360" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
-    <hyperlink ref="E369" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
-    <hyperlink ref="E370" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
-    <hyperlink ref="E368" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
-    <hyperlink ref="D379" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
-    <hyperlink ref="E385" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
-    <hyperlink ref="E382" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
-    <hyperlink ref="E386" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
-    <hyperlink ref="F377" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
-    <hyperlink ref="F378" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
-    <hyperlink ref="E380" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
-    <hyperlink ref="G382" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
-    <hyperlink ref="D395" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
-    <hyperlink ref="E387" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
-    <hyperlink ref="E390" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
-    <hyperlink ref="E389" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
-    <hyperlink ref="F294" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
-    <hyperlink ref="E295" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
-    <hyperlink ref="E296" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
-    <hyperlink ref="E297" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
-    <hyperlink ref="G311" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
-    <hyperlink ref="E306" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
-    <hyperlink ref="E307" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
-    <hyperlink ref="E312" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
-    <hyperlink ref="F175" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
-    <hyperlink ref="F180" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
-    <hyperlink ref="F181" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
-    <hyperlink ref="F188" r:id="rId114" xr:uid="{2B03B1F0-535A-3E4F-8FB3-35D2DE847218}"/>
-    <hyperlink ref="G193" r:id="rId115" xr:uid="{11045522-E183-B14C-B43D-5EA36E454600}"/>
-    <hyperlink ref="E215" r:id="rId116" xr:uid="{F1098A8C-3BC0-DB4F-8F9C-48B31145FEC1}"/>
-    <hyperlink ref="F195" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
-    <hyperlink ref="F189" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
-    <hyperlink ref="F198" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
-    <hyperlink ref="H290" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
-    <hyperlink ref="F402" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
-    <hyperlink ref="G416" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
-    <hyperlink ref="F403" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
-    <hyperlink ref="G418" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
-    <hyperlink ref="G420" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
-    <hyperlink ref="G423" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
-    <hyperlink ref="G427" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
-    <hyperlink ref="G452" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
-    <hyperlink ref="G450" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
-    <hyperlink ref="G455" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
-    <hyperlink ref="G461" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
-    <hyperlink ref="G465" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
-    <hyperlink ref="G478" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
-    <hyperlink ref="G483" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
-    <hyperlink ref="G508" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
+    <hyperlink ref="E84" r:id="rId5" xr:uid="{5081034D-5E40-F340-99D2-B8E4DFC0468C}"/>
+    <hyperlink ref="E87" r:id="rId6" location=":~:text=You%20can%20verify%20whether%20it,password%20and%20ESSID%20are%20correct." xr:uid="{3BA51E9E-8709-874E-B6EC-40074894ACA9}"/>
+    <hyperlink ref="E82" r:id="rId7" xr:uid="{30BD9D61-AAB4-2544-987A-0386CA068398}"/>
+    <hyperlink ref="E90" r:id="rId8" xr:uid="{1824F9BF-1BD9-3842-A565-00C06FF5E50F}"/>
+    <hyperlink ref="D161" r:id="rId9" xr:uid="{E488AECD-B504-A04E-8F27-807A3A08802C}"/>
+    <hyperlink ref="D115" r:id="rId10" location="89804" xr:uid="{E34C14F5-E723-0A48-894F-222B3F74BBF9}"/>
+    <hyperlink ref="D116" r:id="rId11" xr:uid="{6C20672B-9F8F-094F-9AC8-3D1FC1C85319}"/>
+    <hyperlink ref="D117" r:id="rId12" xr:uid="{BA9A8F05-4D7F-4942-886C-F8152208F0EA}"/>
+    <hyperlink ref="F121" r:id="rId13" xr:uid="{22AE585F-7255-3F41-8A2E-808446F3A9AA}"/>
+    <hyperlink ref="F123" r:id="rId14" xr:uid="{93472772-CF6C-D045-B634-2D574A3EE034}"/>
+    <hyperlink ref="E219" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
+    <hyperlink ref="F220" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
+    <hyperlink ref="D251" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
+    <hyperlink ref="D252" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
+    <hyperlink ref="F124" r:id="rId19" xr:uid="{92BE3560-5393-C545-9D2D-2B773359B28F}"/>
+    <hyperlink ref="E268" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
+    <hyperlink ref="E269" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
+    <hyperlink ref="E270" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
+    <hyperlink ref="E98" r:id="rId23" xr:uid="{1526D7DA-27DA-1443-928C-BEDA9E425734}"/>
+    <hyperlink ref="E99" r:id="rId24" xr:uid="{4F363062-BE49-AB4F-8956-2C1F31D9B898}"/>
+    <hyperlink ref="H125" r:id="rId25" xr:uid="{D9E13355-D59B-054F-B544-34A5A285A9E0}"/>
+    <hyperlink ref="G93" r:id="rId26" xr:uid="{170917BF-0643-9848-BCA9-A3BF5219EE3E}"/>
+    <hyperlink ref="F128" r:id="rId27" xr:uid="{5D45F2D3-11BC-6E43-BEFF-29E4E04A041E}"/>
+    <hyperlink ref="I129" r:id="rId28" xr:uid="{7D985D09-6A9A-FF4D-9F4A-4C56CC604DCE}"/>
+    <hyperlink ref="D118" r:id="rId29" xr:uid="{784C3F11-339F-8242-911D-6E4E893DD319}"/>
+    <hyperlink ref="E118" r:id="rId30" xr:uid="{FC907203-09BF-654B-9028-A8528783DAFE}"/>
+    <hyperlink ref="F130" r:id="rId31" xr:uid="{EFD3653A-B2F2-614F-8DEE-A2CB34111C94}"/>
+    <hyperlink ref="F131" r:id="rId32" xr:uid="{774B592D-11A5-9C49-BB9A-61014C8D8C81}"/>
+    <hyperlink ref="F132" r:id="rId33" xr:uid="{BD793670-4C63-C04D-B52D-974AF8E59FA4}"/>
+    <hyperlink ref="F133" r:id="rId34" location="96077" xr:uid="{B9804BBD-5312-714B-97EA-CC7D2C647F2C}"/>
+    <hyperlink ref="H126" r:id="rId35" xr:uid="{7BC5BAB5-D297-0043-BAAF-45AD255D5C84}"/>
+    <hyperlink ref="I125" r:id="rId36" xr:uid="{A03C56E4-1156-A148-A568-F50A5C33DB5C}"/>
+    <hyperlink ref="F134" r:id="rId37" xr:uid="{12AC219C-4678-4E43-B328-6595FA10B8D3}"/>
+    <hyperlink ref="E136" r:id="rId38" xr:uid="{44409621-28A2-704A-B283-3DCE1EFB1603}"/>
+    <hyperlink ref="E274" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
+    <hyperlink ref="F137" r:id="rId40" xr:uid="{A9D0D792-87D1-8144-872F-5CA060D3C28F}"/>
+    <hyperlink ref="F138" r:id="rId41" xr:uid="{87EF989D-17E9-1E45-A075-CD862D0B60F4}"/>
+    <hyperlink ref="F140" r:id="rId42" xr:uid="{8406C6F0-DC69-A64D-AAD8-60A33C12D00B}"/>
+    <hyperlink ref="F141" r:id="rId43" location="108593" xr:uid="{3C38F59E-6E71-4048-9BCA-CBC77D3907E0}"/>
+    <hyperlink ref="F143" r:id="rId44" xr:uid="{EEBE2A3E-36CA-F94F-9B1D-EE463DB6425F}"/>
+    <hyperlink ref="F144" r:id="rId45" xr:uid="{3782B43D-9E6F-2940-A013-34AA5D6B4DB3}"/>
+    <hyperlink ref="F145" r:id="rId46" xr:uid="{3D1C62DB-D9B7-BE42-B21D-4EEBC4C9EFE1}"/>
+    <hyperlink ref="F146" r:id="rId47" xr:uid="{F5021A21-70A2-D34E-B055-64CAC326E7EF}"/>
+    <hyperlink ref="F147" r:id="rId48" xr:uid="{A8C010A1-8EE1-264B-8688-3BEA1B62E535}"/>
+    <hyperlink ref="E275" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
+    <hyperlink ref="F142" r:id="rId50" location="113521" xr:uid="{EE1413C5-3B38-7D4D-8DF1-634A12F0BD81}"/>
+    <hyperlink ref="E100" r:id="rId51" xr:uid="{00B1EF4A-7791-0343-8D8C-9A1E83248FC9}"/>
+    <hyperlink ref="E336" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
+    <hyperlink ref="E337" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
+    <hyperlink ref="F149" r:id="rId54" xr:uid="{40A4B6A0-2F7E-A84D-8CC6-D814A33F5953}"/>
+    <hyperlink ref="E276" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
+    <hyperlink ref="E277" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
+    <hyperlink ref="E278" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
+    <hyperlink ref="E279" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
+    <hyperlink ref="E338" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
+    <hyperlink ref="D253" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
+    <hyperlink ref="D254" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
+    <hyperlink ref="D255" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
+    <hyperlink ref="E280" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
+    <hyperlink ref="E339" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
+    <hyperlink ref="E340" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
+    <hyperlink ref="E342" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
+    <hyperlink ref="E343" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
+    <hyperlink ref="F337" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
+    <hyperlink ref="G337" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
+    <hyperlink ref="E344" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
+    <hyperlink ref="E345" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
+    <hyperlink ref="E346" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
+    <hyperlink ref="E221" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
+    <hyperlink ref="E341" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
+    <hyperlink ref="E347" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
+    <hyperlink ref="E348" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
+    <hyperlink ref="E102" r:id="rId77" location="code" xr:uid="{C0475FF8-517D-E949-887E-9A42D86E9640}"/>
+    <hyperlink ref="E350" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
+    <hyperlink ref="E103" r:id="rId79" xr:uid="{277DBE6F-F3E5-8B4C-8DD8-BD92445D1A99}"/>
+    <hyperlink ref="E352" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
+    <hyperlink ref="E357" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
+    <hyperlink ref="E259" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
+    <hyperlink ref="E260" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
+    <hyperlink ref="F170" r:id="rId84" xr:uid="{EB604865-A16B-0646-A5B5-0D047467449D}"/>
+    <hyperlink ref="E282" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
+    <hyperlink ref="D366" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
+    <hyperlink ref="D367" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
+    <hyperlink ref="E376" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
+    <hyperlink ref="E377" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
+    <hyperlink ref="E375" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
+    <hyperlink ref="D386" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
+    <hyperlink ref="E392" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
+    <hyperlink ref="E389" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
+    <hyperlink ref="E393" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
+    <hyperlink ref="F384" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
+    <hyperlink ref="F385" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
+    <hyperlink ref="E387" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
+    <hyperlink ref="G389" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
+    <hyperlink ref="D402" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
+    <hyperlink ref="E394" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
+    <hyperlink ref="E397" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
+    <hyperlink ref="E396" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
+    <hyperlink ref="F301" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
+    <hyperlink ref="E302" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
+    <hyperlink ref="E303" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
+    <hyperlink ref="E304" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
+    <hyperlink ref="G318" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
+    <hyperlink ref="E313" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
+    <hyperlink ref="E314" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
+    <hyperlink ref="E319" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
+    <hyperlink ref="F182" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
+    <hyperlink ref="F187" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
+    <hyperlink ref="F188" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
+    <hyperlink ref="F195" r:id="rId114" xr:uid="{2B03B1F0-535A-3E4F-8FB3-35D2DE847218}"/>
+    <hyperlink ref="G200" r:id="rId115" xr:uid="{11045522-E183-B14C-B43D-5EA36E454600}"/>
+    <hyperlink ref="E222" r:id="rId116" xr:uid="{F1098A8C-3BC0-DB4F-8F9C-48B31145FEC1}"/>
+    <hyperlink ref="F202" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
+    <hyperlink ref="F196" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
+    <hyperlink ref="F205" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
+    <hyperlink ref="H297" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
+    <hyperlink ref="F409" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
+    <hyperlink ref="G423" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
+    <hyperlink ref="F410" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
+    <hyperlink ref="G425" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
+    <hyperlink ref="G427" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
+    <hyperlink ref="G430" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
+    <hyperlink ref="G434" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
+    <hyperlink ref="G459" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
+    <hyperlink ref="G457" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
+    <hyperlink ref="G462" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
+    <hyperlink ref="G468" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
+    <hyperlink ref="G472" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
+    <hyperlink ref="G485" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
+    <hyperlink ref="G490" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
+    <hyperlink ref="G515" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
     <hyperlink ref="E35" r:id="rId136" xr:uid="{809CA2D1-39E9-0045-A4DF-E4C0C2E97FA2}"/>
     <hyperlink ref="E36" r:id="rId137" xr:uid="{5DC44543-F2B9-F841-9097-6DB19C5EBD82}"/>
-    <hyperlink ref="G493" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
-    <hyperlink ref="G467" r:id="rId139" xr:uid="{7F4EA1D7-8774-1A4B-BF25-18ED0416CB20}"/>
-    <hyperlink ref="F233" r:id="rId140" xr:uid="{101513F3-87A1-DA41-8BF5-E4029309ECB8}"/>
-    <hyperlink ref="F218" r:id="rId141" xr:uid="{494E255E-6912-8643-B5CD-1D65E0DDCFFC}"/>
-    <hyperlink ref="F219" r:id="rId142" xr:uid="{828F749D-83DE-C14E-B637-56047AC1B384}"/>
-    <hyperlink ref="F234" r:id="rId143" xr:uid="{435D9B3C-98B6-5E49-BD30-EAA53523CDB7}"/>
-    <hyperlink ref="F235" r:id="rId144" xr:uid="{7D905409-0097-E04E-9593-2DEEBEEA0D0F}"/>
-    <hyperlink ref="F167" r:id="rId145" xr:uid="{64451146-E88A-9A47-9888-71BEAC8B984E}"/>
-    <hyperlink ref="F223" r:id="rId146" xr:uid="{28F6BA28-EB9B-374C-A8A0-4077C800D23A}"/>
-    <hyperlink ref="G435" r:id="rId147" xr:uid="{20B4F69E-7592-784A-8C2E-123726A51D93}"/>
-    <hyperlink ref="F226" r:id="rId148" xr:uid="{E3C3D7C6-1E6E-FF40-8CC7-6CF1C77457E4}"/>
-    <hyperlink ref="G515" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
-    <hyperlink ref="G188" r:id="rId150" xr:uid="{9BECD448-C575-B64B-BA3F-BEE8D1CBBD43}"/>
-    <hyperlink ref="G521" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
-    <hyperlink ref="G522" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
-    <hyperlink ref="G523" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
-    <hyperlink ref="G526" r:id="rId154" xr:uid="{FB93E0B8-2537-FD47-8420-84D2A706F697}"/>
-    <hyperlink ref="G527" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
-    <hyperlink ref="F201" r:id="rId156" location="2116892" xr:uid="{FF1C16E6-B146-B548-B694-396AC9D0B975}"/>
-    <hyperlink ref="G186" r:id="rId157" xr:uid="{ED09A21C-0057-1146-8BFF-213A32FC88DF}"/>
-    <hyperlink ref="G439" r:id="rId158" xr:uid="{F933A5C4-6DD5-5547-8BB3-B5D3FBA7A852}"/>
-    <hyperlink ref="G532" r:id="rId159" location=".YLoDxOvTXX8" xr:uid="{8886E3AC-3A64-6449-A070-17D95B586F83}"/>
-    <hyperlink ref="F204" r:id="rId160" xr:uid="{5140C3EB-4DFC-5A4A-9C02-C2EBFA052A41}"/>
+    <hyperlink ref="G500" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
+    <hyperlink ref="G474" r:id="rId139" xr:uid="{7F4EA1D7-8774-1A4B-BF25-18ED0416CB20}"/>
+    <hyperlink ref="F240" r:id="rId140" xr:uid="{101513F3-87A1-DA41-8BF5-E4029309ECB8}"/>
+    <hyperlink ref="F225" r:id="rId141" xr:uid="{494E255E-6912-8643-B5CD-1D65E0DDCFFC}"/>
+    <hyperlink ref="F226" r:id="rId142" xr:uid="{828F749D-83DE-C14E-B637-56047AC1B384}"/>
+    <hyperlink ref="F241" r:id="rId143" xr:uid="{435D9B3C-98B6-5E49-BD30-EAA53523CDB7}"/>
+    <hyperlink ref="F242" r:id="rId144" xr:uid="{7D905409-0097-E04E-9593-2DEEBEEA0D0F}"/>
+    <hyperlink ref="F174" r:id="rId145" xr:uid="{64451146-E88A-9A47-9888-71BEAC8B984E}"/>
+    <hyperlink ref="F230" r:id="rId146" xr:uid="{28F6BA28-EB9B-374C-A8A0-4077C800D23A}"/>
+    <hyperlink ref="G442" r:id="rId147" xr:uid="{20B4F69E-7592-784A-8C2E-123726A51D93}"/>
+    <hyperlink ref="F233" r:id="rId148" xr:uid="{E3C3D7C6-1E6E-FF40-8CC7-6CF1C77457E4}"/>
+    <hyperlink ref="G522" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
+    <hyperlink ref="G195" r:id="rId150" xr:uid="{9BECD448-C575-B64B-BA3F-BEE8D1CBBD43}"/>
+    <hyperlink ref="G528" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
+    <hyperlink ref="G529" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
+    <hyperlink ref="G530" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
+    <hyperlink ref="G533" r:id="rId154" xr:uid="{FB93E0B8-2537-FD47-8420-84D2A706F697}"/>
+    <hyperlink ref="G534" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
+    <hyperlink ref="F208" r:id="rId156" location="2116892" xr:uid="{FF1C16E6-B146-B548-B694-396AC9D0B975}"/>
+    <hyperlink ref="G193" r:id="rId157" xr:uid="{ED09A21C-0057-1146-8BFF-213A32FC88DF}"/>
+    <hyperlink ref="G446" r:id="rId158" xr:uid="{F933A5C4-6DD5-5547-8BB3-B5D3FBA7A852}"/>
+    <hyperlink ref="G539" r:id="rId159" location=".YLoDxOvTXX8" xr:uid="{8886E3AC-3A64-6449-A070-17D95B586F83}"/>
+    <hyperlink ref="F211" r:id="rId160" xr:uid="{5140C3EB-4DFC-5A4A-9C02-C2EBFA052A41}"/>
     <hyperlink ref="F28" r:id="rId161" xr:uid="{99992829-3CC1-2B43-BA73-7F09EAA955A4}"/>
-    <hyperlink ref="G470" r:id="rId162" xr:uid="{01E9516A-34A1-6D40-BED9-61916E777090}"/>
-    <hyperlink ref="H497" r:id="rId163" xr:uid="{D3C22B64-1D55-1D47-8F15-25C4AA3D5B90}"/>
-    <hyperlink ref="G499" r:id="rId164" xr:uid="{8E28D310-73EF-1C47-A666-DEE78634BFDF}"/>
-    <hyperlink ref="H496" r:id="rId165" xr:uid="{66476745-9FC4-9E4B-952E-C3E33F678E5D}"/>
-    <hyperlink ref="G535" r:id="rId166" xr:uid="{04D185B2-C246-8B4F-8813-F5A12B741A26}"/>
-    <hyperlink ref="G545" r:id="rId167" xr:uid="{D89D9875-8DF0-3044-BF56-09B8E52D068E}"/>
+    <hyperlink ref="G477" r:id="rId162" xr:uid="{01E9516A-34A1-6D40-BED9-61916E777090}"/>
+    <hyperlink ref="H504" r:id="rId163" xr:uid="{D3C22B64-1D55-1D47-8F15-25C4AA3D5B90}"/>
+    <hyperlink ref="G506" r:id="rId164" xr:uid="{8E28D310-73EF-1C47-A666-DEE78634BFDF}"/>
+    <hyperlink ref="H503" r:id="rId165" xr:uid="{66476745-9FC4-9E4B-952E-C3E33F678E5D}"/>
+    <hyperlink ref="G542" r:id="rId166" xr:uid="{04D185B2-C246-8B4F-8813-F5A12B741A26}"/>
+    <hyperlink ref="G552" r:id="rId167" xr:uid="{D89D9875-8DF0-3044-BF56-09B8E52D068E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed font style for one tip.
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5AED25-5B5D-094B-A153-4F80630E70D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4616DF-8282-BE42-B07F-C8AE4D4B6EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2480" yWindow="4200" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -2724,14 +2724,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2769,15 +2768,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3164,8 +3163,8 @@
   <dimension ref="B1:I552"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D73" sqref="D73"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3178,15 +3177,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
@@ -3738,7 +3737,7 @@
       </c>
     </row>
     <row r="103" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D103" s="3" t="s">
+      <c r="D103" s="7" t="s">
         <v>333</v>
       </c>
       <c r="E103" s="1" t="s">
@@ -4766,7 +4765,7 @@
       </c>
     </row>
     <row r="268" spans="2:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="C268" s="4" t="s">
+      <c r="C268" s="3" t="s">
         <v>184</v>
       </c>
       <c r="D268" s="2" t="s">
@@ -7334,7 +7333,7 @@
       <c r="C2" s="1" t="s">
         <v>753</v>
       </c>
-      <c r="D2" s="7"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">

</xml_diff>

<commit_message>
added cheatsheet on regx
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4616DF-8282-BE42-B07F-C8AE4D4B6EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3076C7D4-82E3-134F-A2DC-AEA6F2C68BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="889">
   <si>
     <t>docker</t>
   </si>
@@ -2699,6 +2699,15 @@
   </si>
   <si>
     <t>docker tag old_name:version new_name:version</t>
+  </si>
+  <si>
+    <t>Nginx</t>
+  </si>
+  <si>
+    <t>https://www.digitalocean.com/community/tutorials/understanding-nginx-server-and-location-block-selection-algorithms</t>
+  </si>
+  <si>
+    <t>Understanding Nginx Server and Location Block Selection Algorithms</t>
   </si>
 </sst>
 </file>
@@ -3162,7 +3171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
   <dimension ref="B1:I552"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D103" sqref="D103"/>
     </sheetView>
@@ -7314,10 +7323,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069EEB69-0D57-C040-8545-840D5862E858}">
-  <dimension ref="B2:D17"/>
+  <dimension ref="B2:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7391,12 +7400,25 @@
         <v>873</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>874</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>875</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>888</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>887</v>
       </c>
     </row>
   </sheetData>
@@ -7407,6 +7429,7 @@
     <hyperlink ref="D13" r:id="rId4" xr:uid="{285EBC06-8ECF-4C47-AB0D-38C1776297C3}"/>
     <hyperlink ref="D7" r:id="rId5" xr:uid="{DA30C5A1-BF15-2449-AD30-BFE122EB375C}"/>
     <hyperlink ref="D17" r:id="rId6" xr:uid="{C1FD43E4-7E41-194B-A364-D7DEDEF40A3C}"/>
+    <hyperlink ref="D20" r:id="rId7" xr:uid="{9836BE79-9331-8F4F-B63E-FD3D6FE0005D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added article for regex
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3076C7D4-82E3-134F-A2DC-AEA6F2C68BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB3C163-37C3-8346-89ED-02CB5616907B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="889">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="892">
   <si>
     <t>docker</t>
   </si>
@@ -2708,6 +2708,15 @@
   </si>
   <si>
     <t>Understanding Nginx Server and Location Block Selection Algorithms</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/14596884/remove-text-between-and</t>
+  </si>
+  <si>
+    <t>re.sub("[\(\[].*?[\)\]]", "", x)</t>
+  </si>
+  <si>
+    <t>Remove text between () and []</t>
   </si>
 </sst>
 </file>
@@ -3172,8 +3181,8 @@
   <dimension ref="B1:I552"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D103" sqref="D103"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6483,10 +6492,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G65"/>
+  <dimension ref="B2:G66"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7099,123 +7108,134 @@
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>771</v>
-      </c>
-      <c r="C56" t="s">
-        <v>467</v>
+        <v>891</v>
       </c>
       <c r="E56" t="s">
-        <v>769</v>
+        <v>890</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>770</v>
+        <v>889</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>723</v>
+        <v>771</v>
+      </c>
+      <c r="C57" t="s">
+        <v>467</v>
       </c>
       <c r="E57" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>722</v>
+        <v>770</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>774</v>
+        <v>723</v>
+      </c>
+      <c r="E58" t="s">
+        <v>772</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>773</v>
+        <v>722</v>
       </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>775</v>
-      </c>
-      <c r="C59" t="s">
-        <v>467</v>
-      </c>
-      <c r="E59" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>783</v>
+        <v>775</v>
+      </c>
+      <c r="C60" t="s">
+        <v>467</v>
       </c>
       <c r="E60" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>782</v>
+        <v>777</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>786</v>
-      </c>
-      <c r="D61" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="E61" t="s">
-        <v>784</v>
+        <v>781</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>782</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>787</v>
-      </c>
-      <c r="C62" t="s">
-        <v>789</v>
+        <v>786</v>
+      </c>
+      <c r="D62" t="s">
+        <v>785</v>
       </c>
       <c r="E62" t="s">
-        <v>790</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="C63" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
       <c r="E63" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>795</v>
+        <v>791</v>
+      </c>
+      <c r="C64" t="s">
+        <v>794</v>
       </c>
       <c r="E64" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
+        <v>795</v>
+      </c>
+      <c r="E65" t="s">
+        <v>797</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
         <v>798</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>648</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E66" t="s">
         <v>799</v>
       </c>
-      <c r="F65" s="1" t="s">
+      <c r="F66" s="1" t="s">
         <v>800</v>
       </c>
     </row>
@@ -7274,15 +7294,16 @@
     <hyperlink ref="F50" r:id="rId51" xr:uid="{B9356038-CF05-854A-AFF1-D7384A989DFB}"/>
     <hyperlink ref="F54" r:id="rId52" xr:uid="{61072865-D316-554C-A5B2-DE65C0BB4955}"/>
     <hyperlink ref="F55" r:id="rId53" xr:uid="{3D288582-752C-394F-85D5-4AC8FCF2210E}"/>
-    <hyperlink ref="F56" r:id="rId54" xr:uid="{634A44CB-CBAB-AE4D-898A-98A6804C37BE}"/>
-    <hyperlink ref="F57" r:id="rId55" xr:uid="{CBA3AB68-A9B5-7E45-AAF4-E420DC08CECB}"/>
-    <hyperlink ref="F58" r:id="rId56" xr:uid="{6513D8D1-CA9F-DB4F-8EE3-BB85344F470E}"/>
-    <hyperlink ref="F59" r:id="rId57" xr:uid="{F0C558B0-9D09-2E47-9A73-03B1EBC298EA}"/>
-    <hyperlink ref="F60" r:id="rId58" xr:uid="{0E6940AA-CCE2-A845-B000-88634DEE5413}"/>
-    <hyperlink ref="F62" r:id="rId59" xr:uid="{DB6C6106-7A38-1843-B3AC-F9FB615E4977}"/>
-    <hyperlink ref="F63" r:id="rId60" xr:uid="{8AED1472-61F4-E646-89E7-A2D566BEF7A0}"/>
-    <hyperlink ref="F64" r:id="rId61" xr:uid="{D5875307-B681-3841-BE35-59A92CDCD038}"/>
-    <hyperlink ref="F65" r:id="rId62" xr:uid="{E6DDA861-2175-8242-9563-08D5A89ACF52}"/>
+    <hyperlink ref="F57" r:id="rId54" xr:uid="{634A44CB-CBAB-AE4D-898A-98A6804C37BE}"/>
+    <hyperlink ref="F58" r:id="rId55" xr:uid="{CBA3AB68-A9B5-7E45-AAF4-E420DC08CECB}"/>
+    <hyperlink ref="F59" r:id="rId56" xr:uid="{6513D8D1-CA9F-DB4F-8EE3-BB85344F470E}"/>
+    <hyperlink ref="F60" r:id="rId57" xr:uid="{F0C558B0-9D09-2E47-9A73-03B1EBC298EA}"/>
+    <hyperlink ref="F61" r:id="rId58" xr:uid="{0E6940AA-CCE2-A845-B000-88634DEE5413}"/>
+    <hyperlink ref="F63" r:id="rId59" xr:uid="{DB6C6106-7A38-1843-B3AC-F9FB615E4977}"/>
+    <hyperlink ref="F64" r:id="rId60" xr:uid="{8AED1472-61F4-E646-89E7-A2D566BEF7A0}"/>
+    <hyperlink ref="F65" r:id="rId61" xr:uid="{D5875307-B681-3841-BE35-59A92CDCD038}"/>
+    <hyperlink ref="F66" r:id="rId62" xr:uid="{E6DDA861-2175-8242-9563-08D5A89ACF52}"/>
+    <hyperlink ref="F56" r:id="rId63" xr:uid="{EDECDF4B-3198-4348-9F78-BF6E9FF8C9A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7325,7 +7346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069EEB69-0D57-C040-8545-840D5862E858}">
   <dimension ref="B2:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
merged with version on 15' Mac
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB3C163-37C3-8346-89ED-02CB5616907B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E6AECF-AFCD-FD4A-B01B-4B8F294518F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="898">
   <si>
     <t>docker</t>
   </si>
@@ -2717,6 +2717,24 @@
   </si>
   <si>
     <t>Remove text between () and []</t>
+  </si>
+  <si>
+    <t>remove search highlights</t>
+  </si>
+  <si>
+    <t>:noh</t>
+  </si>
+  <si>
+    <t>https://vi.stackexchange.com/questions/184/how-can-i-clear-word-highlighting-in-the-current-document-e-g-such-as-after-se</t>
+  </si>
+  <si>
+    <t>Vim tips</t>
+  </si>
+  <si>
+    <t>Boost Your Coding Fu With Visual Studio Code and Vim</t>
+  </si>
+  <si>
+    <t>https://www.barbarianmeetscoding.com/blog/boost-your-coding-fu-with-vscode-and-vim</t>
   </si>
 </sst>
 </file>
@@ -3181,8 +3199,8 @@
   <dimension ref="B1:I552"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+      <pane ySplit="1" topLeftCell="A535" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C478" sqref="C478:G479"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5901,10 +5919,18 @@
       </c>
     </row>
     <row r="478" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C478" t="s">
+        <v>892</v>
+      </c>
       <c r="G478" s="1"/>
     </row>
     <row r="479" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="G479" s="1"/>
+      <c r="D479" t="s">
+        <v>893</v>
+      </c>
+      <c r="G479" s="1" t="s">
+        <v>894</v>
+      </c>
     </row>
     <row r="480" spans="3:7" x14ac:dyDescent="0.2">
       <c r="G480" s="1"/>
@@ -6485,6 +6511,7 @@
     <hyperlink ref="H503" r:id="rId165" xr:uid="{66476745-9FC4-9E4B-952E-C3E33F678E5D}"/>
     <hyperlink ref="G542" r:id="rId166" xr:uid="{04D185B2-C246-8B4F-8813-F5A12B741A26}"/>
     <hyperlink ref="G552" r:id="rId167" xr:uid="{D89D9875-8DF0-3044-BF56-09B8E52D068E}"/>
+    <hyperlink ref="G479" r:id="rId168" xr:uid="{951EA3E4-9D93-CC44-96EE-1FAB3FE8B169}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6494,7 +6521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
   <dimension ref="B2:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
@@ -7344,10 +7371,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069EEB69-0D57-C040-8545-840D5862E858}">
-  <dimension ref="B2:D20"/>
+  <dimension ref="B2:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7442,6 +7469,19 @@
         <v>887</v>
       </c>
     </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>896</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{87D156EE-D133-464D-8B0D-7B076D239955}"/>
@@ -7451,6 +7491,7 @@
     <hyperlink ref="D7" r:id="rId5" xr:uid="{DA30C5A1-BF15-2449-AD30-BFE122EB375C}"/>
     <hyperlink ref="D17" r:id="rId6" xr:uid="{C1FD43E4-7E41-194B-A364-D7DEDEF40A3C}"/>
     <hyperlink ref="D20" r:id="rId7" xr:uid="{9836BE79-9331-8F4F-B63E-FD3D6FE0005D}"/>
+    <hyperlink ref="D23" r:id="rId8" xr:uid="{2580CEB1-57A9-FD4B-8778-D0742AF03763}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for regex and ssh key
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E6AECF-AFCD-FD4A-B01B-4B8F294518F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7C1BFF-CEAD-0443-B4A2-D94095E0C629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="909">
   <si>
     <t>docker</t>
   </si>
@@ -2735,6 +2735,39 @@
   </si>
   <si>
     <t>https://www.barbarianmeetscoding.com/blog/boost-your-coding-fu-with-vscode-and-vim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Option 1, manually </t>
+  </si>
+  <si>
+    <t>Open the known_hosts file, and delete the line specified in the warning message</t>
+  </si>
+  <si>
+    <t>Option 2, by using ssh-keygen</t>
+  </si>
+  <si>
+    <t>Fix: "WARNING: REMOTE HOST IDENTIFICATION HAS CHANGED"</t>
+  </si>
+  <si>
+    <t>https://stackabuse.com/how-to-fix-warning-remote-host-identification-has-changed-on-mac-and-linux</t>
+  </si>
+  <si>
+    <t>ssh-keygen -R "[hostname-or-IP]:Port"</t>
+  </si>
+  <si>
+    <t>note: port must be appended if it exists</t>
+  </si>
+  <si>
+    <t>for remote server, it's normally in ~.ssh/authorized_keys</t>
+  </si>
+  <si>
+    <t>https://www.guru99.com/python-regular-expressions-complete-tutorial.html#5</t>
+  </si>
+  <si>
+    <t>find pattern with re.match and group</t>
+  </si>
+  <si>
+    <t>re.match('(group1)(group2)(group3)')</t>
   </si>
 </sst>
 </file>
@@ -3196,17 +3229,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I552"/>
+  <dimension ref="B1:I553"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A535" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C478" sqref="C478:G479"/>
+      <pane ySplit="1" topLeftCell="A470" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="25.1640625" customWidth="1"/>
-    <col min="3" max="3" width="45.33203125" customWidth="1"/>
+    <col min="3" max="3" width="47.1640625" customWidth="1"/>
     <col min="4" max="4" width="44.83203125" customWidth="1"/>
     <col min="5" max="5" width="38.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
@@ -3396,734 +3429,763 @@
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D28" t="s">
+      <c r="E28" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
         <v>832</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" t="s">
         <v>833</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>834</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C35" t="s">
-        <v>589</v>
-      </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1" t="s">
-        <v>590</v>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>898</v>
+      </c>
+      <c r="E32" t="s">
+        <v>899</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>900</v>
+      </c>
+      <c r="E33" t="s">
+        <v>903</v>
+      </c>
+      <c r="F33" t="s">
+        <v>904</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
+        <v>589</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
         <v>591</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>593</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C39" t="s">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D42">
         <v>2</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E42" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C42" t="s">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D43">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D44">
         <v>1</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E44" t="s">
         <v>22</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F44" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C45" t="s">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D46">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D47">
         <v>1</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E47" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C47" t="s">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D48">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D49">
         <v>1</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C49" t="s">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
         <v>835</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D50">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D51">
         <v>1</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E51" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C55" t="s">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
         <v>30</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C58" t="s">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C59" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D59" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D60" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E61" t="s">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E62" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C62" t="s">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C63" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D63" t="s">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D64" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E64" t="s">
+    <row r="65" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E65" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C65" t="s">
+    <row r="66" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C66" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D66" t="s">
+    <row r="67" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
         <v>35</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E67" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D67" t="s">
+    <row r="68" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
         <v>30</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="E68" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C69" t="s">
+    <row r="70" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C70" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D70" t="s">
+    <row r="71" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D71" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E71" t="s">
+    <row r="72" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E72" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C72" t="s">
+    <row r="73" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C73" t="s">
         <v>880</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D73" t="s">
+    <row r="74" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D74" t="s">
         <v>38</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E74" t="s">
         <v>881</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C74" t="s">
+    <row r="75" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C75" t="s">
         <v>882</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D75" t="s">
+    <row r="76" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D76" t="s">
         <v>38</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E76" t="s">
         <v>883</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C76" t="s">
+    <row r="77" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C77" t="s">
         <v>884</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D77" t="s">
+    <row r="78" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D78" t="s">
         <v>38</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E78" t="s">
         <v>885</v>
       </c>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B80" t="s">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C81" t="s">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C82" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D82" t="s">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D83" t="s">
         <v>47</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="E83" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C83" t="s">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C84" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D84" t="s">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D85" t="s">
         <v>50</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="E85" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D85" t="s">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D86" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C86" t="s">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C87" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D87" t="s">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D88" t="s">
         <v>53</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="E88" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C89" t="s">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D90" t="s">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D91" t="s">
         <v>57</v>
       </c>
-      <c r="E90" s="1" t="s">
+      <c r="E91" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E91" s="1"/>
-    </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C92" t="s">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E92" s="1"/>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C93" t="s">
         <v>198</v>
       </c>
-      <c r="E92" s="1"/>
-    </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D93" t="s">
+      <c r="E93" s="1"/>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
         <v>203</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E94" t="s">
         <v>53</v>
       </c>
-      <c r="F93" t="s">
+      <c r="F94" t="s">
         <v>200</v>
       </c>
-      <c r="G93" s="1" t="s">
+      <c r="G94" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="94" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D94" t="s">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D95" t="s">
         <v>204</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E95" t="s">
         <v>201</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F95" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="95" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E95" s="1"/>
-    </row>
-    <row r="96" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E96" s="1"/>
     </row>
     <row r="97" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C97" t="s">
+      <c r="E97" s="1"/>
+    </row>
+    <row r="98" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C98" t="s">
         <v>192</v>
       </c>
-      <c r="E97" s="1"/>
-    </row>
-    <row r="98" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D98" t="s">
+      <c r="E98" s="1"/>
+    </row>
+    <row r="99" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D99" t="s">
         <v>193</v>
       </c>
-      <c r="E98" s="1" t="s">
+      <c r="E99" s="1" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="99" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E99" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="100" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E100" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="101" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E101" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="101" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E101" s="1"/>
-    </row>
     <row r="102" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D102" t="s">
+      <c r="E102" s="1"/>
+    </row>
+    <row r="103" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D103" t="s">
         <v>328</v>
       </c>
-      <c r="E102" s="1" t="s">
+      <c r="E103" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="103" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D103" s="7" t="s">
+    <row r="104" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D104" s="7" t="s">
         <v>333</v>
       </c>
-      <c r="E103" s="1" t="s">
+      <c r="E104" s="1" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="104" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E104" s="1"/>
-    </row>
-    <row r="114" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B114" t="s">
+    <row r="105" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E105" s="1"/>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B115" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C115" t="s">
-        <v>156</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C116" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C117" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C118" t="s">
+        <v>159</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="119" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C119" t="s">
         <v>218</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="D119" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E118" s="1" t="s">
+      <c r="E119" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="120" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C120" t="s">
+    <row r="121" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C121" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="121" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D121" t="s">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D122" t="s">
         <v>163</v>
       </c>
-      <c r="E121" t="s">
+      <c r="E122" t="s">
         <v>162</v>
       </c>
-      <c r="F121" s="1" t="s">
+      <c r="F122" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="122" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="E122" t="s">
+    <row r="123" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E123" t="s">
         <v>274</v>
       </c>
-      <c r="F122" s="1"/>
-    </row>
-    <row r="123" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D123" t="s">
-        <v>165</v>
-      </c>
-      <c r="E123" t="s">
-        <v>166</v>
-      </c>
-      <c r="F123" s="1" t="s">
-        <v>167</v>
-      </c>
+      <c r="F123" s="1"/>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D124" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E124" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D125" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="E125" t="s">
-        <v>191</v>
-      </c>
-      <c r="F125" t="s">
-        <v>195</v>
-      </c>
-      <c r="G125" t="s">
-        <v>190</v>
-      </c>
-      <c r="H125" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="I125" s="1" t="s">
-        <v>197</v>
+        <v>180</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D126" t="s">
-        <v>231</v>
+        <v>189</v>
       </c>
       <c r="E126" t="s">
-        <v>233</v>
+        <v>191</v>
+      </c>
+      <c r="F126" t="s">
+        <v>195</v>
+      </c>
+      <c r="G126" t="s">
+        <v>190</v>
       </c>
       <c r="H126" s="1" t="s">
         <v>196</v>
       </c>
+      <c r="I126" s="1" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D127" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E127" t="s">
-        <v>234</v>
-      </c>
-      <c r="H127" s="1"/>
+        <v>233</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D128" t="s">
-        <v>205</v>
+        <v>232</v>
       </c>
       <c r="E128" t="s">
-        <v>206</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>207</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="H128" s="1"/>
     </row>
     <row r="129" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D129" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E129" t="s">
-        <v>209</v>
-      </c>
-      <c r="F129" t="s">
-        <v>210</v>
-      </c>
-      <c r="G129" t="s">
-        <v>213</v>
-      </c>
-      <c r="H129" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="I129" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="130" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D130" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="E130" t="s">
-        <v>220</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>221</v>
+        <v>209</v>
+      </c>
+      <c r="F130" t="s">
+        <v>210</v>
+      </c>
+      <c r="G130" t="s">
+        <v>213</v>
+      </c>
+      <c r="H130" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="I130" s="1" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="131" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D131" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E131" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="132" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D132" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E132" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="133" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D133" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E133" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="134" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D134" t="s">
+        <v>228</v>
+      </c>
+      <c r="E134" t="s">
+        <v>229</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="135" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D135" t="s">
         <v>235</v>
       </c>
-      <c r="E134" t="s">
+      <c r="E135" t="s">
         <v>236</v>
       </c>
-      <c r="F134" s="1" t="s">
+      <c r="F135" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="135" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="E135" t="s">
+    <row r="136" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E136" t="s">
         <v>237</v>
-      </c>
-      <c r="F135" s="1"/>
-    </row>
-    <row r="136" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D136" t="s">
-        <v>239</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="F136" s="1"/>
     </row>
     <row r="137" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D137" t="s">
-        <v>246</v>
-      </c>
-      <c r="E137" t="s">
-        <v>245</v>
-      </c>
-      <c r="F137" s="1" t="s">
-        <v>244</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F137" s="1"/>
     </row>
     <row r="138" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D138" t="s">
-        <v>247</v>
+        <v>246</v>
+      </c>
+      <c r="E138" t="s">
+        <v>245</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="139" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D139" t="s">
-        <v>249</v>
-      </c>
-      <c r="E139" t="s">
-        <v>206</v>
+        <v>247</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="140" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D140" t="s">
-        <v>251</v>
-      </c>
-      <c r="F140" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
+      </c>
+      <c r="E140" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="141" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D141" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="142" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D142" t="s">
-        <v>272</v>
+        <v>253</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
     </row>
     <row r="143" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D143" t="s">
-        <v>254</v>
-      </c>
-      <c r="E143" t="s">
-        <v>255</v>
+        <v>272</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>256</v>
+        <v>273</v>
       </c>
     </row>
     <row r="144" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D144" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E144" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="145" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D145" t="s">
-        <v>261</v>
+        <v>257</v>
+      </c>
+      <c r="E145" t="s">
+        <v>258</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="146" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D146" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="147" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D147" t="s">
+        <v>263</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D148" t="s">
         <v>265</v>
       </c>
-      <c r="E147" t="s">
+      <c r="E148" t="s">
         <v>264</v>
       </c>
-      <c r="F147" s="1" t="s">
+      <c r="F148" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E148" t="s">
+    <row r="149" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E149" t="s">
         <v>267</v>
       </c>
-      <c r="F148" s="1"/>
-    </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D149" t="s">
+      <c r="F149" s="1"/>
+    </row>
+    <row r="150" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D150" t="s">
         <v>282</v>
       </c>
-      <c r="F149" s="1" t="s">
+      <c r="F150" s="1" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F150" s="1"/>
     </row>
     <row r="151" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F151" s="1"/>
@@ -4138,522 +4200,522 @@
       <c r="F154" s="1"/>
     </row>
     <row r="155" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B155" t="s">
+      <c r="F155" s="1"/>
+    </row>
+    <row r="156" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B156" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C156" t="s">
+    <row r="157" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C157" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D157" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="158" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D158" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="159" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D159" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="160" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C160" t="s">
+    <row r="161" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C161" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="161" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D161" s="1" t="s">
+    <row r="162" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D162" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="163" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C163" t="s">
+    <row r="164" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C164" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="164" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D164" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="165" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D165" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="166" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D166" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="167" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D167" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="168" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D168" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="169" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C169" t="s">
+    <row r="170" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C170" t="s">
         <v>346</v>
-      </c>
-    </row>
-    <row r="170" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D170" t="s">
-        <v>349</v>
-      </c>
-      <c r="E170" t="s">
-        <v>347</v>
-      </c>
-      <c r="F170" s="1" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="171" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D171" t="s">
+        <v>349</v>
+      </c>
+      <c r="E171" t="s">
+        <v>347</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="172" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D172" t="s">
         <v>350</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E172" t="s">
         <v>351</v>
       </c>
-      <c r="F171" t="s">
+      <c r="F172" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="173" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C173" t="s">
+    <row r="174" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C174" t="s">
         <v>674</v>
-      </c>
-    </row>
-    <row r="174" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D174" t="s">
-        <v>675</v>
-      </c>
-      <c r="E174" t="s">
-        <v>676</v>
-      </c>
-      <c r="F174" s="1" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="175" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D175" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="E175" t="s">
-        <v>678</v>
+        <v>676</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="176" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D176" t="s">
+        <v>677</v>
+      </c>
+      <c r="E176" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="177" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D177" t="s">
         <v>679</v>
       </c>
-      <c r="E176" t="s">
+      <c r="E177" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="178" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C178" t="s">
+    <row r="179" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C179" t="s">
         <v>357</v>
-      </c>
-    </row>
-    <row r="179" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D179" t="s">
-        <v>354</v>
-      </c>
-      <c r="E179" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="180" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D180" t="s">
+        <v>354</v>
+      </c>
+      <c r="E180" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="181" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D181" t="s">
         <v>355</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E181" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="182" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C182" t="s">
+    <row r="183" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C183" t="s">
         <v>369</v>
       </c>
-      <c r="F182" s="1" t="s">
+      <c r="F183" s="1" t="s">
         <v>378</v>
-      </c>
-    </row>
-    <row r="183" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D183" t="s">
-        <v>370</v>
-      </c>
-      <c r="E183" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="184" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D184" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E184" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="185" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D185" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E185" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="186" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D186" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E186" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="187" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D187" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="E187" t="s">
-        <v>386</v>
-      </c>
-      <c r="F187" s="1" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
     </row>
     <row r="188" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D188" t="s">
+        <v>385</v>
+      </c>
+      <c r="E188" t="s">
+        <v>386</v>
+      </c>
+      <c r="F188" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="189" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D189" t="s">
         <v>388</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E189" t="s">
         <v>389</v>
       </c>
-      <c r="F188" s="1" t="s">
+      <c r="F189" s="1" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="190" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C190" t="s">
+    <row r="191" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C191" t="s">
         <v>379</v>
-      </c>
-    </row>
-    <row r="191" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D191" t="s">
-        <v>380</v>
-      </c>
-      <c r="E191" t="s">
-        <v>381</v>
-      </c>
-      <c r="F191" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="192" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D192" t="s">
-        <v>808</v>
+        <v>380</v>
       </c>
       <c r="E192" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F192" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="193" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D193" t="s">
+        <v>808</v>
+      </c>
+      <c r="E193" t="s">
+        <v>382</v>
+      </c>
+      <c r="F193" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="194" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D194" t="s">
         <v>759</v>
       </c>
-      <c r="E193" t="s">
+      <c r="E194" t="s">
         <v>760</v>
       </c>
-      <c r="G193" s="1" t="s">
+      <c r="G194" s="1" t="s">
         <v>761</v>
       </c>
     </row>
-    <row r="194" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="F194" s="1"/>
-    </row>
     <row r="195" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C195" t="s">
+      <c r="F195" s="1"/>
+    </row>
+    <row r="196" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C196" t="s">
         <v>391</v>
       </c>
-      <c r="D195" t="s">
+      <c r="D196" t="s">
         <v>419</v>
       </c>
-      <c r="E195" t="s">
+      <c r="E196" t="s">
         <v>392</v>
       </c>
-      <c r="F195" s="1" t="s">
+      <c r="F196" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G195" s="1" t="s">
+      <c r="G196" s="1" t="s">
         <v>724</v>
-      </c>
-    </row>
-    <row r="196" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D196" t="s">
-        <v>420</v>
-      </c>
-      <c r="E196" t="s">
-        <v>421</v>
-      </c>
-      <c r="F196" s="1" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="197" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D197" t="s">
+        <v>420</v>
+      </c>
+      <c r="E197" t="s">
+        <v>421</v>
+      </c>
+      <c r="F197" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="198" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D198" t="s">
         <v>423</v>
       </c>
-      <c r="E197" t="s">
+      <c r="E198" t="s">
         <v>424</v>
       </c>
-      <c r="F197" s="1"/>
-    </row>
-    <row r="198" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C198" t="s">
+      <c r="F198" s="1"/>
+    </row>
+    <row r="199" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C199" t="s">
         <v>393</v>
-      </c>
-      <c r="F198" s="1"/>
-    </row>
-    <row r="199" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D199" t="s">
-        <v>395</v>
-      </c>
-      <c r="E199" t="s">
-        <v>394</v>
       </c>
       <c r="F199" s="1"/>
     </row>
     <row r="200" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D200" t="s">
+        <v>395</v>
+      </c>
+      <c r="E200" t="s">
+        <v>394</v>
+      </c>
+      <c r="F200" s="1"/>
+    </row>
+    <row r="201" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D201" t="s">
         <v>396</v>
       </c>
-      <c r="F200" t="s">
+      <c r="F201" t="s">
         <v>397</v>
       </c>
-      <c r="G200" s="1" t="s">
+      <c r="G201" s="1" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="201" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C201" t="s">
+    <row r="202" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C202" t="s">
         <v>415</v>
-      </c>
-      <c r="G201" s="1"/>
-    </row>
-    <row r="202" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E202" t="s">
-        <v>416</v>
-      </c>
-      <c r="F202" s="1" t="s">
-        <v>418</v>
       </c>
       <c r="G202" s="1"/>
     </row>
     <row r="203" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E203" t="s">
+        <v>416</v>
+      </c>
+      <c r="F203" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="G203" s="1"/>
+    </row>
+    <row r="204" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E204" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="204" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C204" t="s">
+    <row r="205" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C205" t="s">
         <v>430</v>
-      </c>
-    </row>
-    <row r="205" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D205" t="s">
-        <v>431</v>
-      </c>
-      <c r="E205" t="s">
-        <v>433</v>
-      </c>
-      <c r="F205" s="1" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="206" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D206" t="s">
+        <v>431</v>
+      </c>
+      <c r="E206" t="s">
+        <v>433</v>
+      </c>
+      <c r="F206" s="1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="207" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D207" t="s">
         <v>432</v>
       </c>
-      <c r="E206" t="s">
+      <c r="E207" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="207" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C207" t="s">
+    <row r="208" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C208" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="208" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D208" t="s">
+    <row r="209" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D209" t="s">
         <v>757</v>
       </c>
-      <c r="E208" t="s">
+      <c r="E209" t="s">
         <v>756</v>
       </c>
-      <c r="F208" s="1" t="s">
+      <c r="F209" s="1" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="209" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E209" t="s">
+    <row r="210" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E210" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="210" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C210" t="s">
+    <row r="211" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C211" t="s">
         <v>809</v>
       </c>
     </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D211" t="s">
+    <row r="212" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D212" t="s">
         <v>811</v>
       </c>
-      <c r="E211" t="s">
+      <c r="E212" t="s">
         <v>810</v>
       </c>
-      <c r="F211" s="1" t="s">
+      <c r="F212" s="1" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="217" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B217" t="s">
+    <row r="218" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B218" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="218" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C218" t="s">
+    <row r="219" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C219" t="s">
         <v>169</v>
-      </c>
-    </row>
-    <row r="219" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D219" t="s">
-        <v>170</v>
-      </c>
-      <c r="E219" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="220" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D220" t="s">
+        <v>170</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="221" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D221" t="s">
         <v>174</v>
       </c>
-      <c r="E220" t="s">
+      <c r="E221" t="s">
         <v>172</v>
       </c>
-      <c r="F220" s="1" t="s">
+      <c r="F221" s="1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="221" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C221" t="s">
-        <v>321</v>
-      </c>
-      <c r="E221" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="F221" s="1"/>
     </row>
     <row r="222" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C222" t="s">
+        <v>321</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="F222" s="1"/>
+    </row>
+    <row r="223" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C223" t="s">
         <v>404</v>
       </c>
-      <c r="D222" t="s">
+      <c r="D223" t="s">
         <v>405</v>
       </c>
-      <c r="E222" s="1" t="s">
+      <c r="E223" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="F222" s="1"/>
-    </row>
-    <row r="223" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D223" t="s">
+      <c r="F223" s="1"/>
+    </row>
+    <row r="224" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D224" t="s">
         <v>406</v>
       </c>
-      <c r="F223" s="1"/>
-    </row>
-    <row r="224" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F224" s="1"/>
     </row>
     <row r="225" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C225" t="s">
-        <v>615</v>
-      </c>
-      <c r="D225" t="s">
-        <v>616</v>
-      </c>
-      <c r="F225" s="1" t="s">
-        <v>617</v>
-      </c>
+      <c r="F225" s="1"/>
     </row>
     <row r="226" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C226" t="s">
+        <v>615</v>
+      </c>
+      <c r="D226" t="s">
+        <v>616</v>
+      </c>
+      <c r="F226" s="1" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="227" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C227" t="s">
         <v>619</v>
       </c>
-      <c r="D226" t="s">
+      <c r="D227" t="s">
         <v>618</v>
       </c>
-      <c r="F226" s="1" t="s">
+      <c r="F227" s="1" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="227" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F227" s="1"/>
     </row>
     <row r="228" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F228" s="1"/>
     </row>
     <row r="229" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B229" t="s">
+      <c r="F229" s="1"/>
+    </row>
+    <row r="230" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B230" t="s">
         <v>682</v>
       </c>
-      <c r="F229" s="1"/>
-    </row>
-    <row r="230" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C230" t="s">
-        <v>683</v>
-      </c>
-      <c r="D230" t="s">
-        <v>685</v>
-      </c>
-      <c r="F230" s="1" t="s">
-        <v>687</v>
-      </c>
+      <c r="F230" s="1"/>
     </row>
     <row r="231" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C231" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D231" t="s">
-        <v>686</v>
-      </c>
-      <c r="F231" s="1"/>
+        <v>685</v>
+      </c>
+      <c r="F231" s="1" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="232" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C232" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="D232" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="F232" s="1"/>
     </row>
     <row r="233" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C233" t="s">
+        <v>688</v>
+      </c>
+      <c r="D233" t="s">
+        <v>689</v>
+      </c>
+      <c r="F233" s="1"/>
+    </row>
+    <row r="234" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C234" t="s">
         <v>703</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D234" t="s">
         <v>704</v>
       </c>
-      <c r="F233" s="1" t="s">
+      <c r="F234" s="1" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="234" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F234" s="1"/>
     </row>
     <row r="235" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F235" s="1"/>
@@ -4664,130 +4726,130 @@
     <row r="237" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F237" s="1"/>
     </row>
-    <row r="239" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B239" t="s">
+    <row r="238" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F238" s="1"/>
+    </row>
+    <row r="240" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B240" t="s">
         <v>446</v>
-      </c>
-    </row>
-    <row r="240" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C240" t="s">
-        <v>613</v>
-      </c>
-      <c r="D240" t="s">
-        <v>612</v>
-      </c>
-      <c r="F240" s="1" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="241" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C241" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="D241" t="s">
-        <v>622</v>
+        <v>612</v>
       </c>
       <c r="F241" s="1" t="s">
-        <v>623</v>
+        <v>614</v>
       </c>
     </row>
     <row r="242" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C242" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D242" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="F242" s="1" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
     </row>
     <row r="243" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C243" t="s">
+        <v>625</v>
+      </c>
+      <c r="D243" t="s">
+        <v>624</v>
+      </c>
+      <c r="F243" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="244" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C244" t="s">
         <v>628</v>
       </c>
-      <c r="D243" t="s">
+      <c r="D244" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="250" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B250" t="s">
+    <row r="251" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B251" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="251" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C251" t="s">
-        <v>175</v>
-      </c>
-      <c r="D251" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="252" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C252" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="253" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C253" t="s">
-        <v>292</v>
+        <v>177</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>291</v>
+        <v>178</v>
       </c>
     </row>
     <row r="254" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C254" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="255" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C255" t="s">
+        <v>293</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="256" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C256" t="s">
         <v>296</v>
       </c>
-      <c r="D255" s="1" t="s">
+      <c r="D256" s="1" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="256" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D256" s="1"/>
     </row>
     <row r="257" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D257" s="1"/>
     </row>
     <row r="258" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B258" t="s">
+      <c r="D258" s="1"/>
+    </row>
+    <row r="259" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B259" t="s">
         <v>342</v>
       </c>
-      <c r="D258" s="1"/>
-    </row>
-    <row r="259" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C259" t="s">
+      <c r="D259" s="1"/>
+    </row>
+    <row r="260" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C260" t="s">
         <v>343</v>
       </c>
-      <c r="D259" t="s">
+      <c r="D260" t="s">
         <v>368</v>
       </c>
-      <c r="E259" s="1" t="s">
+      <c r="E260" s="1" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="260" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D260" t="s">
+    <row r="261" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D261" t="s">
         <v>367</v>
       </c>
-      <c r="E260" s="1" t="s">
+      <c r="E261" s="1" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="261" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D261" s="1"/>
     </row>
     <row r="262" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D262" s="1"/>
@@ -4795,115 +4857,115 @@
     <row r="263" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D263" s="1"/>
     </row>
-    <row r="267" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B267" t="s">
+    <row r="264" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D264" s="1"/>
+    </row>
+    <row r="268" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B268" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="268" spans="2:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="C268" s="3" t="s">
+    <row r="269" spans="2:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="C269" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D268" s="2" t="s">
+      <c r="D269" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E268" s="1" t="s">
+      <c r="E269" s="1" t="s">
         <v>185</v>
-      </c>
-    </row>
-    <row r="269" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C269" t="s">
-        <v>186</v>
-      </c>
-      <c r="E269" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="270" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C270" t="s">
+        <v>186</v>
+      </c>
+      <c r="E270" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="271" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C271" t="s">
         <v>214</v>
       </c>
-      <c r="E270" s="1" t="s">
+      <c r="E271" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="272" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D272" t="s">
+    <row r="273" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D273" t="s">
         <v>215</v>
-      </c>
-    </row>
-    <row r="274" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C274" t="s">
-        <v>241</v>
-      </c>
-      <c r="D274" t="s">
-        <v>242</v>
-      </c>
-      <c r="E274" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="275" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C275" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
       <c r="D275" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>270</v>
+        <v>243</v>
       </c>
     </row>
     <row r="276" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C276" t="s">
+        <v>268</v>
+      </c>
+      <c r="D276" t="s">
+        <v>269</v>
+      </c>
+      <c r="E276" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="277" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C277" t="s">
         <v>283</v>
       </c>
-      <c r="E276" s="1" t="s">
+      <c r="E277" s="1" t="s">
         <v>284</v>
-      </c>
-    </row>
-    <row r="277" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E277" s="1" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="278" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E278" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="279" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E279" s="1" t="s">
         <v>286</v>
-      </c>
-    </row>
-    <row r="279" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C279" t="s">
-        <v>287</v>
-      </c>
-      <c r="E279" s="1" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="280" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C280" t="s">
+        <v>287</v>
+      </c>
+      <c r="E280" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="281" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C281" t="s">
         <v>298</v>
       </c>
-      <c r="E280" s="1" t="s">
+      <c r="E281" s="1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="281" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E281" s="1"/>
-    </row>
     <row r="282" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C282" t="s">
+      <c r="E282" s="1"/>
+    </row>
+    <row r="283" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C283" t="s">
         <v>358</v>
       </c>
-      <c r="D282" t="s">
+      <c r="D283" t="s">
         <v>359</v>
       </c>
-      <c r="E282" s="1" t="s">
+      <c r="E283" s="1" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="283" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E283" s="1"/>
     </row>
     <row r="284" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E284" s="1"/>
@@ -4927,1418 +4989,1421 @@
       <c r="E290" s="1"/>
     </row>
     <row r="291" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C291" t="s">
+      <c r="E291" s="1"/>
+    </row>
+    <row r="292" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C292" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="292" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D292" t="s">
-        <v>134</v>
-      </c>
-      <c r="E292" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="293" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D293" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E293" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="294" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D294" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E294" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="295" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D295" t="s">
-        <v>136</v>
+        <v>139</v>
+      </c>
+      <c r="E295" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="296" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D296" t="s">
-        <v>141</v>
-      </c>
-      <c r="E296" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="297" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D297" t="s">
-        <v>482</v>
+        <v>141</v>
       </c>
       <c r="E297" t="s">
-        <v>484</v>
-      </c>
-      <c r="F297" t="s">
-        <v>488</v>
-      </c>
-      <c r="G297" t="s">
-        <v>483</v>
-      </c>
-      <c r="H297" s="1" t="s">
-        <v>489</v>
+        <v>142</v>
       </c>
     </row>
     <row r="298" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D298" t="s">
+        <v>482</v>
+      </c>
+      <c r="E298" t="s">
+        <v>484</v>
+      </c>
+      <c r="F298" t="s">
+        <v>488</v>
+      </c>
+      <c r="G298" t="s">
+        <v>483</v>
+      </c>
+      <c r="H298" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="299" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D299" t="s">
         <v>485</v>
       </c>
-      <c r="E298" t="s">
+      <c r="E299" t="s">
         <v>486</v>
       </c>
-      <c r="G298" t="s">
+      <c r="G299" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="300" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C300" t="s">
+    <row r="301" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C301" t="s">
         <v>366</v>
-      </c>
-    </row>
-    <row r="301" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D301" t="s">
-        <v>72</v>
-      </c>
-      <c r="E301" t="s">
-        <v>73</v>
-      </c>
-      <c r="F301" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="302" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D302" t="s">
-        <v>75</v>
-      </c>
-      <c r="E302" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="E302" t="s">
+        <v>73</v>
+      </c>
+      <c r="F302" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="303" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D303" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E303" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="304" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D304" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E304" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="305" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D305" t="s">
-        <v>361</v>
-      </c>
-      <c r="E305" t="s">
-        <v>364</v>
+        <v>80</v>
+      </c>
+      <c r="E305" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="306" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D306" t="s">
+        <v>361</v>
+      </c>
+      <c r="E306" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="307" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D307" t="s">
         <v>362</v>
       </c>
-      <c r="E306" t="s">
+      <c r="E307" t="s">
         <v>363</v>
-      </c>
-    </row>
-    <row r="308" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D308" t="s">
-        <v>81</v>
-      </c>
-      <c r="E308" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="309" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D309" t="s">
+        <v>81</v>
+      </c>
+      <c r="E309" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="310" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D310" t="s">
         <v>83</v>
       </c>
-      <c r="E309" t="s">
+      <c r="E310" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="311" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C311" t="s">
+    <row r="312" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C312" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="312" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D312" t="s">
-        <v>72</v>
-      </c>
-      <c r="E312" t="s">
-        <v>130</v>
-      </c>
-      <c r="F312" s="1"/>
     </row>
     <row r="313" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D313" t="s">
-        <v>146</v>
-      </c>
-      <c r="E313" s="1" t="s">
-        <v>147</v>
+        <v>72</v>
+      </c>
+      <c r="E313" t="s">
+        <v>130</v>
       </c>
       <c r="F313" s="1"/>
     </row>
     <row r="314" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D314" t="s">
+        <v>146</v>
+      </c>
+      <c r="E314" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F314" s="1"/>
+    </row>
+    <row r="315" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D315" t="s">
         <v>75</v>
       </c>
-      <c r="E314" s="1" t="s">
+      <c r="E315" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="315" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E315" s="1"/>
-    </row>
     <row r="316" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D316" t="s">
+      <c r="E316" s="1"/>
+    </row>
+    <row r="317" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D317" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="317" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E317" t="s">
-        <v>150</v>
-      </c>
-      <c r="F317" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="318" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E318" t="s">
+        <v>150</v>
+      </c>
+      <c r="F318" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="319" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E319" t="s">
         <v>151</v>
       </c>
-      <c r="F318" t="s">
+      <c r="F319" t="s">
         <v>144</v>
       </c>
-      <c r="G318" s="1" t="s">
+      <c r="G319" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="319" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D319" t="s">
+    <row r="320" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D320" t="s">
         <v>152</v>
       </c>
-      <c r="E319" s="1" t="s">
+      <c r="E320" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G319" s="1"/>
-    </row>
-    <row r="333" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E333" s="1"/>
-    </row>
-    <row r="335" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B335" t="s">
+      <c r="G320" s="1"/>
+    </row>
+    <row r="334" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E334" s="1"/>
+    </row>
+    <row r="336" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B336" t="s">
         <v>275</v>
-      </c>
-    </row>
-    <row r="336" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C336" t="s">
-        <v>276</v>
-      </c>
-      <c r="D336" t="s">
-        <v>278</v>
-      </c>
-      <c r="E336" s="1" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="337" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C337" t="s">
-        <v>280</v>
+        <v>276</v>
+      </c>
+      <c r="D337" t="s">
+        <v>278</v>
       </c>
       <c r="E337" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F337" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="G337" s="1" t="s">
-        <v>313</v>
+        <v>277</v>
       </c>
     </row>
     <row r="338" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C338" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="E338" s="1" t="s">
-        <v>290</v>
+        <v>279</v>
+      </c>
+      <c r="F338" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="G338" s="1" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="339" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C339" t="s">
+        <v>289</v>
+      </c>
+      <c r="E339" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="340" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C340" t="s">
         <v>303</v>
       </c>
-      <c r="E339" s="1" t="s">
+      <c r="E340" s="1" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="340" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D340" t="s">
+    <row r="341" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D341" t="s">
         <v>305</v>
       </c>
-      <c r="E340" s="1" t="s">
+      <c r="E341" s="1" t="s">
         <v>306</v>
-      </c>
-    </row>
-    <row r="341" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C341" t="s">
-        <v>323</v>
-      </c>
-      <c r="E341" s="1" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="342" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C342" t="s">
-        <v>307</v>
-      </c>
-      <c r="D342" t="s">
-        <v>308</v>
+        <v>323</v>
       </c>
       <c r="E342" s="1" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
     </row>
     <row r="343" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C343" t="s">
-        <v>310</v>
+        <v>307</v>
+      </c>
+      <c r="D343" t="s">
+        <v>308</v>
       </c>
       <c r="E343" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="344" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C344" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="E344" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="345" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C345" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E345" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="346" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C346" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E346" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="347" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C347" t="s">
+        <v>318</v>
+      </c>
+      <c r="E347" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="348" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C348" t="s">
         <v>325</v>
       </c>
-      <c r="D347" t="s">
+      <c r="D348" t="s">
         <v>332</v>
       </c>
-      <c r="E347" s="1" t="s">
+      <c r="E348" s="1" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="348" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D348" t="s">
+    <row r="349" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D349" t="s">
         <v>327</v>
       </c>
-      <c r="E348" s="1" t="s">
+      <c r="E349" s="1" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="350" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C350" t="s">
+    <row r="351" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C351" t="s">
         <v>329</v>
       </c>
-      <c r="D350" t="s">
+      <c r="D351" t="s">
         <v>330</v>
       </c>
-      <c r="E350" s="1" t="s">
+      <c r="E351" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="352" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C352" t="s">
+    <row r="353" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C353" t="s">
         <v>335</v>
       </c>
-      <c r="D352" t="s">
+      <c r="D353" t="s">
         <v>337</v>
       </c>
-      <c r="E352" s="1" t="s">
+      <c r="E353" s="1" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="356" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B356" t="s">
+    <row r="357" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B357" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="357" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C357" t="s">
+    <row r="358" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C358" t="s">
         <v>341</v>
       </c>
-      <c r="D357" t="s">
+      <c r="D358" t="s">
         <v>339</v>
       </c>
-      <c r="E357" s="1" t="s">
+      <c r="E358" s="1" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="363" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B363" t="s">
+    <row r="364" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B364" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="364" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C364" t="s">
-        <v>86</v>
-      </c>
-      <c r="D364" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="365" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C365" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D365" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="366" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C366" t="s">
-        <v>95</v>
-      </c>
-      <c r="D366" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
+      </c>
+      <c r="D366" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="367" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C367" t="s">
+        <v>95</v>
+      </c>
+      <c r="D367" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="368" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C368" t="s">
         <v>97</v>
       </c>
-      <c r="D367" s="1" t="s">
+      <c r="D368" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="369" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B369" t="s">
+    <row r="370" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B370" t="s">
         <v>90</v>
       </c>
-      <c r="C369" t="s">
+      <c r="C370" t="s">
         <v>91</v>
       </c>
-      <c r="D369" t="s">
+      <c r="D370" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="370" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C370" t="s">
+    <row r="371" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C371" t="s">
         <v>93</v>
       </c>
-      <c r="D370" t="s">
+      <c r="D371" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="373" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B373" t="s">
+    <row r="374" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B374" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="374" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C374" t="s">
+    <row r="375" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C375" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="375" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D375" t="s">
+    <row r="376" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D376" t="s">
         <v>104</v>
       </c>
-      <c r="E375" s="1" t="s">
+      <c r="E376" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="376" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D376" t="s">
+    <row r="377" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D377" t="s">
         <v>101</v>
       </c>
-      <c r="E376" s="1" t="s">
+      <c r="E377" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="377" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D377" t="s">
+    <row r="378" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D378" t="s">
         <v>102</v>
       </c>
-      <c r="E377" s="1" t="s">
+      <c r="E378" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="378" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D378" t="s">
+    <row r="379" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D379" t="s">
         <v>107</v>
       </c>
-      <c r="E378" t="s">
+      <c r="E379" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="380" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B380" t="s">
+    <row r="381" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B381" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="381" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C381" t="s">
+    <row r="382" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C382" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="382" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D382" t="s">
+    <row r="383" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D383" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="383" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D383" t="s">
+    <row r="384" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D384" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="384" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F384" s="1" t="s">
+    <row r="385" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F385" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="385" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B385" t="s">
+    <row r="386" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B386" t="s">
         <v>1</v>
       </c>
-      <c r="F385" s="1" t="s">
+      <c r="F386" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="386" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C386" t="s">
+    <row r="387" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C387" t="s">
         <v>112</v>
       </c>
-      <c r="D386" s="1" t="s">
+      <c r="D387" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="387" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D387" t="s">
+    <row r="388" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D388" t="s">
         <v>126</v>
       </c>
-      <c r="E387" s="1" t="s">
+      <c r="E388" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="388" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C388" t="s">
+    <row r="389" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C389" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="389" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D389" t="s">
+    <row r="390" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D390" t="s">
         <v>115</v>
       </c>
-      <c r="E389" s="1" t="s">
+      <c r="E390" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F389" t="s">
+      <c r="F390" t="s">
         <v>128</v>
       </c>
-      <c r="G389" s="1" t="s">
+      <c r="G390" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="390" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E390" t="s">
-        <v>121</v>
-      </c>
-      <c r="G390" s="1"/>
     </row>
     <row r="391" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E391" t="s">
+        <v>121</v>
+      </c>
+      <c r="G391" s="1"/>
+    </row>
+    <row r="392" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E392" t="s">
         <v>124</v>
-      </c>
-      <c r="G391" s="1"/>
-    </row>
-    <row r="392" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D392" t="s">
-        <v>117</v>
-      </c>
-      <c r="E392" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="G392" s="1"/>
     </row>
     <row r="393" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D393" t="s">
+        <v>117</v>
+      </c>
+      <c r="E393" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G393" s="1"/>
+    </row>
+    <row r="394" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D394" t="s">
         <v>119</v>
       </c>
-      <c r="E393" s="1" t="s">
+      <c r="E394" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G393" s="1"/>
-    </row>
-    <row r="394" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E394" s="1" t="s">
+      <c r="G394" s="1"/>
+    </row>
+    <row r="395" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E395" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="G394" s="1"/>
-    </row>
-    <row r="395" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E395" t="s">
+      <c r="G395" s="1"/>
+    </row>
+    <row r="396" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E396" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="396" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D396" t="s">
-        <v>301</v>
-      </c>
-      <c r="E396" s="1" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="397" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D397" t="s">
+        <v>301</v>
+      </c>
+      <c r="E397" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="398" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D398" t="s">
         <v>300</v>
       </c>
-      <c r="E397" s="1" t="s">
+      <c r="E398" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="402" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C402" t="s">
+    <row r="403" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C403" t="s">
         <v>131</v>
       </c>
-      <c r="D402" s="1" t="s">
+      <c r="D403" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="406" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B406" t="s">
+    <row r="407" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B407" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="407" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C407" t="s">
+    <row r="408" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C408" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="408" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D408" t="s">
+    <row r="409" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D409" t="s">
         <v>493</v>
-      </c>
-    </row>
-    <row r="409" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E409" t="s">
-        <v>492</v>
-      </c>
-      <c r="F409" s="1" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="410" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E410" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="F410" s="1" t="s">
-        <v>511</v>
+        <v>491</v>
       </c>
     </row>
     <row r="411" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E411" t="s">
+        <v>494</v>
+      </c>
+      <c r="F411" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="412" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E412" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="412" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D412" t="s">
+    <row r="413" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D413" t="s">
         <v>496</v>
-      </c>
-    </row>
-    <row r="413" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E413" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="414" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E414" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="415" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E415" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="415" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D415" t="s">
+    <row r="416" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D416" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="416" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E416" t="s">
+    <row r="417" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E417" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="417" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C417" t="s">
+    <row r="418" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C418" t="s">
         <v>500</v>
-      </c>
-    </row>
-    <row r="418" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D418" t="s">
-        <v>503</v>
-      </c>
-      <c r="E418" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="419" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D419" t="s">
+        <v>503</v>
+      </c>
+      <c r="E419" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="420" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D420" t="s">
         <v>501</v>
       </c>
-      <c r="E419" t="s">
+      <c r="E420" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="421" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C421" t="s">
+    <row r="422" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C422" t="s">
         <v>505</v>
-      </c>
-    </row>
-    <row r="422" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D422" t="s">
-        <v>508</v>
-      </c>
-      <c r="E422" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="423" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D423" t="s">
+        <v>508</v>
+      </c>
+      <c r="E423" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="424" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D424" t="s">
         <v>509</v>
       </c>
-      <c r="E423" t="s">
+      <c r="E424" t="s">
         <v>507</v>
       </c>
-      <c r="G423" s="1" t="s">
+      <c r="G424" s="1" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="425" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C425" t="s">
+    <row r="426" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C426" t="s">
         <v>512</v>
       </c>
-      <c r="G425" s="1" t="s">
+      <c r="G426" s="1" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="427" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C427" t="s">
+    <row r="428" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C428" t="s">
         <v>513</v>
       </c>
-      <c r="E427" t="s">
+      <c r="E428" t="s">
         <v>514</v>
       </c>
-      <c r="G427" s="1" t="s">
+      <c r="G428" s="1" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="429" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C429" t="s">
+    <row r="430" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C430" t="s">
         <v>516</v>
-      </c>
-    </row>
-    <row r="430" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D430" t="s">
-        <v>518</v>
-      </c>
-      <c r="E430" t="s">
-        <v>517</v>
-      </c>
-      <c r="G430" s="1" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="431" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D431" t="s">
+        <v>518</v>
+      </c>
+      <c r="E431" t="s">
+        <v>517</v>
+      </c>
+      <c r="G431" s="1" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="432" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D432" t="s">
         <v>519</v>
       </c>
-      <c r="E431" t="s">
+      <c r="E432" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="433" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C433" t="s">
+    <row r="434" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C434" t="s">
         <v>522</v>
-      </c>
-    </row>
-    <row r="434" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D434" t="s">
-        <v>528</v>
-      </c>
-      <c r="E434" t="s">
-        <v>524</v>
-      </c>
-      <c r="G434" s="1" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="435" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D435" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="E435" t="s">
-        <v>523</v>
+        <v>524</v>
+      </c>
+      <c r="G435" s="1" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="436" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D436" t="s">
+        <v>526</v>
+      </c>
+      <c r="E436" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="437" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D437" t="s">
         <v>527</v>
       </c>
-      <c r="E436" t="s">
+      <c r="E437" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="437" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C437" t="s">
+    <row r="438" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C438" t="s">
         <v>629</v>
-      </c>
-    </row>
-    <row r="438" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D438" t="s">
-        <v>630</v>
-      </c>
-      <c r="E438" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="439" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D439" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="E439" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="440" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D440" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E440" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="441" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D441" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="E441" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="442" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D442" t="s">
+        <v>637</v>
+      </c>
+      <c r="E442" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="443" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D443" t="s">
         <v>693</v>
       </c>
-      <c r="E442" t="s">
+      <c r="E443" t="s">
         <v>695</v>
       </c>
-      <c r="G442" s="1" t="s">
+      <c r="G443" s="1" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="445" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B445" t="s">
+    <row r="446" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B446" t="s">
         <v>778</v>
       </c>
     </row>
-    <row r="446" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C446" t="s">
+    <row r="447" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C447" t="s">
         <v>779</v>
       </c>
-      <c r="G446" s="1" t="s">
+      <c r="G447" s="1" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="455" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B455" t="s">
+    <row r="456" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B456" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="456" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C456" t="s">
+    <row r="457" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C457" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="457" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D457" t="s">
+    <row r="458" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D458" t="s">
         <v>541</v>
       </c>
-      <c r="G457" s="1" t="s">
+      <c r="G458" s="1" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="458" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C458" t="s">
+    <row r="459" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C459" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="459" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D459" t="s">
+    <row r="460" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D460" t="s">
         <v>543</v>
       </c>
-      <c r="E459" t="s">
+      <c r="E460" t="s">
         <v>544</v>
       </c>
-      <c r="G459" s="1" t="s">
+      <c r="G460" s="1" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="461" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C461" t="s">
+    <row r="462" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C462" t="s">
         <v>547</v>
-      </c>
-    </row>
-    <row r="462" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D462" t="s">
-        <v>548</v>
-      </c>
-      <c r="E462" t="s">
-        <v>549</v>
-      </c>
-      <c r="G462" s="1" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="463" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D463" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="E463" t="s">
-        <v>551</v>
+        <v>549</v>
+      </c>
+      <c r="G463" s="1" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="464" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D464" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E464" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="465" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D465" t="s">
+        <v>552</v>
+      </c>
+      <c r="E465" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="466" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D466" t="s">
         <v>554</v>
       </c>
-      <c r="E465" t="s">
+      <c r="E466" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="467" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C467" t="s">
+    <row r="468" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C468" t="s">
         <v>557</v>
-      </c>
-    </row>
-    <row r="468" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D468" t="s">
-        <v>558</v>
-      </c>
-      <c r="E468" t="s">
-        <v>560</v>
-      </c>
-      <c r="G468" s="1" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="469" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D469" t="s">
+        <v>558</v>
+      </c>
+      <c r="E469" t="s">
+        <v>560</v>
+      </c>
+      <c r="G469" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="470" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D470" t="s">
         <v>559</v>
       </c>
-      <c r="E469" t="s">
+      <c r="E470" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="471" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C471" t="s">
+    <row r="472" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C472" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="472" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D472" t="s">
+    <row r="473" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D473" t="s">
         <v>565</v>
       </c>
-      <c r="G472" s="1" t="s">
+      <c r="G473" s="1" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="473" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C473" t="s">
+    <row r="474" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C474" t="s">
         <v>608</v>
       </c>
-      <c r="G473" s="1"/>
-    </row>
-    <row r="474" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D474" t="s">
+      <c r="G474" s="1"/>
+    </row>
+    <row r="475" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D475" t="s">
         <v>609</v>
       </c>
-      <c r="E474" t="s">
+      <c r="E475" t="s">
         <v>610</v>
       </c>
-      <c r="G474" s="1" t="s">
+      <c r="G475" s="1" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="475" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="G475" s="1"/>
-    </row>
     <row r="476" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C476" t="s">
+      <c r="G476" s="1"/>
+    </row>
+    <row r="477" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C477" t="s">
         <v>836</v>
       </c>
-      <c r="G476" s="1"/>
-    </row>
-    <row r="477" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D477" t="s">
+      <c r="G477" s="1"/>
+    </row>
+    <row r="478" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D478" t="s">
         <v>837</v>
       </c>
-      <c r="G477" s="1" t="s">
+      <c r="G478" s="1" t="s">
         <v>838</v>
       </c>
     </row>
-    <row r="478" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C478" t="s">
+    <row r="479" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C479" t="s">
         <v>892</v>
       </c>
-      <c r="G478" s="1"/>
-    </row>
-    <row r="479" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D479" t="s">
+      <c r="G479" s="1"/>
+    </row>
+    <row r="480" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D480" t="s">
         <v>893</v>
       </c>
-      <c r="G479" s="1" t="s">
+      <c r="G480" s="1" t="s">
         <v>894</v>
       </c>
     </row>
-    <row r="480" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="G480" s="1"/>
-    </row>
-    <row r="483" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B483" t="s">
+    <row r="481" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G481" s="1"/>
+    </row>
+    <row r="484" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B484" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="484" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C484" t="s">
+    <row r="485" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C485" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="485" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E485" t="s">
+    <row r="486" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E486" t="s">
         <v>568</v>
       </c>
-      <c r="G485" s="1" t="s">
+      <c r="G486" s="1" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="488" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B488" t="s">
+    <row r="489" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B489" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="489" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C489" t="s">
+    <row r="490" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C490" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="490" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D490" t="s">
+    <row r="491" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D491" t="s">
         <v>572</v>
       </c>
-      <c r="E490" t="s">
+      <c r="E491" t="s">
         <v>573</v>
       </c>
-      <c r="F490" t="s">
+      <c r="F491" t="s">
         <v>574</v>
       </c>
-      <c r="G490" s="1" t="s">
+      <c r="G491" s="1" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="491" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E491" t="s">
+    <row r="492" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E492" t="s">
         <v>576</v>
       </c>
-      <c r="F491" t="s">
+      <c r="F492" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="492" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C492" t="s">
+    <row r="493" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C493" t="s">
         <v>594</v>
-      </c>
-    </row>
-    <row r="493" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D493" t="s">
-        <v>595</v>
-      </c>
-      <c r="E493" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="494" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D494" t="s">
+        <v>595</v>
+      </c>
+      <c r="E494" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="495" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D495" t="s">
         <v>598</v>
       </c>
-      <c r="E494" t="s">
+      <c r="E495" t="s">
         <v>597</v>
-      </c>
-    </row>
-    <row r="496" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D496" t="s">
-        <v>599</v>
-      </c>
-      <c r="E496" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="497" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D497" t="s">
+        <v>599</v>
+      </c>
+      <c r="E497" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="498" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D498" t="s">
         <v>601</v>
       </c>
-      <c r="E497" t="s">
+      <c r="E498" t="s">
         <v>602</v>
-      </c>
-    </row>
-    <row r="499" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D499" t="s">
-        <v>840</v>
-      </c>
-      <c r="E499" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="500" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D500" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="E500" t="s">
-        <v>603</v>
-      </c>
-      <c r="G500" s="1" t="s">
-        <v>607</v>
+        <v>839</v>
       </c>
     </row>
     <row r="501" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D501" t="s">
+        <v>841</v>
+      </c>
+      <c r="E501" t="s">
+        <v>603</v>
+      </c>
+      <c r="G501" s="1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="502" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D502" t="s">
         <v>604</v>
       </c>
-      <c r="E501" t="s">
+      <c r="E502" t="s">
         <v>605</v>
       </c>
-      <c r="F501" t="s">
+      <c r="F502" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="503" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D503" t="s">
+    <row r="504" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D504" t="s">
         <v>842</v>
       </c>
-      <c r="E503" t="s">
+      <c r="E504" t="s">
         <v>851</v>
       </c>
-      <c r="F503" t="s">
+      <c r="F504" t="s">
         <v>853</v>
       </c>
-      <c r="H503" s="1" t="s">
+      <c r="H504" s="1" t="s">
         <v>852</v>
       </c>
     </row>
-    <row r="504" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E504" t="s">
+    <row r="505" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E505" t="s">
         <v>850</v>
       </c>
-      <c r="F504" t="s">
+      <c r="F505" t="s">
         <v>843</v>
       </c>
-      <c r="G504" t="s">
+      <c r="G505" t="s">
         <v>844</v>
       </c>
-      <c r="H504" s="1" t="s">
+      <c r="H505" s="1" t="s">
         <v>845</v>
       </c>
     </row>
-    <row r="505" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="G505" s="1"/>
-    </row>
     <row r="506" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D506" t="s">
+      <c r="G506" s="1"/>
+    </row>
+    <row r="507" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D507" t="s">
         <v>846</v>
       </c>
-      <c r="E506" t="s">
+      <c r="E507" t="s">
         <v>847</v>
       </c>
-      <c r="G506" s="1" t="s">
+      <c r="G507" s="1" t="s">
         <v>849</v>
       </c>
     </row>
-    <row r="507" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E507" t="s">
+    <row r="508" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E508" t="s">
         <v>848</v>
       </c>
-      <c r="G507" s="1"/>
-    </row>
-    <row r="508" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C508" t="s">
+      <c r="G508" s="1"/>
+    </row>
+    <row r="509" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C509" t="s">
         <v>862</v>
-      </c>
-      <c r="G508" s="1"/>
-    </row>
-    <row r="509" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D509" t="s">
-        <v>863</v>
-      </c>
-      <c r="E509" t="s">
-        <v>574</v>
       </c>
       <c r="G509" s="1"/>
     </row>
     <row r="510" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D510" t="s">
+        <v>863</v>
+      </c>
+      <c r="E510" t="s">
+        <v>574</v>
+      </c>
+      <c r="G510" s="1"/>
+    </row>
+    <row r="511" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D511" t="s">
         <v>864</v>
       </c>
-      <c r="E510" t="s">
+      <c r="E511" t="s">
         <v>577</v>
       </c>
-      <c r="G510" s="1"/>
-    </row>
-    <row r="511" spans="3:8" x14ac:dyDescent="0.2">
       <c r="G511" s="1"/>
     </row>
-    <row r="513" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B513" t="s">
+    <row r="512" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="G512" s="1"/>
+    </row>
+    <row r="514" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B514" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="514" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C514" t="s">
+    <row r="515" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C515" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="515" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D515" t="s">
+    <row r="516" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D516" t="s">
         <v>581</v>
       </c>
-      <c r="E515" t="s">
+      <c r="E516" t="s">
         <v>582</v>
       </c>
-      <c r="F515" t="s">
+      <c r="F516" t="s">
         <v>580</v>
       </c>
-      <c r="G515" s="1" t="s">
+      <c r="G516" s="1" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="516" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E516" t="s">
+    <row r="517" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E517" t="s">
         <v>583</v>
       </c>
-      <c r="F516" t="s">
+      <c r="F517" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="518" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D518" t="s">
+    <row r="519" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D519" t="s">
         <v>586</v>
       </c>
-      <c r="E518" t="s">
+      <c r="E519" t="s">
         <v>588</v>
       </c>
-      <c r="F518" t="s">
+      <c r="F519" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="521" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B521" t="s">
+    <row r="522" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B522" t="s">
         <v>706</v>
-      </c>
-    </row>
-    <row r="522" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C522" t="s">
-        <v>707</v>
-      </c>
-      <c r="D522" t="s">
-        <v>710</v>
-      </c>
-      <c r="G522" s="1" t="s">
-        <v>713</v>
       </c>
     </row>
     <row r="523" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C523" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D523" t="s">
-        <v>711</v>
+        <v>710</v>
+      </c>
+      <c r="G523" s="1" t="s">
+        <v>713</v>
       </c>
     </row>
     <row r="524" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C524" t="s">
+        <v>708</v>
+      </c>
+      <c r="D524" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="525" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C525" t="s">
         <v>709</v>
       </c>
-      <c r="D524" t="s">
+      <c r="D525" t="s">
         <v>712</v>
       </c>
     </row>
-    <row r="527" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B527" t="s">
+    <row r="528" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B528" t="s">
         <v>730</v>
-      </c>
-    </row>
-    <row r="528" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C528" t="s">
-        <v>731</v>
-      </c>
-      <c r="G528" s="1" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="529" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C529" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="G529" s="1" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="530" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C530" t="s">
+        <v>733</v>
+      </c>
+      <c r="G530" s="1" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="531" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C531" t="s">
         <v>737</v>
       </c>
-      <c r="F530" t="s">
+      <c r="F531" t="s">
         <v>735</v>
       </c>
-      <c r="G530" s="1" t="s">
+      <c r="G531" s="1" t="s">
         <v>736</v>
       </c>
     </row>
-    <row r="532" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B532" t="s">
+    <row r="533" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B533" t="s">
         <v>742</v>
-      </c>
-    </row>
-    <row r="533" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C533" t="s">
-        <v>743</v>
-      </c>
-      <c r="D533" t="s">
-        <v>744</v>
-      </c>
-      <c r="G533" s="1" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="534" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C534" t="s">
+        <v>743</v>
+      </c>
+      <c r="D534" t="s">
+        <v>744</v>
+      </c>
+      <c r="G534" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="535" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C535" t="s">
         <v>746</v>
       </c>
-      <c r="D534" t="s">
+      <c r="D535" t="s">
         <v>747</v>
       </c>
-      <c r="G534" s="1" t="s">
+      <c r="G535" s="1" t="s">
         <v>748</v>
       </c>
     </row>
-    <row r="538" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B538" t="s">
+    <row r="539" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B539" t="s">
         <v>801</v>
-      </c>
-    </row>
-    <row r="539" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C539" t="s">
-        <v>802</v>
-      </c>
-      <c r="D539" t="s">
-        <v>803</v>
-      </c>
-      <c r="E539" t="s">
-        <v>804</v>
-      </c>
-      <c r="G539" s="1" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="540" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C540" t="s">
+        <v>802</v>
+      </c>
+      <c r="D540" t="s">
+        <v>803</v>
+      </c>
+      <c r="E540" t="s">
+        <v>804</v>
+      </c>
+      <c r="G540" s="1" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="541" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C541" t="s">
         <v>806</v>
       </c>
-      <c r="E540" t="s">
+      <c r="E541" t="s">
         <v>807</v>
       </c>
     </row>
-    <row r="542" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B542" t="s">
+    <row r="543" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B543" t="s">
         <v>854</v>
       </c>
-      <c r="G542" s="1" t="s">
+      <c r="G543" s="1" t="s">
         <v>861</v>
       </c>
     </row>
-    <row r="543" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C543" t="s">
+    <row r="544" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C544" t="s">
         <v>855</v>
       </c>
     </row>
-    <row r="544" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D544" t="s">
+    <row r="545" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D545" t="s">
         <v>858</v>
       </c>
     </row>
-    <row r="545" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C545" t="s">
+    <row r="546" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C546" t="s">
         <v>856</v>
       </c>
     </row>
-    <row r="546" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D546" t="s">
+    <row r="547" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D547" t="s">
         <v>859</v>
       </c>
     </row>
-    <row r="547" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C547" t="s">
+    <row r="548" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C548" t="s">
         <v>857</v>
       </c>
     </row>
-    <row r="548" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D548" t="s">
+    <row r="549" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D549" t="s">
         <v>860</v>
       </c>
     </row>
-    <row r="551" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B551" t="s">
+    <row r="552" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B552" t="s">
         <v>876</v>
       </c>
     </row>
-    <row r="552" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C552" t="s">
+    <row r="553" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C553" t="s">
         <v>877</v>
       </c>
-      <c r="D552" t="s">
+      <c r="D553" t="s">
         <v>878</v>
       </c>
-      <c r="G552" s="1" t="s">
+      <c r="G553" s="1" t="s">
         <v>879</v>
       </c>
     </row>
@@ -6346,172 +6411,173 @@
   <hyperlinks>
     <hyperlink ref="C15" r:id="rId1" xr:uid="{18CCA2F1-1074-664C-AB52-48BBB42F9065}"/>
     <hyperlink ref="D18" r:id="rId2" xr:uid="{02227101-F5A2-3446-ADC1-32F3342C625C}"/>
-    <hyperlink ref="D55" r:id="rId3" xr:uid="{6360CC1D-0E6F-6B45-B16E-E9F323959E32}"/>
-    <hyperlink ref="E67" r:id="rId4" xr:uid="{96980E2B-5D77-D04D-8463-2374C6B90C21}"/>
-    <hyperlink ref="E84" r:id="rId5" xr:uid="{5081034D-5E40-F340-99D2-B8E4DFC0468C}"/>
-    <hyperlink ref="E87" r:id="rId6" location=":~:text=You%20can%20verify%20whether%20it,password%20and%20ESSID%20are%20correct." xr:uid="{3BA51E9E-8709-874E-B6EC-40074894ACA9}"/>
-    <hyperlink ref="E82" r:id="rId7" xr:uid="{30BD9D61-AAB4-2544-987A-0386CA068398}"/>
-    <hyperlink ref="E90" r:id="rId8" xr:uid="{1824F9BF-1BD9-3842-A565-00C06FF5E50F}"/>
-    <hyperlink ref="D161" r:id="rId9" xr:uid="{E488AECD-B504-A04E-8F27-807A3A08802C}"/>
-    <hyperlink ref="D115" r:id="rId10" location="89804" xr:uid="{E34C14F5-E723-0A48-894F-222B3F74BBF9}"/>
-    <hyperlink ref="D116" r:id="rId11" xr:uid="{6C20672B-9F8F-094F-9AC8-3D1FC1C85319}"/>
-    <hyperlink ref="D117" r:id="rId12" xr:uid="{BA9A8F05-4D7F-4942-886C-F8152208F0EA}"/>
-    <hyperlink ref="F121" r:id="rId13" xr:uid="{22AE585F-7255-3F41-8A2E-808446F3A9AA}"/>
-    <hyperlink ref="F123" r:id="rId14" xr:uid="{93472772-CF6C-D045-B634-2D574A3EE034}"/>
-    <hyperlink ref="E219" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
-    <hyperlink ref="F220" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
-    <hyperlink ref="D251" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
-    <hyperlink ref="D252" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
-    <hyperlink ref="F124" r:id="rId19" xr:uid="{92BE3560-5393-C545-9D2D-2B773359B28F}"/>
-    <hyperlink ref="E268" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
-    <hyperlink ref="E269" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
-    <hyperlink ref="E270" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
-    <hyperlink ref="E98" r:id="rId23" xr:uid="{1526D7DA-27DA-1443-928C-BEDA9E425734}"/>
-    <hyperlink ref="E99" r:id="rId24" xr:uid="{4F363062-BE49-AB4F-8956-2C1F31D9B898}"/>
-    <hyperlink ref="H125" r:id="rId25" xr:uid="{D9E13355-D59B-054F-B544-34A5A285A9E0}"/>
-    <hyperlink ref="G93" r:id="rId26" xr:uid="{170917BF-0643-9848-BCA9-A3BF5219EE3E}"/>
-    <hyperlink ref="F128" r:id="rId27" xr:uid="{5D45F2D3-11BC-6E43-BEFF-29E4E04A041E}"/>
-    <hyperlink ref="I129" r:id="rId28" xr:uid="{7D985D09-6A9A-FF4D-9F4A-4C56CC604DCE}"/>
-    <hyperlink ref="D118" r:id="rId29" xr:uid="{784C3F11-339F-8242-911D-6E4E893DD319}"/>
-    <hyperlink ref="E118" r:id="rId30" xr:uid="{FC907203-09BF-654B-9028-A8528783DAFE}"/>
-    <hyperlink ref="F130" r:id="rId31" xr:uid="{EFD3653A-B2F2-614F-8DEE-A2CB34111C94}"/>
-    <hyperlink ref="F131" r:id="rId32" xr:uid="{774B592D-11A5-9C49-BB9A-61014C8D8C81}"/>
-    <hyperlink ref="F132" r:id="rId33" xr:uid="{BD793670-4C63-C04D-B52D-974AF8E59FA4}"/>
-    <hyperlink ref="F133" r:id="rId34" location="96077" xr:uid="{B9804BBD-5312-714B-97EA-CC7D2C647F2C}"/>
-    <hyperlink ref="H126" r:id="rId35" xr:uid="{7BC5BAB5-D297-0043-BAAF-45AD255D5C84}"/>
-    <hyperlink ref="I125" r:id="rId36" xr:uid="{A03C56E4-1156-A148-A568-F50A5C33DB5C}"/>
-    <hyperlink ref="F134" r:id="rId37" xr:uid="{12AC219C-4678-4E43-B328-6595FA10B8D3}"/>
-    <hyperlink ref="E136" r:id="rId38" xr:uid="{44409621-28A2-704A-B283-3DCE1EFB1603}"/>
-    <hyperlink ref="E274" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
-    <hyperlink ref="F137" r:id="rId40" xr:uid="{A9D0D792-87D1-8144-872F-5CA060D3C28F}"/>
-    <hyperlink ref="F138" r:id="rId41" xr:uid="{87EF989D-17E9-1E45-A075-CD862D0B60F4}"/>
-    <hyperlink ref="F140" r:id="rId42" xr:uid="{8406C6F0-DC69-A64D-AAD8-60A33C12D00B}"/>
-    <hyperlink ref="F141" r:id="rId43" location="108593" xr:uid="{3C38F59E-6E71-4048-9BCA-CBC77D3907E0}"/>
-    <hyperlink ref="F143" r:id="rId44" xr:uid="{EEBE2A3E-36CA-F94F-9B1D-EE463DB6425F}"/>
-    <hyperlink ref="F144" r:id="rId45" xr:uid="{3782B43D-9E6F-2940-A013-34AA5D6B4DB3}"/>
-    <hyperlink ref="F145" r:id="rId46" xr:uid="{3D1C62DB-D9B7-BE42-B21D-4EEBC4C9EFE1}"/>
-    <hyperlink ref="F146" r:id="rId47" xr:uid="{F5021A21-70A2-D34E-B055-64CAC326E7EF}"/>
-    <hyperlink ref="F147" r:id="rId48" xr:uid="{A8C010A1-8EE1-264B-8688-3BEA1B62E535}"/>
-    <hyperlink ref="E275" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
-    <hyperlink ref="F142" r:id="rId50" location="113521" xr:uid="{EE1413C5-3B38-7D4D-8DF1-634A12F0BD81}"/>
-    <hyperlink ref="E100" r:id="rId51" xr:uid="{00B1EF4A-7791-0343-8D8C-9A1E83248FC9}"/>
-    <hyperlink ref="E336" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
-    <hyperlink ref="E337" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
-    <hyperlink ref="F149" r:id="rId54" xr:uid="{40A4B6A0-2F7E-A84D-8CC6-D814A33F5953}"/>
-    <hyperlink ref="E276" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
-    <hyperlink ref="E277" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
-    <hyperlink ref="E278" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
-    <hyperlink ref="E279" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
-    <hyperlink ref="E338" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
-    <hyperlink ref="D253" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
-    <hyperlink ref="D254" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
-    <hyperlink ref="D255" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
-    <hyperlink ref="E280" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
-    <hyperlink ref="E339" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
-    <hyperlink ref="E340" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
-    <hyperlink ref="E342" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
-    <hyperlink ref="E343" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
-    <hyperlink ref="F337" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
-    <hyperlink ref="G337" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
-    <hyperlink ref="E344" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
-    <hyperlink ref="E345" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
-    <hyperlink ref="E346" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
-    <hyperlink ref="E221" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
-    <hyperlink ref="E341" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
-    <hyperlink ref="E347" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
-    <hyperlink ref="E348" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
-    <hyperlink ref="E102" r:id="rId77" location="code" xr:uid="{C0475FF8-517D-E949-887E-9A42D86E9640}"/>
-    <hyperlink ref="E350" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
-    <hyperlink ref="E103" r:id="rId79" xr:uid="{277DBE6F-F3E5-8B4C-8DD8-BD92445D1A99}"/>
-    <hyperlink ref="E352" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
-    <hyperlink ref="E357" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
-    <hyperlink ref="E259" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
-    <hyperlink ref="E260" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
-    <hyperlink ref="F170" r:id="rId84" xr:uid="{EB604865-A16B-0646-A5B5-0D047467449D}"/>
-    <hyperlink ref="E282" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
-    <hyperlink ref="D366" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
-    <hyperlink ref="D367" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
-    <hyperlink ref="E376" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
-    <hyperlink ref="E377" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
-    <hyperlink ref="E375" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
-    <hyperlink ref="D386" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
-    <hyperlink ref="E392" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
-    <hyperlink ref="E389" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
-    <hyperlink ref="E393" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
-    <hyperlink ref="F384" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
-    <hyperlink ref="F385" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
-    <hyperlink ref="E387" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
-    <hyperlink ref="G389" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
-    <hyperlink ref="D402" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
-    <hyperlink ref="E394" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
-    <hyperlink ref="E397" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
-    <hyperlink ref="E396" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
-    <hyperlink ref="F301" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
-    <hyperlink ref="E302" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
-    <hyperlink ref="E303" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
-    <hyperlink ref="E304" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
-    <hyperlink ref="G318" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
-    <hyperlink ref="E313" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
-    <hyperlink ref="E314" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
-    <hyperlink ref="E319" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
-    <hyperlink ref="F182" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
-    <hyperlink ref="F187" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
-    <hyperlink ref="F188" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
-    <hyperlink ref="F195" r:id="rId114" xr:uid="{2B03B1F0-535A-3E4F-8FB3-35D2DE847218}"/>
-    <hyperlink ref="G200" r:id="rId115" xr:uid="{11045522-E183-B14C-B43D-5EA36E454600}"/>
-    <hyperlink ref="E222" r:id="rId116" xr:uid="{F1098A8C-3BC0-DB4F-8F9C-48B31145FEC1}"/>
-    <hyperlink ref="F202" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
-    <hyperlink ref="F196" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
-    <hyperlink ref="F205" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
-    <hyperlink ref="H297" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
-    <hyperlink ref="F409" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
-    <hyperlink ref="G423" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
-    <hyperlink ref="F410" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
-    <hyperlink ref="G425" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
-    <hyperlink ref="G427" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
-    <hyperlink ref="G430" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
-    <hyperlink ref="G434" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
-    <hyperlink ref="G459" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
-    <hyperlink ref="G457" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
-    <hyperlink ref="G462" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
-    <hyperlink ref="G468" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
-    <hyperlink ref="G472" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
-    <hyperlink ref="G485" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
-    <hyperlink ref="G490" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
-    <hyperlink ref="G515" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
-    <hyperlink ref="E35" r:id="rId136" xr:uid="{809CA2D1-39E9-0045-A4DF-E4C0C2E97FA2}"/>
-    <hyperlink ref="E36" r:id="rId137" xr:uid="{5DC44543-F2B9-F841-9097-6DB19C5EBD82}"/>
-    <hyperlink ref="G500" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
-    <hyperlink ref="G474" r:id="rId139" xr:uid="{7F4EA1D7-8774-1A4B-BF25-18ED0416CB20}"/>
-    <hyperlink ref="F240" r:id="rId140" xr:uid="{101513F3-87A1-DA41-8BF5-E4029309ECB8}"/>
-    <hyperlink ref="F225" r:id="rId141" xr:uid="{494E255E-6912-8643-B5CD-1D65E0DDCFFC}"/>
-    <hyperlink ref="F226" r:id="rId142" xr:uid="{828F749D-83DE-C14E-B637-56047AC1B384}"/>
-    <hyperlink ref="F241" r:id="rId143" xr:uid="{435D9B3C-98B6-5E49-BD30-EAA53523CDB7}"/>
-    <hyperlink ref="F242" r:id="rId144" xr:uid="{7D905409-0097-E04E-9593-2DEEBEEA0D0F}"/>
-    <hyperlink ref="F174" r:id="rId145" xr:uid="{64451146-E88A-9A47-9888-71BEAC8B984E}"/>
-    <hyperlink ref="F230" r:id="rId146" xr:uid="{28F6BA28-EB9B-374C-A8A0-4077C800D23A}"/>
-    <hyperlink ref="G442" r:id="rId147" xr:uid="{20B4F69E-7592-784A-8C2E-123726A51D93}"/>
-    <hyperlink ref="F233" r:id="rId148" xr:uid="{E3C3D7C6-1E6E-FF40-8CC7-6CF1C77457E4}"/>
-    <hyperlink ref="G522" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
-    <hyperlink ref="G195" r:id="rId150" xr:uid="{9BECD448-C575-B64B-BA3F-BEE8D1CBBD43}"/>
-    <hyperlink ref="G528" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
-    <hyperlink ref="G529" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
-    <hyperlink ref="G530" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
-    <hyperlink ref="G533" r:id="rId154" xr:uid="{FB93E0B8-2537-FD47-8420-84D2A706F697}"/>
-    <hyperlink ref="G534" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
-    <hyperlink ref="F208" r:id="rId156" location="2116892" xr:uid="{FF1C16E6-B146-B548-B694-396AC9D0B975}"/>
-    <hyperlink ref="G193" r:id="rId157" xr:uid="{ED09A21C-0057-1146-8BFF-213A32FC88DF}"/>
-    <hyperlink ref="G446" r:id="rId158" xr:uid="{F933A5C4-6DD5-5547-8BB3-B5D3FBA7A852}"/>
-    <hyperlink ref="G539" r:id="rId159" location=".YLoDxOvTXX8" xr:uid="{8886E3AC-3A64-6449-A070-17D95B586F83}"/>
-    <hyperlink ref="F211" r:id="rId160" xr:uid="{5140C3EB-4DFC-5A4A-9C02-C2EBFA052A41}"/>
-    <hyperlink ref="F28" r:id="rId161" xr:uid="{99992829-3CC1-2B43-BA73-7F09EAA955A4}"/>
-    <hyperlink ref="G477" r:id="rId162" xr:uid="{01E9516A-34A1-6D40-BED9-61916E777090}"/>
-    <hyperlink ref="H504" r:id="rId163" xr:uid="{D3C22B64-1D55-1D47-8F15-25C4AA3D5B90}"/>
-    <hyperlink ref="G506" r:id="rId164" xr:uid="{8E28D310-73EF-1C47-A666-DEE78634BFDF}"/>
-    <hyperlink ref="H503" r:id="rId165" xr:uid="{66476745-9FC4-9E4B-952E-C3E33F678E5D}"/>
-    <hyperlink ref="G542" r:id="rId166" xr:uid="{04D185B2-C246-8B4F-8813-F5A12B741A26}"/>
-    <hyperlink ref="G552" r:id="rId167" xr:uid="{D89D9875-8DF0-3044-BF56-09B8E52D068E}"/>
-    <hyperlink ref="G479" r:id="rId168" xr:uid="{951EA3E4-9D93-CC44-96EE-1FAB3FE8B169}"/>
+    <hyperlink ref="D56" r:id="rId3" xr:uid="{6360CC1D-0E6F-6B45-B16E-E9F323959E32}"/>
+    <hyperlink ref="E68" r:id="rId4" xr:uid="{96980E2B-5D77-D04D-8463-2374C6B90C21}"/>
+    <hyperlink ref="E85" r:id="rId5" xr:uid="{5081034D-5E40-F340-99D2-B8E4DFC0468C}"/>
+    <hyperlink ref="E88" r:id="rId6" location=":~:text=You%20can%20verify%20whether%20it,password%20and%20ESSID%20are%20correct." xr:uid="{3BA51E9E-8709-874E-B6EC-40074894ACA9}"/>
+    <hyperlink ref="E83" r:id="rId7" xr:uid="{30BD9D61-AAB4-2544-987A-0386CA068398}"/>
+    <hyperlink ref="E91" r:id="rId8" xr:uid="{1824F9BF-1BD9-3842-A565-00C06FF5E50F}"/>
+    <hyperlink ref="D162" r:id="rId9" xr:uid="{E488AECD-B504-A04E-8F27-807A3A08802C}"/>
+    <hyperlink ref="D116" r:id="rId10" location="89804" xr:uid="{E34C14F5-E723-0A48-894F-222B3F74BBF9}"/>
+    <hyperlink ref="D117" r:id="rId11" xr:uid="{6C20672B-9F8F-094F-9AC8-3D1FC1C85319}"/>
+    <hyperlink ref="D118" r:id="rId12" xr:uid="{BA9A8F05-4D7F-4942-886C-F8152208F0EA}"/>
+    <hyperlink ref="F122" r:id="rId13" xr:uid="{22AE585F-7255-3F41-8A2E-808446F3A9AA}"/>
+    <hyperlink ref="F124" r:id="rId14" xr:uid="{93472772-CF6C-D045-B634-2D574A3EE034}"/>
+    <hyperlink ref="E220" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
+    <hyperlink ref="F221" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
+    <hyperlink ref="D252" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
+    <hyperlink ref="D253" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
+    <hyperlink ref="F125" r:id="rId19" xr:uid="{92BE3560-5393-C545-9D2D-2B773359B28F}"/>
+    <hyperlink ref="E269" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
+    <hyperlink ref="E270" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
+    <hyperlink ref="E271" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
+    <hyperlink ref="E99" r:id="rId23" xr:uid="{1526D7DA-27DA-1443-928C-BEDA9E425734}"/>
+    <hyperlink ref="E100" r:id="rId24" xr:uid="{4F363062-BE49-AB4F-8956-2C1F31D9B898}"/>
+    <hyperlink ref="H126" r:id="rId25" xr:uid="{D9E13355-D59B-054F-B544-34A5A285A9E0}"/>
+    <hyperlink ref="G94" r:id="rId26" xr:uid="{170917BF-0643-9848-BCA9-A3BF5219EE3E}"/>
+    <hyperlink ref="F129" r:id="rId27" xr:uid="{5D45F2D3-11BC-6E43-BEFF-29E4E04A041E}"/>
+    <hyperlink ref="I130" r:id="rId28" xr:uid="{7D985D09-6A9A-FF4D-9F4A-4C56CC604DCE}"/>
+    <hyperlink ref="D119" r:id="rId29" xr:uid="{784C3F11-339F-8242-911D-6E4E893DD319}"/>
+    <hyperlink ref="E119" r:id="rId30" xr:uid="{FC907203-09BF-654B-9028-A8528783DAFE}"/>
+    <hyperlink ref="F131" r:id="rId31" xr:uid="{EFD3653A-B2F2-614F-8DEE-A2CB34111C94}"/>
+    <hyperlink ref="F132" r:id="rId32" xr:uid="{774B592D-11A5-9C49-BB9A-61014C8D8C81}"/>
+    <hyperlink ref="F133" r:id="rId33" xr:uid="{BD793670-4C63-C04D-B52D-974AF8E59FA4}"/>
+    <hyperlink ref="F134" r:id="rId34" location="96077" xr:uid="{B9804BBD-5312-714B-97EA-CC7D2C647F2C}"/>
+    <hyperlink ref="H127" r:id="rId35" xr:uid="{7BC5BAB5-D297-0043-BAAF-45AD255D5C84}"/>
+    <hyperlink ref="I126" r:id="rId36" xr:uid="{A03C56E4-1156-A148-A568-F50A5C33DB5C}"/>
+    <hyperlink ref="F135" r:id="rId37" xr:uid="{12AC219C-4678-4E43-B328-6595FA10B8D3}"/>
+    <hyperlink ref="E137" r:id="rId38" xr:uid="{44409621-28A2-704A-B283-3DCE1EFB1603}"/>
+    <hyperlink ref="E275" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
+    <hyperlink ref="F138" r:id="rId40" xr:uid="{A9D0D792-87D1-8144-872F-5CA060D3C28F}"/>
+    <hyperlink ref="F139" r:id="rId41" xr:uid="{87EF989D-17E9-1E45-A075-CD862D0B60F4}"/>
+    <hyperlink ref="F141" r:id="rId42" xr:uid="{8406C6F0-DC69-A64D-AAD8-60A33C12D00B}"/>
+    <hyperlink ref="F142" r:id="rId43" location="108593" xr:uid="{3C38F59E-6E71-4048-9BCA-CBC77D3907E0}"/>
+    <hyperlink ref="F144" r:id="rId44" xr:uid="{EEBE2A3E-36CA-F94F-9B1D-EE463DB6425F}"/>
+    <hyperlink ref="F145" r:id="rId45" xr:uid="{3782B43D-9E6F-2940-A013-34AA5D6B4DB3}"/>
+    <hyperlink ref="F146" r:id="rId46" xr:uid="{3D1C62DB-D9B7-BE42-B21D-4EEBC4C9EFE1}"/>
+    <hyperlink ref="F147" r:id="rId47" xr:uid="{F5021A21-70A2-D34E-B055-64CAC326E7EF}"/>
+    <hyperlink ref="F148" r:id="rId48" xr:uid="{A8C010A1-8EE1-264B-8688-3BEA1B62E535}"/>
+    <hyperlink ref="E276" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
+    <hyperlink ref="F143" r:id="rId50" location="113521" xr:uid="{EE1413C5-3B38-7D4D-8DF1-634A12F0BD81}"/>
+    <hyperlink ref="E101" r:id="rId51" xr:uid="{00B1EF4A-7791-0343-8D8C-9A1E83248FC9}"/>
+    <hyperlink ref="E337" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
+    <hyperlink ref="E338" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
+    <hyperlink ref="F150" r:id="rId54" xr:uid="{40A4B6A0-2F7E-A84D-8CC6-D814A33F5953}"/>
+    <hyperlink ref="E277" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
+    <hyperlink ref="E278" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
+    <hyperlink ref="E279" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
+    <hyperlink ref="E280" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
+    <hyperlink ref="E339" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
+    <hyperlink ref="D254" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
+    <hyperlink ref="D255" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
+    <hyperlink ref="D256" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
+    <hyperlink ref="E281" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
+    <hyperlink ref="E340" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
+    <hyperlink ref="E341" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
+    <hyperlink ref="E343" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
+    <hyperlink ref="E344" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
+    <hyperlink ref="F338" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
+    <hyperlink ref="G338" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
+    <hyperlink ref="E345" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
+    <hyperlink ref="E346" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
+    <hyperlink ref="E347" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
+    <hyperlink ref="E222" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
+    <hyperlink ref="E342" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
+    <hyperlink ref="E348" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
+    <hyperlink ref="E349" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
+    <hyperlink ref="E103" r:id="rId77" location="code" xr:uid="{C0475FF8-517D-E949-887E-9A42D86E9640}"/>
+    <hyperlink ref="E351" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
+    <hyperlink ref="E104" r:id="rId79" xr:uid="{277DBE6F-F3E5-8B4C-8DD8-BD92445D1A99}"/>
+    <hyperlink ref="E353" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
+    <hyperlink ref="E358" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
+    <hyperlink ref="E260" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
+    <hyperlink ref="E261" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
+    <hyperlink ref="F171" r:id="rId84" xr:uid="{EB604865-A16B-0646-A5B5-0D047467449D}"/>
+    <hyperlink ref="E283" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
+    <hyperlink ref="D367" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
+    <hyperlink ref="D368" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
+    <hyperlink ref="E377" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
+    <hyperlink ref="E378" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
+    <hyperlink ref="E376" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
+    <hyperlink ref="D387" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
+    <hyperlink ref="E393" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
+    <hyperlink ref="E390" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
+    <hyperlink ref="E394" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
+    <hyperlink ref="F385" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
+    <hyperlink ref="F386" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
+    <hyperlink ref="E388" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
+    <hyperlink ref="G390" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
+    <hyperlink ref="D403" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
+    <hyperlink ref="E395" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
+    <hyperlink ref="E398" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
+    <hyperlink ref="E397" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
+    <hyperlink ref="F302" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
+    <hyperlink ref="E303" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
+    <hyperlink ref="E304" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
+    <hyperlink ref="E305" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
+    <hyperlink ref="G319" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
+    <hyperlink ref="E314" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
+    <hyperlink ref="E315" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
+    <hyperlink ref="E320" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
+    <hyperlink ref="F183" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
+    <hyperlink ref="F188" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
+    <hyperlink ref="F189" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
+    <hyperlink ref="F196" r:id="rId114" xr:uid="{2B03B1F0-535A-3E4F-8FB3-35D2DE847218}"/>
+    <hyperlink ref="G201" r:id="rId115" xr:uid="{11045522-E183-B14C-B43D-5EA36E454600}"/>
+    <hyperlink ref="E223" r:id="rId116" xr:uid="{F1098A8C-3BC0-DB4F-8F9C-48B31145FEC1}"/>
+    <hyperlink ref="F203" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
+    <hyperlink ref="F197" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
+    <hyperlink ref="F206" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
+    <hyperlink ref="H298" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
+    <hyperlink ref="F410" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
+    <hyperlink ref="G424" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
+    <hyperlink ref="F411" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
+    <hyperlink ref="G426" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
+    <hyperlink ref="G428" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
+    <hyperlink ref="G431" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
+    <hyperlink ref="G435" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
+    <hyperlink ref="G460" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
+    <hyperlink ref="G458" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
+    <hyperlink ref="G463" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
+    <hyperlink ref="G469" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
+    <hyperlink ref="G473" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
+    <hyperlink ref="G486" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
+    <hyperlink ref="G491" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
+    <hyperlink ref="G516" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
+    <hyperlink ref="E36" r:id="rId136" xr:uid="{809CA2D1-39E9-0045-A4DF-E4C0C2E97FA2}"/>
+    <hyperlink ref="E37" r:id="rId137" xr:uid="{5DC44543-F2B9-F841-9097-6DB19C5EBD82}"/>
+    <hyperlink ref="G501" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
+    <hyperlink ref="G475" r:id="rId139" xr:uid="{7F4EA1D7-8774-1A4B-BF25-18ED0416CB20}"/>
+    <hyperlink ref="F241" r:id="rId140" xr:uid="{101513F3-87A1-DA41-8BF5-E4029309ECB8}"/>
+    <hyperlink ref="F226" r:id="rId141" xr:uid="{494E255E-6912-8643-B5CD-1D65E0DDCFFC}"/>
+    <hyperlink ref="F227" r:id="rId142" xr:uid="{828F749D-83DE-C14E-B637-56047AC1B384}"/>
+    <hyperlink ref="F242" r:id="rId143" xr:uid="{435D9B3C-98B6-5E49-BD30-EAA53523CDB7}"/>
+    <hyperlink ref="F243" r:id="rId144" xr:uid="{7D905409-0097-E04E-9593-2DEEBEEA0D0F}"/>
+    <hyperlink ref="F175" r:id="rId145" xr:uid="{64451146-E88A-9A47-9888-71BEAC8B984E}"/>
+    <hyperlink ref="F231" r:id="rId146" xr:uid="{28F6BA28-EB9B-374C-A8A0-4077C800D23A}"/>
+    <hyperlink ref="G443" r:id="rId147" xr:uid="{20B4F69E-7592-784A-8C2E-123726A51D93}"/>
+    <hyperlink ref="F234" r:id="rId148" xr:uid="{E3C3D7C6-1E6E-FF40-8CC7-6CF1C77457E4}"/>
+    <hyperlink ref="G523" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
+    <hyperlink ref="G196" r:id="rId150" xr:uid="{9BECD448-C575-B64B-BA3F-BEE8D1CBBD43}"/>
+    <hyperlink ref="G529" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
+    <hyperlink ref="G530" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
+    <hyperlink ref="G531" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
+    <hyperlink ref="G534" r:id="rId154" xr:uid="{FB93E0B8-2537-FD47-8420-84D2A706F697}"/>
+    <hyperlink ref="G535" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
+    <hyperlink ref="F209" r:id="rId156" location="2116892" xr:uid="{FF1C16E6-B146-B548-B694-396AC9D0B975}"/>
+    <hyperlink ref="G194" r:id="rId157" xr:uid="{ED09A21C-0057-1146-8BFF-213A32FC88DF}"/>
+    <hyperlink ref="G447" r:id="rId158" xr:uid="{F933A5C4-6DD5-5547-8BB3-B5D3FBA7A852}"/>
+    <hyperlink ref="G540" r:id="rId159" location=".YLoDxOvTXX8" xr:uid="{8886E3AC-3A64-6449-A070-17D95B586F83}"/>
+    <hyperlink ref="F212" r:id="rId160" xr:uid="{5140C3EB-4DFC-5A4A-9C02-C2EBFA052A41}"/>
+    <hyperlink ref="F29" r:id="rId161" xr:uid="{99992829-3CC1-2B43-BA73-7F09EAA955A4}"/>
+    <hyperlink ref="G478" r:id="rId162" xr:uid="{01E9516A-34A1-6D40-BED9-61916E777090}"/>
+    <hyperlink ref="H505" r:id="rId163" xr:uid="{D3C22B64-1D55-1D47-8F15-25C4AA3D5B90}"/>
+    <hyperlink ref="G507" r:id="rId164" xr:uid="{8E28D310-73EF-1C47-A666-DEE78634BFDF}"/>
+    <hyperlink ref="H504" r:id="rId165" xr:uid="{66476745-9FC4-9E4B-952E-C3E33F678E5D}"/>
+    <hyperlink ref="G543" r:id="rId166" xr:uid="{04D185B2-C246-8B4F-8813-F5A12B741A26}"/>
+    <hyperlink ref="G553" r:id="rId167" xr:uid="{D89D9875-8DF0-3044-BF56-09B8E52D068E}"/>
+    <hyperlink ref="G480" r:id="rId168" xr:uid="{951EA3E4-9D93-CC44-96EE-1FAB3FE8B169}"/>
+    <hyperlink ref="F32" r:id="rId169" xr:uid="{A2E3FF8D-D95C-A149-813C-65DD0F6ADE93}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6519,10 +6585,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G66"/>
+  <dimension ref="B2:G67"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7137,6 +7203,9 @@
       <c r="B56" t="s">
         <v>891</v>
       </c>
+      <c r="D56" t="s">
+        <v>766</v>
+      </c>
       <c r="E56" t="s">
         <v>890</v>
       </c>
@@ -7146,123 +7215,137 @@
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>771</v>
-      </c>
-      <c r="C57" t="s">
-        <v>467</v>
+        <v>907</v>
+      </c>
+      <c r="D57" t="s">
+        <v>766</v>
       </c>
       <c r="E57" t="s">
-        <v>769</v>
+        <v>908</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>770</v>
+        <v>906</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>723</v>
+        <v>771</v>
+      </c>
+      <c r="C58" t="s">
+        <v>467</v>
       </c>
       <c r="E58" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>722</v>
+        <v>770</v>
       </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>774</v>
+        <v>723</v>
+      </c>
+      <c r="E59" t="s">
+        <v>772</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>773</v>
+        <v>722</v>
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>775</v>
-      </c>
-      <c r="C60" t="s">
-        <v>467</v>
-      </c>
-      <c r="E60" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>783</v>
+        <v>775</v>
+      </c>
+      <c r="C61" t="s">
+        <v>467</v>
       </c>
       <c r="E61" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>782</v>
+        <v>777</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>786</v>
-      </c>
-      <c r="D62" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="E62" t="s">
-        <v>784</v>
+        <v>781</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>782</v>
       </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>787</v>
-      </c>
-      <c r="C63" t="s">
-        <v>789</v>
+        <v>786</v>
+      </c>
+      <c r="D63" t="s">
+        <v>785</v>
       </c>
       <c r="E63" t="s">
-        <v>790</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="C64" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
       <c r="E64" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>795</v>
+        <v>791</v>
+      </c>
+      <c r="C65" t="s">
+        <v>794</v>
       </c>
       <c r="E65" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
+        <v>795</v>
+      </c>
+      <c r="E66" t="s">
+        <v>797</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
         <v>798</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C67" t="s">
         <v>648</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E67" t="s">
         <v>799</v>
       </c>
-      <c r="F66" s="1" t="s">
+      <c r="F67" s="1" t="s">
         <v>800</v>
       </c>
     </row>
@@ -7321,16 +7404,17 @@
     <hyperlink ref="F50" r:id="rId51" xr:uid="{B9356038-CF05-854A-AFF1-D7384A989DFB}"/>
     <hyperlink ref="F54" r:id="rId52" xr:uid="{61072865-D316-554C-A5B2-DE65C0BB4955}"/>
     <hyperlink ref="F55" r:id="rId53" xr:uid="{3D288582-752C-394F-85D5-4AC8FCF2210E}"/>
-    <hyperlink ref="F57" r:id="rId54" xr:uid="{634A44CB-CBAB-AE4D-898A-98A6804C37BE}"/>
-    <hyperlink ref="F58" r:id="rId55" xr:uid="{CBA3AB68-A9B5-7E45-AAF4-E420DC08CECB}"/>
-    <hyperlink ref="F59" r:id="rId56" xr:uid="{6513D8D1-CA9F-DB4F-8EE3-BB85344F470E}"/>
-    <hyperlink ref="F60" r:id="rId57" xr:uid="{F0C558B0-9D09-2E47-9A73-03B1EBC298EA}"/>
-    <hyperlink ref="F61" r:id="rId58" xr:uid="{0E6940AA-CCE2-A845-B000-88634DEE5413}"/>
-    <hyperlink ref="F63" r:id="rId59" xr:uid="{DB6C6106-7A38-1843-B3AC-F9FB615E4977}"/>
-    <hyperlink ref="F64" r:id="rId60" xr:uid="{8AED1472-61F4-E646-89E7-A2D566BEF7A0}"/>
-    <hyperlink ref="F65" r:id="rId61" xr:uid="{D5875307-B681-3841-BE35-59A92CDCD038}"/>
-    <hyperlink ref="F66" r:id="rId62" xr:uid="{E6DDA861-2175-8242-9563-08D5A89ACF52}"/>
+    <hyperlink ref="F58" r:id="rId54" xr:uid="{634A44CB-CBAB-AE4D-898A-98A6804C37BE}"/>
+    <hyperlink ref="F59" r:id="rId55" xr:uid="{CBA3AB68-A9B5-7E45-AAF4-E420DC08CECB}"/>
+    <hyperlink ref="F60" r:id="rId56" xr:uid="{6513D8D1-CA9F-DB4F-8EE3-BB85344F470E}"/>
+    <hyperlink ref="F61" r:id="rId57" xr:uid="{F0C558B0-9D09-2E47-9A73-03B1EBC298EA}"/>
+    <hyperlink ref="F62" r:id="rId58" xr:uid="{0E6940AA-CCE2-A845-B000-88634DEE5413}"/>
+    <hyperlink ref="F64" r:id="rId59" xr:uid="{DB6C6106-7A38-1843-B3AC-F9FB615E4977}"/>
+    <hyperlink ref="F65" r:id="rId60" xr:uid="{8AED1472-61F4-E646-89E7-A2D566BEF7A0}"/>
+    <hyperlink ref="F66" r:id="rId61" xr:uid="{D5875307-B681-3841-BE35-59A92CDCD038}"/>
+    <hyperlink ref="F67" r:id="rId62" xr:uid="{E6DDA861-2175-8242-9563-08D5A89ACF52}"/>
     <hyperlink ref="F56" r:id="rId63" xr:uid="{EDECDF4B-3198-4348-9F78-BF6E9FF8C9A6}"/>
+    <hyperlink ref="F57" r:id="rId64" location="5" xr:uid="{3C28890A-3BF2-2647-AB92-79793D3ADD6E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7373,7 +7457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069EEB69-0D57-C040-8545-840D5862E858}">
   <dimension ref="B2:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B22" sqref="B22:D23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added blank rows under ssh_key
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7C1BFF-CEAD-0443-B4A2-D94095E0C629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0C7C6B-3BF8-B447-966D-908567311EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -3229,11 +3229,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I553"/>
+  <dimension ref="B1:I559"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A470" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3491,51 +3491,14 @@
         <v>592</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C40" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D42">
-        <v>2</v>
-      </c>
-      <c r="E42" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C43" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
-        <v>22</v>
-      </c>
-      <c r="F44" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.2">
@@ -3543,1316 +3506,1319 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
+        <v>22</v>
+      </c>
+      <c r="F50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C48" t="s">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D49">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D55">
         <v>1</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E55" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C50" t="s">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
         <v>835</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D51">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D57">
         <v>1</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E57" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C56" t="s">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C62" t="s">
         <v>30</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D62" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C59" t="s">
+    <row r="65" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C65" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D60" t="s">
+    <row r="66" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D61" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E62" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C63" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D64" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E65" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C66" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="67" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D67" t="s">
         <v>35</v>
       </c>
-      <c r="E67" t="s">
+    </row>
+    <row r="68" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E68" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="69" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C69" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="70" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="71" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E71" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C72" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D73" t="s">
+        <v>35</v>
+      </c>
+      <c r="E73" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D68" t="s">
-        <v>30</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="70" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C70" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="71" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D71" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="72" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E72" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="73" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C73" t="s">
-        <v>880</v>
       </c>
     </row>
     <row r="74" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="76" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C76" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="77" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D77" t="s">
         <v>38</v>
       </c>
-      <c r="E74" t="s">
+    </row>
+    <row r="78" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E78" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C79" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="80" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D80" t="s">
+        <v>38</v>
+      </c>
+      <c r="E80" t="s">
         <v>881</v>
       </c>
     </row>
-    <row r="75" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C75" t="s">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C81" t="s">
         <v>882</v>
       </c>
     </row>
-    <row r="76" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D76" t="s">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D82" t="s">
         <v>38</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E82" t="s">
         <v>883</v>
       </c>
     </row>
-    <row r="77" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C77" t="s">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C83" t="s">
         <v>884</v>
       </c>
     </row>
-    <row r="78" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D78" t="s">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D84" t="s">
         <v>38</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E84" t="s">
         <v>885</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B81" t="s">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C82" t="s">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C88" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D83" t="s">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D89" t="s">
         <v>47</v>
       </c>
-      <c r="E83" s="1" t="s">
+      <c r="E89" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C84" t="s">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D85" t="s">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D91" t="s">
         <v>50</v>
       </c>
-      <c r="E85" s="1" t="s">
+      <c r="E91" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D86" t="s">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D92" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C87" t="s">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C93" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D88" t="s">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
         <v>53</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="E94" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C90" t="s">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C96" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D91" t="s">
+    <row r="97" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D97" t="s">
         <v>57</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="E97" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E92" s="1"/>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C93" t="s">
+    <row r="98" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E98" s="1"/>
+    </row>
+    <row r="99" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C99" t="s">
         <v>198</v>
       </c>
-      <c r="E93" s="1"/>
-    </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D94" t="s">
+      <c r="E99" s="1"/>
+    </row>
+    <row r="100" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D100" t="s">
         <v>203</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E100" t="s">
         <v>53</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F100" t="s">
         <v>200</v>
       </c>
-      <c r="G94" s="1" t="s">
+      <c r="G100" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D95" t="s">
+    <row r="101" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D101" t="s">
         <v>204</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E101" t="s">
         <v>201</v>
       </c>
-      <c r="F95" t="s">
+      <c r="F101" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E96" s="1"/>
-    </row>
-    <row r="97" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E97" s="1"/>
-    </row>
-    <row r="98" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C98" t="s">
+    <row r="102" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E102" s="1"/>
+    </row>
+    <row r="103" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E103" s="1"/>
+    </row>
+    <row r="104" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C104" t="s">
         <v>192</v>
       </c>
-      <c r="E98" s="1"/>
-    </row>
-    <row r="99" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D99" t="s">
+      <c r="E104" s="1"/>
+    </row>
+    <row r="105" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D105" t="s">
         <v>193</v>
       </c>
-      <c r="E99" s="1" t="s">
+      <c r="E105" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="100" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E100" s="1" t="s">
+    <row r="106" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E106" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="101" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E101" s="1" t="s">
+    <row r="107" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E107" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="102" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E102" s="1"/>
-    </row>
-    <row r="103" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D103" t="s">
+    <row r="108" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E108" s="1"/>
+    </row>
+    <row r="109" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D109" t="s">
         <v>328</v>
       </c>
-      <c r="E103" s="1" t="s">
+      <c r="E109" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="104" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D104" s="7" t="s">
+    <row r="110" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D110" s="7" t="s">
         <v>333</v>
       </c>
-      <c r="E104" s="1" t="s">
+      <c r="E110" s="1" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="105" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E105" s="1"/>
-    </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B115" t="s">
+    <row r="111" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E111" s="1"/>
+    </row>
+    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B121" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="116" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C116" t="s">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C122" t="s">
         <v>156</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D122" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="117" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C117" t="s">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C123" t="s">
         <v>158</v>
       </c>
-      <c r="D117" s="1" t="s">
+      <c r="D123" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="118" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C118" t="s">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C124" t="s">
         <v>159</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="D124" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="119" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C119" t="s">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C125" t="s">
         <v>218</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="D125" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E119" s="1" t="s">
+      <c r="E125" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="121" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C121" t="s">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C127" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="122" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D122" t="s">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D128" t="s">
         <v>163</v>
       </c>
-      <c r="E122" t="s">
+      <c r="E128" t="s">
         <v>162</v>
       </c>
-      <c r="F122" s="1" t="s">
+      <c r="F128" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="123" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="E123" t="s">
+    <row r="129" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E129" t="s">
         <v>274</v>
       </c>
-      <c r="F123" s="1"/>
-    </row>
-    <row r="124" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D124" t="s">
-        <v>165</v>
-      </c>
-      <c r="E124" t="s">
-        <v>166</v>
-      </c>
-      <c r="F124" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="125" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D125" t="s">
-        <v>179</v>
-      </c>
-      <c r="E125" t="s">
-        <v>180</v>
-      </c>
-      <c r="F125" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="126" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D126" t="s">
-        <v>189</v>
-      </c>
-      <c r="E126" t="s">
-        <v>191</v>
-      </c>
-      <c r="F126" t="s">
-        <v>195</v>
-      </c>
-      <c r="G126" t="s">
-        <v>190</v>
-      </c>
-      <c r="H126" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="I126" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="127" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D127" t="s">
-        <v>231</v>
-      </c>
-      <c r="E127" t="s">
-        <v>233</v>
-      </c>
-      <c r="H127" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="128" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D128" t="s">
-        <v>232</v>
-      </c>
-      <c r="E128" t="s">
-        <v>234</v>
-      </c>
-      <c r="H128" s="1"/>
-    </row>
-    <row r="129" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D129" t="s">
-        <v>205</v>
-      </c>
-      <c r="E129" t="s">
-        <v>206</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>207</v>
-      </c>
+      <c r="F129" s="1"/>
     </row>
     <row r="130" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D130" t="s">
-        <v>208</v>
+        <v>165</v>
       </c>
       <c r="E130" t="s">
-        <v>209</v>
-      </c>
-      <c r="F130" t="s">
-        <v>210</v>
-      </c>
-      <c r="G130" t="s">
-        <v>213</v>
-      </c>
-      <c r="H130" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="I130" s="1" t="s">
-        <v>212</v>
+        <v>166</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="131" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D131" t="s">
-        <v>219</v>
+        <v>179</v>
       </c>
       <c r="E131" t="s">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>221</v>
+        <v>181</v>
       </c>
     </row>
     <row r="132" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D132" t="s">
-        <v>223</v>
+        <v>189</v>
       </c>
       <c r="E132" t="s">
-        <v>222</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>224</v>
+        <v>191</v>
+      </c>
+      <c r="F132" t="s">
+        <v>195</v>
+      </c>
+      <c r="G132" t="s">
+        <v>190</v>
+      </c>
+      <c r="H132" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="I132" s="1" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="133" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D133" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="E133" t="s">
-        <v>226</v>
-      </c>
-      <c r="F133" s="1" t="s">
-        <v>227</v>
+        <v>233</v>
+      </c>
+      <c r="H133" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="134" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D134" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="E134" t="s">
-        <v>229</v>
-      </c>
-      <c r="F134" s="1" t="s">
-        <v>230</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="H134" s="1"/>
     </row>
     <row r="135" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D135" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="E135" t="s">
-        <v>236</v>
+        <v>206</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>238</v>
+        <v>207</v>
       </c>
     </row>
     <row r="136" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D136" t="s">
+        <v>208</v>
+      </c>
       <c r="E136" t="s">
-        <v>237</v>
-      </c>
-      <c r="F136" s="1"/>
+        <v>209</v>
+      </c>
+      <c r="F136" t="s">
+        <v>210</v>
+      </c>
+      <c r="G136" t="s">
+        <v>213</v>
+      </c>
+      <c r="H136" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="I136" s="1" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="137" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D137" t="s">
-        <v>239</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F137" s="1"/>
+        <v>219</v>
+      </c>
+      <c r="E137" t="s">
+        <v>220</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="138" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D138" t="s">
-        <v>246</v>
+        <v>223</v>
       </c>
       <c r="E138" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
     </row>
     <row r="139" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D139" t="s">
-        <v>247</v>
+        <v>225</v>
+      </c>
+      <c r="E139" t="s">
+        <v>226</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
     </row>
     <row r="140" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D140" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="E140" t="s">
-        <v>206</v>
+        <v>229</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="141" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D141" t="s">
-        <v>251</v>
+        <v>235</v>
+      </c>
+      <c r="E141" t="s">
+        <v>236</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
     </row>
     <row r="142" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D142" t="s">
-        <v>253</v>
-      </c>
-      <c r="F142" s="1" t="s">
-        <v>252</v>
-      </c>
+      <c r="E142" t="s">
+        <v>237</v>
+      </c>
+      <c r="F142" s="1"/>
     </row>
     <row r="143" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D143" t="s">
-        <v>272</v>
-      </c>
-      <c r="F143" s="1" t="s">
-        <v>273</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F143" s="1"/>
     </row>
     <row r="144" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D144" t="s">
+        <v>246</v>
+      </c>
+      <c r="E144" t="s">
+        <v>245</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="145" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D145" t="s">
+        <v>247</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="146" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D146" t="s">
+        <v>249</v>
+      </c>
+      <c r="E146" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="147" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D147" t="s">
+        <v>251</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="148" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D148" t="s">
+        <v>253</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="149" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D149" t="s">
+        <v>272</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="150" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D150" t="s">
         <v>254</v>
       </c>
-      <c r="E144" t="s">
+      <c r="E150" t="s">
         <v>255</v>
       </c>
-      <c r="F144" s="1" t="s">
+      <c r="F150" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D145" t="s">
+    <row r="151" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D151" t="s">
         <v>257</v>
       </c>
-      <c r="E145" t="s">
+      <c r="E151" t="s">
         <v>258</v>
       </c>
-      <c r="F145" s="1" t="s">
+      <c r="F151" s="1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D146" t="s">
+    <row r="152" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D152" t="s">
         <v>261</v>
       </c>
-      <c r="F146" s="1" t="s">
+      <c r="F152" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D147" t="s">
+    <row r="153" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D153" t="s">
         <v>263</v>
       </c>
-      <c r="F147" s="1" t="s">
+      <c r="F153" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D148" t="s">
+    <row r="154" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D154" t="s">
         <v>265</v>
       </c>
-      <c r="E148" t="s">
+      <c r="E154" t="s">
         <v>264</v>
       </c>
-      <c r="F148" s="1" t="s">
+      <c r="F154" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E149" t="s">
+    <row r="155" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E155" t="s">
         <v>267</v>
       </c>
-      <c r="F149" s="1"/>
-    </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D150" t="s">
+      <c r="F155" s="1"/>
+    </row>
+    <row r="156" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D156" t="s">
         <v>282</v>
       </c>
-      <c r="F150" s="1" t="s">
+      <c r="F156" s="1" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F151" s="1"/>
-    </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F152" s="1"/>
-    </row>
-    <row r="153" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F153" s="1"/>
-    </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F154" s="1"/>
-    </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F155" s="1"/>
-    </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B156" t="s">
+    <row r="157" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="F157" s="1"/>
+    </row>
+    <row r="158" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="F158" s="1"/>
+    </row>
+    <row r="159" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="F159" s="1"/>
+    </row>
+    <row r="160" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="F160" s="1"/>
+    </row>
+    <row r="161" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F161" s="1"/>
+    </row>
+    <row r="162" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B162" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C157" t="s">
+    <row r="163" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C163" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="158" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D158" t="s">
+    <row r="164" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D164" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="159" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D159" t="s">
+    <row r="165" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D165" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="161" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C161" t="s">
+    <row r="167" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C167" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="162" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D162" s="1" t="s">
+    <row r="168" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D168" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="164" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C164" t="s">
+    <row r="170" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C170" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="165" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D165" t="s">
+    <row r="171" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D171" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="166" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D166" t="s">
+    <row r="172" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D172" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="167" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D167" t="s">
+    <row r="173" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D173" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="168" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D168" t="s">
+    <row r="174" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D174" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="170" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C170" t="s">
+    <row r="176" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C176" t="s">
         <v>346</v>
-      </c>
-    </row>
-    <row r="171" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D171" t="s">
-        <v>349</v>
-      </c>
-      <c r="E171" t="s">
-        <v>347</v>
-      </c>
-      <c r="F171" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="172" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D172" t="s">
-        <v>350</v>
-      </c>
-      <c r="E172" t="s">
-        <v>351</v>
-      </c>
-      <c r="F172" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="174" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C174" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="175" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D175" t="s">
-        <v>675</v>
-      </c>
-      <c r="E175" t="s">
-        <v>676</v>
-      </c>
-      <c r="F175" s="1" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="176" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D176" t="s">
-        <v>677</v>
-      </c>
-      <c r="E176" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="177" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D177" t="s">
-        <v>679</v>
+        <v>349</v>
       </c>
       <c r="E177" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="179" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C179" t="s">
-        <v>357</v>
+        <v>347</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="178" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D178" t="s">
+        <v>350</v>
+      </c>
+      <c r="E178" t="s">
+        <v>351</v>
+      </c>
+      <c r="F178" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="180" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D180" t="s">
-        <v>354</v>
-      </c>
-      <c r="E180" t="s">
-        <v>353</v>
+      <c r="C180" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="181" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D181" t="s">
-        <v>355</v>
+        <v>675</v>
       </c>
       <c r="E181" t="s">
-        <v>356</v>
+        <v>676</v>
+      </c>
+      <c r="F181" s="1" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="182" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D182" t="s">
+        <v>677</v>
+      </c>
+      <c r="E182" t="s">
+        <v>678</v>
       </c>
     </row>
     <row r="183" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C183" t="s">
-        <v>369</v>
-      </c>
-      <c r="F183" s="1" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="184" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D184" t="s">
-        <v>370</v>
-      </c>
-      <c r="E184" t="s">
-        <v>371</v>
+      <c r="D183" t="s">
+        <v>679</v>
+      </c>
+      <c r="E183" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="185" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D185" t="s">
-        <v>372</v>
-      </c>
-      <c r="E185" t="s">
-        <v>373</v>
+      <c r="C185" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="186" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D186" t="s">
-        <v>374</v>
+        <v>354</v>
       </c>
       <c r="E186" t="s">
-        <v>375</v>
+        <v>353</v>
       </c>
     </row>
     <row r="187" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D187" t="s">
-        <v>376</v>
+        <v>355</v>
       </c>
       <c r="E187" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="188" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D188" t="s">
-        <v>385</v>
-      </c>
-      <c r="E188" t="s">
-        <v>386</v>
-      </c>
-      <c r="F188" s="1" t="s">
-        <v>387</v>
+        <v>356</v>
       </c>
     </row>
     <row r="189" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D189" t="s">
-        <v>388</v>
-      </c>
-      <c r="E189" t="s">
-        <v>389</v>
+      <c r="C189" t="s">
+        <v>369</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>390</v>
+        <v>378</v>
+      </c>
+    </row>
+    <row r="190" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D190" t="s">
+        <v>370</v>
+      </c>
+      <c r="E190" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="191" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C191" t="s">
-        <v>379</v>
+      <c r="D191" t="s">
+        <v>372</v>
+      </c>
+      <c r="E191" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="192" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D192" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="E192" t="s">
-        <v>381</v>
-      </c>
-      <c r="F192" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
     </row>
     <row r="193" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D193" t="s">
-        <v>808</v>
+        <v>376</v>
       </c>
       <c r="E193" t="s">
-        <v>382</v>
-      </c>
-      <c r="F193" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
     </row>
     <row r="194" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D194" t="s">
-        <v>759</v>
+        <v>385</v>
       </c>
       <c r="E194" t="s">
-        <v>760</v>
-      </c>
-      <c r="G194" s="1" t="s">
-        <v>761</v>
+        <v>386</v>
+      </c>
+      <c r="F194" s="1" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="195" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="F195" s="1"/>
-    </row>
-    <row r="196" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C196" t="s">
-        <v>391</v>
-      </c>
-      <c r="D196" t="s">
-        <v>419</v>
-      </c>
-      <c r="E196" t="s">
-        <v>392</v>
-      </c>
-      <c r="F196" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G196" s="1" t="s">
-        <v>724</v>
+      <c r="D195" t="s">
+        <v>388</v>
+      </c>
+      <c r="E195" t="s">
+        <v>389</v>
+      </c>
+      <c r="F195" s="1" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="197" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D197" t="s">
-        <v>420</v>
-      </c>
-      <c r="E197" t="s">
-        <v>421</v>
-      </c>
-      <c r="F197" s="1" t="s">
-        <v>422</v>
+      <c r="C197" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="198" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D198" t="s">
-        <v>423</v>
+        <v>380</v>
       </c>
       <c r="E198" t="s">
-        <v>424</v>
-      </c>
-      <c r="F198" s="1"/>
+        <v>381</v>
+      </c>
+      <c r="F198" t="s">
+        <v>383</v>
+      </c>
     </row>
     <row r="199" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C199" t="s">
-        <v>393</v>
-      </c>
-      <c r="F199" s="1"/>
+      <c r="D199" t="s">
+        <v>808</v>
+      </c>
+      <c r="E199" t="s">
+        <v>382</v>
+      </c>
+      <c r="F199" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="200" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D200" t="s">
-        <v>395</v>
+        <v>759</v>
       </c>
       <c r="E200" t="s">
-        <v>394</v>
-      </c>
-      <c r="F200" s="1"/>
+        <v>760</v>
+      </c>
+      <c r="G200" s="1" t="s">
+        <v>761</v>
+      </c>
     </row>
     <row r="201" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D201" t="s">
-        <v>396</v>
-      </c>
-      <c r="F201" t="s">
-        <v>397</v>
-      </c>
-      <c r="G201" s="1" t="s">
-        <v>398</v>
-      </c>
+      <c r="F201" s="1"/>
     </row>
     <row r="202" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C202" t="s">
-        <v>415</v>
-      </c>
-      <c r="G202" s="1"/>
+        <v>391</v>
+      </c>
+      <c r="D202" t="s">
+        <v>419</v>
+      </c>
+      <c r="E202" t="s">
+        <v>392</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G202" s="1" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="203" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D203" t="s">
+        <v>420</v>
+      </c>
       <c r="E203" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="F203" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="G203" s="1"/>
+        <v>422</v>
+      </c>
     </row>
     <row r="204" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D204" t="s">
+        <v>423</v>
+      </c>
       <c r="E204" t="s">
-        <v>417</v>
-      </c>
+        <v>424</v>
+      </c>
+      <c r="F204" s="1"/>
     </row>
     <row r="205" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C205" t="s">
-        <v>430</v>
-      </c>
+        <v>393</v>
+      </c>
+      <c r="F205" s="1"/>
     </row>
     <row r="206" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D206" t="s">
-        <v>431</v>
+        <v>395</v>
       </c>
       <c r="E206" t="s">
-        <v>433</v>
-      </c>
-      <c r="F206" s="1" t="s">
-        <v>435</v>
-      </c>
+        <v>394</v>
+      </c>
+      <c r="F206" s="1"/>
     </row>
     <row r="207" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D207" t="s">
-        <v>432</v>
-      </c>
-      <c r="E207" t="s">
-        <v>434</v>
+        <v>396</v>
+      </c>
+      <c r="F207" t="s">
+        <v>397</v>
+      </c>
+      <c r="G207" s="1" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="208" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C208" t="s">
+        <v>415</v>
+      </c>
+      <c r="G208" s="1"/>
+    </row>
+    <row r="209" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E209" t="s">
+        <v>416</v>
+      </c>
+      <c r="F209" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="G209" s="1"/>
+    </row>
+    <row r="210" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E210" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="211" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C211" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="212" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D212" t="s">
+        <v>431</v>
+      </c>
+      <c r="E212" t="s">
+        <v>433</v>
+      </c>
+      <c r="F212" s="1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="213" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D213" t="s">
+        <v>432</v>
+      </c>
+      <c r="E213" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="214" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C214" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="209" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D209" t="s">
+    <row r="215" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D215" t="s">
         <v>757</v>
       </c>
-      <c r="E209" t="s">
+      <c r="E215" t="s">
         <v>756</v>
       </c>
-      <c r="F209" s="1" t="s">
+      <c r="F215" s="1" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="210" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E210" t="s">
+    <row r="216" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E216" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C211" t="s">
+    <row r="217" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C217" t="s">
         <v>809</v>
       </c>
     </row>
-    <row r="212" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D212" t="s">
+    <row r="218" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D218" t="s">
         <v>811</v>
       </c>
-      <c r="E212" t="s">
+      <c r="E218" t="s">
         <v>810</v>
       </c>
-      <c r="F212" s="1" t="s">
+      <c r="F218" s="1" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="218" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B218" t="s">
+    <row r="224" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B224" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="219" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C219" t="s">
+    <row r="225" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C225" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="220" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D220" t="s">
+    <row r="226" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D226" t="s">
         <v>170</v>
       </c>
-      <c r="E220" s="1" t="s">
+      <c r="E226" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="221" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D221" t="s">
+    <row r="227" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D227" t="s">
         <v>174</v>
       </c>
-      <c r="E221" t="s">
+      <c r="E227" t="s">
         <v>172</v>
       </c>
-      <c r="F221" s="1" t="s">
+      <c r="F227" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="222" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C222" t="s">
+    <row r="228" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C228" t="s">
         <v>321</v>
       </c>
-      <c r="E222" s="1" t="s">
+      <c r="E228" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="F222" s="1"/>
-    </row>
-    <row r="223" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C223" t="s">
+      <c r="F228" s="1"/>
+    </row>
+    <row r="229" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C229" t="s">
         <v>404</v>
       </c>
-      <c r="D223" t="s">
+      <c r="D229" t="s">
         <v>405</v>
       </c>
-      <c r="E223" s="1" t="s">
+      <c r="E229" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="F223" s="1"/>
-    </row>
-    <row r="224" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D224" t="s">
+      <c r="F229" s="1"/>
+    </row>
+    <row r="230" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D230" t="s">
         <v>406</v>
       </c>
-      <c r="F224" s="1"/>
-    </row>
-    <row r="225" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F225" s="1"/>
-    </row>
-    <row r="226" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C226" t="s">
-        <v>615</v>
-      </c>
-      <c r="D226" t="s">
-        <v>616</v>
-      </c>
-      <c r="F226" s="1" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="227" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C227" t="s">
-        <v>619</v>
-      </c>
-      <c r="D227" t="s">
-        <v>618</v>
-      </c>
-      <c r="F227" s="1" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="228" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F228" s="1"/>
-    </row>
-    <row r="229" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F229" s="1"/>
-    </row>
-    <row r="230" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B230" t="s">
-        <v>682</v>
-      </c>
       <c r="F230" s="1"/>
     </row>
     <row r="231" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C231" t="s">
-        <v>683</v>
-      </c>
-      <c r="D231" t="s">
-        <v>685</v>
-      </c>
-      <c r="F231" s="1" t="s">
-        <v>687</v>
-      </c>
+      <c r="F231" s="1"/>
     </row>
     <row r="232" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C232" t="s">
-        <v>684</v>
+        <v>615</v>
       </c>
       <c r="D232" t="s">
-        <v>686</v>
-      </c>
-      <c r="F232" s="1"/>
+        <v>616</v>
+      </c>
+      <c r="F232" s="1" t="s">
+        <v>617</v>
+      </c>
     </row>
     <row r="233" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C233" t="s">
-        <v>688</v>
+        <v>619</v>
       </c>
       <c r="D233" t="s">
-        <v>689</v>
-      </c>
-      <c r="F233" s="1"/>
+        <v>618</v>
+      </c>
+      <c r="F233" s="1" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="234" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C234" t="s">
-        <v>703</v>
-      </c>
-      <c r="D234" t="s">
-        <v>704</v>
-      </c>
-      <c r="F234" s="1" t="s">
-        <v>705</v>
-      </c>
+      <c r="F234" s="1"/>
     </row>
     <row r="235" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F235" s="1"/>
     </row>
     <row r="236" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B236" t="s">
+        <v>682</v>
+      </c>
       <c r="F236" s="1"/>
     </row>
     <row r="237" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F237" s="1"/>
+      <c r="C237" t="s">
+        <v>683</v>
+      </c>
+      <c r="D237" t="s">
+        <v>685</v>
+      </c>
+      <c r="F237" s="1" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="238" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C238" t="s">
+        <v>684</v>
+      </c>
+      <c r="D238" t="s">
+        <v>686</v>
+      </c>
       <c r="F238" s="1"/>
     </row>
+    <row r="239" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C239" t="s">
+        <v>688</v>
+      </c>
+      <c r="D239" t="s">
+        <v>689</v>
+      </c>
+      <c r="F239" s="1"/>
+    </row>
     <row r="240" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B240" t="s">
+      <c r="C240" t="s">
+        <v>703</v>
+      </c>
+      <c r="D240" t="s">
+        <v>704</v>
+      </c>
+      <c r="F240" s="1" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="241" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F241" s="1"/>
+    </row>
+    <row r="242" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F242" s="1"/>
+    </row>
+    <row r="243" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F243" s="1"/>
+    </row>
+    <row r="244" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F244" s="1"/>
+    </row>
+    <row r="246" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B246" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="241" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C241" t="s">
+    <row r="247" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C247" t="s">
         <v>613</v>
       </c>
-      <c r="D241" t="s">
+      <c r="D247" t="s">
         <v>612</v>
       </c>
-      <c r="F241" s="1" t="s">
+      <c r="F247" s="1" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="242" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C242" t="s">
+    <row r="248" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C248" t="s">
         <v>621</v>
       </c>
-      <c r="D242" t="s">
+      <c r="D248" t="s">
         <v>622</v>
       </c>
-      <c r="F242" s="1" t="s">
+      <c r="F248" s="1" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="243" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C243" t="s">
+    <row r="249" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C249" t="s">
         <v>625</v>
       </c>
-      <c r="D243" t="s">
+      <c r="D249" t="s">
         <v>624</v>
       </c>
-      <c r="F243" s="1" t="s">
+      <c r="F249" s="1" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="244" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C244" t="s">
+    <row r="250" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C250" t="s">
         <v>628</v>
       </c>
-      <c r="D244" t="s">
+      <c r="D250" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="251" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B251" t="s">
+    <row r="257" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B257" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="252" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C252" t="s">
+    <row r="258" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C258" t="s">
         <v>175</v>
       </c>
-      <c r="D252" s="1" t="s">
+      <c r="D258" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="253" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C253" t="s">
+    <row r="259" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C259" t="s">
         <v>177</v>
       </c>
-      <c r="D253" s="1" t="s">
+      <c r="D259" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="254" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C254" t="s">
-        <v>292</v>
-      </c>
-      <c r="D254" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="255" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C255" t="s">
-        <v>293</v>
-      </c>
-      <c r="D255" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="256" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C256" t="s">
-        <v>296</v>
-      </c>
-      <c r="D256" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="257" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D257" s="1"/>
-    </row>
-    <row r="258" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D258" s="1"/>
-    </row>
-    <row r="259" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B259" t="s">
-        <v>342</v>
-      </c>
-      <c r="D259" s="1"/>
     </row>
     <row r="260" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C260" t="s">
-        <v>343</v>
-      </c>
-      <c r="D260" t="s">
-        <v>368</v>
-      </c>
-      <c r="E260" s="1" t="s">
-        <v>344</v>
+        <v>292</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="261" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D261" t="s">
-        <v>367</v>
-      </c>
-      <c r="E261" s="1" t="s">
-        <v>345</v>
+      <c r="C261" t="s">
+        <v>293</v>
+      </c>
+      <c r="D261" s="1" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="262" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D262" s="1"/>
+      <c r="C262" t="s">
+        <v>296</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="263" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D263" s="1"/>
@@ -4860,130 +4826,146 @@
     <row r="264" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D264" s="1"/>
     </row>
+    <row r="265" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B265" t="s">
+        <v>342</v>
+      </c>
+      <c r="D265" s="1"/>
+    </row>
+    <row r="266" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C266" t="s">
+        <v>343</v>
+      </c>
+      <c r="D266" t="s">
+        <v>368</v>
+      </c>
+      <c r="E266" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="267" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D267" t="s">
+        <v>367</v>
+      </c>
+      <c r="E267" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
     <row r="268" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B268" t="s">
+      <c r="D268" s="1"/>
+    </row>
+    <row r="269" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D269" s="1"/>
+    </row>
+    <row r="270" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D270" s="1"/>
+    </row>
+    <row r="274" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B274" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="269" spans="2:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="C269" s="3" t="s">
+    <row r="275" spans="2:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="C275" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D269" s="2" t="s">
+      <c r="D275" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E269" s="1" t="s">
+      <c r="E275" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="270" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C270" t="s">
+    <row r="276" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C276" t="s">
         <v>186</v>
       </c>
-      <c r="E270" s="1" t="s">
+      <c r="E276" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="271" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C271" t="s">
+    <row r="277" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C277" t="s">
         <v>214</v>
       </c>
-      <c r="E271" s="1" t="s">
+      <c r="E277" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="273" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D273" t="s">
+    <row r="279" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D279" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="275" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C275" t="s">
+    <row r="281" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C281" t="s">
         <v>241</v>
       </c>
-      <c r="D275" t="s">
+      <c r="D281" t="s">
         <v>242</v>
       </c>
-      <c r="E275" s="1" t="s">
+      <c r="E281" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="276" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C276" t="s">
+    <row r="282" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C282" t="s">
         <v>268</v>
       </c>
-      <c r="D276" t="s">
+      <c r="D282" t="s">
         <v>269</v>
       </c>
-      <c r="E276" s="1" t="s">
+      <c r="E282" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="277" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C277" t="s">
+    <row r="283" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C283" t="s">
         <v>283</v>
       </c>
-      <c r="E277" s="1" t="s">
+      <c r="E283" s="1" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="278" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E278" s="1" t="s">
+    <row r="284" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E284" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="279" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E279" s="1" t="s">
+    <row r="285" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E285" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="280" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C280" t="s">
+    <row r="286" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C286" t="s">
         <v>287</v>
       </c>
-      <c r="E280" s="1" t="s">
+      <c r="E286" s="1" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="281" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C281" t="s">
+    <row r="287" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C287" t="s">
         <v>298</v>
       </c>
-      <c r="E281" s="1" t="s">
+      <c r="E287" s="1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="282" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E282" s="1"/>
-    </row>
-    <row r="283" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C283" t="s">
+    <row r="288" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E288" s="1"/>
+    </row>
+    <row r="289" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C289" t="s">
         <v>358</v>
       </c>
-      <c r="D283" t="s">
+      <c r="D289" t="s">
         <v>359</v>
       </c>
-      <c r="E283" s="1" t="s">
+      <c r="E289" s="1" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="284" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E284" s="1"/>
-    </row>
-    <row r="285" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E285" s="1"/>
-    </row>
-    <row r="286" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E286" s="1"/>
-    </row>
-    <row r="287" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E287" s="1"/>
-    </row>
-    <row r="288" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E288" s="1"/>
-    </row>
-    <row r="289" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E289" s="1"/>
     </row>
     <row r="290" spans="3:8" x14ac:dyDescent="0.2">
       <c r="E290" s="1"/>
@@ -4992,1418 +4974,1436 @@
       <c r="E291" s="1"/>
     </row>
     <row r="292" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C292" t="s">
+      <c r="E292" s="1"/>
+    </row>
+    <row r="293" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E293" s="1"/>
+    </row>
+    <row r="294" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E294" s="1"/>
+    </row>
+    <row r="295" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E295" s="1"/>
+    </row>
+    <row r="296" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E296" s="1"/>
+    </row>
+    <row r="297" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E297" s="1"/>
+    </row>
+    <row r="298" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C298" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="293" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D293" t="s">
-        <v>134</v>
-      </c>
-      <c r="E293" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="294" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D294" t="s">
-        <v>135</v>
-      </c>
-      <c r="E294" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="295" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D295" t="s">
-        <v>139</v>
-      </c>
-      <c r="E295" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="296" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D296" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="297" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D297" t="s">
-        <v>141</v>
-      </c>
-      <c r="E297" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="298" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D298" t="s">
-        <v>482</v>
-      </c>
-      <c r="E298" t="s">
-        <v>484</v>
-      </c>
-      <c r="F298" t="s">
-        <v>488</v>
-      </c>
-      <c r="G298" t="s">
-        <v>483</v>
-      </c>
-      <c r="H298" s="1" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="299" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D299" t="s">
-        <v>485</v>
+        <v>134</v>
       </c>
       <c r="E299" t="s">
-        <v>486</v>
-      </c>
-      <c r="G299" t="s">
-        <v>487</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="300" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D300" t="s">
+        <v>135</v>
+      </c>
+      <c r="E300" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="301" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C301" t="s">
-        <v>366</v>
+      <c r="D301" t="s">
+        <v>139</v>
+      </c>
+      <c r="E301" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="302" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D302" t="s">
-        <v>72</v>
-      </c>
-      <c r="E302" t="s">
-        <v>73</v>
-      </c>
-      <c r="F302" s="1" t="s">
-        <v>74</v>
+        <v>136</v>
       </c>
     </row>
     <row r="303" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D303" t="s">
-        <v>75</v>
-      </c>
-      <c r="E303" s="1" t="s">
-        <v>76</v>
+        <v>141</v>
+      </c>
+      <c r="E303" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="304" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D304" t="s">
-        <v>77</v>
-      </c>
-      <c r="E304" s="1" t="s">
-        <v>78</v>
+        <v>482</v>
+      </c>
+      <c r="E304" t="s">
+        <v>484</v>
+      </c>
+      <c r="F304" t="s">
+        <v>488</v>
+      </c>
+      <c r="G304" t="s">
+        <v>483</v>
+      </c>
+      <c r="H304" s="1" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="305" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D305" t="s">
-        <v>80</v>
-      </c>
-      <c r="E305" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="306" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D306" t="s">
-        <v>361</v>
-      </c>
-      <c r="E306" t="s">
-        <v>364</v>
+        <v>485</v>
+      </c>
+      <c r="E305" t="s">
+        <v>486</v>
+      </c>
+      <c r="G305" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="307" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D307" t="s">
-        <v>362</v>
-      </c>
-      <c r="E307" t="s">
-        <v>363</v>
+      <c r="C307" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="308" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D308" t="s">
+        <v>72</v>
+      </c>
+      <c r="E308" t="s">
+        <v>73</v>
+      </c>
+      <c r="F308" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="309" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D309" t="s">
-        <v>81</v>
-      </c>
-      <c r="E309" t="s">
-        <v>82</v>
+        <v>75</v>
+      </c>
+      <c r="E309" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="310" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D310" t="s">
-        <v>83</v>
-      </c>
-      <c r="E310" t="s">
-        <v>84</v>
+        <v>77</v>
+      </c>
+      <c r="E310" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="311" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D311" t="s">
+        <v>80</v>
+      </c>
+      <c r="E311" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="312" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C312" t="s">
-        <v>365</v>
+      <c r="D312" t="s">
+        <v>361</v>
+      </c>
+      <c r="E312" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="313" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D313" t="s">
-        <v>72</v>
+        <v>362</v>
       </c>
       <c r="E313" t="s">
-        <v>130</v>
-      </c>
-      <c r="F313" s="1"/>
-    </row>
-    <row r="314" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D314" t="s">
-        <v>146</v>
-      </c>
-      <c r="E314" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F314" s="1"/>
+        <v>363</v>
+      </c>
     </row>
     <row r="315" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D315" t="s">
-        <v>75</v>
-      </c>
-      <c r="E315" s="1" t="s">
-        <v>148</v>
+        <v>81</v>
+      </c>
+      <c r="E315" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="316" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E316" s="1"/>
-    </row>
-    <row r="317" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D317" t="s">
-        <v>143</v>
+      <c r="D316" t="s">
+        <v>83</v>
+      </c>
+      <c r="E316" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="318" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E318" t="s">
-        <v>150</v>
-      </c>
-      <c r="F318" t="s">
-        <v>149</v>
+      <c r="C318" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="319" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D319" t="s">
+        <v>72</v>
+      </c>
       <c r="E319" t="s">
-        <v>151</v>
-      </c>
-      <c r="F319" t="s">
-        <v>144</v>
-      </c>
-      <c r="G319" s="1" t="s">
-        <v>145</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="F319" s="1"/>
     </row>
     <row r="320" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D320" t="s">
+        <v>146</v>
+      </c>
+      <c r="E320" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F320" s="1"/>
+    </row>
+    <row r="321" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D321" t="s">
+        <v>75</v>
+      </c>
+      <c r="E321" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="322" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E322" s="1"/>
+    </row>
+    <row r="323" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D323" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="324" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E324" t="s">
+        <v>150</v>
+      </c>
+      <c r="F324" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="325" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E325" t="s">
+        <v>151</v>
+      </c>
+      <c r="F325" t="s">
+        <v>144</v>
+      </c>
+      <c r="G325" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="326" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D326" t="s">
         <v>152</v>
       </c>
-      <c r="E320" s="1" t="s">
+      <c r="E326" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G320" s="1"/>
-    </row>
-    <row r="334" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E334" s="1"/>
-    </row>
-    <row r="336" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B336" t="s">
+      <c r="G326" s="1"/>
+    </row>
+    <row r="340" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E340" s="1"/>
+    </row>
+    <row r="342" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B342" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="337" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C337" t="s">
+    <row r="343" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C343" t="s">
         <v>276</v>
       </c>
-      <c r="D337" t="s">
+      <c r="D343" t="s">
         <v>278</v>
       </c>
-      <c r="E337" s="1" t="s">
+      <c r="E343" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="338" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C338" t="s">
+    <row r="344" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C344" t="s">
         <v>280</v>
       </c>
-      <c r="E338" s="1" t="s">
+      <c r="E344" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="F338" s="1" t="s">
+      <c r="F344" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="G338" s="1" t="s">
+      <c r="G344" s="1" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="339" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C339" t="s">
+    <row r="345" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C345" t="s">
         <v>289</v>
       </c>
-      <c r="E339" s="1" t="s">
+      <c r="E345" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="340" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C340" t="s">
+    <row r="346" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C346" t="s">
         <v>303</v>
       </c>
-      <c r="E340" s="1" t="s">
+      <c r="E346" s="1" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="341" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D341" t="s">
+    <row r="347" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D347" t="s">
         <v>305</v>
       </c>
-      <c r="E341" s="1" t="s">
+      <c r="E347" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="342" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C342" t="s">
+    <row r="348" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C348" t="s">
         <v>323</v>
       </c>
-      <c r="E342" s="1" t="s">
+      <c r="E348" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="343" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C343" t="s">
+    <row r="349" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C349" t="s">
         <v>307</v>
       </c>
-      <c r="D343" t="s">
+      <c r="D349" t="s">
         <v>308</v>
       </c>
-      <c r="E343" s="1" t="s">
+      <c r="E349" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="344" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C344" t="s">
+    <row r="350" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C350" t="s">
         <v>310</v>
       </c>
-      <c r="E344" s="1" t="s">
+      <c r="E350" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="345" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C345" t="s">
+    <row r="351" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C351" t="s">
         <v>315</v>
       </c>
-      <c r="E345" s="1" t="s">
+      <c r="E351" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="346" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C346" t="s">
+    <row r="352" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C352" t="s">
         <v>316</v>
       </c>
-      <c r="E346" s="1" t="s">
+      <c r="E352" s="1" t="s">
         <v>317</v>
-      </c>
-    </row>
-    <row r="347" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C347" t="s">
-        <v>318</v>
-      </c>
-      <c r="E347" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="348" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C348" t="s">
-        <v>325</v>
-      </c>
-      <c r="D348" t="s">
-        <v>332</v>
-      </c>
-      <c r="E348" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="349" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D349" t="s">
-        <v>327</v>
-      </c>
-      <c r="E349" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="351" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C351" t="s">
-        <v>329</v>
-      </c>
-      <c r="D351" t="s">
-        <v>330</v>
-      </c>
-      <c r="E351" s="1" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="353" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C353" t="s">
+        <v>318</v>
+      </c>
+      <c r="E353" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="354" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C354" t="s">
+        <v>325</v>
+      </c>
+      <c r="D354" t="s">
+        <v>332</v>
+      </c>
+      <c r="E354" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="355" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D355" t="s">
+        <v>327</v>
+      </c>
+      <c r="E355" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="357" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C357" t="s">
+        <v>329</v>
+      </c>
+      <c r="D357" t="s">
+        <v>330</v>
+      </c>
+      <c r="E357" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="359" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C359" t="s">
         <v>335</v>
       </c>
-      <c r="D353" t="s">
+      <c r="D359" t="s">
         <v>337</v>
       </c>
-      <c r="E353" s="1" t="s">
+      <c r="E359" s="1" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="357" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B357" t="s">
+    <row r="363" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B363" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="358" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C358" t="s">
+    <row r="364" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C364" t="s">
         <v>341</v>
       </c>
-      <c r="D358" t="s">
+      <c r="D364" t="s">
         <v>339</v>
       </c>
-      <c r="E358" s="1" t="s">
+      <c r="E364" s="1" t="s">
         <v>340</v>
-      </c>
-    </row>
-    <row r="364" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B364" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="365" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C365" t="s">
-        <v>86</v>
-      </c>
-      <c r="D365" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="366" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C366" t="s">
-        <v>88</v>
-      </c>
-      <c r="D366" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="367" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C367" t="s">
-        <v>95</v>
-      </c>
-      <c r="D367" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="368" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C368" t="s">
-        <v>97</v>
-      </c>
-      <c r="D368" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="370" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B370" t="s">
-        <v>90</v>
-      </c>
-      <c r="C370" t="s">
-        <v>91</v>
-      </c>
-      <c r="D370" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="371" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C371" t="s">
+        <v>86</v>
+      </c>
+      <c r="D371" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="372" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C372" t="s">
+        <v>88</v>
+      </c>
+      <c r="D372" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="373" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C373" t="s">
+        <v>95</v>
+      </c>
+      <c r="D373" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="374" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C374" t="s">
+        <v>97</v>
+      </c>
+      <c r="D374" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="376" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B376" t="s">
+        <v>90</v>
+      </c>
+      <c r="C376" t="s">
+        <v>91</v>
+      </c>
+      <c r="D376" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="377" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C377" t="s">
         <v>93</v>
       </c>
-      <c r="D371" t="s">
+      <c r="D377" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="374" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B374" t="s">
+    <row r="380" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B380" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="375" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C375" t="s">
+    <row r="381" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C381" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="376" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D376" t="s">
+    <row r="382" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D382" t="s">
         <v>104</v>
       </c>
-      <c r="E376" s="1" t="s">
+      <c r="E382" s="1" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="377" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D377" t="s">
-        <v>101</v>
-      </c>
-      <c r="E377" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="378" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D378" t="s">
-        <v>102</v>
-      </c>
-      <c r="E378" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="379" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D379" t="s">
-        <v>107</v>
-      </c>
-      <c r="E379" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="381" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B381" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="382" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C382" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="383" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D383" t="s">
-        <v>110</v>
+        <v>101</v>
+      </c>
+      <c r="E383" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="384" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D384" t="s">
-        <v>111</v>
+        <v>102</v>
+      </c>
+      <c r="E384" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="385" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F385" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="386" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B386" t="s">
-        <v>1</v>
-      </c>
-      <c r="F386" s="1" t="s">
-        <v>123</v>
+      <c r="D385" t="s">
+        <v>107</v>
+      </c>
+      <c r="E385" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="387" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C387" t="s">
-        <v>112</v>
-      </c>
-      <c r="D387" s="1" t="s">
-        <v>113</v>
+      <c r="B387" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="388" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D388" t="s">
-        <v>126</v>
-      </c>
-      <c r="E388" s="1" t="s">
-        <v>125</v>
+      <c r="C388" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="389" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C389" t="s">
-        <v>114</v>
+      <c r="D389" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="390" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D390" t="s">
-        <v>115</v>
-      </c>
-      <c r="E390" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F390" t="s">
-        <v>128</v>
-      </c>
-      <c r="G390" s="1" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
     </row>
     <row r="391" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E391" t="s">
-        <v>121</v>
-      </c>
-      <c r="G391" s="1"/>
+      <c r="F391" s="1" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="392" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E392" t="s">
-        <v>124</v>
-      </c>
-      <c r="G392" s="1"/>
+      <c r="B392" t="s">
+        <v>1</v>
+      </c>
+      <c r="F392" s="1" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="393" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D393" t="s">
-        <v>117</v>
-      </c>
-      <c r="E393" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G393" s="1"/>
+      <c r="C393" t="s">
+        <v>112</v>
+      </c>
+      <c r="D393" s="1" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="394" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D394" t="s">
+        <v>126</v>
+      </c>
+      <c r="E394" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="395" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C395" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="396" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D396" t="s">
+        <v>115</v>
+      </c>
+      <c r="E396" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F396" t="s">
+        <v>128</v>
+      </c>
+      <c r="G396" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="397" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E397" t="s">
+        <v>121</v>
+      </c>
+      <c r="G397" s="1"/>
+    </row>
+    <row r="398" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E398" t="s">
+        <v>124</v>
+      </c>
+      <c r="G398" s="1"/>
+    </row>
+    <row r="399" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D399" t="s">
+        <v>117</v>
+      </c>
+      <c r="E399" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G399" s="1"/>
+    </row>
+    <row r="400" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D400" t="s">
         <v>119</v>
       </c>
-      <c r="E394" s="1" t="s">
+      <c r="E400" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G394" s="1"/>
-    </row>
-    <row r="395" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E395" s="1" t="s">
+      <c r="G400" s="1"/>
+    </row>
+    <row r="401" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E401" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="G395" s="1"/>
-    </row>
-    <row r="396" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E396" t="s">
+      <c r="G401" s="1"/>
+    </row>
+    <row r="402" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E402" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="397" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D397" t="s">
+    <row r="403" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D403" t="s">
         <v>301</v>
       </c>
-      <c r="E397" s="1" t="s">
+      <c r="E403" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="398" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D398" t="s">
+    <row r="404" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D404" t="s">
         <v>300</v>
       </c>
-      <c r="E398" s="1" t="s">
+      <c r="E404" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="403" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C403" t="s">
+    <row r="409" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C409" t="s">
         <v>131</v>
       </c>
-      <c r="D403" s="1" t="s">
+      <c r="D409" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="407" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B407" t="s">
+    <row r="413" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B413" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="408" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C408" t="s">
+    <row r="414" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C414" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="409" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D409" t="s">
+    <row r="415" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D415" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="410" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E410" t="s">
+    <row r="416" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E416" t="s">
         <v>492</v>
       </c>
-      <c r="F410" s="1" t="s">
+      <c r="F416" s="1" t="s">
         <v>491</v>
-      </c>
-    </row>
-    <row r="411" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E411" t="s">
-        <v>494</v>
-      </c>
-      <c r="F411" s="1" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="412" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E412" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="413" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D413" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="414" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E414" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="415" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E415" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="416" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D416" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="417" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E417" t="s">
-        <v>499</v>
+        <v>494</v>
+      </c>
+      <c r="F417" s="1" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="418" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C418" t="s">
-        <v>500</v>
+      <c r="E418" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="419" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D419" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="420" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E420" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="421" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E421" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="422" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D422" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="423" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E423" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="424" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C424" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="425" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D425" t="s">
         <v>503</v>
       </c>
-      <c r="E419" t="s">
+      <c r="E425" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="420" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D420" t="s">
+    <row r="426" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D426" t="s">
         <v>501</v>
       </c>
-      <c r="E420" t="s">
+      <c r="E426" t="s">
         <v>502</v>
-      </c>
-    </row>
-    <row r="422" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C422" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="423" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D423" t="s">
-        <v>508</v>
-      </c>
-      <c r="E423" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="424" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D424" t="s">
-        <v>509</v>
-      </c>
-      <c r="E424" t="s">
-        <v>507</v>
-      </c>
-      <c r="G424" s="1" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="426" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C426" t="s">
-        <v>512</v>
-      </c>
-      <c r="G426" s="1" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="428" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C428" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="429" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D429" t="s">
+        <v>508</v>
+      </c>
+      <c r="E429" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="430" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D430" t="s">
+        <v>509</v>
+      </c>
+      <c r="E430" t="s">
+        <v>507</v>
+      </c>
+      <c r="G430" s="1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="432" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C432" t="s">
+        <v>512</v>
+      </c>
+      <c r="G432" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="434" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C434" t="s">
         <v>513</v>
       </c>
-      <c r="E428" t="s">
+      <c r="E434" t="s">
         <v>514</v>
       </c>
-      <c r="G428" s="1" t="s">
+      <c r="G434" s="1" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="430" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C430" t="s">
+    <row r="436" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C436" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="431" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D431" t="s">
+    <row r="437" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D437" t="s">
         <v>518</v>
       </c>
-      <c r="E431" t="s">
+      <c r="E437" t="s">
         <v>517</v>
       </c>
-      <c r="G431" s="1" t="s">
+      <c r="G437" s="1" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="432" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D432" t="s">
+    <row r="438" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D438" t="s">
         <v>519</v>
       </c>
-      <c r="E432" t="s">
+      <c r="E438" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="434" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C434" t="s">
+    <row r="440" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C440" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="435" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D435" t="s">
+    <row r="441" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D441" t="s">
         <v>528</v>
       </c>
-      <c r="E435" t="s">
+      <c r="E441" t="s">
         <v>524</v>
       </c>
-      <c r="G435" s="1" t="s">
+      <c r="G441" s="1" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="436" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D436" t="s">
+    <row r="442" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D442" t="s">
         <v>526</v>
       </c>
-      <c r="E436" t="s">
+      <c r="E442" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="437" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D437" t="s">
+    <row r="443" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D443" t="s">
         <v>527</v>
       </c>
-      <c r="E437" t="s">
+      <c r="E443" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="438" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C438" t="s">
+    <row r="444" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C444" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="439" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D439" t="s">
+    <row r="445" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D445" t="s">
         <v>630</v>
       </c>
-      <c r="E439" t="s">
+      <c r="E445" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="440" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D440" t="s">
+    <row r="446" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D446" t="s">
         <v>632</v>
       </c>
-      <c r="E440" t="s">
+      <c r="E446" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="441" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D441" t="s">
+    <row r="447" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D447" t="s">
         <v>634</v>
       </c>
-      <c r="E441" t="s">
+      <c r="E447" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="442" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D442" t="s">
+    <row r="448" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D448" t="s">
         <v>637</v>
       </c>
-      <c r="E442" t="s">
+      <c r="E448" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="443" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D443" t="s">
+    <row r="449" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D449" t="s">
         <v>693</v>
       </c>
-      <c r="E443" t="s">
+      <c r="E449" t="s">
         <v>695</v>
       </c>
-      <c r="G443" s="1" t="s">
+      <c r="G449" s="1" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="446" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B446" t="s">
+    <row r="452" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B452" t="s">
         <v>778</v>
       </c>
     </row>
-    <row r="447" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C447" t="s">
+    <row r="453" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C453" t="s">
         <v>779</v>
       </c>
-      <c r="G447" s="1" t="s">
+      <c r="G453" s="1" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="456" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B456" t="s">
+    <row r="462" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B462" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="457" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C457" t="s">
+    <row r="463" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C463" t="s">
         <v>540</v>
-      </c>
-    </row>
-    <row r="458" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D458" t="s">
-        <v>541</v>
-      </c>
-      <c r="G458" s="1" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="459" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C459" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="460" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D460" t="s">
-        <v>543</v>
-      </c>
-      <c r="E460" t="s">
-        <v>544</v>
-      </c>
-      <c r="G460" s="1" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="462" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C462" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="463" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D463" t="s">
-        <v>548</v>
-      </c>
-      <c r="E463" t="s">
-        <v>549</v>
-      </c>
-      <c r="G463" s="1" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="464" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D464" t="s">
-        <v>550</v>
-      </c>
-      <c r="E464" t="s">
-        <v>551</v>
+        <v>541</v>
+      </c>
+      <c r="G464" s="1" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="465" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D465" t="s">
-        <v>552</v>
-      </c>
-      <c r="E465" t="s">
-        <v>553</v>
+      <c r="C465" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="466" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D466" t="s">
-        <v>554</v>
+        <v>543</v>
       </c>
       <c r="E466" t="s">
-        <v>555</v>
+        <v>544</v>
+      </c>
+      <c r="G466" s="1" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="468" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C468" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
     </row>
     <row r="469" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D469" t="s">
-        <v>558</v>
+        <v>548</v>
       </c>
       <c r="E469" t="s">
-        <v>560</v>
+        <v>549</v>
       </c>
       <c r="G469" s="1" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
     </row>
     <row r="470" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D470" t="s">
-        <v>559</v>
+        <v>550</v>
       </c>
       <c r="E470" t="s">
-        <v>561</v>
+        <v>551</v>
+      </c>
+    </row>
+    <row r="471" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D471" t="s">
+        <v>552</v>
+      </c>
+      <c r="E471" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="472" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C472" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="473" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D473" t="s">
-        <v>565</v>
-      </c>
-      <c r="G473" s="1" t="s">
-        <v>564</v>
+      <c r="D472" t="s">
+        <v>554</v>
+      </c>
+      <c r="E472" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="474" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C474" t="s">
-        <v>608</v>
-      </c>
-      <c r="G474" s="1"/>
+        <v>557</v>
+      </c>
     </row>
     <row r="475" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D475" t="s">
+        <v>558</v>
+      </c>
+      <c r="E475" t="s">
+        <v>560</v>
+      </c>
+      <c r="G475" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="476" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D476" t="s">
+        <v>559</v>
+      </c>
+      <c r="E476" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="478" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C478" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="479" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D479" t="s">
+        <v>565</v>
+      </c>
+      <c r="G479" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="480" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C480" t="s">
+        <v>608</v>
+      </c>
+      <c r="G480" s="1"/>
+    </row>
+    <row r="481" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D481" t="s">
         <v>609</v>
       </c>
-      <c r="E475" t="s">
+      <c r="E481" t="s">
         <v>610</v>
       </c>
-      <c r="G475" s="1" t="s">
+      <c r="G481" s="1" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="476" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="G476" s="1"/>
-    </row>
-    <row r="477" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C477" t="s">
+    <row r="482" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G482" s="1"/>
+    </row>
+    <row r="483" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C483" t="s">
         <v>836</v>
       </c>
-      <c r="G477" s="1"/>
-    </row>
-    <row r="478" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D478" t="s">
+      <c r="G483" s="1"/>
+    </row>
+    <row r="484" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D484" t="s">
         <v>837</v>
       </c>
-      <c r="G478" s="1" t="s">
+      <c r="G484" s="1" t="s">
         <v>838</v>
-      </c>
-    </row>
-    <row r="479" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C479" t="s">
-        <v>892</v>
-      </c>
-      <c r="G479" s="1"/>
-    </row>
-    <row r="480" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D480" t="s">
-        <v>893</v>
-      </c>
-      <c r="G480" s="1" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="481" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G481" s="1"/>
-    </row>
-    <row r="484" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B484" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="485" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C485" t="s">
+        <v>892</v>
+      </c>
+      <c r="G485" s="1"/>
+    </row>
+    <row r="486" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D486" t="s">
+        <v>893</v>
+      </c>
+      <c r="G486" s="1" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="487" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G487" s="1"/>
+    </row>
+    <row r="490" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B490" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="491" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C491" t="s">
         <v>567</v>
-      </c>
-    </row>
-    <row r="486" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E486" t="s">
-        <v>568</v>
-      </c>
-      <c r="G486" s="1" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="489" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B489" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="490" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C490" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="491" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D491" t="s">
-        <v>572</v>
-      </c>
-      <c r="E491" t="s">
-        <v>573</v>
-      </c>
-      <c r="F491" t="s">
-        <v>574</v>
-      </c>
-      <c r="G491" s="1" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="492" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E492" t="s">
-        <v>576</v>
-      </c>
-      <c r="F492" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="493" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C493" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="494" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D494" t="s">
-        <v>595</v>
-      </c>
-      <c r="E494" t="s">
-        <v>596</v>
+        <v>568</v>
+      </c>
+      <c r="G492" s="1" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="495" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D495" t="s">
-        <v>598</v>
-      </c>
-      <c r="E495" t="s">
-        <v>597</v>
+      <c r="B495" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="496" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C496" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="497" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D497" t="s">
-        <v>599</v>
+        <v>572</v>
       </c>
       <c r="E497" t="s">
-        <v>600</v>
+        <v>573</v>
+      </c>
+      <c r="F497" t="s">
+        <v>574</v>
+      </c>
+      <c r="G497" s="1" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="498" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D498" t="s">
-        <v>601</v>
-      </c>
       <c r="E498" t="s">
-        <v>602</v>
+        <v>576</v>
+      </c>
+      <c r="F498" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="499" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C499" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="500" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D500" t="s">
-        <v>840</v>
+        <v>595</v>
       </c>
       <c r="E500" t="s">
-        <v>839</v>
+        <v>596</v>
       </c>
     </row>
     <row r="501" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D501" t="s">
-        <v>841</v>
+        <v>598</v>
       </c>
       <c r="E501" t="s">
-        <v>603</v>
-      </c>
-      <c r="G501" s="1" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="502" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D502" t="s">
-        <v>604</v>
-      </c>
-      <c r="E502" t="s">
-        <v>605</v>
-      </c>
-      <c r="F502" t="s">
-        <v>606</v>
+        <v>597</v>
+      </c>
+    </row>
+    <row r="503" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D503" t="s">
+        <v>599</v>
+      </c>
+      <c r="E503" t="s">
+        <v>600</v>
       </c>
     </row>
     <row r="504" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D504" t="s">
-        <v>842</v>
+        <v>601</v>
       </c>
       <c r="E504" t="s">
-        <v>851</v>
-      </c>
-      <c r="F504" t="s">
-        <v>853</v>
-      </c>
-      <c r="H504" s="1" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="505" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E505" t="s">
-        <v>850</v>
-      </c>
-      <c r="F505" t="s">
-        <v>843</v>
-      </c>
-      <c r="G505" t="s">
-        <v>844</v>
-      </c>
-      <c r="H505" s="1" t="s">
-        <v>845</v>
+        <v>602</v>
       </c>
     </row>
     <row r="506" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="G506" s="1"/>
+      <c r="D506" t="s">
+        <v>840</v>
+      </c>
+      <c r="E506" t="s">
+        <v>839</v>
+      </c>
     </row>
     <row r="507" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D507" t="s">
-        <v>846</v>
+        <v>841</v>
       </c>
       <c r="E507" t="s">
-        <v>847</v>
+        <v>603</v>
       </c>
       <c r="G507" s="1" t="s">
-        <v>849</v>
+        <v>607</v>
       </c>
     </row>
     <row r="508" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D508" t="s">
+        <v>604</v>
+      </c>
       <c r="E508" t="s">
-        <v>848</v>
-      </c>
-      <c r="G508" s="1"/>
-    </row>
-    <row r="509" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C509" t="s">
-        <v>862</v>
-      </c>
-      <c r="G509" s="1"/>
+        <v>605</v>
+      </c>
+      <c r="F508" t="s">
+        <v>606</v>
+      </c>
     </row>
     <row r="510" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D510" t="s">
-        <v>863</v>
+        <v>842</v>
       </c>
       <c r="E510" t="s">
-        <v>574</v>
-      </c>
-      <c r="G510" s="1"/>
+        <v>851</v>
+      </c>
+      <c r="F510" t="s">
+        <v>853</v>
+      </c>
+      <c r="H510" s="1" t="s">
+        <v>852</v>
+      </c>
     </row>
     <row r="511" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D511" t="s">
-        <v>864</v>
-      </c>
       <c r="E511" t="s">
-        <v>577</v>
-      </c>
-      <c r="G511" s="1"/>
+        <v>850</v>
+      </c>
+      <c r="F511" t="s">
+        <v>843</v>
+      </c>
+      <c r="G511" t="s">
+        <v>844</v>
+      </c>
+      <c r="H511" s="1" t="s">
+        <v>845</v>
+      </c>
     </row>
     <row r="512" spans="3:8" x14ac:dyDescent="0.2">
       <c r="G512" s="1"/>
     </row>
+    <row r="513" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D513" t="s">
+        <v>846</v>
+      </c>
+      <c r="E513" t="s">
+        <v>847</v>
+      </c>
+      <c r="G513" s="1" t="s">
+        <v>849</v>
+      </c>
+    </row>
     <row r="514" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B514" t="s">
-        <v>578</v>
-      </c>
+      <c r="E514" t="s">
+        <v>848</v>
+      </c>
+      <c r="G514" s="1"/>
     </row>
     <row r="515" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C515" t="s">
-        <v>579</v>
-      </c>
+        <v>862</v>
+      </c>
+      <c r="G515" s="1"/>
     </row>
     <row r="516" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D516" t="s">
+        <v>863</v>
+      </c>
+      <c r="E516" t="s">
+        <v>574</v>
+      </c>
+      <c r="G516" s="1"/>
+    </row>
+    <row r="517" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D517" t="s">
+        <v>864</v>
+      </c>
+      <c r="E517" t="s">
+        <v>577</v>
+      </c>
+      <c r="G517" s="1"/>
+    </row>
+    <row r="518" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G518" s="1"/>
+    </row>
+    <row r="520" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B520" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="521" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C521" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="522" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D522" t="s">
         <v>581</v>
       </c>
-      <c r="E516" t="s">
+      <c r="E522" t="s">
         <v>582</v>
       </c>
-      <c r="F516" t="s">
+      <c r="F522" t="s">
         <v>580</v>
       </c>
-      <c r="G516" s="1" t="s">
+      <c r="G522" s="1" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="517" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E517" t="s">
+    <row r="523" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E523" t="s">
         <v>583</v>
       </c>
-      <c r="F517" t="s">
+      <c r="F523" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="519" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D519" t="s">
+    <row r="525" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D525" t="s">
         <v>586</v>
       </c>
-      <c r="E519" t="s">
+      <c r="E525" t="s">
         <v>588</v>
       </c>
-      <c r="F519" t="s">
+      <c r="F525" t="s">
         <v>587</v>
-      </c>
-    </row>
-    <row r="522" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B522" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="523" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C523" t="s">
-        <v>707</v>
-      </c>
-      <c r="D523" t="s">
-        <v>710</v>
-      </c>
-      <c r="G523" s="1" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="524" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C524" t="s">
-        <v>708</v>
-      </c>
-      <c r="D524" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="525" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C525" t="s">
-        <v>709</v>
-      </c>
-      <c r="D525" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="528" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B528" t="s">
-        <v>730</v>
+        <v>706</v>
       </c>
     </row>
     <row r="529" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C529" t="s">
-        <v>731</v>
+        <v>707</v>
+      </c>
+      <c r="D529" t="s">
+        <v>710</v>
       </c>
       <c r="G529" s="1" t="s">
-        <v>732</v>
+        <v>713</v>
       </c>
     </row>
     <row r="530" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C530" t="s">
-        <v>733</v>
-      </c>
-      <c r="G530" s="1" t="s">
-        <v>734</v>
+        <v>708</v>
+      </c>
+      <c r="D530" t="s">
+        <v>711</v>
       </c>
     </row>
     <row r="531" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C531" t="s">
-        <v>737</v>
-      </c>
-      <c r="F531" t="s">
-        <v>735</v>
-      </c>
-      <c r="G531" s="1" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="533" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B533" t="s">
-        <v>742</v>
+        <v>709</v>
+      </c>
+      <c r="D531" t="s">
+        <v>712</v>
       </c>
     </row>
     <row r="534" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C534" t="s">
-        <v>743</v>
-      </c>
-      <c r="D534" t="s">
-        <v>744</v>
-      </c>
-      <c r="G534" s="1" t="s">
-        <v>745</v>
+      <c r="B534" t="s">
+        <v>730</v>
       </c>
     </row>
     <row r="535" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C535" t="s">
-        <v>746</v>
-      </c>
-      <c r="D535" t="s">
-        <v>747</v>
+        <v>731</v>
       </c>
       <c r="G535" s="1" t="s">
-        <v>748</v>
+        <v>732</v>
+      </c>
+    </row>
+    <row r="536" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C536" t="s">
+        <v>733</v>
+      </c>
+      <c r="G536" s="1" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="537" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C537" t="s">
+        <v>737</v>
+      </c>
+      <c r="F537" t="s">
+        <v>735</v>
+      </c>
+      <c r="G537" s="1" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="539" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B539" t="s">
-        <v>801</v>
+        <v>742</v>
       </c>
     </row>
     <row r="540" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C540" t="s">
-        <v>802</v>
+        <v>743</v>
       </c>
       <c r="D540" t="s">
-        <v>803</v>
-      </c>
-      <c r="E540" t="s">
-        <v>804</v>
+        <v>744</v>
       </c>
       <c r="G540" s="1" t="s">
-        <v>805</v>
+        <v>745</v>
       </c>
     </row>
     <row r="541" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C541" t="s">
-        <v>806</v>
-      </c>
-      <c r="E541" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="543" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B543" t="s">
-        <v>854</v>
-      </c>
-      <c r="G543" s="1" t="s">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="544" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C544" t="s">
-        <v>855</v>
+        <v>746</v>
+      </c>
+      <c r="D541" t="s">
+        <v>747</v>
+      </c>
+      <c r="G541" s="1" t="s">
+        <v>748</v>
       </c>
     </row>
     <row r="545" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D545" t="s">
-        <v>858</v>
+      <c r="B545" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="546" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C546" t="s">
+        <v>802</v>
+      </c>
+      <c r="D546" t="s">
+        <v>803</v>
+      </c>
+      <c r="E546" t="s">
+        <v>804</v>
+      </c>
+      <c r="G546" s="1" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="547" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C547" t="s">
+        <v>806</v>
+      </c>
+      <c r="E547" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="549" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B549" t="s">
+        <v>854</v>
+      </c>
+      <c r="G549" s="1" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="550" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C550" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="551" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D551" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="552" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C552" t="s">
         <v>856</v>
       </c>
     </row>
-    <row r="547" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D547" t="s">
+    <row r="553" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D553" t="s">
         <v>859</v>
       </c>
     </row>
-    <row r="548" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C548" t="s">
+    <row r="554" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C554" t="s">
         <v>857</v>
       </c>
     </row>
-    <row r="549" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D549" t="s">
+    <row r="555" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D555" t="s">
         <v>860</v>
       </c>
     </row>
-    <row r="552" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B552" t="s">
+    <row r="558" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B558" t="s">
         <v>876</v>
       </c>
     </row>
-    <row r="553" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C553" t="s">
+    <row r="559" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C559" t="s">
         <v>877</v>
       </c>
-      <c r="D553" t="s">
+      <c r="D559" t="s">
         <v>878</v>
       </c>
-      <c r="G553" s="1" t="s">
+      <c r="G559" s="1" t="s">
         <v>879</v>
       </c>
     </row>
@@ -6411,172 +6411,172 @@
   <hyperlinks>
     <hyperlink ref="C15" r:id="rId1" xr:uid="{18CCA2F1-1074-664C-AB52-48BBB42F9065}"/>
     <hyperlink ref="D18" r:id="rId2" xr:uid="{02227101-F5A2-3446-ADC1-32F3342C625C}"/>
-    <hyperlink ref="D56" r:id="rId3" xr:uid="{6360CC1D-0E6F-6B45-B16E-E9F323959E32}"/>
-    <hyperlink ref="E68" r:id="rId4" xr:uid="{96980E2B-5D77-D04D-8463-2374C6B90C21}"/>
-    <hyperlink ref="E85" r:id="rId5" xr:uid="{5081034D-5E40-F340-99D2-B8E4DFC0468C}"/>
-    <hyperlink ref="E88" r:id="rId6" location=":~:text=You%20can%20verify%20whether%20it,password%20and%20ESSID%20are%20correct." xr:uid="{3BA51E9E-8709-874E-B6EC-40074894ACA9}"/>
-    <hyperlink ref="E83" r:id="rId7" xr:uid="{30BD9D61-AAB4-2544-987A-0386CA068398}"/>
-    <hyperlink ref="E91" r:id="rId8" xr:uid="{1824F9BF-1BD9-3842-A565-00C06FF5E50F}"/>
-    <hyperlink ref="D162" r:id="rId9" xr:uid="{E488AECD-B504-A04E-8F27-807A3A08802C}"/>
-    <hyperlink ref="D116" r:id="rId10" location="89804" xr:uid="{E34C14F5-E723-0A48-894F-222B3F74BBF9}"/>
-    <hyperlink ref="D117" r:id="rId11" xr:uid="{6C20672B-9F8F-094F-9AC8-3D1FC1C85319}"/>
-    <hyperlink ref="D118" r:id="rId12" xr:uid="{BA9A8F05-4D7F-4942-886C-F8152208F0EA}"/>
-    <hyperlink ref="F122" r:id="rId13" xr:uid="{22AE585F-7255-3F41-8A2E-808446F3A9AA}"/>
-    <hyperlink ref="F124" r:id="rId14" xr:uid="{93472772-CF6C-D045-B634-2D574A3EE034}"/>
-    <hyperlink ref="E220" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
-    <hyperlink ref="F221" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
-    <hyperlink ref="D252" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
-    <hyperlink ref="D253" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
-    <hyperlink ref="F125" r:id="rId19" xr:uid="{92BE3560-5393-C545-9D2D-2B773359B28F}"/>
-    <hyperlink ref="E269" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
-    <hyperlink ref="E270" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
-    <hyperlink ref="E271" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
-    <hyperlink ref="E99" r:id="rId23" xr:uid="{1526D7DA-27DA-1443-928C-BEDA9E425734}"/>
-    <hyperlink ref="E100" r:id="rId24" xr:uid="{4F363062-BE49-AB4F-8956-2C1F31D9B898}"/>
-    <hyperlink ref="H126" r:id="rId25" xr:uid="{D9E13355-D59B-054F-B544-34A5A285A9E0}"/>
-    <hyperlink ref="G94" r:id="rId26" xr:uid="{170917BF-0643-9848-BCA9-A3BF5219EE3E}"/>
-    <hyperlink ref="F129" r:id="rId27" xr:uid="{5D45F2D3-11BC-6E43-BEFF-29E4E04A041E}"/>
-    <hyperlink ref="I130" r:id="rId28" xr:uid="{7D985D09-6A9A-FF4D-9F4A-4C56CC604DCE}"/>
-    <hyperlink ref="D119" r:id="rId29" xr:uid="{784C3F11-339F-8242-911D-6E4E893DD319}"/>
-    <hyperlink ref="E119" r:id="rId30" xr:uid="{FC907203-09BF-654B-9028-A8528783DAFE}"/>
-    <hyperlink ref="F131" r:id="rId31" xr:uid="{EFD3653A-B2F2-614F-8DEE-A2CB34111C94}"/>
-    <hyperlink ref="F132" r:id="rId32" xr:uid="{774B592D-11A5-9C49-BB9A-61014C8D8C81}"/>
-    <hyperlink ref="F133" r:id="rId33" xr:uid="{BD793670-4C63-C04D-B52D-974AF8E59FA4}"/>
-    <hyperlink ref="F134" r:id="rId34" location="96077" xr:uid="{B9804BBD-5312-714B-97EA-CC7D2C647F2C}"/>
-    <hyperlink ref="H127" r:id="rId35" xr:uid="{7BC5BAB5-D297-0043-BAAF-45AD255D5C84}"/>
-    <hyperlink ref="I126" r:id="rId36" xr:uid="{A03C56E4-1156-A148-A568-F50A5C33DB5C}"/>
-    <hyperlink ref="F135" r:id="rId37" xr:uid="{12AC219C-4678-4E43-B328-6595FA10B8D3}"/>
-    <hyperlink ref="E137" r:id="rId38" xr:uid="{44409621-28A2-704A-B283-3DCE1EFB1603}"/>
-    <hyperlink ref="E275" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
-    <hyperlink ref="F138" r:id="rId40" xr:uid="{A9D0D792-87D1-8144-872F-5CA060D3C28F}"/>
-    <hyperlink ref="F139" r:id="rId41" xr:uid="{87EF989D-17E9-1E45-A075-CD862D0B60F4}"/>
-    <hyperlink ref="F141" r:id="rId42" xr:uid="{8406C6F0-DC69-A64D-AAD8-60A33C12D00B}"/>
-    <hyperlink ref="F142" r:id="rId43" location="108593" xr:uid="{3C38F59E-6E71-4048-9BCA-CBC77D3907E0}"/>
-    <hyperlink ref="F144" r:id="rId44" xr:uid="{EEBE2A3E-36CA-F94F-9B1D-EE463DB6425F}"/>
-    <hyperlink ref="F145" r:id="rId45" xr:uid="{3782B43D-9E6F-2940-A013-34AA5D6B4DB3}"/>
-    <hyperlink ref="F146" r:id="rId46" xr:uid="{3D1C62DB-D9B7-BE42-B21D-4EEBC4C9EFE1}"/>
-    <hyperlink ref="F147" r:id="rId47" xr:uid="{F5021A21-70A2-D34E-B055-64CAC326E7EF}"/>
-    <hyperlink ref="F148" r:id="rId48" xr:uid="{A8C010A1-8EE1-264B-8688-3BEA1B62E535}"/>
-    <hyperlink ref="E276" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
-    <hyperlink ref="F143" r:id="rId50" location="113521" xr:uid="{EE1413C5-3B38-7D4D-8DF1-634A12F0BD81}"/>
-    <hyperlink ref="E101" r:id="rId51" xr:uid="{00B1EF4A-7791-0343-8D8C-9A1E83248FC9}"/>
-    <hyperlink ref="E337" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
-    <hyperlink ref="E338" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
-    <hyperlink ref="F150" r:id="rId54" xr:uid="{40A4B6A0-2F7E-A84D-8CC6-D814A33F5953}"/>
-    <hyperlink ref="E277" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
-    <hyperlink ref="E278" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
-    <hyperlink ref="E279" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
-    <hyperlink ref="E280" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
-    <hyperlink ref="E339" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
-    <hyperlink ref="D254" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
-    <hyperlink ref="D255" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
-    <hyperlink ref="D256" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
-    <hyperlink ref="E281" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
-    <hyperlink ref="E340" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
-    <hyperlink ref="E341" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
-    <hyperlink ref="E343" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
-    <hyperlink ref="E344" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
-    <hyperlink ref="F338" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
-    <hyperlink ref="G338" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
-    <hyperlink ref="E345" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
-    <hyperlink ref="E346" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
-    <hyperlink ref="E347" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
-    <hyperlink ref="E222" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
-    <hyperlink ref="E342" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
-    <hyperlink ref="E348" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
-    <hyperlink ref="E349" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
-    <hyperlink ref="E103" r:id="rId77" location="code" xr:uid="{C0475FF8-517D-E949-887E-9A42D86E9640}"/>
-    <hyperlink ref="E351" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
-    <hyperlink ref="E104" r:id="rId79" xr:uid="{277DBE6F-F3E5-8B4C-8DD8-BD92445D1A99}"/>
-    <hyperlink ref="E353" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
-    <hyperlink ref="E358" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
-    <hyperlink ref="E260" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
-    <hyperlink ref="E261" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
-    <hyperlink ref="F171" r:id="rId84" xr:uid="{EB604865-A16B-0646-A5B5-0D047467449D}"/>
-    <hyperlink ref="E283" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
-    <hyperlink ref="D367" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
-    <hyperlink ref="D368" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
-    <hyperlink ref="E377" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
-    <hyperlink ref="E378" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
-    <hyperlink ref="E376" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
-    <hyperlink ref="D387" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
-    <hyperlink ref="E393" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
-    <hyperlink ref="E390" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
-    <hyperlink ref="E394" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
-    <hyperlink ref="F385" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
-    <hyperlink ref="F386" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
-    <hyperlink ref="E388" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
-    <hyperlink ref="G390" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
-    <hyperlink ref="D403" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
-    <hyperlink ref="E395" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
-    <hyperlink ref="E398" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
-    <hyperlink ref="E397" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
-    <hyperlink ref="F302" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
-    <hyperlink ref="E303" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
-    <hyperlink ref="E304" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
-    <hyperlink ref="E305" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
-    <hyperlink ref="G319" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
-    <hyperlink ref="E314" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
-    <hyperlink ref="E315" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
-    <hyperlink ref="E320" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
-    <hyperlink ref="F183" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
-    <hyperlink ref="F188" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
-    <hyperlink ref="F189" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
-    <hyperlink ref="F196" r:id="rId114" xr:uid="{2B03B1F0-535A-3E4F-8FB3-35D2DE847218}"/>
-    <hyperlink ref="G201" r:id="rId115" xr:uid="{11045522-E183-B14C-B43D-5EA36E454600}"/>
-    <hyperlink ref="E223" r:id="rId116" xr:uid="{F1098A8C-3BC0-DB4F-8F9C-48B31145FEC1}"/>
-    <hyperlink ref="F203" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
-    <hyperlink ref="F197" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
-    <hyperlink ref="F206" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
-    <hyperlink ref="H298" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
-    <hyperlink ref="F410" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
-    <hyperlink ref="G424" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
-    <hyperlink ref="F411" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
-    <hyperlink ref="G426" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
-    <hyperlink ref="G428" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
-    <hyperlink ref="G431" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
-    <hyperlink ref="G435" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
-    <hyperlink ref="G460" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
-    <hyperlink ref="G458" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
-    <hyperlink ref="G463" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
-    <hyperlink ref="G469" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
-    <hyperlink ref="G473" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
-    <hyperlink ref="G486" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
-    <hyperlink ref="G491" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
-    <hyperlink ref="G516" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
+    <hyperlink ref="D62" r:id="rId3" xr:uid="{6360CC1D-0E6F-6B45-B16E-E9F323959E32}"/>
+    <hyperlink ref="E74" r:id="rId4" xr:uid="{96980E2B-5D77-D04D-8463-2374C6B90C21}"/>
+    <hyperlink ref="E91" r:id="rId5" xr:uid="{5081034D-5E40-F340-99D2-B8E4DFC0468C}"/>
+    <hyperlink ref="E94" r:id="rId6" location=":~:text=You%20can%20verify%20whether%20it,password%20and%20ESSID%20are%20correct." xr:uid="{3BA51E9E-8709-874E-B6EC-40074894ACA9}"/>
+    <hyperlink ref="E89" r:id="rId7" xr:uid="{30BD9D61-AAB4-2544-987A-0386CA068398}"/>
+    <hyperlink ref="E97" r:id="rId8" xr:uid="{1824F9BF-1BD9-3842-A565-00C06FF5E50F}"/>
+    <hyperlink ref="D168" r:id="rId9" xr:uid="{E488AECD-B504-A04E-8F27-807A3A08802C}"/>
+    <hyperlink ref="D122" r:id="rId10" location="89804" xr:uid="{E34C14F5-E723-0A48-894F-222B3F74BBF9}"/>
+    <hyperlink ref="D123" r:id="rId11" xr:uid="{6C20672B-9F8F-094F-9AC8-3D1FC1C85319}"/>
+    <hyperlink ref="D124" r:id="rId12" xr:uid="{BA9A8F05-4D7F-4942-886C-F8152208F0EA}"/>
+    <hyperlink ref="F128" r:id="rId13" xr:uid="{22AE585F-7255-3F41-8A2E-808446F3A9AA}"/>
+    <hyperlink ref="F130" r:id="rId14" xr:uid="{93472772-CF6C-D045-B634-2D574A3EE034}"/>
+    <hyperlink ref="E226" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
+    <hyperlink ref="F227" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
+    <hyperlink ref="D258" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
+    <hyperlink ref="D259" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
+    <hyperlink ref="F131" r:id="rId19" xr:uid="{92BE3560-5393-C545-9D2D-2B773359B28F}"/>
+    <hyperlink ref="E275" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
+    <hyperlink ref="E276" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
+    <hyperlink ref="E277" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
+    <hyperlink ref="E105" r:id="rId23" xr:uid="{1526D7DA-27DA-1443-928C-BEDA9E425734}"/>
+    <hyperlink ref="E106" r:id="rId24" xr:uid="{4F363062-BE49-AB4F-8956-2C1F31D9B898}"/>
+    <hyperlink ref="H132" r:id="rId25" xr:uid="{D9E13355-D59B-054F-B544-34A5A285A9E0}"/>
+    <hyperlink ref="G100" r:id="rId26" xr:uid="{170917BF-0643-9848-BCA9-A3BF5219EE3E}"/>
+    <hyperlink ref="F135" r:id="rId27" xr:uid="{5D45F2D3-11BC-6E43-BEFF-29E4E04A041E}"/>
+    <hyperlink ref="I136" r:id="rId28" xr:uid="{7D985D09-6A9A-FF4D-9F4A-4C56CC604DCE}"/>
+    <hyperlink ref="D125" r:id="rId29" xr:uid="{784C3F11-339F-8242-911D-6E4E893DD319}"/>
+    <hyperlink ref="E125" r:id="rId30" xr:uid="{FC907203-09BF-654B-9028-A8528783DAFE}"/>
+    <hyperlink ref="F137" r:id="rId31" xr:uid="{EFD3653A-B2F2-614F-8DEE-A2CB34111C94}"/>
+    <hyperlink ref="F138" r:id="rId32" xr:uid="{774B592D-11A5-9C49-BB9A-61014C8D8C81}"/>
+    <hyperlink ref="F139" r:id="rId33" xr:uid="{BD793670-4C63-C04D-B52D-974AF8E59FA4}"/>
+    <hyperlink ref="F140" r:id="rId34" location="96077" xr:uid="{B9804BBD-5312-714B-97EA-CC7D2C647F2C}"/>
+    <hyperlink ref="H133" r:id="rId35" xr:uid="{7BC5BAB5-D297-0043-BAAF-45AD255D5C84}"/>
+    <hyperlink ref="I132" r:id="rId36" xr:uid="{A03C56E4-1156-A148-A568-F50A5C33DB5C}"/>
+    <hyperlink ref="F141" r:id="rId37" xr:uid="{12AC219C-4678-4E43-B328-6595FA10B8D3}"/>
+    <hyperlink ref="E143" r:id="rId38" xr:uid="{44409621-28A2-704A-B283-3DCE1EFB1603}"/>
+    <hyperlink ref="E281" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
+    <hyperlink ref="F144" r:id="rId40" xr:uid="{A9D0D792-87D1-8144-872F-5CA060D3C28F}"/>
+    <hyperlink ref="F145" r:id="rId41" xr:uid="{87EF989D-17E9-1E45-A075-CD862D0B60F4}"/>
+    <hyperlink ref="F147" r:id="rId42" xr:uid="{8406C6F0-DC69-A64D-AAD8-60A33C12D00B}"/>
+    <hyperlink ref="F148" r:id="rId43" location="108593" xr:uid="{3C38F59E-6E71-4048-9BCA-CBC77D3907E0}"/>
+    <hyperlink ref="F150" r:id="rId44" xr:uid="{EEBE2A3E-36CA-F94F-9B1D-EE463DB6425F}"/>
+    <hyperlink ref="F151" r:id="rId45" xr:uid="{3782B43D-9E6F-2940-A013-34AA5D6B4DB3}"/>
+    <hyperlink ref="F152" r:id="rId46" xr:uid="{3D1C62DB-D9B7-BE42-B21D-4EEBC4C9EFE1}"/>
+    <hyperlink ref="F153" r:id="rId47" xr:uid="{F5021A21-70A2-D34E-B055-64CAC326E7EF}"/>
+    <hyperlink ref="F154" r:id="rId48" xr:uid="{A8C010A1-8EE1-264B-8688-3BEA1B62E535}"/>
+    <hyperlink ref="E282" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
+    <hyperlink ref="F149" r:id="rId50" location="113521" xr:uid="{EE1413C5-3B38-7D4D-8DF1-634A12F0BD81}"/>
+    <hyperlink ref="E107" r:id="rId51" xr:uid="{00B1EF4A-7791-0343-8D8C-9A1E83248FC9}"/>
+    <hyperlink ref="E343" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
+    <hyperlink ref="E344" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
+    <hyperlink ref="F156" r:id="rId54" xr:uid="{40A4B6A0-2F7E-A84D-8CC6-D814A33F5953}"/>
+    <hyperlink ref="E283" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
+    <hyperlink ref="E284" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
+    <hyperlink ref="E285" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
+    <hyperlink ref="E286" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
+    <hyperlink ref="E345" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
+    <hyperlink ref="D260" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
+    <hyperlink ref="D261" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
+    <hyperlink ref="D262" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
+    <hyperlink ref="E287" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
+    <hyperlink ref="E346" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
+    <hyperlink ref="E347" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
+    <hyperlink ref="E349" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
+    <hyperlink ref="E350" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
+    <hyperlink ref="F344" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
+    <hyperlink ref="G344" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
+    <hyperlink ref="E351" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
+    <hyperlink ref="E352" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
+    <hyperlink ref="E353" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
+    <hyperlink ref="E228" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
+    <hyperlink ref="E348" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
+    <hyperlink ref="E354" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
+    <hyperlink ref="E355" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
+    <hyperlink ref="E109" r:id="rId77" location="code" xr:uid="{C0475FF8-517D-E949-887E-9A42D86E9640}"/>
+    <hyperlink ref="E357" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
+    <hyperlink ref="E110" r:id="rId79" xr:uid="{277DBE6F-F3E5-8B4C-8DD8-BD92445D1A99}"/>
+    <hyperlink ref="E359" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
+    <hyperlink ref="E364" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
+    <hyperlink ref="E266" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
+    <hyperlink ref="E267" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
+    <hyperlink ref="F177" r:id="rId84" xr:uid="{EB604865-A16B-0646-A5B5-0D047467449D}"/>
+    <hyperlink ref="E289" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
+    <hyperlink ref="D373" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
+    <hyperlink ref="D374" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
+    <hyperlink ref="E383" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
+    <hyperlink ref="E384" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
+    <hyperlink ref="E382" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
+    <hyperlink ref="D393" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
+    <hyperlink ref="E399" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
+    <hyperlink ref="E396" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
+    <hyperlink ref="E400" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
+    <hyperlink ref="F391" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
+    <hyperlink ref="F392" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
+    <hyperlink ref="E394" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
+    <hyperlink ref="G396" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
+    <hyperlink ref="D409" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
+    <hyperlink ref="E401" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
+    <hyperlink ref="E404" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
+    <hyperlink ref="E403" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
+    <hyperlink ref="F308" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
+    <hyperlink ref="E309" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
+    <hyperlink ref="E310" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
+    <hyperlink ref="E311" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
+    <hyperlink ref="G325" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
+    <hyperlink ref="E320" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
+    <hyperlink ref="E321" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
+    <hyperlink ref="E326" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
+    <hyperlink ref="F189" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
+    <hyperlink ref="F194" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
+    <hyperlink ref="F195" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
+    <hyperlink ref="F202" r:id="rId114" xr:uid="{2B03B1F0-535A-3E4F-8FB3-35D2DE847218}"/>
+    <hyperlink ref="G207" r:id="rId115" xr:uid="{11045522-E183-B14C-B43D-5EA36E454600}"/>
+    <hyperlink ref="E229" r:id="rId116" xr:uid="{F1098A8C-3BC0-DB4F-8F9C-48B31145FEC1}"/>
+    <hyperlink ref="F209" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
+    <hyperlink ref="F203" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
+    <hyperlink ref="F212" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
+    <hyperlink ref="H304" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
+    <hyperlink ref="F416" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
+    <hyperlink ref="G430" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
+    <hyperlink ref="F417" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
+    <hyperlink ref="G432" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
+    <hyperlink ref="G434" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
+    <hyperlink ref="G437" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
+    <hyperlink ref="G441" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
+    <hyperlink ref="G466" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
+    <hyperlink ref="G464" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
+    <hyperlink ref="G469" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
+    <hyperlink ref="G475" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
+    <hyperlink ref="G479" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
+    <hyperlink ref="G492" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
+    <hyperlink ref="G497" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
+    <hyperlink ref="G522" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
     <hyperlink ref="E36" r:id="rId136" xr:uid="{809CA2D1-39E9-0045-A4DF-E4C0C2E97FA2}"/>
     <hyperlink ref="E37" r:id="rId137" xr:uid="{5DC44543-F2B9-F841-9097-6DB19C5EBD82}"/>
-    <hyperlink ref="G501" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
-    <hyperlink ref="G475" r:id="rId139" xr:uid="{7F4EA1D7-8774-1A4B-BF25-18ED0416CB20}"/>
-    <hyperlink ref="F241" r:id="rId140" xr:uid="{101513F3-87A1-DA41-8BF5-E4029309ECB8}"/>
-    <hyperlink ref="F226" r:id="rId141" xr:uid="{494E255E-6912-8643-B5CD-1D65E0DDCFFC}"/>
-    <hyperlink ref="F227" r:id="rId142" xr:uid="{828F749D-83DE-C14E-B637-56047AC1B384}"/>
-    <hyperlink ref="F242" r:id="rId143" xr:uid="{435D9B3C-98B6-5E49-BD30-EAA53523CDB7}"/>
-    <hyperlink ref="F243" r:id="rId144" xr:uid="{7D905409-0097-E04E-9593-2DEEBEEA0D0F}"/>
-    <hyperlink ref="F175" r:id="rId145" xr:uid="{64451146-E88A-9A47-9888-71BEAC8B984E}"/>
-    <hyperlink ref="F231" r:id="rId146" xr:uid="{28F6BA28-EB9B-374C-A8A0-4077C800D23A}"/>
-    <hyperlink ref="G443" r:id="rId147" xr:uid="{20B4F69E-7592-784A-8C2E-123726A51D93}"/>
-    <hyperlink ref="F234" r:id="rId148" xr:uid="{E3C3D7C6-1E6E-FF40-8CC7-6CF1C77457E4}"/>
-    <hyperlink ref="G523" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
-    <hyperlink ref="G196" r:id="rId150" xr:uid="{9BECD448-C575-B64B-BA3F-BEE8D1CBBD43}"/>
-    <hyperlink ref="G529" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
-    <hyperlink ref="G530" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
-    <hyperlink ref="G531" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
-    <hyperlink ref="G534" r:id="rId154" xr:uid="{FB93E0B8-2537-FD47-8420-84D2A706F697}"/>
-    <hyperlink ref="G535" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
-    <hyperlink ref="F209" r:id="rId156" location="2116892" xr:uid="{FF1C16E6-B146-B548-B694-396AC9D0B975}"/>
-    <hyperlink ref="G194" r:id="rId157" xr:uid="{ED09A21C-0057-1146-8BFF-213A32FC88DF}"/>
-    <hyperlink ref="G447" r:id="rId158" xr:uid="{F933A5C4-6DD5-5547-8BB3-B5D3FBA7A852}"/>
-    <hyperlink ref="G540" r:id="rId159" location=".YLoDxOvTXX8" xr:uid="{8886E3AC-3A64-6449-A070-17D95B586F83}"/>
-    <hyperlink ref="F212" r:id="rId160" xr:uid="{5140C3EB-4DFC-5A4A-9C02-C2EBFA052A41}"/>
+    <hyperlink ref="G507" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
+    <hyperlink ref="G481" r:id="rId139" xr:uid="{7F4EA1D7-8774-1A4B-BF25-18ED0416CB20}"/>
+    <hyperlink ref="F247" r:id="rId140" xr:uid="{101513F3-87A1-DA41-8BF5-E4029309ECB8}"/>
+    <hyperlink ref="F232" r:id="rId141" xr:uid="{494E255E-6912-8643-B5CD-1D65E0DDCFFC}"/>
+    <hyperlink ref="F233" r:id="rId142" xr:uid="{828F749D-83DE-C14E-B637-56047AC1B384}"/>
+    <hyperlink ref="F248" r:id="rId143" xr:uid="{435D9B3C-98B6-5E49-BD30-EAA53523CDB7}"/>
+    <hyperlink ref="F249" r:id="rId144" xr:uid="{7D905409-0097-E04E-9593-2DEEBEEA0D0F}"/>
+    <hyperlink ref="F181" r:id="rId145" xr:uid="{64451146-E88A-9A47-9888-71BEAC8B984E}"/>
+    <hyperlink ref="F237" r:id="rId146" xr:uid="{28F6BA28-EB9B-374C-A8A0-4077C800D23A}"/>
+    <hyperlink ref="G449" r:id="rId147" xr:uid="{20B4F69E-7592-784A-8C2E-123726A51D93}"/>
+    <hyperlink ref="F240" r:id="rId148" xr:uid="{E3C3D7C6-1E6E-FF40-8CC7-6CF1C77457E4}"/>
+    <hyperlink ref="G529" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
+    <hyperlink ref="G202" r:id="rId150" xr:uid="{9BECD448-C575-B64B-BA3F-BEE8D1CBBD43}"/>
+    <hyperlink ref="G535" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
+    <hyperlink ref="G536" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
+    <hyperlink ref="G537" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
+    <hyperlink ref="G540" r:id="rId154" xr:uid="{FB93E0B8-2537-FD47-8420-84D2A706F697}"/>
+    <hyperlink ref="G541" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
+    <hyperlink ref="F215" r:id="rId156" location="2116892" xr:uid="{FF1C16E6-B146-B548-B694-396AC9D0B975}"/>
+    <hyperlink ref="G200" r:id="rId157" xr:uid="{ED09A21C-0057-1146-8BFF-213A32FC88DF}"/>
+    <hyperlink ref="G453" r:id="rId158" xr:uid="{F933A5C4-6DD5-5547-8BB3-B5D3FBA7A852}"/>
+    <hyperlink ref="G546" r:id="rId159" location=".YLoDxOvTXX8" xr:uid="{8886E3AC-3A64-6449-A070-17D95B586F83}"/>
+    <hyperlink ref="F218" r:id="rId160" xr:uid="{5140C3EB-4DFC-5A4A-9C02-C2EBFA052A41}"/>
     <hyperlink ref="F29" r:id="rId161" xr:uid="{99992829-3CC1-2B43-BA73-7F09EAA955A4}"/>
-    <hyperlink ref="G478" r:id="rId162" xr:uid="{01E9516A-34A1-6D40-BED9-61916E777090}"/>
-    <hyperlink ref="H505" r:id="rId163" xr:uid="{D3C22B64-1D55-1D47-8F15-25C4AA3D5B90}"/>
-    <hyperlink ref="G507" r:id="rId164" xr:uid="{8E28D310-73EF-1C47-A666-DEE78634BFDF}"/>
-    <hyperlink ref="H504" r:id="rId165" xr:uid="{66476745-9FC4-9E4B-952E-C3E33F678E5D}"/>
-    <hyperlink ref="G543" r:id="rId166" xr:uid="{04D185B2-C246-8B4F-8813-F5A12B741A26}"/>
-    <hyperlink ref="G553" r:id="rId167" xr:uid="{D89D9875-8DF0-3044-BF56-09B8E52D068E}"/>
-    <hyperlink ref="G480" r:id="rId168" xr:uid="{951EA3E4-9D93-CC44-96EE-1FAB3FE8B169}"/>
+    <hyperlink ref="G484" r:id="rId162" xr:uid="{01E9516A-34A1-6D40-BED9-61916E777090}"/>
+    <hyperlink ref="H511" r:id="rId163" xr:uid="{D3C22B64-1D55-1D47-8F15-25C4AA3D5B90}"/>
+    <hyperlink ref="G513" r:id="rId164" xr:uid="{8E28D310-73EF-1C47-A666-DEE78634BFDF}"/>
+    <hyperlink ref="H510" r:id="rId165" xr:uid="{66476745-9FC4-9E4B-952E-C3E33F678E5D}"/>
+    <hyperlink ref="G549" r:id="rId166" xr:uid="{04D185B2-C246-8B4F-8813-F5A12B741A26}"/>
+    <hyperlink ref="G559" r:id="rId167" xr:uid="{D89D9875-8DF0-3044-BF56-09B8E52D068E}"/>
+    <hyperlink ref="G486" r:id="rId168" xr:uid="{951EA3E4-9D93-CC44-96EE-1FAB3FE8B169}"/>
     <hyperlink ref="F32" r:id="rId169" xr:uid="{A2E3FF8D-D95C-A149-813C-65DD0F6ADE93}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6587,7 +6587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
   <dimension ref="B2:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added cheatsheet websites for markdown and iterm2
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0C7C6B-3BF8-B447-966D-908567311EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCB69DA-244B-A842-8F22-C34AF8E46FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="909">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="918">
   <si>
     <t>docker</t>
   </si>
@@ -2768,6 +2768,33 @@
   </si>
   <si>
     <t>re.match('(group1)(group2)(group3)')</t>
+  </si>
+  <si>
+    <t>Markdown</t>
+  </si>
+  <si>
+    <t>Basic Syntax</t>
+  </si>
+  <si>
+    <t>https://www.markdownguide.org/basic-syntax/#lists-1</t>
+  </si>
+  <si>
+    <t>https://github.com/adam-p/markdown-here/wiki/Markdown-Cheatsheet#lines</t>
+  </si>
+  <si>
+    <t>iterm2/bash</t>
+  </si>
+  <si>
+    <t>Shortcuts to move faster in Bash command line</t>
+  </si>
+  <si>
+    <t>http://teohm.com/blog/shortcuts-to-move-faster-in-bash-command-line/</t>
+  </si>
+  <si>
+    <t>iterm2 cheatsheet</t>
+  </si>
+  <si>
+    <t>https://gist.github.com/squarism/ae3613daf5c01a98ba3a</t>
   </si>
 </sst>
 </file>
@@ -3231,7 +3258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
   <dimension ref="B1:I559"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A39" sqref="A39:XFD44"/>
     </sheetView>
@@ -7455,10 +7482,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069EEB69-0D57-C040-8545-840D5862E858}">
-  <dimension ref="B2:D23"/>
+  <dimension ref="B2:D32"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:D23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7566,6 +7593,48 @@
         <v>897</v>
       </c>
     </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>402</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>910</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>914</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>916</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>917</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{87D156EE-D133-464D-8B0D-7B076D239955}"/>
@@ -7576,6 +7645,10 @@
     <hyperlink ref="D17" r:id="rId6" xr:uid="{C1FD43E4-7E41-194B-A364-D7DEDEF40A3C}"/>
     <hyperlink ref="D20" r:id="rId7" xr:uid="{9836BE79-9331-8F4F-B63E-FD3D6FE0005D}"/>
     <hyperlink ref="D23" r:id="rId8" xr:uid="{2580CEB1-57A9-FD4B-8778-D0742AF03763}"/>
+    <hyperlink ref="D27" r:id="rId9" location="lists-1" xr:uid="{ECD9F99F-B3FE-394E-AD77-33893B9374DE}"/>
+    <hyperlink ref="D26" r:id="rId10" location="lines" xr:uid="{17AF0CCA-02DE-B342-8716-B8979D9E6FC9}"/>
+    <hyperlink ref="D31" r:id="rId11" xr:uid="{A678A0F1-CAC4-5F4E-8F54-086B5EDAC60A}"/>
+    <hyperlink ref="D32" r:id="rId12" xr:uid="{2D4A5A5D-FBA9-784D-968F-2A1AC692F8BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tip for pandas to_excel
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCB69DA-244B-A842-8F22-C34AF8E46FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE4FB3A-952D-9147-B614-A3768B5E4DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="918">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="921">
   <si>
     <t>docker</t>
   </si>
@@ -2795,6 +2795,15 @@
   </si>
   <si>
     <t>https://gist.github.com/squarism/ae3613daf5c01a98ba3a</t>
+  </si>
+  <si>
+    <t>Pandas write to excel</t>
+  </si>
+  <si>
+    <t>df1.to_excel("output.xlsx", sheet_name='Sheet_name_1')</t>
+  </si>
+  <si>
+    <t>https://pandas.pydata.org/docs/reference/api/pandas.DataFrame.to_excel.html</t>
   </si>
 </sst>
 </file>
@@ -6612,10 +6621,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G67"/>
+  <dimension ref="B2:G68"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7374,6 +7383,23 @@
       </c>
       <c r="F67" s="1" t="s">
         <v>800</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>918</v>
+      </c>
+      <c r="C68" t="s">
+        <v>467</v>
+      </c>
+      <c r="D68" t="s">
+        <v>446</v>
+      </c>
+      <c r="E68" t="s">
+        <v>919</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>920</v>
       </c>
     </row>
   </sheetData>
@@ -7442,6 +7468,7 @@
     <hyperlink ref="F67" r:id="rId62" xr:uid="{E6DDA861-2175-8242-9563-08D5A89ACF52}"/>
     <hyperlink ref="F56" r:id="rId63" xr:uid="{EDECDF4B-3198-4348-9F78-BF6E9FF8C9A6}"/>
     <hyperlink ref="F57" r:id="rId64" location="5" xr:uid="{3C28890A-3BF2-2647-AB92-79793D3ADD6E}"/>
+    <hyperlink ref="F68" r:id="rId65" xr:uid="{617D9CE6-3964-1449-9C40-052E2D590E6C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7484,7 +7511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069EEB69-0D57-C040-8545-840D5862E858}">
   <dimension ref="B2:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added tips on git
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE4FB3A-952D-9147-B614-A3768B5E4DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9D9D44-D63C-0E42-87C1-723BD612AF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="930">
   <si>
     <t>docker</t>
   </si>
@@ -2804,6 +2804,33 @@
   </si>
   <si>
     <t>https://pandas.pydata.org/docs/reference/api/pandas.DataFrame.to_excel.html</t>
+  </si>
+  <si>
+    <t>Change each 'foo' to 'bar', but ask for confirmation first.</t>
+  </si>
+  <si>
+    <t>:%s/foo/bar/gc</t>
+  </si>
+  <si>
+    <t>https://vim.fandom.com/wiki/Search_and_replace</t>
+  </si>
+  <si>
+    <t>14. check the statistics from a previous commit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Option 1: </t>
+  </si>
+  <si>
+    <t>git log -1 --stat</t>
+  </si>
+  <si>
+    <t>git show --name-only</t>
+  </si>
+  <si>
+    <t>Option 2: (better)</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/2231546/git-see-my-last-commit</t>
   </si>
 </sst>
 </file>
@@ -3267,9 +3294,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
   <dimension ref="B1:I559"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39:XFD44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F222" sqref="F222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4620,6 +4647,30 @@
         <v>812</v>
       </c>
     </row>
+    <row r="220" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C220" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="221" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D221" t="s">
+        <v>925</v>
+      </c>
+      <c r="E221" t="s">
+        <v>926</v>
+      </c>
+      <c r="F221" s="1" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="222" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D222" t="s">
+        <v>928</v>
+      </c>
+      <c r="E222" t="s">
+        <v>927</v>
+      </c>
+    </row>
     <row r="224" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B224" t="s">
         <v>168</v>
@@ -6034,7 +6085,18 @@
       </c>
     </row>
     <row r="487" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C487" t="s">
+        <v>921</v>
+      </c>
       <c r="G487" s="1"/>
+    </row>
+    <row r="488" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D488" t="s">
+        <v>922</v>
+      </c>
+      <c r="G488" s="1" t="s">
+        <v>923</v>
+      </c>
     </row>
     <row r="490" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B490" t="s">
@@ -6614,6 +6676,8 @@
     <hyperlink ref="G559" r:id="rId167" xr:uid="{D89D9875-8DF0-3044-BF56-09B8E52D068E}"/>
     <hyperlink ref="G486" r:id="rId168" xr:uid="{951EA3E4-9D93-CC44-96EE-1FAB3FE8B169}"/>
     <hyperlink ref="F32" r:id="rId169" xr:uid="{A2E3FF8D-D95C-A149-813C-65DD0F6ADE93}"/>
+    <hyperlink ref="G488" r:id="rId170" xr:uid="{8D957F13-4686-CB46-B81C-03912C517BD5}"/>
+    <hyperlink ref="F221" r:id="rId171" xr:uid="{01C94714-673D-0E4A-A2BF-59A21207E597}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6623,8 +6687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
   <dimension ref="B2:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added tips for nginx server config
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9D9D44-D63C-0E42-87C1-723BD612AF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0FEC54-97B0-8342-8B47-9756514E49B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="930">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="946">
   <si>
     <t>docker</t>
   </si>
@@ -2831,6 +2831,54 @@
   </si>
   <si>
     <t>https://stackoverflow.com/questions/2231546/git-see-my-last-commit</t>
+  </si>
+  <si>
+    <t>nginx server config</t>
+  </si>
+  <si>
+    <t>Steps for deploying new sites</t>
+  </si>
+  <si>
+    <t>1. set a subdomain by adding an A record on the host server</t>
+  </si>
+  <si>
+    <t>name: images.codyyang.info, type: A, TTL: 1h, Data: 178.62.13.248</t>
+  </si>
+  <si>
+    <t>Examples</t>
+  </si>
+  <si>
+    <t>name: www.images.codyyang.info, type: A, TTL: 1h, Data: 178.62.13.248</t>
+  </si>
+  <si>
+    <t>2. create config file under /etc/nginx/sites-available/</t>
+  </si>
+  <si>
+    <t>Note: for simplicity, it can created from existing ones</t>
+  </si>
+  <si>
+    <t>3. create soft link under /etc/nginx/sites-enabled/</t>
+  </si>
+  <si>
+    <t>sudo ln -s /etc/nginx/sites-available/myproject /etc/nginx/sites-enabled</t>
+  </si>
+  <si>
+    <t>4. test syntex correctness</t>
+  </si>
+  <si>
+    <t>sudo nginx -t</t>
+  </si>
+  <si>
+    <t>sudo systemctl reload nginx.service</t>
+  </si>
+  <si>
+    <t>5. reload nginx service</t>
+  </si>
+  <si>
+    <t>6. setup ssl security and certificates</t>
+  </si>
+  <si>
+    <t>https://docs.nginx.com/nginx/admin-guide/web-server/serving-static-content/</t>
   </si>
 </sst>
 </file>
@@ -3292,18 +3340,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I559"/>
+  <dimension ref="B1:I568"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F222" sqref="F222"/>
+      <pane ySplit="1" topLeftCell="A541" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E557" sqref="E557"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="25.1640625" customWidth="1"/>
     <col min="3" max="3" width="47.1640625" customWidth="1"/>
-    <col min="4" max="4" width="44.83203125" customWidth="1"/>
+    <col min="4" max="4" width="45.83203125" customWidth="1"/>
     <col min="5" max="5" width="38.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
   </cols>
@@ -6503,6 +6551,79 @@
       </c>
       <c r="G559" s="1" t="s">
         <v>879</v>
+      </c>
+    </row>
+    <row r="561" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B561" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="562" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C562" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="563" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D563" t="s">
+        <v>932</v>
+      </c>
+      <c r="E563" t="s">
+        <v>934</v>
+      </c>
+      <c r="F563" t="s">
+        <v>933</v>
+      </c>
+      <c r="G563" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="564" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D564" t="s">
+        <v>936</v>
+      </c>
+      <c r="E564" t="s">
+        <v>937</v>
+      </c>
+      <c r="G564" s="1" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="565" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D565" t="s">
+        <v>938</v>
+      </c>
+      <c r="E565" t="s">
+        <v>939</v>
+      </c>
+      <c r="G565" s="1" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="566" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D566" t="s">
+        <v>940</v>
+      </c>
+      <c r="E566" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="567" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D567" t="s">
+        <v>943</v>
+      </c>
+      <c r="E567" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="568" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D568" t="s">
+        <v>944</v>
+      </c>
+      <c r="E568" t="s">
+        <v>860</v>
+      </c>
+      <c r="G568" s="1" t="s">
+        <v>861</v>
       </c>
     </row>
   </sheetData>
@@ -6678,6 +6799,9 @@
     <hyperlink ref="F32" r:id="rId169" xr:uid="{A2E3FF8D-D95C-A149-813C-65DD0F6ADE93}"/>
     <hyperlink ref="G488" r:id="rId170" xr:uid="{8D957F13-4686-CB46-B81C-03912C517BD5}"/>
     <hyperlink ref="F221" r:id="rId171" xr:uid="{01C94714-673D-0E4A-A2BF-59A21207E597}"/>
+    <hyperlink ref="G564" r:id="rId172" xr:uid="{EB9D8B2D-C3FD-5F45-A2EA-DFAAED649D1E}"/>
+    <hyperlink ref="G568" r:id="rId173" xr:uid="{959A5135-36C7-954E-811F-BF84A9FC3E4F}"/>
+    <hyperlink ref="G565" r:id="rId174" xr:uid="{59635D47-1CA8-4B4D-BF2C-6399A8020C4E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6687,7 +6811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
   <dimension ref="B2:G68"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A65" workbookViewId="0">
       <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
@@ -7575,8 +7699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069EEB69-0D57-C040-8545-840D5862E858}">
   <dimension ref="B2:D32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added tips about ssh_key
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0FEC54-97B0-8342-8B47-9756514E49B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6E44DC-D213-504C-9011-CFB5F8C72666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="950">
   <si>
     <t>docker</t>
   </si>
@@ -2518,15 +2518,9 @@
     <t>to avoid typing passphrase each time you use your SSH keys</t>
   </si>
   <si>
-    <t>1. start the ssh-agent in background</t>
-  </si>
-  <si>
     <t>eval "$(ssh-agent -s)"</t>
   </si>
   <si>
-    <t>2. add your SSH private key to the ssh-agent:</t>
-  </si>
-  <si>
     <t>ssh-add ~/.ssh/id_rsa</t>
   </si>
   <si>
@@ -2737,15 +2731,9 @@
     <t>https://www.barbarianmeetscoding.com/blog/boost-your-coding-fu-with-vscode-and-vim</t>
   </si>
   <si>
-    <t xml:space="preserve">Option 1, manually </t>
-  </si>
-  <si>
     <t>Open the known_hosts file, and delete the line specified in the warning message</t>
   </si>
   <si>
-    <t>Option 2, by using ssh-keygen</t>
-  </si>
-  <si>
     <t>Fix: "WARNING: REMOTE HOST IDENTIFICATION HAS CHANGED"</t>
   </si>
   <si>
@@ -2879,6 +2867,30 @@
   </si>
   <si>
     <t>https://docs.nginx.com/nginx/admin-guide/web-server/serving-static-content/</t>
+  </si>
+  <si>
+    <t>eval $(ssh-agent)</t>
+  </si>
+  <si>
+    <t>ssh-add</t>
+  </si>
+  <si>
+    <t>option 1</t>
+  </si>
+  <si>
+    <t>option 2 (better)</t>
+  </si>
+  <si>
+    <t>1. start the ssh-agent in background (if it is not on)</t>
+  </si>
+  <si>
+    <t>2. add your SSH private key to the ssh-agent (you can try this step before step 1):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Option 1, remove existing entry manually </t>
+  </si>
+  <si>
+    <t>Option 2, remove existing entry by using ssh-keygen</t>
   </si>
 </sst>
 </file>
@@ -3343,8 +3355,8 @@
   <dimension ref="B1:I568"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A541" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E557" sqref="E557"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3352,8 +3364,9 @@
     <col min="2" max="2" width="25.1640625" customWidth="1"/>
     <col min="3" max="3" width="47.1640625" customWidth="1"/>
     <col min="4" max="4" width="45.83203125" customWidth="1"/>
-    <col min="5" max="5" width="38.6640625" customWidth="1"/>
+    <col min="5" max="5" width="45.5" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3454,12 +3467,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>30</v>
       </c>
@@ -3467,7 +3480,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
         <v>814</v>
       </c>
@@ -3475,7 +3488,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
         <v>816</v>
       </c>
@@ -3483,7 +3496,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
         <v>818</v>
       </c>
@@ -3497,89 +3510,101 @@
         <v>822</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
         <v>821</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
         <v>823</v>
       </c>
       <c r="E23" t="s">
         <v>824</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>944</v>
+      </c>
+      <c r="I23" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E24" t="s">
+        <v>946</v>
+      </c>
+      <c r="G24" t="s">
         <v>825</v>
       </c>
-      <c r="F24" t="s">
+      <c r="I24" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>947</v>
+      </c>
+      <c r="G25" t="s">
         <v>826</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E25" t="s">
+      <c r="I25" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
         <v>827</v>
       </c>
-      <c r="F25" t="s">
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
         <v>828</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>829</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D27" t="s">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
         <v>830</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E29" t="s">
         <v>831</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E28" t="s">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D29" t="s">
+      <c r="F29" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="E29" t="s">
-        <v>833</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
+        <v>948</v>
+      </c>
+      <c r="E32" t="s">
+        <v>896</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>898</v>
-      </c>
-      <c r="E32" t="s">
-        <v>899</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>902</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
+        <v>949</v>
+      </c>
+      <c r="E33" t="s">
+        <v>899</v>
+      </c>
+      <c r="F33" t="s">
         <v>900</v>
-      </c>
-      <c r="E33" t="s">
-        <v>903</v>
-      </c>
-      <c r="F33" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
@@ -3672,7 +3697,7 @@
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C56" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.2">
@@ -3774,7 +3799,7 @@
     </row>
     <row r="79" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C79" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="80" spans="3:5" x14ac:dyDescent="0.2">
@@ -3782,12 +3807,12 @@
         <v>38</v>
       </c>
       <c r="E80" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C81" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.2">
@@ -3795,12 +3820,12 @@
         <v>38</v>
       </c>
       <c r="E82" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C83" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.2">
@@ -3808,7 +3833,7 @@
         <v>38</v>
       </c>
       <c r="E84" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.2">
@@ -4697,26 +4722,26 @@
     </row>
     <row r="220" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C220" t="s">
-        <v>924</v>
+        <v>920</v>
       </c>
     </row>
     <row r="221" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D221" t="s">
+        <v>921</v>
+      </c>
+      <c r="E221" t="s">
+        <v>922</v>
+      </c>
+      <c r="F221" s="1" t="s">
         <v>925</v>
-      </c>
-      <c r="E221" t="s">
-        <v>926</v>
-      </c>
-      <c r="F221" s="1" t="s">
-        <v>929</v>
       </c>
     </row>
     <row r="222" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D222" t="s">
-        <v>928</v>
+        <v>924</v>
       </c>
       <c r="E222" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
     </row>
     <row r="224" spans="2:7" x14ac:dyDescent="0.2">
@@ -6106,44 +6131,44 @@
     </row>
     <row r="483" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C483" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="G483" s="1"/>
     </row>
     <row r="484" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D484" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="G484" s="1" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
     <row r="485" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C485" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="G485" s="1"/>
     </row>
     <row r="486" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D486" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="G486" s="1" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row r="487" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C487" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
       <c r="G487" s="1"/>
     </row>
     <row r="488" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D488" t="s">
-        <v>922</v>
+        <v>918</v>
       </c>
       <c r="G488" s="1" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
     </row>
     <row r="490" spans="2:7" x14ac:dyDescent="0.2">
@@ -6235,15 +6260,15 @@
     </row>
     <row r="506" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D506" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="E506" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
     </row>
     <row r="507" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D507" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="E507" t="s">
         <v>603</v>
@@ -6265,30 +6290,30 @@
     </row>
     <row r="510" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D510" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="E510" t="s">
+        <v>849</v>
+      </c>
+      <c r="F510" t="s">
         <v>851</v>
       </c>
-      <c r="F510" t="s">
-        <v>853</v>
-      </c>
       <c r="H510" s="1" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="511" spans="3:8" x14ac:dyDescent="0.2">
       <c r="E511" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="F511" t="s">
+        <v>841</v>
+      </c>
+      <c r="G511" t="s">
+        <v>842</v>
+      </c>
+      <c r="H511" s="1" t="s">
         <v>843</v>
-      </c>
-      <c r="G511" t="s">
-        <v>844</v>
-      </c>
-      <c r="H511" s="1" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="512" spans="3:8" x14ac:dyDescent="0.2">
@@ -6296,30 +6321,30 @@
     </row>
     <row r="513" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D513" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="E513" t="s">
+        <v>845</v>
+      </c>
+      <c r="G513" s="1" t="s">
         <v>847</v>
-      </c>
-      <c r="G513" s="1" t="s">
-        <v>849</v>
       </c>
     </row>
     <row r="514" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E514" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="G514" s="1"/>
     </row>
     <row r="515" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C515" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="G515" s="1"/>
     </row>
     <row r="516" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D516" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="E516" t="s">
         <v>574</v>
@@ -6328,7 +6353,7 @@
     </row>
     <row r="517" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D517" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="E517" t="s">
         <v>577</v>
@@ -6501,129 +6526,129 @@
     </row>
     <row r="549" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B549" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="G549" s="1" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
     </row>
     <row r="550" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C550" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="551" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D551" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="552" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C552" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
     </row>
     <row r="553" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D553" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="554" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C554" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="555" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D555" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
     </row>
     <row r="558" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B558" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="559" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C559" t="s">
+        <v>875</v>
+      </c>
+      <c r="D559" t="s">
+        <v>876</v>
+      </c>
+      <c r="G559" s="1" t="s">
         <v>877</v>
-      </c>
-      <c r="D559" t="s">
-        <v>878</v>
-      </c>
-      <c r="G559" s="1" t="s">
-        <v>879</v>
       </c>
     </row>
     <row r="561" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B561" t="s">
-        <v>930</v>
+        <v>926</v>
       </c>
     </row>
     <row r="562" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C562" t="s">
-        <v>931</v>
+        <v>927</v>
       </c>
     </row>
     <row r="563" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D563" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="E563" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
       <c r="F563" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
       <c r="G563" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
     </row>
     <row r="564" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D564" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
       <c r="E564" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="G564" s="1" t="s">
-        <v>945</v>
+        <v>941</v>
       </c>
     </row>
     <row r="565" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D565" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
       <c r="E565" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="G565" s="1" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
     </row>
     <row r="566" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D566" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
       <c r="E566" t="s">
-        <v>941</v>
+        <v>937</v>
       </c>
     </row>
     <row r="567" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D567" t="s">
-        <v>943</v>
+        <v>939</v>
       </c>
       <c r="E567" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
     </row>
     <row r="568" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D568" t="s">
-        <v>944</v>
+        <v>940</v>
       </c>
       <c r="E568" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="G568" s="1" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
     </row>
   </sheetData>
@@ -7425,30 +7450,30 @@
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="D56" t="s">
         <v>766</v>
       </c>
       <c r="E56" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>907</v>
+        <v>903</v>
       </c>
       <c r="D57" t="s">
         <v>766</v>
       </c>
       <c r="E57" t="s">
-        <v>908</v>
+        <v>904</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.2">
@@ -7575,7 +7600,7 @@
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
       <c r="C68" t="s">
         <v>467</v>
@@ -7584,10 +7609,10 @@
         <v>446</v>
       </c>
       <c r="E68" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
     </row>
   </sheetData>
@@ -7720,20 +7745,20 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>414</v>
@@ -7741,10 +7766,10 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
@@ -7758,59 +7783,59 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
@@ -7818,36 +7843,36 @@
         <v>402</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>911</v>
+        <v>907</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
-        <v>916</v>
+        <v>912</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tips for proxy server
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6E44DC-D213-504C-9011-CFB5F8C72666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C385E628-0992-9246-948C-EE02CD433896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="950">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="955">
   <si>
     <t>docker</t>
   </si>
@@ -2891,6 +2891,21 @@
   </si>
   <si>
     <t>Option 2, remove existing entry by using ssh-keygen</t>
+  </si>
+  <si>
+    <t>monitor logs in realtime</t>
+  </si>
+  <si>
+    <t>sudo tail -f /var/log/squid/access.log</t>
+  </si>
+  <si>
+    <t>option two</t>
+  </si>
+  <si>
+    <t>option one (better)</t>
+  </si>
+  <si>
+    <t>https://www.tecmint.com/watch-or-monitor-linux-log-files-in-real-time/</t>
   </si>
 </sst>
 </file>
@@ -3355,8 +3370,8 @@
   <dimension ref="B1:I568"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
+      <pane ySplit="1" topLeftCell="A305" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F330" sqref="F330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5316,7 +5331,7 @@
       </c>
       <c r="F320" s="1"/>
     </row>
-    <row r="321" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="321" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D321" t="s">
         <v>75</v>
       </c>
@@ -5324,15 +5339,15 @@
         <v>148</v>
       </c>
     </row>
-    <row r="322" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="322" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E322" s="1"/>
     </row>
-    <row r="323" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="323" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D323" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="324" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="324" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E324" t="s">
         <v>150</v>
       </c>
@@ -5340,7 +5355,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="325" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="325" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E325" t="s">
         <v>151</v>
       </c>
@@ -5351,7 +5366,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="326" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="326" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D326" t="s">
         <v>152</v>
       </c>
@@ -5359,6 +5374,30 @@
         <v>153</v>
       </c>
       <c r="G326" s="1"/>
+    </row>
+    <row r="328" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C328" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="329" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D329" t="s">
+        <v>953</v>
+      </c>
+      <c r="E329" t="s">
+        <v>951</v>
+      </c>
+      <c r="F329" s="1" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="330" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D330" t="s">
+        <v>952</v>
+      </c>
+      <c r="E330" t="s">
+        <v>951</v>
+      </c>
     </row>
     <row r="340" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E340" s="1"/>
@@ -6827,6 +6866,7 @@
     <hyperlink ref="G564" r:id="rId172" xr:uid="{EB9D8B2D-C3FD-5F45-A2EA-DFAAED649D1E}"/>
     <hyperlink ref="G568" r:id="rId173" xr:uid="{959A5135-36C7-954E-811F-BF84A9FC3E4F}"/>
     <hyperlink ref="G565" r:id="rId174" xr:uid="{59635D47-1CA8-4B4D-BF2C-6399A8020C4E}"/>
+    <hyperlink ref="F329" r:id="rId175" xr:uid="{DD2C246D-5C95-1645-B391-7EF7D3167AF4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips on webpage management
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA2DA7A-C63E-EF42-BA2D-60F03498254A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCDFB91-8CDD-3B4E-A555-0D0D67212C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="962">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="973">
   <si>
     <t>docker</t>
   </si>
@@ -2927,6 +2927,39 @@
   </si>
   <si>
     <t>https://linuxstep.wordpress.com/step-by-step-configuration-squid-to-block-streaming-media-online/</t>
+  </si>
+  <si>
+    <t>matplotlib</t>
+  </si>
+  <si>
+    <t>webpage management</t>
+  </si>
+  <si>
+    <t>download file from url</t>
+  </si>
+  <si>
+    <t>2. To save with a different name</t>
+  </si>
+  <si>
+    <t>curl -O https://www.address.com/file.png</t>
+  </si>
+  <si>
+    <t>curl -o https://www.address.com/file.png</t>
+  </si>
+  <si>
+    <t>1. To keep the original name, use</t>
+  </si>
+  <si>
+    <t>write in txt file</t>
+  </si>
+  <si>
+    <t>with open('readme.txt', 'w') as f:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    f.write('\n'.join(lines))</t>
+  </si>
+  <si>
+    <t>https://www.pythontutorial.net/python-basics/python-write-text-file/</t>
   </si>
 </sst>
 </file>
@@ -3388,11 +3421,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I575"/>
+  <dimension ref="B1:I590"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A554" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D573" sqref="D573"/>
+      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C235" sqref="C235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3401,7 +3434,7 @@
     <col min="3" max="3" width="47.1640625" customWidth="1"/>
     <col min="4" max="4" width="45.83203125" customWidth="1"/>
     <col min="5" max="5" width="45.5" customWidth="1"/>
-    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="35.5" customWidth="1"/>
     <col min="8" max="8" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4785,12 +4818,12 @@
         <v>168</v>
       </c>
     </row>
-    <row r="225" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="225" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C225" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="226" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="226" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D226" t="s">
         <v>170</v>
       </c>
@@ -4798,7 +4831,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="227" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="227" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D227" t="s">
         <v>174</v>
       </c>
@@ -4809,7 +4842,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="228" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="228" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C228" t="s">
         <v>321</v>
       </c>
@@ -4818,7 +4851,7 @@
       </c>
       <c r="F228" s="1"/>
     </row>
-    <row r="229" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="229" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C229" t="s">
         <v>404</v>
       </c>
@@ -4830,16 +4863,16 @@
       </c>
       <c r="F229" s="1"/>
     </row>
-    <row r="230" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="230" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D230" t="s">
         <v>406</v>
       </c>
       <c r="F230" s="1"/>
     </row>
-    <row r="231" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="231" spans="3:6" x14ac:dyDescent="0.2">
       <c r="F231" s="1"/>
     </row>
-    <row r="232" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="232" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C232" t="s">
         <v>615</v>
       </c>
@@ -4850,7 +4883,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="233" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="233" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C233" t="s">
         <v>619</v>
       </c>
@@ -4861,1882 +4894,1952 @@
         <v>620</v>
       </c>
     </row>
-    <row r="234" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="234" spans="3:6" x14ac:dyDescent="0.2">
       <c r="F234" s="1"/>
     </row>
-    <row r="235" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F235" s="1"/>
-    </row>
-    <row r="236" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B236" t="s">
-        <v>682</v>
+    <row r="235" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C235" t="s">
+        <v>969</v>
+      </c>
+      <c r="D235" s="2"/>
+      <c r="E235" t="s">
+        <v>970</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="236" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="E236" t="s">
+        <v>971</v>
       </c>
       <c r="F236" s="1"/>
     </row>
-    <row r="237" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C237" t="s">
-        <v>683</v>
-      </c>
-      <c r="D237" t="s">
-        <v>685</v>
-      </c>
-      <c r="F237" s="1" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="238" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C238" t="s">
-        <v>684</v>
-      </c>
-      <c r="D238" t="s">
-        <v>686</v>
-      </c>
+    <row r="237" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="F237" s="1"/>
+    </row>
+    <row r="238" spans="3:6" x14ac:dyDescent="0.2">
       <c r="F238" s="1"/>
     </row>
-    <row r="239" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C239" t="s">
-        <v>688</v>
-      </c>
-      <c r="D239" t="s">
-        <v>689</v>
-      </c>
+    <row r="239" spans="3:6" x14ac:dyDescent="0.2">
       <c r="F239" s="1"/>
     </row>
-    <row r="240" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C240" t="s">
-        <v>703</v>
-      </c>
-      <c r="D240" t="s">
-        <v>704</v>
-      </c>
-      <c r="F240" s="1" t="s">
-        <v>705</v>
-      </c>
+    <row r="240" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="F240" s="1"/>
     </row>
     <row r="241" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F241" s="1"/>
     </row>
     <row r="242" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B242" t="s">
+        <v>682</v>
+      </c>
       <c r="F242" s="1"/>
     </row>
     <row r="243" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F243" s="1"/>
+      <c r="C243" t="s">
+        <v>683</v>
+      </c>
+      <c r="D243" t="s">
+        <v>685</v>
+      </c>
+      <c r="F243" s="1" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="244" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C244" t="s">
+        <v>684</v>
+      </c>
+      <c r="D244" t="s">
+        <v>686</v>
+      </c>
       <c r="F244" s="1"/>
     </row>
+    <row r="245" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C245" t="s">
+        <v>688</v>
+      </c>
+      <c r="D245" t="s">
+        <v>689</v>
+      </c>
+      <c r="F245" s="1"/>
+    </row>
     <row r="246" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B246" t="s">
+      <c r="C246" t="s">
+        <v>703</v>
+      </c>
+      <c r="D246" t="s">
+        <v>704</v>
+      </c>
+      <c r="F246" s="1" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="247" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F247" s="1"/>
+    </row>
+    <row r="248" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F248" s="1"/>
+    </row>
+    <row r="249" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F249" s="1"/>
+    </row>
+    <row r="250" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F250" s="1"/>
+    </row>
+    <row r="252" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B252" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="247" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C247" t="s">
+    <row r="253" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C253" t="s">
         <v>613</v>
       </c>
-      <c r="D247" t="s">
+      <c r="D253" t="s">
         <v>612</v>
       </c>
-      <c r="F247" s="1" t="s">
+      <c r="F253" s="1" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="248" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C248" t="s">
+    <row r="254" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C254" t="s">
         <v>621</v>
       </c>
-      <c r="D248" t="s">
+      <c r="D254" t="s">
         <v>622</v>
       </c>
-      <c r="F248" s="1" t="s">
+      <c r="F254" s="1" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="249" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C249" t="s">
+    <row r="255" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C255" t="s">
         <v>625</v>
       </c>
-      <c r="D249" t="s">
+      <c r="D255" t="s">
         <v>624</v>
       </c>
-      <c r="F249" s="1" t="s">
+      <c r="F255" s="1" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="250" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C250" t="s">
+    <row r="256" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C256" t="s">
         <v>628</v>
       </c>
-      <c r="D250" t="s">
+      <c r="D256" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="257" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B257" t="s">
+    <row r="258" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B258" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="259" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C259" t="s">
+        <v>775</v>
+      </c>
+      <c r="D259" t="s">
+        <v>776</v>
+      </c>
+      <c r="F259" s="1" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="272" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B272" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="258" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C258" t="s">
+    <row r="273" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C273" t="s">
         <v>175</v>
       </c>
-      <c r="D258" s="1" t="s">
+      <c r="D273" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="259" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C259" t="s">
+    <row r="274" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C274" t="s">
         <v>177</v>
       </c>
-      <c r="D259" s="1" t="s">
+      <c r="D274" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="260" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C260" t="s">
+    <row r="275" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C275" t="s">
         <v>292</v>
       </c>
-      <c r="D260" s="1" t="s">
+      <c r="D275" s="1" t="s">
         <v>291</v>
-      </c>
-    </row>
-    <row r="261" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C261" t="s">
-        <v>293</v>
-      </c>
-      <c r="D261" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="262" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C262" t="s">
-        <v>296</v>
-      </c>
-      <c r="D262" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="263" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D263" s="1"/>
-    </row>
-    <row r="264" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D264" s="1"/>
-    </row>
-    <row r="265" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B265" t="s">
-        <v>342</v>
-      </c>
-      <c r="D265" s="1"/>
-    </row>
-    <row r="266" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C266" t="s">
-        <v>343</v>
-      </c>
-      <c r="D266" t="s">
-        <v>368</v>
-      </c>
-      <c r="E266" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="267" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D267" t="s">
-        <v>367</v>
-      </c>
-      <c r="E267" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="268" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D268" s="1"/>
-    </row>
-    <row r="269" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D269" s="1"/>
-    </row>
-    <row r="270" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D270" s="1"/>
-    </row>
-    <row r="274" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B274" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="275" spans="2:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="C275" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D275" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="E275" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="276" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C276" t="s">
-        <v>186</v>
-      </c>
-      <c r="E276" s="1" t="s">
-        <v>187</v>
+        <v>293</v>
+      </c>
+      <c r="D276" s="1" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="277" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C277" t="s">
-        <v>214</v>
-      </c>
-      <c r="E277" s="1" t="s">
-        <v>188</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="D277" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="278" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D278" s="1"/>
     </row>
     <row r="279" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D279" t="s">
-        <v>215</v>
-      </c>
+      <c r="D279" s="1"/>
+    </row>
+    <row r="280" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B280" t="s">
+        <v>342</v>
+      </c>
+      <c r="D280" s="1"/>
     </row>
     <row r="281" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C281" t="s">
+        <v>343</v>
+      </c>
+      <c r="D281" t="s">
+        <v>368</v>
+      </c>
+      <c r="E281" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="282" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D282" t="s">
+        <v>367</v>
+      </c>
+      <c r="E282" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="283" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D283" s="1"/>
+    </row>
+    <row r="284" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D284" s="1"/>
+    </row>
+    <row r="285" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D285" s="1"/>
+    </row>
+    <row r="289" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B289" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="290" spans="2:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="C290" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D290" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E290" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="291" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C291" t="s">
+        <v>186</v>
+      </c>
+      <c r="E291" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="292" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C292" t="s">
+        <v>214</v>
+      </c>
+      <c r="E292" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="294" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D294" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="296" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C296" t="s">
         <v>241</v>
       </c>
-      <c r="D281" t="s">
+      <c r="D296" t="s">
         <v>242</v>
       </c>
-      <c r="E281" s="1" t="s">
+      <c r="E296" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="282" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C282" t="s">
+    <row r="297" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C297" t="s">
         <v>268</v>
       </c>
-      <c r="D282" t="s">
+      <c r="D297" t="s">
         <v>269</v>
       </c>
-      <c r="E282" s="1" t="s">
+      <c r="E297" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="283" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C283" t="s">
+    <row r="298" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C298" t="s">
         <v>283</v>
       </c>
-      <c r="E283" s="1" t="s">
+      <c r="E298" s="1" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="284" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E284" s="1" t="s">
+    <row r="299" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E299" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="285" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E285" s="1" t="s">
+    <row r="300" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E300" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="286" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C286" t="s">
+    <row r="301" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C301" t="s">
         <v>287</v>
       </c>
-      <c r="E286" s="1" t="s">
+      <c r="E301" s="1" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="287" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C287" t="s">
+    <row r="302" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C302" t="s">
         <v>298</v>
       </c>
-      <c r="E287" s="1" t="s">
+      <c r="E302" s="1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="288" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E288" s="1"/>
-    </row>
-    <row r="289" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C289" t="s">
+    <row r="303" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E303" s="1"/>
+    </row>
+    <row r="304" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C304" t="s">
         <v>358</v>
       </c>
-      <c r="D289" t="s">
+      <c r="D304" t="s">
         <v>359</v>
       </c>
-      <c r="E289" s="1" t="s">
+      <c r="E304" s="1" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="290" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E290" s="1"/>
-    </row>
-    <row r="291" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E291" s="1"/>
-    </row>
-    <row r="292" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E292" s="1"/>
-    </row>
-    <row r="293" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E293" s="1"/>
-    </row>
-    <row r="294" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E294" s="1"/>
-    </row>
-    <row r="295" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E295" s="1"/>
-    </row>
-    <row r="296" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E296" s="1"/>
-    </row>
-    <row r="297" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E297" s="1"/>
-    </row>
-    <row r="298" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C298" t="s">
+    <row r="305" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E305" s="1"/>
+    </row>
+    <row r="306" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E306" s="1"/>
+    </row>
+    <row r="307" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E307" s="1"/>
+    </row>
+    <row r="308" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E308" s="1"/>
+    </row>
+    <row r="309" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E309" s="1"/>
+    </row>
+    <row r="310" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E310" s="1"/>
+    </row>
+    <row r="311" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E311" s="1"/>
+    </row>
+    <row r="312" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E312" s="1"/>
+    </row>
+    <row r="313" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C313" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="299" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D299" t="s">
+    <row r="314" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D314" t="s">
         <v>134</v>
       </c>
-      <c r="E299" t="s">
+      <c r="E314" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="300" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D300" t="s">
+    <row r="315" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D315" t="s">
         <v>135</v>
       </c>
-      <c r="E300" t="s">
+      <c r="E315" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="301" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D301" t="s">
+    <row r="316" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D316" t="s">
         <v>139</v>
       </c>
-      <c r="E301" t="s">
+      <c r="E316" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="302" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D302" t="s">
+    <row r="317" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D317" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="303" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D303" t="s">
+    <row r="318" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D318" t="s">
         <v>141</v>
       </c>
-      <c r="E303" t="s">
+      <c r="E318" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="304" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D304" t="s">
+    <row r="319" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D319" t="s">
         <v>482</v>
       </c>
-      <c r="E304" t="s">
+      <c r="E319" t="s">
         <v>484</v>
       </c>
-      <c r="F304" t="s">
+      <c r="F319" t="s">
         <v>488</v>
       </c>
-      <c r="G304" t="s">
+      <c r="G319" t="s">
         <v>483</v>
       </c>
-      <c r="H304" s="1" t="s">
+      <c r="H319" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="305" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D305" t="s">
+    <row r="320" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D320" t="s">
         <v>485</v>
       </c>
-      <c r="E305" t="s">
+      <c r="E320" t="s">
         <v>486</v>
       </c>
-      <c r="G305" t="s">
+      <c r="G320" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="307" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C307" t="s">
+    <row r="322" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C322" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="308" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D308" t="s">
+    <row r="323" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D323" t="s">
         <v>72</v>
       </c>
-      <c r="E308" t="s">
+      <c r="E323" t="s">
         <v>73</v>
       </c>
-      <c r="F308" s="1" t="s">
+      <c r="F323" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="309" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D309" t="s">
+    <row r="324" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D324" t="s">
         <v>75</v>
       </c>
-      <c r="E309" s="1" t="s">
+      <c r="E324" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="310" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D310" t="s">
+    <row r="325" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D325" t="s">
         <v>77</v>
       </c>
-      <c r="E310" s="1" t="s">
+      <c r="E325" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="311" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D311" t="s">
+    <row r="326" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D326" t="s">
         <v>80</v>
       </c>
-      <c r="E311" s="1" t="s">
+      <c r="E326" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="312" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D312" t="s">
+    <row r="327" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D327" t="s">
         <v>361</v>
       </c>
-      <c r="E312" t="s">
+      <c r="E327" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="313" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D313" t="s">
+    <row r="328" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D328" t="s">
         <v>362</v>
       </c>
-      <c r="E313" t="s">
+      <c r="E328" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="315" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D315" t="s">
+    <row r="330" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D330" t="s">
         <v>81</v>
       </c>
-      <c r="E315" t="s">
+      <c r="E330" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="316" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D316" t="s">
+    <row r="331" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D331" t="s">
         <v>83</v>
       </c>
-      <c r="E316" t="s">
+      <c r="E331" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="318" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C318" t="s">
+    <row r="333" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C333" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="319" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D319" t="s">
+    <row r="334" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D334" t="s">
         <v>72</v>
       </c>
-      <c r="E319" t="s">
+      <c r="E334" t="s">
         <v>130</v>
       </c>
-      <c r="F319" s="1"/>
-    </row>
-    <row r="320" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D320" t="s">
+      <c r="F334" s="1"/>
+    </row>
+    <row r="335" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D335" t="s">
         <v>146</v>
       </c>
-      <c r="E320" s="1" t="s">
+      <c r="E335" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F320" s="1"/>
-    </row>
-    <row r="321" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D321" t="s">
+      <c r="F335" s="1"/>
+    </row>
+    <row r="336" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D336" t="s">
         <v>75</v>
       </c>
-      <c r="E321" s="1" t="s">
+      <c r="E336" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="322" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E322" s="1"/>
-    </row>
-    <row r="323" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D323" t="s">
+    <row r="337" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E337" s="1"/>
+    </row>
+    <row r="338" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D338" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="324" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E324" t="s">
+    <row r="339" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E339" t="s">
         <v>150</v>
       </c>
-      <c r="F324" t="s">
+      <c r="F339" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="325" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E325" t="s">
+    <row r="340" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E340" t="s">
         <v>151</v>
       </c>
-      <c r="F325" t="s">
+      <c r="F340" t="s">
         <v>144</v>
       </c>
-      <c r="G325" s="1" t="s">
+      <c r="G340" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="326" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D326" t="s">
+    <row r="341" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D341" t="s">
         <v>152</v>
       </c>
-      <c r="E326" s="1" t="s">
+      <c r="E341" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G326" s="1"/>
-    </row>
-    <row r="328" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C328" t="s">
+      <c r="G341" s="1"/>
+    </row>
+    <row r="343" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C343" t="s">
         <v>950</v>
       </c>
     </row>
-    <row r="329" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D329" t="s">
+    <row r="344" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D344" t="s">
         <v>953</v>
       </c>
-      <c r="E329" t="s">
+      <c r="E344" t="s">
         <v>951</v>
       </c>
-      <c r="F329" s="1" t="s">
+      <c r="F344" s="1" t="s">
         <v>954</v>
       </c>
     </row>
-    <row r="330" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D330" t="s">
+    <row r="345" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D345" t="s">
         <v>952</v>
       </c>
-      <c r="E330" t="s">
+      <c r="E345" t="s">
         <v>951</v>
       </c>
     </row>
-    <row r="340" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E340" s="1"/>
-    </row>
-    <row r="342" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B342" t="s">
+    <row r="347" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C347" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="348" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D348" t="s">
+        <v>964</v>
+      </c>
+      <c r="E348" t="s">
+        <v>968</v>
+      </c>
+      <c r="F348" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="349" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E349" t="s">
+        <v>965</v>
+      </c>
+      <c r="F349" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="355" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E355" s="1"/>
+    </row>
+    <row r="357" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B357" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="343" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C343" t="s">
+    <row r="358" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C358" t="s">
         <v>276</v>
       </c>
-      <c r="D343" t="s">
+      <c r="D358" t="s">
         <v>278</v>
       </c>
-      <c r="E343" s="1" t="s">
+      <c r="E358" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="344" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C344" t="s">
+    <row r="359" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C359" t="s">
         <v>280</v>
       </c>
-      <c r="E344" s="1" t="s">
+      <c r="E359" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="F344" s="1" t="s">
+      <c r="F359" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="G344" s="1" t="s">
+      <c r="G359" s="1" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="345" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C345" t="s">
+    <row r="360" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C360" t="s">
         <v>289</v>
       </c>
-      <c r="E345" s="1" t="s">
+      <c r="E360" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="346" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C346" t="s">
+    <row r="361" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C361" t="s">
         <v>303</v>
       </c>
-      <c r="E346" s="1" t="s">
+      <c r="E361" s="1" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="347" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D347" t="s">
+    <row r="362" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D362" t="s">
         <v>305</v>
       </c>
-      <c r="E347" s="1" t="s">
+      <c r="E362" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="348" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C348" t="s">
+    <row r="363" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C363" t="s">
         <v>323</v>
       </c>
-      <c r="E348" s="1" t="s">
+      <c r="E363" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="349" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C349" t="s">
+    <row r="364" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C364" t="s">
         <v>307</v>
       </c>
-      <c r="D349" t="s">
+      <c r="D364" t="s">
         <v>308</v>
       </c>
-      <c r="E349" s="1" t="s">
+      <c r="E364" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="350" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C350" t="s">
+    <row r="365" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C365" t="s">
         <v>310</v>
       </c>
-      <c r="E350" s="1" t="s">
+      <c r="E365" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="351" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C351" t="s">
+    <row r="366" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C366" t="s">
         <v>315</v>
       </c>
-      <c r="E351" s="1" t="s">
+      <c r="E366" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="352" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C352" t="s">
+    <row r="367" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C367" t="s">
         <v>316</v>
       </c>
-      <c r="E352" s="1" t="s">
+      <c r="E367" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="353" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C353" t="s">
+    <row r="368" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C368" t="s">
         <v>318</v>
       </c>
-      <c r="E353" s="1" t="s">
+      <c r="E368" s="1" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="354" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C354" t="s">
+    <row r="369" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C369" t="s">
         <v>325</v>
       </c>
-      <c r="D354" t="s">
+      <c r="D369" t="s">
         <v>332</v>
       </c>
-      <c r="E354" s="1" t="s">
+      <c r="E369" s="1" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="355" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D355" t="s">
+    <row r="370" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D370" t="s">
         <v>327</v>
       </c>
-      <c r="E355" s="1" t="s">
+      <c r="E370" s="1" t="s">
         <v>326</v>
-      </c>
-    </row>
-    <row r="357" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C357" t="s">
-        <v>329</v>
-      </c>
-      <c r="D357" t="s">
-        <v>330</v>
-      </c>
-      <c r="E357" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="359" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C359" t="s">
-        <v>335</v>
-      </c>
-      <c r="D359" t="s">
-        <v>337</v>
-      </c>
-      <c r="E359" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="363" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B363" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="364" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C364" t="s">
-        <v>341</v>
-      </c>
-      <c r="D364" t="s">
-        <v>339</v>
-      </c>
-      <c r="E364" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="370" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B370" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="371" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C371" t="s">
-        <v>86</v>
-      </c>
-      <c r="D371" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="372" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C372" t="s">
-        <v>88</v>
+        <v>329</v>
       </c>
       <c r="D372" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="373" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C373" t="s">
-        <v>95</v>
-      </c>
-      <c r="D373" s="1" t="s">
-        <v>96</v>
+        <v>330</v>
+      </c>
+      <c r="E372" s="1" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="374" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C374" t="s">
+        <v>335</v>
+      </c>
+      <c r="D374" t="s">
+        <v>337</v>
+      </c>
+      <c r="E374" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="378" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B378" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="379" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C379" t="s">
+        <v>341</v>
+      </c>
+      <c r="D379" t="s">
+        <v>339</v>
+      </c>
+      <c r="E379" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="385" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B385" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="386" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C386" t="s">
+        <v>86</v>
+      </c>
+      <c r="D386" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="387" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C387" t="s">
+        <v>88</v>
+      </c>
+      <c r="D387" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="388" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C388" t="s">
+        <v>95</v>
+      </c>
+      <c r="D388" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="389" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C389" t="s">
         <v>97</v>
       </c>
-      <c r="D374" s="1" t="s">
+      <c r="D389" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="376" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B376" t="s">
+    <row r="391" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B391" t="s">
         <v>90</v>
       </c>
-      <c r="C376" t="s">
+      <c r="C391" t="s">
         <v>91</v>
       </c>
-      <c r="D376" t="s">
+      <c r="D391" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="377" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C377" t="s">
+    <row r="392" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C392" t="s">
         <v>93</v>
       </c>
-      <c r="D377" t="s">
+      <c r="D392" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="380" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B380" t="s">
+    <row r="395" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B395" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="381" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C381" t="s">
+    <row r="396" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C396" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="382" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D382" t="s">
+    <row r="397" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D397" t="s">
         <v>104</v>
       </c>
-      <c r="E382" s="1" t="s">
+      <c r="E397" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="383" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D383" t="s">
+    <row r="398" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D398" t="s">
         <v>101</v>
       </c>
-      <c r="E383" s="1" t="s">
+      <c r="E398" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="384" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D384" t="s">
+    <row r="399" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D399" t="s">
         <v>102</v>
       </c>
-      <c r="E384" s="1" t="s">
+      <c r="E399" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="385" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D385" t="s">
+    <row r="400" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D400" t="s">
         <v>107</v>
       </c>
-      <c r="E385" t="s">
+      <c r="E400" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="387" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B387" t="s">
+    <row r="402" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B402" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="388" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C388" t="s">
+    <row r="403" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C403" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="389" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D389" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="390" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D390" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="391" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F391" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="392" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B392" t="s">
-        <v>1</v>
-      </c>
-      <c r="F392" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="393" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C393" t="s">
-        <v>112</v>
-      </c>
-      <c r="D393" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="394" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D394" t="s">
-        <v>126</v>
-      </c>
-      <c r="E394" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="395" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C395" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="396" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D396" t="s">
-        <v>115</v>
-      </c>
-      <c r="E396" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F396" t="s">
-        <v>128</v>
-      </c>
-      <c r="G396" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="397" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E397" t="s">
-        <v>121</v>
-      </c>
-      <c r="G397" s="1"/>
-    </row>
-    <row r="398" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E398" t="s">
-        <v>124</v>
-      </c>
-      <c r="G398" s="1"/>
-    </row>
-    <row r="399" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D399" t="s">
-        <v>117</v>
-      </c>
-      <c r="E399" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G399" s="1"/>
-    </row>
-    <row r="400" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D400" t="s">
-        <v>119</v>
-      </c>
-      <c r="E400" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G400" s="1"/>
-    </row>
-    <row r="401" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E401" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="G401" s="1"/>
-    </row>
-    <row r="402" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E402" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="403" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D403" t="s">
-        <v>301</v>
-      </c>
-      <c r="E403" s="1" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="404" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D404" t="s">
-        <v>300</v>
-      </c>
-      <c r="E404" s="1" t="s">
-        <v>299</v>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="405" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D405" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="406" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F406" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="407" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B407" t="s">
+        <v>1</v>
+      </c>
+      <c r="F407" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="408" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C408" t="s">
+        <v>112</v>
+      </c>
+      <c r="D408" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="409" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C409" t="s">
-        <v>131</v>
-      </c>
-      <c r="D409" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="D409" t="s">
+        <v>126</v>
+      </c>
+      <c r="E409" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="410" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C410" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="411" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D411" t="s">
+        <v>115</v>
+      </c>
+      <c r="E411" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F411" t="s">
+        <v>128</v>
+      </c>
+      <c r="G411" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="412" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E412" t="s">
+        <v>121</v>
+      </c>
+      <c r="G412" s="1"/>
     </row>
     <row r="413" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B413" t="s">
-        <v>481</v>
-      </c>
+      <c r="E413" t="s">
+        <v>124</v>
+      </c>
+      <c r="G413" s="1"/>
     </row>
     <row r="414" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C414" t="s">
-        <v>490</v>
-      </c>
+      <c r="D414" t="s">
+        <v>117</v>
+      </c>
+      <c r="E414" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G414" s="1"/>
     </row>
     <row r="415" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D415" t="s">
+        <v>119</v>
+      </c>
+      <c r="E415" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G415" s="1"/>
+    </row>
+    <row r="416" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E416" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="G416" s="1"/>
+    </row>
+    <row r="417" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E417" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="418" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D418" t="s">
+        <v>301</v>
+      </c>
+      <c r="E418" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="419" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D419" t="s">
+        <v>300</v>
+      </c>
+      <c r="E419" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="424" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C424" t="s">
+        <v>131</v>
+      </c>
+      <c r="D424" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="428" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B428" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="429" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C429" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="430" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D430" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="416" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E416" t="s">
+    <row r="431" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E431" t="s">
         <v>492</v>
       </c>
-      <c r="F416" s="1" t="s">
+      <c r="F431" s="1" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="417" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E417" t="s">
+    <row r="432" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E432" t="s">
         <v>494</v>
       </c>
-      <c r="F417" s="1" t="s">
+      <c r="F432" s="1" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="418" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E418" t="s">
+    <row r="433" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E433" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="419" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D419" t="s">
+    <row r="434" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D434" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="420" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E420" t="s">
+    <row r="435" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E435" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="421" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E421" t="s">
+    <row r="436" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E436" t="s">
         <v>495</v>
-      </c>
-    </row>
-    <row r="422" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D422" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="423" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E423" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="424" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C424" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="425" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D425" t="s">
-        <v>503</v>
-      </c>
-      <c r="E425" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="426" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D426" t="s">
-        <v>501</v>
-      </c>
-      <c r="E426" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="428" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C428" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="429" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D429" t="s">
-        <v>508</v>
-      </c>
-      <c r="E429" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="430" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D430" t="s">
-        <v>509</v>
-      </c>
-      <c r="E430" t="s">
-        <v>507</v>
-      </c>
-      <c r="G430" s="1" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="432" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C432" t="s">
-        <v>512</v>
-      </c>
-      <c r="G432" s="1" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="434" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C434" t="s">
-        <v>513</v>
-      </c>
-      <c r="E434" t="s">
-        <v>514</v>
-      </c>
-      <c r="G434" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="436" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C436" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="437" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D437" t="s">
-        <v>518</v>
-      </c>
-      <c r="E437" t="s">
-        <v>517</v>
-      </c>
-      <c r="G437" s="1" t="s">
-        <v>521</v>
+        <v>498</v>
       </c>
     </row>
     <row r="438" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D438" t="s">
-        <v>519</v>
-      </c>
       <c r="E438" t="s">
-        <v>520</v>
+        <v>499</v>
+      </c>
+    </row>
+    <row r="439" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C439" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="440" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C440" t="s">
-        <v>522</v>
+      <c r="D440" t="s">
+        <v>503</v>
+      </c>
+      <c r="E440" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="441" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D441" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="E441" t="s">
-        <v>524</v>
-      </c>
-      <c r="G441" s="1" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="442" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D442" t="s">
-        <v>526</v>
-      </c>
-      <c r="E442" t="s">
-        <v>523</v>
+        <v>502</v>
       </c>
     </row>
     <row r="443" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D443" t="s">
-        <v>527</v>
-      </c>
-      <c r="E443" t="s">
-        <v>525</v>
+      <c r="C443" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="444" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C444" t="s">
-        <v>629</v>
+      <c r="D444" t="s">
+        <v>508</v>
+      </c>
+      <c r="E444" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="445" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D445" t="s">
+        <v>509</v>
+      </c>
+      <c r="E445" t="s">
+        <v>507</v>
+      </c>
+      <c r="G445" s="1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="447" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C447" t="s">
+        <v>512</v>
+      </c>
+      <c r="G447" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="449" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C449" t="s">
+        <v>513</v>
+      </c>
+      <c r="E449" t="s">
+        <v>514</v>
+      </c>
+      <c r="G449" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="451" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C451" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="452" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D452" t="s">
+        <v>518</v>
+      </c>
+      <c r="E452" t="s">
+        <v>517</v>
+      </c>
+      <c r="G452" s="1" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="453" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D453" t="s">
+        <v>519</v>
+      </c>
+      <c r="E453" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="455" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C455" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="456" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D456" t="s">
+        <v>528</v>
+      </c>
+      <c r="E456" t="s">
+        <v>524</v>
+      </c>
+      <c r="G456" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="457" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D457" t="s">
+        <v>526</v>
+      </c>
+      <c r="E457" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="458" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D458" t="s">
+        <v>527</v>
+      </c>
+      <c r="E458" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="459" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C459" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="460" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D460" t="s">
         <v>630</v>
       </c>
-      <c r="E445" t="s">
+      <c r="E460" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="446" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D446" t="s">
+    <row r="461" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D461" t="s">
         <v>632</v>
       </c>
-      <c r="E446" t="s">
+      <c r="E461" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="447" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D447" t="s">
+    <row r="462" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D462" t="s">
         <v>634</v>
       </c>
-      <c r="E447" t="s">
+      <c r="E462" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="448" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D448" t="s">
+    <row r="463" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D463" t="s">
         <v>637</v>
       </c>
-      <c r="E448" t="s">
+      <c r="E463" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="449" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D449" t="s">
+    <row r="464" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D464" t="s">
         <v>693</v>
       </c>
-      <c r="E449" t="s">
+      <c r="E464" t="s">
         <v>695</v>
       </c>
-      <c r="G449" s="1" t="s">
+      <c r="G464" s="1" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="452" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B452" t="s">
+    <row r="467" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B467" t="s">
         <v>778</v>
       </c>
     </row>
-    <row r="453" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C453" t="s">
+    <row r="468" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C468" t="s">
         <v>779</v>
       </c>
-      <c r="G453" s="1" t="s">
+      <c r="G468" s="1" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="462" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B462" t="s">
+    <row r="477" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B477" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="463" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C463" t="s">
+    <row r="478" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C478" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="464" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D464" t="s">
+    <row r="479" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D479" t="s">
         <v>541</v>
       </c>
-      <c r="G464" s="1" t="s">
+      <c r="G479" s="1" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="465" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C465" t="s">
+    <row r="480" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C480" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="466" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D466" t="s">
+    <row r="481" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D481" t="s">
         <v>543</v>
       </c>
-      <c r="E466" t="s">
+      <c r="E481" t="s">
         <v>544</v>
       </c>
-      <c r="G466" s="1" t="s">
+      <c r="G481" s="1" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="468" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C468" t="s">
+    <row r="483" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C483" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="469" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D469" t="s">
+    <row r="484" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D484" t="s">
         <v>548</v>
       </c>
-      <c r="E469" t="s">
+      <c r="E484" t="s">
         <v>549</v>
       </c>
-      <c r="G469" s="1" t="s">
+      <c r="G484" s="1" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="470" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D470" t="s">
+    <row r="485" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D485" t="s">
         <v>550</v>
       </c>
-      <c r="E470" t="s">
+      <c r="E485" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="471" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D471" t="s">
+    <row r="486" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D486" t="s">
         <v>552</v>
       </c>
-      <c r="E471" t="s">
+      <c r="E486" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="472" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D472" t="s">
+    <row r="487" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D487" t="s">
         <v>554</v>
       </c>
-      <c r="E472" t="s">
+      <c r="E487" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="474" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C474" t="s">
+    <row r="489" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C489" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="475" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D475" t="s">
+    <row r="490" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D490" t="s">
         <v>558</v>
       </c>
-      <c r="E475" t="s">
+      <c r="E490" t="s">
         <v>560</v>
       </c>
-      <c r="G475" s="1" t="s">
+      <c r="G490" s="1" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="476" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D476" t="s">
+    <row r="491" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D491" t="s">
         <v>559</v>
       </c>
-      <c r="E476" t="s">
+      <c r="E491" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="478" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C478" t="s">
+    <row r="493" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C493" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="479" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D479" t="s">
+    <row r="494" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D494" t="s">
         <v>565</v>
       </c>
-      <c r="G479" s="1" t="s">
+      <c r="G494" s="1" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="480" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C480" t="s">
+    <row r="495" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C495" t="s">
         <v>608</v>
       </c>
-      <c r="G480" s="1"/>
-    </row>
-    <row r="481" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D481" t="s">
+      <c r="G495" s="1"/>
+    </row>
+    <row r="496" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D496" t="s">
         <v>609</v>
       </c>
-      <c r="E481" t="s">
+      <c r="E496" t="s">
         <v>610</v>
       </c>
-      <c r="G481" s="1" t="s">
+      <c r="G496" s="1" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="482" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G482" s="1"/>
-    </row>
-    <row r="483" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C483" t="s">
+    <row r="497" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G497" s="1"/>
+    </row>
+    <row r="498" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C498" t="s">
         <v>834</v>
       </c>
-      <c r="G483" s="1"/>
-    </row>
-    <row r="484" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D484" t="s">
+      <c r="G498" s="1"/>
+    </row>
+    <row r="499" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D499" t="s">
         <v>835</v>
       </c>
-      <c r="G484" s="1" t="s">
+      <c r="G499" s="1" t="s">
         <v>836</v>
       </c>
     </row>
-    <row r="485" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C485" t="s">
+    <row r="500" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C500" t="s">
         <v>890</v>
       </c>
-      <c r="G485" s="1"/>
-    </row>
-    <row r="486" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D486" t="s">
+      <c r="G500" s="1"/>
+    </row>
+    <row r="501" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D501" t="s">
         <v>891</v>
       </c>
-      <c r="G486" s="1" t="s">
+      <c r="G501" s="1" t="s">
         <v>892</v>
       </c>
     </row>
-    <row r="487" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C487" t="s">
+    <row r="502" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C502" t="s">
         <v>917</v>
       </c>
-      <c r="G487" s="1"/>
-    </row>
-    <row r="488" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D488" t="s">
+      <c r="G502" s="1"/>
+    </row>
+    <row r="503" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D503" t="s">
         <v>918</v>
       </c>
-      <c r="G488" s="1" t="s">
+      <c r="G503" s="1" t="s">
         <v>919</v>
       </c>
     </row>
-    <row r="490" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B490" t="s">
+    <row r="505" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B505" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="491" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C491" t="s">
+    <row r="506" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C506" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="492" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E492" t="s">
+    <row r="507" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E507" t="s">
         <v>568</v>
       </c>
-      <c r="G492" s="1" t="s">
+      <c r="G507" s="1" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="495" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B495" t="s">
+    <row r="510" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B510" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="496" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C496" t="s">
+    <row r="511" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C511" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="497" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D497" t="s">
+    <row r="512" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D512" t="s">
         <v>572</v>
       </c>
-      <c r="E497" t="s">
+      <c r="E512" t="s">
         <v>573</v>
       </c>
-      <c r="F497" t="s">
+      <c r="F512" t="s">
         <v>574</v>
       </c>
-      <c r="G497" s="1" t="s">
+      <c r="G512" s="1" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="498" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E498" t="s">
+    <row r="513" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E513" t="s">
         <v>576</v>
       </c>
-      <c r="F498" t="s">
+      <c r="F513" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="499" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C499" t="s">
+    <row r="514" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C514" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="500" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D500" t="s">
+    <row r="515" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D515" t="s">
         <v>595</v>
       </c>
-      <c r="E500" t="s">
+      <c r="E515" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="501" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D501" t="s">
+    <row r="516" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D516" t="s">
         <v>598</v>
       </c>
-      <c r="E501" t="s">
+      <c r="E516" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="503" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D503" t="s">
+    <row r="518" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D518" t="s">
         <v>599</v>
       </c>
-      <c r="E503" t="s">
+      <c r="E518" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="504" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D504" t="s">
+    <row r="519" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D519" t="s">
         <v>601</v>
       </c>
-      <c r="E504" t="s">
+      <c r="E519" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="506" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D506" t="s">
+    <row r="521" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D521" t="s">
         <v>838</v>
       </c>
-      <c r="E506" t="s">
+      <c r="E521" t="s">
         <v>837</v>
       </c>
     </row>
-    <row r="507" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D507" t="s">
+    <row r="522" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D522" t="s">
         <v>839</v>
       </c>
-      <c r="E507" t="s">
+      <c r="E522" t="s">
         <v>603</v>
       </c>
-      <c r="G507" s="1" t="s">
+      <c r="G522" s="1" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="508" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D508" t="s">
+    <row r="523" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D523" t="s">
         <v>604</v>
       </c>
-      <c r="E508" t="s">
+      <c r="E523" t="s">
         <v>605</v>
       </c>
-      <c r="F508" t="s">
+      <c r="F523" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="510" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D510" t="s">
+    <row r="525" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D525" t="s">
         <v>840</v>
       </c>
-      <c r="E510" t="s">
+      <c r="E525" t="s">
         <v>849</v>
       </c>
-      <c r="F510" t="s">
+      <c r="F525" t="s">
         <v>851</v>
       </c>
-      <c r="H510" s="1" t="s">
+      <c r="H525" s="1" t="s">
         <v>850</v>
       </c>
     </row>
-    <row r="511" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E511" t="s">
+    <row r="526" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E526" t="s">
         <v>848</v>
       </c>
-      <c r="F511" t="s">
+      <c r="F526" t="s">
         <v>841</v>
       </c>
-      <c r="G511" t="s">
+      <c r="G526" t="s">
         <v>842</v>
       </c>
-      <c r="H511" s="1" t="s">
+      <c r="H526" s="1" t="s">
         <v>843</v>
       </c>
     </row>
-    <row r="512" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="G512" s="1"/>
-    </row>
-    <row r="513" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D513" t="s">
+    <row r="527" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="G527" s="1"/>
+    </row>
+    <row r="528" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D528" t="s">
         <v>844</v>
       </c>
-      <c r="E513" t="s">
+      <c r="E528" t="s">
         <v>845</v>
       </c>
-      <c r="G513" s="1" t="s">
+      <c r="G528" s="1" t="s">
         <v>847</v>
       </c>
     </row>
-    <row r="514" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E514" t="s">
+    <row r="529" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E529" t="s">
         <v>846</v>
       </c>
-      <c r="G514" s="1"/>
-    </row>
-    <row r="515" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C515" t="s">
-        <v>860</v>
-      </c>
-      <c r="G515" s="1"/>
-    </row>
-    <row r="516" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D516" t="s">
-        <v>861</v>
-      </c>
-      <c r="E516" t="s">
-        <v>574</v>
-      </c>
-      <c r="G516" s="1"/>
-    </row>
-    <row r="517" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D517" t="s">
-        <v>862</v>
-      </c>
-      <c r="E517" t="s">
-        <v>577</v>
-      </c>
-      <c r="G517" s="1"/>
-    </row>
-    <row r="518" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G518" s="1"/>
-    </row>
-    <row r="520" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B520" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="521" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C521" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="522" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D522" t="s">
-        <v>581</v>
-      </c>
-      <c r="E522" t="s">
-        <v>582</v>
-      </c>
-      <c r="F522" t="s">
-        <v>580</v>
-      </c>
-      <c r="G522" s="1" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="523" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E523" t="s">
-        <v>583</v>
-      </c>
-      <c r="F523" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="525" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D525" t="s">
-        <v>586</v>
-      </c>
-      <c r="E525" t="s">
-        <v>588</v>
-      </c>
-      <c r="F525" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="528" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B528" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="529" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C529" t="s">
-        <v>707</v>
-      </c>
-      <c r="D529" t="s">
-        <v>710</v>
-      </c>
-      <c r="G529" s="1" t="s">
-        <v>713</v>
-      </c>
+      <c r="G529" s="1"/>
     </row>
     <row r="530" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C530" t="s">
-        <v>708</v>
-      </c>
-      <c r="D530" t="s">
-        <v>711</v>
-      </c>
+        <v>860</v>
+      </c>
+      <c r="G530" s="1"/>
     </row>
     <row r="531" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C531" t="s">
-        <v>709</v>
-      </c>
       <c r="D531" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="534" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B534" t="s">
-        <v>730</v>
-      </c>
+        <v>861</v>
+      </c>
+      <c r="E531" t="s">
+        <v>574</v>
+      </c>
+      <c r="G531" s="1"/>
+    </row>
+    <row r="532" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D532" t="s">
+        <v>862</v>
+      </c>
+      <c r="E532" t="s">
+        <v>577</v>
+      </c>
+      <c r="G532" s="1"/>
+    </row>
+    <row r="533" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G533" s="1"/>
     </row>
     <row r="535" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C535" t="s">
-        <v>731</v>
-      </c>
-      <c r="G535" s="1" t="s">
-        <v>732</v>
+      <c r="B535" t="s">
+        <v>578</v>
       </c>
     </row>
     <row r="536" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C536" t="s">
-        <v>733</v>
-      </c>
-      <c r="G536" s="1" t="s">
-        <v>734</v>
+        <v>579</v>
       </c>
     </row>
     <row r="537" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C537" t="s">
-        <v>737</v>
+      <c r="D537" t="s">
+        <v>581</v>
+      </c>
+      <c r="E537" t="s">
+        <v>582</v>
       </c>
       <c r="F537" t="s">
-        <v>735</v>
+        <v>580</v>
       </c>
       <c r="G537" s="1" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="539" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B539" t="s">
-        <v>742</v>
+        <v>585</v>
+      </c>
+    </row>
+    <row r="538" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E538" t="s">
+        <v>583</v>
+      </c>
+      <c r="F538" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="540" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C540" t="s">
-        <v>743</v>
-      </c>
       <c r="D540" t="s">
-        <v>744</v>
-      </c>
-      <c r="G540" s="1" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="541" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C541" t="s">
-        <v>746</v>
-      </c>
-      <c r="D541" t="s">
-        <v>747</v>
-      </c>
-      <c r="G541" s="1" t="s">
-        <v>748</v>
+        <v>586</v>
+      </c>
+      <c r="E540" t="s">
+        <v>588</v>
+      </c>
+      <c r="F540" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="543" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B543" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="544" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C544" t="s">
+        <v>707</v>
+      </c>
+      <c r="D544" t="s">
+        <v>710</v>
+      </c>
+      <c r="G544" s="1" t="s">
+        <v>713</v>
       </c>
     </row>
     <row r="545" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B545" t="s">
-        <v>801</v>
+      <c r="C545" t="s">
+        <v>708</v>
+      </c>
+      <c r="D545" t="s">
+        <v>711</v>
       </c>
     </row>
     <row r="546" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C546" t="s">
-        <v>802</v>
+        <v>709</v>
       </c>
       <c r="D546" t="s">
-        <v>803</v>
-      </c>
-      <c r="E546" t="s">
-        <v>804</v>
-      </c>
-      <c r="G546" s="1" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="547" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C547" t="s">
-        <v>806</v>
-      </c>
-      <c r="E547" t="s">
-        <v>807</v>
+        <v>712</v>
       </c>
     </row>
     <row r="549" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B549" t="s">
-        <v>852</v>
-      </c>
-      <c r="G549" s="1" t="s">
-        <v>859</v>
+        <v>730</v>
       </c>
     </row>
     <row r="550" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C550" t="s">
-        <v>853</v>
+        <v>731</v>
+      </c>
+      <c r="G550" s="1" t="s">
+        <v>732</v>
       </c>
     </row>
     <row r="551" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D551" t="s">
-        <v>856</v>
+      <c r="C551" t="s">
+        <v>733</v>
+      </c>
+      <c r="G551" s="1" t="s">
+        <v>734</v>
       </c>
     </row>
     <row r="552" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C552" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="553" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D553" t="s">
-        <v>857</v>
+        <v>737</v>
+      </c>
+      <c r="F552" t="s">
+        <v>735</v>
+      </c>
+      <c r="G552" s="1" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="554" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C554" t="s">
-        <v>855</v>
+      <c r="B554" t="s">
+        <v>742</v>
       </c>
     </row>
     <row r="555" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C555" t="s">
+        <v>743</v>
+      </c>
       <c r="D555" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="558" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B558" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="559" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C559" t="s">
-        <v>875</v>
-      </c>
-      <c r="D559" t="s">
-        <v>876</v>
-      </c>
-      <c r="G559" s="1" t="s">
-        <v>877</v>
+        <v>744</v>
+      </c>
+      <c r="G555" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="556" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C556" t="s">
+        <v>746</v>
+      </c>
+      <c r="D556" t="s">
+        <v>747</v>
+      </c>
+      <c r="G556" s="1" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="560" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B560" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="561" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B561" t="s">
-        <v>926</v>
+      <c r="C561" t="s">
+        <v>802</v>
+      </c>
+      <c r="D561" t="s">
+        <v>803</v>
+      </c>
+      <c r="E561" t="s">
+        <v>804</v>
+      </c>
+      <c r="G561" s="1" t="s">
+        <v>805</v>
       </c>
     </row>
     <row r="562" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C562" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="563" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D563" t="s">
-        <v>928</v>
-      </c>
-      <c r="E563" t="s">
-        <v>930</v>
-      </c>
-      <c r="F563" t="s">
-        <v>929</v>
-      </c>
-      <c r="G563" t="s">
-        <v>931</v>
+        <v>806</v>
+      </c>
+      <c r="E562" t="s">
+        <v>807</v>
       </c>
     </row>
     <row r="564" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D564" t="s">
-        <v>932</v>
-      </c>
-      <c r="E564" t="s">
-        <v>933</v>
+      <c r="B564" t="s">
+        <v>852</v>
       </c>
       <c r="G564" s="1" t="s">
-        <v>941</v>
+        <v>859</v>
       </c>
     </row>
     <row r="565" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D565" t="s">
-        <v>934</v>
-      </c>
-      <c r="E565" t="s">
-        <v>935</v>
-      </c>
-      <c r="G565" s="1" t="s">
-        <v>859</v>
+      <c r="C565" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="566" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D566" t="s">
-        <v>936</v>
-      </c>
-      <c r="E566" t="s">
-        <v>937</v>
+        <v>856</v>
       </c>
     </row>
     <row r="567" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D567" t="s">
-        <v>939</v>
-      </c>
-      <c r="E567" t="s">
-        <v>938</v>
+      <c r="C567" t="s">
+        <v>854</v>
       </c>
     </row>
     <row r="568" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D568" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="569" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C569" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="570" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D570" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="573" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B573" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="574" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C574" t="s">
+        <v>875</v>
+      </c>
+      <c r="D574" t="s">
+        <v>876</v>
+      </c>
+      <c r="G574" s="1" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="576" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B576" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="577" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C577" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="578" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D578" t="s">
+        <v>928</v>
+      </c>
+      <c r="E578" t="s">
+        <v>930</v>
+      </c>
+      <c r="F578" t="s">
+        <v>929</v>
+      </c>
+      <c r="G578" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="579" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D579" t="s">
+        <v>932</v>
+      </c>
+      <c r="E579" t="s">
+        <v>933</v>
+      </c>
+      <c r="G579" s="1" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="580" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D580" t="s">
+        <v>934</v>
+      </c>
+      <c r="E580" t="s">
+        <v>935</v>
+      </c>
+      <c r="G580" s="1" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="581" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D581" t="s">
+        <v>936</v>
+      </c>
+      <c r="E581" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="582" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D582" t="s">
+        <v>939</v>
+      </c>
+      <c r="E582" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="583" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D583" t="s">
         <v>940</v>
       </c>
-      <c r="E568" t="s">
+      <c r="E583" t="s">
         <v>858</v>
       </c>
-      <c r="G568" s="1" t="s">
+      <c r="G583" s="1" t="s">
         <v>859</v>
       </c>
     </row>
-    <row r="572" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B572" t="s">
+    <row r="587" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B587" t="s">
         <v>955</v>
       </c>
     </row>
-    <row r="573" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C573" t="s">
+    <row r="588" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C588" t="s">
         <v>956</v>
       </c>
     </row>
-    <row r="574" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D574" t="s">
+    <row r="589" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D589" t="s">
         <v>957</v>
       </c>
-      <c r="G574" s="1" t="s">
+      <c r="G589" s="1" t="s">
         <v>958</v>
       </c>
     </row>
-    <row r="575" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C575" t="s">
+    <row r="590" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C590" t="s">
         <v>959</v>
       </c>
-      <c r="D575" t="s">
+      <c r="D590" t="s">
         <v>960</v>
       </c>
-      <c r="G575" s="1" t="s">
+      <c r="G590" s="1" t="s">
         <v>961</v>
       </c>
     </row>
@@ -6758,12 +6861,12 @@
     <hyperlink ref="F130" r:id="rId14" xr:uid="{93472772-CF6C-D045-B634-2D574A3EE034}"/>
     <hyperlink ref="E226" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
     <hyperlink ref="F227" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
-    <hyperlink ref="D258" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
-    <hyperlink ref="D259" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
+    <hyperlink ref="D273" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
+    <hyperlink ref="D274" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
     <hyperlink ref="F131" r:id="rId19" xr:uid="{92BE3560-5393-C545-9D2D-2B773359B28F}"/>
-    <hyperlink ref="E275" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
-    <hyperlink ref="E276" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
-    <hyperlink ref="E277" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
+    <hyperlink ref="E290" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
+    <hyperlink ref="E291" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
+    <hyperlink ref="E292" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
     <hyperlink ref="E105" r:id="rId23" xr:uid="{1526D7DA-27DA-1443-928C-BEDA9E425734}"/>
     <hyperlink ref="E106" r:id="rId24" xr:uid="{4F363062-BE49-AB4F-8956-2C1F31D9B898}"/>
     <hyperlink ref="H132" r:id="rId25" xr:uid="{D9E13355-D59B-054F-B544-34A5A285A9E0}"/>
@@ -6780,7 +6883,7 @@
     <hyperlink ref="I132" r:id="rId36" xr:uid="{A03C56E4-1156-A148-A568-F50A5C33DB5C}"/>
     <hyperlink ref="F141" r:id="rId37" xr:uid="{12AC219C-4678-4E43-B328-6595FA10B8D3}"/>
     <hyperlink ref="E143" r:id="rId38" xr:uid="{44409621-28A2-704A-B283-3DCE1EFB1603}"/>
-    <hyperlink ref="E281" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
+    <hyperlink ref="E296" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
     <hyperlink ref="F144" r:id="rId40" xr:uid="{A9D0D792-87D1-8144-872F-5CA060D3C28F}"/>
     <hyperlink ref="F145" r:id="rId41" xr:uid="{87EF989D-17E9-1E45-A075-CD862D0B60F4}"/>
     <hyperlink ref="F147" r:id="rId42" xr:uid="{8406C6F0-DC69-A64D-AAD8-60A33C12D00B}"/>
@@ -6790,68 +6893,68 @@
     <hyperlink ref="F152" r:id="rId46" xr:uid="{3D1C62DB-D9B7-BE42-B21D-4EEBC4C9EFE1}"/>
     <hyperlink ref="F153" r:id="rId47" xr:uid="{F5021A21-70A2-D34E-B055-64CAC326E7EF}"/>
     <hyperlink ref="F154" r:id="rId48" xr:uid="{A8C010A1-8EE1-264B-8688-3BEA1B62E535}"/>
-    <hyperlink ref="E282" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
+    <hyperlink ref="E297" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
     <hyperlink ref="F149" r:id="rId50" location="113521" xr:uid="{EE1413C5-3B38-7D4D-8DF1-634A12F0BD81}"/>
     <hyperlink ref="E107" r:id="rId51" xr:uid="{00B1EF4A-7791-0343-8D8C-9A1E83248FC9}"/>
-    <hyperlink ref="E343" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
-    <hyperlink ref="E344" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
+    <hyperlink ref="E358" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
+    <hyperlink ref="E359" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
     <hyperlink ref="F156" r:id="rId54" xr:uid="{40A4B6A0-2F7E-A84D-8CC6-D814A33F5953}"/>
-    <hyperlink ref="E283" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
-    <hyperlink ref="E284" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
-    <hyperlink ref="E285" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
-    <hyperlink ref="E286" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
-    <hyperlink ref="E345" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
-    <hyperlink ref="D260" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
-    <hyperlink ref="D261" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
-    <hyperlink ref="D262" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
-    <hyperlink ref="E287" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
-    <hyperlink ref="E346" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
-    <hyperlink ref="E347" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
-    <hyperlink ref="E349" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
-    <hyperlink ref="E350" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
-    <hyperlink ref="F344" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
-    <hyperlink ref="G344" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
-    <hyperlink ref="E351" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
-    <hyperlink ref="E352" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
-    <hyperlink ref="E353" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
+    <hyperlink ref="E298" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
+    <hyperlink ref="E299" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
+    <hyperlink ref="E300" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
+    <hyperlink ref="E301" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
+    <hyperlink ref="E360" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
+    <hyperlink ref="D275" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
+    <hyperlink ref="D276" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
+    <hyperlink ref="D277" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
+    <hyperlink ref="E302" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
+    <hyperlink ref="E361" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
+    <hyperlink ref="E362" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
+    <hyperlink ref="E364" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
+    <hyperlink ref="E365" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
+    <hyperlink ref="F359" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
+    <hyperlink ref="G359" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
+    <hyperlink ref="E366" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
+    <hyperlink ref="E367" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
+    <hyperlink ref="E368" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
     <hyperlink ref="E228" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
-    <hyperlink ref="E348" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
-    <hyperlink ref="E354" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
-    <hyperlink ref="E355" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
+    <hyperlink ref="E363" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
+    <hyperlink ref="E369" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
+    <hyperlink ref="E370" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
     <hyperlink ref="E109" r:id="rId77" location="code" xr:uid="{C0475FF8-517D-E949-887E-9A42D86E9640}"/>
-    <hyperlink ref="E357" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
+    <hyperlink ref="E372" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
     <hyperlink ref="E110" r:id="rId79" xr:uid="{277DBE6F-F3E5-8B4C-8DD8-BD92445D1A99}"/>
-    <hyperlink ref="E359" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
-    <hyperlink ref="E364" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
-    <hyperlink ref="E266" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
-    <hyperlink ref="E267" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
+    <hyperlink ref="E374" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
+    <hyperlink ref="E379" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
+    <hyperlink ref="E281" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
+    <hyperlink ref="E282" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
     <hyperlink ref="F177" r:id="rId84" xr:uid="{EB604865-A16B-0646-A5B5-0D047467449D}"/>
-    <hyperlink ref="E289" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
-    <hyperlink ref="D373" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
-    <hyperlink ref="D374" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
-    <hyperlink ref="E383" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
-    <hyperlink ref="E384" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
-    <hyperlink ref="E382" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
-    <hyperlink ref="D393" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
-    <hyperlink ref="E399" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
-    <hyperlink ref="E396" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
-    <hyperlink ref="E400" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
-    <hyperlink ref="F391" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
-    <hyperlink ref="F392" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
-    <hyperlink ref="E394" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
-    <hyperlink ref="G396" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
-    <hyperlink ref="D409" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
-    <hyperlink ref="E401" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
-    <hyperlink ref="E404" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
-    <hyperlink ref="E403" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
-    <hyperlink ref="F308" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
-    <hyperlink ref="E309" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
-    <hyperlink ref="E310" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
-    <hyperlink ref="E311" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
-    <hyperlink ref="G325" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
-    <hyperlink ref="E320" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
-    <hyperlink ref="E321" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
-    <hyperlink ref="E326" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
+    <hyperlink ref="E304" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
+    <hyperlink ref="D388" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
+    <hyperlink ref="D389" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
+    <hyperlink ref="E398" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
+    <hyperlink ref="E399" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
+    <hyperlink ref="E397" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
+    <hyperlink ref="D408" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
+    <hyperlink ref="E414" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
+    <hyperlink ref="E411" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
+    <hyperlink ref="E415" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
+    <hyperlink ref="F406" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
+    <hyperlink ref="F407" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
+    <hyperlink ref="E409" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
+    <hyperlink ref="G411" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
+    <hyperlink ref="D424" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
+    <hyperlink ref="E416" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
+    <hyperlink ref="E419" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
+    <hyperlink ref="E418" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
+    <hyperlink ref="F323" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
+    <hyperlink ref="E324" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
+    <hyperlink ref="E325" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
+    <hyperlink ref="E326" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
+    <hyperlink ref="G340" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
+    <hyperlink ref="E335" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
+    <hyperlink ref="E336" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
+    <hyperlink ref="E341" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
     <hyperlink ref="F189" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
     <hyperlink ref="F194" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
     <hyperlink ref="F195" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
@@ -6861,64 +6964,66 @@
     <hyperlink ref="F209" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
     <hyperlink ref="F203" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
     <hyperlink ref="F212" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
-    <hyperlink ref="H304" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
-    <hyperlink ref="F416" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
-    <hyperlink ref="G430" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
-    <hyperlink ref="F417" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
-    <hyperlink ref="G432" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
-    <hyperlink ref="G434" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
-    <hyperlink ref="G437" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
-    <hyperlink ref="G441" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
-    <hyperlink ref="G466" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
-    <hyperlink ref="G464" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
-    <hyperlink ref="G469" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
-    <hyperlink ref="G475" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
-    <hyperlink ref="G479" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
-    <hyperlink ref="G492" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
-    <hyperlink ref="G497" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
-    <hyperlink ref="G522" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
+    <hyperlink ref="H319" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
+    <hyperlink ref="F431" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
+    <hyperlink ref="G445" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
+    <hyperlink ref="F432" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
+    <hyperlink ref="G447" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
+    <hyperlink ref="G449" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
+    <hyperlink ref="G452" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
+    <hyperlink ref="G456" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
+    <hyperlink ref="G481" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
+    <hyperlink ref="G479" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
+    <hyperlink ref="G484" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
+    <hyperlink ref="G490" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
+    <hyperlink ref="G494" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
+    <hyperlink ref="G507" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
+    <hyperlink ref="G512" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
+    <hyperlink ref="G537" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
     <hyperlink ref="E36" r:id="rId136" xr:uid="{809CA2D1-39E9-0045-A4DF-E4C0C2E97FA2}"/>
     <hyperlink ref="E37" r:id="rId137" xr:uid="{5DC44543-F2B9-F841-9097-6DB19C5EBD82}"/>
-    <hyperlink ref="G507" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
-    <hyperlink ref="G481" r:id="rId139" xr:uid="{7F4EA1D7-8774-1A4B-BF25-18ED0416CB20}"/>
-    <hyperlink ref="F247" r:id="rId140" xr:uid="{101513F3-87A1-DA41-8BF5-E4029309ECB8}"/>
+    <hyperlink ref="G522" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
+    <hyperlink ref="G496" r:id="rId139" xr:uid="{7F4EA1D7-8774-1A4B-BF25-18ED0416CB20}"/>
+    <hyperlink ref="F253" r:id="rId140" xr:uid="{101513F3-87A1-DA41-8BF5-E4029309ECB8}"/>
     <hyperlink ref="F232" r:id="rId141" xr:uid="{494E255E-6912-8643-B5CD-1D65E0DDCFFC}"/>
     <hyperlink ref="F233" r:id="rId142" xr:uid="{828F749D-83DE-C14E-B637-56047AC1B384}"/>
-    <hyperlink ref="F248" r:id="rId143" xr:uid="{435D9B3C-98B6-5E49-BD30-EAA53523CDB7}"/>
-    <hyperlink ref="F249" r:id="rId144" xr:uid="{7D905409-0097-E04E-9593-2DEEBEEA0D0F}"/>
+    <hyperlink ref="F254" r:id="rId143" xr:uid="{435D9B3C-98B6-5E49-BD30-EAA53523CDB7}"/>
+    <hyperlink ref="F255" r:id="rId144" xr:uid="{7D905409-0097-E04E-9593-2DEEBEEA0D0F}"/>
     <hyperlink ref="F181" r:id="rId145" xr:uid="{64451146-E88A-9A47-9888-71BEAC8B984E}"/>
-    <hyperlink ref="F237" r:id="rId146" xr:uid="{28F6BA28-EB9B-374C-A8A0-4077C800D23A}"/>
-    <hyperlink ref="G449" r:id="rId147" xr:uid="{20B4F69E-7592-784A-8C2E-123726A51D93}"/>
-    <hyperlink ref="F240" r:id="rId148" xr:uid="{E3C3D7C6-1E6E-FF40-8CC7-6CF1C77457E4}"/>
-    <hyperlink ref="G529" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
+    <hyperlink ref="F243" r:id="rId146" xr:uid="{28F6BA28-EB9B-374C-A8A0-4077C800D23A}"/>
+    <hyperlink ref="G464" r:id="rId147" xr:uid="{20B4F69E-7592-784A-8C2E-123726A51D93}"/>
+    <hyperlink ref="F246" r:id="rId148" xr:uid="{E3C3D7C6-1E6E-FF40-8CC7-6CF1C77457E4}"/>
+    <hyperlink ref="G544" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
     <hyperlink ref="G202" r:id="rId150" xr:uid="{9BECD448-C575-B64B-BA3F-BEE8D1CBBD43}"/>
-    <hyperlink ref="G535" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
-    <hyperlink ref="G536" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
-    <hyperlink ref="G537" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
-    <hyperlink ref="G540" r:id="rId154" xr:uid="{FB93E0B8-2537-FD47-8420-84D2A706F697}"/>
-    <hyperlink ref="G541" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
+    <hyperlink ref="G550" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
+    <hyperlink ref="G551" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
+    <hyperlink ref="G552" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
+    <hyperlink ref="G555" r:id="rId154" xr:uid="{FB93E0B8-2537-FD47-8420-84D2A706F697}"/>
+    <hyperlink ref="G556" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
     <hyperlink ref="F215" r:id="rId156" location="2116892" xr:uid="{FF1C16E6-B146-B548-B694-396AC9D0B975}"/>
     <hyperlink ref="G200" r:id="rId157" xr:uid="{ED09A21C-0057-1146-8BFF-213A32FC88DF}"/>
-    <hyperlink ref="G453" r:id="rId158" xr:uid="{F933A5C4-6DD5-5547-8BB3-B5D3FBA7A852}"/>
-    <hyperlink ref="G546" r:id="rId159" location=".YLoDxOvTXX8" xr:uid="{8886E3AC-3A64-6449-A070-17D95B586F83}"/>
+    <hyperlink ref="G468" r:id="rId158" xr:uid="{F933A5C4-6DD5-5547-8BB3-B5D3FBA7A852}"/>
+    <hyperlink ref="G561" r:id="rId159" location=".YLoDxOvTXX8" xr:uid="{8886E3AC-3A64-6449-A070-17D95B586F83}"/>
     <hyperlink ref="F218" r:id="rId160" xr:uid="{5140C3EB-4DFC-5A4A-9C02-C2EBFA052A41}"/>
     <hyperlink ref="F29" r:id="rId161" xr:uid="{99992829-3CC1-2B43-BA73-7F09EAA955A4}"/>
-    <hyperlink ref="G484" r:id="rId162" xr:uid="{01E9516A-34A1-6D40-BED9-61916E777090}"/>
-    <hyperlink ref="H511" r:id="rId163" xr:uid="{D3C22B64-1D55-1D47-8F15-25C4AA3D5B90}"/>
-    <hyperlink ref="G513" r:id="rId164" xr:uid="{8E28D310-73EF-1C47-A666-DEE78634BFDF}"/>
-    <hyperlink ref="H510" r:id="rId165" xr:uid="{66476745-9FC4-9E4B-952E-C3E33F678E5D}"/>
-    <hyperlink ref="G549" r:id="rId166" xr:uid="{04D185B2-C246-8B4F-8813-F5A12B741A26}"/>
-    <hyperlink ref="G559" r:id="rId167" xr:uid="{D89D9875-8DF0-3044-BF56-09B8E52D068E}"/>
-    <hyperlink ref="G486" r:id="rId168" xr:uid="{951EA3E4-9D93-CC44-96EE-1FAB3FE8B169}"/>
+    <hyperlink ref="G499" r:id="rId162" xr:uid="{01E9516A-34A1-6D40-BED9-61916E777090}"/>
+    <hyperlink ref="H526" r:id="rId163" xr:uid="{D3C22B64-1D55-1D47-8F15-25C4AA3D5B90}"/>
+    <hyperlink ref="G528" r:id="rId164" xr:uid="{8E28D310-73EF-1C47-A666-DEE78634BFDF}"/>
+    <hyperlink ref="H525" r:id="rId165" xr:uid="{66476745-9FC4-9E4B-952E-C3E33F678E5D}"/>
+    <hyperlink ref="G564" r:id="rId166" xr:uid="{04D185B2-C246-8B4F-8813-F5A12B741A26}"/>
+    <hyperlink ref="G574" r:id="rId167" xr:uid="{D89D9875-8DF0-3044-BF56-09B8E52D068E}"/>
+    <hyperlink ref="G501" r:id="rId168" xr:uid="{951EA3E4-9D93-CC44-96EE-1FAB3FE8B169}"/>
     <hyperlink ref="F32" r:id="rId169" xr:uid="{A2E3FF8D-D95C-A149-813C-65DD0F6ADE93}"/>
-    <hyperlink ref="G488" r:id="rId170" xr:uid="{8D957F13-4686-CB46-B81C-03912C517BD5}"/>
+    <hyperlink ref="G503" r:id="rId170" xr:uid="{8D957F13-4686-CB46-B81C-03912C517BD5}"/>
     <hyperlink ref="F221" r:id="rId171" xr:uid="{01C94714-673D-0E4A-A2BF-59A21207E597}"/>
-    <hyperlink ref="G564" r:id="rId172" xr:uid="{EB9D8B2D-C3FD-5F45-A2EA-DFAAED649D1E}"/>
-    <hyperlink ref="G568" r:id="rId173" xr:uid="{959A5135-36C7-954E-811F-BF84A9FC3E4F}"/>
-    <hyperlink ref="G565" r:id="rId174" xr:uid="{59635D47-1CA8-4B4D-BF2C-6399A8020C4E}"/>
-    <hyperlink ref="F329" r:id="rId175" xr:uid="{DD2C246D-5C95-1645-B391-7EF7D3167AF4}"/>
-    <hyperlink ref="G574" r:id="rId176" xr:uid="{DDFFFCAD-BF74-1D48-AF86-5B31F6DB75DD}"/>
-    <hyperlink ref="G575" r:id="rId177" xr:uid="{6BFF710C-507C-844E-AFBE-9B133475C781}"/>
+    <hyperlink ref="G579" r:id="rId172" xr:uid="{EB9D8B2D-C3FD-5F45-A2EA-DFAAED649D1E}"/>
+    <hyperlink ref="G583" r:id="rId173" xr:uid="{959A5135-36C7-954E-811F-BF84A9FC3E4F}"/>
+    <hyperlink ref="G580" r:id="rId174" xr:uid="{59635D47-1CA8-4B4D-BF2C-6399A8020C4E}"/>
+    <hyperlink ref="F344" r:id="rId175" xr:uid="{DD2C246D-5C95-1645-B391-7EF7D3167AF4}"/>
+    <hyperlink ref="G589" r:id="rId176" xr:uid="{DDFFFCAD-BF74-1D48-AF86-5B31F6DB75DD}"/>
+    <hyperlink ref="G590" r:id="rId177" xr:uid="{6BFF710C-507C-844E-AFBE-9B133475C781}"/>
+    <hyperlink ref="F259" r:id="rId178" xr:uid="{C710D804-CFB3-2F46-9AAE-375A3EC37F04}"/>
+    <hyperlink ref="F235" r:id="rId179" xr:uid="{05F4B29A-A0A0-5444-B283-0B6193A59DB2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6926,10 +7031,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G68"/>
+  <dimension ref="B2:G67"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7603,107 +7708,93 @@
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>775</v>
-      </c>
-      <c r="C61" t="s">
-        <v>467</v>
+        <v>783</v>
       </c>
       <c r="E61" t="s">
-        <v>776</v>
+        <v>781</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>777</v>
+        <v>782</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>783</v>
+        <v>786</v>
+      </c>
+      <c r="D62" t="s">
+        <v>785</v>
       </c>
       <c r="E62" t="s">
-        <v>781</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>786</v>
-      </c>
-      <c r="D63" t="s">
-        <v>785</v>
+        <v>787</v>
+      </c>
+      <c r="C63" t="s">
+        <v>789</v>
       </c>
       <c r="E63" t="s">
-        <v>784</v>
+        <v>790</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>788</v>
       </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>787</v>
+        <v>791</v>
       </c>
       <c r="C64" t="s">
-        <v>789</v>
+        <v>794</v>
       </c>
       <c r="E64" t="s">
-        <v>790</v>
+        <v>793</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>791</v>
-      </c>
-      <c r="C65" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="E65" t="s">
-        <v>793</v>
+        <v>797</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>792</v>
+        <v>796</v>
       </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>795</v>
+        <v>798</v>
+      </c>
+      <c r="C66" t="s">
+        <v>648</v>
       </c>
       <c r="E66" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>796</v>
+        <v>800</v>
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>798</v>
+        <v>914</v>
       </c>
       <c r="C67" t="s">
-        <v>648</v>
+        <v>467</v>
+      </c>
+      <c r="D67" t="s">
+        <v>446</v>
       </c>
       <c r="E67" t="s">
-        <v>799</v>
+        <v>915</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
-        <v>914</v>
-      </c>
-      <c r="C68" t="s">
-        <v>467</v>
-      </c>
-      <c r="D68" t="s">
-        <v>446</v>
-      </c>
-      <c r="E68" t="s">
-        <v>915</v>
-      </c>
-      <c r="F68" s="1" t="s">
         <v>916</v>
       </c>
     </row>
@@ -7765,15 +7856,14 @@
     <hyperlink ref="F58" r:id="rId54" xr:uid="{634A44CB-CBAB-AE4D-898A-98A6804C37BE}"/>
     <hyperlink ref="F59" r:id="rId55" xr:uid="{CBA3AB68-A9B5-7E45-AAF4-E420DC08CECB}"/>
     <hyperlink ref="F60" r:id="rId56" xr:uid="{6513D8D1-CA9F-DB4F-8EE3-BB85344F470E}"/>
-    <hyperlink ref="F61" r:id="rId57" xr:uid="{F0C558B0-9D09-2E47-9A73-03B1EBC298EA}"/>
-    <hyperlink ref="F62" r:id="rId58" xr:uid="{0E6940AA-CCE2-A845-B000-88634DEE5413}"/>
-    <hyperlink ref="F64" r:id="rId59" xr:uid="{DB6C6106-7A38-1843-B3AC-F9FB615E4977}"/>
-    <hyperlink ref="F65" r:id="rId60" xr:uid="{8AED1472-61F4-E646-89E7-A2D566BEF7A0}"/>
-    <hyperlink ref="F66" r:id="rId61" xr:uid="{D5875307-B681-3841-BE35-59A92CDCD038}"/>
-    <hyperlink ref="F67" r:id="rId62" xr:uid="{E6DDA861-2175-8242-9563-08D5A89ACF52}"/>
-    <hyperlink ref="F56" r:id="rId63" xr:uid="{EDECDF4B-3198-4348-9F78-BF6E9FF8C9A6}"/>
-    <hyperlink ref="F57" r:id="rId64" location="5" xr:uid="{3C28890A-3BF2-2647-AB92-79793D3ADD6E}"/>
-    <hyperlink ref="F68" r:id="rId65" xr:uid="{617D9CE6-3964-1449-9C40-052E2D590E6C}"/>
+    <hyperlink ref="F61" r:id="rId57" xr:uid="{0E6940AA-CCE2-A845-B000-88634DEE5413}"/>
+    <hyperlink ref="F63" r:id="rId58" xr:uid="{DB6C6106-7A38-1843-B3AC-F9FB615E4977}"/>
+    <hyperlink ref="F64" r:id="rId59" xr:uid="{8AED1472-61F4-E646-89E7-A2D566BEF7A0}"/>
+    <hyperlink ref="F65" r:id="rId60" xr:uid="{D5875307-B681-3841-BE35-59A92CDCD038}"/>
+    <hyperlink ref="F66" r:id="rId61" xr:uid="{E6DDA861-2175-8242-9563-08D5A89ACF52}"/>
+    <hyperlink ref="F56" r:id="rId62" xr:uid="{EDECDF4B-3198-4348-9F78-BF6E9FF8C9A6}"/>
+    <hyperlink ref="F57" r:id="rId63" location="5" xr:uid="{3C28890A-3BF2-2647-AB92-79793D3ADD6E}"/>
+    <hyperlink ref="F67" r:id="rId64" xr:uid="{617D9CE6-3964-1449-9C40-052E2D590E6C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added link for installing dnsmasq on macos
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED472D5A-9E76-7A46-99F7-D712898B3C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29C130F-C215-E346-A228-AD5825597998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Tips" sheetId="5" r:id="rId3"/>
     <sheet name="Websites" sheetId="6" r:id="rId4"/>
     <sheet name="Suggested by Others" sheetId="7" r:id="rId5"/>
+    <sheet name="added from macbook pro 13" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="984">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="986">
   <si>
     <t>docker</t>
   </si>
@@ -2994,6 +2995,12 @@
   </si>
   <si>
     <t>Business Movers</t>
+  </si>
+  <si>
+    <t>https://passingcuriosity.com/2013/dnsmasq-dev-osx/</t>
+  </si>
+  <si>
+    <t>Using Dnsmasq for local development on OS X</t>
   </si>
 </sst>
 </file>
@@ -8114,7 +8121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9928DD2B-0E52-0541-9E14-AF63C29120ED}">
   <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -8184,4 +8191,27 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C477A64-6885-F242-8D4E-EC1D72EF7EB5}">
+  <dimension ref="B2:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>985</v>
+      </c>
+      <c r="D2" t="s">
+        <v>984</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added tips for installing dnsmasq
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29C130F-C215-E346-A228-AD5825597998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AB2567-B3B4-8345-A20C-96A5BB91C314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Tips" sheetId="5" r:id="rId3"/>
     <sheet name="Websites" sheetId="6" r:id="rId4"/>
     <sheet name="Suggested by Others" sheetId="7" r:id="rId5"/>
-    <sheet name="added from macbook pro 13" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="986">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="990">
   <si>
     <t>docker</t>
   </si>
@@ -2997,10 +2996,22 @@
     <t>Business Movers</t>
   </si>
   <si>
+    <t>jupyter notebook</t>
+  </si>
+  <si>
+    <t>install extensions</t>
+  </si>
+  <si>
+    <t>pip install jupyter_contrib_nbextensions &amp;&amp; jupyter contrib nbextension install</t>
+  </si>
+  <si>
+    <t>https://towardsdatascience.com/jupyter-notebook-extensions-517fa69d2231</t>
+  </si>
+  <si>
+    <t>Using Dnsmasq for local development on OS X</t>
+  </si>
+  <si>
     <t>https://passingcuriosity.com/2013/dnsmasq-dev-osx/</t>
-  </si>
-  <si>
-    <t>Using Dnsmasq for local development on OS X</t>
   </si>
 </sst>
 </file>
@@ -3462,11 +3473,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I590"/>
+  <dimension ref="B1:I595"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C243" sqref="C243:D246"/>
+      <pane ySplit="1" topLeftCell="A579" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G468" sqref="G468"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6882,6 +6893,24 @@
       </c>
       <c r="G590" s="1" t="s">
         <v>961</v>
+      </c>
+    </row>
+    <row r="593" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B593" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="594" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C594" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="595" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D595" t="s">
+        <v>986</v>
+      </c>
+      <c r="G595" s="1" t="s">
+        <v>987</v>
       </c>
     </row>
   </sheetData>
@@ -7065,6 +7094,7 @@
     <hyperlink ref="G590" r:id="rId177" xr:uid="{6BFF710C-507C-844E-AFBE-9B133475C781}"/>
     <hyperlink ref="F259" r:id="rId178" xr:uid="{C710D804-CFB3-2F46-9AAE-375A3EC37F04}"/>
     <hyperlink ref="F235" r:id="rId179" xr:uid="{05F4B29A-A0A0-5444-B283-0B6193A59DB2}"/>
+    <hyperlink ref="G595" r:id="rId180" xr:uid="{1504BD14-5428-4E4B-A4D1-F56A3711952B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7072,10 +7102,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G67"/>
+  <dimension ref="B2:G68"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="B38" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7837,6 +7867,14 @@
       </c>
       <c r="F67" s="1" t="s">
         <v>916</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>988</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>989</v>
       </c>
     </row>
   </sheetData>
@@ -7905,6 +7943,7 @@
     <hyperlink ref="F56" r:id="rId62" xr:uid="{EDECDF4B-3198-4348-9F78-BF6E9FF8C9A6}"/>
     <hyperlink ref="F57" r:id="rId63" location="5" xr:uid="{3C28890A-3BF2-2647-AB92-79793D3ADD6E}"/>
     <hyperlink ref="F67" r:id="rId64" xr:uid="{617D9CE6-3964-1449-9C40-052E2D590E6C}"/>
+    <hyperlink ref="F68" r:id="rId65" xr:uid="{84D99383-F8E9-FB47-9939-D071EBFEC595}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8191,27 +8230,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C477A64-6885-F242-8D4E-EC1D72EF7EB5}">
-  <dimension ref="B2:D2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>985</v>
-      </c>
-      <c r="D2" t="s">
-        <v>984</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added tips for data type in sparrk
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AB2567-B3B4-8345-A20C-96A5BB91C314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787EBA4B-063F-0942-875F-78C1B3D779FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="990">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="994">
   <si>
     <t>docker</t>
   </si>
@@ -3012,6 +3012,18 @@
   </si>
   <si>
     <t>https://passingcuriosity.com/2013/dnsmasq-dev-osx/</t>
+  </si>
+  <si>
+    <t>spark</t>
+  </si>
+  <si>
+    <t>datatype</t>
+  </si>
+  <si>
+    <t>data types in spark</t>
+  </si>
+  <si>
+    <t>https://spark.apache.org/docs/latest/sql-ref-datatypes.html</t>
   </si>
 </sst>
 </file>
@@ -7102,10 +7114,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G68"/>
+  <dimension ref="B2:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B38" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7875,6 +7887,20 @@
       </c>
       <c r="F68" s="1" t="s">
         <v>989</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>992</v>
+      </c>
+      <c r="C69" t="s">
+        <v>990</v>
+      </c>
+      <c r="D69" t="s">
+        <v>991</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>993</v>
       </c>
     </row>
   </sheetData>
@@ -7944,6 +7970,7 @@
     <hyperlink ref="F57" r:id="rId63" location="5" xr:uid="{3C28890A-3BF2-2647-AB92-79793D3ADD6E}"/>
     <hyperlink ref="F67" r:id="rId64" xr:uid="{617D9CE6-3964-1449-9C40-052E2D590E6C}"/>
     <hyperlink ref="F68" r:id="rId65" xr:uid="{84D99383-F8E9-FB47-9939-D071EBFEC595}"/>
+    <hyperlink ref="F69" r:id="rId66" xr:uid="{339043D2-2CCF-D446-9816-25139E0CACB7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips about pandas dataframe
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787EBA4B-063F-0942-875F-78C1B3D779FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904F694B-0911-884B-8461-EEBC2A205760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
-    <sheet name="Random Articles" sheetId="4" r:id="rId2"/>
-    <sheet name="Tips" sheetId="5" r:id="rId3"/>
-    <sheet name="Websites" sheetId="6" r:id="rId4"/>
-    <sheet name="Suggested by Others" sheetId="7" r:id="rId5"/>
+    <sheet name="To do list" sheetId="9" r:id="rId2"/>
+    <sheet name="Random Articles" sheetId="4" r:id="rId3"/>
+    <sheet name="Tips" sheetId="5" r:id="rId4"/>
+    <sheet name="Websites" sheetId="6" r:id="rId5"/>
+    <sheet name="Documentations" sheetId="8" r:id="rId6"/>
+    <sheet name="Suggested by Others" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="994">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="1026">
   <si>
     <t>docker</t>
   </si>
@@ -3024,6 +3026,102 @@
   </si>
   <si>
     <t>https://spark.apache.org/docs/latest/sql-ref-datatypes.html</t>
+  </si>
+  <si>
+    <t>Note: this is frequently used to change the authentication method from password to ssh key</t>
+  </si>
+  <si>
+    <t>https://www.thenbs.com/knowledge/what-is-cobie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is COBie? </t>
+  </si>
+  <si>
+    <t>thenbs.com</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/67469221/timescale-db-not-creating-hypertable</t>
+  </si>
+  <si>
+    <t>Spark</t>
+  </si>
+  <si>
+    <t>Database sink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">streamingDF.writeStream.foreachBatch(foreach_batch_function).start() </t>
+  </si>
+  <si>
+    <t>https://spark.apache.org/docs/latest/structured-streaming-programming-guide.html</t>
+  </si>
+  <si>
+    <t>change datatype to timestamp</t>
+  </si>
+  <si>
+    <t>to_timestamp</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/57496087/correct-timestamp-with-milliseconds-format-in-spark</t>
+  </si>
+  <si>
+    <t>for index, row in df.iterrows(): print (row["Name"], row["Age"])</t>
+  </si>
+  <si>
+    <t>Iterate over rows in pandas dataframe</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/different-ways-to-iterate-over-rows-in-pandas-dataframe/</t>
+  </si>
+  <si>
+    <t>add new empty rows to dataframe</t>
+  </si>
+  <si>
+    <t>with index name</t>
+  </si>
+  <si>
+    <t>without index name</t>
+  </si>
+  <si>
+    <t>df.append(pandas.Series(), ignore_index=True)</t>
+  </si>
+  <si>
+    <t>Grafana HTTP API</t>
+  </si>
+  <si>
+    <t>https://grafana.com/docs/grafana/latest/http_api/</t>
+  </si>
+  <si>
+    <t>grafanalib</t>
+  </si>
+  <si>
+    <t>https://grafanalib.readthedocs.io/en/stable/getting-started.html</t>
+  </si>
+  <si>
+    <t>transfer data string to dataframe</t>
+  </si>
+  <si>
+    <t>df = pd.DataFrame([x.split(';') for x in data.split('\n')])</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/22604564/create-pandas-dataframe-from-a-string</t>
+  </si>
+  <si>
+    <t>Run Spark with Jupyter Notebook</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>Jupyter Notebook &amp; Spark on Kubernetes</t>
+  </si>
+  <si>
+    <t>https://towardsdatascience.com/jupyter-notebook-spark-on-kubernetes-880af7e06351</t>
+  </si>
+  <si>
+    <t>https://www.bmc.com/blogs/jupyter-notebooks-apache-spark/</t>
+  </si>
+  <si>
+    <t>How to Use Jupyter Notebooks with Apache Spark</t>
   </si>
 </sst>
 </file>
@@ -3485,11 +3583,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I595"/>
+  <dimension ref="B1:I610"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A579" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G468" sqref="G468"/>
+      <pane ySplit="1" topLeftCell="A235" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F263" sqref="F263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4637,6 +4735,9 @@
       <c r="E192" t="s">
         <v>375</v>
       </c>
+      <c r="F192" t="s">
+        <v>994</v>
+      </c>
     </row>
     <row r="193" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D193" t="s">
@@ -5098,1831 +5199,1905 @@
         <v>627</v>
       </c>
     </row>
-    <row r="258" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B258" t="s">
-        <v>962</v>
+    <row r="257" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C257" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D257" t="s">
+        <v>1006</v>
+      </c>
+      <c r="F257" s="1" t="s">
+        <v>1008</v>
       </c>
     </row>
     <row r="259" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C259" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D259" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E259" t="s">
+        <v>460</v>
+      </c>
+      <c r="F259" s="1" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="260" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D260" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E260" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="262" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C262" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D262" t="s">
+        <v>1018</v>
+      </c>
+      <c r="F262" s="1" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="269" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B269" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="270" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C270" t="s">
         <v>775</v>
       </c>
-      <c r="D259" t="s">
+      <c r="D270" t="s">
         <v>776</v>
       </c>
-      <c r="F259" s="1" t="s">
+      <c r="F270" s="1" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="272" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B272" t="s">
+    <row r="283" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B283" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="273" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C273" t="s">
+    <row r="284" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C284" t="s">
         <v>175</v>
       </c>
-      <c r="D273" s="1" t="s">
+      <c r="D284" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="274" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C274" t="s">
+    <row r="285" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C285" t="s">
         <v>177</v>
       </c>
-      <c r="D274" s="1" t="s">
+      <c r="D285" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="275" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C275" t="s">
+    <row r="286" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C286" t="s">
         <v>292</v>
       </c>
-      <c r="D275" s="1" t="s">
+      <c r="D286" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="276" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C276" t="s">
+    <row r="287" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C287" t="s">
         <v>293</v>
       </c>
-      <c r="D276" s="1" t="s">
+      <c r="D287" s="1" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="277" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C277" t="s">
+    <row r="288" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C288" t="s">
         <v>296</v>
       </c>
-      <c r="D277" s="1" t="s">
+      <c r="D288" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="278" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D278" s="1"/>
-    </row>
-    <row r="279" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D279" s="1"/>
-    </row>
-    <row r="280" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B280" t="s">
+    <row r="289" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D289" s="1"/>
+    </row>
+    <row r="290" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D290" s="1"/>
+    </row>
+    <row r="291" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B291" t="s">
         <v>342</v>
       </c>
-      <c r="D280" s="1"/>
-    </row>
-    <row r="281" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C281" t="s">
-        <v>343</v>
-      </c>
-      <c r="D281" t="s">
-        <v>368</v>
-      </c>
-      <c r="E281" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="282" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D282" t="s">
-        <v>367</v>
-      </c>
-      <c r="E282" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="283" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D283" s="1"/>
-    </row>
-    <row r="284" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D284" s="1"/>
-    </row>
-    <row r="285" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D285" s="1"/>
-    </row>
-    <row r="289" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B289" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="290" spans="2:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="C290" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D290" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="E290" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="291" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C291" t="s">
-        <v>186</v>
-      </c>
-      <c r="E291" s="1" t="s">
-        <v>187</v>
-      </c>
+      <c r="D291" s="1"/>
     </row>
     <row r="292" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C292" t="s">
-        <v>214</v>
+        <v>343</v>
+      </c>
+      <c r="D292" t="s">
+        <v>368</v>
       </c>
       <c r="E292" s="1" t="s">
-        <v>188</v>
+        <v>344</v>
+      </c>
+    </row>
+    <row r="293" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D293" t="s">
+        <v>367</v>
+      </c>
+      <c r="E293" s="1" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="294" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D294" t="s">
-        <v>215</v>
-      </c>
+      <c r="D294" s="1"/>
+    </row>
+    <row r="295" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D295" s="1"/>
     </row>
     <row r="296" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C296" t="s">
-        <v>241</v>
-      </c>
-      <c r="D296" t="s">
-        <v>242</v>
-      </c>
-      <c r="E296" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="297" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C297" t="s">
-        <v>268</v>
-      </c>
-      <c r="D297" t="s">
-        <v>269</v>
-      </c>
-      <c r="E297" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="298" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C298" t="s">
-        <v>283</v>
-      </c>
-      <c r="E298" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="299" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E299" s="1" t="s">
-        <v>285</v>
-      </c>
+      <c r="D296" s="1"/>
     </row>
     <row r="300" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E300" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="301" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C301" t="s">
-        <v>287</v>
+      <c r="B300" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="301" spans="2:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="C301" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D301" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="E301" s="1" t="s">
-        <v>288</v>
+        <v>185</v>
       </c>
     </row>
     <row r="302" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C302" t="s">
+        <v>186</v>
+      </c>
+      <c r="E302" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="303" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C303" t="s">
+        <v>214</v>
+      </c>
+      <c r="E303" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="305" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D305" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="307" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C307" t="s">
+        <v>241</v>
+      </c>
+      <c r="D307" t="s">
+        <v>242</v>
+      </c>
+      <c r="E307" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="308" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C308" t="s">
+        <v>268</v>
+      </c>
+      <c r="D308" t="s">
+        <v>269</v>
+      </c>
+      <c r="E308" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="309" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C309" t="s">
+        <v>283</v>
+      </c>
+      <c r="E309" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="310" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E310" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="311" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E311" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="312" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C312" t="s">
+        <v>287</v>
+      </c>
+      <c r="E312" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="313" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C313" t="s">
         <v>298</v>
       </c>
-      <c r="E302" s="1" t="s">
+      <c r="E313" s="1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="303" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E303" s="1"/>
-    </row>
-    <row r="304" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C304" t="s">
+    <row r="314" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E314" s="1"/>
+    </row>
+    <row r="315" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C315" t="s">
         <v>358</v>
       </c>
-      <c r="D304" t="s">
+      <c r="D315" t="s">
         <v>359</v>
       </c>
-      <c r="E304" s="1" t="s">
+      <c r="E315" s="1" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="305" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E305" s="1"/>
-    </row>
-    <row r="306" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E306" s="1"/>
-    </row>
-    <row r="307" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E307" s="1"/>
-    </row>
-    <row r="308" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E308" s="1"/>
-    </row>
-    <row r="309" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E309" s="1"/>
-    </row>
-    <row r="310" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E310" s="1"/>
-    </row>
-    <row r="311" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E311" s="1"/>
-    </row>
-    <row r="312" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E312" s="1"/>
-    </row>
-    <row r="313" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C313" t="s">
+    <row r="316" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E316" s="1"/>
+    </row>
+    <row r="317" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E317" s="1"/>
+    </row>
+    <row r="318" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E318" s="1"/>
+    </row>
+    <row r="319" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E319" s="1"/>
+    </row>
+    <row r="320" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E320" s="1"/>
+    </row>
+    <row r="321" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E321" s="1"/>
+    </row>
+    <row r="322" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E322" s="1"/>
+    </row>
+    <row r="323" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E323" s="1"/>
+    </row>
+    <row r="324" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C324" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="314" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D314" t="s">
+    <row r="325" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D325" t="s">
         <v>134</v>
       </c>
-      <c r="E314" t="s">
+      <c r="E325" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="315" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D315" t="s">
+    <row r="326" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D326" t="s">
         <v>135</v>
       </c>
-      <c r="E315" t="s">
+      <c r="E326" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="316" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D316" t="s">
+    <row r="327" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D327" t="s">
         <v>139</v>
       </c>
-      <c r="E316" t="s">
+      <c r="E327" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="317" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D317" t="s">
+    <row r="328" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D328" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="318" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D318" t="s">
+    <row r="329" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D329" t="s">
         <v>141</v>
       </c>
-      <c r="E318" t="s">
+      <c r="E329" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="319" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D319" t="s">
+    <row r="330" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D330" t="s">
         <v>482</v>
       </c>
-      <c r="E319" t="s">
+      <c r="E330" t="s">
         <v>484</v>
       </c>
-      <c r="F319" t="s">
+      <c r="F330" t="s">
         <v>488</v>
       </c>
-      <c r="G319" t="s">
+      <c r="G330" t="s">
         <v>483</v>
       </c>
-      <c r="H319" s="1" t="s">
+      <c r="H330" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="320" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D320" t="s">
+    <row r="331" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D331" t="s">
         <v>485</v>
       </c>
-      <c r="E320" t="s">
+      <c r="E331" t="s">
         <v>486</v>
       </c>
-      <c r="G320" t="s">
+      <c r="G331" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="322" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C322" t="s">
+    <row r="333" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C333" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="323" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D323" t="s">
-        <v>72</v>
-      </c>
-      <c r="E323" t="s">
-        <v>73</v>
-      </c>
-      <c r="F323" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="324" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D324" t="s">
-        <v>75</v>
-      </c>
-      <c r="E324" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="325" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D325" t="s">
-        <v>77</v>
-      </c>
-      <c r="E325" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="326" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D326" t="s">
-        <v>80</v>
-      </c>
-      <c r="E326" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="327" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D327" t="s">
-        <v>361</v>
-      </c>
-      <c r="E327" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="328" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D328" t="s">
-        <v>362</v>
-      </c>
-      <c r="E328" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="330" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D330" t="s">
-        <v>81</v>
-      </c>
-      <c r="E330" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="331" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D331" t="s">
-        <v>83</v>
-      </c>
-      <c r="E331" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="333" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C333" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="334" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="334" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D334" t="s">
         <v>72</v>
       </c>
       <c r="E334" t="s">
-        <v>130</v>
-      </c>
-      <c r="F334" s="1"/>
-    </row>
-    <row r="335" spans="3:6" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="F334" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="335" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D335" t="s">
-        <v>146</v>
+        <v>75</v>
       </c>
       <c r="E335" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F335" s="1"/>
-    </row>
-    <row r="336" spans="3:6" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="336" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D336" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E336" s="1" t="s">
-        <v>148</v>
+        <v>78</v>
       </c>
     </row>
     <row r="337" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E337" s="1"/>
+      <c r="D337" t="s">
+        <v>80</v>
+      </c>
+      <c r="E337" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="338" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D338" t="s">
-        <v>143</v>
+        <v>361</v>
+      </c>
+      <c r="E338" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="339" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D339" t="s">
+        <v>362</v>
+      </c>
       <c r="E339" t="s">
-        <v>150</v>
-      </c>
-      <c r="F339" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="340" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E340" t="s">
-        <v>151</v>
-      </c>
-      <c r="F340" t="s">
-        <v>144</v>
-      </c>
-      <c r="G340" s="1" t="s">
-        <v>145</v>
+        <v>363</v>
       </c>
     </row>
     <row r="341" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D341" t="s">
-        <v>152</v>
-      </c>
-      <c r="E341" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G341" s="1"/>
-    </row>
-    <row r="343" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C343" t="s">
-        <v>950</v>
+        <v>81</v>
+      </c>
+      <c r="E341" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="342" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D342" t="s">
+        <v>83</v>
+      </c>
+      <c r="E342" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="344" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D344" t="s">
-        <v>953</v>
-      </c>
-      <c r="E344" t="s">
-        <v>951</v>
-      </c>
-      <c r="F344" s="1" t="s">
-        <v>954</v>
+      <c r="C344" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="345" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D345" t="s">
+        <v>72</v>
+      </c>
+      <c r="E345" t="s">
+        <v>130</v>
+      </c>
+      <c r="F345" s="1"/>
+    </row>
+    <row r="346" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D346" t="s">
+        <v>146</v>
+      </c>
+      <c r="E346" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F346" s="1"/>
+    </row>
+    <row r="347" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D347" t="s">
+        <v>75</v>
+      </c>
+      <c r="E347" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="348" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E348" s="1"/>
+    </row>
+    <row r="349" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D349" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="350" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E350" t="s">
+        <v>150</v>
+      </c>
+      <c r="F350" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="351" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E351" t="s">
+        <v>151</v>
+      </c>
+      <c r="F351" t="s">
+        <v>144</v>
+      </c>
+      <c r="G351" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="352" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D352" t="s">
+        <v>152</v>
+      </c>
+      <c r="E352" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G352" s="1"/>
+    </row>
+    <row r="354" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C354" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="355" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D355" t="s">
+        <v>953</v>
+      </c>
+      <c r="E355" t="s">
+        <v>951</v>
+      </c>
+      <c r="F355" s="1" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="356" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D356" t="s">
         <v>952</v>
       </c>
-      <c r="E345" t="s">
+      <c r="E356" t="s">
         <v>951</v>
       </c>
     </row>
-    <row r="347" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C347" t="s">
+    <row r="358" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C358" t="s">
         <v>963</v>
       </c>
     </row>
-    <row r="348" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D348" t="s">
+    <row r="359" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D359" t="s">
         <v>964</v>
       </c>
-      <c r="E348" t="s">
+      <c r="E359" t="s">
         <v>968</v>
       </c>
-      <c r="F348" t="s">
+      <c r="F359" t="s">
         <v>966</v>
       </c>
     </row>
-    <row r="349" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E349" t="s">
+    <row r="360" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E360" t="s">
         <v>965</v>
       </c>
-      <c r="F349" t="s">
+      <c r="F360" t="s">
         <v>967</v>
       </c>
     </row>
-    <row r="355" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E355" s="1"/>
-    </row>
-    <row r="357" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B357" t="s">
+    <row r="366" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E366" s="1"/>
+    </row>
+    <row r="368" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B368" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="358" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C358" t="s">
+    <row r="369" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C369" t="s">
         <v>276</v>
       </c>
-      <c r="D358" t="s">
+      <c r="D369" t="s">
         <v>278</v>
       </c>
-      <c r="E358" s="1" t="s">
+      <c r="E369" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="359" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C359" t="s">
+    <row r="370" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C370" t="s">
         <v>280</v>
       </c>
-      <c r="E359" s="1" t="s">
+      <c r="E370" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="F359" s="1" t="s">
+      <c r="F370" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="G359" s="1" t="s">
+      <c r="G370" s="1" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="360" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C360" t="s">
+    <row r="371" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C371" t="s">
         <v>289</v>
       </c>
-      <c r="E360" s="1" t="s">
+      <c r="E371" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="361" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C361" t="s">
+    <row r="372" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C372" t="s">
         <v>303</v>
       </c>
-      <c r="E361" s="1" t="s">
+      <c r="E372" s="1" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="362" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D362" t="s">
+    <row r="373" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D373" t="s">
         <v>305</v>
       </c>
-      <c r="E362" s="1" t="s">
+      <c r="E373" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="363" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C363" t="s">
+    <row r="374" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C374" t="s">
         <v>323</v>
       </c>
-      <c r="E363" s="1" t="s">
+      <c r="E374" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="364" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C364" t="s">
+    <row r="375" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C375" t="s">
         <v>307</v>
       </c>
-      <c r="D364" t="s">
+      <c r="D375" t="s">
         <v>308</v>
       </c>
-      <c r="E364" s="1" t="s">
+      <c r="E375" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="365" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C365" t="s">
+    <row r="376" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C376" t="s">
         <v>310</v>
       </c>
-      <c r="E365" s="1" t="s">
+      <c r="E376" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="366" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C366" t="s">
+    <row r="377" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C377" t="s">
         <v>315</v>
       </c>
-      <c r="E366" s="1" t="s">
+      <c r="E377" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="367" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C367" t="s">
+    <row r="378" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C378" t="s">
         <v>316</v>
       </c>
-      <c r="E367" s="1" t="s">
+      <c r="E378" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="368" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C368" t="s">
+    <row r="379" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C379" t="s">
         <v>318</v>
       </c>
-      <c r="E368" s="1" t="s">
+      <c r="E379" s="1" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="369" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C369" t="s">
+    <row r="380" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C380" t="s">
         <v>325</v>
       </c>
-      <c r="D369" t="s">
+      <c r="D380" t="s">
         <v>332</v>
       </c>
-      <c r="E369" s="1" t="s">
+      <c r="E380" s="1" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="370" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D370" t="s">
+    <row r="381" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D381" t="s">
         <v>327</v>
       </c>
-      <c r="E370" s="1" t="s">
+      <c r="E381" s="1" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="372" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C372" t="s">
+    <row r="383" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C383" t="s">
         <v>329</v>
       </c>
-      <c r="D372" t="s">
+      <c r="D383" t="s">
         <v>330</v>
       </c>
-      <c r="E372" s="1" t="s">
+      <c r="E383" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="374" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C374" t="s">
+    <row r="385" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C385" t="s">
         <v>335</v>
       </c>
-      <c r="D374" t="s">
+      <c r="D385" t="s">
         <v>337</v>
       </c>
-      <c r="E374" s="1" t="s">
+      <c r="E385" s="1" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="378" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B378" t="s">
+    <row r="389" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B389" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="379" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C379" t="s">
+    <row r="390" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C390" t="s">
         <v>341</v>
       </c>
-      <c r="D379" t="s">
+      <c r="D390" t="s">
         <v>339</v>
       </c>
-      <c r="E379" s="1" t="s">
+      <c r="E390" s="1" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="385" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B385" t="s">
+    <row r="396" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B396" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="386" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C386" t="s">
+    <row r="397" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C397" t="s">
         <v>86</v>
       </c>
-      <c r="D386" t="s">
+      <c r="D397" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="387" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C387" t="s">
+    <row r="398" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C398" t="s">
         <v>88</v>
       </c>
-      <c r="D387" t="s">
+      <c r="D398" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="388" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C388" t="s">
+    <row r="399" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C399" t="s">
         <v>95</v>
       </c>
-      <c r="D388" s="1" t="s">
+      <c r="D399" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="389" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C389" t="s">
+    <row r="400" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C400" t="s">
         <v>97</v>
       </c>
-      <c r="D389" s="1" t="s">
+      <c r="D400" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="391" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B391" t="s">
+    <row r="402" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B402" t="s">
         <v>90</v>
       </c>
-      <c r="C391" t="s">
+      <c r="C402" t="s">
         <v>91</v>
       </c>
-      <c r="D391" t="s">
+      <c r="D402" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="392" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C392" t="s">
+    <row r="403" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C403" t="s">
         <v>93</v>
       </c>
-      <c r="D392" t="s">
+      <c r="D403" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="395" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B395" t="s">
+    <row r="406" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B406" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="396" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C396" t="s">
+    <row r="407" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C407" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="397" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D397" t="s">
+    <row r="408" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D408" t="s">
         <v>104</v>
       </c>
-      <c r="E397" s="1" t="s">
+      <c r="E408" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="398" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D398" t="s">
+    <row r="409" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D409" t="s">
         <v>101</v>
       </c>
-      <c r="E398" s="1" t="s">
+      <c r="E409" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="399" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D399" t="s">
+    <row r="410" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D410" t="s">
         <v>102</v>
       </c>
-      <c r="E399" s="1" t="s">
+      <c r="E410" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="400" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D400" t="s">
+    <row r="411" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D411" t="s">
         <v>107</v>
       </c>
-      <c r="E400" t="s">
+      <c r="E411" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="402" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B402" t="s">
+    <row r="413" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B413" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="403" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C403" t="s">
+    <row r="414" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C414" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="404" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D404" t="s">
+    <row r="415" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D415" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="405" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D405" t="s">
+    <row r="416" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D416" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="406" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F406" s="1" t="s">
+    <row r="417" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F417" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="407" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B407" t="s">
+    <row r="418" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B418" t="s">
         <v>1</v>
       </c>
-      <c r="F407" s="1" t="s">
+      <c r="F418" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="408" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C408" t="s">
+    <row r="419" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C419" t="s">
         <v>112</v>
       </c>
-      <c r="D408" s="1" t="s">
+      <c r="D419" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="409" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D409" t="s">
+    <row r="420" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D420" t="s">
         <v>126</v>
       </c>
-      <c r="E409" s="1" t="s">
+      <c r="E420" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="410" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C410" t="s">
+    <row r="421" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C421" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="411" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D411" t="s">
+    <row r="422" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D422" t="s">
         <v>115</v>
       </c>
-      <c r="E411" s="1" t="s">
+      <c r="E422" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F411" t="s">
+      <c r="F422" t="s">
         <v>128</v>
       </c>
-      <c r="G411" s="1" t="s">
+      <c r="G422" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="412" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E412" t="s">
+    <row r="423" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E423" t="s">
         <v>121</v>
       </c>
-      <c r="G412" s="1"/>
-    </row>
-    <row r="413" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E413" t="s">
+      <c r="G423" s="1"/>
+    </row>
+    <row r="424" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E424" t="s">
         <v>124</v>
       </c>
-      <c r="G413" s="1"/>
-    </row>
-    <row r="414" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D414" t="s">
+      <c r="G424" s="1"/>
+    </row>
+    <row r="425" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D425" t="s">
         <v>117</v>
       </c>
-      <c r="E414" s="1" t="s">
+      <c r="E425" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G414" s="1"/>
-    </row>
-    <row r="415" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D415" t="s">
+      <c r="G425" s="1"/>
+    </row>
+    <row r="426" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D426" t="s">
         <v>119</v>
       </c>
-      <c r="E415" s="1" t="s">
+      <c r="E426" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G415" s="1"/>
-    </row>
-    <row r="416" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E416" s="1" t="s">
+      <c r="G426" s="1"/>
+    </row>
+    <row r="427" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E427" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="G416" s="1"/>
-    </row>
-    <row r="417" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E417" t="s">
+      <c r="G427" s="1"/>
+    </row>
+    <row r="428" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E428" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="418" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D418" t="s">
+    <row r="429" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D429" t="s">
         <v>301</v>
       </c>
-      <c r="E418" s="1" t="s">
+      <c r="E429" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="419" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D419" t="s">
+    <row r="430" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D430" t="s">
         <v>300</v>
       </c>
-      <c r="E419" s="1" t="s">
+      <c r="E430" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="424" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C424" t="s">
+    <row r="435" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C435" t="s">
         <v>131</v>
       </c>
-      <c r="D424" s="1" t="s">
+      <c r="D435" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="428" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B428" t="s">
+    <row r="439" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B439" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="429" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C429" t="s">
+    <row r="440" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C440" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="430" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D430" t="s">
+    <row r="441" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D441" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="431" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E431" t="s">
+    <row r="442" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E442" t="s">
         <v>492</v>
       </c>
-      <c r="F431" s="1" t="s">
+      <c r="F442" s="1" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="432" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E432" t="s">
+    <row r="443" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E443" t="s">
         <v>494</v>
       </c>
-      <c r="F432" s="1" t="s">
+      <c r="F443" s="1" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="433" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E433" t="s">
+    <row r="444" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E444" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="434" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D434" t="s">
+    <row r="445" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D445" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="435" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E435" t="s">
+    <row r="446" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E446" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="436" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E436" t="s">
+    <row r="447" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E447" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="437" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D437" t="s">
+    <row r="448" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D448" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="438" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E438" t="s">
+    <row r="449" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E449" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="439" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C439" t="s">
+    <row r="450" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C450" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="440" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D440" t="s">
+    <row r="451" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D451" t="s">
         <v>503</v>
       </c>
-      <c r="E440" t="s">
+      <c r="E451" t="s">
         <v>504</v>
-      </c>
-    </row>
-    <row r="441" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D441" t="s">
-        <v>501</v>
-      </c>
-      <c r="E441" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="443" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C443" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="444" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D444" t="s">
-        <v>508</v>
-      </c>
-      <c r="E444" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="445" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D445" t="s">
-        <v>509</v>
-      </c>
-      <c r="E445" t="s">
-        <v>507</v>
-      </c>
-      <c r="G445" s="1" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="447" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C447" t="s">
-        <v>512</v>
-      </c>
-      <c r="G447" s="1" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="449" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C449" t="s">
-        <v>513</v>
-      </c>
-      <c r="E449" t="s">
-        <v>514</v>
-      </c>
-      <c r="G449" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="451" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C451" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="452" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D452" t="s">
-        <v>518</v>
+        <v>501</v>
       </c>
       <c r="E452" t="s">
-        <v>517</v>
-      </c>
-      <c r="G452" s="1" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="453" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D453" t="s">
-        <v>519</v>
-      </c>
-      <c r="E453" t="s">
-        <v>520</v>
+        <v>502</v>
+      </c>
+    </row>
+    <row r="454" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C454" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="455" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C455" t="s">
-        <v>522</v>
+      <c r="D455" t="s">
+        <v>508</v>
+      </c>
+      <c r="E455" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="456" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D456" t="s">
-        <v>528</v>
+        <v>509</v>
       </c>
       <c r="E456" t="s">
-        <v>524</v>
+        <v>507</v>
       </c>
       <c r="G456" s="1" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="457" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D457" t="s">
-        <v>526</v>
-      </c>
-      <c r="E457" t="s">
-        <v>523</v>
+        <v>510</v>
       </c>
     </row>
     <row r="458" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D458" t="s">
-        <v>527</v>
-      </c>
-      <c r="E458" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="459" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C459" t="s">
-        <v>629</v>
+      <c r="C458" t="s">
+        <v>512</v>
+      </c>
+      <c r="G458" s="1" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="460" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D460" t="s">
-        <v>630</v>
+      <c r="C460" t="s">
+        <v>513</v>
       </c>
       <c r="E460" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="461" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D461" t="s">
-        <v>632</v>
-      </c>
-      <c r="E461" t="s">
-        <v>633</v>
+        <v>514</v>
+      </c>
+      <c r="G460" s="1" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="462" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D462" t="s">
-        <v>634</v>
-      </c>
-      <c r="E462" t="s">
-        <v>635</v>
+      <c r="C462" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="463" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D463" t="s">
-        <v>637</v>
+        <v>518</v>
       </c>
       <c r="E463" t="s">
-        <v>636</v>
+        <v>517</v>
+      </c>
+      <c r="G463" s="1" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="464" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D464" t="s">
+        <v>519</v>
+      </c>
+      <c r="E464" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="466" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C466" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="467" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D467" t="s">
+        <v>528</v>
+      </c>
+      <c r="E467" t="s">
+        <v>524</v>
+      </c>
+      <c r="G467" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="468" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D468" t="s">
+        <v>526</v>
+      </c>
+      <c r="E468" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="469" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D469" t="s">
+        <v>527</v>
+      </c>
+      <c r="E469" t="s">
+        <v>525</v>
+      </c>
+      <c r="H469" s="1" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="470" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C470" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="471" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D471" t="s">
+        <v>630</v>
+      </c>
+      <c r="E471" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="472" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D472" t="s">
+        <v>632</v>
+      </c>
+      <c r="E472" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="473" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D473" t="s">
+        <v>634</v>
+      </c>
+      <c r="E473" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="474" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D474" t="s">
+        <v>637</v>
+      </c>
+      <c r="E474" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="475" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D475" t="s">
         <v>693</v>
       </c>
-      <c r="E464" t="s">
+      <c r="E475" t="s">
         <v>695</v>
       </c>
-      <c r="G464" s="1" t="s">
+      <c r="G475" s="1" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="467" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B467" t="s">
+    <row r="478" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B478" t="s">
         <v>778</v>
       </c>
     </row>
-    <row r="468" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C468" t="s">
+    <row r="479" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C479" t="s">
         <v>779</v>
       </c>
-      <c r="G468" s="1" t="s">
+      <c r="G479" s="1" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="477" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B477" t="s">
+    <row r="488" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B488" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="478" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C478" t="s">
+    <row r="489" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C489" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="479" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D479" t="s">
+    <row r="490" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D490" t="s">
         <v>541</v>
       </c>
-      <c r="G479" s="1" t="s">
+      <c r="G490" s="1" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="480" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C480" t="s">
+    <row r="491" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C491" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="481" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D481" t="s">
+    <row r="492" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D492" t="s">
         <v>543</v>
       </c>
-      <c r="E481" t="s">
+      <c r="E492" t="s">
         <v>544</v>
       </c>
-      <c r="G481" s="1" t="s">
+      <c r="G492" s="1" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="483" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C483" t="s">
+    <row r="494" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C494" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="484" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D484" t="s">
+    <row r="495" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D495" t="s">
         <v>548</v>
       </c>
-      <c r="E484" t="s">
+      <c r="E495" t="s">
         <v>549</v>
       </c>
-      <c r="G484" s="1" t="s">
+      <c r="G495" s="1" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="485" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D485" t="s">
+    <row r="496" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D496" t="s">
         <v>550</v>
       </c>
-      <c r="E485" t="s">
+      <c r="E496" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="486" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D486" t="s">
+    <row r="497" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D497" t="s">
         <v>552</v>
       </c>
-      <c r="E486" t="s">
+      <c r="E497" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="487" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D487" t="s">
+    <row r="498" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D498" t="s">
         <v>554</v>
       </c>
-      <c r="E487" t="s">
+      <c r="E498" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="489" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C489" t="s">
+    <row r="500" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C500" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="490" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D490" t="s">
+    <row r="501" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D501" t="s">
         <v>558</v>
       </c>
-      <c r="E490" t="s">
+      <c r="E501" t="s">
         <v>560</v>
       </c>
-      <c r="G490" s="1" t="s">
+      <c r="G501" s="1" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="491" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D491" t="s">
+    <row r="502" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D502" t="s">
         <v>559</v>
       </c>
-      <c r="E491" t="s">
+      <c r="E502" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="493" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C493" t="s">
+    <row r="504" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C504" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="494" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D494" t="s">
+    <row r="505" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D505" t="s">
         <v>565</v>
       </c>
-      <c r="G494" s="1" t="s">
+      <c r="G505" s="1" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="495" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C495" t="s">
+    <row r="506" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C506" t="s">
         <v>608</v>
       </c>
-      <c r="G495" s="1"/>
-    </row>
-    <row r="496" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D496" t="s">
+      <c r="G506" s="1"/>
+    </row>
+    <row r="507" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D507" t="s">
         <v>609</v>
       </c>
-      <c r="E496" t="s">
+      <c r="E507" t="s">
         <v>610</v>
       </c>
-      <c r="G496" s="1" t="s">
+      <c r="G507" s="1" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="497" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G497" s="1"/>
-    </row>
-    <row r="498" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C498" t="s">
+    <row r="508" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G508" s="1"/>
+    </row>
+    <row r="509" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C509" t="s">
         <v>834</v>
       </c>
-      <c r="G498" s="1"/>
-    </row>
-    <row r="499" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D499" t="s">
+      <c r="G509" s="1"/>
+    </row>
+    <row r="510" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D510" t="s">
         <v>835</v>
       </c>
-      <c r="G499" s="1" t="s">
+      <c r="G510" s="1" t="s">
         <v>836</v>
       </c>
     </row>
-    <row r="500" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C500" t="s">
+    <row r="511" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C511" t="s">
         <v>890</v>
       </c>
-      <c r="G500" s="1"/>
-    </row>
-    <row r="501" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D501" t="s">
+      <c r="G511" s="1"/>
+    </row>
+    <row r="512" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D512" t="s">
         <v>891</v>
       </c>
-      <c r="G501" s="1" t="s">
+      <c r="G512" s="1" t="s">
         <v>892</v>
       </c>
     </row>
-    <row r="502" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C502" t="s">
+    <row r="513" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C513" t="s">
         <v>917</v>
       </c>
-      <c r="G502" s="1"/>
-    </row>
-    <row r="503" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D503" t="s">
+      <c r="G513" s="1"/>
+    </row>
+    <row r="514" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D514" t="s">
         <v>918</v>
       </c>
-      <c r="G503" s="1" t="s">
+      <c r="G514" s="1" t="s">
         <v>919</v>
       </c>
     </row>
-    <row r="505" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B505" t="s">
+    <row r="516" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B516" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="506" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C506" t="s">
+    <row r="517" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C517" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="507" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E507" t="s">
+    <row r="518" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E518" t="s">
         <v>568</v>
       </c>
-      <c r="G507" s="1" t="s">
+      <c r="G518" s="1" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="510" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B510" t="s">
+    <row r="521" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B521" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="511" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C511" t="s">
+    <row r="522" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C522" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="512" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D512" t="s">
+    <row r="523" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D523" t="s">
         <v>572</v>
       </c>
-      <c r="E512" t="s">
+      <c r="E523" t="s">
         <v>573</v>
       </c>
-      <c r="F512" t="s">
+      <c r="F523" t="s">
         <v>574</v>
       </c>
-      <c r="G512" s="1" t="s">
+      <c r="G523" s="1" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="513" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E513" t="s">
+    <row r="524" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E524" t="s">
         <v>576</v>
       </c>
-      <c r="F513" t="s">
+      <c r="F524" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="514" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C514" t="s">
+    <row r="525" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C525" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="515" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D515" t="s">
+    <row r="526" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D526" t="s">
         <v>595</v>
       </c>
-      <c r="E515" t="s">
+      <c r="E526" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="516" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D516" t="s">
+    <row r="527" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D527" t="s">
         <v>598</v>
       </c>
-      <c r="E516" t="s">
+      <c r="E527" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="518" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D518" t="s">
+    <row r="529" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D529" t="s">
         <v>599</v>
       </c>
-      <c r="E518" t="s">
+      <c r="E529" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="519" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D519" t="s">
+    <row r="530" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D530" t="s">
         <v>601</v>
       </c>
-      <c r="E519" t="s">
+      <c r="E530" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="521" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D521" t="s">
+    <row r="532" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D532" t="s">
         <v>838</v>
       </c>
-      <c r="E521" t="s">
+      <c r="E532" t="s">
         <v>837</v>
       </c>
     </row>
-    <row r="522" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D522" t="s">
+    <row r="533" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D533" t="s">
         <v>839</v>
       </c>
-      <c r="E522" t="s">
+      <c r="E533" t="s">
         <v>603</v>
       </c>
-      <c r="G522" s="1" t="s">
+      <c r="G533" s="1" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="523" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D523" t="s">
+    <row r="534" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D534" t="s">
         <v>604</v>
       </c>
-      <c r="E523" t="s">
+      <c r="E534" t="s">
         <v>605</v>
       </c>
-      <c r="F523" t="s">
+      <c r="F534" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="525" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D525" t="s">
+    <row r="536" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D536" t="s">
         <v>840</v>
       </c>
-      <c r="E525" t="s">
+      <c r="E536" t="s">
         <v>849</v>
       </c>
-      <c r="F525" t="s">
+      <c r="F536" t="s">
         <v>851</v>
       </c>
-      <c r="H525" s="1" t="s">
+      <c r="H536" s="1" t="s">
         <v>850</v>
       </c>
     </row>
-    <row r="526" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="E526" t="s">
+    <row r="537" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E537" t="s">
         <v>848</v>
       </c>
-      <c r="F526" t="s">
+      <c r="F537" t="s">
         <v>841</v>
       </c>
-      <c r="G526" t="s">
+      <c r="G537" t="s">
         <v>842</v>
       </c>
-      <c r="H526" s="1" t="s">
+      <c r="H537" s="1" t="s">
         <v>843</v>
       </c>
     </row>
-    <row r="527" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="G527" s="1"/>
-    </row>
-    <row r="528" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D528" t="s">
+    <row r="538" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="G538" s="1"/>
+    </row>
+    <row r="539" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D539" t="s">
         <v>844</v>
       </c>
-      <c r="E528" t="s">
+      <c r="E539" t="s">
         <v>845</v>
       </c>
-      <c r="G528" s="1" t="s">
+      <c r="G539" s="1" t="s">
         <v>847</v>
       </c>
     </row>
-    <row r="529" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E529" t="s">
+    <row r="540" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="E540" t="s">
         <v>846</v>
       </c>
-      <c r="G529" s="1"/>
-    </row>
-    <row r="530" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C530" t="s">
+      <c r="G540" s="1"/>
+    </row>
+    <row r="541" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C541" t="s">
         <v>860</v>
       </c>
-      <c r="G530" s="1"/>
-    </row>
-    <row r="531" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D531" t="s">
+      <c r="G541" s="1"/>
+    </row>
+    <row r="542" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D542" t="s">
         <v>861</v>
       </c>
-      <c r="E531" t="s">
+      <c r="E542" t="s">
         <v>574</v>
       </c>
-      <c r="G531" s="1"/>
-    </row>
-    <row r="532" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D532" t="s">
+      <c r="G542" s="1"/>
+    </row>
+    <row r="543" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D543" t="s">
         <v>862</v>
       </c>
-      <c r="E532" t="s">
+      <c r="E543" t="s">
         <v>577</v>
       </c>
-      <c r="G532" s="1"/>
-    </row>
-    <row r="533" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G533" s="1"/>
-    </row>
-    <row r="535" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B535" t="s">
+      <c r="G543" s="1"/>
+    </row>
+    <row r="544" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="G544" s="1"/>
+    </row>
+    <row r="546" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B546" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="536" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C536" t="s">
+    <row r="547" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C547" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="537" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D537" t="s">
+    <row r="548" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D548" t="s">
         <v>581</v>
       </c>
-      <c r="E537" t="s">
+      <c r="E548" t="s">
         <v>582</v>
       </c>
-      <c r="F537" t="s">
+      <c r="F548" t="s">
         <v>580</v>
       </c>
-      <c r="G537" s="1" t="s">
+      <c r="G548" s="1" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="538" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E538" t="s">
+    <row r="549" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E549" t="s">
         <v>583</v>
       </c>
-      <c r="F538" t="s">
+      <c r="F549" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="540" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D540" t="s">
+    <row r="551" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D551" t="s">
         <v>586</v>
       </c>
-      <c r="E540" t="s">
+      <c r="E551" t="s">
         <v>588</v>
       </c>
-      <c r="F540" t="s">
+      <c r="F551" t="s">
         <v>587</v>
-      </c>
-    </row>
-    <row r="543" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B543" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="544" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C544" t="s">
-        <v>707</v>
-      </c>
-      <c r="D544" t="s">
-        <v>710</v>
-      </c>
-      <c r="G544" s="1" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="545" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C545" t="s">
-        <v>708</v>
-      </c>
-      <c r="D545" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="546" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C546" t="s">
-        <v>709</v>
-      </c>
-      <c r="D546" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="549" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B549" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="550" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C550" t="s">
-        <v>731</v>
-      </c>
-      <c r="G550" s="1" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="551" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C551" t="s">
-        <v>733</v>
-      </c>
-      <c r="G551" s="1" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="552" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C552" t="s">
-        <v>737</v>
-      </c>
-      <c r="F552" t="s">
-        <v>735</v>
-      </c>
-      <c r="G552" s="1" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="554" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B554" t="s">
-        <v>742</v>
+        <v>706</v>
       </c>
     </row>
     <row r="555" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C555" t="s">
-        <v>743</v>
+        <v>707</v>
       </c>
       <c r="D555" t="s">
-        <v>744</v>
+        <v>710</v>
       </c>
       <c r="G555" s="1" t="s">
-        <v>745</v>
+        <v>713</v>
       </c>
     </row>
     <row r="556" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C556" t="s">
-        <v>746</v>
+        <v>708</v>
       </c>
       <c r="D556" t="s">
-        <v>747</v>
-      </c>
-      <c r="G556" s="1" t="s">
-        <v>748</v>
+        <v>711</v>
+      </c>
+    </row>
+    <row r="557" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C557" t="s">
+        <v>709</v>
+      </c>
+      <c r="D557" t="s">
+        <v>712</v>
       </c>
     </row>
     <row r="560" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B560" t="s">
-        <v>801</v>
+        <v>730</v>
       </c>
     </row>
     <row r="561" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C561" t="s">
-        <v>802</v>
-      </c>
-      <c r="D561" t="s">
-        <v>803</v>
-      </c>
-      <c r="E561" t="s">
-        <v>804</v>
+        <v>731</v>
       </c>
       <c r="G561" s="1" t="s">
-        <v>805</v>
+        <v>732</v>
       </c>
     </row>
     <row r="562" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C562" t="s">
-        <v>806</v>
-      </c>
-      <c r="E562" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="564" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B564" t="s">
-        <v>852</v>
-      </c>
-      <c r="G564" s="1" t="s">
-        <v>859</v>
+        <v>733</v>
+      </c>
+      <c r="G562" s="1" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="563" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C563" t="s">
+        <v>737</v>
+      </c>
+      <c r="F563" t="s">
+        <v>735</v>
+      </c>
+      <c r="G563" s="1" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="565" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C565" t="s">
-        <v>853</v>
+      <c r="B565" t="s">
+        <v>742</v>
       </c>
     </row>
     <row r="566" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C566" t="s">
+        <v>743</v>
+      </c>
       <c r="D566" t="s">
-        <v>856</v>
+        <v>744</v>
+      </c>
+      <c r="G566" s="1" t="s">
+        <v>745</v>
       </c>
     </row>
     <row r="567" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C567" t="s">
+        <v>746</v>
+      </c>
+      <c r="D567" t="s">
+        <v>747</v>
+      </c>
+      <c r="G567" s="1" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="571" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B571" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="572" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C572" t="s">
+        <v>802</v>
+      </c>
+      <c r="D572" t="s">
+        <v>803</v>
+      </c>
+      <c r="E572" t="s">
+        <v>804</v>
+      </c>
+      <c r="G572" s="1" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="573" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C573" t="s">
+        <v>806</v>
+      </c>
+      <c r="E573" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="575" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B575" t="s">
+        <v>852</v>
+      </c>
+      <c r="G575" s="1" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="576" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C576" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="577" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D577" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="578" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C578" t="s">
         <v>854</v>
-      </c>
-    </row>
-    <row r="568" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D568" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="569" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C569" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="570" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D570" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="573" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B573" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="574" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C574" t="s">
-        <v>875</v>
-      </c>
-      <c r="D574" t="s">
-        <v>876</v>
-      </c>
-      <c r="G574" s="1" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="576" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B576" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="577" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C577" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="578" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D578" t="s">
-        <v>928</v>
-      </c>
-      <c r="E578" t="s">
-        <v>930</v>
-      </c>
-      <c r="F578" t="s">
-        <v>929</v>
-      </c>
-      <c r="G578" t="s">
-        <v>931</v>
       </c>
     </row>
     <row r="579" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D579" t="s">
-        <v>932</v>
-      </c>
-      <c r="E579" t="s">
-        <v>933</v>
-      </c>
-      <c r="G579" s="1" t="s">
-        <v>941</v>
+        <v>857</v>
       </c>
     </row>
     <row r="580" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D580" t="s">
-        <v>934</v>
-      </c>
-      <c r="E580" t="s">
-        <v>935</v>
-      </c>
-      <c r="G580" s="1" t="s">
-        <v>859</v>
+      <c r="C580" t="s">
+        <v>855</v>
       </c>
     </row>
     <row r="581" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D581" t="s">
-        <v>936</v>
-      </c>
-      <c r="E581" t="s">
-        <v>937</v>
-      </c>
-    </row>
-    <row r="582" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D582" t="s">
-        <v>939</v>
-      </c>
-      <c r="E582" t="s">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="583" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D583" t="s">
-        <v>940</v>
-      </c>
-      <c r="E583" t="s">
         <v>858</v>
       </c>
-      <c r="G583" s="1" t="s">
-        <v>859</v>
+    </row>
+    <row r="584" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B584" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="585" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C585" t="s">
+        <v>875</v>
+      </c>
+      <c r="D585" t="s">
+        <v>876</v>
+      </c>
+      <c r="G585" s="1" t="s">
+        <v>877</v>
       </c>
     </row>
     <row r="587" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B587" t="s">
-        <v>955</v>
+        <v>926</v>
       </c>
     </row>
     <row r="588" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C588" t="s">
-        <v>956</v>
+        <v>927</v>
       </c>
     </row>
     <row r="589" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D589" t="s">
+        <v>928</v>
+      </c>
+      <c r="E589" t="s">
+        <v>930</v>
+      </c>
+      <c r="F589" t="s">
+        <v>929</v>
+      </c>
+      <c r="G589" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="590" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D590" t="s">
+        <v>932</v>
+      </c>
+      <c r="E590" t="s">
+        <v>933</v>
+      </c>
+      <c r="G590" s="1" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="591" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D591" t="s">
+        <v>934</v>
+      </c>
+      <c r="E591" t="s">
+        <v>935</v>
+      </c>
+      <c r="G591" s="1" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="592" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D592" t="s">
+        <v>936</v>
+      </c>
+      <c r="E592" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="593" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D593" t="s">
+        <v>939</v>
+      </c>
+      <c r="E593" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="594" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D594" t="s">
+        <v>940</v>
+      </c>
+      <c r="E594" t="s">
+        <v>858</v>
+      </c>
+      <c r="G594" s="1" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="598" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B598" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="599" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C599" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="600" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D600" t="s">
         <v>957</v>
       </c>
-      <c r="G589" s="1" t="s">
+      <c r="G600" s="1" t="s">
         <v>958</v>
       </c>
     </row>
-    <row r="590" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C590" t="s">
+    <row r="601" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C601" t="s">
         <v>959</v>
       </c>
-      <c r="D590" t="s">
+      <c r="D601" t="s">
         <v>960</v>
       </c>
-      <c r="G590" s="1" t="s">
+      <c r="G601" s="1" t="s">
         <v>961</v>
       </c>
     </row>
-    <row r="593" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B593" t="s">
+    <row r="604" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B604" t="s">
         <v>984</v>
       </c>
     </row>
-    <row r="594" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C594" t="s">
+    <row r="605" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C605" t="s">
         <v>985</v>
       </c>
     </row>
-    <row r="595" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D595" t="s">
+    <row r="606" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D606" t="s">
         <v>986</v>
       </c>
-      <c r="G595" s="1" t="s">
+      <c r="G606" s="1" t="s">
         <v>987</v>
+      </c>
+    </row>
+    <row r="608" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B608" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="609" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C609" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D609" t="s">
+        <v>1001</v>
+      </c>
+      <c r="G609" s="1" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="610" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C610" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D610" t="s">
+        <v>1004</v>
+      </c>
+      <c r="G610" s="1" t="s">
+        <v>1005</v>
       </c>
     </row>
   </sheetData>
@@ -6943,12 +7118,12 @@
     <hyperlink ref="F130" r:id="rId14" xr:uid="{93472772-CF6C-D045-B634-2D574A3EE034}"/>
     <hyperlink ref="E226" r:id="rId15" xr:uid="{F91B4647-0CF3-1D4E-BC20-56E6AEBE70E0}"/>
     <hyperlink ref="F227" r:id="rId16" xr:uid="{2554F581-5597-194D-9C01-DD28DA8905CB}"/>
-    <hyperlink ref="D273" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
-    <hyperlink ref="D274" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
+    <hyperlink ref="D284" r:id="rId17" xr:uid="{A581FA90-25A3-C746-B703-AD2E44558A29}"/>
+    <hyperlink ref="D285" r:id="rId18" xr:uid="{B0BA48BD-8E0E-C444-A248-FBE2F1010B1C}"/>
     <hyperlink ref="F131" r:id="rId19" xr:uid="{92BE3560-5393-C545-9D2D-2B773359B28F}"/>
-    <hyperlink ref="E290" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
-    <hyperlink ref="E291" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
-    <hyperlink ref="E292" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
+    <hyperlink ref="E301" r:id="rId20" xr:uid="{7FD08787-2C60-C444-A72D-A400BA149236}"/>
+    <hyperlink ref="E302" r:id="rId21" xr:uid="{1425A86D-F799-AE43-8F48-AB9342684FDE}"/>
+    <hyperlink ref="E303" r:id="rId22" xr:uid="{58120A51-3D68-C948-B7E2-68D54080E3E3}"/>
     <hyperlink ref="E105" r:id="rId23" xr:uid="{1526D7DA-27DA-1443-928C-BEDA9E425734}"/>
     <hyperlink ref="E106" r:id="rId24" xr:uid="{4F363062-BE49-AB4F-8956-2C1F31D9B898}"/>
     <hyperlink ref="H132" r:id="rId25" xr:uid="{D9E13355-D59B-054F-B544-34A5A285A9E0}"/>
@@ -6965,7 +7140,7 @@
     <hyperlink ref="I132" r:id="rId36" xr:uid="{A03C56E4-1156-A148-A568-F50A5C33DB5C}"/>
     <hyperlink ref="F141" r:id="rId37" xr:uid="{12AC219C-4678-4E43-B328-6595FA10B8D3}"/>
     <hyperlink ref="E143" r:id="rId38" xr:uid="{44409621-28A2-704A-B283-3DCE1EFB1603}"/>
-    <hyperlink ref="E296" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
+    <hyperlink ref="E307" r:id="rId39" xr:uid="{B0EF938C-2A20-B147-87B7-179A63BDBE41}"/>
     <hyperlink ref="F144" r:id="rId40" xr:uid="{A9D0D792-87D1-8144-872F-5CA060D3C28F}"/>
     <hyperlink ref="F145" r:id="rId41" xr:uid="{87EF989D-17E9-1E45-A075-CD862D0B60F4}"/>
     <hyperlink ref="F147" r:id="rId42" xr:uid="{8406C6F0-DC69-A64D-AAD8-60A33C12D00B}"/>
@@ -6975,68 +7150,68 @@
     <hyperlink ref="F152" r:id="rId46" xr:uid="{3D1C62DB-D9B7-BE42-B21D-4EEBC4C9EFE1}"/>
     <hyperlink ref="F153" r:id="rId47" xr:uid="{F5021A21-70A2-D34E-B055-64CAC326E7EF}"/>
     <hyperlink ref="F154" r:id="rId48" xr:uid="{A8C010A1-8EE1-264B-8688-3BEA1B62E535}"/>
-    <hyperlink ref="E297" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
+    <hyperlink ref="E308" r:id="rId49" xr:uid="{B22E0CAC-5E5B-EF42-AF55-F4D92AFD880F}"/>
     <hyperlink ref="F149" r:id="rId50" location="113521" xr:uid="{EE1413C5-3B38-7D4D-8DF1-634A12F0BD81}"/>
     <hyperlink ref="E107" r:id="rId51" xr:uid="{00B1EF4A-7791-0343-8D8C-9A1E83248FC9}"/>
-    <hyperlink ref="E358" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
-    <hyperlink ref="E359" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
+    <hyperlink ref="E369" r:id="rId52" xr:uid="{78EA2D8D-2A85-F646-B486-2D6FD86F3AC2}"/>
+    <hyperlink ref="E370" r:id="rId53" xr:uid="{7FFACFDF-9304-EB4D-AC90-53DF595E17F9}"/>
     <hyperlink ref="F156" r:id="rId54" xr:uid="{40A4B6A0-2F7E-A84D-8CC6-D814A33F5953}"/>
-    <hyperlink ref="E298" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
-    <hyperlink ref="E299" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
-    <hyperlink ref="E300" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
-    <hyperlink ref="E301" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
-    <hyperlink ref="E360" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
-    <hyperlink ref="D275" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
-    <hyperlink ref="D276" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
-    <hyperlink ref="D277" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
-    <hyperlink ref="E302" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
-    <hyperlink ref="E361" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
-    <hyperlink ref="E362" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
-    <hyperlink ref="E364" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
-    <hyperlink ref="E365" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
-    <hyperlink ref="F359" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
-    <hyperlink ref="G359" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
-    <hyperlink ref="E366" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
-    <hyperlink ref="E367" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
-    <hyperlink ref="E368" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
+    <hyperlink ref="E309" r:id="rId55" location="8_Filter_logs_based_on_Process_PID" xr:uid="{597310EA-3F55-5F43-BD43-95DE67A650ED}"/>
+    <hyperlink ref="E310" r:id="rId56" xr:uid="{B415D34D-5EF3-DF40-859C-A4167A61D802}"/>
+    <hyperlink ref="E311" r:id="rId57" xr:uid="{46A9346F-E40B-5D44-8D4D-FA7813E3F7EC}"/>
+    <hyperlink ref="E312" r:id="rId58" xr:uid="{74ED29B8-C650-C74C-98E8-B6AF0449E59B}"/>
+    <hyperlink ref="E371" r:id="rId59" xr:uid="{E79F241F-0BC1-1945-920A-4C9939ACE2BF}"/>
+    <hyperlink ref="D286" r:id="rId60" xr:uid="{DE7521C2-CC92-CA44-830F-F0BFF8B241F9}"/>
+    <hyperlink ref="D287" r:id="rId61" xr:uid="{F8F40386-14A0-8E44-9CE7-818879790B33}"/>
+    <hyperlink ref="D288" r:id="rId62" xr:uid="{CDF21BC4-2C17-9743-B9E4-AF7A1F54F332}"/>
+    <hyperlink ref="E313" r:id="rId63" xr:uid="{CBF40FC5-771F-824A-BB09-7F814B4C8592}"/>
+    <hyperlink ref="E372" r:id="rId64" xr:uid="{030B8CC6-7764-EB4D-83CC-DF52547F6085}"/>
+    <hyperlink ref="E373" r:id="rId65" xr:uid="{06E0F6AC-303A-4641-B502-29E15511E767}"/>
+    <hyperlink ref="E375" r:id="rId66" xr:uid="{431626B3-ABD9-2E48-A9A1-32C4FAAABF09}"/>
+    <hyperlink ref="E376" r:id="rId67" xr:uid="{92EF1FB5-D61B-F143-93C1-3673A0527D53}"/>
+    <hyperlink ref="F370" r:id="rId68" xr:uid="{2089F98F-21D4-1C4B-8E91-3D882F3A3857}"/>
+    <hyperlink ref="G370" r:id="rId69" xr:uid="{B216A770-FD13-A947-8A0D-5C17D8D3FA09}"/>
+    <hyperlink ref="E377" r:id="rId70" xr:uid="{7B92AF17-947F-3F44-9353-C8EE50F88988}"/>
+    <hyperlink ref="E378" r:id="rId71" xr:uid="{CAEC0942-93EC-384F-8253-16C124888753}"/>
+    <hyperlink ref="E379" r:id="rId72" xr:uid="{78CF3156-49D0-BE4D-A33A-AAA08CCCC01F}"/>
     <hyperlink ref="E228" r:id="rId73" xr:uid="{1997C012-A8A9-184A-85E2-9DAE23299CD7}"/>
-    <hyperlink ref="E363" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
-    <hyperlink ref="E369" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
-    <hyperlink ref="E370" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
+    <hyperlink ref="E374" r:id="rId74" xr:uid="{63CDF3C0-95DB-3F42-A0EC-748DD0B7FAC3}"/>
+    <hyperlink ref="E380" r:id="rId75" xr:uid="{59A66FC8-468B-A744-844F-5B4E1034BAB6}"/>
+    <hyperlink ref="E381" r:id="rId76" xr:uid="{CC6D1845-66DF-A94C-ABE1-A45EEECC0651}"/>
     <hyperlink ref="E109" r:id="rId77" location="code" xr:uid="{C0475FF8-517D-E949-887E-9A42D86E9640}"/>
-    <hyperlink ref="E372" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
+    <hyperlink ref="E383" r:id="rId78" xr:uid="{5983A4CF-9C88-AB45-B871-23797665F595}"/>
     <hyperlink ref="E110" r:id="rId79" xr:uid="{277DBE6F-F3E5-8B4C-8DD8-BD92445D1A99}"/>
-    <hyperlink ref="E374" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
-    <hyperlink ref="E379" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
-    <hyperlink ref="E281" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
-    <hyperlink ref="E282" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
+    <hyperlink ref="E385" r:id="rId80" xr:uid="{0A427868-1D44-D94E-B54A-11B9BA22A3EB}"/>
+    <hyperlink ref="E390" r:id="rId81" location="alias-patterns" xr:uid="{9A4B2195-DE80-AF47-AACD-550CFB45D23E}"/>
+    <hyperlink ref="E292" r:id="rId82" xr:uid="{087C5A65-D06D-C645-A353-FA506CC8DE4C}"/>
+    <hyperlink ref="E293" r:id="rId83" xr:uid="{ADD5E36A-5A9A-C544-B034-0F0FAD4830CB}"/>
     <hyperlink ref="F177" r:id="rId84" xr:uid="{EB604865-A16B-0646-A5B5-0D047467449D}"/>
-    <hyperlink ref="E304" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
-    <hyperlink ref="D388" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
-    <hyperlink ref="D389" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
-    <hyperlink ref="E398" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
-    <hyperlink ref="E399" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
-    <hyperlink ref="E397" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
-    <hyperlink ref="D408" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
-    <hyperlink ref="E414" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
-    <hyperlink ref="E411" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
-    <hyperlink ref="E415" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
-    <hyperlink ref="F406" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
-    <hyperlink ref="F407" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
-    <hyperlink ref="E409" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
-    <hyperlink ref="G411" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
-    <hyperlink ref="D424" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
-    <hyperlink ref="E416" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
-    <hyperlink ref="E419" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
-    <hyperlink ref="E418" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
-    <hyperlink ref="F323" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
-    <hyperlink ref="E324" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
-    <hyperlink ref="E325" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
-    <hyperlink ref="E326" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
-    <hyperlink ref="G340" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
-    <hyperlink ref="E335" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
-    <hyperlink ref="E336" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
-    <hyperlink ref="E341" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
+    <hyperlink ref="E315" r:id="rId85" xr:uid="{C3B6CF3C-D7F9-0949-BFA0-2820BB4EA4F3}"/>
+    <hyperlink ref="D399" r:id="rId86" xr:uid="{E90D6A40-E049-224F-9B6F-92C982AB4598}"/>
+    <hyperlink ref="D400" r:id="rId87" xr:uid="{0CBD599B-154F-0442-AA4F-3E4A1A51CC20}"/>
+    <hyperlink ref="E409" r:id="rId88" xr:uid="{6B5798A9-1903-AC43-AE3C-B2C06FDAA31A}"/>
+    <hyperlink ref="E410" r:id="rId89" xr:uid="{A7AC8A25-E374-E646-BCC1-E7D509173590}"/>
+    <hyperlink ref="E408" r:id="rId90" xr:uid="{8E9DFB03-D262-8047-8E71-3664BB185B02}"/>
+    <hyperlink ref="D419" r:id="rId91" xr:uid="{86BA74B9-9447-B942-8D74-17CC766530C2}"/>
+    <hyperlink ref="E425" r:id="rId92" xr:uid="{B5A4937F-2803-CC44-B17D-484692F431C1}"/>
+    <hyperlink ref="E422" r:id="rId93" xr:uid="{CE2EB753-2604-2145-BBD0-28C93B556411}"/>
+    <hyperlink ref="E426" r:id="rId94" xr:uid="{50DDECA1-6EA9-2F41-B5F7-FFEB65F19975}"/>
+    <hyperlink ref="F417" r:id="rId95" xr:uid="{2FB22EF1-C52A-AF46-AB86-8BD5853A6661}"/>
+    <hyperlink ref="F418" r:id="rId96" xr:uid="{D681D68E-84D2-2E47-B599-6A72961CB40F}"/>
+    <hyperlink ref="E420" r:id="rId97" xr:uid="{D6092947-1364-2044-ABB7-1A5F87CF08A8}"/>
+    <hyperlink ref="G422" r:id="rId98" location="c73492" xr:uid="{62D2C7A0-B7CF-4149-8055-EE4F1D0EE26A}"/>
+    <hyperlink ref="D435" r:id="rId99" xr:uid="{531449FE-9611-A143-8841-2F1B1481D831}"/>
+    <hyperlink ref="E427" r:id="rId100" xr:uid="{4624033D-1E3B-BF44-8FB9-F88DD732DEEC}"/>
+    <hyperlink ref="E430" r:id="rId101" xr:uid="{035C43FB-6870-1647-B7E5-9140D3A07CCE}"/>
+    <hyperlink ref="E429" r:id="rId102" location="code" xr:uid="{7507BB17-AD8C-5E4F-A9F8-6E5B97D851BD}"/>
+    <hyperlink ref="F334" r:id="rId103" xr:uid="{BE613991-D925-EE42-B6F2-7690DBF8D142}"/>
+    <hyperlink ref="E335" r:id="rId104" xr:uid="{5B21BD82-8098-6743-A1B2-845BB63A09E2}"/>
+    <hyperlink ref="E336" r:id="rId105" xr:uid="{1527914A-C192-8445-ABE4-02C0DB94E69C}"/>
+    <hyperlink ref="E337" r:id="rId106" xr:uid="{F54C5FD1-ABC1-DB45-AE49-F4B533BA9D06}"/>
+    <hyperlink ref="G351" r:id="rId107" xr:uid="{20C9805E-DEDD-5F4A-8407-D1089BA03BAD}"/>
+    <hyperlink ref="E346" r:id="rId108" xr:uid="{00970AB1-294E-9848-A353-1DDB13A7A479}"/>
+    <hyperlink ref="E347" r:id="rId109" xr:uid="{F03E7AFF-1A5F-2F44-91D0-5BFA97D26508}"/>
+    <hyperlink ref="E352" r:id="rId110" location="set-up-authentication" xr:uid="{2587E339-DB7B-DD4E-AE36-A2BFED7C7CB8}"/>
     <hyperlink ref="F189" r:id="rId111" xr:uid="{D7610A53-EE58-6E4E-8FFA-DB9620A43569}"/>
     <hyperlink ref="F194" r:id="rId112" xr:uid="{0206C9A9-91F9-C24E-8F80-6D63D5D37F07}"/>
     <hyperlink ref="F195" r:id="rId113" xr:uid="{3326350E-5904-7C46-A8F8-6A33B27DA548}"/>
@@ -7046,26 +7221,26 @@
     <hyperlink ref="F209" r:id="rId117" xr:uid="{8D4681E8-2CC3-6747-85F6-48B1F67AA35B}"/>
     <hyperlink ref="F203" r:id="rId118" xr:uid="{A0936DFE-E4CE-E449-A124-685EBE191DAC}"/>
     <hyperlink ref="F212" r:id="rId119" xr:uid="{60A137D0-788D-B249-8D4E-F2130D4FFB68}"/>
-    <hyperlink ref="H319" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
-    <hyperlink ref="F431" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
-    <hyperlink ref="G445" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
-    <hyperlink ref="F432" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
-    <hyperlink ref="G447" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
-    <hyperlink ref="G449" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
-    <hyperlink ref="G452" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
-    <hyperlink ref="G456" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
-    <hyperlink ref="G481" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
-    <hyperlink ref="G479" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
-    <hyperlink ref="G484" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
-    <hyperlink ref="G490" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
-    <hyperlink ref="G494" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
-    <hyperlink ref="G507" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
-    <hyperlink ref="G512" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
-    <hyperlink ref="G537" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
+    <hyperlink ref="H330" r:id="rId120" xr:uid="{4651B684-1FC8-5C4A-A36B-A7509BAE7E90}"/>
+    <hyperlink ref="F442" r:id="rId121" xr:uid="{E9B3D7B3-21DC-C745-B0AC-9E8D4325FC05}"/>
+    <hyperlink ref="G456" r:id="rId122" xr:uid="{D6CE76A4-9A97-C94D-BFDA-64BA5E68B101}"/>
+    <hyperlink ref="F443" r:id="rId123" xr:uid="{831CBC54-62BE-7043-A7BF-ADCD10752065}"/>
+    <hyperlink ref="G458" r:id="rId124" xr:uid="{BCB4B9B8-090E-FE4B-AC0B-EE41FAEB20F9}"/>
+    <hyperlink ref="G460" r:id="rId125" xr:uid="{CDCD658F-CA25-EB41-8E58-A4FCF0D2A231}"/>
+    <hyperlink ref="G463" r:id="rId126" xr:uid="{54185267-32F5-7348-A3C3-E36B7E2EA896}"/>
+    <hyperlink ref="G467" r:id="rId127" xr:uid="{657F690C-B54C-EA4B-B127-9E82D392DC93}"/>
+    <hyperlink ref="G492" r:id="rId128" xr:uid="{40F672C4-35DD-CC44-8C20-BB57B801AAD4}"/>
+    <hyperlink ref="G490" r:id="rId129" xr:uid="{23D42B80-CE35-7A4B-AD00-A35F8544B26E}"/>
+    <hyperlink ref="G495" r:id="rId130" xr:uid="{2913A053-F276-E841-A9EA-8E285DCBF0F2}"/>
+    <hyperlink ref="G501" r:id="rId131" xr:uid="{170379E3-F619-EF40-8400-EB0EF3D9614F}"/>
+    <hyperlink ref="G505" r:id="rId132" xr:uid="{2A5CE97D-8251-C849-9FD3-19396032C503}"/>
+    <hyperlink ref="G518" r:id="rId133" xr:uid="{91F38F45-D8F8-2746-A541-3BFE857169D4}"/>
+    <hyperlink ref="G523" r:id="rId134" xr:uid="{F481A3CC-6E3F-B947-8A09-84DB3DBF7E7F}"/>
+    <hyperlink ref="G548" r:id="rId135" xr:uid="{13F6E18F-E7C0-264C-B483-9DEE07F0BCB2}"/>
     <hyperlink ref="E36" r:id="rId136" xr:uid="{809CA2D1-39E9-0045-A4DF-E4C0C2E97FA2}"/>
     <hyperlink ref="E37" r:id="rId137" xr:uid="{5DC44543-F2B9-F841-9097-6DB19C5EBD82}"/>
-    <hyperlink ref="G522" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
-    <hyperlink ref="G496" r:id="rId139" xr:uid="{7F4EA1D7-8774-1A4B-BF25-18ED0416CB20}"/>
+    <hyperlink ref="G533" r:id="rId138" xr:uid="{15CD079D-88D8-904E-9944-491A0BC2BA17}"/>
+    <hyperlink ref="G507" r:id="rId139" xr:uid="{7F4EA1D7-8774-1A4B-BF25-18ED0416CB20}"/>
     <hyperlink ref="F253" r:id="rId140" xr:uid="{101513F3-87A1-DA41-8BF5-E4029309ECB8}"/>
     <hyperlink ref="F232" r:id="rId141" xr:uid="{494E255E-6912-8643-B5CD-1D65E0DDCFFC}"/>
     <hyperlink ref="F233" r:id="rId142" xr:uid="{828F749D-83DE-C14E-B637-56047AC1B384}"/>
@@ -7073,50 +7248,104 @@
     <hyperlink ref="F255" r:id="rId144" xr:uid="{7D905409-0097-E04E-9593-2DEEBEEA0D0F}"/>
     <hyperlink ref="F181" r:id="rId145" xr:uid="{64451146-E88A-9A47-9888-71BEAC8B984E}"/>
     <hyperlink ref="F243" r:id="rId146" xr:uid="{28F6BA28-EB9B-374C-A8A0-4077C800D23A}"/>
-    <hyperlink ref="G464" r:id="rId147" xr:uid="{20B4F69E-7592-784A-8C2E-123726A51D93}"/>
+    <hyperlink ref="G475" r:id="rId147" xr:uid="{20B4F69E-7592-784A-8C2E-123726A51D93}"/>
     <hyperlink ref="F246" r:id="rId148" xr:uid="{E3C3D7C6-1E6E-FF40-8CC7-6CF1C77457E4}"/>
-    <hyperlink ref="G544" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
+    <hyperlink ref="G555" r:id="rId149" xr:uid="{3DA141F6-ED95-8E4B-9243-375C0C154952}"/>
     <hyperlink ref="G202" r:id="rId150" xr:uid="{9BECD448-C575-B64B-BA3F-BEE8D1CBBD43}"/>
-    <hyperlink ref="G550" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
-    <hyperlink ref="G551" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
-    <hyperlink ref="G552" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
-    <hyperlink ref="G555" r:id="rId154" xr:uid="{FB93E0B8-2537-FD47-8420-84D2A706F697}"/>
-    <hyperlink ref="G556" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
+    <hyperlink ref="G561" r:id="rId151" xr:uid="{649A3CE6-B889-BD4A-8FAF-8C85BFAA8971}"/>
+    <hyperlink ref="G562" r:id="rId152" xr:uid="{F4CA207C-0C61-8B47-9909-BA7F05082D4C}"/>
+    <hyperlink ref="G563" r:id="rId153" xr:uid="{2F5075DF-B3E0-E14C-825C-84931B35E0B4}"/>
+    <hyperlink ref="G566" r:id="rId154" xr:uid="{FB93E0B8-2537-FD47-8420-84D2A706F697}"/>
+    <hyperlink ref="G567" r:id="rId155" xr:uid="{F0B001DD-A90F-9646-8761-71407B9588B8}"/>
     <hyperlink ref="F215" r:id="rId156" location="2116892" xr:uid="{FF1C16E6-B146-B548-B694-396AC9D0B975}"/>
     <hyperlink ref="G200" r:id="rId157" xr:uid="{ED09A21C-0057-1146-8BFF-213A32FC88DF}"/>
-    <hyperlink ref="G468" r:id="rId158" xr:uid="{F933A5C4-6DD5-5547-8BB3-B5D3FBA7A852}"/>
-    <hyperlink ref="G561" r:id="rId159" location=".YLoDxOvTXX8" xr:uid="{8886E3AC-3A64-6449-A070-17D95B586F83}"/>
+    <hyperlink ref="G479" r:id="rId158" xr:uid="{F933A5C4-6DD5-5547-8BB3-B5D3FBA7A852}"/>
+    <hyperlink ref="G572" r:id="rId159" location=".YLoDxOvTXX8" xr:uid="{8886E3AC-3A64-6449-A070-17D95B586F83}"/>
     <hyperlink ref="F218" r:id="rId160" xr:uid="{5140C3EB-4DFC-5A4A-9C02-C2EBFA052A41}"/>
     <hyperlink ref="F29" r:id="rId161" xr:uid="{99992829-3CC1-2B43-BA73-7F09EAA955A4}"/>
-    <hyperlink ref="G499" r:id="rId162" xr:uid="{01E9516A-34A1-6D40-BED9-61916E777090}"/>
-    <hyperlink ref="H526" r:id="rId163" xr:uid="{D3C22B64-1D55-1D47-8F15-25C4AA3D5B90}"/>
-    <hyperlink ref="G528" r:id="rId164" xr:uid="{8E28D310-73EF-1C47-A666-DEE78634BFDF}"/>
-    <hyperlink ref="H525" r:id="rId165" xr:uid="{66476745-9FC4-9E4B-952E-C3E33F678E5D}"/>
-    <hyperlink ref="G564" r:id="rId166" xr:uid="{04D185B2-C246-8B4F-8813-F5A12B741A26}"/>
-    <hyperlink ref="G574" r:id="rId167" xr:uid="{D89D9875-8DF0-3044-BF56-09B8E52D068E}"/>
-    <hyperlink ref="G501" r:id="rId168" xr:uid="{951EA3E4-9D93-CC44-96EE-1FAB3FE8B169}"/>
+    <hyperlink ref="G510" r:id="rId162" xr:uid="{01E9516A-34A1-6D40-BED9-61916E777090}"/>
+    <hyperlink ref="H537" r:id="rId163" xr:uid="{D3C22B64-1D55-1D47-8F15-25C4AA3D5B90}"/>
+    <hyperlink ref="G539" r:id="rId164" xr:uid="{8E28D310-73EF-1C47-A666-DEE78634BFDF}"/>
+    <hyperlink ref="H536" r:id="rId165" xr:uid="{66476745-9FC4-9E4B-952E-C3E33F678E5D}"/>
+    <hyperlink ref="G575" r:id="rId166" xr:uid="{04D185B2-C246-8B4F-8813-F5A12B741A26}"/>
+    <hyperlink ref="G585" r:id="rId167" xr:uid="{D89D9875-8DF0-3044-BF56-09B8E52D068E}"/>
+    <hyperlink ref="G512" r:id="rId168" xr:uid="{951EA3E4-9D93-CC44-96EE-1FAB3FE8B169}"/>
     <hyperlink ref="F32" r:id="rId169" xr:uid="{A2E3FF8D-D95C-A149-813C-65DD0F6ADE93}"/>
-    <hyperlink ref="G503" r:id="rId170" xr:uid="{8D957F13-4686-CB46-B81C-03912C517BD5}"/>
+    <hyperlink ref="G514" r:id="rId170" xr:uid="{8D957F13-4686-CB46-B81C-03912C517BD5}"/>
     <hyperlink ref="F221" r:id="rId171" xr:uid="{01C94714-673D-0E4A-A2BF-59A21207E597}"/>
-    <hyperlink ref="G579" r:id="rId172" xr:uid="{EB9D8B2D-C3FD-5F45-A2EA-DFAAED649D1E}"/>
-    <hyperlink ref="G583" r:id="rId173" xr:uid="{959A5135-36C7-954E-811F-BF84A9FC3E4F}"/>
-    <hyperlink ref="G580" r:id="rId174" xr:uid="{59635D47-1CA8-4B4D-BF2C-6399A8020C4E}"/>
-    <hyperlink ref="F344" r:id="rId175" xr:uid="{DD2C246D-5C95-1645-B391-7EF7D3167AF4}"/>
-    <hyperlink ref="G589" r:id="rId176" xr:uid="{DDFFFCAD-BF74-1D48-AF86-5B31F6DB75DD}"/>
-    <hyperlink ref="G590" r:id="rId177" xr:uid="{6BFF710C-507C-844E-AFBE-9B133475C781}"/>
-    <hyperlink ref="F259" r:id="rId178" xr:uid="{C710D804-CFB3-2F46-9AAE-375A3EC37F04}"/>
+    <hyperlink ref="G590" r:id="rId172" xr:uid="{EB9D8B2D-C3FD-5F45-A2EA-DFAAED649D1E}"/>
+    <hyperlink ref="G594" r:id="rId173" xr:uid="{959A5135-36C7-954E-811F-BF84A9FC3E4F}"/>
+    <hyperlink ref="G591" r:id="rId174" xr:uid="{59635D47-1CA8-4B4D-BF2C-6399A8020C4E}"/>
+    <hyperlink ref="F355" r:id="rId175" xr:uid="{DD2C246D-5C95-1645-B391-7EF7D3167AF4}"/>
+    <hyperlink ref="G600" r:id="rId176" xr:uid="{DDFFFCAD-BF74-1D48-AF86-5B31F6DB75DD}"/>
+    <hyperlink ref="G601" r:id="rId177" xr:uid="{6BFF710C-507C-844E-AFBE-9B133475C781}"/>
+    <hyperlink ref="F270" r:id="rId178" xr:uid="{C710D804-CFB3-2F46-9AAE-375A3EC37F04}"/>
     <hyperlink ref="F235" r:id="rId179" xr:uid="{05F4B29A-A0A0-5444-B283-0B6193A59DB2}"/>
-    <hyperlink ref="G595" r:id="rId180" xr:uid="{1504BD14-5428-4E4B-A4D1-F56A3711952B}"/>
+    <hyperlink ref="G606" r:id="rId180" xr:uid="{1504BD14-5428-4E4B-A4D1-F56A3711952B}"/>
+    <hyperlink ref="H469" r:id="rId181" xr:uid="{0977EE18-6440-3C43-BBA1-304B1B20C07F}"/>
+    <hyperlink ref="G609" r:id="rId182" xr:uid="{15A18F7D-EC19-BE45-BC7A-C687D7DEF78E}"/>
+    <hyperlink ref="G610" r:id="rId183" xr:uid="{B5691172-9ECD-AB4B-85E2-E85152A59B95}"/>
+    <hyperlink ref="F257" r:id="rId184" xr:uid="{536DC379-2D75-944E-9F45-7EA99700958C}"/>
+    <hyperlink ref="F259" r:id="rId185" xr:uid="{C5480CD8-1423-CE42-A49E-85683A2BB759}"/>
+    <hyperlink ref="F262" r:id="rId186" xr:uid="{4FBC6415-B8E7-704D-8D4B-AF605D75514A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C546159-CB90-4141-B53C-C9065786FB56}">
+  <dimension ref="B2:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{6074E5E0-EF55-1A40-B793-F1FA926B2174}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{9377A784-A8C2-FA4A-87AA-A7606D580B5F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
   <dimension ref="B2:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
@@ -7976,7 +8205,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0197339E-8847-2643-B704-6685D2B6003F}">
   <dimension ref="B2:E2"/>
   <sheetViews>
@@ -8009,7 +8238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069EEB69-0D57-C040-8545-840D5862E858}">
   <dimension ref="B2:D32"/>
   <sheetViews>
@@ -8183,12 +8412,50 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9928DD2B-0E52-0541-9E14-AF63C29120ED}">
-  <dimension ref="B2:D13"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DA0B776-BFAF-A24A-9DE9-FDDB22250009}">
+  <dimension ref="B3:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{FE66197A-41FB-804D-8AF9-7235C5734A87}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{E05B4524-5693-7042-89B8-167D92DF73E2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9928DD2B-0E52-0541-9E14-AF63C29120ED}">
+  <dimension ref="B2:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8233,18 +8500,31 @@
         <v>976</v>
       </c>
     </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>997</v>
+      </c>
+      <c r="D10" t="s">
+        <v>996</v>
+      </c>
+    </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+      <c r="D11" s="1" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>981</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
         <v>983</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D13" s="1" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D21" s="1" t="s">
         <v>982</v>
       </c>
     </row>
@@ -8253,7 +8533,8 @@
     <hyperlink ref="D4" r:id="rId1" xr:uid="{87406F13-D2B8-4945-8826-741A2ED58F0A}"/>
     <hyperlink ref="D5" r:id="rId2" display="https://www.senseye.io/hubfs/Starter_Packs_brochure_final.pdf?utm_campaign=Senseye%20PdM%20Starter%20Pack%20Launch&amp;utm_medium=email&amp;_hsmi=133877864&amp;_hsenc=p2ANqtz-82eqB84CbmqoZdOE4FsvoB88ghkbptGuYpRAUjAhIuCzxwXyD2U8qfhq4-zBNbjWJ7X7Lf-hR0SB-eotWyFCG2J42lIphISeyTDi7r__N961fhx0g&amp;utm_content=133877864&amp;utm_source=hs_automation" xr:uid="{F586B172-2D6E-714E-8E2D-8B7F048EF627}"/>
     <hyperlink ref="D8" r:id="rId3" xr:uid="{BA4CB187-A8E6-6146-8132-987D175D6FB7}"/>
-    <hyperlink ref="D13" r:id="rId4" xr:uid="{8BDCC0FC-F5DF-2142-9AD2-AC87EBC32887}"/>
+    <hyperlink ref="D21" r:id="rId4" xr:uid="{8BDCC0FC-F5DF-2142-9AD2-AC87EBC32887}"/>
+    <hyperlink ref="D11" r:id="rId5" xr:uid="{CE3E2EAD-3377-924C-8458-0EE71FF97863}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for pandas
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07EEFFC-ADC3-0F46-A62C-9AD652B1A4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277BA3E0-6E4B-914D-A67B-D91D8ED8C135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="1033">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="1036">
   <si>
     <t>docker</t>
   </si>
@@ -3143,6 +3143,15 @@
   </si>
   <si>
     <t>https://www.w3schools.com/sql/sql_orderby.asp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set dataframe index name </t>
+  </si>
+  <si>
+    <t>df.index = df.index.set_names(['foo'])</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/40914200/can-i-assign-a-reset-index-a-name</t>
   </si>
 </sst>
 </file>
@@ -3607,8 +3616,8 @@
   <dimension ref="B1:I613"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A543" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G565" sqref="G565"/>
+      <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E267" sqref="E267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5262,6 +5271,17 @@
       </c>
       <c r="F262" s="1" t="s">
         <v>1019</v>
+      </c>
+    </row>
+    <row r="263" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C263" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D263" t="s">
+        <v>1034</v>
+      </c>
+      <c r="F263" s="1" t="s">
+        <v>1035</v>
       </c>
     </row>
     <row r="269" spans="2:6" x14ac:dyDescent="0.2">
@@ -7327,6 +7347,7 @@
     <hyperlink ref="F259" r:id="rId185" xr:uid="{C5480CD8-1423-CE42-A49E-85683A2BB759}"/>
     <hyperlink ref="F262" r:id="rId186" xr:uid="{4FBC6415-B8E7-704D-8D4B-AF605D75514A}"/>
     <hyperlink ref="G564" r:id="rId187" xr:uid="{A1D4F400-6905-AA4B-BD02-F794EBE64730}"/>
+    <hyperlink ref="F263" r:id="rId188" xr:uid="{21B01167-CE07-4147-8370-E31132B70F1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips on excel
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EE3D77-F2EF-8E42-B9CC-A7A8DFA8DB99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B15DA5E-18E8-3141-AC38-8FA09EFEA008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="1049">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="1054">
   <si>
     <t>docker</t>
   </si>
@@ -3191,6 +3191,21 @@
   </si>
   <si>
     <t>https://f.hubspotusercontent40.net/hubfs/3485049/Insight%20brochure.pdf</t>
+  </si>
+  <si>
+    <t>excel</t>
+  </si>
+  <si>
+    <t>weekdays</t>
+  </si>
+  <si>
+    <t>CHOOSE(WEEKDAY(B4),"Sun","Mon","Tue","Wed","Thu","Fri","Sat")</t>
+  </si>
+  <si>
+    <t>https://superuser.com/questions/477385/change-excel-day-name-to-other-languages/477395</t>
+  </si>
+  <si>
+    <t>Change Excel day name to other languages</t>
   </si>
 </sst>
 </file>
@@ -3654,8 +3669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
   <dimension ref="B1:I613"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A401" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A514" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D409" sqref="D409"/>
     </sheetView>
   </sheetViews>
@@ -7442,10 +7457,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G69"/>
+  <dimension ref="B2:G70"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8229,6 +8244,23 @@
       </c>
       <c r="F69" s="1" t="s">
         <v>993</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1050</v>
+      </c>
+      <c r="E70" t="s">
+        <v>1051</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>1052</v>
       </c>
     </row>
   </sheetData>
@@ -8299,6 +8331,7 @@
     <hyperlink ref="F67" r:id="rId64" xr:uid="{617D9CE6-3964-1449-9C40-052E2D590E6C}"/>
     <hyperlink ref="F68" r:id="rId65" xr:uid="{84D99383-F8E9-FB47-9939-D071EBFEC595}"/>
     <hyperlink ref="F69" r:id="rId66" xr:uid="{339043D2-2CCF-D446-9816-25139E0CACB7}"/>
+    <hyperlink ref="F70" r:id="rId67" xr:uid="{9C97F50F-8C04-AE45-917D-B573E2D8ACE4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated with random articles on postgres
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7102B9-AFA5-AC45-88E5-1E5C4987B44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840266DA-CF61-7247-ACEA-A75BF826EB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="13800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="1049">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="1101">
   <si>
     <t>docker</t>
   </si>
@@ -3191,6 +3191,162 @@
   </si>
   <si>
     <t>https://f.hubspotusercontent40.net/hubfs/3485049/Insight%20brochure.pdf</t>
+  </si>
+  <si>
+    <t>https://www.statology.org/matplotlib-rectangle/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How to Draw Rectangles in Matplotlib </t>
+  </si>
+  <si>
+    <t>ax.add_patch(Rectangle((1, 1), 2, 6))</t>
+  </si>
+  <si>
+    <t>Matplotlib</t>
+  </si>
+  <si>
+    <t>f"{1:02d}"</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/134934/display-number-with-leading-zeros</t>
+  </si>
+  <si>
+    <t>Display number with leading zeros</t>
+  </si>
+  <si>
+    <t>https://www.quora.com/What-happens-if-loads-are-unbalanced-in-3-phases</t>
+  </si>
+  <si>
+    <t>What happens if loads are unbalanced in 3 phases?</t>
+  </si>
+  <si>
+    <t>phase imbalance</t>
+  </si>
+  <si>
+    <t>sudo du -h --max-depth=1 /var</t>
+  </si>
+  <si>
+    <t>How to Get the Size of a Directory in Linux</t>
+  </si>
+  <si>
+    <t>https://linuxize.com/post/how-get-size-of-file-directory-linux/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linux </t>
+  </si>
+  <si>
+    <t>du</t>
+  </si>
+  <si>
+    <t>du -sh /* | sort -h</t>
+  </si>
+  <si>
+    <t>https://superuser.com/questions/162749/how-to-get-the-summarized-sizes-of-directories-and-their-subdirectories</t>
+  </si>
+  <si>
+    <t>How to get the summarized sizes of directories and their subdirectories?</t>
+  </si>
+  <si>
+    <t>SELECT sum("diskBytes") FROM "_internal".."tsm1_filestore" WHERE time &gt;= now() - 6h GROUP BY time(30s), "database"</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/52428018/how-to-get-influxdb-measurement-size</t>
+  </si>
+  <si>
+    <t>How to get InfluxDB measurement size?</t>
+  </si>
+  <si>
+    <t>influxdb</t>
+  </si>
+  <si>
+    <t>filesize</t>
+  </si>
+  <si>
+    <t>df.withColumn('time', date_format('datetime', 'HH:mm:ss'))</t>
+  </si>
+  <si>
+    <t>Extract time from timestamp in pyspark</t>
+  </si>
+  <si>
+    <t>pyspark</t>
+  </si>
+  <si>
+    <t>date_format</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/63691162/how-to-extract-time-from-timestamp-in-pyspark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">df.loc[df.groupby(["sp", "mt"])["count"].idxmax()] </t>
+  </si>
+  <si>
+    <t>.idxmax()</t>
+  </si>
+  <si>
+    <t>Get the row(s) which have the max value in groups using groupby</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/15705630/get-the-rows-which-have-the-max-value-in-groups-using-groupby</t>
+  </si>
+  <si>
+    <t>Spark Dataframe :How to add a index Column</t>
+  </si>
+  <si>
+    <t>df.withColumn("id",monotonicallyIncreasingId)</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/43406887/spark-dataframe-how-to-add-a-index-column-aka-distributed-data-index</t>
+  </si>
+  <si>
+    <t>monotonicallyIncreasingId</t>
+  </si>
+  <si>
+    <t>https://community.grafana.com/t/bar-gauge-how-to-show-series-name-from-a-querys-row-value-mysql/17809/14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$__cell_0 </t>
+  </si>
+  <si>
+    <t>PostgresQL query, show series name from cell value (note: one underscore after cell)</t>
+  </si>
+  <si>
+    <t>Query failed when aggregating: operator does not exist: uuid = text</t>
+  </si>
+  <si>
+    <t>postgres</t>
+  </si>
+  <si>
+    <t>grafana</t>
+  </si>
+  <si>
+    <t>WHERE (("_0_root.base"."id") = ("sesi_id")::uuid) )</t>
+  </si>
+  <si>
+    <t>https://github.com/hasura/graphql-engine/issues/2041</t>
+  </si>
+  <si>
+    <t>select * from (values('foo','bar','fooBar')) s(a,b,c);</t>
+  </si>
+  <si>
+    <t>Select hardcoded values without table</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/15948614/select-hardcoded-values-without-table/15948727</t>
+  </si>
+  <si>
+    <t>ax.set_xticklabels</t>
+  </si>
+  <si>
+    <t>Date axis in heatmap seaborn</t>
+  </si>
+  <si>
+    <t>Online tools</t>
+  </si>
+  <si>
+    <t>Epoch Converter</t>
+  </si>
+  <si>
+    <t>https://www.epochconverter.com</t>
   </si>
 </sst>
 </file>
@@ -3652,11 +3808,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I613"/>
+  <dimension ref="B1:I617"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A404" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D409" sqref="D409"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A598" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G618" sqref="G618"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5977,6 +6133,17 @@
         <v>340</v>
       </c>
     </row>
+    <row r="391" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C391" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D391" t="s">
+        <v>1086</v>
+      </c>
+      <c r="E391" s="1" t="s">
+        <v>1085</v>
+      </c>
+    </row>
     <row r="396" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B396" t="s">
         <v>85</v>
@@ -7195,6 +7362,19 @@
       </c>
       <c r="G613" s="1" t="s">
         <v>1005</v>
+      </c>
+    </row>
+    <row r="616" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B616" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="617" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C617" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G617" s="1" t="s">
+        <v>1100</v>
       </c>
     </row>
   </sheetData>
@@ -7387,6 +7567,8 @@
     <hyperlink ref="F262" r:id="rId186" xr:uid="{4FBC6415-B8E7-704D-8D4B-AF605D75514A}"/>
     <hyperlink ref="G564" r:id="rId187" xr:uid="{A1D4F400-6905-AA4B-BD02-F794EBE64730}"/>
     <hyperlink ref="F263" r:id="rId188" xr:uid="{21B01167-CE07-4147-8370-E31132B70F1F}"/>
+    <hyperlink ref="E391" r:id="rId189" xr:uid="{6D3F9FEF-F197-1A45-8D75-0B7C56B3031F}"/>
+    <hyperlink ref="G617" r:id="rId190" xr:uid="{87985A53-CC6B-9044-8BA8-C1AD329C2A47}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7442,10 +7624,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G69"/>
+  <dimension ref="B2:G81"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8229,6 +8411,195 @@
       </c>
       <c r="F69" s="1" t="s">
         <v>993</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E70" t="s">
+        <v>1051</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C71" t="s">
+        <v>467</v>
+      </c>
+      <c r="E71" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1058</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D73" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E73" t="s">
+        <v>1059</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E74" t="s">
+        <v>1064</v>
+      </c>
+      <c r="F74" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D75" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E75" t="s">
+        <v>1067</v>
+      </c>
+      <c r="F75" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C76" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D76" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E76" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D77" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E77" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C78" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D78" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E78" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D79" t="s">
+        <v>1090</v>
+      </c>
+      <c r="E79" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B80" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D80" t="s">
+        <v>1090</v>
+      </c>
+      <c r="E80" t="s">
+        <v>1093</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C81" t="s">
+        <v>467</v>
+      </c>
+      <c r="D81" t="s">
+        <v>962</v>
+      </c>
+      <c r="E81" t="s">
+        <v>1096</v>
       </c>
     </row>
   </sheetData>
@@ -8299,6 +8670,15 @@
     <hyperlink ref="F67" r:id="rId64" xr:uid="{617D9CE6-3964-1449-9C40-052E2D590E6C}"/>
     <hyperlink ref="F68" r:id="rId65" xr:uid="{84D99383-F8E9-FB47-9939-D071EBFEC595}"/>
     <hyperlink ref="F69" r:id="rId66" xr:uid="{339043D2-2CCF-D446-9816-25139E0CACB7}"/>
+    <hyperlink ref="F70" r:id="rId67" xr:uid="{4C714D52-96BD-F240-89A0-F733608C1B2D}"/>
+    <hyperlink ref="F71" r:id="rId68" xr:uid="{B5A8891C-7156-1B4B-A837-D4FC167EAAAB}"/>
+    <hyperlink ref="F72" r:id="rId69" xr:uid="{A0BCE8B5-0AD3-0644-A190-137160A69157}"/>
+    <hyperlink ref="F73" r:id="rId70" xr:uid="{E6200351-F377-7A4F-8B0A-8E85D96B4A16}"/>
+    <hyperlink ref="F76" r:id="rId71" xr:uid="{35C0D2D3-3E12-4349-B74E-A8B0597D94F4}"/>
+    <hyperlink ref="F77" r:id="rId72" xr:uid="{496160A3-690D-8644-9927-892347F57591}"/>
+    <hyperlink ref="F78" r:id="rId73" xr:uid="{743341AF-D853-634E-B5BE-90CE576C88D3}"/>
+    <hyperlink ref="F79" r:id="rId74" xr:uid="{B2BF3EBF-40A1-0B42-A4B4-C8128749CA5E}"/>
+    <hyperlink ref="F80" r:id="rId75" xr:uid="{E2480C24-834E-CB4A-8CC7-DF9C847C2270}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8571,8 +8951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9928DD2B-0E52-0541-9E14-AF63C29120ED}">
   <dimension ref="B2:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added tips for generating pdf reports
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840266DA-CF61-7247-ACEA-A75BF826EB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B098942-D383-944C-B844-61D3F1AF6D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="13800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="13800" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="1101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="1109">
   <si>
     <t>docker</t>
   </si>
@@ -3347,6 +3347,30 @@
   </si>
   <si>
     <t>https://www.epochconverter.com</t>
+  </si>
+  <si>
+    <t>PDF Report generator - reportlab</t>
+  </si>
+  <si>
+    <t>reportlab</t>
+  </si>
+  <si>
+    <t>https://www.pythonguis.com/examples/python-pdf-report-generator/</t>
+  </si>
+  <si>
+    <t>from PyQt5.QtWidgets import QPushButton, QLineEdit</t>
+  </si>
+  <si>
+    <t>https://pypi.org/project/gilfoyle/</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>gilfoyle</t>
+  </si>
+  <si>
+    <t>Gilfoyle is a report generation tool for Python which makes it quick and easy to create stylish looking reports</t>
   </si>
 </sst>
 </file>
@@ -3810,9 +3834,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
   <dimension ref="B1:I617"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+    <sheetView zoomScale="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A598" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G618" sqref="G618"/>
+      <selection pane="bottomLeft" activeCell="B621" sqref="B621"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7624,10 +7648,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G81"/>
+  <dimension ref="B2:G83"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8588,7 +8612,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>1097</v>
       </c>
@@ -8600,6 +8624,40 @@
       </c>
       <c r="E81" t="s">
         <v>1096</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B82" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C82" t="s">
+        <v>467</v>
+      </c>
+      <c r="D82" t="s">
+        <v>1102</v>
+      </c>
+      <c r="E82" t="s">
+        <v>1104</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B83" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C83" t="s">
+        <v>467</v>
+      </c>
+      <c r="D83" t="s">
+        <v>1107</v>
+      </c>
+      <c r="E83" t="s">
+        <v>1106</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>1105</v>
       </c>
     </row>
   </sheetData>
@@ -8679,6 +8737,8 @@
     <hyperlink ref="F78" r:id="rId73" xr:uid="{743341AF-D853-634E-B5BE-90CE576C88D3}"/>
     <hyperlink ref="F79" r:id="rId74" xr:uid="{B2BF3EBF-40A1-0B42-A4B4-C8128749CA5E}"/>
     <hyperlink ref="F80" r:id="rId75" xr:uid="{E2480C24-834E-CB4A-8CC7-DF9C847C2270}"/>
+    <hyperlink ref="F82" r:id="rId76" xr:uid="{ACF43B1E-D282-BC42-9354-4906649896A3}"/>
+    <hyperlink ref="F83" r:id="rId77" xr:uid="{573870E9-82E2-DA46-8635-94B1ADBB794B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for postgres and grafan and spark
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B098942-D383-944C-B844-61D3F1AF6D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1605CE71-A1A2-474D-8675-53714F5AB945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="13800" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="13800" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="1109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="1172">
   <si>
     <t>docker</t>
   </si>
@@ -3371,6 +3371,197 @@
   </si>
   <si>
     <t>Gilfoyle is a report generation tool for Python which makes it quick and easy to create stylish looking reports</t>
+  </si>
+  <si>
+    <t>Bar Gauge : How to show Series name from a query’s row value (MySQL)?</t>
+  </si>
+  <si>
+    <t>https://community.grafana.com/t/bar-gauge-how-to-show-series-name-from-a-querys-row-value-mysql/17809</t>
+  </si>
+  <si>
+    <t>type $__cell_0 in the Field title template</t>
+  </si>
+  <si>
+    <t>sql</t>
+  </si>
+  <si>
+    <t>DROP TABLE [IF EXISTS] table_name</t>
+  </si>
+  <si>
+    <t>https://www.postgresqltutorial.com/postgresql-drop-table/</t>
+  </si>
+  <si>
+    <t>Posgres Drop Table</t>
+  </si>
+  <si>
+    <t>Division ( / ) not giving my answer in postgresql</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/34504497/division-not-giving-my-answer-in-postgresql</t>
+  </si>
+  <si>
+    <t>select dev_cost::decimal / sell_cost from software ;</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/12147632/padding-a-string-in-postgresql-with-rpad-without-truncating-it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT greatest('foo',rpad('foo', 5));  -- 'foo  ' </t>
+  </si>
+  <si>
+    <t>Padding a string in Postgresql with rpad without truncating it</t>
+  </si>
+  <si>
+    <t>Posgres Union All</t>
+  </si>
+  <si>
+    <t>SELECT * FROM top_rated_films
+UNION ALL
+SELECT * FROM most_popular_films</t>
+  </si>
+  <si>
+    <t>https://www.postgresqltutorial.com/postgresql-union/</t>
+  </si>
+  <si>
+    <t>SELECT * FROM some_measurement WHERE some_tag =~ /a|b|c/</t>
+  </si>
+  <si>
+    <t>Querying for tag values in a given list</t>
+  </si>
+  <si>
+    <t>df.set_index('timestamp').groupby([pd.Grouper(freq='20Min'), 'name']).mean()</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/35898667/group-by-time-and-other-column-in-pandas</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/32063055/querying-for-tag-values-in-a-given-list</t>
+  </si>
+  <si>
+    <t>group by time and other column in pandas</t>
+  </si>
+  <si>
+    <t>The Python Graph Gallery</t>
+  </si>
+  <si>
+    <t>https://www.python-graph-gallery.com</t>
+  </si>
+  <si>
+    <t>graphs</t>
+  </si>
+  <si>
+    <t>pandas.set_option('display.max_rows', None)</t>
+  </si>
+  <si>
+    <t>https://dev.to/chanduthedev/how-to-display-all-rows-from-data-frame-using-pandas-dha</t>
+  </si>
+  <si>
+    <t>How to display all rows from data frame using pandas</t>
+  </si>
+  <si>
+    <t>consumer.topics()</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/36641755/kafka-python-retrieve-the-list-of-topics</t>
+  </si>
+  <si>
+    <t>Kafka-python retrieve the list of topics</t>
+  </si>
+  <si>
+    <t>Get values from first and last row per group</t>
+  </si>
+  <si>
+    <t>first_value(value) over (partition by name order by week)</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/25170215/get-values-from-first-and-last-row-per-group</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/49603073/postgresql-last-value-of-column-while-using-aggregate-functions</t>
+  </si>
+  <si>
+    <t>df.dropDuplicates(['id', 'name']).show()</t>
+  </si>
+  <si>
+    <t>https://towardsdatascience.com/distinct-vs-dropduplicates-in-spark-3e28af1f793c</t>
+  </si>
+  <si>
+    <t>distinct() vs dropDuplicates() in Apache Spark</t>
+  </si>
+  <si>
+    <t>databricks</t>
+  </si>
+  <si>
+    <t>df.groupBy($"KEY", window($"time", "5 minutes")).sum("metric")</t>
+  </si>
+  <si>
+    <t>How to group by time interval in Spark SQL</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/37632238/how-to-group-by-time-interval-in-spark-sql</t>
+  </si>
+  <si>
+    <t>select  'some value' :: TEXT AS field_name;</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/33583034/postgresql-hard-code-string-in-sql</t>
+  </si>
+  <si>
+    <t>PostgreSQL: Hard code string in SQL</t>
+  </si>
+  <si>
+    <t>InfluxDB storage size on disk</t>
+  </si>
+  <si>
+    <t>du -sh /var/lib/influxdb/data/&lt;db name&gt;</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/44454836/influxdb-storage-size-on-disk</t>
+  </si>
+  <si>
+    <t>Forward-fill missing data in Spark</t>
+  </si>
+  <si>
+    <t>filled_column = last(spark_df['temperature'], ignorenulls=True).over(window)</t>
+  </si>
+  <si>
+    <t>https://johnpaton.net/posts/forward-fill-spark/</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/36343482/fill-in-null-with-previously-known-good-value-with-pyspark</t>
+  </si>
+  <si>
+    <t>To check</t>
+  </si>
+  <si>
+    <t>Hashura</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=UmN2_R4KEg8</t>
+  </si>
+  <si>
+    <t>pdf by python</t>
+  </si>
+  <si>
+    <t>https://www.justintodata.com/generate-reports-with-python/</t>
+  </si>
+  <si>
+    <t>https://pbpython.com/pdf-reports.html</t>
+  </si>
+  <si>
+    <t>https://practicaldatascience.co.uk/data-science/how-to-create-pdf-reports-in-python-using-pandas-and-gilfoyle</t>
+  </si>
+  <si>
+    <t>https://towardsdatascience.com/how-to-create-pdf-reports-with-python-the-essential-guide-c08dd3ebf2ee</t>
+  </si>
+  <si>
+    <t>Since Grafana 6.x, panels are ReactJS components.</t>
+  </si>
+  <si>
+    <t>grafana plugin</t>
+  </si>
+  <si>
+    <t>https://grafana.com/tutorials/build-a-panel-plugin/</t>
   </si>
 </sst>
 </file>
@@ -3835,8 +4026,8 @@
   <dimension ref="B1:I617"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A598" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B621" sqref="B621"/>
+      <pane ySplit="1" topLeftCell="A464" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G479" sqref="G479"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7600,10 +7791,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C546159-CB90-4141-B53C-C9065786FB56}">
-  <dimension ref="B2:E5"/>
+  <dimension ref="B2:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7637,10 +7828,76 @@
         <v>1024</v>
       </c>
     </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D13" s="1" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C15" s="1" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C17" s="1" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C19" s="1" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C21" s="1" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D24" s="1" t="s">
+        <v>1171</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" xr:uid="{6074E5E0-EF55-1A40-B793-F1FA926B2174}"/>
     <hyperlink ref="E5" r:id="rId2" xr:uid="{9377A784-A8C2-FA4A-87AA-A7606D580B5F}"/>
+    <hyperlink ref="D13" r:id="rId3" xr:uid="{852FE153-D4B9-D340-8ECE-F9F6ABC32445}"/>
+    <hyperlink ref="C15" r:id="rId4" xr:uid="{E77BF68B-EE92-214C-971F-0FE13F85FF8E}"/>
+    <hyperlink ref="C17" r:id="rId5" xr:uid="{3C28C1C8-0904-FB4F-86C4-D6E3F03C2A99}"/>
+    <hyperlink ref="C19" r:id="rId6" xr:uid="{612DF92D-8E78-124D-BE38-75176D36119D}"/>
+    <hyperlink ref="C21" r:id="rId7" xr:uid="{A434E790-D64D-FD4F-8070-68AB9AA0EF8A}"/>
+    <hyperlink ref="D24" r:id="rId8" xr:uid="{8A7D84DD-A955-E04B-A617-B1DF645998EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7648,1097 +7905,1387 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:G83"/>
+  <dimension ref="C2:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="68.83203125" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
-    <col min="5" max="5" width="55.5" customWidth="1"/>
+    <col min="3" max="3" width="68.83203125" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="6" max="6" width="55.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
+    <row r="2" spans="3:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
         <v>436</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
         <v>399</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>401</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
         <v>402</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
         <v>408</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
         <v>411</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>412</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
         <v>413</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
         <v>426</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>425</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
         <v>428</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
         <v>439</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>438</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>441</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
         <v>442</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>168</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
         <v>445</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>168</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>446</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
         <v>448</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>449</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+    <row r="14" spans="3:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
         <v>452</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>168</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
         <v>454</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
         <v>457</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>168</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>455</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
         <v>458</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
         <v>462</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>168</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>460</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
         <v>463</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>168</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>446</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
         <v>468</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>467</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>446</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
         <v>470</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>446</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
         <v>474</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>168</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>473</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
         <v>477</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>446</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>475</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
         <v>479</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
         <v>531</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>481</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
         <v>530</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>532</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
         <v>535</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>533</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
         <v>537</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>446</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>536</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
         <v>639</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>168</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>640</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
         <v>641</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>642</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="E31" s="2" t="s">
+    <row r="31" spans="3:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="F31" s="2" t="s">
         <v>658</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
         <v>644</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>645</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
         <v>649</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>647</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>648</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>650</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
         <v>652</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>168</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>446</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>653</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="35" spans="2:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
+    <row r="35" spans="3:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
         <v>655</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>657</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
         <v>660</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>662</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
         <v>663</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>446</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>664</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
         <v>666</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>667</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
         <v>669</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>670</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
         <v>673</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
         <v>697</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>168</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>446</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>698</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E42" t="s">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F42" t="s">
         <v>699</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>700</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
         <v>702</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
         <v>715</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
         <v>726</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>725</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
         <v>721</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>717</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
         <v>720</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>718</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
         <v>723</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
         <v>728</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>446</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>729</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
         <v>749</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>750</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>751</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
         <v>738</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>739</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>740</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F53" s="1" t="s">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G53" s="1" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
         <v>762</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>763</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="G54" s="1" t="s">
         <v>764</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
         <v>765</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>467</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>766</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>767</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="G55" s="1" t="s">
         <v>768</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
         <v>889</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>766</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>888</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="G56" s="1" t="s">
         <v>887</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C57" t="s">
         <v>903</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>766</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>904</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="G57" s="1" t="s">
         <v>902</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C58" t="s">
         <v>771</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>467</v>
       </c>
-      <c r="E58" t="s">
+      <c r="F58" t="s">
         <v>769</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="G58" s="1" t="s">
         <v>770</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C59" t="s">
         <v>723</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>772</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="G59" s="1" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B60" t="s">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C60" t="s">
         <v>774</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="G60" s="1" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C61" t="s">
         <v>783</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>781</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="G61" s="1" t="s">
         <v>782</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B62" t="s">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C62" t="s">
         <v>786</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>785</v>
       </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B63" t="s">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C63" t="s">
         <v>787</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>789</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>790</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="G63" s="1" t="s">
         <v>788</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C64" t="s">
         <v>791</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>794</v>
       </c>
-      <c r="E64" t="s">
+      <c r="F64" t="s">
         <v>793</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="G64" s="1" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B65" t="s">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C65" t="s">
         <v>795</v>
       </c>
-      <c r="E65" t="s">
+      <c r="F65" t="s">
         <v>797</v>
       </c>
-      <c r="F65" s="1" t="s">
+      <c r="G65" s="1" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B66" t="s">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C66" t="s">
         <v>798</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>648</v>
       </c>
-      <c r="E66" t="s">
+      <c r="F66" t="s">
         <v>799</v>
       </c>
-      <c r="F66" s="1" t="s">
+      <c r="G66" s="1" t="s">
         <v>800</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C67" t="s">
         <v>914</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>467</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>446</v>
       </c>
-      <c r="E67" t="s">
+      <c r="F67" t="s">
         <v>915</v>
       </c>
-      <c r="F67" s="1" t="s">
+      <c r="G67" s="1" t="s">
         <v>916</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
+    <row r="68" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C68" t="s">
         <v>988</v>
       </c>
-      <c r="F68" s="1" t="s">
+      <c r="G68" s="1" t="s">
         <v>989</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B69" t="s">
+    <row r="69" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C69" t="s">
         <v>992</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>990</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>991</v>
       </c>
-      <c r="F69" s="1" t="s">
+      <c r="G69" s="1" t="s">
         <v>993</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B70" t="s">
+    <row r="70" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C70" t="s">
         <v>1050</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>1052</v>
       </c>
-      <c r="E70" t="s">
+      <c r="F70" t="s">
         <v>1051</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="G70" s="1" t="s">
         <v>1049</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B71" t="s">
+    <row r="71" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C71" t="s">
         <v>1055</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>467</v>
       </c>
-      <c r="E71" t="s">
+      <c r="F71" t="s">
         <v>1053</v>
       </c>
-      <c r="F71" s="1" t="s">
+      <c r="G71" s="1" t="s">
         <v>1054</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B72" t="s">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C72" t="s">
         <v>1057</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
         <v>1058</v>
       </c>
-      <c r="F72" s="1" t="s">
+      <c r="G72" s="1" t="s">
         <v>1056</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B73" t="s">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C73" t="s">
         <v>1060</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>1062</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
         <v>1063</v>
       </c>
-      <c r="E73" t="s">
+      <c r="F73" t="s">
         <v>1059</v>
       </c>
-      <c r="F73" s="1" t="s">
+      <c r="G73" s="1" t="s">
         <v>1061</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B74" t="s">
+    <row r="74" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C74" t="s">
         <v>1066</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>1062</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E74" t="s">
         <v>1063</v>
       </c>
-      <c r="E74" t="s">
+      <c r="F74" t="s">
         <v>1064</v>
       </c>
-      <c r="F74" t="s">
+      <c r="G74" t="s">
         <v>1065</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B75" t="s">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C75" t="s">
         <v>1069</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>1070</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>1071</v>
       </c>
-      <c r="E75" t="s">
+      <c r="F75" t="s">
         <v>1067</v>
       </c>
-      <c r="F75" t="s">
+      <c r="G75" t="s">
         <v>1068</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B76" t="s">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C76" t="s">
         <v>1073</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
         <v>1074</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>1075</v>
       </c>
-      <c r="E76" t="s">
+      <c r="F76" t="s">
         <v>1072</v>
       </c>
-      <c r="F76" s="1" t="s">
+      <c r="G76" s="1" t="s">
         <v>1076</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B77" t="s">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C77" t="s">
         <v>1079</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>1074</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>1078</v>
       </c>
-      <c r="E77" t="s">
+      <c r="F77" t="s">
         <v>1077</v>
       </c>
-      <c r="F77" s="1" t="s">
+      <c r="G77" s="1" t="s">
         <v>1080</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B78" t="s">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C78" t="s">
         <v>1081</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>1074</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>1084</v>
       </c>
-      <c r="E78" t="s">
+      <c r="F78" t="s">
         <v>1082</v>
       </c>
-      <c r="F78" s="1" t="s">
+      <c r="G78" s="1" t="s">
         <v>1083</v>
       </c>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B79" t="s">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C79" t="s">
         <v>1088</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
         <v>1089</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
         <v>1090</v>
       </c>
-      <c r="E79" t="s">
+      <c r="F79" t="s">
         <v>1091</v>
       </c>
-      <c r="F79" s="1" t="s">
+      <c r="G79" s="1" t="s">
         <v>1092</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B80" t="s">
+    <row r="80" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C80" t="s">
         <v>1094</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
         <v>1089</v>
       </c>
-      <c r="D80" t="s">
+      <c r="E80" t="s">
         <v>1090</v>
       </c>
-      <c r="E80" t="s">
+      <c r="F80" t="s">
         <v>1093</v>
       </c>
-      <c r="F80" s="1" t="s">
+      <c r="G80" s="1" t="s">
         <v>1095</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B81" t="s">
+    <row r="81" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C81" t="s">
         <v>1097</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
         <v>467</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>962</v>
       </c>
-      <c r="E81" t="s">
+      <c r="F81" t="s">
         <v>1096</v>
       </c>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B82" t="s">
+    <row r="82" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C82" t="s">
         <v>1101</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
         <v>467</v>
       </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>1102</v>
       </c>
-      <c r="E82" t="s">
+      <c r="F82" t="s">
         <v>1104</v>
       </c>
-      <c r="F82" s="1" t="s">
+      <c r="G82" s="1" t="s">
         <v>1103</v>
       </c>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B83" t="s">
+    <row r="83" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C83" t="s">
         <v>1108</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
         <v>467</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>1107</v>
       </c>
-      <c r="E83" t="s">
+      <c r="F83" t="s">
         <v>1106</v>
       </c>
-      <c r="F83" s="1" t="s">
+      <c r="G83" s="1" t="s">
         <v>1105</v>
+      </c>
+    </row>
+    <row r="84" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C84" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D84" t="s">
+        <v>1090</v>
+      </c>
+      <c r="E84" t="s">
+        <v>1112</v>
+      </c>
+      <c r="F84" t="s">
+        <v>1111</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="85" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C85" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D85" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E85" t="s">
+        <v>1112</v>
+      </c>
+      <c r="F85" t="s">
+        <v>1113</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="86" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C86" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D86" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E86" t="s">
+        <v>1090</v>
+      </c>
+      <c r="F86" t="s">
+        <v>1118</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="87" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C87" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D87" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E87" t="s">
+        <v>1090</v>
+      </c>
+      <c r="F87" t="s">
+        <v>1120</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="88" spans="3:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="C88" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D88" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E88" t="s">
+        <v>1090</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>1123</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="89" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C89" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D89" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E89" t="s">
+        <v>1090</v>
+      </c>
+      <c r="F89" t="s">
+        <v>1125</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="90" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D90" t="s">
+        <v>467</v>
+      </c>
+      <c r="E90" t="s">
+        <v>446</v>
+      </c>
+      <c r="F90" t="s">
+        <v>1127</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="91" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C91" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D91" t="s">
+        <v>467</v>
+      </c>
+      <c r="E91" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="92" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C92" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D92" t="s">
+        <v>467</v>
+      </c>
+      <c r="E92" t="s">
+        <v>446</v>
+      </c>
+      <c r="F92" t="s">
+        <v>1134</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="93" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C93" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D93" t="s">
+        <v>467</v>
+      </c>
+      <c r="E93" t="s">
+        <v>71</v>
+      </c>
+      <c r="F93" t="s">
+        <v>1137</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="94" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C94" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D94" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E94" t="s">
+        <v>1090</v>
+      </c>
+      <c r="F94" t="s">
+        <v>1141</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>1142</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="95" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C95" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D95" t="s">
+        <v>990</v>
+      </c>
+      <c r="E95" t="s">
+        <v>1147</v>
+      </c>
+      <c r="F95" t="s">
+        <v>1144</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="96" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C96" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D96" t="s">
+        <v>990</v>
+      </c>
+      <c r="E96" t="s">
+        <v>168</v>
+      </c>
+      <c r="F96" t="s">
+        <v>1148</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="97" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C97" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D97" t="s">
+        <v>1089</v>
+      </c>
+      <c r="F97" t="s">
+        <v>1151</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="98" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C98" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D98" t="s">
+        <v>1062</v>
+      </c>
+      <c r="E98" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F98" t="s">
+        <v>1155</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="99" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C99" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D99" t="s">
+        <v>990</v>
+      </c>
+      <c r="E99" t="s">
+        <v>168</v>
+      </c>
+      <c r="F99" t="s">
+        <v>1158</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>1159</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>1160</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{622F8353-6ECE-5D45-BC71-7C0259CBCD6A}"/>
-    <hyperlink ref="F4" r:id="rId2" xr:uid="{E4AE5252-D67B-B04F-A57B-B5558D672E63}"/>
-    <hyperlink ref="F5" r:id="rId3" xr:uid="{824EDC81-FF73-F84B-B472-EEB71B3799F7}"/>
-    <hyperlink ref="F6" r:id="rId4" xr:uid="{5C86DC30-81A0-FA42-BE56-47F24B9E943B}"/>
-    <hyperlink ref="F7" r:id="rId5" xr:uid="{88B61246-4C8E-624B-9227-4D7DCA52085C}"/>
-    <hyperlink ref="F8" r:id="rId6" xr:uid="{FAEF115B-DD10-6B4F-8BA2-91D7F10AF164}"/>
-    <hyperlink ref="F9" r:id="rId7" xr:uid="{D5678B1D-BFC1-2849-92FC-22CDFD8907E7}"/>
-    <hyperlink ref="F10" r:id="rId8" xr:uid="{3870A6DA-3C8E-DB44-8768-9877BF1D68EA}"/>
-    <hyperlink ref="F11" r:id="rId9" xr:uid="{A9A7EB14-73E0-AD42-B419-977E7EA5FEA3}"/>
-    <hyperlink ref="F12" r:id="rId10" xr:uid="{E34E01E9-471A-6049-815A-36E8427E6F6A}"/>
-    <hyperlink ref="F13" r:id="rId11" location="new_database" xr:uid="{577051C3-DDDF-5E4F-91C9-9CBAB9110EE4}"/>
-    <hyperlink ref="F14" r:id="rId12" xr:uid="{F2391AB1-1689-A54C-9F5B-26BE8FB2E2FC}"/>
-    <hyperlink ref="F15" r:id="rId13" xr:uid="{ED23432D-49E3-7E45-9EED-344C56C72772}"/>
-    <hyperlink ref="F16" r:id="rId14" xr:uid="{5BF3F427-7AAD-2E4E-8B94-0CCA5B622D7B}"/>
-    <hyperlink ref="F17" r:id="rId15" xr:uid="{8BA5C196-EB9C-E84F-B9F5-C8338CF09D11}"/>
-    <hyperlink ref="F18" r:id="rId16" xr:uid="{7BCA621A-E7EA-6E4C-BA64-F2B0A16726AE}"/>
-    <hyperlink ref="G19" r:id="rId17" xr:uid="{A760BED8-9A16-4E43-AF9B-7E7413F07B65}"/>
-    <hyperlink ref="F19" r:id="rId18" location="basics-dtypes" xr:uid="{03E583DC-4B6E-B245-90FE-C5B686C536F3}"/>
-    <hyperlink ref="F20" r:id="rId19" xr:uid="{4999D3D1-32C0-E242-BEA5-80DC6B5BA313}"/>
-    <hyperlink ref="F21" r:id="rId20" xr:uid="{7B7BCB9E-9875-A240-88E7-9FC795942531}"/>
-    <hyperlink ref="G21" r:id="rId21" xr:uid="{DBFCC3ED-E1BC-1D4B-864D-767A27A012CB}"/>
-    <hyperlink ref="F22" r:id="rId22" xr:uid="{B2FC5726-790C-6D4F-AFBE-486B456C2104}"/>
-    <hyperlink ref="F23" r:id="rId23" xr:uid="{3BA61085-9387-0646-AC67-98A9E3A8AD5C}"/>
-    <hyperlink ref="B25" r:id="rId24" display="https://kb.objectrocket.com/timescaledb/managing-tables-with-timescaledb-1601-z" xr:uid="{3E826681-457D-1A40-AC0B-12F435FE47ED}"/>
-    <hyperlink ref="F25" r:id="rId25" xr:uid="{E62BCFDF-C9A7-0D42-B80E-EEE34097BDCF}"/>
-    <hyperlink ref="F26" r:id="rId26" xr:uid="{3B04ECD2-7215-E44A-B2BA-78117512C321}"/>
-    <hyperlink ref="F27" r:id="rId27" xr:uid="{72C1FF05-0698-1044-AD35-779549D5FEE1}"/>
-    <hyperlink ref="F28" r:id="rId28" xr:uid="{FD52415E-DA54-844A-937E-E667C2082DAB}"/>
-    <hyperlink ref="F29" r:id="rId29" xr:uid="{F49660D1-75B0-5640-A7B4-03E135260182}"/>
-    <hyperlink ref="F30" r:id="rId30" xr:uid="{0AD2DAAC-BAD7-6D4C-83DC-113CEB8ED428}"/>
-    <hyperlink ref="F32" r:id="rId31" xr:uid="{79BAFF11-A009-8142-B115-6F128D0D4E78}"/>
-    <hyperlink ref="F33" r:id="rId32" xr:uid="{4C21BF54-5FF1-7A46-8901-7EAE678178C0}"/>
-    <hyperlink ref="F34" r:id="rId33" xr:uid="{EA4A36B0-31D2-EC4D-891B-C199FD1AD007}"/>
-    <hyperlink ref="F35" r:id="rId34" xr:uid="{F9B90E3A-71B9-B343-8FAA-E06A737DA877}"/>
-    <hyperlink ref="F31" r:id="rId35" xr:uid="{A7216F86-E62C-AC48-B73F-76B2F894E6AD}"/>
-    <hyperlink ref="F36" r:id="rId36" xr:uid="{EF122EDE-6CCB-2440-885D-B71D42E7B9FC}"/>
-    <hyperlink ref="F37" r:id="rId37" xr:uid="{BF8E0884-4A84-1F45-BA3C-ED13206AFD16}"/>
-    <hyperlink ref="F38" r:id="rId38" xr:uid="{9681BD46-5396-7440-B882-B1583CAE5943}"/>
-    <hyperlink ref="F39" r:id="rId39" xr:uid="{39C3E3AB-01D7-2F4D-9A3A-06298BFC708F}"/>
-    <hyperlink ref="B40" r:id="rId40" display="https://www.psycopg.org/docs/usage.html" xr:uid="{C9644E87-5A6B-A846-9339-6FA311DD0BA2}"/>
-    <hyperlink ref="F40" r:id="rId41" xr:uid="{E6B6E8F4-8639-C840-8681-46C64199EB24}"/>
-    <hyperlink ref="F41" r:id="rId42" xr:uid="{40E80A1C-8ED4-6A46-9A85-FCDFAE78A259}"/>
-    <hyperlink ref="F42" r:id="rId43" xr:uid="{9D29BD03-9629-9E49-96DD-B8A60F3ED613}"/>
-    <hyperlink ref="F44" r:id="rId44" xr:uid="{534D43BE-9A8C-7046-82FA-3CCA4C01475A}"/>
-    <hyperlink ref="F46" r:id="rId45" xr:uid="{721A8C5E-A827-9D4D-A7B9-B660588D9790}"/>
-    <hyperlink ref="F48" r:id="rId46" xr:uid="{84D26437-907E-7D45-A77A-85E9B9E6A208}"/>
-    <hyperlink ref="F45" r:id="rId47" xr:uid="{40310FEF-9179-3C46-97A9-94459A181192}"/>
-    <hyperlink ref="F49" r:id="rId48" xr:uid="{23062DE1-DBA6-6945-AC55-802C0A2CD844}"/>
-    <hyperlink ref="F52" r:id="rId49" xr:uid="{FF9072C2-3183-A945-AF8E-32D4E261E3A9}"/>
-    <hyperlink ref="F53" r:id="rId50" xr:uid="{3C8AC7EE-5054-294D-87D4-1A6913F0B8B2}"/>
-    <hyperlink ref="F50" r:id="rId51" xr:uid="{B9356038-CF05-854A-AFF1-D7384A989DFB}"/>
-    <hyperlink ref="F54" r:id="rId52" xr:uid="{61072865-D316-554C-A5B2-DE65C0BB4955}"/>
-    <hyperlink ref="F55" r:id="rId53" xr:uid="{3D288582-752C-394F-85D5-4AC8FCF2210E}"/>
-    <hyperlink ref="F58" r:id="rId54" xr:uid="{634A44CB-CBAB-AE4D-898A-98A6804C37BE}"/>
-    <hyperlink ref="F59" r:id="rId55" xr:uid="{CBA3AB68-A9B5-7E45-AAF4-E420DC08CECB}"/>
-    <hyperlink ref="F60" r:id="rId56" xr:uid="{6513D8D1-CA9F-DB4F-8EE3-BB85344F470E}"/>
-    <hyperlink ref="F61" r:id="rId57" xr:uid="{0E6940AA-CCE2-A845-B000-88634DEE5413}"/>
-    <hyperlink ref="F63" r:id="rId58" xr:uid="{DB6C6106-7A38-1843-B3AC-F9FB615E4977}"/>
-    <hyperlink ref="F64" r:id="rId59" xr:uid="{8AED1472-61F4-E646-89E7-A2D566BEF7A0}"/>
-    <hyperlink ref="F65" r:id="rId60" xr:uid="{D5875307-B681-3841-BE35-59A92CDCD038}"/>
-    <hyperlink ref="F66" r:id="rId61" xr:uid="{E6DDA861-2175-8242-9563-08D5A89ACF52}"/>
-    <hyperlink ref="F56" r:id="rId62" xr:uid="{EDECDF4B-3198-4348-9F78-BF6E9FF8C9A6}"/>
-    <hyperlink ref="F57" r:id="rId63" location="5" xr:uid="{3C28890A-3BF2-2647-AB92-79793D3ADD6E}"/>
-    <hyperlink ref="F67" r:id="rId64" xr:uid="{617D9CE6-3964-1449-9C40-052E2D590E6C}"/>
-    <hyperlink ref="F68" r:id="rId65" xr:uid="{84D99383-F8E9-FB47-9939-D071EBFEC595}"/>
-    <hyperlink ref="F69" r:id="rId66" xr:uid="{339043D2-2CCF-D446-9816-25139E0CACB7}"/>
-    <hyperlink ref="F70" r:id="rId67" xr:uid="{4C714D52-96BD-F240-89A0-F733608C1B2D}"/>
-    <hyperlink ref="F71" r:id="rId68" xr:uid="{B5A8891C-7156-1B4B-A837-D4FC167EAAAB}"/>
-    <hyperlink ref="F72" r:id="rId69" xr:uid="{A0BCE8B5-0AD3-0644-A190-137160A69157}"/>
-    <hyperlink ref="F73" r:id="rId70" xr:uid="{E6200351-F377-7A4F-8B0A-8E85D96B4A16}"/>
-    <hyperlink ref="F76" r:id="rId71" xr:uid="{35C0D2D3-3E12-4349-B74E-A8B0597D94F4}"/>
-    <hyperlink ref="F77" r:id="rId72" xr:uid="{496160A3-690D-8644-9927-892347F57591}"/>
-    <hyperlink ref="F78" r:id="rId73" xr:uid="{743341AF-D853-634E-B5BE-90CE576C88D3}"/>
-    <hyperlink ref="F79" r:id="rId74" xr:uid="{B2BF3EBF-40A1-0B42-A4B4-C8128749CA5E}"/>
-    <hyperlink ref="F80" r:id="rId75" xr:uid="{E2480C24-834E-CB4A-8CC7-DF9C847C2270}"/>
-    <hyperlink ref="F82" r:id="rId76" xr:uid="{ACF43B1E-D282-BC42-9354-4906649896A3}"/>
-    <hyperlink ref="F83" r:id="rId77" xr:uid="{573870E9-82E2-DA46-8635-94B1ADBB794B}"/>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{622F8353-6ECE-5D45-BC71-7C0259CBCD6A}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{E4AE5252-D67B-B04F-A57B-B5558D672E63}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{824EDC81-FF73-F84B-B472-EEB71B3799F7}"/>
+    <hyperlink ref="G6" r:id="rId4" xr:uid="{5C86DC30-81A0-FA42-BE56-47F24B9E943B}"/>
+    <hyperlink ref="G7" r:id="rId5" xr:uid="{88B61246-4C8E-624B-9227-4D7DCA52085C}"/>
+    <hyperlink ref="G8" r:id="rId6" xr:uid="{FAEF115B-DD10-6B4F-8BA2-91D7F10AF164}"/>
+    <hyperlink ref="G9" r:id="rId7" xr:uid="{D5678B1D-BFC1-2849-92FC-22CDFD8907E7}"/>
+    <hyperlink ref="G10" r:id="rId8" xr:uid="{3870A6DA-3C8E-DB44-8768-9877BF1D68EA}"/>
+    <hyperlink ref="G11" r:id="rId9" xr:uid="{A9A7EB14-73E0-AD42-B419-977E7EA5FEA3}"/>
+    <hyperlink ref="G12" r:id="rId10" xr:uid="{E34E01E9-471A-6049-815A-36E8427E6F6A}"/>
+    <hyperlink ref="G13" r:id="rId11" location="new_database" xr:uid="{577051C3-DDDF-5E4F-91C9-9CBAB9110EE4}"/>
+    <hyperlink ref="G14" r:id="rId12" xr:uid="{F2391AB1-1689-A54C-9F5B-26BE8FB2E2FC}"/>
+    <hyperlink ref="G15" r:id="rId13" xr:uid="{ED23432D-49E3-7E45-9EED-344C56C72772}"/>
+    <hyperlink ref="G16" r:id="rId14" xr:uid="{5BF3F427-7AAD-2E4E-8B94-0CCA5B622D7B}"/>
+    <hyperlink ref="G17" r:id="rId15" xr:uid="{8BA5C196-EB9C-E84F-B9F5-C8338CF09D11}"/>
+    <hyperlink ref="G18" r:id="rId16" xr:uid="{7BCA621A-E7EA-6E4C-BA64-F2B0A16726AE}"/>
+    <hyperlink ref="H19" r:id="rId17" xr:uid="{A760BED8-9A16-4E43-AF9B-7E7413F07B65}"/>
+    <hyperlink ref="G19" r:id="rId18" location="basics-dtypes" xr:uid="{03E583DC-4B6E-B245-90FE-C5B686C536F3}"/>
+    <hyperlink ref="G20" r:id="rId19" xr:uid="{4999D3D1-32C0-E242-BEA5-80DC6B5BA313}"/>
+    <hyperlink ref="G21" r:id="rId20" xr:uid="{7B7BCB9E-9875-A240-88E7-9FC795942531}"/>
+    <hyperlink ref="H21" r:id="rId21" xr:uid="{DBFCC3ED-E1BC-1D4B-864D-767A27A012CB}"/>
+    <hyperlink ref="G22" r:id="rId22" xr:uid="{B2FC5726-790C-6D4F-AFBE-486B456C2104}"/>
+    <hyperlink ref="G23" r:id="rId23" xr:uid="{3BA61085-9387-0646-AC67-98A9E3A8AD5C}"/>
+    <hyperlink ref="C25" r:id="rId24" display="https://kb.objectrocket.com/timescaledb/managing-tables-with-timescaledb-1601-z" xr:uid="{3E826681-457D-1A40-AC0B-12F435FE47ED}"/>
+    <hyperlink ref="G25" r:id="rId25" xr:uid="{E62BCFDF-C9A7-0D42-B80E-EEE34097BDCF}"/>
+    <hyperlink ref="G26" r:id="rId26" xr:uid="{3B04ECD2-7215-E44A-B2BA-78117512C321}"/>
+    <hyperlink ref="G27" r:id="rId27" xr:uid="{72C1FF05-0698-1044-AD35-779549D5FEE1}"/>
+    <hyperlink ref="G28" r:id="rId28" xr:uid="{FD52415E-DA54-844A-937E-E667C2082DAB}"/>
+    <hyperlink ref="G29" r:id="rId29" xr:uid="{F49660D1-75B0-5640-A7B4-03E135260182}"/>
+    <hyperlink ref="G30" r:id="rId30" xr:uid="{0AD2DAAC-BAD7-6D4C-83DC-113CEB8ED428}"/>
+    <hyperlink ref="G32" r:id="rId31" xr:uid="{79BAFF11-A009-8142-B115-6F128D0D4E78}"/>
+    <hyperlink ref="G33" r:id="rId32" xr:uid="{4C21BF54-5FF1-7A46-8901-7EAE678178C0}"/>
+    <hyperlink ref="G34" r:id="rId33" xr:uid="{EA4A36B0-31D2-EC4D-891B-C199FD1AD007}"/>
+    <hyperlink ref="G35" r:id="rId34" xr:uid="{F9B90E3A-71B9-B343-8FAA-E06A737DA877}"/>
+    <hyperlink ref="G31" r:id="rId35" xr:uid="{A7216F86-E62C-AC48-B73F-76B2F894E6AD}"/>
+    <hyperlink ref="G36" r:id="rId36" xr:uid="{EF122EDE-6CCB-2440-885D-B71D42E7B9FC}"/>
+    <hyperlink ref="G37" r:id="rId37" xr:uid="{BF8E0884-4A84-1F45-BA3C-ED13206AFD16}"/>
+    <hyperlink ref="G38" r:id="rId38" xr:uid="{9681BD46-5396-7440-B882-B1583CAE5943}"/>
+    <hyperlink ref="G39" r:id="rId39" xr:uid="{39C3E3AB-01D7-2F4D-9A3A-06298BFC708F}"/>
+    <hyperlink ref="C40" r:id="rId40" display="https://www.psycopg.org/docs/usage.html" xr:uid="{C9644E87-5A6B-A846-9339-6FA311DD0BA2}"/>
+    <hyperlink ref="G40" r:id="rId41" xr:uid="{E6B6E8F4-8639-C840-8681-46C64199EB24}"/>
+    <hyperlink ref="G41" r:id="rId42" xr:uid="{40E80A1C-8ED4-6A46-9A85-FCDFAE78A259}"/>
+    <hyperlink ref="G42" r:id="rId43" xr:uid="{9D29BD03-9629-9E49-96DD-B8A60F3ED613}"/>
+    <hyperlink ref="G44" r:id="rId44" xr:uid="{534D43BE-9A8C-7046-82FA-3CCA4C01475A}"/>
+    <hyperlink ref="G46" r:id="rId45" xr:uid="{721A8C5E-A827-9D4D-A7B9-B660588D9790}"/>
+    <hyperlink ref="G48" r:id="rId46" xr:uid="{84D26437-907E-7D45-A77A-85E9B9E6A208}"/>
+    <hyperlink ref="G45" r:id="rId47" xr:uid="{40310FEF-9179-3C46-97A9-94459A181192}"/>
+    <hyperlink ref="G49" r:id="rId48" xr:uid="{23062DE1-DBA6-6945-AC55-802C0A2CD844}"/>
+    <hyperlink ref="G52" r:id="rId49" xr:uid="{FF9072C2-3183-A945-AF8E-32D4E261E3A9}"/>
+    <hyperlink ref="G53" r:id="rId50" xr:uid="{3C8AC7EE-5054-294D-87D4-1A6913F0B8B2}"/>
+    <hyperlink ref="G50" r:id="rId51" xr:uid="{B9356038-CF05-854A-AFF1-D7384A989DFB}"/>
+    <hyperlink ref="G54" r:id="rId52" xr:uid="{61072865-D316-554C-A5B2-DE65C0BB4955}"/>
+    <hyperlink ref="G55" r:id="rId53" xr:uid="{3D288582-752C-394F-85D5-4AC8FCF2210E}"/>
+    <hyperlink ref="G58" r:id="rId54" xr:uid="{634A44CB-CBAB-AE4D-898A-98A6804C37BE}"/>
+    <hyperlink ref="G59" r:id="rId55" xr:uid="{CBA3AB68-A9B5-7E45-AAF4-E420DC08CECB}"/>
+    <hyperlink ref="G60" r:id="rId56" xr:uid="{6513D8D1-CA9F-DB4F-8EE3-BB85344F470E}"/>
+    <hyperlink ref="G61" r:id="rId57" xr:uid="{0E6940AA-CCE2-A845-B000-88634DEE5413}"/>
+    <hyperlink ref="G63" r:id="rId58" xr:uid="{DB6C6106-7A38-1843-B3AC-F9FB615E4977}"/>
+    <hyperlink ref="G64" r:id="rId59" xr:uid="{8AED1472-61F4-E646-89E7-A2D566BEF7A0}"/>
+    <hyperlink ref="G65" r:id="rId60" xr:uid="{D5875307-B681-3841-BE35-59A92CDCD038}"/>
+    <hyperlink ref="G66" r:id="rId61" xr:uid="{E6DDA861-2175-8242-9563-08D5A89ACF52}"/>
+    <hyperlink ref="G56" r:id="rId62" xr:uid="{EDECDF4B-3198-4348-9F78-BF6E9FF8C9A6}"/>
+    <hyperlink ref="G57" r:id="rId63" location="5" xr:uid="{3C28890A-3BF2-2647-AB92-79793D3ADD6E}"/>
+    <hyperlink ref="G67" r:id="rId64" xr:uid="{617D9CE6-3964-1449-9C40-052E2D590E6C}"/>
+    <hyperlink ref="G68" r:id="rId65" xr:uid="{84D99383-F8E9-FB47-9939-D071EBFEC595}"/>
+    <hyperlink ref="G69" r:id="rId66" xr:uid="{339043D2-2CCF-D446-9816-25139E0CACB7}"/>
+    <hyperlink ref="G70" r:id="rId67" xr:uid="{4C714D52-96BD-F240-89A0-F733608C1B2D}"/>
+    <hyperlink ref="G71" r:id="rId68" xr:uid="{B5A8891C-7156-1B4B-A837-D4FC167EAAAB}"/>
+    <hyperlink ref="G72" r:id="rId69" xr:uid="{A0BCE8B5-0AD3-0644-A190-137160A69157}"/>
+    <hyperlink ref="G73" r:id="rId70" xr:uid="{E6200351-F377-7A4F-8B0A-8E85D96B4A16}"/>
+    <hyperlink ref="G76" r:id="rId71" xr:uid="{35C0D2D3-3E12-4349-B74E-A8B0597D94F4}"/>
+    <hyperlink ref="G77" r:id="rId72" xr:uid="{496160A3-690D-8644-9927-892347F57591}"/>
+    <hyperlink ref="G78" r:id="rId73" xr:uid="{743341AF-D853-634E-B5BE-90CE576C88D3}"/>
+    <hyperlink ref="G79" r:id="rId74" xr:uid="{B2BF3EBF-40A1-0B42-A4B4-C8128749CA5E}"/>
+    <hyperlink ref="G80" r:id="rId75" xr:uid="{E2480C24-834E-CB4A-8CC7-DF9C847C2270}"/>
+    <hyperlink ref="G82" r:id="rId76" xr:uid="{ACF43B1E-D282-BC42-9354-4906649896A3}"/>
+    <hyperlink ref="G83" r:id="rId77" xr:uid="{573870E9-82E2-DA46-8635-94B1ADBB794B}"/>
+    <hyperlink ref="G84" r:id="rId78" xr:uid="{C945C8A4-E4EC-4644-8B54-BD2288335805}"/>
+    <hyperlink ref="G85" r:id="rId79" xr:uid="{0719809F-1E3E-F843-B7C8-DF51D3206B28}"/>
+    <hyperlink ref="G86" r:id="rId80" xr:uid="{E99C8221-D0BE-224F-B43B-E9F138CAA6DC}"/>
+    <hyperlink ref="G87" r:id="rId81" xr:uid="{1ECDA9E7-DF0A-3D41-A437-5096F655132F}"/>
+    <hyperlink ref="G88" r:id="rId82" xr:uid="{16C2158A-753F-3847-980D-7B38F628AB3A}"/>
+    <hyperlink ref="G90" r:id="rId83" xr:uid="{363FDDBF-BD7C-9743-9E0A-1EDD405ABF32}"/>
+    <hyperlink ref="G89" r:id="rId84" xr:uid="{B0BB428D-C231-EE47-B83C-DAC49355FD97}"/>
+    <hyperlink ref="G91" r:id="rId85" xr:uid="{1FBABADA-1916-AD44-A919-183A8BD243EC}"/>
+    <hyperlink ref="G92" r:id="rId86" xr:uid="{52A3A357-7E58-264D-87F1-C91512C3A9F9}"/>
+    <hyperlink ref="G93" r:id="rId87" xr:uid="{CA05EC4D-249B-7E4B-B582-B5393864F8EA}"/>
+    <hyperlink ref="G94" r:id="rId88" xr:uid="{00AB9602-5FF3-7F4E-B542-1F8992B26FC9}"/>
+    <hyperlink ref="H94" r:id="rId89" xr:uid="{EA335430-4AD6-6546-BED8-D997A3E787D7}"/>
+    <hyperlink ref="G95" r:id="rId90" xr:uid="{0D5C6143-9DEB-4A4A-8D9D-551874E0560D}"/>
+    <hyperlink ref="G96" r:id="rId91" xr:uid="{5309BF1B-1D5C-6A4F-9399-AF784EBCEA38}"/>
+    <hyperlink ref="G97" r:id="rId92" xr:uid="{8BDA6316-5052-464E-A7A7-6380B545F5AB}"/>
+    <hyperlink ref="G98" r:id="rId93" xr:uid="{F773C828-F195-7A42-8579-10F12922000E}"/>
+    <hyperlink ref="G99" r:id="rId94" xr:uid="{C2EBC299-06C6-7341-8802-5A8DEDC75924}"/>
+    <hyperlink ref="H99" r:id="rId95" xr:uid="{444CF4AD-4051-C243-B21D-D4F4272644D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for excel
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1605CE71-A1A2-474D-8675-53714F5AB945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B261A725-47A8-BB45-8043-485D2D78A772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="13800" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="1172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="1177">
   <si>
     <t>docker</t>
   </si>
@@ -3562,6 +3562,21 @@
   </si>
   <si>
     <t>https://grafana.com/tutorials/build-a-panel-plugin/</t>
+  </si>
+  <si>
+    <t>Change Excel day name to other languages</t>
+  </si>
+  <si>
+    <t>excel</t>
+  </si>
+  <si>
+    <t>weekdays</t>
+  </si>
+  <si>
+    <t>CHOOSE(WEEKDAY(B4),"Sun","Mon","Tue","Wed","Thu","Fri","Sat")</t>
+  </si>
+  <si>
+    <t>https://superuser.com/questions/477385/change-excel-day-name-to-other-languages/477395</t>
   </si>
 </sst>
 </file>
@@ -7793,7 +7808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C546159-CB90-4141-B53C-C9065786FB56}">
   <dimension ref="B2:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -7905,10 +7920,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="C2:H99"/>
+  <dimension ref="C2:H100"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69:G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8682,77 +8697,77 @@
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
-        <v>992</v>
+        <v>1172</v>
       </c>
       <c r="D69" t="s">
-        <v>990</v>
+        <v>1173</v>
       </c>
       <c r="E69" t="s">
-        <v>991</v>
+        <v>1174</v>
+      </c>
+      <c r="F69" t="s">
+        <v>1175</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>993</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
-        <v>1050</v>
+        <v>992</v>
       </c>
       <c r="D70" t="s">
-        <v>1052</v>
-      </c>
-      <c r="F70" t="s">
-        <v>1051</v>
+        <v>990</v>
+      </c>
+      <c r="E70" t="s">
+        <v>991</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>1049</v>
+        <v>993</v>
       </c>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C71" t="s">
-        <v>1055</v>
+        <v>1050</v>
       </c>
       <c r="D71" t="s">
-        <v>467</v>
+        <v>1052</v>
       </c>
       <c r="F71" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>1054</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C72" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="D72" t="s">
-        <v>1058</v>
+        <v>467</v>
+      </c>
+      <c r="F72" t="s">
+        <v>1053</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C73" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="D73" t="s">
-        <v>1062</v>
-      </c>
-      <c r="E73" t="s">
-        <v>1063</v>
-      </c>
-      <c r="F73" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>1061</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C74" t="s">
-        <v>1066</v>
+        <v>1060</v>
       </c>
       <c r="D74" t="s">
         <v>1062</v>
@@ -8761,100 +8776,100 @@
         <v>1063</v>
       </c>
       <c r="F74" t="s">
-        <v>1064</v>
-      </c>
-      <c r="G74" t="s">
-        <v>1065</v>
+        <v>1059</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>1061</v>
       </c>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C75" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="D75" t="s">
-        <v>1070</v>
+        <v>1062</v>
       </c>
       <c r="E75" t="s">
-        <v>1071</v>
+        <v>1063</v>
       </c>
       <c r="F75" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="G75" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
-        <v>1073</v>
+        <v>1069</v>
       </c>
       <c r="D76" t="s">
-        <v>1074</v>
+        <v>1070</v>
       </c>
       <c r="E76" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
       <c r="F76" t="s">
-        <v>1072</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>1076</v>
+        <v>1067</v>
+      </c>
+      <c r="G76" t="s">
+        <v>1068</v>
       </c>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C77" t="s">
-        <v>1079</v>
+        <v>1073</v>
       </c>
       <c r="D77" t="s">
         <v>1074</v>
       </c>
       <c r="E77" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="F77" t="s">
-        <v>1077</v>
+        <v>1072</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>1080</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C78" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="D78" t="s">
         <v>1074</v>
       </c>
       <c r="E78" t="s">
-        <v>1084</v>
+        <v>1078</v>
       </c>
       <c r="F78" t="s">
-        <v>1082</v>
+        <v>1077</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>1083</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C79" t="s">
-        <v>1088</v>
+        <v>1081</v>
       </c>
       <c r="D79" t="s">
-        <v>1089</v>
+        <v>1074</v>
       </c>
       <c r="E79" t="s">
-        <v>1090</v>
+        <v>1084</v>
       </c>
       <c r="F79" t="s">
-        <v>1091</v>
+        <v>1082</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>1092</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C80" t="s">
-        <v>1094</v>
+        <v>1088</v>
       </c>
       <c r="D80" t="s">
         <v>1089</v>
@@ -8863,114 +8878,114 @@
         <v>1090</v>
       </c>
       <c r="F80" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="81" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C81" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="D81" t="s">
-        <v>467</v>
+        <v>1089</v>
       </c>
       <c r="E81" t="s">
-        <v>962</v>
+        <v>1090</v>
       </c>
       <c r="F81" t="s">
-        <v>1096</v>
+        <v>1093</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>1095</v>
       </c>
     </row>
     <row r="82" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C82" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="D82" t="s">
         <v>467</v>
       </c>
       <c r="E82" t="s">
-        <v>1102</v>
+        <v>962</v>
       </c>
       <c r="F82" t="s">
-        <v>1104</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>1103</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="83" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C83" t="s">
-        <v>1108</v>
+        <v>1101</v>
       </c>
       <c r="D83" t="s">
         <v>467</v>
       </c>
       <c r="E83" t="s">
-        <v>1107</v>
+        <v>1102</v>
       </c>
       <c r="F83" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="84" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="D84" t="s">
-        <v>1090</v>
+        <v>467</v>
       </c>
       <c r="E84" t="s">
-        <v>1112</v>
+        <v>1107</v>
       </c>
       <c r="F84" t="s">
-        <v>1111</v>
+        <v>1106</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>1110</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="85" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C85" t="s">
-        <v>1115</v>
+        <v>1109</v>
       </c>
       <c r="D85" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="E85" t="s">
         <v>1112</v>
       </c>
       <c r="F85" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="86" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C86" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="D86" t="s">
         <v>1089</v>
       </c>
       <c r="E86" t="s">
-        <v>1090</v>
+        <v>1112</v>
       </c>
       <c r="F86" t="s">
-        <v>1118</v>
+        <v>1113</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="87" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C87" t="s">
-        <v>1121</v>
+        <v>1116</v>
       </c>
       <c r="D87" t="s">
         <v>1089</v>
@@ -8979,15 +8994,15 @@
         <v>1090</v>
       </c>
       <c r="F87" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>1119</v>
-      </c>
-    </row>
-    <row r="88" spans="3:8" ht="48" x14ac:dyDescent="0.2">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="88" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C88" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="D88" t="s">
         <v>1089</v>
@@ -8995,197 +9010,214 @@
       <c r="E88" t="s">
         <v>1090</v>
       </c>
-      <c r="F88" s="2" t="s">
-        <v>1123</v>
+      <c r="F88" t="s">
+        <v>1120</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>1124</v>
-      </c>
-    </row>
-    <row r="89" spans="3:8" x14ac:dyDescent="0.2">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="89" spans="3:8" ht="48" x14ac:dyDescent="0.2">
       <c r="C89" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
       <c r="D89" t="s">
-        <v>1070</v>
+        <v>1089</v>
       </c>
       <c r="E89" t="s">
         <v>1090</v>
       </c>
-      <c r="F89" t="s">
-        <v>1125</v>
+      <c r="F89" s="2" t="s">
+        <v>1123</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>1129</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="90" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C90" t="s">
-        <v>1130</v>
+        <v>1126</v>
       </c>
       <c r="D90" t="s">
-        <v>467</v>
+        <v>1070</v>
       </c>
       <c r="E90" t="s">
-        <v>446</v>
+        <v>1090</v>
       </c>
       <c r="F90" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="91" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C91" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="D91" t="s">
         <v>467</v>
       </c>
       <c r="E91" t="s">
-        <v>1133</v>
+        <v>446</v>
+      </c>
+      <c r="F91" t="s">
+        <v>1127</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>1132</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="92" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C92" t="s">
-        <v>1136</v>
+        <v>1131</v>
       </c>
       <c r="D92" t="s">
         <v>467</v>
       </c>
       <c r="E92" t="s">
-        <v>446</v>
-      </c>
-      <c r="F92" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>1135</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="93" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C93" t="s">
-        <v>1139</v>
+        <v>1136</v>
       </c>
       <c r="D93" t="s">
         <v>467</v>
       </c>
       <c r="E93" t="s">
-        <v>71</v>
+        <v>446</v>
       </c>
       <c r="F93" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>1138</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="94" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C94" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="D94" t="s">
-        <v>1089</v>
+        <v>467</v>
       </c>
       <c r="E94" t="s">
-        <v>1090</v>
+        <v>71</v>
       </c>
       <c r="F94" t="s">
-        <v>1141</v>
+        <v>1137</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>1142</v>
-      </c>
-      <c r="H94" s="1" t="s">
-        <v>1143</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="95" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C95" t="s">
-        <v>1146</v>
+        <v>1140</v>
       </c>
       <c r="D95" t="s">
-        <v>990</v>
+        <v>1089</v>
       </c>
       <c r="E95" t="s">
-        <v>1147</v>
+        <v>1090</v>
       </c>
       <c r="F95" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>1145</v>
+        <v>1142</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>1143</v>
       </c>
     </row>
     <row r="96" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C96" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
       <c r="D96" t="s">
         <v>990</v>
       </c>
       <c r="E96" t="s">
-        <v>168</v>
+        <v>1147</v>
       </c>
       <c r="F96" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>1150</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="97" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C97" t="s">
-        <v>1153</v>
+        <v>1149</v>
       </c>
       <c r="D97" t="s">
-        <v>1089</v>
+        <v>990</v>
+      </c>
+      <c r="E97" t="s">
+        <v>168</v>
       </c>
       <c r="F97" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="98" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C98" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="D98" t="s">
-        <v>1062</v>
-      </c>
-      <c r="E98" t="s">
-        <v>1070</v>
+        <v>1089</v>
       </c>
       <c r="F98" t="s">
-        <v>1155</v>
+        <v>1151</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>1156</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="99" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C99" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D99" t="s">
+        <v>1062</v>
+      </c>
+      <c r="E99" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F99" t="s">
+        <v>1155</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="100" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C100" t="s">
         <v>1157</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D100" t="s">
         <v>990</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E100" t="s">
         <v>168</v>
       </c>
-      <c r="F99" t="s">
+      <c r="F100" t="s">
         <v>1158</v>
       </c>
-      <c r="G99" s="1" t="s">
+      <c r="G100" s="1" t="s">
         <v>1159</v>
       </c>
-      <c r="H99" s="1" t="s">
+      <c r="H100" s="1" t="s">
         <v>1160</v>
       </c>
     </row>
@@ -9256,36 +9288,37 @@
     <hyperlink ref="G57" r:id="rId63" location="5" xr:uid="{3C28890A-3BF2-2647-AB92-79793D3ADD6E}"/>
     <hyperlink ref="G67" r:id="rId64" xr:uid="{617D9CE6-3964-1449-9C40-052E2D590E6C}"/>
     <hyperlink ref="G68" r:id="rId65" xr:uid="{84D99383-F8E9-FB47-9939-D071EBFEC595}"/>
-    <hyperlink ref="G69" r:id="rId66" xr:uid="{339043D2-2CCF-D446-9816-25139E0CACB7}"/>
-    <hyperlink ref="G70" r:id="rId67" xr:uid="{4C714D52-96BD-F240-89A0-F733608C1B2D}"/>
-    <hyperlink ref="G71" r:id="rId68" xr:uid="{B5A8891C-7156-1B4B-A837-D4FC167EAAAB}"/>
-    <hyperlink ref="G72" r:id="rId69" xr:uid="{A0BCE8B5-0AD3-0644-A190-137160A69157}"/>
-    <hyperlink ref="G73" r:id="rId70" xr:uid="{E6200351-F377-7A4F-8B0A-8E85D96B4A16}"/>
-    <hyperlink ref="G76" r:id="rId71" xr:uid="{35C0D2D3-3E12-4349-B74E-A8B0597D94F4}"/>
-    <hyperlink ref="G77" r:id="rId72" xr:uid="{496160A3-690D-8644-9927-892347F57591}"/>
-    <hyperlink ref="G78" r:id="rId73" xr:uid="{743341AF-D853-634E-B5BE-90CE576C88D3}"/>
-    <hyperlink ref="G79" r:id="rId74" xr:uid="{B2BF3EBF-40A1-0B42-A4B4-C8128749CA5E}"/>
-    <hyperlink ref="G80" r:id="rId75" xr:uid="{E2480C24-834E-CB4A-8CC7-DF9C847C2270}"/>
-    <hyperlink ref="G82" r:id="rId76" xr:uid="{ACF43B1E-D282-BC42-9354-4906649896A3}"/>
-    <hyperlink ref="G83" r:id="rId77" xr:uid="{573870E9-82E2-DA46-8635-94B1ADBB794B}"/>
-    <hyperlink ref="G84" r:id="rId78" xr:uid="{C945C8A4-E4EC-4644-8B54-BD2288335805}"/>
-    <hyperlink ref="G85" r:id="rId79" xr:uid="{0719809F-1E3E-F843-B7C8-DF51D3206B28}"/>
-    <hyperlink ref="G86" r:id="rId80" xr:uid="{E99C8221-D0BE-224F-B43B-E9F138CAA6DC}"/>
-    <hyperlink ref="G87" r:id="rId81" xr:uid="{1ECDA9E7-DF0A-3D41-A437-5096F655132F}"/>
-    <hyperlink ref="G88" r:id="rId82" xr:uid="{16C2158A-753F-3847-980D-7B38F628AB3A}"/>
-    <hyperlink ref="G90" r:id="rId83" xr:uid="{363FDDBF-BD7C-9743-9E0A-1EDD405ABF32}"/>
-    <hyperlink ref="G89" r:id="rId84" xr:uid="{B0BB428D-C231-EE47-B83C-DAC49355FD97}"/>
-    <hyperlink ref="G91" r:id="rId85" xr:uid="{1FBABADA-1916-AD44-A919-183A8BD243EC}"/>
-    <hyperlink ref="G92" r:id="rId86" xr:uid="{52A3A357-7E58-264D-87F1-C91512C3A9F9}"/>
-    <hyperlink ref="G93" r:id="rId87" xr:uid="{CA05EC4D-249B-7E4B-B582-B5393864F8EA}"/>
-    <hyperlink ref="G94" r:id="rId88" xr:uid="{00AB9602-5FF3-7F4E-B542-1F8992B26FC9}"/>
-    <hyperlink ref="H94" r:id="rId89" xr:uid="{EA335430-4AD6-6546-BED8-D997A3E787D7}"/>
-    <hyperlink ref="G95" r:id="rId90" xr:uid="{0D5C6143-9DEB-4A4A-8D9D-551874E0560D}"/>
-    <hyperlink ref="G96" r:id="rId91" xr:uid="{5309BF1B-1D5C-6A4F-9399-AF784EBCEA38}"/>
-    <hyperlink ref="G97" r:id="rId92" xr:uid="{8BDA6316-5052-464E-A7A7-6380B545F5AB}"/>
-    <hyperlink ref="G98" r:id="rId93" xr:uid="{F773C828-F195-7A42-8579-10F12922000E}"/>
-    <hyperlink ref="G99" r:id="rId94" xr:uid="{C2EBC299-06C6-7341-8802-5A8DEDC75924}"/>
-    <hyperlink ref="H99" r:id="rId95" xr:uid="{444CF4AD-4051-C243-B21D-D4F4272644D4}"/>
+    <hyperlink ref="G70" r:id="rId66" xr:uid="{339043D2-2CCF-D446-9816-25139E0CACB7}"/>
+    <hyperlink ref="G71" r:id="rId67" xr:uid="{4C714D52-96BD-F240-89A0-F733608C1B2D}"/>
+    <hyperlink ref="G72" r:id="rId68" xr:uid="{B5A8891C-7156-1B4B-A837-D4FC167EAAAB}"/>
+    <hyperlink ref="G73" r:id="rId69" xr:uid="{A0BCE8B5-0AD3-0644-A190-137160A69157}"/>
+    <hyperlink ref="G74" r:id="rId70" xr:uid="{E6200351-F377-7A4F-8B0A-8E85D96B4A16}"/>
+    <hyperlink ref="G77" r:id="rId71" xr:uid="{35C0D2D3-3E12-4349-B74E-A8B0597D94F4}"/>
+    <hyperlink ref="G78" r:id="rId72" xr:uid="{496160A3-690D-8644-9927-892347F57591}"/>
+    <hyperlink ref="G79" r:id="rId73" xr:uid="{743341AF-D853-634E-B5BE-90CE576C88D3}"/>
+    <hyperlink ref="G80" r:id="rId74" xr:uid="{B2BF3EBF-40A1-0B42-A4B4-C8128749CA5E}"/>
+    <hyperlink ref="G81" r:id="rId75" xr:uid="{E2480C24-834E-CB4A-8CC7-DF9C847C2270}"/>
+    <hyperlink ref="G83" r:id="rId76" xr:uid="{ACF43B1E-D282-BC42-9354-4906649896A3}"/>
+    <hyperlink ref="G84" r:id="rId77" xr:uid="{573870E9-82E2-DA46-8635-94B1ADBB794B}"/>
+    <hyperlink ref="G85" r:id="rId78" xr:uid="{C945C8A4-E4EC-4644-8B54-BD2288335805}"/>
+    <hyperlink ref="G86" r:id="rId79" xr:uid="{0719809F-1E3E-F843-B7C8-DF51D3206B28}"/>
+    <hyperlink ref="G87" r:id="rId80" xr:uid="{E99C8221-D0BE-224F-B43B-E9F138CAA6DC}"/>
+    <hyperlink ref="G88" r:id="rId81" xr:uid="{1ECDA9E7-DF0A-3D41-A437-5096F655132F}"/>
+    <hyperlink ref="G89" r:id="rId82" xr:uid="{16C2158A-753F-3847-980D-7B38F628AB3A}"/>
+    <hyperlink ref="G91" r:id="rId83" xr:uid="{363FDDBF-BD7C-9743-9E0A-1EDD405ABF32}"/>
+    <hyperlink ref="G90" r:id="rId84" xr:uid="{B0BB428D-C231-EE47-B83C-DAC49355FD97}"/>
+    <hyperlink ref="G92" r:id="rId85" xr:uid="{1FBABADA-1916-AD44-A919-183A8BD243EC}"/>
+    <hyperlink ref="G93" r:id="rId86" xr:uid="{52A3A357-7E58-264D-87F1-C91512C3A9F9}"/>
+    <hyperlink ref="G94" r:id="rId87" xr:uid="{CA05EC4D-249B-7E4B-B582-B5393864F8EA}"/>
+    <hyperlink ref="G95" r:id="rId88" xr:uid="{00AB9602-5FF3-7F4E-B542-1F8992B26FC9}"/>
+    <hyperlink ref="H95" r:id="rId89" xr:uid="{EA335430-4AD6-6546-BED8-D997A3E787D7}"/>
+    <hyperlink ref="G96" r:id="rId90" xr:uid="{0D5C6143-9DEB-4A4A-8D9D-551874E0560D}"/>
+    <hyperlink ref="G97" r:id="rId91" xr:uid="{5309BF1B-1D5C-6A4F-9399-AF784EBCEA38}"/>
+    <hyperlink ref="G98" r:id="rId92" xr:uid="{8BDA6316-5052-464E-A7A7-6380B545F5AB}"/>
+    <hyperlink ref="G99" r:id="rId93" xr:uid="{F773C828-F195-7A42-8579-10F12922000E}"/>
+    <hyperlink ref="G100" r:id="rId94" xr:uid="{C2EBC299-06C6-7341-8802-5A8DEDC75924}"/>
+    <hyperlink ref="H100" r:id="rId95" xr:uid="{444CF4AD-4051-C243-B21D-D4F4272644D4}"/>
+    <hyperlink ref="G69" r:id="rId96" xr:uid="{240944C2-24CE-134B-89FB-155FDDF84458}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for webhook
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B261A725-47A8-BB45-8043-485D2D78A772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2882EE4E-CE87-3545-9CC2-8B18E06CEE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="1177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="1195">
   <si>
     <t>docker</t>
   </si>
@@ -3577,6 +3577,60 @@
   </si>
   <si>
     <t>https://superuser.com/questions/477385/change-excel-day-name-to-other-languages/477395</t>
+  </si>
+  <si>
+    <t>flask</t>
+  </si>
+  <si>
+    <t>request.headers.get('your-header-name')</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/29386995/how-to-get-http-headers-in-flask</t>
+  </si>
+  <si>
+    <t>How to get http headers in flask?</t>
+  </si>
+  <si>
+    <t>bytes(whatever_unicode.encode("utf-8"))</t>
+  </si>
+  <si>
+    <t>How do I convert a unicode header to byte string in Flask?</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/22364955/how-do-i-convert-a-unicode-header-to-byte-string-in-flask</t>
+  </si>
+  <si>
+    <t>Webhook Signature Validation in Python</t>
+  </si>
+  <si>
+    <t>1. Get the signature from the header</t>
+  </si>
+  <si>
+    <t>2. Generate the signature by webook_key, payload, sha_type</t>
+  </si>
+  <si>
+    <t>3. Compare the two signatures</t>
+  </si>
+  <si>
+    <t>digest = hmac.new(b"[Key set in orchestrator webhook]", str(event.body).encode(‘utf-8’), hashlib.sha256).digest()</t>
+  </si>
+  <si>
+    <t>string_signature = base64.b64encode(digest)</t>
+  </si>
+  <si>
+    <t>header_signature = request.headers.get("X-Fractal-Signature"</t>
+  </si>
+  <si>
+    <t>print(hmac.compare_digest(string_signature, header_signature))</t>
+  </si>
+  <si>
+    <t>https://forum.uipath.com/t/webhook-signature-validation-in-python/158438</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/61878177/how-to-verify-a-post-request-signature-using-flask-python-when-documentation-is</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/35486389/how-to-validate-a-webhook-signature-using-python-and-openssl</t>
   </si>
 </sst>
 </file>
@@ -4038,11 +4092,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
-  <dimension ref="B1:I617"/>
+  <dimension ref="B1:I624"/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A464" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G479" sqref="G479"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A605" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G624" sqref="G624"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7605,6 +7659,49 @@
       </c>
       <c r="G617" s="1" t="s">
         <v>1100</v>
+      </c>
+    </row>
+    <row r="620" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B620" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="621" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C621" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D621" t="s">
+        <v>1190</v>
+      </c>
+      <c r="G621" s="1" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="622" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C622" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D622" t="s">
+        <v>1188</v>
+      </c>
+      <c r="G622" s="1" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="623" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D623" t="s">
+        <v>1189</v>
+      </c>
+      <c r="G623" s="1" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="624" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C624" t="s">
+        <v>1187</v>
+      </c>
+      <c r="D624" t="s">
+        <v>1191</v>
       </c>
     </row>
   </sheetData>
@@ -7799,6 +7896,9 @@
     <hyperlink ref="F263" r:id="rId188" xr:uid="{21B01167-CE07-4147-8370-E31132B70F1F}"/>
     <hyperlink ref="E391" r:id="rId189" xr:uid="{6D3F9FEF-F197-1A45-8D75-0B7C56B3031F}"/>
     <hyperlink ref="G617" r:id="rId190" xr:uid="{87985A53-CC6B-9044-8BA8-C1AD329C2A47}"/>
+    <hyperlink ref="G621" r:id="rId191" xr:uid="{3A4CBC7F-0C0F-7C4E-99DC-F5DBCA5BC2A9}"/>
+    <hyperlink ref="G622" r:id="rId192" xr:uid="{C198EB95-1539-E94F-B42C-CC6B1387B433}"/>
+    <hyperlink ref="G623" r:id="rId193" xr:uid="{6610772D-08FF-9A4C-B013-336B2BBE1418}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7920,10 +8020,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="C2:H100"/>
+  <dimension ref="C2:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69:G69"/>
+    <sheetView topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="F103" sqref="F103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9219,6 +9319,40 @@
       </c>
       <c r="H100" s="1" t="s">
         <v>1160</v>
+      </c>
+    </row>
+    <row r="101" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C101" t="s">
+        <v>1180</v>
+      </c>
+      <c r="D101" t="s">
+        <v>1177</v>
+      </c>
+      <c r="E101" t="s">
+        <v>168</v>
+      </c>
+      <c r="F101" t="s">
+        <v>1178</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="102" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C102" t="s">
+        <v>1182</v>
+      </c>
+      <c r="D102" t="s">
+        <v>1177</v>
+      </c>
+      <c r="E102" t="s">
+        <v>168</v>
+      </c>
+      <c r="F102" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>1183</v>
       </c>
     </row>
   </sheetData>
@@ -9319,6 +9453,8 @@
     <hyperlink ref="G100" r:id="rId94" xr:uid="{C2EBC299-06C6-7341-8802-5A8DEDC75924}"/>
     <hyperlink ref="H100" r:id="rId95" xr:uid="{444CF4AD-4051-C243-B21D-D4F4272644D4}"/>
     <hyperlink ref="G69" r:id="rId96" xr:uid="{240944C2-24CE-134B-89FB-155FDDF84458}"/>
+    <hyperlink ref="G101" r:id="rId97" xr:uid="{ADC01694-CECF-F54F-8E00-FEF20E4E0A75}"/>
+    <hyperlink ref="G102" r:id="rId98" xr:uid="{EBB6F486-E8CA-BD40-92CF-C97C0C53C4F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for python url parser
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips.git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips _git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2882EE4E-CE87-3545-9CC2-8B18E06CEE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA50E78-8890-1C45-9754-62DF59CC9C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="1195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="1198">
   <si>
     <t>docker</t>
   </si>
@@ -3631,6 +3631,15 @@
   </si>
   <si>
     <t>https://stackoverflow.com/questions/35486389/how-to-validate-a-webhook-signature-using-python-and-openssl</t>
+  </si>
+  <si>
+    <t>URL query parameters to dict python</t>
+  </si>
+  <si>
+    <t>parse.parse_qs(parse.urlsplit(url).query)</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/21584545/url-query-parameters-to-dict-python</t>
   </si>
 </sst>
 </file>
@@ -4094,7 +4103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
   <dimension ref="B1:I624"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+    <sheetView zoomScale="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A605" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G624" sqref="G624"/>
     </sheetView>
@@ -8020,10 +8029,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="C2:H102"/>
+  <dimension ref="C2:H103"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="F103" sqref="F103"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="G104" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9353,6 +9362,20 @@
       </c>
       <c r="G102" s="1" t="s">
         <v>1183</v>
+      </c>
+    </row>
+    <row r="103" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C103" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D103" t="s">
+        <v>467</v>
+      </c>
+      <c r="F103" t="s">
+        <v>1196</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>1197</v>
       </c>
     </row>
   </sheetData>
@@ -9455,6 +9478,7 @@
     <hyperlink ref="G69" r:id="rId96" xr:uid="{240944C2-24CE-134B-89FB-155FDDF84458}"/>
     <hyperlink ref="G101" r:id="rId97" xr:uid="{ADC01694-CECF-F54F-8E00-FEF20E4E0A75}"/>
     <hyperlink ref="G102" r:id="rId98" xr:uid="{EBB6F486-E8CA-BD40-92CF-C97C0C53C4F0}"/>
+    <hyperlink ref="G103" r:id="rId99" xr:uid="{33FA6D6C-6910-3F4C-9FCE-C0BF08EC1B3F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for requests.post
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips _git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA50E78-8890-1C45-9754-62DF59CC9C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDCA951-664A-E84A-B1C6-BA17B94EB09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="1198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="1202">
   <si>
     <t>docker</t>
   </si>
@@ -3640,6 +3640,18 @@
   </si>
   <si>
     <t>https://stackoverflow.com/questions/21584545/url-query-parameters-to-dict-python</t>
+  </si>
+  <si>
+    <t>requests</t>
+  </si>
+  <si>
+    <t>r = requests.post('http://httpbin.org/post', json={"key": "value"})</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/9733638/how-to-post-json-data-with-python-requests</t>
+  </si>
+  <si>
+    <t>How to POST JSON data with Python Requests?</t>
   </si>
 </sst>
 </file>
@@ -8029,10 +8041,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="C2:H103"/>
+  <dimension ref="C2:H104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="G104" sqref="G104"/>
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9376,6 +9388,23 @@
       </c>
       <c r="G103" s="1" t="s">
         <v>1197</v>
+      </c>
+    </row>
+    <row r="104" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C104" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D104" t="s">
+        <v>467</v>
+      </c>
+      <c r="E104" t="s">
+        <v>1198</v>
+      </c>
+      <c r="F104" t="s">
+        <v>1199</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>1200</v>
       </c>
     </row>
   </sheetData>
@@ -9479,6 +9508,7 @@
     <hyperlink ref="G101" r:id="rId97" xr:uid="{ADC01694-CECF-F54F-8E00-FEF20E4E0A75}"/>
     <hyperlink ref="G102" r:id="rId98" xr:uid="{EBB6F486-E8CA-BD40-92CF-C97C0C53C4F0}"/>
     <hyperlink ref="G103" r:id="rId99" xr:uid="{33FA6D6C-6910-3F4C-9FCE-C0BF08EC1B3F}"/>
+    <hyperlink ref="G104" r:id="rId100" xr:uid="{135F043F-F8AF-D64A-84FB-0C590C5E985F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for elastic search and ui design
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips _git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDCA951-664A-E84A-B1C6-BA17B94EB09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651AD758-8D61-DC4A-BCC2-7607134C21EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="Random Articles" sheetId="4" r:id="rId3"/>
     <sheet name="Tips" sheetId="5" r:id="rId4"/>
     <sheet name="Websites" sheetId="6" r:id="rId5"/>
-    <sheet name="Documentations" sheetId="8" r:id="rId6"/>
-    <sheet name="Suggested by Others" sheetId="7" r:id="rId7"/>
+    <sheet name="Blogs" sheetId="10" r:id="rId6"/>
+    <sheet name="Documentations" sheetId="8" r:id="rId7"/>
+    <sheet name="Suggested by Others" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="1202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="1232">
   <si>
     <t>docker</t>
   </si>
@@ -3652,13 +3653,103 @@
   </si>
   <si>
     <t>How to POST JSON data with Python Requests?</t>
+  </si>
+  <si>
+    <t>Color Paleate</t>
+  </si>
+  <si>
+    <t>https://colorpalettes.net/category/warm-colors/page/4/</t>
+  </si>
+  <si>
+    <t>https://graf1x.com/shades-of-orange-color-palette/</t>
+  </si>
+  <si>
+    <t>https://colorhunt.co/palettes/orange</t>
+  </si>
+  <si>
+    <t>24 Shades of Orange</t>
+  </si>
+  <si>
+    <t>ColorPaleate</t>
+  </si>
+  <si>
+    <t>Color Hunt</t>
+  </si>
+  <si>
+    <t>https://stripe.com/blog/connect-front-end-experience</t>
+  </si>
+  <si>
+    <t>Connect: behind the front-end experience</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>Stripe</t>
+  </si>
+  <si>
+    <t>https://leerob.io/blog/style-guides-component-libraries-design-systems</t>
+  </si>
+  <si>
+    <t>Everything I Know About Style Guides, Design Systems, and Component Libraries</t>
+  </si>
+  <si>
+    <t>Lee Robinson</t>
+  </si>
+  <si>
+    <t>Style Guide, Component Library, Design System</t>
+  </si>
+  <si>
+    <t>How Stripe Designs Beautiful Websites</t>
+  </si>
+  <si>
+    <t>https://leerob.io/blog/how-stripe-designs-beautiful-websites</t>
+  </si>
+  <si>
+    <t>https://themeforest.net/item/pickbazar-react-graphql-ecommerce-template/25283305?irgwc=1&amp;clickid=xee2PS28yxyIWx9x9uVMuSBVUkBS0SRZmUjpxk0&amp;iradid=275988&amp;irpid=1351249&amp;iradtype=ONLINE_TRACKING_LINK&amp;irmptype=mediapartner&amp;mp_value1=&amp;utm_campaign=af_impact_radius_1351249&amp;utm_medium=affiliate&amp;utm_source=impact_radius</t>
+  </si>
+  <si>
+    <t>PickBazar - React Ecommerce Template with React Hooks, Next JS, GraphQL &amp; REST API</t>
+  </si>
+  <si>
+    <t>PickBazar</t>
+  </si>
+  <si>
+    <t>Template with React Hooks, Next JS, GraphQL &amp; REST API</t>
+  </si>
+  <si>
+    <t>https://coreui.io/react/</t>
+  </si>
+  <si>
+    <t>Free React.js Admin Template</t>
+  </si>
+  <si>
+    <t>CoreUI</t>
+  </si>
+  <si>
+    <t>React.js</t>
+  </si>
+  <si>
+    <t>CSS Framework</t>
+  </si>
+  <si>
+    <t>https://tailwindcss.com</t>
+  </si>
+  <si>
+    <t>tailwind</t>
+  </si>
+  <si>
+    <t>https://www.knowi.com/blog/what-is-elastic-search/</t>
+  </si>
+  <si>
+    <t>Elasticsearch: What It Is, How It Works, And What It’s Used For</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3686,6 +3777,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -3715,7 +3812,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3730,6 +3827,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4116,7 +4214,7 @@
   <dimension ref="B1:I624"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A605" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A603" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G624" sqref="G624"/>
     </sheetView>
   </sheetViews>
@@ -7929,7 +8027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C546159-CB90-4141-B53C-C9065786FB56}">
   <dimension ref="B2:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -8041,10 +8139,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="C2:H104"/>
+  <dimension ref="C2:H109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9405,6 +9503,79 @@
       </c>
       <c r="G104" s="1" t="s">
         <v>1200</v>
+      </c>
+    </row>
+    <row r="105" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C105" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D105" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E105" t="s">
+        <v>1212</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="106" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C106" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D106" t="s">
+        <v>1215</v>
+      </c>
+      <c r="F106" t="s">
+        <v>1216</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="107" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C107" t="s">
+        <v>1217</v>
+      </c>
+      <c r="D107" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E107" t="s">
+        <v>1212</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="108" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C108" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D108" t="s">
+        <v>863</v>
+      </c>
+      <c r="E108" t="s">
+        <v>1221</v>
+      </c>
+      <c r="F108" t="s">
+        <v>1222</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="109" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C109" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D109" t="s">
+        <v>1225</v>
+      </c>
+      <c r="E109" t="s">
+        <v>1226</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>1223</v>
       </c>
     </row>
   </sheetData>
@@ -9509,6 +9680,11 @@
     <hyperlink ref="G102" r:id="rId98" xr:uid="{EBB6F486-E8CA-BD40-92CF-C97C0C53C4F0}"/>
     <hyperlink ref="G103" r:id="rId99" xr:uid="{33FA6D6C-6910-3F4C-9FCE-C0BF08EC1B3F}"/>
     <hyperlink ref="G104" r:id="rId100" xr:uid="{135F043F-F8AF-D64A-84FB-0C590C5E985F}"/>
+    <hyperlink ref="G105" r:id="rId101" xr:uid="{8529328C-AB52-3C4B-B6DC-DCD1FE5024A3}"/>
+    <hyperlink ref="G106" r:id="rId102" xr:uid="{41084259-4C36-4B49-84E3-48FE20C31217}"/>
+    <hyperlink ref="G107" r:id="rId103" xr:uid="{5354CB1E-7CA6-F441-8887-B5DFC48B5EED}"/>
+    <hyperlink ref="G108" r:id="rId104" display="https://themeforest.net/item/pickbazar-react-graphql-ecommerce-template/25283305?irgwc=1&amp;clickid=xee2PS28yxyIWx9x9uVMuSBVUkBS0SRZmUjpxk0&amp;iradid=275988&amp;irpid=1351249&amp;iradtype=ONLINE_TRACKING_LINK&amp;irmptype=mediapartner&amp;mp_value1=&amp;utm_campaign=af_impact_radius_1351249&amp;utm_medium=affiliate&amp;utm_source=impact_radius" xr:uid="{D121A6D9-CFC1-ED4C-A849-11256EC8926F}"/>
+    <hyperlink ref="G109" r:id="rId105" xr:uid="{FE2E1D34-3743-6C40-A478-EBB13FC4442B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9549,10 +9725,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069EEB69-0D57-C040-8545-840D5862E858}">
-  <dimension ref="B2:D32"/>
+  <dimension ref="B2:D40"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9700,6 +9876,48 @@
       </c>
       <c r="D32" s="1" t="s">
         <v>913</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>1207</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>1206</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>1228</v>
       </c>
     </row>
   </sheetData>
@@ -9716,12 +9934,45 @@
     <hyperlink ref="D26" r:id="rId10" location="lines" xr:uid="{17AF0CCA-02DE-B342-8716-B8979D9E6FC9}"/>
     <hyperlink ref="D31" r:id="rId11" xr:uid="{A678A0F1-CAC4-5F4E-8F54-086B5EDAC60A}"/>
     <hyperlink ref="D32" r:id="rId12" xr:uid="{2D4A5A5D-FBA9-784D-968F-2A1AC692F8BB}"/>
+    <hyperlink ref="D35" r:id="rId13" xr:uid="{DB886D49-57B6-7D41-A436-8840785C78BE}"/>
+    <hyperlink ref="D36" r:id="rId14" xr:uid="{D153F6EC-1842-344B-8EC8-3993A72C9B4A}"/>
+    <hyperlink ref="D37" r:id="rId15" xr:uid="{FFDCB414-8515-644B-9331-D421F0FB3141}"/>
+    <hyperlink ref="D40" r:id="rId16" xr:uid="{EE5BBEAA-E76E-5D48-878C-52E3AAE02ACC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30136A4-A5CE-4241-BCB0-A2D5FDA4EAE2}">
+  <dimension ref="B3:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="69.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="8" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{2E6A48F9-40CF-8248-87FD-1774B1B17209}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DA0B776-BFAF-A24A-9DE9-FDDB22250009}">
   <dimension ref="B3:D6"/>
   <sheetViews>
@@ -9777,11 +10028,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9928DD2B-0E52-0541-9E14-AF63C29120ED}">
   <dimension ref="B2:D36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add the tips for installing postgresql
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips _git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651AD758-8D61-DC4A-BCC2-7607134C21EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364FCED3-B374-7342-A0EA-9E021D2AE9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="1232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="1238">
   <si>
     <t>docker</t>
   </si>
@@ -3743,6 +3743,24 @@
   </si>
   <si>
     <t>Elasticsearch: What It Is, How It Works, And What It’s Used For</t>
+  </si>
+  <si>
+    <t>Installation on Macbook</t>
+  </si>
+  <si>
+    <t>1. install the Homebrew implementation of PostgreSQL</t>
+  </si>
+  <si>
+    <t>2. reinstall the Python adapter</t>
+  </si>
+  <si>
+    <t>brew install postgresql</t>
+  </si>
+  <si>
+    <t>pip install psycopg2</t>
+  </si>
+  <si>
+    <t>https://towardsdatascience.com/python-and-postgresql-how-to-access-a-postgresql-database-like-a-data-scientist-b5a9c5a0ea43</t>
   </si>
 </sst>
 </file>
@@ -4213,9 +4231,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
   <dimension ref="B1:I624"/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A603" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G624" sqref="G624"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A460" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G483" sqref="G483"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6824,7 +6842,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="447" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="447" spans="2:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E447" t="s">
         <v>495</v>
       </c>
@@ -7021,6 +7039,30 @@
       </c>
       <c r="G479" s="1" t="s">
         <v>780</v>
+      </c>
+    </row>
+    <row r="481" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C481" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="482" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D482" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E482" t="s">
+        <v>1235</v>
+      </c>
+      <c r="G482" s="1" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="483" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D483" t="s">
+        <v>1234</v>
+      </c>
+      <c r="E483" t="s">
+        <v>1236</v>
       </c>
     </row>
     <row r="488" spans="2:7" x14ac:dyDescent="0.2">
@@ -8018,6 +8060,7 @@
     <hyperlink ref="G621" r:id="rId191" xr:uid="{3A4CBC7F-0C0F-7C4E-99DC-F5DBCA5BC2A9}"/>
     <hyperlink ref="G622" r:id="rId192" xr:uid="{C198EB95-1539-E94F-B42C-CC6B1387B433}"/>
     <hyperlink ref="G623" r:id="rId193" xr:uid="{6610772D-08FF-9A4C-B013-336B2BBE1418}"/>
+    <hyperlink ref="G482" r:id="rId194" xr:uid="{312F784E-10E5-9349-B872-76C7948C5D3F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9947,7 +9990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30136A4-A5CE-4241-BCB0-A2D5FDA4EAE2}">
   <dimension ref="B3:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added tips for postgresql and pandas
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips _git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364FCED3-B374-7342-A0EA-9E021D2AE9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625D231C-6F62-5848-99BC-DF5C193CB7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="1238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="1251">
   <si>
     <t>docker</t>
   </si>
@@ -3761,6 +3761,45 @@
   </si>
   <si>
     <t>https://towardsdatascience.com/python-and-postgresql-how-to-access-a-postgresql-database-like-a-data-scientist-b5a9c5a0ea43</t>
+  </si>
+  <si>
+    <t>https://medium.com/dunder-data/selecting-subsets-of-data-in-pandas-39e811c81a0c</t>
+  </si>
+  <si>
+    <t>Selecting Subsets of Data in Pandas: Part 2</t>
+  </si>
+  <si>
+    <t>Pandas</t>
+  </si>
+  <si>
+    <t>Boolean Indexing</t>
+  </si>
+  <si>
+    <t>https://www.postgresqltutorial.com/postgresql-joins/</t>
+  </si>
+  <si>
+    <t>PostgreSQL Joins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PostgreSQL </t>
+  </si>
+  <si>
+    <t>Joins</t>
+  </si>
+  <si>
+    <t>Different joins with where statement and graphs</t>
+  </si>
+  <si>
+    <t>How to do/workaround a conditional join in python Pandas?</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/23508351/how-to-do-workaround-a-conditional-join-in-python-pandas</t>
+  </si>
+  <si>
+    <t>Conditional Join</t>
+  </si>
+  <si>
+    <t>df = df.merge(windows,on='company',how='left')</t>
   </si>
 </sst>
 </file>
@@ -4231,8 +4270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5B14D6-E341-F449-8650-5CC3D2E3CE40}">
   <dimension ref="B1:I624"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A460" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A467" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G483" sqref="G483"/>
     </sheetView>
   </sheetViews>
@@ -8182,10 +8221,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="C2:H109"/>
+  <dimension ref="C2:H112"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="E110" sqref="E110"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9619,6 +9658,54 @@
       </c>
       <c r="G109" s="1" t="s">
         <v>1223</v>
+      </c>
+    </row>
+    <row r="110" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C110" t="s">
+        <v>1239</v>
+      </c>
+      <c r="D110" t="s">
+        <v>1240</v>
+      </c>
+      <c r="E110" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="111" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C111" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D111" t="s">
+        <v>1244</v>
+      </c>
+      <c r="E111" t="s">
+        <v>1245</v>
+      </c>
+      <c r="F111" t="s">
+        <v>1246</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="112" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C112" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D112" t="s">
+        <v>1240</v>
+      </c>
+      <c r="E112" t="s">
+        <v>1249</v>
+      </c>
+      <c r="F112" t="s">
+        <v>1250</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>1248</v>
       </c>
     </row>
   </sheetData>
@@ -9728,6 +9815,9 @@
     <hyperlink ref="G107" r:id="rId103" xr:uid="{5354CB1E-7CA6-F441-8887-B5DFC48B5EED}"/>
     <hyperlink ref="G108" r:id="rId104" display="https://themeforest.net/item/pickbazar-react-graphql-ecommerce-template/25283305?irgwc=1&amp;clickid=xee2PS28yxyIWx9x9uVMuSBVUkBS0SRZmUjpxk0&amp;iradid=275988&amp;irpid=1351249&amp;iradtype=ONLINE_TRACKING_LINK&amp;irmptype=mediapartner&amp;mp_value1=&amp;utm_campaign=af_impact_radius_1351249&amp;utm_medium=affiliate&amp;utm_source=impact_radius" xr:uid="{D121A6D9-CFC1-ED4C-A849-11256EC8926F}"/>
     <hyperlink ref="G109" r:id="rId105" xr:uid="{FE2E1D34-3743-6C40-A478-EBB13FC4442B}"/>
+    <hyperlink ref="G110" r:id="rId106" xr:uid="{E27C5FE5-8BD9-3441-BA07-649C4A91DB65}"/>
+    <hyperlink ref="G111" r:id="rId107" xr:uid="{709A123B-9909-A445-B840-62BE94B21BD8}"/>
+    <hyperlink ref="G112" r:id="rId108" xr:uid="{29CA3589-9D94-F64F-B149-D086D712D169}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for pandas conditional merge, forward fill for each group
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips _git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625D231C-6F62-5848-99BC-DF5C193CB7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A5BA0E-02F9-D84D-8317-1056BB269A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="1251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="1258">
   <si>
     <t>docker</t>
   </si>
@@ -3800,6 +3800,27 @@
   </si>
   <si>
     <t>df = df.merge(windows,on='company',how='left')</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/34272501/sql-fill-in-gaps-with-last-value-untill-new-value-occurs</t>
+  </si>
+  <si>
+    <t>SQL Fill in Gaps with last value untill new value occurs</t>
+  </si>
+  <si>
+    <t>SUM(IIF(Status IS NULL, 0,1)) OVER (ORDER BY Date_of_data ASC) AS 'Grp'</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/53696707/how-to-do-forward-filling-for-each-group-in-pandas</t>
+  </si>
+  <si>
+    <t>df[['id'] + cols] = df.groupby('id')[cols].ffill().fillna(0).astype(int)</t>
+  </si>
+  <si>
+    <t>How to do forward filling for each group in pandas</t>
+  </si>
+  <si>
+    <t>ffill</t>
   </si>
 </sst>
 </file>
@@ -8221,10 +8242,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="C2:H112"/>
+  <dimension ref="C2:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="F113" sqref="F113"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9706,6 +9727,37 @@
       </c>
       <c r="G112" s="1" t="s">
         <v>1248</v>
+      </c>
+    </row>
+    <row r="113" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C113" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D113" t="s">
+        <v>730</v>
+      </c>
+      <c r="F113" t="s">
+        <v>1253</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="114" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C114" t="s">
+        <v>1256</v>
+      </c>
+      <c r="D114" t="s">
+        <v>1240</v>
+      </c>
+      <c r="E114" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F114" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>1254</v>
       </c>
     </row>
   </sheetData>
@@ -9818,6 +9870,8 @@
     <hyperlink ref="G110" r:id="rId106" xr:uid="{E27C5FE5-8BD9-3441-BA07-649C4A91DB65}"/>
     <hyperlink ref="G111" r:id="rId107" xr:uid="{709A123B-9909-A445-B840-62BE94B21BD8}"/>
     <hyperlink ref="G112" r:id="rId108" xr:uid="{29CA3589-9D94-F64F-B149-D086D712D169}"/>
+    <hyperlink ref="G113" r:id="rId109" xr:uid="{4DA0142F-316E-A241-875A-75EE55DF5FB5}"/>
+    <hyperlink ref="G114" r:id="rId110" xr:uid="{C0EEB598-C448-644C-B867-BA95DB72F3DE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips about email with python
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips _git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A5BA0E-02F9-D84D-8317-1056BB269A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C958095F-0A20-694A-B812-06874AF95447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="1258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="1262">
   <si>
     <t>docker</t>
   </si>
@@ -3821,6 +3821,18 @@
   </si>
   <si>
     <t>ffill</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/6541271/python-poplib-get-attachment</t>
+  </si>
+  <si>
+    <t>python poplib get attachment</t>
+  </si>
+  <si>
+    <t>if part.get_content_type() in allowed_mimetypes:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email </t>
   </si>
 </sst>
 </file>
@@ -8242,10 +8254,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="C2:H114"/>
+  <dimension ref="C2:H115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9758,6 +9770,23 @@
       </c>
       <c r="G114" s="1" t="s">
         <v>1254</v>
+      </c>
+    </row>
+    <row r="115" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C115" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D115" t="s">
+        <v>467</v>
+      </c>
+      <c r="E115" t="s">
+        <v>1261</v>
+      </c>
+      <c r="F115" t="s">
+        <v>1260</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>1258</v>
       </c>
     </row>
   </sheetData>
@@ -9872,6 +9901,7 @@
     <hyperlink ref="G112" r:id="rId108" xr:uid="{29CA3589-9D94-F64F-B149-D086D712D169}"/>
     <hyperlink ref="G113" r:id="rId109" xr:uid="{4DA0142F-316E-A241-875A-75EE55DF5FB5}"/>
     <hyperlink ref="G114" r:id="rId110" xr:uid="{C0EEB598-C448-644C-B867-BA95DB72F3DE}"/>
+    <hyperlink ref="G115" r:id="rId111" xr:uid="{FFD2DFDE-1A4F-8C42-B8F7-EA734D4656E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added links for co2 converter that suggested by Daniel
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/Documents/Technical Tips _git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C958095F-0A20-694A-B812-06874AF95447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55346A8C-DF59-9749-9234-D0768B6BCEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="1262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="1264">
   <si>
     <t>docker</t>
   </si>
@@ -3833,6 +3833,12 @@
   </si>
   <si>
     <t xml:space="preserve">email </t>
+  </si>
+  <si>
+    <t>kWh to CO2e</t>
+  </si>
+  <si>
+    <t>https://www.rensmart.com/Calculators/KWH-to-CO2</t>
   </si>
 </sst>
 </file>
@@ -4304,7 +4310,7 @@
   <dimension ref="B1:I624"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A467" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A598" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G483" sqref="G483"/>
     </sheetView>
   </sheetViews>
@@ -8256,7 +8262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
   <dimension ref="C2:H115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+    <sheetView topLeftCell="A96" workbookViewId="0">
       <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
@@ -10247,10 +10253,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9928DD2B-0E52-0541-9E14-AF63C29120ED}">
-  <dimension ref="B2:D36"/>
+  <dimension ref="B2:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10395,14 +10401,24 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D33" s="1" t="s">
         <v>1036</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D36" s="1" t="s">
         <v>1048</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D39" s="1" t="s">
+        <v>1263</v>
       </c>
     </row>
   </sheetData>
@@ -10418,6 +10434,7 @@
     <hyperlink ref="D20" r:id="rId9" xr:uid="{614DF81B-23CA-D149-B6B6-382BC4B96C5F}"/>
     <hyperlink ref="D23" r:id="rId10" xr:uid="{26AA8E92-5A0E-DC40-B89B-30A95B18A6FE}"/>
     <hyperlink ref="D36" r:id="rId11" xr:uid="{4DFB4F19-5176-ED42-BFA9-87315363848F}"/>
+    <hyperlink ref="D39" r:id="rId12" xr:uid="{717B3FD6-5FA5-E645-AB6E-ED65A4DC2B4D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added suggested sites from colleagues
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55346A8C-DF59-9749-9234-D0768B6BCEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48EF5B0-D9A9-B841-A608-917515B1723C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="1264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="1279">
   <si>
     <t>docker</t>
   </si>
@@ -3839,6 +3839,51 @@
   </si>
   <si>
     <t>https://www.rensmart.com/Calculators/KWH-to-CO2</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>How to Iterate Through a Dictionary in Python</t>
+  </si>
+  <si>
+    <t>dict</t>
+  </si>
+  <si>
+    <t>prices_dict.items()</t>
+  </si>
+  <si>
+    <t>https://realpython.com/iterate-through-dictionary-python/</t>
+  </si>
+  <si>
+    <t>Matthew</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/63018871/how-do-you-get-the-run-parameters-and-runid-within-databricks-notebook#63018872</t>
+  </si>
+  <si>
+    <t>How do you get the run parameters and runId within Databricks notebook?</t>
+  </si>
+  <si>
+    <t>Jack's Handover</t>
+  </si>
+  <si>
+    <t>https://cloudfmgroupltd.sharepoint.com/sites/Mindsett/Shared%20Documents/Forms/AllItems.aspx?id=%2Fsites%2FMindsett%2FShared%20Documents%2FJS%20Documents&amp;viewid=b8533075%2Da592%2D4ad4%2D9a3e%2D13e7c31509c8</t>
+  </si>
+  <si>
+    <t>Sharepoint</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/azure/key-vault/secrets/quick-create-python</t>
+  </si>
+  <si>
+    <t>Quickstart: Azure Key Vault secret client library for Python</t>
+  </si>
+  <si>
+    <t>Sean's Telemetry</t>
+  </si>
+  <si>
+    <t>http://iotdev.cloudfmsystems.com/grafana/d/D533eUfMk/reboot-monitoring?orgId=1&amp;from=now-7d&amp;to=now</t>
   </si>
 </sst>
 </file>
@@ -3908,7 +3953,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3924,6 +3969,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -8260,10 +8306,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="C2:H115"/>
+  <dimension ref="B2:H116"/>
   <sheetViews>
-    <sheetView topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="G117" sqref="G117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8273,7 +8319,10 @@
     <col min="6" max="6" width="55.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>1264</v>
+      </c>
       <c r="D2" t="s">
         <v>436</v>
       </c>
@@ -8281,7 +8330,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>399</v>
       </c>
@@ -8292,7 +8341,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>402</v>
       </c>
@@ -8300,7 +8349,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>408</v>
       </c>
@@ -8308,7 +8357,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>411</v>
       </c>
@@ -8319,7 +8368,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>413</v>
       </c>
@@ -8327,7 +8376,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>426</v>
       </c>
@@ -8338,7 +8387,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>428</v>
       </c>
@@ -8346,7 +8395,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>439</v>
       </c>
@@ -8360,7 +8409,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>442</v>
       </c>
@@ -8371,7 +8420,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>445</v>
       </c>
@@ -8385,7 +8434,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>448</v>
       </c>
@@ -8396,7 +8445,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="14" spans="3:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>452</v>
       </c>
@@ -8410,7 +8459,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>454</v>
       </c>
@@ -8418,7 +8467,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>457</v>
       </c>
@@ -9747,7 +9796,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="113" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C113" t="s">
         <v>1252</v>
       </c>
@@ -9761,7 +9810,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="114" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C114" t="s">
         <v>1256</v>
       </c>
@@ -9778,7 +9827,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="115" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C115" t="s">
         <v>1259</v>
       </c>
@@ -9793,6 +9842,26 @@
       </c>
       <c r="G115" s="1" t="s">
         <v>1258</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B116" s="9">
+        <v>44524</v>
+      </c>
+      <c r="C116" t="s">
+        <v>1265</v>
+      </c>
+      <c r="D116" t="s">
+        <v>467</v>
+      </c>
+      <c r="E116" t="s">
+        <v>1266</v>
+      </c>
+      <c r="F116" t="s">
+        <v>1267</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>1268</v>
       </c>
     </row>
   </sheetData>
@@ -9908,6 +9977,7 @@
     <hyperlink ref="G113" r:id="rId109" xr:uid="{4DA0142F-316E-A241-875A-75EE55DF5FB5}"/>
     <hyperlink ref="G114" r:id="rId110" xr:uid="{C0EEB598-C448-644C-B867-BA95DB72F3DE}"/>
     <hyperlink ref="G115" r:id="rId111" xr:uid="{FFD2DFDE-1A4F-8C42-B8F7-EA734D4656E9}"/>
+    <hyperlink ref="G116" r:id="rId112" xr:uid="{B8C3285A-89F3-8B49-A095-416E499CEE2E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10253,10 +10323,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9928DD2B-0E52-0541-9E14-AF63C29120ED}">
-  <dimension ref="B2:D39"/>
+  <dimension ref="B2:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10401,24 +10471,75 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D33" s="1" t="s">
         <v>1036</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D36" s="1" t="s">
         <v>1048</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
         <v>1262</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D39" s="1" t="s">
         <v>1263</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D44" s="1" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D46" s="1" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
+        <v>1090</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>1278</v>
       </c>
     </row>
   </sheetData>
@@ -10435,6 +10556,10 @@
     <hyperlink ref="D23" r:id="rId10" xr:uid="{26AA8E92-5A0E-DC40-B89B-30A95B18A6FE}"/>
     <hyperlink ref="D36" r:id="rId11" xr:uid="{4DFB4F19-5176-ED42-BFA9-87315363848F}"/>
     <hyperlink ref="D39" r:id="rId12" xr:uid="{717B3FD6-5FA5-E645-AB6E-ED65A4DC2B4D}"/>
+    <hyperlink ref="D44" r:id="rId13" location="63018872" xr:uid="{1EFDD214-998A-7741-9153-ABD74A7BDA0B}"/>
+    <hyperlink ref="D51" r:id="rId14" xr:uid="{34ED556E-13EA-0B4A-A668-E4EF22D775AA}"/>
+    <hyperlink ref="D46" r:id="rId15" xr:uid="{06402D88-63D7-A44F-9E4A-636701CD5ACA}"/>
+    <hyperlink ref="D54" r:id="rId16" xr:uid="{1D3E2E5A-219B-D34A-9975-451CB19E4DC8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated the suggestion from others
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48EF5B0-D9A9-B841-A608-917515B1723C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26540661-5FC9-CA43-B910-96D758003F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="1279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="1283">
   <si>
     <t>docker</t>
   </si>
@@ -3884,6 +3884,18 @@
   </si>
   <si>
     <t>http://iotdev.cloudfmsystems.com/grafana/d/D533eUfMk/reboot-monitoring?orgId=1&amp;from=now-7d&amp;to=now</t>
+  </si>
+  <si>
+    <t>https://sile-typesetter.org/examples/packages.html</t>
+  </si>
+  <si>
+    <t>The SILE Typesetter</t>
+  </si>
+  <si>
+    <t>miro board</t>
+  </si>
+  <si>
+    <t>https://miro.com/app/board/o9J_lsdr1vs=/</t>
   </si>
 </sst>
 </file>
@@ -10325,8 +10337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9928DD2B-0E52-0541-9E14-AF63C29120ED}">
   <dimension ref="B2:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10443,7 +10455,12 @@
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D25" s="1"/>
+      <c r="C25" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>1282</v>
+      </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D26" s="1"/>
@@ -10514,6 +10531,16 @@
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D46" s="1" t="s">
         <v>1275</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D48" s="1" t="s">
+        <v>1279</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
@@ -10560,6 +10587,8 @@
     <hyperlink ref="D51" r:id="rId14" xr:uid="{34ED556E-13EA-0B4A-A668-E4EF22D775AA}"/>
     <hyperlink ref="D46" r:id="rId15" xr:uid="{06402D88-63D7-A44F-9E4A-636701CD5ACA}"/>
     <hyperlink ref="D54" r:id="rId16" xr:uid="{1D3E2E5A-219B-D34A-9975-451CB19E4DC8}"/>
+    <hyperlink ref="D48" r:id="rId17" xr:uid="{DA3AE831-E86C-244D-9C06-FCD4B10825B3}"/>
+    <hyperlink ref="D25" r:id="rId18" xr:uid="{74691449-22EB-0040-B8BA-6AC66502E250}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added the link for Rajitha's PowerBI
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26540661-5FC9-CA43-B910-96D758003F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6DED9C-A4C1-644E-BFBB-B826D87FCFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="1283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="1286">
   <si>
     <t>docker</t>
   </si>
@@ -3896,6 +3896,15 @@
   </si>
   <si>
     <t>https://miro.com/app/board/o9J_lsdr1vs=/</t>
+  </si>
+  <si>
+    <t>Rajitha</t>
+  </si>
+  <si>
+    <t>PowerBI Dashboard</t>
+  </si>
+  <si>
+    <t>https://app.powerbi.com/links/jiIfWaJDAO?ctid=132e8831-e8a8-4370-981b-e6f196ffd575&amp;pbi_source=linkShare</t>
   </si>
 </sst>
 </file>
@@ -10335,10 +10344,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9928DD2B-0E52-0541-9E14-AF63C29120ED}">
-  <dimension ref="B2:D54"/>
+  <dimension ref="B2:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10567,6 +10576,19 @@
       </c>
       <c r="D54" s="1" t="s">
         <v>1278</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C60" t="s">
+        <v>1284</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>1285</v>
       </c>
     </row>
   </sheetData>
@@ -10589,6 +10611,7 @@
     <hyperlink ref="D54" r:id="rId16" xr:uid="{1D3E2E5A-219B-D34A-9975-451CB19E4DC8}"/>
     <hyperlink ref="D48" r:id="rId17" xr:uid="{DA3AE831-E86C-244D-9C06-FCD4B10825B3}"/>
     <hyperlink ref="D25" r:id="rId18" xr:uid="{74691449-22EB-0040-B8BA-6AC66502E250}"/>
+    <hyperlink ref="D60" r:id="rId19" xr:uid="{E6C7961F-BD9E-FA45-9891-6E3A392A86EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tips for python, pandas, and databricks
</commit_message>
<xml_diff>
--- a/Technical Tips.xlsx
+++ b/Technical Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyyang/OneDrive - Cloudfm Integrated Services Ltd - Backup/KTP Project/Cloudfm/IT Team/Learning Projects/Technical Tips.git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6DED9C-A4C1-644E-BFBB-B826D87FCFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DEACF1-909F-1545-AD98-F6D9C4EBD37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2900" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technical Skills" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="1286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="1322">
   <si>
     <t>docker</t>
   </si>
@@ -3905,6 +3905,114 @@
   </si>
   <si>
     <t>https://app.powerbi.com/links/jiIfWaJDAO?ctid=132e8831-e8a8-4370-981b-e6f196ffd575&amp;pbi_source=linkShare</t>
+  </si>
+  <si>
+    <t>Pat</t>
+  </si>
+  <si>
+    <t>TimescaleDB Hyper-Functions</t>
+  </si>
+  <si>
+    <t>https://docs.timescale.com/api/latest/hyperfunctions/#hyperfunctions</t>
+  </si>
+  <si>
+    <t>legend</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/27174425/how-to-add-a-string-as-the-artist-in-matplotlib-legend</t>
+  </si>
+  <si>
+    <t>class AnyObjectHandler(object):</t>
+  </si>
+  <si>
+    <t>How to add a string as the artist in matplotlib legend?</t>
+  </si>
+  <si>
+    <t>https://moonbooks.org/Articles/How-to-insert-an-image-a-picture-or-a-photo-in-a-matplotlib-figure/</t>
+  </si>
+  <si>
+    <t>ab = AnnotationBbox(imagebox, (0.4, 0.6))</t>
+  </si>
+  <si>
+    <t>AnnotationBbox</t>
+  </si>
+  <si>
+    <t>How to insert an image (a picture or a photo) in a matplotlib figure</t>
+  </si>
+  <si>
+    <t>_nolegend_'</t>
+  </si>
+  <si>
+    <t>How to exclude the elements from the legend in python?</t>
+  </si>
+  <si>
+    <t>https://discuss.analyticsvidhya.com/t/how-to-exclude-the-elements-from-the-legend-in-python/5393</t>
+  </si>
+  <si>
+    <t>ax.plot(randn(1000).cumsum(), 'k.', label='_nolegend_')</t>
+  </si>
+  <si>
+    <t>pandas &amp; jupyter</t>
+  </si>
+  <si>
+    <t>pandas.set_option('display.max_rows', 10)</t>
+  </si>
+  <si>
+    <t>f.write(df.to_csv(index=False))</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/55248832/how-to-transfer-pandas-dataframe-to-csv-on-sftp-using-paramiko-library-in-pytho</t>
+  </si>
+  <si>
+    <t>Transfer Pandas DataFrame to .csv on SFTP using Paramiko Library in Python?</t>
+  </si>
+  <si>
+    <t>sftp &amp; paramiko</t>
+  </si>
+  <si>
+    <t>https://docs.databricks.com/dev-tools/databricks-utils.html#file-system-utility-dbutilsfs</t>
+  </si>
+  <si>
+    <t>Azure</t>
+  </si>
+  <si>
+    <t>Databricks Utilities</t>
+  </si>
+  <si>
+    <t>dbutils.fs.mounts() / dbutils.fs.unmount("/mnt/&lt;mount-name&gt;")</t>
+  </si>
+  <si>
+    <t>pd.read_excel(path, engine = 'openpyxl')</t>
+  </si>
+  <si>
+    <t>Pandas read_excel removed support for xlsx files</t>
+  </si>
+  <si>
+    <t>read_excel</t>
+  </si>
+  <si>
+    <t>https://strategyanalytics.medium.com/pandas-read-excel-removed-support-for-xlsx-files-426e4acfde89</t>
+  </si>
+  <si>
+    <t>pd.set_option('mode.chained_assignment',None)</t>
+  </si>
+  <si>
+    <t>How to ignore SettingWithCopyWarning using warnings.simplefilter()?</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/54197853/how-to-ignore-settingwithcopywarning-using-warnings-simplefilter</t>
+  </si>
+  <si>
+    <t>exception</t>
+  </si>
+  <si>
+    <t>raise Exception('My error!')</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/13957829/how-to-use-raise-keyword-in-python</t>
+  </si>
+  <si>
+    <t>How to use "raise" keyword in Python [duplicate]</t>
   </si>
 </sst>
 </file>
@@ -3974,7 +4082,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3991,6 +4099,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4377,8 +4486,8 @@
   <dimension ref="B1:I624"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A598" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G483" sqref="G483"/>
+      <pane ySplit="1" topLeftCell="A614" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D637" sqref="D637"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8327,16 +8436,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C994678-E560-3F41-B029-FB176D770DB0}">
-  <dimension ref="B2:H116"/>
+  <dimension ref="B2:H125"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="G117" sqref="G117"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="68.83203125" customWidth="1"/>
     <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" customWidth="1"/>
     <col min="6" max="6" width="55.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9883,6 +9993,171 @@
       </c>
       <c r="G116" s="1" t="s">
         <v>1268</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B117" s="9">
+        <v>44550</v>
+      </c>
+      <c r="C117" t="s">
+        <v>1292</v>
+      </c>
+      <c r="D117" t="s">
+        <v>467</v>
+      </c>
+      <c r="E117" t="s">
+        <v>1289</v>
+      </c>
+      <c r="F117" t="s">
+        <v>1291</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B118" s="9">
+        <v>44550</v>
+      </c>
+      <c r="C118" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D118" t="s">
+        <v>467</v>
+      </c>
+      <c r="E118" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F118" t="s">
+        <v>1294</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B119" s="9">
+        <v>44550</v>
+      </c>
+      <c r="C119" t="s">
+        <v>1298</v>
+      </c>
+      <c r="D119" t="s">
+        <v>467</v>
+      </c>
+      <c r="E119" s="10" t="s">
+        <v>1297</v>
+      </c>
+      <c r="F119" t="s">
+        <v>1300</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B120" s="9">
+        <v>44550</v>
+      </c>
+      <c r="C120" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D120" t="s">
+        <v>467</v>
+      </c>
+      <c r="E120" t="s">
+        <v>1301</v>
+      </c>
+      <c r="F120" t="s">
+        <v>1302</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="121" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C121" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D121" t="s">
+        <v>467</v>
+      </c>
+      <c r="E121" t="s">
+        <v>1306</v>
+      </c>
+      <c r="F121" t="s">
+        <v>1303</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C122" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D122" t="s">
+        <v>1308</v>
+      </c>
+      <c r="E122" t="s">
+        <v>1309</v>
+      </c>
+      <c r="F122" t="s">
+        <v>1310</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C123" t="s">
+        <v>1312</v>
+      </c>
+      <c r="D123" t="s">
+        <v>446</v>
+      </c>
+      <c r="E123" t="s">
+        <v>1313</v>
+      </c>
+      <c r="F123" t="s">
+        <v>1311</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="124" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C124" t="s">
+        <v>1316</v>
+      </c>
+      <c r="D124" t="s">
+        <v>467</v>
+      </c>
+      <c r="E124" t="s">
+        <v>446</v>
+      </c>
+      <c r="F124" t="s">
+        <v>1315</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="125" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C125" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D125" t="s">
+        <v>467</v>
+      </c>
+      <c r="E125" t="s">
+        <v>1318</v>
+      </c>
+      <c r="F125" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>1320</v>
       </c>
     </row>
   </sheetData>
@@ -9999,6 +10274,15 @@
     <hyperlink ref="G114" r:id="rId110" xr:uid="{C0EEB598-C448-644C-B867-BA95DB72F3DE}"/>
     <hyperlink ref="G115" r:id="rId111" xr:uid="{FFD2DFDE-1A4F-8C42-B8F7-EA734D4656E9}"/>
     <hyperlink ref="G116" r:id="rId112" xr:uid="{B8C3285A-89F3-8B49-A095-416E499CEE2E}"/>
+    <hyperlink ref="G117" r:id="rId113" xr:uid="{8A967ADB-FC20-7040-8E11-6F60D541DE53}"/>
+    <hyperlink ref="G118" r:id="rId114" xr:uid="{93C768FA-9FCA-E545-A7EC-E2D796632255}"/>
+    <hyperlink ref="G119" r:id="rId115" xr:uid="{B88EB8D9-8899-314D-90D4-80A0543C83E6}"/>
+    <hyperlink ref="G120" r:id="rId116" xr:uid="{77488B43-1741-9745-9BE8-DC88147214EC}"/>
+    <hyperlink ref="G121" r:id="rId117" xr:uid="{BCC31FF7-CE83-AF4F-AA14-876DF797EB55}"/>
+    <hyperlink ref="G122" r:id="rId118" location="file-system-utility-dbutilsfs" xr:uid="{1CF5BE52-41A3-624D-B469-73F82F24D781}"/>
+    <hyperlink ref="G123" r:id="rId119" xr:uid="{526BDDC7-E425-6348-86E6-6F4B25448230}"/>
+    <hyperlink ref="G124" r:id="rId120" xr:uid="{AF1781ED-3E52-6E47-B6D1-CD4C127A7F9D}"/>
+    <hyperlink ref="G125" r:id="rId121" xr:uid="{37BCE9E0-C3E4-1E4D-9BDF-F5BDFFCB2A45}